<commit_message>
fix some resolusion problem, use pixel instead of point
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassic\Trunk\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
   </bookViews>
   <sheets>
     <sheet name="标准" sheetId="1" r:id="rId1"/>
@@ -3697,10 +3697,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,"F","R",15,mouse,"aurora")){im.Hit*=s.Help/100;im.DHit.Source*=(1+s.Help/100);}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,"E","R",15,mouse,"rocket"))im.OnMagicDamage(s.Damage,7);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3734,10 +3730,6 @@
   </si>
   <si>
     <t>farsummon</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>m.UpdateCellOwner(mouse,0);foreach(IMonster im in m.GetRangeMonster(p.IsLeft,"E","R",15,mouse,"farsummon"))im.DHit.Source*=(1+s.Help/100);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -3894,6 +3886,14 @@
   </si>
   <si>
     <t>永久提高我方单体{3:0.0}%魔法</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,"F","R",15,mouse,"aurora")){}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>m.UpdateCellOwner(mouse,0);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -7302,7 +7302,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7451,11 +7450,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-688691056"/>
-        <c:axId val="-688703024"/>
+        <c:axId val="222937840"/>
+        <c:axId val="225299968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-688691056"/>
+        <c:axId val="222937840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7498,7 +7497,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-688703024"/>
+        <c:crossAx val="225299968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7506,7 +7505,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-688703024"/>
+        <c:axId val="225299968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7557,7 +7556,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-688691056"/>
+        <c:crossAx val="222937840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8585,28 +8584,28 @@
   <dimension ref="A1:Y128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q38" sqref="Q38"/>
+      <selection pane="bottomRight" activeCell="S85" sqref="S85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.625" customWidth="1"/>
-    <col min="2" max="3" width="7.875" customWidth="1"/>
-    <col min="4" max="4" width="4.375" customWidth="1"/>
-    <col min="5" max="5" width="3.125" customWidth="1"/>
-    <col min="6" max="6" width="3.625" customWidth="1"/>
-    <col min="7" max="8" width="3.125" customWidth="1"/>
-    <col min="9" max="9" width="3.875" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
+    <col min="2" max="3" width="7.88671875" customWidth="1"/>
+    <col min="4" max="4" width="4.33203125" customWidth="1"/>
+    <col min="5" max="5" width="3.109375" customWidth="1"/>
+    <col min="6" max="6" width="3.6640625" customWidth="1"/>
+    <col min="7" max="8" width="3.109375" customWidth="1"/>
+    <col min="9" max="9" width="3.88671875" customWidth="1"/>
     <col min="10" max="10" width="4" customWidth="1"/>
-    <col min="11" max="15" width="3.125" customWidth="1"/>
-    <col min="16" max="16" width="5.375" customWidth="1"/>
-    <col min="17" max="17" width="5.75" customWidth="1"/>
-    <col min="18" max="18" width="23.5" customWidth="1"/>
-    <col min="19" max="19" width="24.375" customWidth="1"/>
-    <col min="20" max="20" width="7.875" customWidth="1"/>
+    <col min="11" max="15" width="3.109375" customWidth="1"/>
+    <col min="16" max="16" width="5.33203125" customWidth="1"/>
+    <col min="17" max="17" width="5.77734375" customWidth="1"/>
+    <col min="18" max="18" width="23.44140625" customWidth="1"/>
+    <col min="19" max="19" width="24.33203125" customWidth="1"/>
+    <col min="20" max="20" width="7.88671875" customWidth="1"/>
     <col min="21" max="24" width="4" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8817,7 +8816,7 @@
         <v>661</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="S3" s="6" t="s">
         <v>470</v>
@@ -8841,7 +8840,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="36">
+    <row r="4" spans="1:25" ht="45.6">
       <c r="A4">
         <v>53000001</v>
       </c>
@@ -8918,7 +8917,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="14.25">
+    <row r="5" spans="1:25" ht="26.4">
       <c r="A5">
         <v>53000002</v>
       </c>
@@ -8995,7 +8994,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="24">
+    <row r="6" spans="1:25" ht="26.4">
       <c r="A6">
         <v>53000003</v>
       </c>
@@ -9072,7 +9071,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="36">
+    <row r="7" spans="1:25" ht="34.200000000000003">
       <c r="A7">
         <v>53000004</v>
       </c>
@@ -9125,7 +9124,7 @@
         <v>2000</v>
       </c>
       <c r="R7" s="12" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="S7" s="7" t="s">
         <v>657</v>
@@ -9149,7 +9148,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="24">
+    <row r="8" spans="1:25" ht="26.4">
       <c r="A8">
         <v>53000005</v>
       </c>
@@ -9202,7 +9201,7 @@
         <v>900</v>
       </c>
       <c r="R8" s="12" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="S8" s="7" t="s">
         <v>546</v>
@@ -9226,7 +9225,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="48">
+    <row r="9" spans="1:25" ht="57">
       <c r="A9">
         <v>53000006</v>
       </c>
@@ -9303,7 +9302,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="48">
+    <row r="10" spans="1:25" ht="57">
       <c r="A10">
         <v>53000007</v>
       </c>
@@ -9380,7 +9379,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="48">
+    <row r="11" spans="1:25" ht="57">
       <c r="A11">
         <v>53000008</v>
       </c>
@@ -9457,7 +9456,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="48">
+    <row r="12" spans="1:25" ht="57">
       <c r="A12">
         <v>53000009</v>
       </c>
@@ -9534,7 +9533,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="48">
+    <row r="13" spans="1:25" ht="57">
       <c r="A13">
         <v>53000010</v>
       </c>
@@ -9611,7 +9610,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="48">
+    <row r="14" spans="1:25" ht="57">
       <c r="A14">
         <v>53000011</v>
       </c>
@@ -9688,7 +9687,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="48">
+    <row r="15" spans="1:25" ht="57">
       <c r="A15">
         <v>53000012</v>
       </c>
@@ -9765,7 +9764,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="48">
+    <row r="16" spans="1:25" ht="57">
       <c r="A16">
         <v>53000013</v>
       </c>
@@ -9842,7 +9841,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="48">
+    <row r="17" spans="1:25" ht="57">
       <c r="A17">
         <v>53000014</v>
       </c>
@@ -9919,7 +9918,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="14.25">
+    <row r="18" spans="1:25" ht="26.4">
       <c r="A18">
         <v>53000015</v>
       </c>
@@ -9996,7 +9995,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="24">
+    <row r="19" spans="1:25" ht="26.4">
       <c r="A19">
         <v>53000016</v>
       </c>
@@ -10049,7 +10048,7 @@
         <v>1200</v>
       </c>
       <c r="R19" s="12" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="S19" s="7" t="s">
         <v>508</v>
@@ -10073,7 +10072,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="24">
+    <row r="20" spans="1:25" ht="26.4">
       <c r="A20">
         <v>53000017</v>
       </c>
@@ -10126,7 +10125,7 @@
         <v>8000</v>
       </c>
       <c r="R20" s="12" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="S20" s="7" t="s">
         <v>509</v>
@@ -10150,7 +10149,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="48">
+    <row r="21" spans="1:25" ht="45.6">
       <c r="A21">
         <v>53000018</v>
       </c>
@@ -10227,7 +10226,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="60">
+    <row r="22" spans="1:25" ht="57">
       <c r="A22">
         <v>53000019</v>
       </c>
@@ -10304,7 +10303,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="60">
+    <row r="23" spans="1:25" ht="57">
       <c r="A23">
         <v>53000020</v>
       </c>
@@ -10381,7 +10380,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="60">
+    <row r="24" spans="1:25" ht="57">
       <c r="A24">
         <v>53000021</v>
       </c>
@@ -10458,7 +10457,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="24">
+    <row r="25" spans="1:25" ht="26.4">
       <c r="A25">
         <v>53000022</v>
       </c>
@@ -10535,7 +10534,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="24">
+    <row r="26" spans="1:25" ht="26.4">
       <c r="A26">
         <v>53000023</v>
       </c>
@@ -10612,7 +10611,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="24">
+    <row r="27" spans="1:25" ht="26.4">
       <c r="A27">
         <v>53000024</v>
       </c>
@@ -10689,7 +10688,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="48">
+    <row r="28" spans="1:25" ht="45.6">
       <c r="A28">
         <v>53000025</v>
       </c>
@@ -10766,7 +10765,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="24">
+    <row r="29" spans="1:25" ht="26.4">
       <c r="A29">
         <v>53000026</v>
       </c>
@@ -10843,7 +10842,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="24">
+    <row r="30" spans="1:25" ht="26.4">
       <c r="A30">
         <v>53000027</v>
       </c>
@@ -10920,7 +10919,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="24">
+    <row r="31" spans="1:25" ht="26.4">
       <c r="A31">
         <v>53000028</v>
       </c>
@@ -10997,7 +10996,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="24">
+    <row r="32" spans="1:25" ht="26.4">
       <c r="A32">
         <v>53000029</v>
       </c>
@@ -11074,7 +11073,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="33" spans="1:25" ht="24">
+    <row r="33" spans="1:25" ht="26.4">
       <c r="A33">
         <v>53000030</v>
       </c>
@@ -11127,7 +11126,7 @@
         <v>1500</v>
       </c>
       <c r="R33" s="12" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="S33" s="1" t="s">
         <v>818</v>
@@ -11151,7 +11150,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="34" spans="1:25" ht="24">
+    <row r="34" spans="1:25" ht="26.4">
       <c r="A34">
         <v>53000031</v>
       </c>
@@ -11204,7 +11203,7 @@
         <v>1500</v>
       </c>
       <c r="R34" s="12" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="S34" s="1" t="s">
         <v>823</v>
@@ -11228,7 +11227,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="35" spans="1:25" ht="48">
+    <row r="35" spans="1:25" ht="45.6">
       <c r="A35">
         <v>53000035</v>
       </c>
@@ -11281,7 +11280,7 @@
         <v>2000</v>
       </c>
       <c r="R35" s="12" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="S35" s="7" t="s">
         <v>513</v>
@@ -11305,7 +11304,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="36" spans="1:25" ht="48">
+    <row r="36" spans="1:25" ht="57">
       <c r="A36">
         <v>53000036</v>
       </c>
@@ -11381,7 +11380,7 @@
       </c>
       <c r="Y36" s="27"/>
     </row>
-    <row r="37" spans="1:25" ht="24">
+    <row r="37" spans="1:25" ht="26.4">
       <c r="A37">
         <v>53000037</v>
       </c>
@@ -11458,7 +11457,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="38" spans="1:25" ht="24">
+    <row r="38" spans="1:25" ht="26.4">
       <c r="A38">
         <v>53000038</v>
       </c>
@@ -11511,10 +11510,10 @@
         <v>1200</v>
       </c>
       <c r="R38" s="12" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="S38" s="7" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="T38" s="1" t="s">
         <v>63</v>
@@ -11535,7 +11534,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="24">
+    <row r="39" spans="1:25" ht="26.4">
       <c r="A39">
         <v>53000039</v>
       </c>
@@ -11588,7 +11587,7 @@
         <v>1700</v>
       </c>
       <c r="R39" s="12" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="S39" s="1" t="s">
         <v>812</v>
@@ -11612,7 +11611,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="40" spans="1:25" ht="24">
+    <row r="40" spans="1:25" ht="26.4">
       <c r="A40">
         <v>53000040</v>
       </c>
@@ -11665,7 +11664,7 @@
         <v>2000</v>
       </c>
       <c r="R40" s="12" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="S40" s="1" t="s">
         <v>813</v>
@@ -11689,7 +11688,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="41" spans="1:25" ht="24">
+    <row r="41" spans="1:25" ht="26.4">
       <c r="A41">
         <v>53000041</v>
       </c>
@@ -11766,7 +11765,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="42" spans="1:25" ht="48">
+    <row r="42" spans="1:25" ht="45.6">
       <c r="A42">
         <v>53000042</v>
       </c>
@@ -11819,7 +11818,7 @@
         <v>2000</v>
       </c>
       <c r="R42" s="12" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="S42" s="1" t="s">
         <v>514</v>
@@ -11843,7 +11842,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="43" spans="1:25" ht="24">
+    <row r="43" spans="1:25" ht="26.4">
       <c r="A43">
         <v>53000043</v>
       </c>
@@ -11920,7 +11919,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="44" spans="1:25" ht="24">
+    <row r="44" spans="1:25" ht="26.4">
       <c r="A44">
         <v>53000044</v>
       </c>
@@ -11973,7 +11972,7 @@
         <v>1900</v>
       </c>
       <c r="R44" s="12" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="S44" s="1" t="s">
         <v>814</v>
@@ -11997,7 +11996,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="45" spans="1:25" ht="60">
+    <row r="45" spans="1:25" ht="68.400000000000006">
       <c r="A45">
         <v>53000045</v>
       </c>
@@ -12073,7 +12072,7 @@
       </c>
       <c r="Y45" s="27"/>
     </row>
-    <row r="46" spans="1:25" ht="48">
+    <row r="46" spans="1:25" ht="57">
       <c r="A46">
         <v>53000046</v>
       </c>
@@ -12126,7 +12125,7 @@
         <v>2000</v>
       </c>
       <c r="R46" s="12" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="S46" s="7" t="s">
         <v>528</v>
@@ -12150,7 +12149,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="47" spans="1:25" ht="60">
+    <row r="47" spans="1:25" ht="57">
       <c r="A47">
         <v>53000047</v>
       </c>
@@ -12203,7 +12202,7 @@
         <v>2200</v>
       </c>
       <c r="R47" s="12" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="S47" s="7" t="s">
         <v>529</v>
@@ -12227,7 +12226,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="48" spans="1:25" ht="48">
+    <row r="48" spans="1:25" ht="45.6">
       <c r="A48">
         <v>53000048</v>
       </c>
@@ -12280,7 +12279,7 @@
         <v>2000</v>
       </c>
       <c r="R48" s="12" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="S48" s="1" t="s">
         <v>515</v>
@@ -12304,7 +12303,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="49" spans="1:25" ht="60">
+    <row r="49" spans="1:25" ht="68.400000000000006">
       <c r="A49">
         <v>53000049</v>
       </c>
@@ -12381,7 +12380,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="50" spans="1:25" ht="72">
+    <row r="50" spans="1:25" ht="79.8">
       <c r="A50">
         <v>53000050</v>
       </c>
@@ -12434,7 +12433,7 @@
         <v>1800</v>
       </c>
       <c r="R50" s="12" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="S50" s="7" t="s">
         <v>688</v>
@@ -12458,7 +12457,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="51" spans="1:25" ht="48">
+    <row r="51" spans="1:25" ht="45.6">
       <c r="A51">
         <v>53000051</v>
       </c>
@@ -12511,7 +12510,7 @@
         <v>2000</v>
       </c>
       <c r="R51" s="12" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="S51" s="1" t="s">
         <v>516</v>
@@ -12535,7 +12534,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="52" spans="1:25" ht="48">
+    <row r="52" spans="1:25" ht="45.6">
       <c r="A52">
         <v>53000052</v>
       </c>
@@ -12588,7 +12587,7 @@
         <v>2000</v>
       </c>
       <c r="R52" s="12" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="S52" s="1" t="s">
         <v>517</v>
@@ -12612,7 +12611,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="53" spans="1:25" ht="48">
+    <row r="53" spans="1:25" ht="45.6">
       <c r="A53">
         <v>53000053</v>
       </c>
@@ -12665,7 +12664,7 @@
         <v>2000</v>
       </c>
       <c r="R53" s="12" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="S53" s="1" t="s">
         <v>518</v>
@@ -12689,7 +12688,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="54" spans="1:25" ht="48">
+    <row r="54" spans="1:25" ht="57">
       <c r="A54">
         <v>53000054</v>
       </c>
@@ -12742,7 +12741,7 @@
         <v>1670</v>
       </c>
       <c r="R54" s="12" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="S54" s="7" t="s">
         <v>620</v>
@@ -12766,7 +12765,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="55" spans="1:25" ht="24">
+    <row r="55" spans="1:25" ht="26.4">
       <c r="A55">
         <v>53000055</v>
       </c>
@@ -12843,7 +12842,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="56" spans="1:25" ht="36">
+    <row r="56" spans="1:25" ht="45.6">
       <c r="A56">
         <v>53000056</v>
       </c>
@@ -12920,7 +12919,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="57" spans="1:25" ht="24">
+    <row r="57" spans="1:25" ht="34.200000000000003">
       <c r="A57">
         <v>53000057</v>
       </c>
@@ -12997,7 +12996,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="58" spans="1:25" ht="24">
+    <row r="58" spans="1:25" ht="26.4">
       <c r="A58">
         <v>53000058</v>
       </c>
@@ -13050,7 +13049,7 @@
         <v>1800</v>
       </c>
       <c r="R58" s="12" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="S58" s="7" t="s">
         <v>519</v>
@@ -13074,7 +13073,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="59" spans="1:25" ht="24">
+    <row r="59" spans="1:25" ht="34.200000000000003">
       <c r="A59">
         <v>53000059</v>
       </c>
@@ -13151,7 +13150,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="60" spans="1:25" ht="36">
+    <row r="60" spans="1:25" ht="45.6">
       <c r="A60">
         <v>53000060</v>
       </c>
@@ -13228,7 +13227,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="61" spans="1:25" ht="48">
+    <row r="61" spans="1:25" ht="57">
       <c r="A61">
         <v>53000061</v>
       </c>
@@ -13281,7 +13280,7 @@
         <v>3000</v>
       </c>
       <c r="R61" s="12" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="S61" s="7" t="s">
         <v>571</v>
@@ -13305,7 +13304,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="62" spans="1:25" ht="24">
+    <row r="62" spans="1:25" ht="26.4">
       <c r="A62">
         <v>53000062</v>
       </c>
@@ -13358,7 +13357,7 @@
         <v>3000</v>
       </c>
       <c r="R62" s="12" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="S62" s="7" t="s">
         <v>520</v>
@@ -13382,7 +13381,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="63" spans="1:25" ht="14.25">
+    <row r="63" spans="1:25" ht="26.4">
       <c r="A63">
         <v>53000063</v>
       </c>
@@ -13459,7 +13458,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="64" spans="1:25" ht="24">
+    <row r="64" spans="1:25" ht="26.4">
       <c r="A64">
         <v>53000064</v>
       </c>
@@ -13536,7 +13535,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="65" spans="1:25" ht="48">
+    <row r="65" spans="1:25" ht="45.6">
       <c r="A65">
         <v>53000065</v>
       </c>
@@ -13589,7 +13588,7 @@
         <v>5000</v>
       </c>
       <c r="R65" s="12" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="S65" s="1" t="s">
         <v>713</v>
@@ -13613,7 +13612,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="66" spans="1:25" ht="24">
+    <row r="66" spans="1:25" ht="26.4">
       <c r="A66">
         <v>53000066</v>
       </c>
@@ -13666,7 +13665,7 @@
         <v>1700</v>
       </c>
       <c r="R66" s="12" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="S66" s="1" t="s">
         <v>815</v>
@@ -13690,7 +13689,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="67" spans="1:25" ht="14.25">
+    <row r="67" spans="1:25" ht="26.4">
       <c r="A67">
         <v>53000067</v>
       </c>
@@ -13767,7 +13766,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="68" spans="1:25" ht="60">
+    <row r="68" spans="1:25" ht="57">
       <c r="A68">
         <v>53000068</v>
       </c>
@@ -13820,7 +13819,7 @@
         <v>1200</v>
       </c>
       <c r="R68" s="12" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="S68" s="7" t="s">
         <v>690</v>
@@ -13844,7 +13843,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="69" spans="1:25" ht="24">
+    <row r="69" spans="1:25" ht="26.4">
       <c r="A69">
         <v>53000069</v>
       </c>
@@ -13897,7 +13896,7 @@
         <v>2000</v>
       </c>
       <c r="R69" s="12" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="S69" s="7" t="s">
         <v>521</v>
@@ -13921,7 +13920,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="70" spans="1:25" ht="24">
+    <row r="70" spans="1:25" ht="26.4">
       <c r="A70">
         <v>53000070</v>
       </c>
@@ -13998,7 +13997,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="71" spans="1:25" ht="72">
+    <row r="71" spans="1:25" ht="79.8">
       <c r="A71">
         <v>53000071</v>
       </c>
@@ -14051,7 +14050,7 @@
         <v>2000</v>
       </c>
       <c r="R71" s="12" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="S71" s="7" t="s">
         <v>483</v>
@@ -14073,7 +14072,7 @@
       </c>
       <c r="Y71" s="27"/>
     </row>
-    <row r="72" spans="1:25" ht="48">
+    <row r="72" spans="1:25" ht="57">
       <c r="A72">
         <v>53000072</v>
       </c>
@@ -14126,7 +14125,7 @@
         <v>4000</v>
       </c>
       <c r="R72" s="12" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="S72" s="1" t="s">
         <v>651</v>
@@ -14150,7 +14149,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="73" spans="1:25" ht="48">
+    <row r="73" spans="1:25" ht="45.6">
       <c r="A73">
         <v>53000073</v>
       </c>
@@ -14203,7 +14202,7 @@
         <v>1900</v>
       </c>
       <c r="R73" s="12" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="S73" s="7" t="s">
         <v>522</v>
@@ -14227,7 +14226,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="74" spans="1:25" ht="36">
+    <row r="74" spans="1:25" ht="34.200000000000003">
       <c r="A74">
         <v>53000074</v>
       </c>
@@ -14304,7 +14303,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="75" spans="1:25" ht="108">
+    <row r="75" spans="1:25" ht="125.4">
       <c r="A75">
         <v>53000075</v>
       </c>
@@ -14357,7 +14356,7 @@
         <v>3600</v>
       </c>
       <c r="R75" s="12" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="S75" s="7" t="s">
         <v>523</v>
@@ -14381,7 +14380,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="76" spans="1:25" ht="60">
+    <row r="76" spans="1:25" ht="68.400000000000006">
       <c r="A76">
         <v>53000076</v>
       </c>
@@ -14434,7 +14433,7 @@
         <v>2200</v>
       </c>
       <c r="R76" s="12" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="S76" s="7" t="s">
         <v>691</v>
@@ -14458,7 +14457,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="77" spans="1:25" ht="48">
+    <row r="77" spans="1:25" ht="45.6">
       <c r="A77">
         <v>53000077</v>
       </c>
@@ -14511,7 +14510,7 @@
         <v>1200</v>
       </c>
       <c r="R77" s="12" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="S77" s="7" t="s">
         <v>524</v>
@@ -14535,7 +14534,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="78" spans="1:25" ht="14.25">
+    <row r="78" spans="1:25" ht="26.4">
       <c r="A78">
         <v>53000078</v>
       </c>
@@ -14612,7 +14611,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="79" spans="1:25" ht="72">
+    <row r="79" spans="1:25" ht="45.6">
       <c r="A79">
         <v>53000079</v>
       </c>
@@ -14665,7 +14664,7 @@
         <v>2400</v>
       </c>
       <c r="R79" s="12" t="s">
-        <v>852</v>
+        <v>902</v>
       </c>
       <c r="S79" s="7" t="s">
         <v>720</v>
@@ -14689,7 +14688,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="80" spans="1:25" ht="60">
+    <row r="80" spans="1:25" ht="57">
       <c r="A80">
         <v>53000080</v>
       </c>
@@ -14742,7 +14741,7 @@
         <v>2000</v>
       </c>
       <c r="R80" s="12" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="S80" s="7" t="s">
         <v>525</v>
@@ -14766,7 +14765,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="81" spans="1:25" ht="60">
+    <row r="81" spans="1:25" ht="57">
       <c r="A81">
         <v>53000081</v>
       </c>
@@ -14843,7 +14842,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="82" spans="1:25" ht="36">
+    <row r="82" spans="1:25" ht="34.200000000000003">
       <c r="A82">
         <v>53000082</v>
       </c>
@@ -14920,7 +14919,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="83" spans="1:25" ht="72">
+    <row r="83" spans="1:25" ht="79.8">
       <c r="A83">
         <v>53000083</v>
       </c>
@@ -14973,13 +14972,13 @@
         <v>1200</v>
       </c>
       <c r="R83" s="12" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="S83" s="7" t="s">
         <v>721</v>
       </c>
       <c r="T83" s="1" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="U83" s="1">
         <v>4</v>
@@ -14997,7 +14996,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="84" spans="1:25" ht="72">
+    <row r="84" spans="1:25" ht="26.4">
       <c r="A84">
         <v>53000084</v>
       </c>
@@ -15050,13 +15049,13 @@
         <v>800</v>
       </c>
       <c r="R84" s="12" t="s">
-        <v>862</v>
+        <v>903</v>
       </c>
       <c r="S84" s="7" t="s">
         <v>567</v>
       </c>
       <c r="T84" s="1" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="U84" s="1">
         <v>4</v>
@@ -15074,7 +15073,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="85" spans="1:25" ht="60">
+    <row r="85" spans="1:25" ht="79.8">
       <c r="A85">
         <v>53000085</v>
       </c>
@@ -15127,7 +15126,7 @@
         <v>2000</v>
       </c>
       <c r="R85" s="12" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="S85" s="7" t="s">
         <v>532</v>
@@ -15151,7 +15150,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="86" spans="1:25" ht="60">
+    <row r="86" spans="1:25" ht="68.400000000000006">
       <c r="A86">
         <v>53000086</v>
       </c>
@@ -15228,7 +15227,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="87" spans="1:25" ht="60">
+    <row r="87" spans="1:25" ht="57">
       <c r="A87">
         <v>53000087</v>
       </c>
@@ -15305,7 +15304,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="88" spans="1:25" ht="60">
+    <row r="88" spans="1:25" ht="57">
       <c r="A88">
         <v>53000088</v>
       </c>
@@ -15382,7 +15381,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="89" spans="1:25" ht="60">
+    <row r="89" spans="1:25" ht="57">
       <c r="A89">
         <v>53000089</v>
       </c>
@@ -15435,7 +15434,7 @@
         <v>1800</v>
       </c>
       <c r="R89" s="12" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="S89" s="7" t="s">
         <v>529</v>
@@ -15459,7 +15458,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="90" spans="1:25" ht="60">
+    <row r="90" spans="1:25" ht="57">
       <c r="A90">
         <v>53000090</v>
       </c>
@@ -15512,7 +15511,7 @@
         <v>1650</v>
       </c>
       <c r="R90" s="12" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="S90" s="7" t="s">
         <v>693</v>
@@ -15536,7 +15535,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="91" spans="1:25" ht="36">
+    <row r="91" spans="1:25" ht="34.200000000000003">
       <c r="A91">
         <v>53000091</v>
       </c>
@@ -15613,7 +15612,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="92" spans="1:25" ht="60">
+    <row r="92" spans="1:25" ht="57">
       <c r="A92">
         <v>53000092</v>
       </c>
@@ -15690,7 +15689,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="93" spans="1:25" ht="48">
+    <row r="93" spans="1:25" ht="45.6">
       <c r="A93">
         <v>53000093</v>
       </c>
@@ -15767,7 +15766,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="94" spans="1:25" ht="36">
+    <row r="94" spans="1:25" ht="34.200000000000003">
       <c r="A94">
         <v>53000094</v>
       </c>
@@ -15844,7 +15843,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="95" spans="1:25" ht="48">
+    <row r="95" spans="1:25" ht="57">
       <c r="A95">
         <v>53000095</v>
       </c>
@@ -15921,7 +15920,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="96" spans="1:25" ht="24">
+    <row r="96" spans="1:25" ht="26.4">
       <c r="A96">
         <v>53000096</v>
       </c>
@@ -15996,7 +15995,7 @@
       </c>
       <c r="Y96" s="27"/>
     </row>
-    <row r="97" spans="1:25" ht="60">
+    <row r="97" spans="1:25" ht="57">
       <c r="A97">
         <v>53000097</v>
       </c>
@@ -16049,7 +16048,7 @@
         <v>900</v>
       </c>
       <c r="R97" s="12" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="S97" s="7" t="s">
         <v>526</v>
@@ -16073,7 +16072,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="98" spans="1:25" ht="24">
+    <row r="98" spans="1:25" ht="34.200000000000003">
       <c r="A98">
         <v>53000098</v>
       </c>
@@ -16150,7 +16149,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="99" spans="1:25" ht="24">
+    <row r="99" spans="1:25" ht="34.200000000000003">
       <c r="A99">
         <v>53000099</v>
       </c>
@@ -16227,7 +16226,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="100" spans="1:25" ht="24">
+    <row r="100" spans="1:25" ht="26.4">
       <c r="A100">
         <v>53000100</v>
       </c>
@@ -16304,7 +16303,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="101" spans="1:25" ht="48">
+    <row r="101" spans="1:25" ht="45.6">
       <c r="A101">
         <v>53000101</v>
       </c>
@@ -16379,7 +16378,7 @@
       </c>
       <c r="Y101" s="27"/>
     </row>
-    <row r="102" spans="1:25" ht="24">
+    <row r="102" spans="1:25" ht="26.4">
       <c r="A102">
         <v>53000102</v>
       </c>
@@ -16456,7 +16455,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="103" spans="1:25" ht="72">
+    <row r="103" spans="1:25" ht="79.8">
       <c r="A103">
         <v>53000103</v>
       </c>
@@ -16533,7 +16532,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="104" spans="1:25" ht="60">
+    <row r="104" spans="1:25" ht="57">
       <c r="A104">
         <v>53000104</v>
       </c>
@@ -16610,7 +16609,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="105" spans="1:25" ht="36">
+    <row r="105" spans="1:25" ht="57">
       <c r="A105">
         <v>53000105</v>
       </c>
@@ -16687,7 +16686,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="106" spans="1:25" ht="24">
+    <row r="106" spans="1:25" ht="26.4">
       <c r="A106">
         <v>53000106</v>
       </c>
@@ -16764,7 +16763,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="107" spans="1:25" ht="24">
+    <row r="107" spans="1:25" ht="26.4">
       <c r="A107">
         <v>53000107</v>
       </c>
@@ -16841,7 +16840,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="108" spans="1:25" ht="120">
+    <row r="108" spans="1:25" ht="136.80000000000001">
       <c r="A108">
         <v>53000108</v>
       </c>
@@ -16894,7 +16893,7 @@
         <v>1700</v>
       </c>
       <c r="R108" s="12" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="S108" s="7" t="s">
         <v>527</v>
@@ -16918,7 +16917,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="109" spans="1:25" ht="24">
+    <row r="109" spans="1:25" ht="26.4">
       <c r="A109">
         <v>53000109</v>
       </c>
@@ -16995,7 +16994,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="110" spans="1:25" ht="36">
+    <row r="110" spans="1:25" ht="45.6">
       <c r="A110">
         <v>53000110</v>
       </c>
@@ -17072,7 +17071,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="111" spans="1:25" ht="48">
+    <row r="111" spans="1:25" ht="57">
       <c r="A111">
         <v>53000111</v>
       </c>
@@ -17125,7 +17124,7 @@
         <v>1600</v>
       </c>
       <c r="R111" s="12" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="S111" s="7" t="s">
         <v>541</v>
@@ -17149,7 +17148,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="112" spans="1:25" ht="24">
+    <row r="112" spans="1:25" ht="26.4">
       <c r="A112">
         <v>53000112</v>
       </c>
@@ -17226,7 +17225,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="113" spans="1:25" ht="24">
+    <row r="113" spans="1:25" ht="26.4">
       <c r="A113">
         <v>53000113</v>
       </c>
@@ -17303,7 +17302,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="114" spans="1:25" ht="24">
+    <row r="114" spans="1:25" ht="26.4">
       <c r="A114">
         <v>53000114</v>
       </c>
@@ -17378,7 +17377,7 @@
       </c>
       <c r="Y114" s="27"/>
     </row>
-    <row r="115" spans="1:25" ht="36">
+    <row r="115" spans="1:25" ht="34.200000000000003">
       <c r="A115">
         <v>53000115</v>
       </c>
@@ -17453,7 +17452,7 @@
       </c>
       <c r="Y115" s="27"/>
     </row>
-    <row r="116" spans="1:25" ht="36">
+    <row r="116" spans="1:25" ht="57">
       <c r="A116">
         <v>53000116</v>
       </c>
@@ -17530,7 +17529,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="117" spans="1:25" ht="48">
+    <row r="117" spans="1:25" ht="57">
       <c r="A117">
         <v>53000117</v>
       </c>
@@ -17607,7 +17606,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="118" spans="1:25" ht="48">
+    <row r="118" spans="1:25" ht="57">
       <c r="A118">
         <v>53000118</v>
       </c>
@@ -17684,7 +17683,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="119" spans="1:25" ht="48">
+    <row r="119" spans="1:25" ht="57">
       <c r="A119">
         <v>53000119</v>
       </c>
@@ -17761,7 +17760,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="120" spans="1:25" ht="48">
+    <row r="120" spans="1:25" ht="57">
       <c r="A120">
         <v>53000120</v>
       </c>
@@ -17838,7 +17837,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="121" spans="1:25" ht="48">
+    <row r="121" spans="1:25" ht="57">
       <c r="A121">
         <v>53000121</v>
       </c>
@@ -17915,7 +17914,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="122" spans="1:25" ht="48">
+    <row r="122" spans="1:25" ht="57">
       <c r="A122">
         <v>53000122</v>
       </c>
@@ -17992,7 +17991,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="123" spans="1:25" ht="48">
+    <row r="123" spans="1:25" ht="57">
       <c r="A123">
         <v>53000123</v>
       </c>
@@ -18069,7 +18068,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="124" spans="1:25" ht="48">
+    <row r="124" spans="1:25" ht="57">
       <c r="A124">
         <v>53000124</v>
       </c>
@@ -18146,7 +18145,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="125" spans="1:25" ht="48">
+    <row r="125" spans="1:25" ht="57">
       <c r="A125">
         <v>53000125</v>
       </c>
@@ -18223,7 +18222,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="126" spans="1:25" ht="72">
+    <row r="126" spans="1:25" ht="79.8">
       <c r="A126">
         <v>53000126</v>
       </c>
@@ -18276,13 +18275,13 @@
         <v>2200</v>
       </c>
       <c r="R126" s="12" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="S126" s="7" t="s">
         <v>773</v>
       </c>
       <c r="T126" s="1" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="U126" s="1">
         <v>4</v>
@@ -18300,7 +18299,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="127" spans="1:25" ht="48">
+    <row r="127" spans="1:25" ht="57">
       <c r="A127">
         <v>53000127</v>
       </c>
@@ -18353,7 +18352,7 @@
         <v>3000</v>
       </c>
       <c r="R127" s="12" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="S127" s="7" t="s">
         <v>570</v>
@@ -18377,7 +18376,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="128" spans="1:25" ht="36">
+    <row r="128" spans="1:25" ht="34.200000000000003">
       <c r="A128">
         <v>53000129</v>
       </c>
@@ -18544,22 +18543,22 @@
       <selection pane="bottomRight" activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="3" width="7.875" customWidth="1"/>
-    <col min="4" max="4" width="4.375" customWidth="1"/>
-    <col min="5" max="5" width="3.125" customWidth="1"/>
-    <col min="6" max="6" width="4.625" customWidth="1"/>
-    <col min="7" max="8" width="3.125" customWidth="1"/>
-    <col min="9" max="9" width="3.875" customWidth="1"/>
+    <col min="2" max="3" width="7.88671875" customWidth="1"/>
+    <col min="4" max="4" width="4.33203125" customWidth="1"/>
+    <col min="5" max="5" width="3.109375" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" customWidth="1"/>
+    <col min="7" max="8" width="3.109375" customWidth="1"/>
+    <col min="9" max="9" width="3.88671875" customWidth="1"/>
     <col min="10" max="10" width="4" customWidth="1"/>
-    <col min="11" max="15" width="3.125" customWidth="1"/>
-    <col min="16" max="16" width="5.375" customWidth="1"/>
-    <col min="17" max="17" width="5.75" customWidth="1"/>
-    <col min="18" max="18" width="23.5" customWidth="1"/>
-    <col min="19" max="19" width="27.25" customWidth="1"/>
-    <col min="20" max="20" width="7.875" customWidth="1"/>
+    <col min="11" max="15" width="3.109375" customWidth="1"/>
+    <col min="16" max="16" width="5.33203125" customWidth="1"/>
+    <col min="17" max="17" width="5.77734375" customWidth="1"/>
+    <col min="18" max="18" width="23.44140625" customWidth="1"/>
+    <col min="19" max="19" width="27.21875" customWidth="1"/>
+    <col min="20" max="20" width="7.88671875" customWidth="1"/>
     <col min="21" max="24" width="4" customWidth="1"/>
   </cols>
   <sheetData>
@@ -18794,7 +18793,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="24">
+    <row r="4" spans="1:25" ht="22.8">
       <c r="A4">
         <v>53100000</v>
       </c>
@@ -18865,7 +18864,7 @@
       </c>
       <c r="Y4" s="38"/>
     </row>
-    <row r="5" spans="1:25" ht="14.25">
+    <row r="5" spans="1:25">
       <c r="A5">
         <v>53100001</v>
       </c>
@@ -18936,7 +18935,7 @@
       </c>
       <c r="Y5" s="38"/>
     </row>
-    <row r="6" spans="1:25" ht="24">
+    <row r="6" spans="1:25" ht="34.200000000000003">
       <c r="A6">
         <v>53100002</v>
       </c>
@@ -19007,7 +19006,7 @@
       </c>
       <c r="Y6" s="38"/>
     </row>
-    <row r="7" spans="1:25" ht="14.25">
+    <row r="7" spans="1:25">
       <c r="A7">
         <v>53100003</v>
       </c>
@@ -19078,7 +19077,7 @@
       </c>
       <c r="Y7" s="38"/>
     </row>
-    <row r="8" spans="1:25" ht="36">
+    <row r="8" spans="1:25" ht="34.200000000000003">
       <c r="A8">
         <v>53100004</v>
       </c>
@@ -19149,7 +19148,7 @@
       </c>
       <c r="Y8" s="38"/>
     </row>
-    <row r="9" spans="1:25" ht="24">
+    <row r="9" spans="1:25" ht="22.8">
       <c r="A9">
         <v>53100005</v>
       </c>
@@ -19198,7 +19197,7 @@
         <v>-1</v>
       </c>
       <c r="R9" s="12" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="S9" s="7" t="s">
         <v>640</v>
@@ -19317,22 +19316,22 @@
       <selection pane="bottomRight" activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.75" customWidth="1"/>
-    <col min="2" max="3" width="7.875" customWidth="1"/>
-    <col min="4" max="4" width="4.375" customWidth="1"/>
-    <col min="5" max="5" width="3.125" customWidth="1"/>
-    <col min="6" max="6" width="4.375" customWidth="1"/>
-    <col min="7" max="8" width="3.125" customWidth="1"/>
-    <col min="9" max="9" width="3.875" customWidth="1"/>
+    <col min="1" max="1" width="10.77734375" customWidth="1"/>
+    <col min="2" max="3" width="7.88671875" customWidth="1"/>
+    <col min="4" max="4" width="4.33203125" customWidth="1"/>
+    <col min="5" max="5" width="3.109375" customWidth="1"/>
+    <col min="6" max="6" width="4.33203125" customWidth="1"/>
+    <col min="7" max="8" width="3.109375" customWidth="1"/>
+    <col min="9" max="9" width="3.88671875" customWidth="1"/>
     <col min="10" max="10" width="4" customWidth="1"/>
-    <col min="11" max="15" width="3.125" customWidth="1"/>
-    <col min="16" max="16" width="5.375" customWidth="1"/>
-    <col min="17" max="17" width="5.75" customWidth="1"/>
-    <col min="18" max="18" width="23.5" customWidth="1"/>
-    <col min="19" max="19" width="27.25" customWidth="1"/>
-    <col min="20" max="20" width="7.875" customWidth="1"/>
+    <col min="11" max="15" width="3.109375" customWidth="1"/>
+    <col min="16" max="16" width="5.33203125" customWidth="1"/>
+    <col min="17" max="17" width="5.77734375" customWidth="1"/>
+    <col min="18" max="18" width="23.44140625" customWidth="1"/>
+    <col min="19" max="19" width="27.21875" customWidth="1"/>
+    <col min="20" max="20" width="7.88671875" customWidth="1"/>
     <col min="21" max="21" width="4" customWidth="1"/>
     <col min="22" max="22" width="5" customWidth="1"/>
     <col min="23" max="24" width="4" customWidth="1"/>
@@ -19569,7 +19568,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="36">
+    <row r="4" spans="1:25" ht="45.6">
       <c r="A4">
         <v>53200100</v>
       </c>
@@ -19646,7 +19645,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="24">
+    <row r="5" spans="1:25" ht="26.4">
       <c r="A5">
         <v>53200101</v>
       </c>
@@ -19723,7 +19722,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="40.5">
+    <row r="6" spans="1:25" ht="43.2">
       <c r="A6">
         <v>53200102</v>
       </c>
@@ -19800,7 +19799,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="14.25">
+    <row r="7" spans="1:25" ht="26.4">
       <c r="A7">
         <v>53200103</v>
       </c>
@@ -19877,7 +19876,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="60">
+    <row r="8" spans="1:25" ht="57">
       <c r="A8">
         <v>53200104</v>
       </c>
@@ -19930,7 +19929,7 @@
         <v>1800</v>
       </c>
       <c r="R8" s="12" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="S8" s="7" t="s">
         <v>668</v>
@@ -19954,7 +19953,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="24">
+    <row r="9" spans="1:25" ht="26.4">
       <c r="A9">
         <v>53200105</v>
       </c>
@@ -20007,7 +20006,7 @@
         <v>8000</v>
       </c>
       <c r="R9" s="12" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="S9" s="7" t="s">
         <v>509</v>
@@ -20070,7 +20069,7 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -20119,7 +20118,7 @@
         <v>2.3345235059857505</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15">
+    <row r="5" spans="1:6">
       <c r="A5" s="32" t="s">
         <v>664</v>
       </c>
@@ -20196,7 +20195,7 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" t="s">

</xml_diff>

<commit_message>
close #9 finish card incompelete mark
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="2"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="标准" sheetId="1" r:id="rId1"/>
@@ -717,7 +717,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="896">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1314" uniqueCount="875">
   <si>
     <t>慈悲</t>
   </si>
@@ -3157,31 +3157,155 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>单治,正状</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>单伤</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>count</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>群伤</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>单治</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>正状</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>负状</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>过牌</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>手牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>地形</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>属性</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>单伤，负状</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>群治</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>哥布林巢穴</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>在敌方墓地上尸爆，对1.5卡片距离内敌方单位造成{0}点魔法伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>t.OnMagicDamage(s.Damage,0);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>单伤</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>地形</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>单治</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>单伤,负状</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>单负</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>单伤,负状</t>
+    <t>圣言-痛</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Word Pain</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>WDP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Word Exchange</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>WDE</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>圣言-换</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>将单位的攻速永久升到20,{4:0.0}%几率同时回复{1}点生命</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加目标防御{3:0.0}%的攻击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>正状</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>圣言-停</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Word Stop</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>WDS</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>圣言-速</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Word Haste</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>WDH</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>p.AddLp(p.Mp*s.Help);p.AddMp(-10);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>r.CopyRandomCardFor(p,(int)s.Help);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>圣言-转</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>holy3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Word Roll</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>WDR</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -3189,15 +3313,15 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>手牌</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>单治</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>正状</t>
+    <t>圣言-叛</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Word Betray</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>WDB</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -3205,270 +3329,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>单伤</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>单伤</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>单治,正状</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>单伤</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>count</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>群伤</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>单治</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>正状</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>负状</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>过牌</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>手牌</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>地形</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>手牌</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>群伤</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>属性</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>属性</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>属性</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>群伤</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>单伤，负状</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>负状</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>正状</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>群治</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>群治</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>单伤，负状</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>群伤，负状</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>负状</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>负状</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>单伤</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>负状</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>哥布林巢穴</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>群治</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>属性</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>单治</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>卡牌</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>手牌</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>地形</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>群伤</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>在敌方墓地上尸爆，对1.5卡片距离内敌方单位造成{0}点魔法伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>t.OnMagicDamage(s.Damage,0);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>单伤</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>圣言-痛</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Word Pain</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>WDP</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Word Exchange</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>WDE</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>圣言-换</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>将单位的攻速永久升到20,{4:0.0}%几率同时回复{1}点生命</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>增加目标防御{3:0.0}%的攻击</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>正状</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>圣言-停</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Word Stop</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>WDS</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>圣言-速</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Word Haste</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>WDH</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>p.AddLp(p.Mp*s.Help);p.AddMp(-10);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>r.CopyRandomCardFor(p,(int)s.Help);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>圣言-转</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>holy3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Word Roll</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>WDR</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>群伤</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>圣言-叛</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Word Betray</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>WDB</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>负状</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>p.GetNextNCard(2);if(MathTool.GetRandom(100)&lt;s.Rate) p.GetNextNCard(1);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3489,19 +3349,11 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>陷阱</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>倒虹吸</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>Inverted Siphon</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>陷阱</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -3585,38 +3437,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>属性,基础</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>单状,基础</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>正状，基础</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>正状，基础</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>地形,基础</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>单伤,基础</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>过牌,基础</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>群伤,基础</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,"E","H",40,mouse,"firearrow"))im.OnMagicDamage(s.Damage,7);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3862,6 +3682,80 @@
   </si>
   <si>
     <t>if(MathTool.GetRandom(100)&lt;s.Rate)t.AddHp(s.Cure);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>未完成，单伤,基础</t>
+  </si>
+  <si>
+    <t>未完成，单伤,负状</t>
+  </si>
+  <si>
+    <t>未完成，单状,基础</t>
+  </si>
+  <si>
+    <t>未完成，地形</t>
+  </si>
+  <si>
+    <t>未完成，地形,基础</t>
+  </si>
+  <si>
+    <t>未完成，单治</t>
+  </si>
+  <si>
+    <t>未完成，单负</t>
+  </si>
+  <si>
+    <t>未完成，群伤</t>
+  </si>
+  <si>
+    <t>未完成，手牌</t>
+  </si>
+  <si>
+    <t>未完成，正状，基础</t>
+  </si>
+  <si>
+    <t>未完成，负状</t>
+  </si>
+  <si>
+    <t>未完成，单伤</t>
+  </si>
+  <si>
+    <t>未完成，陷阱</t>
+  </si>
+  <si>
+    <t>未完成，</t>
+  </si>
+  <si>
+    <t>未完成，正状</t>
+  </si>
+  <si>
+    <t>未完成，属性</t>
+  </si>
+  <si>
+    <t>未完成，单伤，负状</t>
+  </si>
+  <si>
+    <t>未完成，群治</t>
+  </si>
+  <si>
+    <t>未完成，群伤，负状</t>
+  </si>
+  <si>
+    <t>未完成，群伤,基础</t>
+  </si>
+  <si>
+    <t>未完成，卡牌</t>
+  </si>
+  <si>
+    <t>未完成，过牌</t>
+  </si>
+  <si>
+    <t>未完成，属性,基础</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>未完成，过牌,基础</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -7270,6 +7164,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7418,11 +7313,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-311405968"/>
-        <c:axId val="-311404336"/>
+        <c:axId val="1969239232"/>
+        <c:axId val="1969239776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-311405968"/>
+        <c:axId val="1969239232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7465,7 +7360,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-311404336"/>
+        <c:crossAx val="1969239776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7473,7 +7368,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-311404336"/>
+        <c:axId val="1969239776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7524,7 +7419,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-311405968"/>
+        <c:crossAx val="1969239232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8551,11 +8446,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y128"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C80" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R81" sqref="R81"/>
+      <selection pane="bottomRight" activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -8707,7 +8602,7 @@
         <v>658</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>801</v>
+        <v>766</v>
       </c>
       <c r="S2" s="11" t="s">
         <v>201</v>
@@ -8784,7 +8679,7 @@
         <v>659</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>852</v>
+        <v>807</v>
       </c>
       <c r="S3" s="6" t="s">
         <v>470</v>
@@ -8861,7 +8756,7 @@
         <v>1704</v>
       </c>
       <c r="R4" s="12" t="s">
-        <v>800</v>
+        <v>765</v>
       </c>
       <c r="S4" s="33" t="s">
         <v>581</v>
@@ -8882,7 +8777,7 @@
         <v>0</v>
       </c>
       <c r="Y4" s="27" t="s">
-        <v>830</v>
+        <v>874</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="14.25">
@@ -8959,7 +8854,7 @@
         <v>0</v>
       </c>
       <c r="Y5" s="27" t="s">
-        <v>824</v>
+        <v>873</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="24">
@@ -9015,7 +8910,7 @@
         <v>2000</v>
       </c>
       <c r="R6" s="12" t="s">
-        <v>772</v>
+        <v>737</v>
       </c>
       <c r="S6" s="7" t="s">
         <v>654</v>
@@ -9036,7 +8931,7 @@
         <v>0</v>
       </c>
       <c r="Y6" s="27" t="s">
-        <v>829</v>
+        <v>851</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="36">
@@ -9092,7 +8987,7 @@
         <v>2000</v>
       </c>
       <c r="R7" s="12" t="s">
-        <v>881</v>
+        <v>836</v>
       </c>
       <c r="S7" s="7" t="s">
         <v>655</v>
@@ -9113,7 +9008,7 @@
         <v>0</v>
       </c>
       <c r="Y7" s="27" t="s">
-        <v>726</v>
+        <v>852</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="24">
@@ -9169,7 +9064,7 @@
         <v>900</v>
       </c>
       <c r="R8" s="12" t="s">
-        <v>870</v>
+        <v>825</v>
       </c>
       <c r="S8" s="7" t="s">
         <v>546</v>
@@ -9190,7 +9085,7 @@
         <v>0</v>
       </c>
       <c r="Y8" s="27" t="s">
-        <v>825</v>
+        <v>853</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="48">
@@ -9267,7 +9162,7 @@
         <v>0</v>
       </c>
       <c r="Y9" s="27" t="s">
-        <v>724</v>
+        <v>854</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="48">
@@ -9344,7 +9239,7 @@
         <v>0</v>
       </c>
       <c r="Y10" s="27" t="s">
-        <v>724</v>
+        <v>854</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="48">
@@ -9421,7 +9316,7 @@
         <v>0</v>
       </c>
       <c r="Y11" s="27" t="s">
-        <v>828</v>
+        <v>855</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="48">
@@ -9498,7 +9393,7 @@
         <v>0</v>
       </c>
       <c r="Y12" s="27" t="s">
-        <v>724</v>
+        <v>854</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="48">
@@ -9575,7 +9470,7 @@
         <v>0</v>
       </c>
       <c r="Y13" s="27" t="s">
-        <v>724</v>
+        <v>854</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="48">
@@ -9652,7 +9547,7 @@
         <v>0</v>
       </c>
       <c r="Y14" s="27" t="s">
-        <v>724</v>
+        <v>854</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="48">
@@ -9729,7 +9624,7 @@
         <v>0</v>
       </c>
       <c r="Y15" s="27" t="s">
-        <v>724</v>
+        <v>854</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="48">
@@ -9806,7 +9701,7 @@
         <v>0</v>
       </c>
       <c r="Y16" s="27" t="s">
-        <v>724</v>
+        <v>854</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="48">
@@ -9883,7 +9778,7 @@
         <v>0</v>
       </c>
       <c r="Y17" s="27" t="s">
-        <v>724</v>
+        <v>854</v>
       </c>
     </row>
     <row r="18" spans="1:25" ht="14.25">
@@ -9960,7 +9855,7 @@
         <v>0</v>
       </c>
       <c r="Y18" s="27" t="s">
-        <v>725</v>
+        <v>856</v>
       </c>
     </row>
     <row r="19" spans="1:25" ht="24">
@@ -10016,7 +9911,7 @@
         <v>1200</v>
       </c>
       <c r="R19" s="12" t="s">
-        <v>871</v>
+        <v>826</v>
       </c>
       <c r="S19" s="7" t="s">
         <v>508</v>
@@ -10037,7 +9932,7 @@
         <v>0</v>
       </c>
       <c r="Y19" s="27" t="s">
-        <v>727</v>
+        <v>857</v>
       </c>
     </row>
     <row r="20" spans="1:25" ht="24">
@@ -10093,7 +9988,7 @@
         <v>8000</v>
       </c>
       <c r="R20" s="12" t="s">
-        <v>872</v>
+        <v>827</v>
       </c>
       <c r="S20" s="7" t="s">
         <v>509</v>
@@ -10114,7 +10009,7 @@
         <v>0</v>
       </c>
       <c r="Y20" s="27" t="s">
-        <v>727</v>
+        <v>857</v>
       </c>
     </row>
     <row r="21" spans="1:25" ht="48">
@@ -10191,7 +10086,7 @@
         <v>0</v>
       </c>
       <c r="Y21" s="27" t="s">
-        <v>728</v>
+        <v>852</v>
       </c>
     </row>
     <row r="22" spans="1:25" ht="60">
@@ -10247,7 +10142,7 @@
         <v>1800</v>
       </c>
       <c r="R22" s="12" t="s">
-        <v>834</v>
+        <v>789</v>
       </c>
       <c r="S22" s="7" t="s">
         <v>666</v>
@@ -10268,7 +10163,7 @@
         <v>0</v>
       </c>
       <c r="Y22" s="27" t="s">
-        <v>729</v>
+        <v>858</v>
       </c>
     </row>
     <row r="23" spans="1:25" ht="60">
@@ -10324,7 +10219,7 @@
         <v>2100</v>
       </c>
       <c r="R23" s="12" t="s">
-        <v>832</v>
+        <v>787</v>
       </c>
       <c r="S23" s="7" t="s">
         <v>667</v>
@@ -10345,7 +10240,7 @@
         <v>0</v>
       </c>
       <c r="Y23" s="27" t="s">
-        <v>729</v>
+        <v>858</v>
       </c>
     </row>
     <row r="24" spans="1:25" ht="60">
@@ -10401,7 +10296,7 @@
         <v>1875</v>
       </c>
       <c r="R24" s="12" t="s">
-        <v>835</v>
+        <v>790</v>
       </c>
       <c r="S24" s="7" t="s">
         <v>668</v>
@@ -10422,7 +10317,7 @@
         <v>0</v>
       </c>
       <c r="Y24" s="27" t="s">
-        <v>729</v>
+        <v>858</v>
       </c>
     </row>
     <row r="25" spans="1:25" ht="24">
@@ -10499,7 +10394,7 @@
         <v>0</v>
       </c>
       <c r="Y25" s="27" t="s">
-        <v>730</v>
+        <v>859</v>
       </c>
     </row>
     <row r="26" spans="1:25" ht="24">
@@ -10576,7 +10471,7 @@
         <v>0</v>
       </c>
       <c r="Y26" s="27" t="s">
-        <v>730</v>
+        <v>859</v>
       </c>
     </row>
     <row r="27" spans="1:25" ht="24">
@@ -10653,7 +10548,7 @@
         <v>0</v>
       </c>
       <c r="Y27" s="27" t="s">
-        <v>730</v>
+        <v>859</v>
       </c>
     </row>
     <row r="28" spans="1:25" ht="48">
@@ -10730,7 +10625,7 @@
         <v>0</v>
       </c>
       <c r="Y28" s="27" t="s">
-        <v>728</v>
+        <v>852</v>
       </c>
     </row>
     <row r="29" spans="1:25" ht="24">
@@ -10807,7 +10702,7 @@
         <v>0</v>
       </c>
       <c r="Y29" s="27" t="s">
-        <v>731</v>
+        <v>856</v>
       </c>
     </row>
     <row r="30" spans="1:25" ht="14.25">
@@ -10882,7 +10777,7 @@
         <v>0</v>
       </c>
       <c r="Y30" s="27" t="s">
-        <v>827</v>
+        <v>860</v>
       </c>
     </row>
     <row r="31" spans="1:25" ht="14.25">
@@ -10957,7 +10852,7 @@
         <v>0</v>
       </c>
       <c r="Y31" s="27" t="s">
-        <v>733</v>
+        <v>861</v>
       </c>
     </row>
     <row r="32" spans="1:25" ht="24">
@@ -11034,7 +10929,7 @@
         <v>0</v>
       </c>
       <c r="Y32" s="27" t="s">
-        <v>734</v>
+        <v>862</v>
       </c>
     </row>
     <row r="33" spans="1:25" ht="24">
@@ -11042,13 +10937,13 @@
         <v>53000030</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>813</v>
+        <v>776</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>814</v>
+        <v>777</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>818</v>
+        <v>781</v>
       </c>
       <c r="E33" s="1">
         <v>2</v>
@@ -11090,10 +10985,10 @@
         <v>1500</v>
       </c>
       <c r="R33" s="12" t="s">
-        <v>863</v>
+        <v>818</v>
       </c>
       <c r="S33" s="1" t="s">
-        <v>815</v>
+        <v>778</v>
       </c>
       <c r="T33" s="1" t="s">
         <v>4</v>
@@ -11111,7 +11006,7 @@
         <v>1</v>
       </c>
       <c r="Y33" s="27" t="s">
-        <v>804</v>
+        <v>863</v>
       </c>
     </row>
     <row r="34" spans="1:25" ht="24">
@@ -11119,13 +11014,13 @@
         <v>53000031</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>816</v>
+        <v>779</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>817</v>
+        <v>780</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>819</v>
+        <v>782</v>
       </c>
       <c r="E34" s="1">
         <v>2</v>
@@ -11167,10 +11062,10 @@
         <v>1500</v>
       </c>
       <c r="R34" s="12" t="s">
-        <v>864</v>
+        <v>819</v>
       </c>
       <c r="S34" s="1" t="s">
-        <v>820</v>
+        <v>783</v>
       </c>
       <c r="T34" s="1" t="s">
         <v>4</v>
@@ -11188,7 +11083,7 @@
         <v>1</v>
       </c>
       <c r="Y34" s="27" t="s">
-        <v>804</v>
+        <v>863</v>
       </c>
     </row>
     <row r="35" spans="1:25" ht="48">
@@ -11244,7 +11139,7 @@
         <v>2000</v>
       </c>
       <c r="R35" s="12" t="s">
-        <v>853</v>
+        <v>808</v>
       </c>
       <c r="S35" s="7" t="s">
         <v>513</v>
@@ -11265,7 +11160,7 @@
         <v>0</v>
       </c>
       <c r="Y35" s="27" t="s">
-        <v>729</v>
+        <v>858</v>
       </c>
     </row>
     <row r="36" spans="1:25" ht="48">
@@ -11342,7 +11237,9 @@
       <c r="X36" s="27">
         <v>0</v>
       </c>
-      <c r="Y36" s="27"/>
+      <c r="Y36" s="27" t="s">
+        <v>864</v>
+      </c>
     </row>
     <row r="37" spans="1:25" ht="14.25">
       <c r="A37">
@@ -11416,7 +11313,7 @@
         <v>0</v>
       </c>
       <c r="Y37" s="27" t="s">
-        <v>826</v>
+        <v>860</v>
       </c>
     </row>
     <row r="38" spans="1:25" ht="14.25">
@@ -11473,7 +11370,7 @@
       </c>
       <c r="R38" s="12"/>
       <c r="S38" s="7" t="s">
-        <v>888</v>
+        <v>843</v>
       </c>
       <c r="T38" s="1" t="s">
         <v>63</v>
@@ -11491,7 +11388,7 @@
         <v>0</v>
       </c>
       <c r="Y38" s="27" t="s">
-        <v>732</v>
+        <v>865</v>
       </c>
     </row>
     <row r="39" spans="1:25" ht="24">
@@ -11499,10 +11396,10 @@
         <v>53000039</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>806</v>
+        <v>770</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>807</v>
+        <v>771</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>374</v>
@@ -11547,10 +11444,10 @@
         <v>1700</v>
       </c>
       <c r="R39" s="12" t="s">
-        <v>865</v>
+        <v>820</v>
       </c>
       <c r="S39" s="1" t="s">
-        <v>809</v>
+        <v>772</v>
       </c>
       <c r="T39" s="1" t="s">
         <v>4</v>
@@ -11568,7 +11465,7 @@
         <v>0</v>
       </c>
       <c r="Y39" s="27" t="s">
-        <v>804</v>
+        <v>863</v>
       </c>
     </row>
     <row r="40" spans="1:25" ht="24">
@@ -11576,7 +11473,7 @@
         <v>53000040</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>802</v>
+        <v>767</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>270</v>
@@ -11624,10 +11521,10 @@
         <v>2000</v>
       </c>
       <c r="R40" s="12" t="s">
-        <v>866</v>
+        <v>821</v>
       </c>
       <c r="S40" s="1" t="s">
-        <v>810</v>
+        <v>773</v>
       </c>
       <c r="T40" s="1" t="s">
         <v>4</v>
@@ -11645,7 +11542,7 @@
         <v>0</v>
       </c>
       <c r="Y40" s="27" t="s">
-        <v>804</v>
+        <v>863</v>
       </c>
     </row>
     <row r="41" spans="1:25" ht="24">
@@ -11722,7 +11619,7 @@
         <v>0</v>
       </c>
       <c r="Y41" s="27" t="s">
-        <v>746</v>
+        <v>859</v>
       </c>
     </row>
     <row r="42" spans="1:25" ht="48">
@@ -11778,7 +11675,7 @@
         <v>2000</v>
       </c>
       <c r="R42" s="12" t="s">
-        <v>854</v>
+        <v>809</v>
       </c>
       <c r="S42" s="1" t="s">
         <v>514</v>
@@ -11799,7 +11696,7 @@
         <v>0</v>
       </c>
       <c r="Y42" s="27" t="s">
-        <v>747</v>
+        <v>858</v>
       </c>
     </row>
     <row r="43" spans="1:25" ht="24">
@@ -11876,7 +11773,7 @@
         <v>0</v>
       </c>
       <c r="Y43" s="27" t="s">
-        <v>749</v>
+        <v>866</v>
       </c>
     </row>
     <row r="44" spans="1:25" ht="24">
@@ -11884,7 +11781,7 @@
         <v>53000044</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>803</v>
+        <v>768</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>274</v>
@@ -11932,10 +11829,10 @@
         <v>1900</v>
       </c>
       <c r="R44" s="12" t="s">
-        <v>867</v>
+        <v>822</v>
       </c>
       <c r="S44" s="1" t="s">
-        <v>811</v>
+        <v>774</v>
       </c>
       <c r="T44" s="1" t="s">
         <v>4</v>
@@ -11953,7 +11850,7 @@
         <v>0</v>
       </c>
       <c r="Y44" s="27" t="s">
-        <v>804</v>
+        <v>863</v>
       </c>
     </row>
     <row r="45" spans="1:25" ht="60">
@@ -12030,7 +11927,9 @@
       <c r="X45" s="27">
         <v>0</v>
       </c>
-      <c r="Y45" s="27"/>
+      <c r="Y45" s="27" t="s">
+        <v>864</v>
+      </c>
     </row>
     <row r="46" spans="1:25" ht="48">
       <c r="A46">
@@ -12085,7 +11984,7 @@
         <v>2000</v>
       </c>
       <c r="R46" s="12" t="s">
-        <v>861</v>
+        <v>816</v>
       </c>
       <c r="S46" s="7" t="s">
         <v>528</v>
@@ -12106,7 +12005,7 @@
         <v>0</v>
       </c>
       <c r="Y46" s="27" t="s">
-        <v>751</v>
+        <v>858</v>
       </c>
     </row>
     <row r="47" spans="1:25" ht="60">
@@ -12162,7 +12061,7 @@
         <v>2200</v>
       </c>
       <c r="R47" s="12" t="s">
-        <v>843</v>
+        <v>798</v>
       </c>
       <c r="S47" s="7" t="s">
         <v>529</v>
@@ -12183,7 +12082,7 @@
         <v>0</v>
       </c>
       <c r="Y47" s="27" t="s">
-        <v>751</v>
+        <v>858</v>
       </c>
     </row>
     <row r="48" spans="1:25" ht="48">
@@ -12239,7 +12138,7 @@
         <v>2000</v>
       </c>
       <c r="R48" s="12" t="s">
-        <v>855</v>
+        <v>810</v>
       </c>
       <c r="S48" s="1" t="s">
         <v>515</v>
@@ -12260,7 +12159,7 @@
         <v>0</v>
       </c>
       <c r="Y48" s="27" t="s">
-        <v>751</v>
+        <v>858</v>
       </c>
     </row>
     <row r="49" spans="1:25" ht="60">
@@ -12316,7 +12215,7 @@
         <v>2200</v>
       </c>
       <c r="R49" s="12" t="s">
-        <v>836</v>
+        <v>791</v>
       </c>
       <c r="S49" s="7" t="s">
         <v>530</v>
@@ -12337,7 +12236,7 @@
         <v>0</v>
       </c>
       <c r="Y49" s="27" t="s">
-        <v>729</v>
+        <v>858</v>
       </c>
     </row>
     <row r="50" spans="1:25" ht="72">
@@ -12393,7 +12292,7 @@
         <v>1800</v>
       </c>
       <c r="R50" s="12" t="s">
-        <v>869</v>
+        <v>824</v>
       </c>
       <c r="S50" s="7" t="s">
         <v>686</v>
@@ -12414,7 +12313,7 @@
         <v>0</v>
       </c>
       <c r="Y50" s="27" t="s">
-        <v>729</v>
+        <v>858</v>
       </c>
     </row>
     <row r="51" spans="1:25" ht="48">
@@ -12470,7 +12369,7 @@
         <v>2000</v>
       </c>
       <c r="R51" s="12" t="s">
-        <v>856</v>
+        <v>811</v>
       </c>
       <c r="S51" s="1" t="s">
         <v>516</v>
@@ -12491,7 +12390,7 @@
         <v>0</v>
       </c>
       <c r="Y51" s="27" t="s">
-        <v>729</v>
+        <v>858</v>
       </c>
     </row>
     <row r="52" spans="1:25" ht="48">
@@ -12547,7 +12446,7 @@
         <v>2000</v>
       </c>
       <c r="R52" s="12" t="s">
-        <v>857</v>
+        <v>812</v>
       </c>
       <c r="S52" s="1" t="s">
         <v>517</v>
@@ -12568,7 +12467,7 @@
         <v>0</v>
       </c>
       <c r="Y52" s="27" t="s">
-        <v>729</v>
+        <v>858</v>
       </c>
     </row>
     <row r="53" spans="1:25" ht="48">
@@ -12624,7 +12523,7 @@
         <v>2000</v>
       </c>
       <c r="R53" s="12" t="s">
-        <v>858</v>
+        <v>813</v>
       </c>
       <c r="S53" s="1" t="s">
         <v>518</v>
@@ -12645,7 +12544,7 @@
         <v>0</v>
       </c>
       <c r="Y53" s="27" t="s">
-        <v>729</v>
+        <v>858</v>
       </c>
     </row>
     <row r="54" spans="1:25" ht="48">
@@ -12701,7 +12600,7 @@
         <v>1670</v>
       </c>
       <c r="R54" s="12" t="s">
-        <v>882</v>
+        <v>837</v>
       </c>
       <c r="S54" s="7" t="s">
         <v>619</v>
@@ -12722,7 +12621,7 @@
         <v>0</v>
       </c>
       <c r="Y54" s="27" t="s">
-        <v>752</v>
+        <v>867</v>
       </c>
     </row>
     <row r="55" spans="1:25" ht="24">
@@ -12799,7 +12698,7 @@
         <v>0</v>
       </c>
       <c r="Y55" s="27" t="s">
-        <v>749</v>
+        <v>866</v>
       </c>
     </row>
     <row r="56" spans="1:25" ht="36">
@@ -12876,7 +12775,7 @@
         <v>0</v>
       </c>
       <c r="Y56" s="27" t="s">
-        <v>749</v>
+        <v>866</v>
       </c>
     </row>
     <row r="57" spans="1:25" ht="24">
@@ -12953,7 +12852,7 @@
         <v>0</v>
       </c>
       <c r="Y57" s="27" t="s">
-        <v>749</v>
+        <v>866</v>
       </c>
     </row>
     <row r="58" spans="1:25" ht="24">
@@ -13009,7 +12908,7 @@
         <v>1800</v>
       </c>
       <c r="R58" s="12" t="s">
-        <v>883</v>
+        <v>838</v>
       </c>
       <c r="S58" s="7" t="s">
         <v>519</v>
@@ -13030,7 +12929,7 @@
         <v>0</v>
       </c>
       <c r="Y58" s="27" t="s">
-        <v>753</v>
+        <v>861</v>
       </c>
     </row>
     <row r="59" spans="1:25" ht="24">
@@ -13086,7 +12985,7 @@
         <v>560</v>
       </c>
       <c r="R59" s="12" t="s">
-        <v>821</v>
+        <v>784</v>
       </c>
       <c r="S59" s="7" t="s">
         <v>579</v>
@@ -13107,7 +13006,7 @@
         <v>0</v>
       </c>
       <c r="Y59" s="27" t="s">
-        <v>754</v>
+        <v>865</v>
       </c>
     </row>
     <row r="60" spans="1:25" ht="36">
@@ -13184,7 +13083,7 @@
         <v>0</v>
       </c>
       <c r="Y60" s="27" t="s">
-        <v>754</v>
+        <v>865</v>
       </c>
     </row>
     <row r="61" spans="1:25" ht="48">
@@ -13240,7 +13139,7 @@
         <v>3000</v>
       </c>
       <c r="R61" s="12" t="s">
-        <v>859</v>
+        <v>814</v>
       </c>
       <c r="S61" s="7" t="s">
         <v>570</v>
@@ -13261,7 +13160,7 @@
         <v>0</v>
       </c>
       <c r="Y61" s="27" t="s">
-        <v>755</v>
+        <v>868</v>
       </c>
     </row>
     <row r="62" spans="1:25" ht="24">
@@ -13317,7 +13216,7 @@
         <v>3000</v>
       </c>
       <c r="R62" s="12" t="s">
-        <v>880</v>
+        <v>835</v>
       </c>
       <c r="S62" s="7" t="s">
         <v>520</v>
@@ -13338,7 +13237,7 @@
         <v>0</v>
       </c>
       <c r="Y62" s="27" t="s">
-        <v>753</v>
+        <v>861</v>
       </c>
     </row>
     <row r="63" spans="1:25" ht="14.25">
@@ -13415,7 +13314,7 @@
         <v>0</v>
       </c>
       <c r="Y63" s="27" t="s">
-        <v>748</v>
+        <v>866</v>
       </c>
     </row>
     <row r="64" spans="1:25" ht="24">
@@ -13471,7 +13370,7 @@
         <v>1500</v>
       </c>
       <c r="R64" s="12" t="s">
-        <v>789</v>
+        <v>754</v>
       </c>
       <c r="S64" s="1" t="s">
         <v>687</v>
@@ -13492,7 +13391,7 @@
         <v>0</v>
       </c>
       <c r="Y64" s="27" t="s">
-        <v>748</v>
+        <v>866</v>
       </c>
     </row>
     <row r="65" spans="1:25" ht="48">
@@ -13548,7 +13447,7 @@
         <v>5000</v>
       </c>
       <c r="R65" s="12" t="s">
-        <v>862</v>
+        <v>817</v>
       </c>
       <c r="S65" s="1" t="s">
         <v>711</v>
@@ -13569,7 +13468,7 @@
         <v>0</v>
       </c>
       <c r="Y65" s="27" t="s">
-        <v>729</v>
+        <v>858</v>
       </c>
     </row>
     <row r="66" spans="1:25" ht="24">
@@ -13625,10 +13524,10 @@
         <v>1700</v>
       </c>
       <c r="R66" s="12" t="s">
-        <v>868</v>
+        <v>823</v>
       </c>
       <c r="S66" s="1" t="s">
-        <v>812</v>
+        <v>775</v>
       </c>
       <c r="T66" s="1" t="s">
         <v>4</v>
@@ -13646,7 +13545,7 @@
         <v>0</v>
       </c>
       <c r="Y66" s="27" t="s">
-        <v>808</v>
+        <v>863</v>
       </c>
     </row>
     <row r="67" spans="1:25" ht="14.25">
@@ -13723,7 +13622,7 @@
         <v>0</v>
       </c>
       <c r="Y67" s="27" t="s">
-        <v>757</v>
+        <v>867</v>
       </c>
     </row>
     <row r="68" spans="1:25" ht="60">
@@ -13779,7 +13678,7 @@
         <v>1200</v>
       </c>
       <c r="R68" s="12" t="s">
-        <v>874</v>
+        <v>829</v>
       </c>
       <c r="S68" s="7" t="s">
         <v>688</v>
@@ -13800,7 +13699,7 @@
         <v>0</v>
       </c>
       <c r="Y68" s="27" t="s">
-        <v>758</v>
+        <v>869</v>
       </c>
     </row>
     <row r="69" spans="1:25" ht="24">
@@ -13856,7 +13755,7 @@
         <v>2000</v>
       </c>
       <c r="R69" s="12" t="s">
-        <v>873</v>
+        <v>828</v>
       </c>
       <c r="S69" s="7" t="s">
         <v>521</v>
@@ -13877,7 +13776,7 @@
         <v>0</v>
       </c>
       <c r="Y69" s="27" t="s">
-        <v>753</v>
+        <v>861</v>
       </c>
     </row>
     <row r="70" spans="1:25" ht="14.25">
@@ -13952,7 +13851,7 @@
         <v>0</v>
       </c>
       <c r="Y70" s="27" t="s">
-        <v>759</v>
+        <v>861</v>
       </c>
     </row>
     <row r="71" spans="1:25" ht="72">
@@ -14008,7 +13907,7 @@
         <v>2000</v>
       </c>
       <c r="R71" s="12" t="s">
-        <v>844</v>
+        <v>799</v>
       </c>
       <c r="S71" s="7" t="s">
         <v>483</v>
@@ -14028,7 +13927,9 @@
       <c r="X71" s="27">
         <v>0</v>
       </c>
-      <c r="Y71" s="27"/>
+      <c r="Y71" s="27" t="s">
+        <v>864</v>
+      </c>
     </row>
     <row r="72" spans="1:25" ht="48">
       <c r="A72">
@@ -14083,7 +13984,7 @@
         <v>4000</v>
       </c>
       <c r="R72" s="12" t="s">
-        <v>875</v>
+        <v>830</v>
       </c>
       <c r="S72" s="1" t="s">
         <v>649</v>
@@ -14104,7 +14005,7 @@
         <v>0</v>
       </c>
       <c r="Y72" s="27" t="s">
-        <v>760</v>
+        <v>861</v>
       </c>
     </row>
     <row r="73" spans="1:25" ht="48">
@@ -14160,7 +14061,7 @@
         <v>1900</v>
       </c>
       <c r="R73" s="12" t="s">
-        <v>879</v>
+        <v>834</v>
       </c>
       <c r="S73" s="7" t="s">
         <v>522</v>
@@ -14181,7 +14082,7 @@
         <v>0</v>
       </c>
       <c r="Y73" s="27" t="s">
-        <v>753</v>
+        <v>861</v>
       </c>
     </row>
     <row r="74" spans="1:25" ht="36">
@@ -14258,7 +14159,7 @@
         <v>0</v>
       </c>
       <c r="Y74" s="27" t="s">
-        <v>761</v>
+        <v>862</v>
       </c>
     </row>
     <row r="75" spans="1:25" ht="108">
@@ -14314,7 +14215,7 @@
         <v>3600</v>
       </c>
       <c r="R75" s="12" t="s">
-        <v>876</v>
+        <v>831</v>
       </c>
       <c r="S75" s="7" t="s">
         <v>523</v>
@@ -14335,7 +14236,7 @@
         <v>0</v>
       </c>
       <c r="Y75" s="27" t="s">
-        <v>760</v>
+        <v>861</v>
       </c>
     </row>
     <row r="76" spans="1:25" ht="60">
@@ -14391,7 +14292,7 @@
         <v>2200</v>
       </c>
       <c r="R76" s="12" t="s">
-        <v>884</v>
+        <v>839</v>
       </c>
       <c r="S76" s="7" t="s">
         <v>689</v>
@@ -14412,7 +14313,7 @@
         <v>0</v>
       </c>
       <c r="Y76" s="27" t="s">
-        <v>753</v>
+        <v>861</v>
       </c>
     </row>
     <row r="77" spans="1:25" ht="48">
@@ -14468,7 +14369,7 @@
         <v>1200</v>
       </c>
       <c r="R77" s="12" t="s">
-        <v>885</v>
+        <v>840</v>
       </c>
       <c r="S77" s="7" t="s">
         <v>524</v>
@@ -14489,7 +14390,7 @@
         <v>0</v>
       </c>
       <c r="Y77" s="27" t="s">
-        <v>753</v>
+        <v>861</v>
       </c>
     </row>
     <row r="78" spans="1:25" ht="14.25">
@@ -14566,7 +14467,7 @@
         <v>0</v>
       </c>
       <c r="Y78" s="27" t="s">
-        <v>749</v>
+        <v>866</v>
       </c>
     </row>
     <row r="79" spans="1:25" ht="48">
@@ -14622,7 +14523,7 @@
         <v>2400</v>
       </c>
       <c r="R79" s="12" t="s">
-        <v>889</v>
+        <v>844</v>
       </c>
       <c r="S79" s="7" t="s">
         <v>718</v>
@@ -14643,7 +14544,7 @@
         <v>0</v>
       </c>
       <c r="Y79" s="27" t="s">
-        <v>732</v>
+        <v>865</v>
       </c>
     </row>
     <row r="80" spans="1:25" ht="60">
@@ -14699,7 +14600,7 @@
         <v>2000</v>
       </c>
       <c r="R80" s="12" t="s">
-        <v>878</v>
+        <v>833</v>
       </c>
       <c r="S80" s="7" t="s">
         <v>525</v>
@@ -14720,7 +14621,7 @@
         <v>0</v>
       </c>
       <c r="Y80" s="27" t="s">
-        <v>762</v>
+        <v>861</v>
       </c>
     </row>
     <row r="81" spans="1:25" ht="60">
@@ -14776,7 +14677,7 @@
         <v>1800</v>
       </c>
       <c r="R81" s="12" t="s">
-        <v>837</v>
+        <v>792</v>
       </c>
       <c r="S81" s="7" t="s">
         <v>531</v>
@@ -14797,7 +14698,7 @@
         <v>0</v>
       </c>
       <c r="Y81" s="27" t="s">
-        <v>729</v>
+        <v>858</v>
       </c>
     </row>
     <row r="82" spans="1:25" ht="24">
@@ -14853,7 +14754,7 @@
         <v>2400</v>
       </c>
       <c r="R82" s="12" t="s">
-        <v>892</v>
+        <v>847</v>
       </c>
       <c r="S82" s="7" t="s">
         <v>720</v>
@@ -14874,7 +14775,7 @@
         <v>0</v>
       </c>
       <c r="Y82" s="27" t="s">
-        <v>754</v>
+        <v>865</v>
       </c>
     </row>
     <row r="83" spans="1:25" ht="24">
@@ -14882,7 +14783,7 @@
         <v>53000083</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>763</v>
+        <v>735</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>306</v>
@@ -14930,13 +14831,13 @@
         <v>1200</v>
       </c>
       <c r="R83" s="12" t="s">
-        <v>893</v>
+        <v>848</v>
       </c>
       <c r="S83" s="7" t="s">
         <v>719</v>
       </c>
       <c r="T83" s="1" t="s">
-        <v>847</v>
+        <v>802</v>
       </c>
       <c r="U83" s="1">
         <v>4</v>
@@ -14951,7 +14852,7 @@
         <v>0</v>
       </c>
       <c r="Y83" s="27" t="s">
-        <v>754</v>
+        <v>865</v>
       </c>
     </row>
     <row r="84" spans="1:25" ht="24">
@@ -15007,13 +14908,13 @@
         <v>800</v>
       </c>
       <c r="R84" s="12" t="s">
-        <v>890</v>
+        <v>845</v>
       </c>
       <c r="S84" s="7" t="s">
         <v>566</v>
       </c>
       <c r="T84" s="1" t="s">
-        <v>848</v>
+        <v>803</v>
       </c>
       <c r="U84" s="1">
         <v>4</v>
@@ -15028,7 +14929,7 @@
         <v>0</v>
       </c>
       <c r="Y84" s="27" t="s">
-        <v>754</v>
+        <v>865</v>
       </c>
     </row>
     <row r="85" spans="1:25" ht="60">
@@ -15084,7 +14985,7 @@
         <v>2000</v>
       </c>
       <c r="R85" s="12" t="s">
-        <v>849</v>
+        <v>804</v>
       </c>
       <c r="S85" s="7" t="s">
         <v>532</v>
@@ -15105,7 +15006,7 @@
         <v>0</v>
       </c>
       <c r="Y85" s="27" t="s">
-        <v>764</v>
+        <v>868</v>
       </c>
     </row>
     <row r="86" spans="1:25" ht="14.25">
@@ -15180,7 +15081,7 @@
         <v>0</v>
       </c>
       <c r="Y86" s="27" t="s">
-        <v>754</v>
+        <v>865</v>
       </c>
     </row>
     <row r="87" spans="1:25" ht="60">
@@ -15236,7 +15137,7 @@
         <v>1500</v>
       </c>
       <c r="R87" s="12" t="s">
-        <v>838</v>
+        <v>793</v>
       </c>
       <c r="S87" s="7" t="s">
         <v>667</v>
@@ -15257,7 +15158,7 @@
         <v>0</v>
       </c>
       <c r="Y87" s="27" t="s">
-        <v>751</v>
+        <v>858</v>
       </c>
     </row>
     <row r="88" spans="1:25" ht="60">
@@ -15313,7 +15214,7 @@
         <v>1750</v>
       </c>
       <c r="R88" s="12" t="s">
-        <v>839</v>
+        <v>794</v>
       </c>
       <c r="S88" s="7" t="s">
         <v>533</v>
@@ -15334,7 +15235,7 @@
         <v>0</v>
       </c>
       <c r="Y88" s="27" t="s">
-        <v>831</v>
+        <v>870</v>
       </c>
     </row>
     <row r="89" spans="1:25" ht="60">
@@ -15390,7 +15291,7 @@
         <v>1800</v>
       </c>
       <c r="R89" s="12" t="s">
-        <v>841</v>
+        <v>796</v>
       </c>
       <c r="S89" s="7" t="s">
         <v>529</v>
@@ -15411,7 +15312,7 @@
         <v>0</v>
       </c>
       <c r="Y89" s="27" t="s">
-        <v>751</v>
+        <v>858</v>
       </c>
     </row>
     <row r="90" spans="1:25" ht="60">
@@ -15467,7 +15368,7 @@
         <v>1650</v>
       </c>
       <c r="R90" s="12" t="s">
-        <v>842</v>
+        <v>797</v>
       </c>
       <c r="S90" s="7" t="s">
         <v>691</v>
@@ -15488,7 +15389,7 @@
         <v>0</v>
       </c>
       <c r="Y90" s="27" t="s">
-        <v>751</v>
+        <v>858</v>
       </c>
     </row>
     <row r="91" spans="1:25" ht="36">
@@ -15565,7 +15466,7 @@
         <v>0</v>
       </c>
       <c r="Y91" s="27" t="s">
-        <v>735</v>
+        <v>862</v>
       </c>
     </row>
     <row r="92" spans="1:25" ht="60">
@@ -15621,7 +15522,7 @@
         <v>1500</v>
       </c>
       <c r="R92" s="12" t="s">
-        <v>840</v>
+        <v>795</v>
       </c>
       <c r="S92" s="7" t="s">
         <v>535</v>
@@ -15642,7 +15543,7 @@
         <v>0</v>
       </c>
       <c r="Y92" s="27" t="s">
-        <v>751</v>
+        <v>858</v>
       </c>
     </row>
     <row r="93" spans="1:25" ht="48">
@@ -15719,7 +15620,7 @@
         <v>0</v>
       </c>
       <c r="Y93" s="27" t="s">
-        <v>735</v>
+        <v>862</v>
       </c>
     </row>
     <row r="94" spans="1:25" ht="36">
@@ -15796,7 +15697,7 @@
         <v>0</v>
       </c>
       <c r="Y94" s="27" t="s">
-        <v>765</v>
+        <v>866</v>
       </c>
     </row>
     <row r="95" spans="1:25" ht="48">
@@ -15852,7 +15753,7 @@
         <v>1600</v>
       </c>
       <c r="R95" s="12" t="s">
-        <v>833</v>
+        <v>788</v>
       </c>
       <c r="S95" s="7" t="s">
         <v>568</v>
@@ -15873,7 +15774,7 @@
         <v>0</v>
       </c>
       <c r="Y95" s="27" t="s">
-        <v>766</v>
+        <v>856</v>
       </c>
     </row>
     <row r="96" spans="1:25" ht="24">
@@ -15949,7 +15850,9 @@
       <c r="X96" s="27">
         <v>0</v>
       </c>
-      <c r="Y96" s="27"/>
+      <c r="Y96" s="27" t="s">
+        <v>864</v>
+      </c>
     </row>
     <row r="97" spans="1:25" ht="60">
       <c r="A97">
@@ -16004,7 +15907,7 @@
         <v>900</v>
       </c>
       <c r="R97" s="12" t="s">
-        <v>886</v>
+        <v>841</v>
       </c>
       <c r="S97" s="7" t="s">
         <v>526</v>
@@ -16025,7 +15928,7 @@
         <v>0</v>
       </c>
       <c r="Y97" s="27" t="s">
-        <v>753</v>
+        <v>861</v>
       </c>
     </row>
     <row r="98" spans="1:25" ht="24">
@@ -16102,7 +16005,7 @@
         <v>0</v>
       </c>
       <c r="Y98" s="27" t="s">
-        <v>723</v>
+        <v>862</v>
       </c>
     </row>
     <row r="99" spans="1:25" ht="24">
@@ -16179,7 +16082,7 @@
         <v>0</v>
       </c>
       <c r="Y99" s="27" t="s">
-        <v>723</v>
+        <v>862</v>
       </c>
     </row>
     <row r="100" spans="1:25" ht="24">
@@ -16256,7 +16159,7 @@
         <v>0</v>
       </c>
       <c r="Y100" s="27" t="s">
-        <v>767</v>
+        <v>871</v>
       </c>
     </row>
     <row r="101" spans="1:25" ht="48">
@@ -16332,7 +16235,9 @@
       <c r="X101" s="27">
         <v>0</v>
       </c>
-      <c r="Y101" s="27"/>
+      <c r="Y101" s="27" t="s">
+        <v>864</v>
+      </c>
     </row>
     <row r="102" spans="1:25" ht="24">
       <c r="A102">
@@ -16408,7 +16313,7 @@
         <v>0</v>
       </c>
       <c r="Y102" s="27" t="s">
-        <v>723</v>
+        <v>862</v>
       </c>
     </row>
     <row r="103" spans="1:25" ht="60">
@@ -16464,7 +16369,7 @@
         <v>1300</v>
       </c>
       <c r="R103" s="12" t="s">
-        <v>891</v>
+        <v>846</v>
       </c>
       <c r="S103" s="7" t="s">
         <v>721</v>
@@ -16485,7 +16390,7 @@
         <v>0</v>
       </c>
       <c r="Y103" s="27" t="s">
-        <v>732</v>
+        <v>865</v>
       </c>
     </row>
     <row r="104" spans="1:25" ht="14.25">
@@ -16560,7 +16465,7 @@
         <v>0</v>
       </c>
       <c r="Y104" s="27" t="s">
-        <v>760</v>
+        <v>861</v>
       </c>
     </row>
     <row r="105" spans="1:25" ht="36">
@@ -16637,7 +16542,7 @@
         <v>0</v>
       </c>
       <c r="Y105" s="27" t="s">
-        <v>748</v>
+        <v>866</v>
       </c>
     </row>
     <row r="106" spans="1:25" ht="24">
@@ -16693,7 +16598,7 @@
         <v>1800</v>
       </c>
       <c r="R106" s="12" t="s">
-        <v>822</v>
+        <v>785</v>
       </c>
       <c r="S106" s="7" t="s">
         <v>702</v>
@@ -16714,7 +16619,7 @@
         <v>0</v>
       </c>
       <c r="Y106" s="27" t="s">
-        <v>732</v>
+        <v>865</v>
       </c>
     </row>
     <row r="107" spans="1:25" ht="24">
@@ -16770,7 +16675,7 @@
         <v>1800</v>
       </c>
       <c r="R107" s="12" t="s">
-        <v>823</v>
+        <v>786</v>
       </c>
       <c r="S107" s="7" t="s">
         <v>560</v>
@@ -16791,7 +16696,7 @@
         <v>0</v>
       </c>
       <c r="Y107" s="27" t="s">
-        <v>760</v>
+        <v>861</v>
       </c>
     </row>
     <row r="108" spans="1:25" ht="120">
@@ -16847,7 +16752,7 @@
         <v>1700</v>
       </c>
       <c r="R108" s="12" t="s">
-        <v>877</v>
+        <v>832</v>
       </c>
       <c r="S108" s="7" t="s">
         <v>527</v>
@@ -16868,7 +16773,7 @@
         <v>0</v>
       </c>
       <c r="Y108" s="27" t="s">
-        <v>760</v>
+        <v>861</v>
       </c>
     </row>
     <row r="109" spans="1:25" ht="24">
@@ -16945,7 +16850,7 @@
         <v>0</v>
       </c>
       <c r="Y109" s="27" t="s">
-        <v>725</v>
+        <v>856</v>
       </c>
     </row>
     <row r="110" spans="1:25" ht="36">
@@ -17022,7 +16927,7 @@
         <v>0</v>
       </c>
       <c r="Y110" s="27" t="s">
-        <v>768</v>
+        <v>859</v>
       </c>
     </row>
     <row r="111" spans="1:25" ht="48">
@@ -17078,7 +16983,7 @@
         <v>1600</v>
       </c>
       <c r="R111" s="12" t="s">
-        <v>860</v>
+        <v>815</v>
       </c>
       <c r="S111" s="7" t="s">
         <v>541</v>
@@ -17099,7 +17004,7 @@
         <v>0</v>
       </c>
       <c r="Y111" s="27" t="s">
-        <v>751</v>
+        <v>858</v>
       </c>
     </row>
     <row r="112" spans="1:25" ht="24">
@@ -17176,7 +17081,7 @@
         <v>0</v>
       </c>
       <c r="Y112" s="27" t="s">
-        <v>768</v>
+        <v>859</v>
       </c>
     </row>
     <row r="113" spans="1:25" ht="24">
@@ -17232,7 +17137,7 @@
         <v>1400</v>
       </c>
       <c r="R113" s="12" t="s">
-        <v>790</v>
+        <v>755</v>
       </c>
       <c r="S113" s="7" t="s">
         <v>710</v>
@@ -17253,7 +17158,7 @@
         <v>0</v>
       </c>
       <c r="Y113" s="27" t="s">
-        <v>768</v>
+        <v>859</v>
       </c>
     </row>
     <row r="114" spans="1:25" ht="24">
@@ -17329,7 +17234,9 @@
       <c r="X114" s="27">
         <v>0</v>
       </c>
-      <c r="Y114" s="27"/>
+      <c r="Y114" s="27" t="s">
+        <v>864</v>
+      </c>
     </row>
     <row r="115" spans="1:25" ht="36">
       <c r="A115">
@@ -17404,7 +17311,9 @@
       <c r="X115" s="27">
         <v>0</v>
       </c>
-      <c r="Y115" s="27"/>
+      <c r="Y115" s="27" t="s">
+        <v>864</v>
+      </c>
     </row>
     <row r="116" spans="1:25" ht="36">
       <c r="A116">
@@ -17480,7 +17389,7 @@
         <v>0</v>
       </c>
       <c r="Y116" s="27" t="s">
-        <v>722</v>
+        <v>872</v>
       </c>
     </row>
     <row r="117" spans="1:25" ht="48">
@@ -17557,7 +17466,7 @@
         <v>0</v>
       </c>
       <c r="Y117" s="27" t="s">
-        <v>769</v>
+        <v>854</v>
       </c>
     </row>
     <row r="118" spans="1:25" ht="48">
@@ -17634,7 +17543,7 @@
         <v>0</v>
       </c>
       <c r="Y118" s="27" t="s">
-        <v>769</v>
+        <v>854</v>
       </c>
     </row>
     <row r="119" spans="1:25" ht="48">
@@ -17711,7 +17620,7 @@
         <v>0</v>
       </c>
       <c r="Y119" s="27" t="s">
-        <v>769</v>
+        <v>854</v>
       </c>
     </row>
     <row r="120" spans="1:25" ht="48">
@@ -17788,7 +17697,7 @@
         <v>0</v>
       </c>
       <c r="Y120" s="27" t="s">
-        <v>769</v>
+        <v>854</v>
       </c>
     </row>
     <row r="121" spans="1:25" ht="48">
@@ -17865,7 +17774,7 @@
         <v>0</v>
       </c>
       <c r="Y121" s="27" t="s">
-        <v>769</v>
+        <v>854</v>
       </c>
     </row>
     <row r="122" spans="1:25" ht="48">
@@ -17942,7 +17851,7 @@
         <v>0</v>
       </c>
       <c r="Y122" s="27" t="s">
-        <v>769</v>
+        <v>854</v>
       </c>
     </row>
     <row r="123" spans="1:25" ht="48">
@@ -18019,7 +17928,7 @@
         <v>0</v>
       </c>
       <c r="Y123" s="27" t="s">
-        <v>769</v>
+        <v>854</v>
       </c>
     </row>
     <row r="124" spans="1:25" ht="48">
@@ -18096,7 +18005,7 @@
         <v>0</v>
       </c>
       <c r="Y124" s="27" t="s">
-        <v>769</v>
+        <v>854</v>
       </c>
     </row>
     <row r="125" spans="1:25" ht="48">
@@ -18173,7 +18082,7 @@
         <v>0</v>
       </c>
       <c r="Y125" s="27" t="s">
-        <v>769</v>
+        <v>854</v>
       </c>
     </row>
     <row r="126" spans="1:25" ht="72">
@@ -18229,13 +18138,13 @@
         <v>2200</v>
       </c>
       <c r="R126" s="12" t="s">
-        <v>851</v>
+        <v>806</v>
       </c>
       <c r="S126" s="7" t="s">
-        <v>771</v>
+        <v>736</v>
       </c>
       <c r="T126" s="1" t="s">
-        <v>850</v>
+        <v>805</v>
       </c>
       <c r="U126" s="1">
         <v>4</v>
@@ -18250,7 +18159,7 @@
         <v>1</v>
       </c>
       <c r="Y126" s="27" t="s">
-        <v>770</v>
+        <v>858</v>
       </c>
     </row>
     <row r="127" spans="1:25" ht="48">
@@ -18306,7 +18215,7 @@
         <v>3000</v>
       </c>
       <c r="R127" s="12" t="s">
-        <v>845</v>
+        <v>800</v>
       </c>
       <c r="S127" s="7" t="s">
         <v>569</v>
@@ -18327,7 +18236,7 @@
         <v>1</v>
       </c>
       <c r="Y127" s="27" t="s">
-        <v>755</v>
+        <v>868</v>
       </c>
     </row>
     <row r="128" spans="1:25" ht="36">
@@ -18404,7 +18313,7 @@
         <v>1</v>
       </c>
       <c r="Y128" s="27" t="s">
-        <v>753</v>
+        <v>861</v>
       </c>
     </row>
   </sheetData>
@@ -19151,7 +19060,7 @@
         <v>-1</v>
       </c>
       <c r="R9" s="12" t="s">
-        <v>887</v>
+        <v>842</v>
       </c>
       <c r="S9" s="7" t="s">
         <v>639</v>
@@ -19263,7 +19172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -19527,13 +19436,13 @@
         <v>53200100</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>783</v>
+        <v>748</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>784</v>
+        <v>749</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>785</v>
+        <v>750</v>
       </c>
       <c r="E4" s="16">
         <v>3</v>
@@ -19575,7 +19484,7 @@
         <v>2300</v>
       </c>
       <c r="R4" s="12" t="s">
-        <v>894</v>
+        <v>849</v>
       </c>
       <c r="S4" s="7" t="s">
         <v>644</v>
@@ -19596,7 +19505,7 @@
         <v>0</v>
       </c>
       <c r="Y4" s="27" t="s">
-        <v>752</v>
+        <v>733</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="24">
@@ -19604,13 +19513,13 @@
         <v>53200101</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>774</v>
+        <v>739</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>775</v>
+        <v>740</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>776</v>
+        <v>741</v>
       </c>
       <c r="E5" s="16">
         <v>3</v>
@@ -19652,7 +19561,7 @@
         <v>1800</v>
       </c>
       <c r="R5" s="12" t="s">
-        <v>772</v>
+        <v>737</v>
       </c>
       <c r="S5" s="7" t="s">
         <v>654</v>
@@ -19673,7 +19582,7 @@
         <v>0</v>
       </c>
       <c r="Y5" s="27" t="s">
-        <v>773</v>
+        <v>738</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="40.5">
@@ -19681,13 +19590,13 @@
         <v>53200102</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>786</v>
+        <v>751</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>787</v>
+        <v>752</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>788</v>
+        <v>753</v>
       </c>
       <c r="E6" s="16">
         <v>3</v>
@@ -19729,10 +19638,10 @@
         <v>2300</v>
       </c>
       <c r="R6" s="12" t="s">
-        <v>895</v>
+        <v>850</v>
       </c>
       <c r="S6" s="34" t="s">
-        <v>780</v>
+        <v>745</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>53</v>
@@ -19750,7 +19659,7 @@
         <v>0</v>
       </c>
       <c r="Y6" s="27" t="s">
-        <v>736</v>
+        <v>722</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="14.25">
@@ -19758,13 +19667,13 @@
         <v>53200103</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>779</v>
+        <v>744</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>777</v>
+        <v>742</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>778</v>
+        <v>743</v>
       </c>
       <c r="E7" s="16">
         <v>3</v>
@@ -19807,7 +19716,7 @@
       </c>
       <c r="R7" s="12"/>
       <c r="S7" s="34" t="s">
-        <v>781</v>
+        <v>746</v>
       </c>
       <c r="T7" s="1" t="s">
         <v>52</v>
@@ -19825,7 +19734,7 @@
         <v>0</v>
       </c>
       <c r="Y7" s="27" t="s">
-        <v>782</v>
+        <v>747</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="60">
@@ -19833,13 +19742,13 @@
         <v>53200104</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>791</v>
+        <v>756</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>793</v>
+        <v>758</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>794</v>
+        <v>759</v>
       </c>
       <c r="E8" s="16">
         <v>3</v>
@@ -19881,13 +19790,13 @@
         <v>1800</v>
       </c>
       <c r="R8" s="12" t="s">
-        <v>846</v>
+        <v>801</v>
       </c>
       <c r="S8" s="7" t="s">
         <v>666</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>792</v>
+        <v>757</v>
       </c>
       <c r="U8" s="1">
         <v>4</v>
@@ -19902,7 +19811,7 @@
         <v>0</v>
       </c>
       <c r="Y8" s="27" t="s">
-        <v>795</v>
+        <v>760</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="24">
@@ -19910,13 +19819,13 @@
         <v>53200105</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>796</v>
+        <v>761</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>797</v>
+        <v>762</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>798</v>
+        <v>763</v>
       </c>
       <c r="E9" s="16">
         <v>3</v>
@@ -19958,7 +19867,7 @@
         <v>8000</v>
       </c>
       <c r="R9" s="12" t="s">
-        <v>872</v>
+        <v>827</v>
       </c>
       <c r="S9" s="7" t="s">
         <v>509</v>
@@ -19979,7 +19888,7 @@
         <v>0</v>
       </c>
       <c r="Y9" s="27" t="s">
-        <v>799</v>
+        <v>764</v>
       </c>
     </row>
   </sheetData>
@@ -20151,12 +20060,12 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" t="s">
-        <v>738</v>
+        <v>724</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>737</v>
+        <v>723</v>
       </c>
       <c r="B2">
         <f>COUNTIF(标准!Y:Y,"*单伤*")</f>
@@ -20165,7 +20074,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>739</v>
+        <v>725</v>
       </c>
       <c r="B3">
         <f>COUNTIF(标准!Y:Y,"*群伤*")</f>
@@ -20174,7 +20083,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>740</v>
+        <v>726</v>
       </c>
       <c r="B4">
         <f>COUNTIF(标准!Y:Y,"*单治*")</f>
@@ -20183,7 +20092,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>756</v>
+        <v>734</v>
       </c>
       <c r="B5">
         <f>COUNTIF(标准!Y:Y,"*群治*")</f>
@@ -20192,7 +20101,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>741</v>
+        <v>727</v>
       </c>
       <c r="B6">
         <f>COUNTIF(标准!Y:Y,"*正状*")</f>
@@ -20201,7 +20110,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>742</v>
+        <v>728</v>
       </c>
       <c r="B7">
         <f>COUNTIF(标准!Y:Y,"*负状*")</f>
@@ -20210,7 +20119,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>744</v>
+        <v>730</v>
       </c>
       <c r="B8">
         <f>COUNTIF(标准!Y:Y,"*手牌*")</f>
@@ -20219,7 +20128,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>743</v>
+        <v>729</v>
       </c>
       <c r="B9">
         <f>COUNTIF(标准!Y:Y,"*过牌*")</f>
@@ -20228,7 +20137,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>805</v>
+        <v>769</v>
       </c>
       <c r="B10">
         <f>COUNTIF(标准!Y:Y,"*陷阱*")</f>
@@ -20237,7 +20146,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>745</v>
+        <v>731</v>
       </c>
       <c r="B11">
         <f>COUNTIF(标准!Y:Y,"*地形*")</f>
@@ -20246,7 +20155,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>750</v>
+        <v>732</v>
       </c>
       <c r="B12">
         <f>COUNTIF(标准!Y:Y,"*属性*")</f>

</xml_diff>

<commit_message>
#8, add basic mon card data
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="标准" sheetId="1" r:id="rId1"/>
@@ -4769,174 +4769,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="137">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
+  <dxfs count="125">
     <dxf>
       <font>
         <b val="0"/>
@@ -4995,284 +4828,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -5287,33 +4842,7 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -5596,6 +5125,34 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -6019,6 +5576,43 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -6302,6 +5896,34 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -6733,6 +6355,138 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -7016,6 +6770,34 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -7445,6 +7227,143 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -7621,11 +7540,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="575560432"/>
-        <c:axId val="727504992"/>
+        <c:axId val="1132320416"/>
+        <c:axId val="1132329120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="575560432"/>
+        <c:axId val="1132320416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7668,7 +7587,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="727504992"/>
+        <c:crossAx val="1132329120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7676,7 +7595,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="727504992"/>
+        <c:axId val="1132329120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7727,7 +7646,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="575560432"/>
+        <c:crossAx val="1132320416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8355,129 +8274,129 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AA128" totalsRowShown="0" headerRowDxfId="136" dataDxfId="135" tableBorderDxfId="134">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AA128" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106" tableBorderDxfId="105">
   <autoFilter ref="A3:AA128"/>
   <sortState ref="A4:Y128">
     <sortCondition ref="A3:A128"/>
   </sortState>
   <tableColumns count="27">
-    <tableColumn id="1" name="Id" dataDxfId="133"/>
-    <tableColumn id="2" name="Name" dataDxfId="132"/>
-    <tableColumn id="20" name="Ename" dataDxfId="131"/>
-    <tableColumn id="21" name="EnameShort" dataDxfId="130"/>
-    <tableColumn id="3" name="Star" dataDxfId="129"/>
-    <tableColumn id="4" name="Type" dataDxfId="128"/>
-    <tableColumn id="5" name="Attr" dataDxfId="127"/>
-    <tableColumn id="8" name="Quality" dataDxfId="1">
-      <calculatedColumnFormula>IF(P4&gt;10,5,IF(P4&gt;4,4,IF(P4&gt;2,3,IF(P4&gt;0,2,IF(P4&gt;-2.5,1,IF(P4&gt;-10,0,6))))))</calculatedColumnFormula>
+    <tableColumn id="1" name="Id" dataDxfId="104"/>
+    <tableColumn id="2" name="Name" dataDxfId="103"/>
+    <tableColumn id="20" name="Ename" dataDxfId="102"/>
+    <tableColumn id="21" name="EnameShort" dataDxfId="101"/>
+    <tableColumn id="3" name="Star" dataDxfId="100"/>
+    <tableColumn id="4" name="Type" dataDxfId="99"/>
+    <tableColumn id="5" name="Attr" dataDxfId="98"/>
+    <tableColumn id="8" name="Quality" dataDxfId="2">
+      <calculatedColumnFormula>IF(P4&gt;10,5,IF(P4&gt;5,4,IF(P4&gt;2.5,3,IF(P4&gt;0,2,IF(P4&gt;-2.5,1,IF(P4&gt;-10,0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="126"/>
-    <tableColumn id="9" name="Damage" dataDxfId="125"/>
-    <tableColumn id="10" name="Cure" dataDxfId="124"/>
-    <tableColumn id="11" name="Time" dataDxfId="123"/>
-    <tableColumn id="13" name="Help" dataDxfId="122"/>
-    <tableColumn id="16" name="Rate" dataDxfId="121"/>
-    <tableColumn id="12" name="Modify" dataDxfId="120"/>
-    <tableColumn id="27" name="Sum" dataDxfId="0">
+    <tableColumn id="7" name="Cost" dataDxfId="97"/>
+    <tableColumn id="9" name="Damage" dataDxfId="96"/>
+    <tableColumn id="10" name="Cure" dataDxfId="95"/>
+    <tableColumn id="11" name="Time" dataDxfId="94"/>
+    <tableColumn id="13" name="Help" dataDxfId="93"/>
+    <tableColumn id="16" name="Rate" dataDxfId="92"/>
+    <tableColumn id="12" name="Modify" dataDxfId="91"/>
+    <tableColumn id="27" name="Sum" dataDxfId="90">
       <calculatedColumnFormula>(S4-2000)/20+O4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="119"/>
-    <tableColumn id="15" name="Target" dataDxfId="118"/>
-    <tableColumn id="25" name="Mark" dataDxfId="117"/>
-    <tableColumn id="22" name="Effect" dataDxfId="116"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="115"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="114"/>
-    <tableColumn id="18" name="Res" dataDxfId="113"/>
-    <tableColumn id="19" name="Icon" dataDxfId="112"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="111"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="110"/>
-    <tableColumn id="26" name="Remark" dataDxfId="109"/>
+    <tableColumn id="6" name="Range" dataDxfId="89"/>
+    <tableColumn id="15" name="Target" dataDxfId="88"/>
+    <tableColumn id="25" name="Mark" dataDxfId="87"/>
+    <tableColumn id="22" name="Effect" dataDxfId="86"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="85"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="84"/>
+    <tableColumn id="18" name="Res" dataDxfId="83"/>
+    <tableColumn id="19" name="Icon" dataDxfId="82"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="81"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="80"/>
+    <tableColumn id="26" name="Remark" dataDxfId="79"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AA9" totalsRowShown="0" headerRowDxfId="108" dataDxfId="107" tableBorderDxfId="106">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AA9" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62" tableBorderDxfId="61">
   <autoFilter ref="A3:AA9"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="27">
-    <tableColumn id="1" name="Id" dataDxfId="105"/>
-    <tableColumn id="2" name="Name" dataDxfId="104"/>
-    <tableColumn id="20" name="Ename" dataDxfId="103"/>
-    <tableColumn id="21" name="EnameShort" dataDxfId="102"/>
-    <tableColumn id="3" name="Star" dataDxfId="101"/>
-    <tableColumn id="4" name="Type" dataDxfId="100"/>
-    <tableColumn id="5" name="Attr" dataDxfId="99"/>
-    <tableColumn id="8" name="Quality" dataDxfId="53">
-      <calculatedColumnFormula>IF(P4&gt;10,5,IF(P4&gt;4,4,IF(P4&gt;2,3,IF(P4&gt;0,2,IF(P4&gt;-2.5,1,IF(P4&gt;-10,0,6))))))</calculatedColumnFormula>
+    <tableColumn id="1" name="Id" dataDxfId="60"/>
+    <tableColumn id="2" name="Name" dataDxfId="59"/>
+    <tableColumn id="20" name="Ename" dataDxfId="58"/>
+    <tableColumn id="21" name="EnameShort" dataDxfId="57"/>
+    <tableColumn id="3" name="Star" dataDxfId="56"/>
+    <tableColumn id="4" name="Type" dataDxfId="55"/>
+    <tableColumn id="5" name="Attr" dataDxfId="54"/>
+    <tableColumn id="8" name="Quality" dataDxfId="1">
+      <calculatedColumnFormula>IF(P4&gt;10,5,IF(P4&gt;5,4,IF(P4&gt;2.5,3,IF(P4&gt;0,2,IF(P4&gt;-2.5,1,IF(P4&gt;-10,0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="98"/>
-    <tableColumn id="9" name="Damage" dataDxfId="97"/>
-    <tableColumn id="10" name="Cure" dataDxfId="96"/>
-    <tableColumn id="11" name="Time" dataDxfId="95"/>
-    <tableColumn id="13" name="Help" dataDxfId="94"/>
-    <tableColumn id="16" name="Rate" dataDxfId="93"/>
-    <tableColumn id="12" name="Modify" dataDxfId="92"/>
-    <tableColumn id="27" name="Sum" dataDxfId="18">
+    <tableColumn id="7" name="Cost" dataDxfId="53"/>
+    <tableColumn id="9" name="Damage" dataDxfId="52"/>
+    <tableColumn id="10" name="Cure" dataDxfId="51"/>
+    <tableColumn id="11" name="Time" dataDxfId="50"/>
+    <tableColumn id="13" name="Help" dataDxfId="49"/>
+    <tableColumn id="16" name="Rate" dataDxfId="48"/>
+    <tableColumn id="12" name="Modify" dataDxfId="47"/>
+    <tableColumn id="27" name="Sum" dataDxfId="46">
       <calculatedColumnFormula>(S4-2000)/20+O4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="91"/>
-    <tableColumn id="15" name="Target" dataDxfId="90"/>
-    <tableColumn id="25" name="Mark" dataDxfId="89"/>
-    <tableColumn id="22" name="Effect" dataDxfId="88"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="87"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="86"/>
-    <tableColumn id="18" name="Res" dataDxfId="85"/>
-    <tableColumn id="19" name="Icon" dataDxfId="84"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="83"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="82"/>
-    <tableColumn id="26" name="Remark" dataDxfId="81"/>
+    <tableColumn id="6" name="Range" dataDxfId="45"/>
+    <tableColumn id="15" name="Target" dataDxfId="44"/>
+    <tableColumn id="25" name="Mark" dataDxfId="43"/>
+    <tableColumn id="22" name="Effect" dataDxfId="42"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="41"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="40"/>
+    <tableColumn id="18" name="Res" dataDxfId="39"/>
+    <tableColumn id="19" name="Icon" dataDxfId="38"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="37"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="36"/>
+    <tableColumn id="26" name="Remark" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_35" displayName="表1_35" ref="A3:AA9" totalsRowShown="0" headerRowDxfId="80" tableBorderDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_35" displayName="表1_35" ref="A3:AA9" totalsRowShown="0" headerRowDxfId="30" tableBorderDxfId="29">
   <autoFilter ref="A3:AA9"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="27">
-    <tableColumn id="1" name="Id" dataDxfId="78"/>
-    <tableColumn id="2" name="Name" dataDxfId="77"/>
-    <tableColumn id="20" name="Ename" dataDxfId="76"/>
-    <tableColumn id="21" name="EnameShort" dataDxfId="75"/>
-    <tableColumn id="3" name="Star" dataDxfId="74"/>
-    <tableColumn id="4" name="Type" dataDxfId="73"/>
-    <tableColumn id="5" name="Attr" dataDxfId="72"/>
-    <tableColumn id="8" name="Quality" dataDxfId="52">
-      <calculatedColumnFormula>IF(P4&gt;10,5,IF(P4&gt;4,4,IF(P4&gt;2,3,IF(P4&gt;0,2,IF(P4&gt;-2.5,1,IF(P4&gt;-10,0,6))))))</calculatedColumnFormula>
+    <tableColumn id="1" name="Id" dataDxfId="28"/>
+    <tableColumn id="2" name="Name" dataDxfId="27"/>
+    <tableColumn id="20" name="Ename" dataDxfId="26"/>
+    <tableColumn id="21" name="EnameShort" dataDxfId="25"/>
+    <tableColumn id="3" name="Star" dataDxfId="24"/>
+    <tableColumn id="4" name="Type" dataDxfId="23"/>
+    <tableColumn id="5" name="Attr" dataDxfId="22"/>
+    <tableColumn id="8" name="Quality" dataDxfId="0">
+      <calculatedColumnFormula>IF(P4&gt;10,5,IF(P4&gt;5,4,IF(P4&gt;2.5,3,IF(P4&gt;0,2,IF(P4&gt;-2.5,1,IF(P4&gt;-10,0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="71"/>
-    <tableColumn id="9" name="Damage" dataDxfId="70"/>
-    <tableColumn id="10" name="Cure" dataDxfId="69"/>
-    <tableColumn id="11" name="Time" dataDxfId="68"/>
-    <tableColumn id="13" name="Help" dataDxfId="67"/>
-    <tableColumn id="16" name="Rate" dataDxfId="66"/>
-    <tableColumn id="12" name="Modify" dataDxfId="65"/>
-    <tableColumn id="27" name="Sum" dataDxfId="19">
+    <tableColumn id="7" name="Cost" dataDxfId="21"/>
+    <tableColumn id="9" name="Damage" dataDxfId="20"/>
+    <tableColumn id="10" name="Cure" dataDxfId="19"/>
+    <tableColumn id="11" name="Time" dataDxfId="18"/>
+    <tableColumn id="13" name="Help" dataDxfId="17"/>
+    <tableColumn id="16" name="Rate" dataDxfId="16"/>
+    <tableColumn id="12" name="Modify" dataDxfId="15"/>
+    <tableColumn id="27" name="Sum" dataDxfId="14">
       <calculatedColumnFormula>(S4-2000)/20+O4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="64"/>
-    <tableColumn id="15" name="Target" dataDxfId="63"/>
-    <tableColumn id="25" name="Mark" dataDxfId="62"/>
-    <tableColumn id="22" name="Effect" dataDxfId="61"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="60"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="59"/>
-    <tableColumn id="18" name="Res" dataDxfId="58"/>
-    <tableColumn id="19" name="Icon" dataDxfId="57"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="56"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="55"/>
-    <tableColumn id="26" name="Remark" dataDxfId="54"/>
+    <tableColumn id="6" name="Range" dataDxfId="13"/>
+    <tableColumn id="15" name="Target" dataDxfId="12"/>
+    <tableColumn id="25" name="Mark" dataDxfId="11"/>
+    <tableColumn id="22" name="Effect" dataDxfId="10"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="9"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="8"/>
+    <tableColumn id="18" name="Res" dataDxfId="7"/>
+    <tableColumn id="19" name="Icon" dataDxfId="6"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="5"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="4"/>
+    <tableColumn id="26" name="Remark" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8772,11 +8691,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L6" sqref="L6"/>
+      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -9072,7 +8991,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="1">
-        <f>IF(P4&gt;10,5,IF(P4&gt;4,4,IF(P4&gt;2,3,IF(P4&gt;0,2,IF(P4&gt;-2.5,1,IF(P4&gt;-10,0,6))))))</f>
+        <f t="shared" ref="H4:H35" si="0">IF(P4&gt;10,5,IF(P4&gt;5,4,IF(P4&gt;2.5,3,IF(P4&gt;0,2,IF(P4&gt;-2.5,1,IF(P4&gt;-10,0,6))))))</f>
         <v>6</v>
       </c>
       <c r="I4" s="1">
@@ -9097,7 +9016,7 @@
         <v>-3</v>
       </c>
       <c r="P4" s="43">
-        <f t="shared" ref="P4:P35" si="0">(S4-2000)/20+O4</f>
+        <f t="shared" ref="P4:P35" si="1">(S4-2000)/20+O4</f>
         <v>-17.8</v>
       </c>
       <c r="Q4" s="1">
@@ -9157,7 +9076,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" ref="H5:H68" si="1">IF(P5&gt;10,5,IF(P5&gt;4,4,IF(P5&gt;2,3,IF(P5&gt;0,2,IF(P5&gt;-2.5,1,IF(P5&gt;-10,0,6))))))</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I5" s="1">
@@ -9182,7 +9101,7 @@
         <v>-3</v>
       </c>
       <c r="P5" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-25.5</v>
       </c>
       <c r="Q5" s="1">
@@ -9242,7 +9161,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I6" s="1">
@@ -9267,7 +9186,7 @@
         <v>-3</v>
       </c>
       <c r="P6" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-3</v>
       </c>
       <c r="Q6" s="1">
@@ -9327,7 +9246,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I7" s="1">
@@ -9352,7 +9271,7 @@
         <v>-2</v>
       </c>
       <c r="P7" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
       <c r="Q7" s="1">
@@ -9412,7 +9331,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I8" s="1">
@@ -9437,7 +9356,7 @@
         <v>-3</v>
       </c>
       <c r="P8" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-58</v>
       </c>
       <c r="Q8" s="1">
@@ -9497,7 +9416,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I9" s="1">
@@ -9522,7 +9441,7 @@
         <v>-3</v>
       </c>
       <c r="P9" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-78</v>
       </c>
       <c r="Q9" s="1">
@@ -9582,7 +9501,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I10" s="1">
@@ -9607,7 +9526,7 @@
         <v>-3</v>
       </c>
       <c r="P10" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-78</v>
       </c>
       <c r="Q10" s="1">
@@ -9667,7 +9586,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I11" s="1">
@@ -9692,7 +9611,7 @@
         <v>-3</v>
       </c>
       <c r="P11" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-78</v>
       </c>
       <c r="Q11" s="1">
@@ -9752,7 +9671,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I12" s="1">
@@ -9777,7 +9696,7 @@
         <v>-3</v>
       </c>
       <c r="P12" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-78</v>
       </c>
       <c r="Q12" s="1">
@@ -9837,7 +9756,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I13" s="1">
@@ -9862,7 +9781,7 @@
         <v>-3</v>
       </c>
       <c r="P13" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-78</v>
       </c>
       <c r="Q13" s="1">
@@ -9922,7 +9841,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I14" s="1">
@@ -9947,7 +9866,7 @@
         <v>-3</v>
       </c>
       <c r="P14" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-78</v>
       </c>
       <c r="Q14" s="1">
@@ -10007,7 +9926,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I15" s="1">
@@ -10032,7 +9951,7 @@
         <v>-3</v>
       </c>
       <c r="P15" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-78</v>
       </c>
       <c r="Q15" s="1">
@@ -10092,7 +10011,7 @@
         <v>0</v>
       </c>
       <c r="H16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I16" s="1">
@@ -10117,7 +10036,7 @@
         <v>-3</v>
       </c>
       <c r="P16" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-78</v>
       </c>
       <c r="Q16" s="1">
@@ -10177,7 +10096,7 @@
         <v>0</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I17" s="1">
@@ -10202,7 +10121,7 @@
         <v>-3</v>
       </c>
       <c r="P17" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-78</v>
       </c>
       <c r="Q17" s="1">
@@ -10262,7 +10181,7 @@
         <v>0</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I18" s="1">
@@ -10287,7 +10206,7 @@
         <v>-3</v>
       </c>
       <c r="P18" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-28</v>
       </c>
       <c r="Q18" s="1">
@@ -10347,7 +10266,7 @@
         <v>0</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I19" s="1">
@@ -10372,7 +10291,7 @@
         <v>-3</v>
       </c>
       <c r="P19" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-43</v>
       </c>
       <c r="Q19" s="1">
@@ -10432,7 +10351,7 @@
         <v>0</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="I20" s="1">
@@ -10457,7 +10376,7 @@
         <v>1</v>
       </c>
       <c r="P20" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>301</v>
       </c>
       <c r="Q20" s="1">
@@ -10517,7 +10436,7 @@
         <v>3</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="I21" s="1">
@@ -10542,7 +10461,7 @@
         <v>0</v>
       </c>
       <c r="P21" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="Q21" s="1">
@@ -10602,7 +10521,7 @@
         <v>3</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I22" s="1">
@@ -10627,7 +10546,7 @@
         <v>1</v>
       </c>
       <c r="P22" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-9</v>
       </c>
       <c r="Q22" s="1">
@@ -10687,7 +10606,7 @@
         <v>7</v>
       </c>
       <c r="H23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="I23" s="1">
@@ -10712,7 +10631,7 @@
         <v>-1</v>
       </c>
       <c r="P23" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="Q23" s="1">
@@ -10772,7 +10691,7 @@
         <v>1</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I24" s="1">
@@ -10797,7 +10716,7 @@
         <v>0</v>
       </c>
       <c r="P24" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-6.25</v>
       </c>
       <c r="Q24" s="1">
@@ -10857,7 +10776,7 @@
         <v>0</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I25" s="1">
@@ -10882,7 +10801,7 @@
         <v>-3</v>
       </c>
       <c r="P25" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-28</v>
       </c>
       <c r="Q25" s="1">
@@ -10942,7 +10861,7 @@
         <v>0</v>
       </c>
       <c r="H26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="I26" s="1">
@@ -10967,7 +10886,7 @@
         <v>1</v>
       </c>
       <c r="P26" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="Q26" s="1">
@@ -11027,7 +10946,7 @@
         <v>0</v>
       </c>
       <c r="H27" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I27" s="1">
@@ -11052,7 +10971,7 @@
         <v>-3</v>
       </c>
       <c r="P27" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-8</v>
       </c>
       <c r="Q27" s="1">
@@ -11112,7 +11031,7 @@
         <v>5</v>
       </c>
       <c r="H28" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="I28" s="1">
@@ -11137,7 +11056,7 @@
         <v>-2</v>
       </c>
       <c r="P28" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="Q28" s="1">
@@ -11197,7 +11116,7 @@
         <v>0</v>
       </c>
       <c r="H29" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I29" s="1">
@@ -11222,7 +11141,7 @@
         <v>3</v>
       </c>
       <c r="P29" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-22</v>
       </c>
       <c r="Q29" s="1">
@@ -11282,7 +11201,7 @@
         <v>0</v>
       </c>
       <c r="H30" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I30" s="1">
@@ -11307,7 +11226,7 @@
         <v>-3</v>
       </c>
       <c r="P30" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-73</v>
       </c>
       <c r="Q30" s="1">
@@ -11365,7 +11284,7 @@
         <v>0</v>
       </c>
       <c r="H31" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I31" s="1">
@@ -11390,7 +11309,7 @@
         <v>-3</v>
       </c>
       <c r="P31" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-73</v>
       </c>
       <c r="Q31" s="1">
@@ -11448,7 +11367,7 @@
         <v>8</v>
       </c>
       <c r="H32" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I32" s="1">
@@ -11473,7 +11392,7 @@
         <v>-1</v>
       </c>
       <c r="P32" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="Q32" s="1">
@@ -11533,7 +11452,7 @@
         <v>5</v>
       </c>
       <c r="H33" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I33" s="1">
@@ -11558,7 +11477,7 @@
         <v>0</v>
       </c>
       <c r="P33" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-25</v>
       </c>
       <c r="Q33" s="1">
@@ -11618,7 +11537,7 @@
         <v>5</v>
       </c>
       <c r="H34" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I34" s="1">
@@ -11643,7 +11562,7 @@
         <v>0</v>
       </c>
       <c r="P34" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-25</v>
       </c>
       <c r="Q34" s="1">
@@ -11703,7 +11622,7 @@
         <v>1</v>
       </c>
       <c r="H35" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I35" s="1">
@@ -11728,7 +11647,7 @@
         <v>-3</v>
       </c>
       <c r="P35" s="43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-3</v>
       </c>
       <c r="Q35" s="1">
@@ -11788,7 +11707,7 @@
         <v>8</v>
       </c>
       <c r="H36" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="H36:H67" si="2">IF(P36&gt;10,5,IF(P36&gt;5,4,IF(P36&gt;2.5,3,IF(P36&gt;0,2,IF(P36&gt;-2.5,1,IF(P36&gt;-10,0,6))))))</f>
         <v>6</v>
       </c>
       <c r="I36" s="1">
@@ -11813,7 +11732,7 @@
         <v>0</v>
       </c>
       <c r="P36" s="43">
-        <f t="shared" ref="P36:P67" si="2">(S36-2000)/20+O36</f>
+        <f t="shared" ref="P36:P67" si="3">(S36-2000)/20+O36</f>
         <v>-39</v>
       </c>
       <c r="Q36" s="1">
@@ -11874,7 +11793,7 @@
         <v>7</v>
       </c>
       <c r="H37" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="I37" s="1">
@@ -11899,7 +11818,7 @@
         <v>-1</v>
       </c>
       <c r="P37" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-11</v>
       </c>
       <c r="Q37" s="1">
@@ -11957,7 +11876,7 @@
         <v>6</v>
       </c>
       <c r="H38" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="I38" s="1">
@@ -11982,7 +11901,7 @@
         <v>-1</v>
       </c>
       <c r="P38" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-41</v>
       </c>
       <c r="Q38" s="1">
@@ -12040,7 +11959,7 @@
         <v>6</v>
       </c>
       <c r="H39" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="I39" s="1">
@@ -12065,7 +11984,7 @@
         <v>0</v>
       </c>
       <c r="P39" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-15</v>
       </c>
       <c r="Q39" s="1">
@@ -12125,7 +12044,7 @@
         <v>0</v>
       </c>
       <c r="H40" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I40" s="1">
@@ -12150,7 +12069,7 @@
         <v>0</v>
       </c>
       <c r="P40" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q40" s="1">
@@ -12210,7 +12129,7 @@
         <v>0</v>
       </c>
       <c r="H41" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I41" s="1">
@@ -12235,7 +12154,7 @@
         <v>-2</v>
       </c>
       <c r="P41" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="Q41" s="1">
@@ -12295,7 +12214,7 @@
         <v>6</v>
       </c>
       <c r="H42" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I42" s="1">
@@ -12320,7 +12239,7 @@
         <v>-3</v>
       </c>
       <c r="P42" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3</v>
       </c>
       <c r="Q42" s="1">
@@ -12380,7 +12299,7 @@
         <v>0</v>
       </c>
       <c r="H43" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I43" s="1">
@@ -12405,7 +12324,7 @@
         <v>0</v>
       </c>
       <c r="P43" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q43" s="1">
@@ -12465,7 +12384,7 @@
         <v>0</v>
       </c>
       <c r="H44" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I44" s="1">
@@ -12490,7 +12409,7 @@
         <v>2</v>
       </c>
       <c r="P44" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3</v>
       </c>
       <c r="Q44" s="1">
@@ -12550,7 +12469,7 @@
         <v>0</v>
       </c>
       <c r="H45" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="I45" s="1">
@@ -12575,7 +12494,7 @@
         <v>0</v>
       </c>
       <c r="P45" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-39</v>
       </c>
       <c r="Q45" s="1">
@@ -12636,7 +12555,7 @@
         <v>2</v>
       </c>
       <c r="H46" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I46" s="1">
@@ -12661,7 +12580,7 @@
         <v>0</v>
       </c>
       <c r="P46" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q46" s="1">
@@ -12721,7 +12640,7 @@
         <v>3</v>
       </c>
       <c r="H47" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I47" s="1">
@@ -12746,7 +12665,7 @@
         <v>3</v>
       </c>
       <c r="P47" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="Q47" s="1">
@@ -12806,7 +12725,7 @@
         <v>3</v>
       </c>
       <c r="H48" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I48" s="1">
@@ -12831,7 +12750,7 @@
         <v>-3</v>
       </c>
       <c r="P48" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3</v>
       </c>
       <c r="Q48" s="1">
@@ -12891,7 +12810,7 @@
         <v>0</v>
       </c>
       <c r="H49" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I49" s="1">
@@ -12916,7 +12835,7 @@
         <v>-1</v>
       </c>
       <c r="P49" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="Q49" s="1">
@@ -12976,7 +12895,7 @@
         <v>4</v>
       </c>
       <c r="H50" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="I50" s="1">
@@ -13001,7 +12920,7 @@
         <v>0</v>
       </c>
       <c r="P50" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-10</v>
       </c>
       <c r="Q50" s="1">
@@ -13061,7 +12980,7 @@
         <v>5</v>
       </c>
       <c r="H51" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I51" s="1">
@@ -13086,7 +13005,7 @@
         <v>-3</v>
       </c>
       <c r="P51" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3</v>
       </c>
       <c r="Q51" s="1">
@@ -13146,7 +13065,7 @@
         <v>4</v>
       </c>
       <c r="H52" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I52" s="1">
@@ -13171,7 +13090,7 @@
         <v>-3</v>
       </c>
       <c r="P52" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3</v>
       </c>
       <c r="Q52" s="1">
@@ -13231,7 +13150,7 @@
         <v>2</v>
       </c>
       <c r="H53" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I53" s="1">
@@ -13256,7 +13175,7 @@
         <v>-3</v>
       </c>
       <c r="P53" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3</v>
       </c>
       <c r="Q53" s="1">
@@ -13316,7 +13235,7 @@
         <v>6</v>
       </c>
       <c r="H54" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="I54" s="1">
@@ -13341,7 +13260,7 @@
         <v>2</v>
       </c>
       <c r="P54" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-14.5</v>
       </c>
       <c r="Q54" s="1">
@@ -13401,7 +13320,7 @@
         <v>7</v>
       </c>
       <c r="H55" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I55" s="1">
@@ -13426,7 +13345,7 @@
         <v>1</v>
       </c>
       <c r="P55" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>51</v>
       </c>
       <c r="Q55" s="1">
@@ -13486,7 +13405,7 @@
         <v>0</v>
       </c>
       <c r="H56" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="I56" s="1">
@@ -13511,7 +13430,7 @@
         <v>0</v>
       </c>
       <c r="P56" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-62.5</v>
       </c>
       <c r="Q56" s="1">
@@ -13571,7 +13490,7 @@
         <v>8</v>
       </c>
       <c r="H57" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="I57" s="1">
@@ -13596,7 +13515,7 @@
         <v>0</v>
       </c>
       <c r="P57" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-25</v>
       </c>
       <c r="Q57" s="1">
@@ -13656,7 +13575,7 @@
         <v>0</v>
       </c>
       <c r="H58" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="I58" s="1">
@@ -13681,7 +13600,7 @@
         <v>0</v>
       </c>
       <c r="P58" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-10</v>
       </c>
       <c r="Q58" s="1">
@@ -13741,7 +13660,7 @@
         <v>0</v>
       </c>
       <c r="H59" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="I59" s="1">
@@ -13766,7 +13685,7 @@
         <v>-2</v>
       </c>
       <c r="P59" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-74</v>
       </c>
       <c r="Q59" s="1">
@@ -13826,7 +13745,7 @@
         <v>0</v>
       </c>
       <c r="H60" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="I60" s="1">
@@ -13851,7 +13770,7 @@
         <v>-3</v>
       </c>
       <c r="P60" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-77</v>
       </c>
       <c r="Q60" s="1">
@@ -13911,7 +13830,7 @@
         <v>7</v>
       </c>
       <c r="H61" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I61" s="1">
@@ -13936,7 +13855,7 @@
         <v>-3</v>
       </c>
       <c r="P61" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>47</v>
       </c>
       <c r="Q61" s="1">
@@ -13996,7 +13915,7 @@
         <v>0</v>
       </c>
       <c r="H62" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I62" s="1">
@@ -14021,7 +13940,7 @@
         <v>-3</v>
       </c>
       <c r="P62" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>47</v>
       </c>
       <c r="Q62" s="1">
@@ -14081,7 +14000,7 @@
         <v>0</v>
       </c>
       <c r="H63" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="I63" s="1">
@@ -14106,7 +14025,7 @@
         <v>3</v>
       </c>
       <c r="P63" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-22</v>
       </c>
       <c r="Q63" s="1">
@@ -14166,7 +14085,7 @@
         <v>0</v>
       </c>
       <c r="H64" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="I64" s="1">
@@ -14191,7 +14110,7 @@
         <v>2</v>
       </c>
       <c r="P64" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-23</v>
       </c>
       <c r="Q64" s="1">
@@ -14251,7 +14170,7 @@
         <v>7</v>
       </c>
       <c r="H65" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I65" s="1">
@@ -14276,7 +14195,7 @@
         <v>3</v>
       </c>
       <c r="P65" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>153</v>
       </c>
       <c r="Q65" s="1">
@@ -14336,7 +14255,7 @@
         <v>6</v>
       </c>
       <c r="H66" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="I66" s="1">
@@ -14361,7 +14280,7 @@
         <v>0</v>
       </c>
       <c r="P66" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-15</v>
       </c>
       <c r="Q66" s="1">
@@ -14421,7 +14340,7 @@
         <v>0</v>
       </c>
       <c r="H67" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I67" s="1">
@@ -14446,7 +14365,7 @@
         <v>1</v>
       </c>
       <c r="P67" s="43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-9</v>
       </c>
       <c r="Q67" s="1">
@@ -14506,7 +14425,7 @@
         <v>0</v>
       </c>
       <c r="H68" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="H68:H99" si="4">IF(P68&gt;10,5,IF(P68&gt;5,4,IF(P68&gt;2.5,3,IF(P68&gt;0,2,IF(P68&gt;-2.5,1,IF(P68&gt;-10,0,6))))))</f>
         <v>6</v>
       </c>
       <c r="I68" s="1">
@@ -14531,7 +14450,7 @@
         <v>0</v>
       </c>
       <c r="P68" s="43">
-        <f t="shared" ref="P68:P99" si="3">(S68-2000)/20+O68</f>
+        <f t="shared" ref="P68:P99" si="5">(S68-2000)/20+O68</f>
         <v>-40</v>
       </c>
       <c r="Q68" s="1">
@@ -14591,7 +14510,7 @@
         <v>0</v>
       </c>
       <c r="H69" s="1">
-        <f t="shared" ref="H69:H128" si="4">IF(P69&gt;10,5,IF(P69&gt;4,4,IF(P69&gt;2,3,IF(P69&gt;0,2,IF(P69&gt;-2.5,1,IF(P69&gt;-10,0,6))))))</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="I69" s="1">
@@ -14616,7 +14535,7 @@
         <v>3</v>
       </c>
       <c r="P69" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="Q69" s="1">
@@ -14701,7 +14620,7 @@
         <v>-1</v>
       </c>
       <c r="P70" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-11</v>
       </c>
       <c r="Q70" s="1">
@@ -14784,7 +14703,7 @@
         <v>2</v>
       </c>
       <c r="P71" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="Q71" s="1">
@@ -14869,7 +14788,7 @@
         <v>2</v>
       </c>
       <c r="P72" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>102</v>
       </c>
       <c r="Q72" s="1">
@@ -14954,7 +14873,7 @@
         <v>3</v>
       </c>
       <c r="P73" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-2</v>
       </c>
       <c r="Q73" s="1">
@@ -15015,7 +14934,7 @@
       </c>
       <c r="H74" s="1">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I74" s="1">
         <v>4</v>
@@ -15039,7 +14958,7 @@
         <v>0</v>
       </c>
       <c r="P74" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="Q74" s="1">
@@ -15124,7 +15043,7 @@
         <v>-3</v>
       </c>
       <c r="P75" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>77</v>
       </c>
       <c r="Q75" s="1">
@@ -15209,7 +15128,7 @@
         <v>0</v>
       </c>
       <c r="P76" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="Q76" s="1">
@@ -15294,7 +15213,7 @@
         <v>0</v>
       </c>
       <c r="P77" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-40</v>
       </c>
       <c r="Q77" s="1">
@@ -15379,7 +15298,7 @@
         <v>0</v>
       </c>
       <c r="P78" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-50</v>
       </c>
       <c r="Q78" s="1">
@@ -15464,7 +15383,7 @@
         <v>-2</v>
       </c>
       <c r="P79" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="Q79" s="1">
@@ -15549,7 +15468,7 @@
         <v>-1</v>
       </c>
       <c r="P80" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="Q80" s="1">
@@ -15634,7 +15553,7 @@
         <v>-1</v>
       </c>
       <c r="P81" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-11</v>
       </c>
       <c r="Q81" s="1">
@@ -15719,7 +15638,7 @@
         <v>0</v>
       </c>
       <c r="P82" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="Q82" s="1">
@@ -15804,7 +15723,7 @@
         <v>3</v>
       </c>
       <c r="P83" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-37</v>
       </c>
       <c r="Q83" s="1">
@@ -15889,7 +15808,7 @@
         <v>3</v>
       </c>
       <c r="P84" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-57</v>
       </c>
       <c r="Q84" s="1">
@@ -15974,7 +15893,7 @@
         <v>1</v>
       </c>
       <c r="P85" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="Q85" s="1">
@@ -16059,7 +15978,7 @@
         <v>0</v>
       </c>
       <c r="P86" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-70</v>
       </c>
       <c r="Q86" s="1">
@@ -16142,7 +16061,7 @@
         <v>3</v>
       </c>
       <c r="P87" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-22</v>
       </c>
       <c r="Q87" s="1">
@@ -16227,7 +16146,7 @@
         <v>2</v>
       </c>
       <c r="P88" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-10.5</v>
       </c>
       <c r="Q88" s="1">
@@ -16312,7 +16231,7 @@
         <v>3</v>
       </c>
       <c r="P89" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-7</v>
       </c>
       <c r="Q89" s="1">
@@ -16397,7 +16316,7 @@
         <v>3</v>
       </c>
       <c r="P90" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-14.5</v>
       </c>
       <c r="Q90" s="1">
@@ -16482,7 +16401,7 @@
         <v>-2</v>
       </c>
       <c r="P91" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-2</v>
       </c>
       <c r="Q91" s="1">
@@ -16567,7 +16486,7 @@
         <v>2</v>
       </c>
       <c r="P92" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-23</v>
       </c>
       <c r="Q92" s="1">
@@ -16652,7 +16571,7 @@
         <v>-2</v>
       </c>
       <c r="P93" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>23</v>
       </c>
       <c r="Q93" s="1">
@@ -16737,7 +16656,7 @@
         <v>0</v>
       </c>
       <c r="P94" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-75</v>
       </c>
       <c r="Q94" s="1">
@@ -16822,7 +16741,7 @@
         <v>3</v>
       </c>
       <c r="P95" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-17</v>
       </c>
       <c r="Q95" s="1">
@@ -16907,7 +16826,7 @@
         <v>-1</v>
       </c>
       <c r="P96" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-51</v>
       </c>
       <c r="Q96" s="1">
@@ -16992,7 +16911,7 @@
         <v>3</v>
       </c>
       <c r="P97" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-52</v>
       </c>
       <c r="Q97" s="1">
@@ -17077,7 +16996,7 @@
         <v>1</v>
       </c>
       <c r="P98" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="Q98" s="1">
@@ -17162,7 +17081,7 @@
         <v>0</v>
       </c>
       <c r="P99" s="43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-5</v>
       </c>
       <c r="Q99" s="1">
@@ -17222,7 +17141,7 @@
         <v>0</v>
       </c>
       <c r="H100" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="H100:H128" si="6">IF(P100&gt;10,5,IF(P100&gt;5,4,IF(P100&gt;2.5,3,IF(P100&gt;0,2,IF(P100&gt;-2.5,1,IF(P100&gt;-10,0,6))))))</f>
         <v>6</v>
       </c>
       <c r="I100" s="1">
@@ -17247,7 +17166,7 @@
         <v>3</v>
       </c>
       <c r="P100" s="43">
-        <f t="shared" ref="P100:P131" si="5">(S100-2000)/20+O100</f>
+        <f t="shared" ref="P100:P128" si="7">(S100-2000)/20+O100</f>
         <v>-17</v>
       </c>
       <c r="Q100" s="1">
@@ -17307,7 +17226,7 @@
         <v>0</v>
       </c>
       <c r="H101" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="I101" s="1">
@@ -17332,7 +17251,7 @@
         <v>0</v>
       </c>
       <c r="P101" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-25</v>
       </c>
       <c r="Q101" s="1">
@@ -17392,7 +17311,7 @@
         <v>2</v>
       </c>
       <c r="H102" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I102" s="1">
@@ -17417,7 +17336,7 @@
         <v>0</v>
       </c>
       <c r="P102" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q102" s="1">
@@ -17477,7 +17396,7 @@
         <v>8</v>
       </c>
       <c r="H103" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="I103" s="1">
@@ -17502,7 +17421,7 @@
         <v>0</v>
       </c>
       <c r="P103" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-35</v>
       </c>
       <c r="Q103" s="1">
@@ -17562,7 +17481,7 @@
         <v>0</v>
       </c>
       <c r="H104" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="I104" s="1">
@@ -17587,7 +17506,7 @@
         <v>0</v>
       </c>
       <c r="P104" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-75</v>
       </c>
       <c r="Q104" s="1">
@@ -17645,7 +17564,7 @@
         <v>0</v>
       </c>
       <c r="H105" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="I105" s="1">
@@ -17670,7 +17589,7 @@
         <v>0</v>
       </c>
       <c r="P105" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-75</v>
       </c>
       <c r="Q105" s="1">
@@ -17730,7 +17649,7 @@
         <v>3</v>
       </c>
       <c r="H106" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="I106" s="1">
@@ -17755,7 +17674,7 @@
         <v>-1</v>
       </c>
       <c r="P106" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-11</v>
       </c>
       <c r="Q106" s="1">
@@ -17815,7 +17734,7 @@
         <v>8</v>
       </c>
       <c r="H107" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="I107" s="1">
@@ -17840,7 +17759,7 @@
         <v>-1</v>
       </c>
       <c r="P107" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-11</v>
       </c>
       <c r="Q107" s="1">
@@ -17900,7 +17819,7 @@
         <v>0</v>
       </c>
       <c r="H108" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="I108" s="1">
@@ -17925,7 +17844,7 @@
         <v>3</v>
       </c>
       <c r="P108" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-12</v>
       </c>
       <c r="Q108" s="1">
@@ -17985,7 +17904,7 @@
         <v>0</v>
       </c>
       <c r="H109" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="I109" s="1">
@@ -18010,7 +17929,7 @@
         <v>0</v>
       </c>
       <c r="P109" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-10</v>
       </c>
       <c r="Q109" s="1">
@@ -18070,8 +17989,8 @@
         <v>0</v>
       </c>
       <c r="H110" s="1">
-        <f t="shared" si="4"/>
-        <v>4</v>
+        <f t="shared" si="6"/>
+        <v>3</v>
       </c>
       <c r="I110" s="1">
         <v>4</v>
@@ -18095,7 +18014,7 @@
         <v>0</v>
       </c>
       <c r="P110" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="Q110" s="1">
@@ -18155,7 +18074,7 @@
         <v>7</v>
       </c>
       <c r="H111" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="I111" s="1">
@@ -18180,7 +18099,7 @@
         <v>3</v>
       </c>
       <c r="P111" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-17</v>
       </c>
       <c r="Q111" s="1">
@@ -18240,7 +18159,7 @@
         <v>8</v>
       </c>
       <c r="H112" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="I112" s="1">
@@ -18265,7 +18184,7 @@
         <v>0</v>
       </c>
       <c r="P112" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
       <c r="Q112" s="1">
@@ -18325,7 +18244,7 @@
         <v>0</v>
       </c>
       <c r="H113" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="I113" s="1">
@@ -18350,7 +18269,7 @@
         <v>2</v>
       </c>
       <c r="P113" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-28</v>
       </c>
       <c r="Q113" s="1">
@@ -18410,7 +18329,7 @@
         <v>0</v>
       </c>
       <c r="H114" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="I114" s="1">
@@ -18435,7 +18354,7 @@
         <v>-1</v>
       </c>
       <c r="P114" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-86</v>
       </c>
       <c r="Q114" s="1">
@@ -18495,7 +18414,7 @@
         <v>0</v>
       </c>
       <c r="H115" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="I115" s="1">
@@ -18520,7 +18439,7 @@
         <v>-1</v>
       </c>
       <c r="P115" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-86</v>
       </c>
       <c r="Q115" s="1">
@@ -18580,7 +18499,7 @@
         <v>0</v>
       </c>
       <c r="H116" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="I116" s="1">
@@ -18605,7 +18524,7 @@
         <v>1</v>
       </c>
       <c r="P116" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-34</v>
       </c>
       <c r="Q116" s="1">
@@ -18665,7 +18584,7 @@
         <v>0</v>
       </c>
       <c r="H117" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="I117" s="1">
@@ -18690,7 +18609,7 @@
         <v>-3</v>
       </c>
       <c r="P117" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-78</v>
       </c>
       <c r="Q117" s="1">
@@ -18750,7 +18669,7 @@
         <v>0</v>
       </c>
       <c r="H118" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="I118" s="1">
@@ -18775,7 +18694,7 @@
         <v>-3</v>
       </c>
       <c r="P118" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-78</v>
       </c>
       <c r="Q118" s="1">
@@ -18835,7 +18754,7 @@
         <v>0</v>
       </c>
       <c r="H119" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="I119" s="1">
@@ -18860,7 +18779,7 @@
         <v>-3</v>
       </c>
       <c r="P119" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-78</v>
       </c>
       <c r="Q119" s="1">
@@ -18920,7 +18839,7 @@
         <v>0</v>
       </c>
       <c r="H120" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="I120" s="1">
@@ -18945,7 +18864,7 @@
         <v>-3</v>
       </c>
       <c r="P120" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-78</v>
       </c>
       <c r="Q120" s="1">
@@ -19005,7 +18924,7 @@
         <v>0</v>
       </c>
       <c r="H121" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="I121" s="1">
@@ -19030,7 +18949,7 @@
         <v>-3</v>
       </c>
       <c r="P121" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-78</v>
       </c>
       <c r="Q121" s="1">
@@ -19090,7 +19009,7 @@
         <v>0</v>
       </c>
       <c r="H122" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="I122" s="1">
@@ -19115,7 +19034,7 @@
         <v>-3</v>
       </c>
       <c r="P122" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-78</v>
       </c>
       <c r="Q122" s="1">
@@ -19175,7 +19094,7 @@
         <v>0</v>
       </c>
       <c r="H123" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="I123" s="1">
@@ -19200,7 +19119,7 @@
         <v>-3</v>
       </c>
       <c r="P123" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-78</v>
       </c>
       <c r="Q123" s="1">
@@ -19260,7 +19179,7 @@
         <v>0</v>
       </c>
       <c r="H124" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="I124" s="1">
@@ -19285,7 +19204,7 @@
         <v>-3</v>
       </c>
       <c r="P124" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-78</v>
       </c>
       <c r="Q124" s="1">
@@ -19345,7 +19264,7 @@
         <v>0</v>
       </c>
       <c r="H125" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="I125" s="1">
@@ -19370,7 +19289,7 @@
         <v>-3</v>
       </c>
       <c r="P125" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-78</v>
       </c>
       <c r="Q125" s="1">
@@ -19430,7 +19349,7 @@
         <v>8</v>
       </c>
       <c r="H126" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="I126" s="1">
@@ -19455,7 +19374,7 @@
         <v>1</v>
       </c>
       <c r="P126" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
       <c r="Q126" s="1">
@@ -19515,7 +19434,7 @@
         <v>7</v>
       </c>
       <c r="H127" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="I127" s="1">
@@ -19540,7 +19459,7 @@
         <v>0</v>
       </c>
       <c r="P127" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>50</v>
       </c>
       <c r="Q127" s="1">
@@ -19600,7 +19519,7 @@
         <v>0</v>
       </c>
       <c r="H128" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I128" s="16">
@@ -19625,7 +19544,7 @@
         <v>3</v>
       </c>
       <c r="P128" s="43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-7</v>
       </c>
       <c r="Q128" s="16">
@@ -19668,81 +19587,81 @@
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I121:I127 I71:I115 I4:I36 I39:I69">
-    <cfRule type="cellIs" dxfId="51" priority="47" operator="notEqual">
+    <cfRule type="cellIs" dxfId="124" priority="47" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J128:P128 J71:P126 J5:P36 J39:P69 J4:O4">
-    <cfRule type="cellIs" dxfId="50" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="46" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I127">
-    <cfRule type="cellIs" dxfId="49" priority="44" operator="notEqual">
+    <cfRule type="cellIs" dxfId="122" priority="44" operator="notEqual">
       <formula>$E127</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I116:I120">
-    <cfRule type="cellIs" dxfId="48" priority="42" operator="notEqual">
+    <cfRule type="cellIs" dxfId="121" priority="42" operator="notEqual">
       <formula>$E116</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I128">
-    <cfRule type="cellIs" dxfId="47" priority="41" operator="notEqual">
+    <cfRule type="cellIs" dxfId="120" priority="41" operator="notEqual">
       <formula>$E128</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J128:P128">
-    <cfRule type="cellIs" dxfId="46" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="40" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J127:P127">
-    <cfRule type="cellIs" dxfId="45" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="26" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I70">
-    <cfRule type="cellIs" dxfId="44" priority="11" operator="notEqual">
+    <cfRule type="cellIs" dxfId="117" priority="11" operator="notEqual">
       <formula>$E70</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J70:P70">
-    <cfRule type="cellIs" dxfId="43" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37">
-    <cfRule type="cellIs" dxfId="42" priority="9" operator="notEqual">
+    <cfRule type="cellIs" dxfId="115" priority="9" operator="notEqual">
       <formula>$E37</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J37:P37">
-    <cfRule type="cellIs" dxfId="41" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38">
-    <cfRule type="cellIs" dxfId="40" priority="7" operator="notEqual">
+    <cfRule type="cellIs" dxfId="113" priority="7" operator="notEqual">
       <formula>$E38</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J38:P38">
-    <cfRule type="cellIs" dxfId="39" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H128">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="4" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="108" priority="5" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19775,7 +19694,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -20067,7 +19986,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="16">
-        <f>IF(P4&gt;10,5,IF(P4&gt;4,4,IF(P4&gt;2,3,IF(P4&gt;0,2,IF(P4&gt;-2.5,1,IF(P4&gt;-10,0,6))))))</f>
+        <f t="shared" ref="H4:H9" si="0">IF(P4&gt;10,5,IF(P4&gt;5,4,IF(P4&gt;2.5,3,IF(P4&gt;0,2,IF(P4&gt;-2.5,1,IF(P4&gt;-10,0,6))))))</f>
         <v>6</v>
       </c>
       <c r="I4" s="16">
@@ -20146,7 +20065,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="16">
-        <f t="shared" ref="H5:H9" si="0">IF(P5&gt;10,5,IF(P5&gt;4,4,IF(P5&gt;2,3,IF(P5&gt;0,2,IF(P5&gt;-2.5,1,IF(P5&gt;-10,0,6))))))</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I5" s="16">
@@ -20171,7 +20090,7 @@
         <v>-3</v>
       </c>
       <c r="P5" s="16">
-        <f t="shared" ref="P4:P9" si="1">(S5-2000)/20+O5</f>
+        <f t="shared" ref="P5:P9" si="1">(S5-2000)/20+O5</f>
         <v>-103.05</v>
       </c>
       <c r="Q5" s="16">
@@ -20525,77 +20444,77 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="J4:P9">
-    <cfRule type="cellIs" dxfId="38" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="31" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:P8">
-    <cfRule type="cellIs" dxfId="37" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="27" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:P4">
-    <cfRule type="cellIs" dxfId="36" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="26" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="35" priority="25" operator="notEqual">
+    <cfRule type="cellIs" dxfId="75" priority="25" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:P4">
-    <cfRule type="cellIs" dxfId="34" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="24" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="33" priority="23" operator="notEqual">
+    <cfRule type="cellIs" dxfId="73" priority="23" operator="notEqual">
       <formula>$E5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:P5">
-    <cfRule type="cellIs" dxfId="32" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="22" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" dxfId="31" priority="21" operator="notEqual">
+    <cfRule type="cellIs" dxfId="71" priority="21" operator="notEqual">
       <formula>$E6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:P6">
-    <cfRule type="cellIs" dxfId="30" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="20" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="29" priority="19" operator="notEqual">
+    <cfRule type="cellIs" dxfId="69" priority="19" operator="notEqual">
       <formula>$E7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:P7">
-    <cfRule type="cellIs" dxfId="28" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="18" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="27" priority="17" operator="notEqual">
+    <cfRule type="cellIs" dxfId="67" priority="17" operator="notEqual">
       <formula>$E8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:P8">
-    <cfRule type="cellIs" dxfId="26" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="16" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="cellIs" dxfId="25" priority="15" operator="notEqual">
+    <cfRule type="cellIs" dxfId="65" priority="15" operator="notEqual">
       <formula>$E9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:P9">
-    <cfRule type="cellIs" dxfId="24" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="14" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20612,11 +20531,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -20914,7 +20833,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="16">
-        <f>IF(P4&gt;10,5,IF(P4&gt;4,4,IF(P4&gt;2,3,IF(P4&gt;0,2,IF(P4&gt;-2.5,1,IF(P4&gt;-10,0,6))))))</f>
+        <f t="shared" ref="H4:H9" si="0">IF(P4&gt;10,5,IF(P4&gt;5,4,IF(P4&gt;2.5,3,IF(P4&gt;0,2,IF(P4&gt;-2.5,1,IF(P4&gt;-10,0,6))))))</f>
         <v>5</v>
       </c>
       <c r="I4" s="16">
@@ -20939,7 +20858,7 @@
         <v>1</v>
       </c>
       <c r="P4" s="1">
-        <f t="shared" ref="P4:P9" si="0">(S4-2000)/20+O4</f>
+        <f t="shared" ref="P4:P9" si="1">(S4-2000)/20+O4</f>
         <v>16</v>
       </c>
       <c r="Q4" s="1">
@@ -20999,7 +20918,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="16">
-        <f t="shared" ref="H5:H9" si="1">IF(P5&gt;10,5,IF(P5&gt;4,4,IF(P5&gt;2,3,IF(P5&gt;0,2,IF(P5&gt;-2.5,1,IF(P5&gt;-10,0,6))))))</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I5" s="16">
@@ -21024,7 +20943,7 @@
         <v>0</v>
       </c>
       <c r="P5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-10</v>
       </c>
       <c r="Q5" s="1">
@@ -21084,7 +21003,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="I6" s="16">
@@ -21109,7 +21028,7 @@
         <v>1</v>
       </c>
       <c r="P6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="Q6" s="1">
@@ -21169,7 +21088,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I7" s="16">
@@ -21194,7 +21113,7 @@
         <v>0</v>
       </c>
       <c r="P7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q7" s="1">
@@ -21252,7 +21171,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I8" s="16">
@@ -21277,7 +21196,7 @@
         <v>1</v>
       </c>
       <c r="P8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-9</v>
       </c>
       <c r="Q8" s="1">
@@ -21337,7 +21256,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="I9" s="16">
@@ -21362,7 +21281,7 @@
         <v>1</v>
       </c>
       <c r="P9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>301</v>
       </c>
       <c r="Q9" s="1">
@@ -21402,22 +21321,22 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I4:I9">
-    <cfRule type="cellIs" dxfId="23" priority="4" operator="notEqual">
+    <cfRule type="cellIs" dxfId="34" priority="4" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:P7">
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:P9">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:P8">
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
building cannot change pos now
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="2"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="标准" sheetId="1" r:id="rId1"/>
@@ -3009,10 +3009,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>m.DragRandomUnitNear(mouse);if(MathTool.GetRandom(100)&lt;s.Rate) p.AddCard(s.Id, s.Level);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>复制一张己方场上怪物到手牌，并提升{3:0}级</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3784,6 +3780,10 @@
   </si>
   <si>
     <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse))im.OnMagicDamage(s.Damage,3);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(MathTool.GetRandom(100)&lt;s.Rate) p.AddCard(s.Id, s.Level);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -4793,393 +4793,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
         <color rgb="FF000000"/>
         <name val="宋体"/>
         <scheme val="none"/>
@@ -5219,6 +4832,33 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -5918,6 +5558,43 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -5987,6 +5664,33 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -6688,6 +6392,138 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -6757,6 +6593,33 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -7456,6 +7319,143 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -7484,6 +7484,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7632,11 +7633,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-84969248"/>
-        <c:axId val="-84960544"/>
+        <c:axId val="1761749920"/>
+        <c:axId val="1761754272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-84969248"/>
+        <c:axId val="1761749920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7679,7 +7680,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-84960544"/>
+        <c:crossAx val="1761754272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7687,7 +7688,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-84960544"/>
+        <c:axId val="1761754272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7738,7 +7739,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-84969248"/>
+        <c:crossAx val="1761749920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8366,138 +8367,132 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AB128" totalsRowShown="0" headerRowDxfId="127" dataDxfId="126" tableBorderDxfId="125">
-  <autoFilter ref="A3:AB128">
-    <filterColumn colId="19">
-      <customFilters>
-        <customFilter val="*GetRangeMonster*"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AB128" totalsRowShown="0" headerRowDxfId="110" dataDxfId="109" tableBorderDxfId="108">
+  <autoFilter ref="A3:AB128"/>
   <sortState ref="A4:Y128">
     <sortCondition ref="A3:A128"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="124"/>
-    <tableColumn id="2" name="Name" dataDxfId="123"/>
-    <tableColumn id="20" name="Ename" dataDxfId="122"/>
-    <tableColumn id="21" name="EnameShort" dataDxfId="121"/>
-    <tableColumn id="3" name="Star" dataDxfId="120"/>
-    <tableColumn id="4" name="Type" dataDxfId="119"/>
-    <tableColumn id="5" name="Attr" dataDxfId="118"/>
-    <tableColumn id="8" name="Quality" dataDxfId="117">
+    <tableColumn id="1" name="Id" dataDxfId="107"/>
+    <tableColumn id="2" name="Name" dataDxfId="106"/>
+    <tableColumn id="20" name="Ename" dataDxfId="105"/>
+    <tableColumn id="21" name="EnameShort" dataDxfId="104"/>
+    <tableColumn id="3" name="Star" dataDxfId="103"/>
+    <tableColumn id="4" name="Type" dataDxfId="102"/>
+    <tableColumn id="5" name="Attr" dataDxfId="101"/>
+    <tableColumn id="8" name="Quality" dataDxfId="100">
       <calculatedColumnFormula>IF(P4&gt;10,5,IF(P4&gt;5,4,IF(P4&gt;2.5,3,IF(P4&gt;0,2,IF(P4&gt;-2.5,1,IF(P4&gt;-10,0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="116"/>
-    <tableColumn id="9" name="Damage" dataDxfId="115"/>
-    <tableColumn id="10" name="Cure" dataDxfId="114"/>
-    <tableColumn id="11" name="Time" dataDxfId="113"/>
-    <tableColumn id="13" name="Help" dataDxfId="112"/>
-    <tableColumn id="16" name="Rate" dataDxfId="111"/>
-    <tableColumn id="12" name="Modify" dataDxfId="110"/>
-    <tableColumn id="27" name="Sum" dataDxfId="109">
+    <tableColumn id="7" name="Cost" dataDxfId="99"/>
+    <tableColumn id="9" name="Damage" dataDxfId="98"/>
+    <tableColumn id="10" name="Cure" dataDxfId="97"/>
+    <tableColumn id="11" name="Time" dataDxfId="96"/>
+    <tableColumn id="13" name="Help" dataDxfId="95"/>
+    <tableColumn id="16" name="Rate" dataDxfId="94"/>
+    <tableColumn id="12" name="Modify" dataDxfId="93"/>
+    <tableColumn id="27" name="Sum" dataDxfId="92">
       <calculatedColumnFormula>(S4-2000)/20+O4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="108"/>
-    <tableColumn id="15" name="Target" dataDxfId="107"/>
-    <tableColumn id="25" name="Mark" dataDxfId="106"/>
-    <tableColumn id="22" name="Effect" dataDxfId="105"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="104"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="103"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="38"/>
-    <tableColumn id="18" name="Res" dataDxfId="102"/>
-    <tableColumn id="19" name="Icon" dataDxfId="101"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="100"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="99"/>
-    <tableColumn id="26" name="Remark" dataDxfId="98"/>
+    <tableColumn id="6" name="Range" dataDxfId="91"/>
+    <tableColumn id="15" name="Target" dataDxfId="90"/>
+    <tableColumn id="25" name="Mark" dataDxfId="89"/>
+    <tableColumn id="22" name="Effect" dataDxfId="88"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="87"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="86"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="85"/>
+    <tableColumn id="18" name="Res" dataDxfId="84"/>
+    <tableColumn id="19" name="Icon" dataDxfId="83"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="82"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="81"/>
+    <tableColumn id="26" name="Remark" dataDxfId="80"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AB9" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96" tableBorderDxfId="95">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AB9" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63" tableBorderDxfId="62">
   <autoFilter ref="A3:AB9"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="94"/>
-    <tableColumn id="2" name="Name" dataDxfId="93"/>
-    <tableColumn id="20" name="Ename" dataDxfId="92"/>
-    <tableColumn id="21" name="EnameShort" dataDxfId="91"/>
-    <tableColumn id="3" name="Star" dataDxfId="90"/>
-    <tableColumn id="4" name="Type" dataDxfId="89"/>
-    <tableColumn id="5" name="Attr" dataDxfId="88"/>
-    <tableColumn id="8" name="Quality" dataDxfId="87">
+    <tableColumn id="1" name="Id" dataDxfId="61"/>
+    <tableColumn id="2" name="Name" dataDxfId="60"/>
+    <tableColumn id="20" name="Ename" dataDxfId="59"/>
+    <tableColumn id="21" name="EnameShort" dataDxfId="58"/>
+    <tableColumn id="3" name="Star" dataDxfId="57"/>
+    <tableColumn id="4" name="Type" dataDxfId="56"/>
+    <tableColumn id="5" name="Attr" dataDxfId="55"/>
+    <tableColumn id="8" name="Quality" dataDxfId="54">
       <calculatedColumnFormula>IF(P4&gt;10,5,IF(P4&gt;5,4,IF(P4&gt;2.5,3,IF(P4&gt;0,2,IF(P4&gt;-2.5,1,IF(P4&gt;-10,0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="86"/>
-    <tableColumn id="9" name="Damage" dataDxfId="85"/>
-    <tableColumn id="10" name="Cure" dataDxfId="84"/>
-    <tableColumn id="11" name="Time" dataDxfId="83"/>
-    <tableColumn id="13" name="Help" dataDxfId="82"/>
-    <tableColumn id="16" name="Rate" dataDxfId="81"/>
-    <tableColumn id="12" name="Modify" dataDxfId="80"/>
-    <tableColumn id="27" name="Sum" dataDxfId="79">
+    <tableColumn id="7" name="Cost" dataDxfId="53"/>
+    <tableColumn id="9" name="Damage" dataDxfId="52"/>
+    <tableColumn id="10" name="Cure" dataDxfId="51"/>
+    <tableColumn id="11" name="Time" dataDxfId="50"/>
+    <tableColumn id="13" name="Help" dataDxfId="49"/>
+    <tableColumn id="16" name="Rate" dataDxfId="48"/>
+    <tableColumn id="12" name="Modify" dataDxfId="47"/>
+    <tableColumn id="27" name="Sum" dataDxfId="46">
       <calculatedColumnFormula>(S4-2000)/20+O4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="78"/>
-    <tableColumn id="15" name="Target" dataDxfId="77"/>
-    <tableColumn id="25" name="Mark" dataDxfId="76"/>
-    <tableColumn id="22" name="Effect" dataDxfId="75"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="74"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="73"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="37"/>
-    <tableColumn id="18" name="Res" dataDxfId="72"/>
-    <tableColumn id="19" name="Icon" dataDxfId="71"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="70"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="69"/>
-    <tableColumn id="26" name="Remark" dataDxfId="68"/>
+    <tableColumn id="6" name="Range" dataDxfId="45"/>
+    <tableColumn id="15" name="Target" dataDxfId="44"/>
+    <tableColumn id="25" name="Mark" dataDxfId="43"/>
+    <tableColumn id="22" name="Effect" dataDxfId="42"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="41"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="40"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="39"/>
+    <tableColumn id="18" name="Res" dataDxfId="38"/>
+    <tableColumn id="19" name="Icon" dataDxfId="37"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="36"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="35"/>
+    <tableColumn id="26" name="Remark" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_35" displayName="表1_35" ref="A3:AB9" totalsRowShown="0" headerRowDxfId="67" tableBorderDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_35" displayName="表1_35" ref="A3:AB9" totalsRowShown="0" headerRowDxfId="29" tableBorderDxfId="28">
   <autoFilter ref="A3:AB9"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="65"/>
-    <tableColumn id="2" name="Name" dataDxfId="64"/>
-    <tableColumn id="20" name="Ename" dataDxfId="63"/>
-    <tableColumn id="21" name="EnameShort" dataDxfId="62"/>
-    <tableColumn id="3" name="Star" dataDxfId="61"/>
-    <tableColumn id="4" name="Type" dataDxfId="60"/>
-    <tableColumn id="5" name="Attr" dataDxfId="59"/>
-    <tableColumn id="8" name="Quality" dataDxfId="58">
+    <tableColumn id="1" name="Id" dataDxfId="27"/>
+    <tableColumn id="2" name="Name" dataDxfId="26"/>
+    <tableColumn id="20" name="Ename" dataDxfId="25"/>
+    <tableColumn id="21" name="EnameShort" dataDxfId="24"/>
+    <tableColumn id="3" name="Star" dataDxfId="23"/>
+    <tableColumn id="4" name="Type" dataDxfId="22"/>
+    <tableColumn id="5" name="Attr" dataDxfId="21"/>
+    <tableColumn id="8" name="Quality" dataDxfId="20">
       <calculatedColumnFormula>IF(P4&gt;10,5,IF(P4&gt;5,4,IF(P4&gt;2.5,3,IF(P4&gt;0,2,IF(P4&gt;-2.5,1,IF(P4&gt;-10,0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="57"/>
-    <tableColumn id="9" name="Damage" dataDxfId="56"/>
-    <tableColumn id="10" name="Cure" dataDxfId="55"/>
-    <tableColumn id="11" name="Time" dataDxfId="54"/>
-    <tableColumn id="13" name="Help" dataDxfId="53"/>
-    <tableColumn id="16" name="Rate" dataDxfId="52"/>
-    <tableColumn id="12" name="Modify" dataDxfId="51"/>
-    <tableColumn id="27" name="Sum" dataDxfId="50">
+    <tableColumn id="7" name="Cost" dataDxfId="19"/>
+    <tableColumn id="9" name="Damage" dataDxfId="18"/>
+    <tableColumn id="10" name="Cure" dataDxfId="17"/>
+    <tableColumn id="11" name="Time" dataDxfId="16"/>
+    <tableColumn id="13" name="Help" dataDxfId="15"/>
+    <tableColumn id="16" name="Rate" dataDxfId="14"/>
+    <tableColumn id="12" name="Modify" dataDxfId="13"/>
+    <tableColumn id="27" name="Sum" dataDxfId="12">
       <calculatedColumnFormula>(S4-2000)/20+O4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="49"/>
-    <tableColumn id="15" name="Target" dataDxfId="48"/>
-    <tableColumn id="25" name="Mark" dataDxfId="47"/>
-    <tableColumn id="22" name="Effect" dataDxfId="46"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="45"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="44"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="0"/>
-    <tableColumn id="18" name="Res" dataDxfId="43"/>
-    <tableColumn id="19" name="Icon" dataDxfId="42"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="41"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="40"/>
-    <tableColumn id="26" name="Remark" dataDxfId="39"/>
+    <tableColumn id="6" name="Range" dataDxfId="11"/>
+    <tableColumn id="15" name="Target" dataDxfId="10"/>
+    <tableColumn id="25" name="Mark" dataDxfId="9"/>
+    <tableColumn id="22" name="Effect" dataDxfId="8"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="7"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="6"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="5"/>
+    <tableColumn id="18" name="Res" dataDxfId="4"/>
+    <tableColumn id="19" name="Icon" dataDxfId="3"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="2"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="1"/>
+    <tableColumn id="26" name="Remark" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8792,11 +8787,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB128"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="T126" sqref="T126"/>
+      <selection pane="bottomRight" activeCell="T36" sqref="T36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -8843,7 +8838,7 @@
         <v>214</v>
       </c>
       <c r="H1" s="40" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>490</v>
@@ -8867,7 +8862,7 @@
         <v>504</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="Q1" s="14" t="s">
         <v>487</v>
@@ -8888,7 +8883,7 @@
         <v>656</v>
       </c>
       <c r="W1" s="14" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="X1" s="14" t="s">
         <v>215</v>
@@ -8903,7 +8898,7 @@
         <v>625</v>
       </c>
       <c r="AB1" s="36" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="2" spans="1:28">
@@ -8953,7 +8948,7 @@
         <v>505</v>
       </c>
       <c r="P2" s="19" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>488</v>
@@ -8965,7 +8960,7 @@
         <v>658</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="U2" s="11" t="s">
         <v>201</v>
@@ -8974,7 +8969,7 @@
         <v>201</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="X2" s="4" t="s">
         <v>200</v>
@@ -9015,7 +9010,7 @@
         <v>206</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>492</v>
@@ -9039,19 +9034,19 @@
         <v>506</v>
       </c>
       <c r="P3" s="42" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>489</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>659</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="U3" s="6" t="s">
         <v>470</v>
@@ -9060,7 +9055,7 @@
         <v>494</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="X3" s="2" t="s">
         <v>208</v>
@@ -9075,10 +9070,10 @@
         <v>626</v>
       </c>
       <c r="AB3" s="28" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="36" hidden="1">
+    <row r="4" spans="1:28" ht="36">
       <c r="A4">
         <v>53000001</v>
       </c>
@@ -9139,7 +9134,7 @@
         <v>1704</v>
       </c>
       <c r="T4" s="12" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="U4" s="33" t="s">
         <v>581</v>
@@ -9161,10 +9156,10 @@
         <v>0</v>
       </c>
       <c r="AB4" s="27" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="14.25" hidden="1">
+    <row r="5" spans="1:28" ht="14.25">
       <c r="A5">
         <v>53000002</v>
       </c>
@@ -9225,7 +9220,7 @@
         <v>1550</v>
       </c>
       <c r="T5" s="12" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="U5" s="7" t="s">
         <v>547</v>
@@ -9247,10 +9242,10 @@
         <v>0</v>
       </c>
       <c r="AB5" s="27" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="24" hidden="1">
+    <row r="6" spans="1:28" ht="24">
       <c r="A6">
         <v>53000003</v>
       </c>
@@ -9311,7 +9306,7 @@
         <v>2000</v>
       </c>
       <c r="T6" s="12" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="U6" s="7" t="s">
         <v>654</v>
@@ -9333,10 +9328,10 @@
         <v>0</v>
       </c>
       <c r="AB6" s="27" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="36" hidden="1">
+    <row r="7" spans="1:28" ht="36">
       <c r="A7">
         <v>53000004</v>
       </c>
@@ -9397,7 +9392,7 @@
         <v>2000</v>
       </c>
       <c r="T7" s="12" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="U7" s="7" t="s">
         <v>655</v>
@@ -9419,10 +9414,10 @@
         <v>0</v>
       </c>
       <c r="AB7" s="27" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="24" hidden="1">
+    <row r="8" spans="1:28" ht="24">
       <c r="A8">
         <v>53000005</v>
       </c>
@@ -9483,7 +9478,7 @@
         <v>900</v>
       </c>
       <c r="T8" s="12" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="U8" s="7" t="s">
         <v>546</v>
@@ -9505,10 +9500,10 @@
         <v>0</v>
       </c>
       <c r="AB8" s="27" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="48" hidden="1">
+    <row r="9" spans="1:28" ht="48">
       <c r="A9">
         <v>53000006</v>
       </c>
@@ -9563,7 +9558,7 @@
         <v>0</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="S9" s="1">
         <v>500</v>
@@ -9591,10 +9586,10 @@
         <v>0</v>
       </c>
       <c r="AB9" s="27" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="48" hidden="1">
+    <row r="10" spans="1:28" ht="48">
       <c r="A10">
         <v>53000007</v>
       </c>
@@ -9649,7 +9644,7 @@
         <v>0</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="S10" s="1">
         <v>500</v>
@@ -9677,10 +9672,10 @@
         <v>0</v>
       </c>
       <c r="AB10" s="27" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="48" hidden="1">
+    <row r="11" spans="1:28" ht="48">
       <c r="A11">
         <v>53000008</v>
       </c>
@@ -9735,7 +9730,7 @@
         <v>0</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="S11" s="1">
         <v>500</v>
@@ -9763,10 +9758,10 @@
         <v>0</v>
       </c>
       <c r="AB11" s="27" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="48" hidden="1">
+    <row r="12" spans="1:28" ht="48">
       <c r="A12">
         <v>53000009</v>
       </c>
@@ -9821,7 +9816,7 @@
         <v>0</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="S12" s="1">
         <v>500</v>
@@ -9849,10 +9844,10 @@
         <v>0</v>
       </c>
       <c r="AB12" s="27" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="48" hidden="1">
+    <row r="13" spans="1:28" ht="48">
       <c r="A13">
         <v>53000010</v>
       </c>
@@ -9907,7 +9902,7 @@
         <v>0</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="S13" s="1">
         <v>500</v>
@@ -9935,10 +9930,10 @@
         <v>0</v>
       </c>
       <c r="AB13" s="27" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="48" hidden="1">
+    <row r="14" spans="1:28" ht="48">
       <c r="A14">
         <v>53000011</v>
       </c>
@@ -9993,7 +9988,7 @@
         <v>0</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="S14" s="1">
         <v>500</v>
@@ -10021,10 +10016,10 @@
         <v>0</v>
       </c>
       <c r="AB14" s="27" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="48" hidden="1">
+    <row r="15" spans="1:28" ht="48">
       <c r="A15">
         <v>53000012</v>
       </c>
@@ -10079,7 +10074,7 @@
         <v>0</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="S15" s="1">
         <v>500</v>
@@ -10107,10 +10102,10 @@
         <v>0</v>
       </c>
       <c r="AB15" s="27" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="48" hidden="1">
+    <row r="16" spans="1:28" ht="48">
       <c r="A16">
         <v>53000013</v>
       </c>
@@ -10165,7 +10160,7 @@
         <v>0</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="S16" s="1">
         <v>500</v>
@@ -10193,10 +10188,10 @@
         <v>0</v>
       </c>
       <c r="AB16" s="27" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="48" hidden="1">
+    <row r="17" spans="1:28" ht="48">
       <c r="A17">
         <v>53000014</v>
       </c>
@@ -10251,7 +10246,7 @@
         <v>0</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="S17" s="1">
         <v>500</v>
@@ -10279,10 +10274,10 @@
         <v>0</v>
       </c>
       <c r="AB17" s="27" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="14.25" hidden="1">
+    <row r="18" spans="1:28" ht="14.25">
       <c r="A18">
         <v>53000015</v>
       </c>
@@ -10365,10 +10360,10 @@
         <v>0</v>
       </c>
       <c r="AB18" s="27" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="24" hidden="1">
+    <row r="19" spans="1:28" ht="24">
       <c r="A19">
         <v>53000016</v>
       </c>
@@ -10429,7 +10424,7 @@
         <v>1200</v>
       </c>
       <c r="T19" s="12" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="U19" s="7" t="s">
         <v>508</v>
@@ -10451,10 +10446,10 @@
         <v>0</v>
       </c>
       <c r="AB19" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="24" hidden="1">
+    <row r="20" spans="1:28" ht="24">
       <c r="A20">
         <v>53000017</v>
       </c>
@@ -10515,7 +10510,7 @@
         <v>8000</v>
       </c>
       <c r="T20" s="12" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="U20" s="7" t="s">
         <v>509</v>
@@ -10537,10 +10532,10 @@
         <v>0</v>
       </c>
       <c r="AB20" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="48" hidden="1">
+    <row r="21" spans="1:28" ht="48">
       <c r="A21">
         <v>53000018</v>
       </c>
@@ -10623,7 +10618,7 @@
         <v>0</v>
       </c>
       <c r="AB21" s="27" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="22" spans="1:28" ht="60">
@@ -10687,7 +10682,7 @@
         <v>1800</v>
       </c>
       <c r="T22" s="12" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="U22" s="7" t="s">
         <v>666</v>
@@ -10711,7 +10706,7 @@
         <v>0</v>
       </c>
       <c r="AB22" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="23" spans="1:28" ht="60">
@@ -10775,7 +10770,7 @@
         <v>2100</v>
       </c>
       <c r="T23" s="12" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="U23" s="7" t="s">
         <v>667</v>
@@ -10799,7 +10794,7 @@
         <v>0</v>
       </c>
       <c r="AB23" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="24" spans="1:28" ht="60">
@@ -10863,7 +10858,7 @@
         <v>1875</v>
       </c>
       <c r="T24" s="12" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="U24" s="7" t="s">
         <v>668</v>
@@ -10887,10 +10882,10 @@
         <v>0</v>
       </c>
       <c r="AB24" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="24" hidden="1">
+    <row r="25" spans="1:28" ht="24">
       <c r="A25">
         <v>53000022</v>
       </c>
@@ -10973,10 +10968,10 @@
         <v>0</v>
       </c>
       <c r="AB25" s="27" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="24" hidden="1">
+    <row r="26" spans="1:28" ht="24">
       <c r="A26">
         <v>53000023</v>
       </c>
@@ -11059,10 +11054,10 @@
         <v>0</v>
       </c>
       <c r="AB26" s="27" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="24" hidden="1">
+    <row r="27" spans="1:28" ht="24">
       <c r="A27">
         <v>53000024</v>
       </c>
@@ -11145,10 +11140,10 @@
         <v>0</v>
       </c>
       <c r="AB27" s="27" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="48" hidden="1">
+    <row r="28" spans="1:28" ht="48">
       <c r="A28">
         <v>53000025</v>
       </c>
@@ -11231,10 +11226,10 @@
         <v>0</v>
       </c>
       <c r="AB28" s="27" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="24" hidden="1">
+    <row r="29" spans="1:28" ht="24">
       <c r="A29">
         <v>53000026</v>
       </c>
@@ -11317,10 +11312,10 @@
         <v>0</v>
       </c>
       <c r="AB29" s="27" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="14.25" hidden="1">
+    <row r="30" spans="1:28" ht="14.25">
       <c r="A30">
         <v>53000027</v>
       </c>
@@ -11382,7 +11377,7 @@
       </c>
       <c r="T30" s="12"/>
       <c r="U30" s="7" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="V30" s="1" t="s">
         <v>46</v>
@@ -11401,10 +11396,10 @@
         <v>0</v>
       </c>
       <c r="AB30" s="27" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
-    <row r="31" spans="1:28" ht="14.25" hidden="1">
+    <row r="31" spans="1:28" ht="14.25">
       <c r="A31">
         <v>53000028</v>
       </c>
@@ -11466,7 +11461,7 @@
       </c>
       <c r="T31" s="12"/>
       <c r="U31" s="7" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="V31" s="1" t="s">
         <v>48</v>
@@ -11485,10 +11480,10 @@
         <v>0</v>
       </c>
       <c r="AB31" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
-    <row r="32" spans="1:28" ht="24" hidden="1">
+    <row r="32" spans="1:28" ht="24">
       <c r="A32">
         <v>53000029</v>
       </c>
@@ -11571,21 +11566,21 @@
         <v>0</v>
       </c>
       <c r="AB32" s="27" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
-    <row r="33" spans="1:28" ht="24" hidden="1">
+    <row r="33" spans="1:28" ht="24">
       <c r="A33">
         <v>53000030</v>
       </c>
       <c r="B33" s="9" t="s">
+        <v>775</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>776</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>777</v>
-      </c>
       <c r="D33" s="8" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="E33" s="1">
         <v>2</v>
@@ -11635,10 +11630,10 @@
         <v>1500</v>
       </c>
       <c r="T33" s="12" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="U33" s="1" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="V33" s="1" t="s">
         <v>4</v>
@@ -11657,21 +11652,21 @@
         <v>1</v>
       </c>
       <c r="AB33" s="27" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
-    <row r="34" spans="1:28" ht="24" hidden="1">
+    <row r="34" spans="1:28" ht="24">
       <c r="A34">
         <v>53000031</v>
       </c>
       <c r="B34" s="9" t="s">
+        <v>778</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>779</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>780</v>
-      </c>
       <c r="D34" s="8" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="E34" s="1">
         <v>2</v>
@@ -11721,10 +11716,10 @@
         <v>1500</v>
       </c>
       <c r="T34" s="12" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="U34" s="1" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="V34" s="1" t="s">
         <v>4</v>
@@ -11743,10 +11738,10 @@
         <v>1</v>
       </c>
       <c r="AB34" s="27" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
-    <row r="35" spans="1:28" ht="48" hidden="1">
+    <row r="35" spans="1:28" ht="48">
       <c r="A35">
         <v>53000035</v>
       </c>
@@ -11807,7 +11802,7 @@
         <v>2000</v>
       </c>
       <c r="T35" s="12" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="U35" s="7" t="s">
         <v>513</v>
@@ -11829,10 +11824,10 @@
         <v>0</v>
       </c>
       <c r="AB35" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
-    <row r="36" spans="1:28" ht="48" hidden="1">
+    <row r="36" spans="1:28" ht="36">
       <c r="A36">
         <v>53000036</v>
       </c>
@@ -11894,7 +11889,7 @@
         <v>1220</v>
       </c>
       <c r="T36" s="12" t="s">
-        <v>683</v>
+        <v>881</v>
       </c>
       <c r="U36" s="1" t="s">
         <v>679</v>
@@ -11916,10 +11911,10 @@
         <v>0</v>
       </c>
       <c r="AB36" s="27" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
-    <row r="37" spans="1:28" ht="14.25" hidden="1">
+    <row r="37" spans="1:28" ht="14.25">
       <c r="A37">
         <v>53000037</v>
       </c>
@@ -12000,10 +11995,10 @@
         <v>0</v>
       </c>
       <c r="AB37" s="27" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
-    <row r="38" spans="1:28" ht="14.25" hidden="1">
+    <row r="38" spans="1:28" ht="14.25">
       <c r="A38">
         <v>53000038</v>
       </c>
@@ -12065,7 +12060,7 @@
       </c>
       <c r="T38" s="12"/>
       <c r="U38" s="7" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="V38" s="1" t="s">
         <v>63</v>
@@ -12084,18 +12079,18 @@
         <v>0</v>
       </c>
       <c r="AB38" s="27" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
-    <row r="39" spans="1:28" ht="24" hidden="1">
+    <row r="39" spans="1:28" ht="24">
       <c r="A39">
         <v>53000039</v>
       </c>
       <c r="B39" s="9" t="s">
+        <v>769</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>770</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>771</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>374</v>
@@ -12148,10 +12143,10 @@
         <v>1700</v>
       </c>
       <c r="T39" s="12" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="U39" s="1" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="V39" s="1" t="s">
         <v>4</v>
@@ -12170,15 +12165,15 @@
         <v>0</v>
       </c>
       <c r="AB39" s="27" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
-    <row r="40" spans="1:28" ht="24" hidden="1">
+    <row r="40" spans="1:28" ht="24">
       <c r="A40">
         <v>53000040</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>270</v>
@@ -12234,10 +12229,10 @@
         <v>2000</v>
       </c>
       <c r="T40" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="U40" s="1" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="V40" s="1" t="s">
         <v>4</v>
@@ -12256,10 +12251,10 @@
         <v>0</v>
       </c>
       <c r="AB40" s="27" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
-    <row r="41" spans="1:28" ht="24" hidden="1">
+    <row r="41" spans="1:28" ht="24">
       <c r="A41">
         <v>53000041</v>
       </c>
@@ -12323,7 +12318,7 @@
         <v>577</v>
       </c>
       <c r="U41" s="7" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="V41" s="1" t="s">
         <v>65</v>
@@ -12342,10 +12337,10 @@
         <v>0</v>
       </c>
       <c r="AB41" s="27" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
-    <row r="42" spans="1:28" ht="48" hidden="1">
+    <row r="42" spans="1:28" ht="48">
       <c r="A42">
         <v>53000042</v>
       </c>
@@ -12406,7 +12401,7 @@
         <v>2000</v>
       </c>
       <c r="T42" s="12" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="U42" s="1" t="s">
         <v>514</v>
@@ -12428,10 +12423,10 @@
         <v>0</v>
       </c>
       <c r="AB42" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
-    <row r="43" spans="1:28" ht="24" hidden="1">
+    <row r="43" spans="1:28" ht="24">
       <c r="A43">
         <v>53000043</v>
       </c>
@@ -12492,7 +12487,7 @@
         <v>2000</v>
       </c>
       <c r="T43" s="12" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="U43" s="1" t="s">
         <v>572</v>
@@ -12514,15 +12509,15 @@
         <v>0</v>
       </c>
       <c r="AB43" s="27" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
-    <row r="44" spans="1:28" ht="24" hidden="1">
+    <row r="44" spans="1:28" ht="24">
       <c r="A44">
         <v>53000044</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>274</v>
@@ -12578,10 +12573,10 @@
         <v>1900</v>
       </c>
       <c r="T44" s="12" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="U44" s="1" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="V44" s="1" t="s">
         <v>4</v>
@@ -12600,10 +12595,10 @@
         <v>0</v>
       </c>
       <c r="AB44" s="27" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
-    <row r="45" spans="1:28" ht="60" hidden="1">
+    <row r="45" spans="1:28" ht="60">
       <c r="A45">
         <v>53000045</v>
       </c>
@@ -12687,10 +12682,10 @@
         <v>0</v>
       </c>
       <c r="AB45" s="27" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
-    <row r="46" spans="1:28" ht="48" hidden="1">
+    <row r="46" spans="1:28" ht="48">
       <c r="A46">
         <v>53000046</v>
       </c>
@@ -12751,7 +12746,7 @@
         <v>2000</v>
       </c>
       <c r="T46" s="12" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="U46" s="7" t="s">
         <v>528</v>
@@ -12773,7 +12768,7 @@
         <v>0</v>
       </c>
       <c r="AB46" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="47" spans="1:28" ht="60">
@@ -12837,7 +12832,7 @@
         <v>2200</v>
       </c>
       <c r="T47" s="12" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="U47" s="7" t="s">
         <v>529</v>
@@ -12861,10 +12856,10 @@
         <v>0</v>
       </c>
       <c r="AB47" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
-    <row r="48" spans="1:28" ht="48" hidden="1">
+    <row r="48" spans="1:28" ht="48">
       <c r="A48">
         <v>53000048</v>
       </c>
@@ -12925,7 +12920,7 @@
         <v>2000</v>
       </c>
       <c r="T48" s="12" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="U48" s="1" t="s">
         <v>515</v>
@@ -12947,7 +12942,7 @@
         <v>0</v>
       </c>
       <c r="AB48" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="49" spans="1:28" ht="60">
@@ -13011,7 +13006,7 @@
         <v>2200</v>
       </c>
       <c r="T49" s="12" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="U49" s="7" t="s">
         <v>530</v>
@@ -13035,10 +13030,10 @@
         <v>0</v>
       </c>
       <c r="AB49" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
-    <row r="50" spans="1:28" ht="72" hidden="1">
+    <row r="50" spans="1:28" ht="72">
       <c r="A50">
         <v>53000050</v>
       </c>
@@ -13093,16 +13088,16 @@
         <v>0</v>
       </c>
       <c r="R50" s="7" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="S50" s="1">
         <v>1800</v>
       </c>
       <c r="T50" s="12" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="U50" s="7" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="V50" s="1" t="s">
         <v>78</v>
@@ -13121,10 +13116,10 @@
         <v>0</v>
       </c>
       <c r="AB50" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
-    <row r="51" spans="1:28" ht="48" hidden="1">
+    <row r="51" spans="1:28" ht="48">
       <c r="A51">
         <v>53000051</v>
       </c>
@@ -13185,7 +13180,7 @@
         <v>2000</v>
       </c>
       <c r="T51" s="12" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="U51" s="1" t="s">
         <v>516</v>
@@ -13207,10 +13202,10 @@
         <v>0</v>
       </c>
       <c r="AB51" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
-    <row r="52" spans="1:28" ht="48" hidden="1">
+    <row r="52" spans="1:28" ht="48">
       <c r="A52">
         <v>53000052</v>
       </c>
@@ -13271,7 +13266,7 @@
         <v>2000</v>
       </c>
       <c r="T52" s="12" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="U52" s="1" t="s">
         <v>517</v>
@@ -13293,10 +13288,10 @@
         <v>0</v>
       </c>
       <c r="AB52" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
-    <row r="53" spans="1:28" ht="48" hidden="1">
+    <row r="53" spans="1:28" ht="48">
       <c r="A53">
         <v>53000053</v>
       </c>
@@ -13357,7 +13352,7 @@
         <v>2000</v>
       </c>
       <c r="T53" s="12" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="U53" s="1" t="s">
         <v>518</v>
@@ -13379,10 +13374,10 @@
         <v>0</v>
       </c>
       <c r="AB53" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
-    <row r="54" spans="1:28" ht="48" hidden="1">
+    <row r="54" spans="1:28" ht="48">
       <c r="A54">
         <v>53000054</v>
       </c>
@@ -13443,7 +13438,7 @@
         <v>1670</v>
       </c>
       <c r="T54" s="12" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="U54" s="7" t="s">
         <v>619</v>
@@ -13465,10 +13460,10 @@
         <v>0</v>
       </c>
       <c r="AB54" s="27" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
-    <row r="55" spans="1:28" ht="24" hidden="1">
+    <row r="55" spans="1:28" ht="24">
       <c r="A55">
         <v>53000055</v>
       </c>
@@ -13529,10 +13524,10 @@
         <v>3000</v>
       </c>
       <c r="T55" s="12" t="s">
+        <v>704</v>
+      </c>
+      <c r="U55" s="1" t="s">
         <v>705</v>
-      </c>
-      <c r="U55" s="1" t="s">
-        <v>706</v>
       </c>
       <c r="V55" s="1" t="s">
         <v>2</v>
@@ -13551,10 +13546,10 @@
         <v>0</v>
       </c>
       <c r="AB55" s="27" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
-    <row r="56" spans="1:28" ht="36" hidden="1">
+    <row r="56" spans="1:28" ht="36">
       <c r="A56">
         <v>53000056</v>
       </c>
@@ -13615,7 +13610,7 @@
         <v>750</v>
       </c>
       <c r="T56" s="12" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="U56" s="1" t="s">
         <v>562</v>
@@ -13637,10 +13632,10 @@
         <v>0</v>
       </c>
       <c r="AB56" s="27" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
-    <row r="57" spans="1:28" ht="24" hidden="1">
+    <row r="57" spans="1:28" ht="24">
       <c r="A57">
         <v>53000057</v>
       </c>
@@ -13695,16 +13690,16 @@
         <v>3</v>
       </c>
       <c r="R57" s="1" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="S57" s="39">
         <v>1500</v>
       </c>
       <c r="T57" s="12" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="U57" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="V57" s="1" t="s">
         <v>2</v>
@@ -13723,10 +13718,10 @@
         <v>0</v>
       </c>
       <c r="AB57" s="27" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
-    <row r="58" spans="1:28" ht="24" hidden="1">
+    <row r="58" spans="1:28" ht="24">
       <c r="A58">
         <v>53000058</v>
       </c>
@@ -13787,7 +13782,7 @@
         <v>1800</v>
       </c>
       <c r="T58" s="12" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="U58" s="7" t="s">
         <v>519</v>
@@ -13809,10 +13804,10 @@
         <v>0</v>
       </c>
       <c r="AB58" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
-    <row r="59" spans="1:28" ht="24" hidden="1">
+    <row r="59" spans="1:28" ht="24">
       <c r="A59">
         <v>53000059</v>
       </c>
@@ -13873,7 +13868,7 @@
         <v>560</v>
       </c>
       <c r="T59" s="12" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="U59" s="7" t="s">
         <v>579</v>
@@ -13895,10 +13890,10 @@
         <v>0</v>
       </c>
       <c r="AB59" s="27" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
-    <row r="60" spans="1:28" ht="36" hidden="1">
+    <row r="60" spans="1:28" ht="36">
       <c r="A60">
         <v>53000060</v>
       </c>
@@ -13981,10 +13976,10 @@
         <v>0</v>
       </c>
       <c r="AB60" s="27" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
-    <row r="61" spans="1:28" ht="48" hidden="1">
+    <row r="61" spans="1:28" ht="48">
       <c r="A61">
         <v>53000061</v>
       </c>
@@ -14045,7 +14040,7 @@
         <v>3000</v>
       </c>
       <c r="T61" s="12" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="U61" s="7" t="s">
         <v>570</v>
@@ -14067,10 +14062,10 @@
         <v>0</v>
       </c>
       <c r="AB61" s="27" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
-    <row r="62" spans="1:28" ht="24" hidden="1">
+    <row r="62" spans="1:28" ht="24">
       <c r="A62">
         <v>53000062</v>
       </c>
@@ -14131,7 +14126,7 @@
         <v>3000</v>
       </c>
       <c r="T62" s="12" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="U62" s="7" t="s">
         <v>520</v>
@@ -14153,10 +14148,10 @@
         <v>0</v>
       </c>
       <c r="AB62" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
-    <row r="63" spans="1:28" ht="14.25" hidden="1">
+    <row r="63" spans="1:28" ht="14.25">
       <c r="A63">
         <v>53000063</v>
       </c>
@@ -14217,7 +14212,7 @@
         <v>1500</v>
       </c>
       <c r="T63" s="12" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="U63" s="7" t="s">
         <v>571</v>
@@ -14239,10 +14234,10 @@
         <v>0</v>
       </c>
       <c r="AB63" s="27" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
-    <row r="64" spans="1:28" ht="24" hidden="1">
+    <row r="64" spans="1:28" ht="24">
       <c r="A64">
         <v>53000064</v>
       </c>
@@ -14303,10 +14298,10 @@
         <v>1500</v>
       </c>
       <c r="T64" s="12" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="U64" s="1" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="V64" s="1" t="s">
         <v>103</v>
@@ -14325,10 +14320,10 @@
         <v>0</v>
       </c>
       <c r="AB64" s="27" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
-    <row r="65" spans="1:28" ht="48" hidden="1">
+    <row r="65" spans="1:28" ht="48">
       <c r="A65">
         <v>53000065</v>
       </c>
@@ -14389,10 +14384,10 @@
         <v>5000</v>
       </c>
       <c r="T65" s="12" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="U65" s="1" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="V65" s="1" t="s">
         <v>104</v>
@@ -14411,10 +14406,10 @@
         <v>0</v>
       </c>
       <c r="AB65" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
-    <row r="66" spans="1:28" ht="24" hidden="1">
+    <row r="66" spans="1:28" ht="24">
       <c r="A66">
         <v>53000066</v>
       </c>
@@ -14475,10 +14470,10 @@
         <v>1700</v>
       </c>
       <c r="T66" s="12" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="U66" s="1" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="V66" s="1" t="s">
         <v>4</v>
@@ -14497,10 +14492,10 @@
         <v>0</v>
       </c>
       <c r="AB66" s="27" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
-    <row r="67" spans="1:28" ht="14.25" hidden="1">
+    <row r="67" spans="1:28" ht="14.25">
       <c r="A67">
         <v>53000067</v>
       </c>
@@ -14561,10 +14556,10 @@
         <v>1800</v>
       </c>
       <c r="T67" s="12" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="U67" s="7" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="V67" s="1" t="s">
         <v>106</v>
@@ -14583,7 +14578,7 @@
         <v>0</v>
       </c>
       <c r="AB67" s="27" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="68" spans="1:28" ht="60">
@@ -14647,10 +14642,10 @@
         <v>1200</v>
       </c>
       <c r="T68" s="12" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="U68" s="7" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="V68" s="1" t="s">
         <v>108</v>
@@ -14671,10 +14666,10 @@
         <v>0</v>
       </c>
       <c r="AB68" s="27" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
-    <row r="69" spans="1:28" ht="24" hidden="1">
+    <row r="69" spans="1:28" ht="24">
       <c r="A69">
         <v>53000069</v>
       </c>
@@ -14735,7 +14730,7 @@
         <v>2000</v>
       </c>
       <c r="T69" s="12" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="U69" s="7" t="s">
         <v>521</v>
@@ -14757,10 +14752,10 @@
         <v>0</v>
       </c>
       <c r="AB69" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
-    <row r="70" spans="1:28" ht="14.25" hidden="1">
+    <row r="70" spans="1:28" ht="14.25">
       <c r="A70">
         <v>53000070</v>
       </c>
@@ -14841,7 +14836,7 @@
         <v>0</v>
       </c>
       <c r="AB70" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="71" spans="1:28" ht="72">
@@ -14905,7 +14900,7 @@
         <v>2000</v>
       </c>
       <c r="T71" s="12" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="U71" s="7" t="s">
         <v>483</v>
@@ -14929,10 +14924,10 @@
         <v>0</v>
       </c>
       <c r="AB71" s="27" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
-    <row r="72" spans="1:28" ht="48" hidden="1">
+    <row r="72" spans="1:28" ht="48">
       <c r="A72">
         <v>53000072</v>
       </c>
@@ -14993,7 +14988,7 @@
         <v>4000</v>
       </c>
       <c r="T72" s="12" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="U72" s="1" t="s">
         <v>649</v>
@@ -15015,10 +15010,10 @@
         <v>0</v>
       </c>
       <c r="AB72" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
-    <row r="73" spans="1:28" ht="48" hidden="1">
+    <row r="73" spans="1:28" ht="48">
       <c r="A73">
         <v>53000073</v>
       </c>
@@ -15079,7 +15074,7 @@
         <v>1900</v>
       </c>
       <c r="T73" s="12" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="U73" s="7" t="s">
         <v>522</v>
@@ -15101,10 +15096,10 @@
         <v>0</v>
       </c>
       <c r="AB73" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
-    <row r="74" spans="1:28" ht="36" hidden="1">
+    <row r="74" spans="1:28" ht="36">
       <c r="A74">
         <v>53000074</v>
       </c>
@@ -15187,10 +15182,10 @@
         <v>0</v>
       </c>
       <c r="AB74" s="27" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
-    <row r="75" spans="1:28" ht="108" hidden="1">
+    <row r="75" spans="1:28" ht="108">
       <c r="A75">
         <v>53000075</v>
       </c>
@@ -15251,7 +15246,7 @@
         <v>3600</v>
       </c>
       <c r="T75" s="12" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="U75" s="7" t="s">
         <v>523</v>
@@ -15273,7 +15268,7 @@
         <v>0</v>
       </c>
       <c r="AB75" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="76" spans="1:28" ht="60">
@@ -15337,10 +15332,10 @@
         <v>2200</v>
       </c>
       <c r="T76" s="12" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="U76" s="7" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="V76" s="1" t="s">
         <v>124</v>
@@ -15361,10 +15356,10 @@
         <v>0</v>
       </c>
       <c r="AB76" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
-    <row r="77" spans="1:28" ht="48" hidden="1">
+    <row r="77" spans="1:28" ht="48">
       <c r="A77">
         <v>53000077</v>
       </c>
@@ -15425,7 +15420,7 @@
         <v>1200</v>
       </c>
       <c r="T77" s="12" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="U77" s="7" t="s">
         <v>524</v>
@@ -15447,10 +15442,10 @@
         <v>0</v>
       </c>
       <c r="AB77" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
-    <row r="78" spans="1:28" ht="14.25" hidden="1">
+    <row r="78" spans="1:28" ht="14.25">
       <c r="A78">
         <v>53000078</v>
       </c>
@@ -15511,10 +15506,10 @@
         <v>1000</v>
       </c>
       <c r="T78" s="7" t="s">
+        <v>715</v>
+      </c>
+      <c r="U78" s="7" t="s">
         <v>716</v>
-      </c>
-      <c r="U78" s="7" t="s">
-        <v>717</v>
       </c>
       <c r="V78" s="1" t="s">
         <v>104</v>
@@ -15533,7 +15528,7 @@
         <v>0</v>
       </c>
       <c r="AB78" s="27" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="79" spans="1:28" ht="48">
@@ -15597,10 +15592,10 @@
         <v>2400</v>
       </c>
       <c r="T79" s="12" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="U79" s="7" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="V79" s="1" t="s">
         <v>128</v>
@@ -15621,7 +15616,7 @@
         <v>0</v>
       </c>
       <c r="AB79" s="27" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="80" spans="1:28" ht="60">
@@ -15685,7 +15680,7 @@
         <v>2000</v>
       </c>
       <c r="T80" s="12" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="U80" s="7" t="s">
         <v>525</v>
@@ -15709,7 +15704,7 @@
         <v>0</v>
       </c>
       <c r="AB80" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="81" spans="1:28" ht="60">
@@ -15773,7 +15768,7 @@
         <v>1800</v>
       </c>
       <c r="T81" s="12" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="U81" s="7" t="s">
         <v>531</v>
@@ -15797,10 +15792,10 @@
         <v>0</v>
       </c>
       <c r="AB81" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
-    <row r="82" spans="1:28" ht="24" hidden="1">
+    <row r="82" spans="1:28" ht="24">
       <c r="A82">
         <v>53000082</v>
       </c>
@@ -15861,10 +15856,10 @@
         <v>2400</v>
       </c>
       <c r="T82" s="12" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="U82" s="7" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="V82" s="1" t="s">
         <v>133</v>
@@ -15883,15 +15878,15 @@
         <v>0</v>
       </c>
       <c r="AB82" s="27" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
-    <row r="83" spans="1:28" ht="24" hidden="1">
+    <row r="83" spans="1:28" ht="24">
       <c r="A83" s="44">
         <v>53000083</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>306</v>
@@ -15947,13 +15942,13 @@
         <v>1200</v>
       </c>
       <c r="T83" s="12" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="U83" s="7" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="V83" s="1" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="W83" s="1"/>
       <c r="X83" s="1">
@@ -15969,10 +15964,10 @@
         <v>0</v>
       </c>
       <c r="AB83" s="27" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
-    <row r="84" spans="1:28" ht="24" hidden="1">
+    <row r="84" spans="1:28" ht="24">
       <c r="A84">
         <v>53000084</v>
       </c>
@@ -16033,13 +16028,13 @@
         <v>800</v>
       </c>
       <c r="T84" s="12" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="U84" s="7" t="s">
         <v>566</v>
       </c>
       <c r="V84" s="1" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="W84" s="1"/>
       <c r="X84" s="1">
@@ -16055,7 +16050,7 @@
         <v>0</v>
       </c>
       <c r="AB84" s="27" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="85" spans="1:28" ht="60">
@@ -16119,7 +16114,7 @@
         <v>2000</v>
       </c>
       <c r="T85" s="12" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="U85" s="7" t="s">
         <v>532</v>
@@ -16143,10 +16138,10 @@
         <v>0</v>
       </c>
       <c r="AB85" s="27" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
-    <row r="86" spans="1:28" ht="14.25" hidden="1">
+    <row r="86" spans="1:28" ht="14.25">
       <c r="A86">
         <v>53000086</v>
       </c>
@@ -16208,7 +16203,7 @@
       </c>
       <c r="T86" s="12"/>
       <c r="U86" s="7" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="V86" s="1" t="s">
         <v>2</v>
@@ -16227,7 +16222,7 @@
         <v>0</v>
       </c>
       <c r="AB86" s="27" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="87" spans="1:28" ht="60">
@@ -16291,7 +16286,7 @@
         <v>1500</v>
       </c>
       <c r="T87" s="12" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="U87" s="7" t="s">
         <v>667</v>
@@ -16315,7 +16310,7 @@
         <v>0</v>
       </c>
       <c r="AB87" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="88" spans="1:28" ht="60">
@@ -16379,7 +16374,7 @@
         <v>1750</v>
       </c>
       <c r="T88" s="12" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="U88" s="7" t="s">
         <v>533</v>
@@ -16403,7 +16398,7 @@
         <v>0</v>
       </c>
       <c r="AB88" s="27" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="89" spans="1:28" ht="60">
@@ -16467,13 +16462,13 @@
         <v>1800</v>
       </c>
       <c r="T89" s="12" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="U89" s="7" t="s">
         <v>529</v>
       </c>
       <c r="V89" s="1" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="W89" s="1" t="s">
         <v>142</v>
@@ -16491,7 +16486,7 @@
         <v>0</v>
       </c>
       <c r="AB89" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="90" spans="1:28" ht="60">
@@ -16555,10 +16550,10 @@
         <v>1650</v>
       </c>
       <c r="T90" s="12" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="U90" s="7" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="V90" s="1" t="s">
         <v>28</v>
@@ -16579,10 +16574,10 @@
         <v>0</v>
       </c>
       <c r="AB90" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
-    <row r="91" spans="1:28" ht="36" hidden="1">
+    <row r="91" spans="1:28" ht="36">
       <c r="A91">
         <v>53000091</v>
       </c>
@@ -16665,7 +16660,7 @@
         <v>0</v>
       </c>
       <c r="AB91" s="27" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="92" spans="1:28" ht="60">
@@ -16729,7 +16724,7 @@
         <v>1500</v>
       </c>
       <c r="T92" s="12" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="U92" s="7" t="s">
         <v>535</v>
@@ -16753,10 +16748,10 @@
         <v>0</v>
       </c>
       <c r="AB92" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
-    <row r="93" spans="1:28" ht="48" hidden="1">
+    <row r="93" spans="1:28" ht="48">
       <c r="A93">
         <v>53000093</v>
       </c>
@@ -16839,10 +16834,10 @@
         <v>0</v>
       </c>
       <c r="AB93" s="27" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
-    <row r="94" spans="1:28" ht="36" hidden="1">
+    <row r="94" spans="1:28" ht="36">
       <c r="A94">
         <v>53000094</v>
       </c>
@@ -16903,7 +16898,7 @@
         <v>500</v>
       </c>
       <c r="T94" s="12" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="U94" s="1" t="s">
         <v>650</v>
@@ -16925,7 +16920,7 @@
         <v>0</v>
       </c>
       <c r="AB94" s="27" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="95" spans="1:28" ht="48">
@@ -16989,7 +16984,7 @@
         <v>1600</v>
       </c>
       <c r="T95" s="12" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="U95" s="7" t="s">
         <v>568</v>
@@ -17013,10 +17008,10 @@
         <v>0</v>
       </c>
       <c r="AB95" s="27" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
-    <row r="96" spans="1:28" ht="24" hidden="1">
+    <row r="96" spans="1:28" ht="24">
       <c r="A96">
         <v>53000096</v>
       </c>
@@ -17099,7 +17094,7 @@
         <v>0</v>
       </c>
       <c r="AB96" s="27" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="97" spans="1:28" ht="60">
@@ -17163,7 +17158,7 @@
         <v>900</v>
       </c>
       <c r="T97" s="12" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="U97" s="7" t="s">
         <v>526</v>
@@ -17187,10 +17182,10 @@
         <v>0</v>
       </c>
       <c r="AB97" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
-    <row r="98" spans="1:28" ht="24" hidden="1">
+    <row r="98" spans="1:28" ht="24">
       <c r="A98">
         <v>53000098</v>
       </c>
@@ -17273,10 +17268,10 @@
         <v>0</v>
       </c>
       <c r="AB98" s="27" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
-    <row r="99" spans="1:28" ht="24" hidden="1">
+    <row r="99" spans="1:28" ht="24">
       <c r="A99">
         <v>53000099</v>
       </c>
@@ -17359,10 +17354,10 @@
         <v>0</v>
       </c>
       <c r="AB99" s="27" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
-    <row r="100" spans="1:28" ht="24" hidden="1">
+    <row r="100" spans="1:28" ht="24">
       <c r="A100">
         <v>53000100</v>
       </c>
@@ -17445,10 +17440,10 @@
         <v>0</v>
       </c>
       <c r="AB100" s="27" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
-    <row r="101" spans="1:28" ht="48" hidden="1">
+    <row r="101" spans="1:28" ht="48">
       <c r="A101">
         <v>53000101</v>
       </c>
@@ -17509,7 +17504,7 @@
         <v>1500</v>
       </c>
       <c r="T101" s="12" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="U101" s="7" t="s">
         <v>578</v>
@@ -17531,10 +17526,10 @@
         <v>0</v>
       </c>
       <c r="AB101" s="27" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
-    <row r="102" spans="1:28" ht="24" hidden="1">
+    <row r="102" spans="1:28" ht="24">
       <c r="A102">
         <v>53000102</v>
       </c>
@@ -17617,7 +17612,7 @@
         <v>0</v>
       </c>
       <c r="AB102" s="27" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="103" spans="1:28" ht="60">
@@ -17681,10 +17676,10 @@
         <v>1300</v>
       </c>
       <c r="T103" s="12" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="U103" s="7" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="V103" s="1" t="s">
         <v>162</v>
@@ -17705,10 +17700,10 @@
         <v>0</v>
       </c>
       <c r="AB103" s="27" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
-    <row r="104" spans="1:28" ht="14.25" hidden="1">
+    <row r="104" spans="1:28" ht="14.25">
       <c r="A104">
         <v>53000104</v>
       </c>
@@ -17770,7 +17765,7 @@
       </c>
       <c r="T104" s="12"/>
       <c r="U104" s="7" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="V104" s="1" t="s">
         <v>164</v>
@@ -17789,10 +17784,10 @@
         <v>0</v>
       </c>
       <c r="AB104" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
-    <row r="105" spans="1:28" ht="36" hidden="1">
+    <row r="105" spans="1:28" ht="36">
       <c r="A105">
         <v>53000105</v>
       </c>
@@ -17853,7 +17848,7 @@
         <v>500</v>
       </c>
       <c r="T105" s="12" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="U105" s="1" t="s">
         <v>563</v>
@@ -17875,10 +17870,10 @@
         <v>0</v>
       </c>
       <c r="AB105" s="27" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
-    <row r="106" spans="1:28" ht="24" hidden="1">
+    <row r="106" spans="1:28" ht="24">
       <c r="A106">
         <v>53000106</v>
       </c>
@@ -17939,10 +17934,10 @@
         <v>1800</v>
       </c>
       <c r="T106" s="12" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="U106" s="7" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="V106" s="1" t="s">
         <v>168</v>
@@ -17961,10 +17956,10 @@
         <v>0</v>
       </c>
       <c r="AB106" s="27" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
-    <row r="107" spans="1:28" ht="24" hidden="1">
+    <row r="107" spans="1:28" ht="24">
       <c r="A107">
         <v>53000107</v>
       </c>
@@ -18025,7 +18020,7 @@
         <v>1800</v>
       </c>
       <c r="T107" s="12" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="U107" s="7" t="s">
         <v>560</v>
@@ -18047,10 +18042,10 @@
         <v>0</v>
       </c>
       <c r="AB107" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
-    <row r="108" spans="1:28" ht="120" hidden="1">
+    <row r="108" spans="1:28" ht="120">
       <c r="A108">
         <v>53000108</v>
       </c>
@@ -18111,7 +18106,7 @@
         <v>1700</v>
       </c>
       <c r="T108" s="12" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="U108" s="7" t="s">
         <v>527</v>
@@ -18133,10 +18128,10 @@
         <v>0</v>
       </c>
       <c r="AB108" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
-    <row r="109" spans="1:28" ht="24" hidden="1">
+    <row r="109" spans="1:28" ht="24">
       <c r="A109">
         <v>53000109</v>
       </c>
@@ -18219,10 +18214,10 @@
         <v>0</v>
       </c>
       <c r="AB109" s="27" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
-    <row r="110" spans="1:28" ht="36" hidden="1">
+    <row r="110" spans="1:28" ht="36">
       <c r="A110">
         <v>53000110</v>
       </c>
@@ -18283,7 +18278,7 @@
         <v>2100</v>
       </c>
       <c r="T110" s="12" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="U110" s="7" t="s">
         <v>621</v>
@@ -18305,10 +18300,10 @@
         <v>0</v>
       </c>
       <c r="AB110" s="27" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
-    <row r="111" spans="1:28" ht="48" hidden="1">
+    <row r="111" spans="1:28" ht="48">
       <c r="A111">
         <v>53000111</v>
       </c>
@@ -18369,7 +18364,7 @@
         <v>1600</v>
       </c>
       <c r="T111" s="12" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="U111" s="7" t="s">
         <v>541</v>
@@ -18391,10 +18386,10 @@
         <v>0</v>
       </c>
       <c r="AB111" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
-    <row r="112" spans="1:28" ht="24" hidden="1">
+    <row r="112" spans="1:28" ht="24">
       <c r="A112">
         <v>53000112</v>
       </c>
@@ -18477,10 +18472,10 @@
         <v>0</v>
       </c>
       <c r="AB112" s="27" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
-    <row r="113" spans="1:28" ht="24" hidden="1">
+    <row r="113" spans="1:28" ht="24">
       <c r="A113">
         <v>53000113</v>
       </c>
@@ -18541,10 +18536,10 @@
         <v>1400</v>
       </c>
       <c r="T113" s="12" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="U113" s="7" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="V113" s="1" t="s">
         <v>181</v>
@@ -18563,10 +18558,10 @@
         <v>0</v>
       </c>
       <c r="AB113" s="27" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
-    <row r="114" spans="1:28" ht="24" hidden="1">
+    <row r="114" spans="1:28" ht="24">
       <c r="A114">
         <v>53000114</v>
       </c>
@@ -18649,10 +18644,10 @@
         <v>0</v>
       </c>
       <c r="AB114" s="27" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
-    <row r="115" spans="1:28" ht="36" hidden="1">
+    <row r="115" spans="1:28" ht="36">
       <c r="A115">
         <v>53000115</v>
       </c>
@@ -18735,10 +18730,10 @@
         <v>0</v>
       </c>
       <c r="AB115" s="27" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
-    <row r="116" spans="1:28" ht="36" hidden="1">
+    <row r="116" spans="1:28" ht="36">
       <c r="A116">
         <v>53000116</v>
       </c>
@@ -18821,10 +18816,10 @@
         <v>0</v>
       </c>
       <c r="AB116" s="27" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
-    <row r="117" spans="1:28" ht="48" hidden="1">
+    <row r="117" spans="1:28" ht="48">
       <c r="A117">
         <v>53000117</v>
       </c>
@@ -18907,10 +18902,10 @@
         <v>0</v>
       </c>
       <c r="AB117" s="27" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
-    <row r="118" spans="1:28" ht="48" hidden="1">
+    <row r="118" spans="1:28" ht="48">
       <c r="A118">
         <v>53000118</v>
       </c>
@@ -18993,10 +18988,10 @@
         <v>0</v>
       </c>
       <c r="AB118" s="27" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
-    <row r="119" spans="1:28" ht="48" hidden="1">
+    <row r="119" spans="1:28" ht="48">
       <c r="A119">
         <v>53000119</v>
       </c>
@@ -19079,10 +19074,10 @@
         <v>0</v>
       </c>
       <c r="AB119" s="27" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
-    <row r="120" spans="1:28" ht="48" hidden="1">
+    <row r="120" spans="1:28" ht="48">
       <c r="A120">
         <v>53000120</v>
       </c>
@@ -19165,10 +19160,10 @@
         <v>0</v>
       </c>
       <c r="AB120" s="27" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
-    <row r="121" spans="1:28" ht="48" hidden="1">
+    <row r="121" spans="1:28" ht="48">
       <c r="A121">
         <v>53000121</v>
       </c>
@@ -19251,10 +19246,10 @@
         <v>0</v>
       </c>
       <c r="AB121" s="27" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
-    <row r="122" spans="1:28" ht="48" hidden="1">
+    <row r="122" spans="1:28" ht="48">
       <c r="A122">
         <v>53000122</v>
       </c>
@@ -19337,10 +19332,10 @@
         <v>0</v>
       </c>
       <c r="AB122" s="27" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
-    <row r="123" spans="1:28" ht="48" hidden="1">
+    <row r="123" spans="1:28" ht="48">
       <c r="A123">
         <v>53000123</v>
       </c>
@@ -19423,10 +19418,10 @@
         <v>0</v>
       </c>
       <c r="AB123" s="27" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
-    <row r="124" spans="1:28" ht="48" hidden="1">
+    <row r="124" spans="1:28" ht="48">
       <c r="A124">
         <v>53000124</v>
       </c>
@@ -19509,10 +19504,10 @@
         <v>0</v>
       </c>
       <c r="AB124" s="27" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
-    <row r="125" spans="1:28" ht="48" hidden="1">
+    <row r="125" spans="1:28" ht="48">
       <c r="A125">
         <v>53000125</v>
       </c>
@@ -19595,7 +19590,7 @@
         <v>0</v>
       </c>
       <c r="AB125" s="27" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="126" spans="1:28" ht="72">
@@ -19659,16 +19654,16 @@
         <v>2200</v>
       </c>
       <c r="T126" s="12" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="U126" s="7" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="V126" s="1" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="W126" s="1" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="X126" s="1">
         <v>4</v>
@@ -19683,7 +19678,7 @@
         <v>1</v>
       </c>
       <c r="AB126" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="127" spans="1:28" ht="48">
@@ -19747,7 +19742,7 @@
         <v>3000</v>
       </c>
       <c r="T127" s="12" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="U127" s="7" t="s">
         <v>569</v>
@@ -19771,10 +19766,10 @@
         <v>1</v>
       </c>
       <c r="AB127" s="27" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
-    <row r="128" spans="1:28" ht="36" hidden="1">
+    <row r="128" spans="1:28" ht="36">
       <c r="A128">
         <v>53000129</v>
       </c>
@@ -19857,7 +19852,7 @@
         <v>1</v>
       </c>
       <c r="AB128" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
   </sheetData>
@@ -19866,81 +19861,81 @@
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I121:I127 I71:I115 I4:I36 I39:I69">
-    <cfRule type="cellIs" dxfId="36" priority="47" operator="notEqual">
+    <cfRule type="cellIs" dxfId="127" priority="47" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J128:P128 J71:P126 J5:P36 J39:P69 J4:O4">
-    <cfRule type="cellIs" dxfId="35" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="46" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I127">
-    <cfRule type="cellIs" dxfId="34" priority="44" operator="notEqual">
+    <cfRule type="cellIs" dxfId="125" priority="44" operator="notEqual">
       <formula>$E127</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I116:I120">
-    <cfRule type="cellIs" dxfId="33" priority="42" operator="notEqual">
+    <cfRule type="cellIs" dxfId="124" priority="42" operator="notEqual">
       <formula>$E116</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I128">
-    <cfRule type="cellIs" dxfId="32" priority="41" operator="notEqual">
+    <cfRule type="cellIs" dxfId="123" priority="41" operator="notEqual">
       <formula>$E128</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J128:P128">
-    <cfRule type="cellIs" dxfId="31" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="40" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J127:P127">
-    <cfRule type="cellIs" dxfId="30" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="26" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I70">
-    <cfRule type="cellIs" dxfId="29" priority="11" operator="notEqual">
+    <cfRule type="cellIs" dxfId="120" priority="11" operator="notEqual">
       <formula>$E70</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J70:P70">
-    <cfRule type="cellIs" dxfId="28" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37">
-    <cfRule type="cellIs" dxfId="27" priority="9" operator="notEqual">
+    <cfRule type="cellIs" dxfId="118" priority="9" operator="notEqual">
       <formula>$E37</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J37:P37">
-    <cfRule type="cellIs" dxfId="26" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38">
-    <cfRule type="cellIs" dxfId="25" priority="7" operator="notEqual">
+    <cfRule type="cellIs" dxfId="116" priority="7" operator="notEqual">
       <formula>$E38</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J38:P38">
-    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H128">
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="4" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="111" priority="5" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20020,7 +20015,7 @@
         <v>214</v>
       </c>
       <c r="H1" s="40" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>490</v>
@@ -20044,7 +20039,7 @@
         <v>504</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="Q1" s="14" t="s">
         <v>487</v>
@@ -20065,7 +20060,7 @@
         <v>656</v>
       </c>
       <c r="W1" s="14" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="X1" s="14" t="s">
         <v>215</v>
@@ -20080,7 +20075,7 @@
         <v>625</v>
       </c>
       <c r="AB1" s="36" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="2" spans="1:28">
@@ -20130,7 +20125,7 @@
         <v>491</v>
       </c>
       <c r="P2" s="19" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>488</v>
@@ -20151,7 +20146,7 @@
         <v>201</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="X2" s="4" t="s">
         <v>200</v>
@@ -20192,7 +20187,7 @@
         <v>206</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>492</v>
@@ -20216,7 +20211,7 @@
         <v>506</v>
       </c>
       <c r="P3" s="42" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>489</v>
@@ -20237,7 +20232,7 @@
         <v>494</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="X3" s="2" t="s">
         <v>208</v>
@@ -20252,7 +20247,7 @@
         <v>626</v>
       </c>
       <c r="AB3" s="28" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="24">
@@ -20552,7 +20547,7 @@
         <v>-1</v>
       </c>
       <c r="T7" s="12" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="U7" s="7" t="s">
         <v>646</v>
@@ -20712,7 +20707,7 @@
         <v>-1</v>
       </c>
       <c r="T9" s="12" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="U9" s="7" t="s">
         <v>639</v>
@@ -20738,77 +20733,77 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="J4:P9">
-    <cfRule type="cellIs" dxfId="19" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="31" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:P8">
-    <cfRule type="cellIs" dxfId="18" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="27" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:P4">
-    <cfRule type="cellIs" dxfId="17" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="26" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="16" priority="25" operator="notEqual">
+    <cfRule type="cellIs" dxfId="76" priority="25" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:P4">
-    <cfRule type="cellIs" dxfId="15" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="24" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="14" priority="23" operator="notEqual">
+    <cfRule type="cellIs" dxfId="74" priority="23" operator="notEqual">
       <formula>$E5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:P5">
-    <cfRule type="cellIs" dxfId="13" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="22" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" dxfId="12" priority="21" operator="notEqual">
+    <cfRule type="cellIs" dxfId="72" priority="21" operator="notEqual">
       <formula>$E6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:P6">
-    <cfRule type="cellIs" dxfId="11" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="20" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="10" priority="19" operator="notEqual">
+    <cfRule type="cellIs" dxfId="70" priority="19" operator="notEqual">
       <formula>$E7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:P7">
-    <cfRule type="cellIs" dxfId="9" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="18" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="8" priority="17" operator="notEqual">
+    <cfRule type="cellIs" dxfId="68" priority="17" operator="notEqual">
       <formula>$E8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:P8">
-    <cfRule type="cellIs" dxfId="7" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="16" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="cellIs" dxfId="6" priority="15" operator="notEqual">
+    <cfRule type="cellIs" dxfId="66" priority="15" operator="notEqual">
       <formula>$E9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:P9">
-    <cfRule type="cellIs" dxfId="5" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="14" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20825,11 +20820,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="T6" sqref="T6"/>
+      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -20878,7 +20873,7 @@
         <v>214</v>
       </c>
       <c r="H1" s="40" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>490</v>
@@ -20902,7 +20897,7 @@
         <v>504</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="Q1" s="14" t="s">
         <v>487</v>
@@ -20923,7 +20918,7 @@
         <v>656</v>
       </c>
       <c r="W1" s="14" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="X1" s="14" t="s">
         <v>215</v>
@@ -20938,7 +20933,7 @@
         <v>625</v>
       </c>
       <c r="AB1" s="36" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="2" spans="1:28">
@@ -20988,7 +20983,7 @@
         <v>491</v>
       </c>
       <c r="P2" s="19" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>488</v>
@@ -21009,7 +21004,7 @@
         <v>201</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="X2" s="4" t="s">
         <v>200</v>
@@ -21050,7 +21045,7 @@
         <v>206</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>492</v>
@@ -21074,7 +21069,7 @@
         <v>506</v>
       </c>
       <c r="P3" s="42" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>489</v>
@@ -21095,7 +21090,7 @@
         <v>494</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="X3" s="2" t="s">
         <v>208</v>
@@ -21110,7 +21105,7 @@
         <v>626</v>
       </c>
       <c r="AB3" s="28" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="36">
@@ -21118,13 +21113,13 @@
         <v>53200100</v>
       </c>
       <c r="B4" s="24" t="s">
+        <v>747</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>748</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="D4" s="8" t="s">
         <v>749</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>750</v>
       </c>
       <c r="E4" s="16">
         <v>3</v>
@@ -21174,7 +21169,7 @@
         <v>2300</v>
       </c>
       <c r="T4" s="12" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="U4" s="7" t="s">
         <v>644</v>
@@ -21196,7 +21191,7 @@
         <v>0</v>
       </c>
       <c r="AB4" s="27" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="24">
@@ -21204,13 +21199,13 @@
         <v>53200101</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>738</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>739</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="8" t="s">
         <v>740</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>741</v>
       </c>
       <c r="E5" s="16">
         <v>3</v>
@@ -21260,7 +21255,7 @@
         <v>1800</v>
       </c>
       <c r="T5" s="12" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="U5" s="7" t="s">
         <v>654</v>
@@ -21282,7 +21277,7 @@
         <v>0</v>
       </c>
       <c r="AB5" s="27" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="40.5">
@@ -21290,13 +21285,13 @@
         <v>53200102</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>750</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>751</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="8" t="s">
         <v>752</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>753</v>
       </c>
       <c r="E6" s="16">
         <v>3</v>
@@ -21346,10 +21341,10 @@
         <v>2300</v>
       </c>
       <c r="T6" s="12" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="U6" s="34" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="V6" s="1" t="s">
         <v>53</v>
@@ -21368,7 +21363,7 @@
         <v>0</v>
       </c>
       <c r="AB6" s="27" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="14.25">
@@ -21376,13 +21371,13 @@
         <v>53200103</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>742</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>743</v>
       </c>
       <c r="E7" s="16">
         <v>3</v>
@@ -21433,7 +21428,7 @@
       </c>
       <c r="T7" s="12"/>
       <c r="U7" s="34" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="V7" s="1" t="s">
         <v>52</v>
@@ -21452,7 +21447,7 @@
         <v>0</v>
       </c>
       <c r="AB7" s="27" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="60">
@@ -21460,13 +21455,13 @@
         <v>53200104</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>758</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>759</v>
       </c>
       <c r="E8" s="16">
         <v>3</v>
@@ -21516,16 +21511,16 @@
         <v>1800</v>
       </c>
       <c r="T8" s="12" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="U8" s="7" t="s">
         <v>666</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="X8" s="1">
         <v>4</v>
@@ -21540,7 +21535,7 @@
         <v>0</v>
       </c>
       <c r="AB8" s="27" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="9" spans="1:28" ht="24">
@@ -21548,13 +21543,13 @@
         <v>53200105</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>760</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>761</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="8" t="s">
         <v>762</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>763</v>
       </c>
       <c r="E9" s="16">
         <v>3</v>
@@ -21604,7 +21599,7 @@
         <v>8000</v>
       </c>
       <c r="T9" s="12" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="U9" s="7" t="s">
         <v>509</v>
@@ -21626,28 +21621,28 @@
         <v>0</v>
       </c>
       <c r="AB9" s="27" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I4:I9">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="notEqual">
+    <cfRule type="cellIs" dxfId="33" priority="4" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:P7">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:P9">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:P8">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21798,12 +21793,12 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B2">
         <f>COUNTIF(标准!AB:AB,"*单伤*")</f>
@@ -21812,7 +21807,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B3">
         <f>COUNTIF(标准!AB:AB,"*群伤*")</f>
@@ -21821,7 +21816,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B4">
         <f>COUNTIF(标准!AB:AB,"*单治*")</f>
@@ -21830,7 +21825,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B5">
         <f>COUNTIF(标准!AB:AB,"*群治*")</f>
@@ -21839,7 +21834,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B6">
         <f>COUNTIF(标准!AB:AB,"*正状*")</f>
@@ -21848,7 +21843,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B7">
         <f>COUNTIF(标准!AB:AB,"*负状*")</f>
@@ -21857,7 +21852,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B8">
         <f>COUNTIF(标准!AB:AB,"*手牌*")</f>
@@ -21866,7 +21861,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B9">
         <f>COUNTIF(标准!AB:AB,"*过牌*")</f>
@@ -21875,7 +21870,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="B10">
         <f>COUNTIF(标准!AB:AB,"*陷阱*")</f>
@@ -21884,7 +21879,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B11">
         <f>COUNTIF(标准!AB:AB,"*地形*")</f>
@@ -21893,7 +21888,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B12">
         <f>COUNTIF(标准!AB:AB,"*属性*")</f>

</xml_diff>

<commit_message>
#23 new system about spike and config data upgrade
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -717,7 +717,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="882">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="881">
   <si>
     <t>慈悲</t>
   </si>
@@ -3126,10 +3126,6 @@
   </si>
   <si>
     <t>使目标减速{3:0}%</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>p.MpCost+=2;p.LpCost-=2;</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -4062,7 +4058,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="44">
+  <fills count="45">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4305,6 +4301,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4599,7 +4601,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4734,6 +4736,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="44" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -7484,7 +7489,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7633,11 +7637,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1761749920"/>
-        <c:axId val="1761754272"/>
+        <c:axId val="1761761344"/>
+        <c:axId val="1761758080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1761749920"/>
+        <c:axId val="1761761344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7680,7 +7684,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1761754272"/>
+        <c:crossAx val="1761758080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7688,7 +7692,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1761754272"/>
+        <c:axId val="1761758080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7739,7 +7743,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1761749920"/>
+        <c:crossAx val="1761761344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8788,10 +8792,10 @@
   <dimension ref="A1:AB128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="T36" sqref="T36"/>
+      <selection pane="bottomRight" activeCell="P77" sqref="P77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -8838,7 +8842,7 @@
         <v>214</v>
       </c>
       <c r="H1" s="40" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>490</v>
@@ -8862,7 +8866,7 @@
         <v>504</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="Q1" s="14" t="s">
         <v>487</v>
@@ -8883,7 +8887,7 @@
         <v>656</v>
       </c>
       <c r="W1" s="14" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="X1" s="14" t="s">
         <v>215</v>
@@ -8948,7 +8952,7 @@
         <v>505</v>
       </c>
       <c r="P2" s="19" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>488</v>
@@ -8960,7 +8964,7 @@
         <v>658</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="U2" s="11" t="s">
         <v>201</v>
@@ -8969,7 +8973,7 @@
         <v>201</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="X2" s="4" t="s">
         <v>200</v>
@@ -9010,7 +9014,7 @@
         <v>206</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>492</v>
@@ -9034,19 +9038,19 @@
         <v>506</v>
       </c>
       <c r="P3" s="42" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>489</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>659</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="U3" s="6" t="s">
         <v>470</v>
@@ -9055,7 +9059,7 @@
         <v>494</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="X3" s="2" t="s">
         <v>208</v>
@@ -9134,7 +9138,7 @@
         <v>1704</v>
       </c>
       <c r="T4" s="12" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="U4" s="33" t="s">
         <v>581</v>
@@ -9156,7 +9160,7 @@
         <v>0</v>
       </c>
       <c r="AB4" s="27" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="14.25">
@@ -9242,7 +9246,7 @@
         <v>0</v>
       </c>
       <c r="AB5" s="27" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="24">
@@ -9306,7 +9310,7 @@
         <v>2000</v>
       </c>
       <c r="T6" s="12" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="U6" s="7" t="s">
         <v>654</v>
@@ -9328,7 +9332,7 @@
         <v>0</v>
       </c>
       <c r="AB6" s="27" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="36">
@@ -9392,7 +9396,7 @@
         <v>2000</v>
       </c>
       <c r="T7" s="12" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="U7" s="7" t="s">
         <v>655</v>
@@ -9414,7 +9418,7 @@
         <v>0</v>
       </c>
       <c r="AB7" s="27" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="24">
@@ -9478,7 +9482,7 @@
         <v>900</v>
       </c>
       <c r="T8" s="12" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="U8" s="7" t="s">
         <v>546</v>
@@ -9500,7 +9504,7 @@
         <v>0</v>
       </c>
       <c r="AB8" s="27" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="9" spans="1:28" ht="48">
@@ -9586,7 +9590,7 @@
         <v>0</v>
       </c>
       <c r="AB9" s="27" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="10" spans="1:28" ht="48">
@@ -9672,7 +9676,7 @@
         <v>0</v>
       </c>
       <c r="AB10" s="27" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="48">
@@ -9758,7 +9762,7 @@
         <v>0</v>
       </c>
       <c r="AB11" s="27" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="12" spans="1:28" ht="48">
@@ -9844,7 +9848,7 @@
         <v>0</v>
       </c>
       <c r="AB12" s="27" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="48">
@@ -9930,7 +9934,7 @@
         <v>0</v>
       </c>
       <c r="AB13" s="27" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="48">
@@ -10016,7 +10020,7 @@
         <v>0</v>
       </c>
       <c r="AB14" s="27" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="15" spans="1:28" ht="48">
@@ -10102,7 +10106,7 @@
         <v>0</v>
       </c>
       <c r="AB15" s="27" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="48">
@@ -10188,7 +10192,7 @@
         <v>0</v>
       </c>
       <c r="AB16" s="27" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="17" spans="1:28" ht="48">
@@ -10274,7 +10278,7 @@
         <v>0</v>
       </c>
       <c r="AB17" s="27" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="18" spans="1:28" ht="14.25">
@@ -10360,7 +10364,7 @@
         <v>0</v>
       </c>
       <c r="AB18" s="27" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="19" spans="1:28" ht="24">
@@ -10424,7 +10428,7 @@
         <v>1200</v>
       </c>
       <c r="T19" s="12" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="U19" s="7" t="s">
         <v>508</v>
@@ -10446,7 +10450,7 @@
         <v>0</v>
       </c>
       <c r="AB19" s="27" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="20" spans="1:28" ht="24">
@@ -10510,7 +10514,7 @@
         <v>8000</v>
       </c>
       <c r="T20" s="12" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="U20" s="7" t="s">
         <v>509</v>
@@ -10532,7 +10536,7 @@
         <v>0</v>
       </c>
       <c r="AB20" s="27" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="21" spans="1:28" ht="48">
@@ -10618,7 +10622,7 @@
         <v>0</v>
       </c>
       <c r="AB21" s="27" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="22" spans="1:28" ht="60">
@@ -10682,7 +10686,7 @@
         <v>1800</v>
       </c>
       <c r="T22" s="12" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="U22" s="7" t="s">
         <v>666</v>
@@ -10706,7 +10710,7 @@
         <v>0</v>
       </c>
       <c r="AB22" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="23" spans="1:28" ht="60">
@@ -10770,7 +10774,7 @@
         <v>2100</v>
       </c>
       <c r="T23" s="12" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="U23" s="7" t="s">
         <v>667</v>
@@ -10794,7 +10798,7 @@
         <v>0</v>
       </c>
       <c r="AB23" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="24" spans="1:28" ht="60">
@@ -10858,7 +10862,7 @@
         <v>1875</v>
       </c>
       <c r="T24" s="12" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="U24" s="7" t="s">
         <v>668</v>
@@ -10882,7 +10886,7 @@
         <v>0</v>
       </c>
       <c r="AB24" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="25" spans="1:28" ht="24">
@@ -10968,7 +10972,7 @@
         <v>0</v>
       </c>
       <c r="AB25" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="26" spans="1:28" ht="24">
@@ -11054,7 +11058,7 @@
         <v>0</v>
       </c>
       <c r="AB26" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="27" spans="1:28" ht="24">
@@ -11140,7 +11144,7 @@
         <v>0</v>
       </c>
       <c r="AB27" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="28" spans="1:28" ht="48">
@@ -11226,7 +11230,7 @@
         <v>0</v>
       </c>
       <c r="AB28" s="27" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="29" spans="1:28" ht="24">
@@ -11312,7 +11316,7 @@
         <v>0</v>
       </c>
       <c r="AB29" s="27" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="30" spans="1:28" ht="14.25">
@@ -11396,7 +11400,7 @@
         <v>0</v>
       </c>
       <c r="AB30" s="27" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="31" spans="1:28" ht="14.25">
@@ -11480,7 +11484,7 @@
         <v>0</v>
       </c>
       <c r="AB31" s="27" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="32" spans="1:28" ht="24">
@@ -11566,7 +11570,7 @@
         <v>0</v>
       </c>
       <c r="AB32" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="33" spans="1:28" ht="24">
@@ -11574,13 +11578,13 @@
         <v>53000030</v>
       </c>
       <c r="B33" s="9" t="s">
+        <v>774</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>775</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>776</v>
-      </c>
       <c r="D33" s="8" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="E33" s="1">
         <v>2</v>
@@ -11630,10 +11634,10 @@
         <v>1500</v>
       </c>
       <c r="T33" s="12" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="U33" s="1" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="V33" s="1" t="s">
         <v>4</v>
@@ -11652,7 +11656,7 @@
         <v>1</v>
       </c>
       <c r="AB33" s="27" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="34" spans="1:28" ht="24">
@@ -11660,13 +11664,13 @@
         <v>53000031</v>
       </c>
       <c r="B34" s="9" t="s">
+        <v>777</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>778</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>779</v>
-      </c>
       <c r="D34" s="8" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="E34" s="1">
         <v>2</v>
@@ -11716,10 +11720,10 @@
         <v>1500</v>
       </c>
       <c r="T34" s="12" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="U34" s="1" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="V34" s="1" t="s">
         <v>4</v>
@@ -11738,7 +11742,7 @@
         <v>1</v>
       </c>
       <c r="AB34" s="27" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="35" spans="1:28" ht="48">
@@ -11802,7 +11806,7 @@
         <v>2000</v>
       </c>
       <c r="T35" s="12" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="U35" s="7" t="s">
         <v>513</v>
@@ -11824,7 +11828,7 @@
         <v>0</v>
       </c>
       <c r="AB35" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="36" spans="1:28" ht="36">
@@ -11889,7 +11893,7 @@
         <v>1220</v>
       </c>
       <c r="T36" s="12" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="U36" s="1" t="s">
         <v>679</v>
@@ -11911,7 +11915,7 @@
         <v>0</v>
       </c>
       <c r="AB36" s="27" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="37" spans="1:28" ht="14.25">
@@ -11995,7 +11999,7 @@
         <v>0</v>
       </c>
       <c r="AB37" s="27" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="38" spans="1:28" ht="14.25">
@@ -12060,7 +12064,7 @@
       </c>
       <c r="T38" s="12"/>
       <c r="U38" s="7" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="V38" s="1" t="s">
         <v>63</v>
@@ -12079,7 +12083,7 @@
         <v>0</v>
       </c>
       <c r="AB38" s="27" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="39" spans="1:28" ht="24">
@@ -12087,10 +12091,10 @@
         <v>53000039</v>
       </c>
       <c r="B39" s="9" t="s">
+        <v>768</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>769</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>770</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>374</v>
@@ -12143,10 +12147,10 @@
         <v>1700</v>
       </c>
       <c r="T39" s="12" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="U39" s="1" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="V39" s="1" t="s">
         <v>4</v>
@@ -12165,7 +12169,7 @@
         <v>0</v>
       </c>
       <c r="AB39" s="27" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="40" spans="1:28" ht="24">
@@ -12173,7 +12177,7 @@
         <v>53000040</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>270</v>
@@ -12229,10 +12233,10 @@
         <v>2000</v>
       </c>
       <c r="T40" s="12" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="U40" s="1" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="V40" s="1" t="s">
         <v>4</v>
@@ -12251,7 +12255,7 @@
         <v>0</v>
       </c>
       <c r="AB40" s="27" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="41" spans="1:28" ht="24">
@@ -12337,7 +12341,7 @@
         <v>0</v>
       </c>
       <c r="AB41" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="42" spans="1:28" ht="48">
@@ -12401,7 +12405,7 @@
         <v>2000</v>
       </c>
       <c r="T42" s="12" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="U42" s="1" t="s">
         <v>514</v>
@@ -12423,7 +12427,7 @@
         <v>0</v>
       </c>
       <c r="AB42" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="43" spans="1:28" ht="24">
@@ -12509,7 +12513,7 @@
         <v>0</v>
       </c>
       <c r="AB43" s="27" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="44" spans="1:28" ht="24">
@@ -12517,7 +12521,7 @@
         <v>53000044</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>274</v>
@@ -12573,10 +12577,10 @@
         <v>1900</v>
       </c>
       <c r="T44" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="U44" s="1" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="V44" s="1" t="s">
         <v>4</v>
@@ -12595,7 +12599,7 @@
         <v>0</v>
       </c>
       <c r="AB44" s="27" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="45" spans="1:28" ht="60">
@@ -12682,7 +12686,7 @@
         <v>0</v>
       </c>
       <c r="AB45" s="27" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="46" spans="1:28" ht="48">
@@ -12746,7 +12750,7 @@
         <v>2000</v>
       </c>
       <c r="T46" s="12" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="U46" s="7" t="s">
         <v>528</v>
@@ -12768,7 +12772,7 @@
         <v>0</v>
       </c>
       <c r="AB46" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="47" spans="1:28" ht="60">
@@ -12832,7 +12836,7 @@
         <v>2200</v>
       </c>
       <c r="T47" s="12" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="U47" s="7" t="s">
         <v>529</v>
@@ -12856,7 +12860,7 @@
         <v>0</v>
       </c>
       <c r="AB47" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="48" spans="1:28" ht="48">
@@ -12920,7 +12924,7 @@
         <v>2000</v>
       </c>
       <c r="T48" s="12" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="U48" s="1" t="s">
         <v>515</v>
@@ -12942,7 +12946,7 @@
         <v>0</v>
       </c>
       <c r="AB48" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="49" spans="1:28" ht="60">
@@ -13006,7 +13010,7 @@
         <v>2200</v>
       </c>
       <c r="T49" s="12" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="U49" s="7" t="s">
         <v>530</v>
@@ -13030,7 +13034,7 @@
         <v>0</v>
       </c>
       <c r="AB49" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="50" spans="1:28" ht="72">
@@ -13094,7 +13098,7 @@
         <v>1800</v>
       </c>
       <c r="T50" s="12" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="U50" s="7" t="s">
         <v>685</v>
@@ -13116,7 +13120,7 @@
         <v>0</v>
       </c>
       <c r="AB50" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="51" spans="1:28" ht="48">
@@ -13180,7 +13184,7 @@
         <v>2000</v>
       </c>
       <c r="T51" s="12" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="U51" s="1" t="s">
         <v>516</v>
@@ -13202,7 +13206,7 @@
         <v>0</v>
       </c>
       <c r="AB51" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="52" spans="1:28" ht="48">
@@ -13266,7 +13270,7 @@
         <v>2000</v>
       </c>
       <c r="T52" s="12" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="U52" s="1" t="s">
         <v>517</v>
@@ -13288,7 +13292,7 @@
         <v>0</v>
       </c>
       <c r="AB52" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="53" spans="1:28" ht="48">
@@ -13352,7 +13356,7 @@
         <v>2000</v>
       </c>
       <c r="T53" s="12" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="U53" s="1" t="s">
         <v>518</v>
@@ -13374,7 +13378,7 @@
         <v>0</v>
       </c>
       <c r="AB53" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="54" spans="1:28" ht="48">
@@ -13438,7 +13442,7 @@
         <v>1670</v>
       </c>
       <c r="T54" s="12" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="U54" s="7" t="s">
         <v>619</v>
@@ -13460,7 +13464,7 @@
         <v>0</v>
       </c>
       <c r="AB54" s="27" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="55" spans="1:28" ht="24">
@@ -13546,7 +13550,7 @@
         <v>0</v>
       </c>
       <c r="AB55" s="27" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="56" spans="1:28" ht="36">
@@ -13632,7 +13636,7 @@
         <v>0</v>
       </c>
       <c r="AB56" s="27" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="57" spans="1:28" ht="24">
@@ -13718,7 +13722,7 @@
         <v>0</v>
       </c>
       <c r="AB57" s="27" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="58" spans="1:28" ht="24">
@@ -13782,7 +13786,7 @@
         <v>1800</v>
       </c>
       <c r="T58" s="12" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="U58" s="7" t="s">
         <v>519</v>
@@ -13804,7 +13808,7 @@
         <v>0</v>
       </c>
       <c r="AB58" s="27" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="59" spans="1:28" ht="24">
@@ -13868,7 +13872,7 @@
         <v>560</v>
       </c>
       <c r="T59" s="12" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="U59" s="7" t="s">
         <v>579</v>
@@ -13890,7 +13894,7 @@
         <v>0</v>
       </c>
       <c r="AB59" s="27" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="60" spans="1:28" ht="36">
@@ -13976,7 +13980,7 @@
         <v>0</v>
       </c>
       <c r="AB60" s="27" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="61" spans="1:28" ht="48">
@@ -14040,7 +14044,7 @@
         <v>3000</v>
       </c>
       <c r="T61" s="12" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="U61" s="7" t="s">
         <v>570</v>
@@ -14062,7 +14066,7 @@
         <v>0</v>
       </c>
       <c r="AB61" s="27" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="62" spans="1:28" ht="24">
@@ -14126,7 +14130,7 @@
         <v>3000</v>
       </c>
       <c r="T62" s="12" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="U62" s="7" t="s">
         <v>520</v>
@@ -14148,7 +14152,7 @@
         <v>0</v>
       </c>
       <c r="AB62" s="27" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="63" spans="1:28" ht="14.25">
@@ -14234,7 +14238,7 @@
         <v>0</v>
       </c>
       <c r="AB63" s="27" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="64" spans="1:28" ht="24">
@@ -14298,7 +14302,7 @@
         <v>1500</v>
       </c>
       <c r="T64" s="12" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="U64" s="1" t="s">
         <v>686</v>
@@ -14320,7 +14324,7 @@
         <v>0</v>
       </c>
       <c r="AB64" s="27" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="65" spans="1:28" ht="48">
@@ -14384,7 +14388,7 @@
         <v>5000</v>
       </c>
       <c r="T65" s="12" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="U65" s="1" t="s">
         <v>710</v>
@@ -14406,7 +14410,7 @@
         <v>0</v>
       </c>
       <c r="AB65" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="66" spans="1:28" ht="24">
@@ -14470,10 +14474,10 @@
         <v>1700</v>
       </c>
       <c r="T66" s="12" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="U66" s="1" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="V66" s="1" t="s">
         <v>4</v>
@@ -14492,7 +14496,7 @@
         <v>0</v>
       </c>
       <c r="AB66" s="27" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="67" spans="1:28" ht="14.25">
@@ -14578,7 +14582,7 @@
         <v>0</v>
       </c>
       <c r="AB67" s="27" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="68" spans="1:28" ht="60">
@@ -14642,7 +14646,7 @@
         <v>1200</v>
       </c>
       <c r="T68" s="12" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="U68" s="7" t="s">
         <v>687</v>
@@ -14666,7 +14670,7 @@
         <v>0</v>
       </c>
       <c r="AB68" s="27" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="69" spans="1:28" ht="24">
@@ -14730,7 +14734,7 @@
         <v>2000</v>
       </c>
       <c r="T69" s="12" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="U69" s="7" t="s">
         <v>521</v>
@@ -14752,7 +14756,7 @@
         <v>0</v>
       </c>
       <c r="AB69" s="27" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="70" spans="1:28" ht="14.25">
@@ -14836,7 +14840,7 @@
         <v>0</v>
       </c>
       <c r="AB70" s="27" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="71" spans="1:28" ht="72">
@@ -14900,7 +14904,7 @@
         <v>2000</v>
       </c>
       <c r="T71" s="12" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="U71" s="7" t="s">
         <v>483</v>
@@ -14924,7 +14928,7 @@
         <v>0</v>
       </c>
       <c r="AB71" s="27" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="72" spans="1:28" ht="48">
@@ -14988,7 +14992,7 @@
         <v>4000</v>
       </c>
       <c r="T72" s="12" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="U72" s="1" t="s">
         <v>649</v>
@@ -15010,7 +15014,7 @@
         <v>0</v>
       </c>
       <c r="AB72" s="27" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="73" spans="1:28" ht="48">
@@ -15074,7 +15078,7 @@
         <v>1900</v>
       </c>
       <c r="T73" s="12" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="U73" s="7" t="s">
         <v>522</v>
@@ -15096,7 +15100,7 @@
         <v>0</v>
       </c>
       <c r="AB73" s="27" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="74" spans="1:28" ht="36">
@@ -15182,7 +15186,7 @@
         <v>0</v>
       </c>
       <c r="AB74" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="75" spans="1:28" ht="108">
@@ -15246,7 +15250,7 @@
         <v>3600</v>
       </c>
       <c r="T75" s="12" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="U75" s="7" t="s">
         <v>523</v>
@@ -15268,7 +15272,7 @@
         <v>0</v>
       </c>
       <c r="AB75" s="27" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="76" spans="1:28" ht="60">
@@ -15332,7 +15336,7 @@
         <v>2200</v>
       </c>
       <c r="T76" s="12" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="U76" s="7" t="s">
         <v>688</v>
@@ -15356,7 +15360,7 @@
         <v>0</v>
       </c>
       <c r="AB76" s="27" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="77" spans="1:28" ht="48">
@@ -15420,7 +15424,7 @@
         <v>1200</v>
       </c>
       <c r="T77" s="12" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="U77" s="7" t="s">
         <v>524</v>
@@ -15442,7 +15446,7 @@
         <v>0</v>
       </c>
       <c r="AB77" s="27" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="78" spans="1:28" ht="14.25">
@@ -15505,11 +15509,9 @@
       <c r="S78" s="1">
         <v>1000</v>
       </c>
-      <c r="T78" s="7" t="s">
+      <c r="T78" s="45"/>
+      <c r="U78" s="7" t="s">
         <v>715</v>
-      </c>
-      <c r="U78" s="7" t="s">
-        <v>716</v>
       </c>
       <c r="V78" s="1" t="s">
         <v>104</v>
@@ -15528,7 +15530,7 @@
         <v>0</v>
       </c>
       <c r="AB78" s="27" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="79" spans="1:28" ht="48">
@@ -15592,10 +15594,10 @@
         <v>2400</v>
       </c>
       <c r="T79" s="12" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="U79" s="7" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="V79" s="1" t="s">
         <v>128</v>
@@ -15616,7 +15618,7 @@
         <v>0</v>
       </c>
       <c r="AB79" s="27" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="80" spans="1:28" ht="60">
@@ -15680,7 +15682,7 @@
         <v>2000</v>
       </c>
       <c r="T80" s="12" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="U80" s="7" t="s">
         <v>525</v>
@@ -15704,7 +15706,7 @@
         <v>0</v>
       </c>
       <c r="AB80" s="27" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="81" spans="1:28" ht="60">
@@ -15768,7 +15770,7 @@
         <v>1800</v>
       </c>
       <c r="T81" s="12" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="U81" s="7" t="s">
         <v>531</v>
@@ -15792,7 +15794,7 @@
         <v>0</v>
       </c>
       <c r="AB81" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="82" spans="1:28" ht="24">
@@ -15856,10 +15858,10 @@
         <v>2400</v>
       </c>
       <c r="T82" s="12" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="U82" s="7" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="V82" s="1" t="s">
         <v>133</v>
@@ -15878,7 +15880,7 @@
         <v>0</v>
       </c>
       <c r="AB82" s="27" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="83" spans="1:28" ht="24">
@@ -15886,7 +15888,7 @@
         <v>53000083</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>306</v>
@@ -15942,13 +15944,13 @@
         <v>1200</v>
       </c>
       <c r="T83" s="12" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="U83" s="7" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="V83" s="1" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="W83" s="1"/>
       <c r="X83" s="1">
@@ -15964,7 +15966,7 @@
         <v>0</v>
       </c>
       <c r="AB83" s="27" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="84" spans="1:28" ht="24">
@@ -16028,13 +16030,13 @@
         <v>800</v>
       </c>
       <c r="T84" s="12" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="U84" s="7" t="s">
         <v>566</v>
       </c>
       <c r="V84" s="1" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="W84" s="1"/>
       <c r="X84" s="1">
@@ -16050,7 +16052,7 @@
         <v>0</v>
       </c>
       <c r="AB84" s="27" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="85" spans="1:28" ht="60">
@@ -16114,7 +16116,7 @@
         <v>2000</v>
       </c>
       <c r="T85" s="12" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="U85" s="7" t="s">
         <v>532</v>
@@ -16138,7 +16140,7 @@
         <v>0</v>
       </c>
       <c r="AB85" s="27" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="86" spans="1:28" ht="14.25">
@@ -16222,7 +16224,7 @@
         <v>0</v>
       </c>
       <c r="AB86" s="27" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="87" spans="1:28" ht="60">
@@ -16286,7 +16288,7 @@
         <v>1500</v>
       </c>
       <c r="T87" s="12" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="U87" s="7" t="s">
         <v>667</v>
@@ -16310,7 +16312,7 @@
         <v>0</v>
       </c>
       <c r="AB87" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="88" spans="1:28" ht="60">
@@ -16374,7 +16376,7 @@
         <v>1750</v>
       </c>
       <c r="T88" s="12" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="U88" s="7" t="s">
         <v>533</v>
@@ -16398,7 +16400,7 @@
         <v>0</v>
       </c>
       <c r="AB88" s="27" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="89" spans="1:28" ht="60">
@@ -16462,13 +16464,13 @@
         <v>1800</v>
       </c>
       <c r="T89" s="12" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="U89" s="7" t="s">
         <v>529</v>
       </c>
       <c r="V89" s="1" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="W89" s="1" t="s">
         <v>142</v>
@@ -16486,7 +16488,7 @@
         <v>0</v>
       </c>
       <c r="AB89" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="90" spans="1:28" ht="60">
@@ -16550,7 +16552,7 @@
         <v>1650</v>
       </c>
       <c r="T90" s="12" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="U90" s="7" t="s">
         <v>690</v>
@@ -16574,7 +16576,7 @@
         <v>0</v>
       </c>
       <c r="AB90" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="91" spans="1:28" ht="36">
@@ -16660,7 +16662,7 @@
         <v>0</v>
       </c>
       <c r="AB91" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="92" spans="1:28" ht="60">
@@ -16724,7 +16726,7 @@
         <v>1500</v>
       </c>
       <c r="T92" s="12" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="U92" s="7" t="s">
         <v>535</v>
@@ -16748,7 +16750,7 @@
         <v>0</v>
       </c>
       <c r="AB92" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="93" spans="1:28" ht="48">
@@ -16834,7 +16836,7 @@
         <v>0</v>
       </c>
       <c r="AB93" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="94" spans="1:28" ht="36">
@@ -16920,7 +16922,7 @@
         <v>0</v>
       </c>
       <c r="AB94" s="27" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="95" spans="1:28" ht="48">
@@ -16984,7 +16986,7 @@
         <v>1600</v>
       </c>
       <c r="T95" s="12" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="U95" s="7" t="s">
         <v>568</v>
@@ -17008,7 +17010,7 @@
         <v>0</v>
       </c>
       <c r="AB95" s="27" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="96" spans="1:28" ht="24">
@@ -17094,7 +17096,7 @@
         <v>0</v>
       </c>
       <c r="AB96" s="27" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="97" spans="1:28" ht="60">
@@ -17158,7 +17160,7 @@
         <v>900</v>
       </c>
       <c r="T97" s="12" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="U97" s="7" t="s">
         <v>526</v>
@@ -17182,7 +17184,7 @@
         <v>0</v>
       </c>
       <c r="AB97" s="27" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="98" spans="1:28" ht="24">
@@ -17268,7 +17270,7 @@
         <v>0</v>
       </c>
       <c r="AB98" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="99" spans="1:28" ht="24">
@@ -17354,7 +17356,7 @@
         <v>0</v>
       </c>
       <c r="AB99" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="100" spans="1:28" ht="24">
@@ -17440,7 +17442,7 @@
         <v>0</v>
       </c>
       <c r="AB100" s="27" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="101" spans="1:28" ht="48">
@@ -17526,7 +17528,7 @@
         <v>0</v>
       </c>
       <c r="AB101" s="27" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="102" spans="1:28" ht="24">
@@ -17612,7 +17614,7 @@
         <v>0</v>
       </c>
       <c r="AB102" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="103" spans="1:28" ht="60">
@@ -17676,10 +17678,10 @@
         <v>1300</v>
       </c>
       <c r="T103" s="12" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="U103" s="7" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="V103" s="1" t="s">
         <v>162</v>
@@ -17700,7 +17702,7 @@
         <v>0</v>
       </c>
       <c r="AB103" s="27" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="104" spans="1:28" ht="14.25">
@@ -17784,7 +17786,7 @@
         <v>0</v>
       </c>
       <c r="AB104" s="27" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="105" spans="1:28" ht="36">
@@ -17870,7 +17872,7 @@
         <v>0</v>
       </c>
       <c r="AB105" s="27" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="106" spans="1:28" ht="24">
@@ -17934,7 +17936,7 @@
         <v>1800</v>
       </c>
       <c r="T106" s="12" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="U106" s="7" t="s">
         <v>701</v>
@@ -17956,7 +17958,7 @@
         <v>0</v>
       </c>
       <c r="AB106" s="27" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="107" spans="1:28" ht="24">
@@ -18020,7 +18022,7 @@
         <v>1800</v>
       </c>
       <c r="T107" s="12" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="U107" s="7" t="s">
         <v>560</v>
@@ -18042,7 +18044,7 @@
         <v>0</v>
       </c>
       <c r="AB107" s="27" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="108" spans="1:28" ht="120">
@@ -18106,7 +18108,7 @@
         <v>1700</v>
       </c>
       <c r="T108" s="12" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="U108" s="7" t="s">
         <v>527</v>
@@ -18128,7 +18130,7 @@
         <v>0</v>
       </c>
       <c r="AB108" s="27" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="109" spans="1:28" ht="24">
@@ -18214,7 +18216,7 @@
         <v>0</v>
       </c>
       <c r="AB109" s="27" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="110" spans="1:28" ht="36">
@@ -18300,7 +18302,7 @@
         <v>0</v>
       </c>
       <c r="AB110" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="111" spans="1:28" ht="48">
@@ -18364,7 +18366,7 @@
         <v>1600</v>
       </c>
       <c r="T111" s="12" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="U111" s="7" t="s">
         <v>541</v>
@@ -18386,7 +18388,7 @@
         <v>0</v>
       </c>
       <c r="AB111" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="112" spans="1:28" ht="24">
@@ -18472,7 +18474,7 @@
         <v>0</v>
       </c>
       <c r="AB112" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="113" spans="1:28" ht="24">
@@ -18536,7 +18538,7 @@
         <v>1400</v>
       </c>
       <c r="T113" s="12" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="U113" s="7" t="s">
         <v>709</v>
@@ -18558,7 +18560,7 @@
         <v>0</v>
       </c>
       <c r="AB113" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="114" spans="1:28" ht="24">
@@ -18644,7 +18646,7 @@
         <v>0</v>
       </c>
       <c r="AB114" s="27" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="115" spans="1:28" ht="36">
@@ -18730,7 +18732,7 @@
         <v>0</v>
       </c>
       <c r="AB115" s="27" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="116" spans="1:28" ht="36">
@@ -18816,7 +18818,7 @@
         <v>0</v>
       </c>
       <c r="AB116" s="27" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="117" spans="1:28" ht="48">
@@ -18902,7 +18904,7 @@
         <v>0</v>
       </c>
       <c r="AB117" s="27" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="118" spans="1:28" ht="48">
@@ -18988,7 +18990,7 @@
         <v>0</v>
       </c>
       <c r="AB118" s="27" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="119" spans="1:28" ht="48">
@@ -19074,7 +19076,7 @@
         <v>0</v>
       </c>
       <c r="AB119" s="27" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="120" spans="1:28" ht="48">
@@ -19160,7 +19162,7 @@
         <v>0</v>
       </c>
       <c r="AB120" s="27" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="121" spans="1:28" ht="48">
@@ -19246,7 +19248,7 @@
         <v>0</v>
       </c>
       <c r="AB121" s="27" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="122" spans="1:28" ht="48">
@@ -19332,7 +19334,7 @@
         <v>0</v>
       </c>
       <c r="AB122" s="27" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="123" spans="1:28" ht="48">
@@ -19418,7 +19420,7 @@
         <v>0</v>
       </c>
       <c r="AB123" s="27" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="124" spans="1:28" ht="48">
@@ -19504,7 +19506,7 @@
         <v>0</v>
       </c>
       <c r="AB124" s="27" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="125" spans="1:28" ht="48">
@@ -19590,7 +19592,7 @@
         <v>0</v>
       </c>
       <c r="AB125" s="27" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="126" spans="1:28" ht="72">
@@ -19654,16 +19656,16 @@
         <v>2200</v>
       </c>
       <c r="T126" s="12" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="U126" s="7" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="V126" s="1" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="W126" s="1" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="X126" s="1">
         <v>4</v>
@@ -19678,7 +19680,7 @@
         <v>1</v>
       </c>
       <c r="AB126" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="127" spans="1:28" ht="48">
@@ -19742,7 +19744,7 @@
         <v>3000</v>
       </c>
       <c r="T127" s="12" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="U127" s="7" t="s">
         <v>569</v>
@@ -19766,7 +19768,7 @@
         <v>1</v>
       </c>
       <c r="AB127" s="27" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="128" spans="1:28" ht="36">
@@ -19852,7 +19854,7 @@
         <v>1</v>
       </c>
       <c r="AB128" s="27" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
   </sheetData>
@@ -20015,7 +20017,7 @@
         <v>214</v>
       </c>
       <c r="H1" s="40" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>490</v>
@@ -20039,7 +20041,7 @@
         <v>504</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="Q1" s="14" t="s">
         <v>487</v>
@@ -20060,7 +20062,7 @@
         <v>656</v>
       </c>
       <c r="W1" s="14" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="X1" s="14" t="s">
         <v>215</v>
@@ -20125,7 +20127,7 @@
         <v>491</v>
       </c>
       <c r="P2" s="19" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>488</v>
@@ -20146,7 +20148,7 @@
         <v>201</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="X2" s="4" t="s">
         <v>200</v>
@@ -20187,7 +20189,7 @@
         <v>206</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>492</v>
@@ -20211,7 +20213,7 @@
         <v>506</v>
       </c>
       <c r="P3" s="42" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>489</v>
@@ -20232,7 +20234,7 @@
         <v>494</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="X3" s="2" t="s">
         <v>208</v>
@@ -20707,7 +20709,7 @@
         <v>-1</v>
       </c>
       <c r="T9" s="12" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="U9" s="7" t="s">
         <v>639</v>
@@ -20873,7 +20875,7 @@
         <v>214</v>
       </c>
       <c r="H1" s="40" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>490</v>
@@ -20897,7 +20899,7 @@
         <v>504</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="Q1" s="14" t="s">
         <v>487</v>
@@ -20918,7 +20920,7 @@
         <v>656</v>
       </c>
       <c r="W1" s="14" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="X1" s="14" t="s">
         <v>215</v>
@@ -20983,7 +20985,7 @@
         <v>491</v>
       </c>
       <c r="P2" s="19" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>488</v>
@@ -21004,7 +21006,7 @@
         <v>201</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="X2" s="4" t="s">
         <v>200</v>
@@ -21045,7 +21047,7 @@
         <v>206</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>492</v>
@@ -21069,7 +21071,7 @@
         <v>506</v>
       </c>
       <c r="P3" s="42" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>489</v>
@@ -21090,7 +21092,7 @@
         <v>494</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="X3" s="2" t="s">
         <v>208</v>
@@ -21113,13 +21115,13 @@
         <v>53200100</v>
       </c>
       <c r="B4" s="24" t="s">
+        <v>746</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>747</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="D4" s="8" t="s">
         <v>748</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>749</v>
       </c>
       <c r="E4" s="16">
         <v>3</v>
@@ -21169,7 +21171,7 @@
         <v>2300</v>
       </c>
       <c r="T4" s="12" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="U4" s="7" t="s">
         <v>644</v>
@@ -21191,7 +21193,7 @@
         <v>0</v>
       </c>
       <c r="AB4" s="27" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="24">
@@ -21199,13 +21201,13 @@
         <v>53200101</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>737</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="8" t="s">
         <v>739</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>740</v>
       </c>
       <c r="E5" s="16">
         <v>3</v>
@@ -21255,7 +21257,7 @@
         <v>1800</v>
       </c>
       <c r="T5" s="12" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="U5" s="7" t="s">
         <v>654</v>
@@ -21277,7 +21279,7 @@
         <v>0</v>
       </c>
       <c r="AB5" s="27" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="40.5">
@@ -21285,13 +21287,13 @@
         <v>53200102</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>749</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>750</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="8" t="s">
         <v>751</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>752</v>
       </c>
       <c r="E6" s="16">
         <v>3</v>
@@ -21341,10 +21343,10 @@
         <v>2300</v>
       </c>
       <c r="T6" s="12" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="U6" s="34" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="V6" s="1" t="s">
         <v>53</v>
@@ -21363,7 +21365,7 @@
         <v>0</v>
       </c>
       <c r="AB6" s="27" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="14.25">
@@ -21371,13 +21373,13 @@
         <v>53200103</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>741</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>742</v>
       </c>
       <c r="E7" s="16">
         <v>3</v>
@@ -21428,7 +21430,7 @@
       </c>
       <c r="T7" s="12"/>
       <c r="U7" s="34" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="V7" s="1" t="s">
         <v>52</v>
@@ -21447,7 +21449,7 @@
         <v>0</v>
       </c>
       <c r="AB7" s="27" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="60">
@@ -21455,13 +21457,13 @@
         <v>53200104</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>757</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>758</v>
       </c>
       <c r="E8" s="16">
         <v>3</v>
@@ -21511,16 +21513,16 @@
         <v>1800</v>
       </c>
       <c r="T8" s="12" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="U8" s="7" t="s">
         <v>666</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="X8" s="1">
         <v>4</v>
@@ -21535,7 +21537,7 @@
         <v>0</v>
       </c>
       <c r="AB8" s="27" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="9" spans="1:28" ht="24">
@@ -21543,13 +21545,13 @@
         <v>53200105</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>759</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>760</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="8" t="s">
         <v>761</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>762</v>
       </c>
       <c r="E9" s="16">
         <v>3</v>
@@ -21599,7 +21601,7 @@
         <v>8000</v>
       </c>
       <c r="T9" s="12" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="U9" s="7" t="s">
         <v>509</v>
@@ -21621,7 +21623,7 @@
         <v>0</v>
       </c>
       <c r="AB9" s="27" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
   </sheetData>
@@ -21793,12 +21795,12 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B2">
         <f>COUNTIF(标准!AB:AB,"*单伤*")</f>
@@ -21807,7 +21809,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B3">
         <f>COUNTIF(标准!AB:AB,"*群伤*")</f>
@@ -21816,7 +21818,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B4">
         <f>COUNTIF(标准!AB:AB,"*单治*")</f>
@@ -21825,7 +21827,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B5">
         <f>COUNTIF(标准!AB:AB,"*群治*")</f>
@@ -21834,7 +21836,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B6">
         <f>COUNTIF(标准!AB:AB,"*正状*")</f>
@@ -21843,7 +21845,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B7">
         <f>COUNTIF(标准!AB:AB,"*负状*")</f>
@@ -21852,7 +21854,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B8">
         <f>COUNTIF(标准!AB:AB,"*手牌*")</f>
@@ -21861,7 +21863,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B9">
         <f>COUNTIF(标准!AB:AB,"*过牌*")</f>
@@ -21870,7 +21872,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B10">
         <f>COUNTIF(标准!AB:AB,"*陷阱*")</f>
@@ -21879,7 +21881,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B11">
         <f>COUNTIF(标准!AB:AB,"*地形*")</f>
@@ -21888,7 +21890,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B12">
         <f>COUNTIF(标准!AB:AB,"*属性*")</f>

</xml_diff>

<commit_message>
#23 autoremoved spike accomplish
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -717,7 +717,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="881">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="883">
   <si>
     <t>慈悲</t>
   </si>
@@ -3126,10 +3126,6 @@
   </si>
   <si>
     <t>使目标减速{3:0}%</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>己方召唤师使用魔法/武器卡消耗+2，使用怪物卡消耗-2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -3780,6 +3776,18 @@
   </si>
   <si>
     <t>if(MathTool.GetRandom(100)&lt;s.Rate) p.AddCard(s.Id, s.Level);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>下一张使用的怪物卡消耗为0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>p.AddSpike(57000006);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NFN</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -8795,7 +8803,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P77" sqref="P77"/>
+      <selection pane="bottomRight" activeCell="R78" sqref="R78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -8842,7 +8850,7 @@
         <v>214</v>
       </c>
       <c r="H1" s="40" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>490</v>
@@ -8866,7 +8874,7 @@
         <v>504</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="Q1" s="14" t="s">
         <v>487</v>
@@ -8887,7 +8895,7 @@
         <v>656</v>
       </c>
       <c r="W1" s="14" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="X1" s="14" t="s">
         <v>215</v>
@@ -8952,7 +8960,7 @@
         <v>505</v>
       </c>
       <c r="P2" s="19" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>488</v>
@@ -8964,7 +8972,7 @@
         <v>658</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="U2" s="11" t="s">
         <v>201</v>
@@ -8973,7 +8981,7 @@
         <v>201</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="X2" s="4" t="s">
         <v>200</v>
@@ -9014,7 +9022,7 @@
         <v>206</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>492</v>
@@ -9038,19 +9046,19 @@
         <v>506</v>
       </c>
       <c r="P3" s="42" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>489</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>659</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="U3" s="6" t="s">
         <v>470</v>
@@ -9059,7 +9067,7 @@
         <v>494</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="X3" s="2" t="s">
         <v>208</v>
@@ -9138,7 +9146,7 @@
         <v>1704</v>
       </c>
       <c r="T4" s="12" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="U4" s="33" t="s">
         <v>581</v>
@@ -9160,7 +9168,7 @@
         <v>0</v>
       </c>
       <c r="AB4" s="27" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="14.25">
@@ -9246,7 +9254,7 @@
         <v>0</v>
       </c>
       <c r="AB5" s="27" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="24">
@@ -9310,7 +9318,7 @@
         <v>2000</v>
       </c>
       <c r="T6" s="12" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="U6" s="7" t="s">
         <v>654</v>
@@ -9332,7 +9340,7 @@
         <v>0</v>
       </c>
       <c r="AB6" s="27" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="36">
@@ -9396,7 +9404,7 @@
         <v>2000</v>
       </c>
       <c r="T7" s="12" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="U7" s="7" t="s">
         <v>655</v>
@@ -9418,7 +9426,7 @@
         <v>0</v>
       </c>
       <c r="AB7" s="27" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="24">
@@ -9482,7 +9490,7 @@
         <v>900</v>
       </c>
       <c r="T8" s="12" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="U8" s="7" t="s">
         <v>546</v>
@@ -9504,7 +9512,7 @@
         <v>0</v>
       </c>
       <c r="AB8" s="27" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="9" spans="1:28" ht="48">
@@ -9590,7 +9598,7 @@
         <v>0</v>
       </c>
       <c r="AB9" s="27" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="10" spans="1:28" ht="48">
@@ -9676,7 +9684,7 @@
         <v>0</v>
       </c>
       <c r="AB10" s="27" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="48">
@@ -9762,7 +9770,7 @@
         <v>0</v>
       </c>
       <c r="AB11" s="27" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="12" spans="1:28" ht="48">
@@ -9848,7 +9856,7 @@
         <v>0</v>
       </c>
       <c r="AB12" s="27" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="48">
@@ -9934,7 +9942,7 @@
         <v>0</v>
       </c>
       <c r="AB13" s="27" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="48">
@@ -10020,7 +10028,7 @@
         <v>0</v>
       </c>
       <c r="AB14" s="27" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="15" spans="1:28" ht="48">
@@ -10106,7 +10114,7 @@
         <v>0</v>
       </c>
       <c r="AB15" s="27" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="48">
@@ -10192,7 +10200,7 @@
         <v>0</v>
       </c>
       <c r="AB16" s="27" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="17" spans="1:28" ht="48">
@@ -10278,7 +10286,7 @@
         <v>0</v>
       </c>
       <c r="AB17" s="27" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="18" spans="1:28" ht="14.25">
@@ -10364,7 +10372,7 @@
         <v>0</v>
       </c>
       <c r="AB18" s="27" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="19" spans="1:28" ht="24">
@@ -10428,7 +10436,7 @@
         <v>1200</v>
       </c>
       <c r="T19" s="12" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="U19" s="7" t="s">
         <v>508</v>
@@ -10450,7 +10458,7 @@
         <v>0</v>
       </c>
       <c r="AB19" s="27" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="20" spans="1:28" ht="24">
@@ -10514,7 +10522,7 @@
         <v>8000</v>
       </c>
       <c r="T20" s="12" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="U20" s="7" t="s">
         <v>509</v>
@@ -10536,7 +10544,7 @@
         <v>0</v>
       </c>
       <c r="AB20" s="27" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="21" spans="1:28" ht="48">
@@ -10622,7 +10630,7 @@
         <v>0</v>
       </c>
       <c r="AB21" s="27" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="22" spans="1:28" ht="60">
@@ -10686,7 +10694,7 @@
         <v>1800</v>
       </c>
       <c r="T22" s="12" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="U22" s="7" t="s">
         <v>666</v>
@@ -10710,7 +10718,7 @@
         <v>0</v>
       </c>
       <c r="AB22" s="27" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="23" spans="1:28" ht="60">
@@ -10774,7 +10782,7 @@
         <v>2100</v>
       </c>
       <c r="T23" s="12" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="U23" s="7" t="s">
         <v>667</v>
@@ -10798,7 +10806,7 @@
         <v>0</v>
       </c>
       <c r="AB23" s="27" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="24" spans="1:28" ht="60">
@@ -10862,7 +10870,7 @@
         <v>1875</v>
       </c>
       <c r="T24" s="12" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="U24" s="7" t="s">
         <v>668</v>
@@ -10886,7 +10894,7 @@
         <v>0</v>
       </c>
       <c r="AB24" s="27" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="25" spans="1:28" ht="24">
@@ -10972,7 +10980,7 @@
         <v>0</v>
       </c>
       <c r="AB25" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="26" spans="1:28" ht="24">
@@ -11058,7 +11066,7 @@
         <v>0</v>
       </c>
       <c r="AB26" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="27" spans="1:28" ht="24">
@@ -11144,7 +11152,7 @@
         <v>0</v>
       </c>
       <c r="AB27" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="28" spans="1:28" ht="48">
@@ -11230,7 +11238,7 @@
         <v>0</v>
       </c>
       <c r="AB28" s="27" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="29" spans="1:28" ht="24">
@@ -11316,7 +11324,7 @@
         <v>0</v>
       </c>
       <c r="AB29" s="27" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="30" spans="1:28" ht="14.25">
@@ -11400,7 +11408,7 @@
         <v>0</v>
       </c>
       <c r="AB30" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="31" spans="1:28" ht="14.25">
@@ -11484,7 +11492,7 @@
         <v>0</v>
       </c>
       <c r="AB31" s="27" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="32" spans="1:28" ht="24">
@@ -11570,7 +11578,7 @@
         <v>0</v>
       </c>
       <c r="AB32" s="27" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="33" spans="1:28" ht="24">
@@ -11578,13 +11586,13 @@
         <v>53000030</v>
       </c>
       <c r="B33" s="9" t="s">
+        <v>773</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>774</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>775</v>
-      </c>
       <c r="D33" s="8" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="E33" s="1">
         <v>2</v>
@@ -11634,10 +11642,10 @@
         <v>1500</v>
       </c>
       <c r="T33" s="12" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="U33" s="1" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="V33" s="1" t="s">
         <v>4</v>
@@ -11656,7 +11664,7 @@
         <v>1</v>
       </c>
       <c r="AB33" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="34" spans="1:28" ht="24">
@@ -11664,13 +11672,13 @@
         <v>53000031</v>
       </c>
       <c r="B34" s="9" t="s">
+        <v>776</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>777</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>778</v>
-      </c>
       <c r="D34" s="8" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="E34" s="1">
         <v>2</v>
@@ -11720,10 +11728,10 @@
         <v>1500</v>
       </c>
       <c r="T34" s="12" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="U34" s="1" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="V34" s="1" t="s">
         <v>4</v>
@@ -11742,7 +11750,7 @@
         <v>1</v>
       </c>
       <c r="AB34" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="35" spans="1:28" ht="48">
@@ -11806,7 +11814,7 @@
         <v>2000</v>
       </c>
       <c r="T35" s="12" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="U35" s="7" t="s">
         <v>513</v>
@@ -11828,7 +11836,7 @@
         <v>0</v>
       </c>
       <c r="AB35" s="27" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="36" spans="1:28" ht="36">
@@ -11893,7 +11901,7 @@
         <v>1220</v>
       </c>
       <c r="T36" s="12" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="U36" s="1" t="s">
         <v>679</v>
@@ -11915,7 +11923,7 @@
         <v>0</v>
       </c>
       <c r="AB36" s="27" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="37" spans="1:28" ht="14.25">
@@ -11999,7 +12007,7 @@
         <v>0</v>
       </c>
       <c r="AB37" s="27" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="38" spans="1:28" ht="14.25">
@@ -12064,7 +12072,7 @@
       </c>
       <c r="T38" s="12"/>
       <c r="U38" s="7" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="V38" s="1" t="s">
         <v>63</v>
@@ -12083,7 +12091,7 @@
         <v>0</v>
       </c>
       <c r="AB38" s="27" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="39" spans="1:28" ht="24">
@@ -12091,10 +12099,10 @@
         <v>53000039</v>
       </c>
       <c r="B39" s="9" t="s">
+        <v>767</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>768</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>769</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>374</v>
@@ -12147,10 +12155,10 @@
         <v>1700</v>
       </c>
       <c r="T39" s="12" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="U39" s="1" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="V39" s="1" t="s">
         <v>4</v>
@@ -12169,7 +12177,7 @@
         <v>0</v>
       </c>
       <c r="AB39" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="40" spans="1:28" ht="24">
@@ -12177,7 +12185,7 @@
         <v>53000040</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>270</v>
@@ -12233,10 +12241,10 @@
         <v>2000</v>
       </c>
       <c r="T40" s="12" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="U40" s="1" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="V40" s="1" t="s">
         <v>4</v>
@@ -12255,7 +12263,7 @@
         <v>0</v>
       </c>
       <c r="AB40" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="41" spans="1:28" ht="24">
@@ -12341,7 +12349,7 @@
         <v>0</v>
       </c>
       <c r="AB41" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="42" spans="1:28" ht="48">
@@ -12405,7 +12413,7 @@
         <v>2000</v>
       </c>
       <c r="T42" s="12" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="U42" s="1" t="s">
         <v>514</v>
@@ -12427,7 +12435,7 @@
         <v>0</v>
       </c>
       <c r="AB42" s="27" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="43" spans="1:28" ht="24">
@@ -12513,7 +12521,7 @@
         <v>0</v>
       </c>
       <c r="AB43" s="27" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="44" spans="1:28" ht="24">
@@ -12521,7 +12529,7 @@
         <v>53000044</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>274</v>
@@ -12577,10 +12585,10 @@
         <v>1900</v>
       </c>
       <c r="T44" s="12" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="U44" s="1" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="V44" s="1" t="s">
         <v>4</v>
@@ -12599,7 +12607,7 @@
         <v>0</v>
       </c>
       <c r="AB44" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="45" spans="1:28" ht="60">
@@ -12686,7 +12694,7 @@
         <v>0</v>
       </c>
       <c r="AB45" s="27" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="46" spans="1:28" ht="48">
@@ -12750,7 +12758,7 @@
         <v>2000</v>
       </c>
       <c r="T46" s="12" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="U46" s="7" t="s">
         <v>528</v>
@@ -12772,7 +12780,7 @@
         <v>0</v>
       </c>
       <c r="AB46" s="27" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="47" spans="1:28" ht="60">
@@ -12836,7 +12844,7 @@
         <v>2200</v>
       </c>
       <c r="T47" s="12" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="U47" s="7" t="s">
         <v>529</v>
@@ -12860,7 +12868,7 @@
         <v>0</v>
       </c>
       <c r="AB47" s="27" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="48" spans="1:28" ht="48">
@@ -12924,7 +12932,7 @@
         <v>2000</v>
       </c>
       <c r="T48" s="12" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="U48" s="1" t="s">
         <v>515</v>
@@ -12946,7 +12954,7 @@
         <v>0</v>
       </c>
       <c r="AB48" s="27" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="49" spans="1:28" ht="60">
@@ -13010,7 +13018,7 @@
         <v>2200</v>
       </c>
       <c r="T49" s="12" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="U49" s="7" t="s">
         <v>530</v>
@@ -13034,7 +13042,7 @@
         <v>0</v>
       </c>
       <c r="AB49" s="27" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="50" spans="1:28" ht="72">
@@ -13098,7 +13106,7 @@
         <v>1800</v>
       </c>
       <c r="T50" s="12" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="U50" s="7" t="s">
         <v>685</v>
@@ -13120,7 +13128,7 @@
         <v>0</v>
       </c>
       <c r="AB50" s="27" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="51" spans="1:28" ht="48">
@@ -13184,7 +13192,7 @@
         <v>2000</v>
       </c>
       <c r="T51" s="12" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="U51" s="1" t="s">
         <v>516</v>
@@ -13206,7 +13214,7 @@
         <v>0</v>
       </c>
       <c r="AB51" s="27" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="52" spans="1:28" ht="48">
@@ -13270,7 +13278,7 @@
         <v>2000</v>
       </c>
       <c r="T52" s="12" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="U52" s="1" t="s">
         <v>517</v>
@@ -13292,7 +13300,7 @@
         <v>0</v>
       </c>
       <c r="AB52" s="27" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="53" spans="1:28" ht="48">
@@ -13356,7 +13364,7 @@
         <v>2000</v>
       </c>
       <c r="T53" s="12" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="U53" s="1" t="s">
         <v>518</v>
@@ -13378,7 +13386,7 @@
         <v>0</v>
       </c>
       <c r="AB53" s="27" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="54" spans="1:28" ht="48">
@@ -13442,7 +13450,7 @@
         <v>1670</v>
       </c>
       <c r="T54" s="12" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="U54" s="7" t="s">
         <v>619</v>
@@ -13464,7 +13472,7 @@
         <v>0</v>
       </c>
       <c r="AB54" s="27" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="55" spans="1:28" ht="24">
@@ -13550,7 +13558,7 @@
         <v>0</v>
       </c>
       <c r="AB55" s="27" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="56" spans="1:28" ht="36">
@@ -13636,7 +13644,7 @@
         <v>0</v>
       </c>
       <c r="AB56" s="27" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="57" spans="1:28" ht="24">
@@ -13722,7 +13730,7 @@
         <v>0</v>
       </c>
       <c r="AB57" s="27" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="58" spans="1:28" ht="24">
@@ -13786,7 +13794,7 @@
         <v>1800</v>
       </c>
       <c r="T58" s="12" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="U58" s="7" t="s">
         <v>519</v>
@@ -13808,7 +13816,7 @@
         <v>0</v>
       </c>
       <c r="AB58" s="27" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="59" spans="1:28" ht="24">
@@ -13872,7 +13880,7 @@
         <v>560</v>
       </c>
       <c r="T59" s="12" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="U59" s="7" t="s">
         <v>579</v>
@@ -13894,7 +13902,7 @@
         <v>0</v>
       </c>
       <c r="AB59" s="27" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="60" spans="1:28" ht="36">
@@ -13980,7 +13988,7 @@
         <v>0</v>
       </c>
       <c r="AB60" s="27" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="61" spans="1:28" ht="48">
@@ -14044,7 +14052,7 @@
         <v>3000</v>
       </c>
       <c r="T61" s="12" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="U61" s="7" t="s">
         <v>570</v>
@@ -14066,7 +14074,7 @@
         <v>0</v>
       </c>
       <c r="AB61" s="27" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="62" spans="1:28" ht="24">
@@ -14130,7 +14138,7 @@
         <v>3000</v>
       </c>
       <c r="T62" s="12" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="U62" s="7" t="s">
         <v>520</v>
@@ -14152,7 +14160,7 @@
         <v>0</v>
       </c>
       <c r="AB62" s="27" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="63" spans="1:28" ht="14.25">
@@ -14238,7 +14246,7 @@
         <v>0</v>
       </c>
       <c r="AB63" s="27" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="64" spans="1:28" ht="24">
@@ -14302,7 +14310,7 @@
         <v>1500</v>
       </c>
       <c r="T64" s="12" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="U64" s="1" t="s">
         <v>686</v>
@@ -14324,7 +14332,7 @@
         <v>0</v>
       </c>
       <c r="AB64" s="27" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="65" spans="1:28" ht="48">
@@ -14388,7 +14396,7 @@
         <v>5000</v>
       </c>
       <c r="T65" s="12" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="U65" s="1" t="s">
         <v>710</v>
@@ -14410,7 +14418,7 @@
         <v>0</v>
       </c>
       <c r="AB65" s="27" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="66" spans="1:28" ht="24">
@@ -14474,10 +14482,10 @@
         <v>1700</v>
       </c>
       <c r="T66" s="12" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="U66" s="1" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="V66" s="1" t="s">
         <v>4</v>
@@ -14496,7 +14504,7 @@
         <v>0</v>
       </c>
       <c r="AB66" s="27" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="67" spans="1:28" ht="14.25">
@@ -14582,7 +14590,7 @@
         <v>0</v>
       </c>
       <c r="AB67" s="27" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="68" spans="1:28" ht="60">
@@ -14646,7 +14654,7 @@
         <v>1200</v>
       </c>
       <c r="T68" s="12" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="U68" s="7" t="s">
         <v>687</v>
@@ -14670,7 +14678,7 @@
         <v>0</v>
       </c>
       <c r="AB68" s="27" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="69" spans="1:28" ht="24">
@@ -14734,7 +14742,7 @@
         <v>2000</v>
       </c>
       <c r="T69" s="12" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="U69" s="7" t="s">
         <v>521</v>
@@ -14756,7 +14764,7 @@
         <v>0</v>
       </c>
       <c r="AB69" s="27" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="70" spans="1:28" ht="14.25">
@@ -14840,7 +14848,7 @@
         <v>0</v>
       </c>
       <c r="AB70" s="27" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="71" spans="1:28" ht="72">
@@ -14904,7 +14912,7 @@
         <v>2000</v>
       </c>
       <c r="T71" s="12" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="U71" s="7" t="s">
         <v>483</v>
@@ -14928,7 +14936,7 @@
         <v>0</v>
       </c>
       <c r="AB71" s="27" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="72" spans="1:28" ht="48">
@@ -14992,7 +15000,7 @@
         <v>4000</v>
       </c>
       <c r="T72" s="12" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="U72" s="1" t="s">
         <v>649</v>
@@ -15014,7 +15022,7 @@
         <v>0</v>
       </c>
       <c r="AB72" s="27" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="73" spans="1:28" ht="48">
@@ -15078,7 +15086,7 @@
         <v>1900</v>
       </c>
       <c r="T73" s="12" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="U73" s="7" t="s">
         <v>522</v>
@@ -15100,7 +15108,7 @@
         <v>0</v>
       </c>
       <c r="AB73" s="27" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="74" spans="1:28" ht="36">
@@ -15186,7 +15194,7 @@
         <v>0</v>
       </c>
       <c r="AB74" s="27" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="75" spans="1:28" ht="108">
@@ -15250,7 +15258,7 @@
         <v>3600</v>
       </c>
       <c r="T75" s="12" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="U75" s="7" t="s">
         <v>523</v>
@@ -15272,7 +15280,7 @@
         <v>0</v>
       </c>
       <c r="AB75" s="27" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="76" spans="1:28" ht="60">
@@ -15336,7 +15344,7 @@
         <v>2200</v>
       </c>
       <c r="T76" s="12" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="U76" s="7" t="s">
         <v>688</v>
@@ -15360,7 +15368,7 @@
         <v>0</v>
       </c>
       <c r="AB76" s="27" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="77" spans="1:28" ht="48">
@@ -15424,7 +15432,7 @@
         <v>1200</v>
       </c>
       <c r="T77" s="12" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="U77" s="7" t="s">
         <v>524</v>
@@ -15446,7 +15454,7 @@
         <v>0</v>
       </c>
       <c r="AB77" s="27" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="78" spans="1:28" ht="14.25">
@@ -15463,7 +15471,7 @@
         <v>411</v>
       </c>
       <c r="E78" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F78">
         <v>202</v>
@@ -15476,7 +15484,7 @@
         <v>6</v>
       </c>
       <c r="I78" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J78" s="1">
         <v>0</v>
@@ -15504,14 +15512,16 @@
         <v>0</v>
       </c>
       <c r="R78" s="1" t="s">
-        <v>1</v>
+        <v>882</v>
       </c>
       <c r="S78" s="1">
         <v>1000</v>
       </c>
-      <c r="T78" s="45"/>
+      <c r="T78" s="45" t="s">
+        <v>881</v>
+      </c>
       <c r="U78" s="7" t="s">
-        <v>715</v>
+        <v>880</v>
       </c>
       <c r="V78" s="1" t="s">
         <v>104</v>
@@ -15530,7 +15540,7 @@
         <v>0</v>
       </c>
       <c r="AB78" s="27" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="79" spans="1:28" ht="48">
@@ -15594,10 +15604,10 @@
         <v>2400</v>
       </c>
       <c r="T79" s="12" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="U79" s="7" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="V79" s="1" t="s">
         <v>128</v>
@@ -15618,7 +15628,7 @@
         <v>0</v>
       </c>
       <c r="AB79" s="27" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="80" spans="1:28" ht="60">
@@ -15682,7 +15692,7 @@
         <v>2000</v>
       </c>
       <c r="T80" s="12" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="U80" s="7" t="s">
         <v>525</v>
@@ -15706,7 +15716,7 @@
         <v>0</v>
       </c>
       <c r="AB80" s="27" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="81" spans="1:28" ht="60">
@@ -15770,7 +15780,7 @@
         <v>1800</v>
       </c>
       <c r="T81" s="12" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="U81" s="7" t="s">
         <v>531</v>
@@ -15794,7 +15804,7 @@
         <v>0</v>
       </c>
       <c r="AB81" s="27" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="82" spans="1:28" ht="24">
@@ -15858,10 +15868,10 @@
         <v>2400</v>
       </c>
       <c r="T82" s="12" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="U82" s="7" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="V82" s="1" t="s">
         <v>133</v>
@@ -15880,7 +15890,7 @@
         <v>0</v>
       </c>
       <c r="AB82" s="27" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="83" spans="1:28" ht="24">
@@ -15888,7 +15898,7 @@
         <v>53000083</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>306</v>
@@ -15944,13 +15954,13 @@
         <v>1200</v>
       </c>
       <c r="T83" s="12" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="U83" s="7" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="V83" s="1" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="W83" s="1"/>
       <c r="X83" s="1">
@@ -15966,7 +15976,7 @@
         <v>0</v>
       </c>
       <c r="AB83" s="27" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="84" spans="1:28" ht="24">
@@ -16030,13 +16040,13 @@
         <v>800</v>
       </c>
       <c r="T84" s="12" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="U84" s="7" t="s">
         <v>566</v>
       </c>
       <c r="V84" s="1" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="W84" s="1"/>
       <c r="X84" s="1">
@@ -16052,7 +16062,7 @@
         <v>0</v>
       </c>
       <c r="AB84" s="27" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="85" spans="1:28" ht="60">
@@ -16116,7 +16126,7 @@
         <v>2000</v>
       </c>
       <c r="T85" s="12" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="U85" s="7" t="s">
         <v>532</v>
@@ -16140,7 +16150,7 @@
         <v>0</v>
       </c>
       <c r="AB85" s="27" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="86" spans="1:28" ht="14.25">
@@ -16224,7 +16234,7 @@
         <v>0</v>
       </c>
       <c r="AB86" s="27" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="87" spans="1:28" ht="60">
@@ -16288,7 +16298,7 @@
         <v>1500</v>
       </c>
       <c r="T87" s="12" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="U87" s="7" t="s">
         <v>667</v>
@@ -16312,7 +16322,7 @@
         <v>0</v>
       </c>
       <c r="AB87" s="27" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="88" spans="1:28" ht="60">
@@ -16376,7 +16386,7 @@
         <v>1750</v>
       </c>
       <c r="T88" s="12" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="U88" s="7" t="s">
         <v>533</v>
@@ -16400,7 +16410,7 @@
         <v>0</v>
       </c>
       <c r="AB88" s="27" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="89" spans="1:28" ht="60">
@@ -16464,13 +16474,13 @@
         <v>1800</v>
       </c>
       <c r="T89" s="12" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="U89" s="7" t="s">
         <v>529</v>
       </c>
       <c r="V89" s="1" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="W89" s="1" t="s">
         <v>142</v>
@@ -16488,7 +16498,7 @@
         <v>0</v>
       </c>
       <c r="AB89" s="27" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="90" spans="1:28" ht="60">
@@ -16552,7 +16562,7 @@
         <v>1650</v>
       </c>
       <c r="T90" s="12" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="U90" s="7" t="s">
         <v>690</v>
@@ -16576,7 +16586,7 @@
         <v>0</v>
       </c>
       <c r="AB90" s="27" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="91" spans="1:28" ht="36">
@@ -16662,7 +16672,7 @@
         <v>0</v>
       </c>
       <c r="AB91" s="27" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="92" spans="1:28" ht="60">
@@ -16726,7 +16736,7 @@
         <v>1500</v>
       </c>
       <c r="T92" s="12" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="U92" s="7" t="s">
         <v>535</v>
@@ -16750,7 +16760,7 @@
         <v>0</v>
       </c>
       <c r="AB92" s="27" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="93" spans="1:28" ht="48">
@@ -16836,7 +16846,7 @@
         <v>0</v>
       </c>
       <c r="AB93" s="27" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="94" spans="1:28" ht="36">
@@ -16922,7 +16932,7 @@
         <v>0</v>
       </c>
       <c r="AB94" s="27" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="95" spans="1:28" ht="48">
@@ -16986,7 +16996,7 @@
         <v>1600</v>
       </c>
       <c r="T95" s="12" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="U95" s="7" t="s">
         <v>568</v>
@@ -17010,7 +17020,7 @@
         <v>0</v>
       </c>
       <c r="AB95" s="27" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="96" spans="1:28" ht="24">
@@ -17096,7 +17106,7 @@
         <v>0</v>
       </c>
       <c r="AB96" s="27" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="97" spans="1:28" ht="60">
@@ -17160,7 +17170,7 @@
         <v>900</v>
       </c>
       <c r="T97" s="12" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="U97" s="7" t="s">
         <v>526</v>
@@ -17184,7 +17194,7 @@
         <v>0</v>
       </c>
       <c r="AB97" s="27" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="98" spans="1:28" ht="24">
@@ -17270,7 +17280,7 @@
         <v>0</v>
       </c>
       <c r="AB98" s="27" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="99" spans="1:28" ht="24">
@@ -17356,7 +17366,7 @@
         <v>0</v>
       </c>
       <c r="AB99" s="27" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="100" spans="1:28" ht="24">
@@ -17442,7 +17452,7 @@
         <v>0</v>
       </c>
       <c r="AB100" s="27" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="101" spans="1:28" ht="48">
@@ -17528,7 +17538,7 @@
         <v>0</v>
       </c>
       <c r="AB101" s="27" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="102" spans="1:28" ht="24">
@@ -17614,7 +17624,7 @@
         <v>0</v>
       </c>
       <c r="AB102" s="27" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="103" spans="1:28" ht="60">
@@ -17678,10 +17688,10 @@
         <v>1300</v>
       </c>
       <c r="T103" s="12" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="U103" s="7" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="V103" s="1" t="s">
         <v>162</v>
@@ -17702,7 +17712,7 @@
         <v>0</v>
       </c>
       <c r="AB103" s="27" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="104" spans="1:28" ht="14.25">
@@ -17786,7 +17796,7 @@
         <v>0</v>
       </c>
       <c r="AB104" s="27" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="105" spans="1:28" ht="36">
@@ -17872,7 +17882,7 @@
         <v>0</v>
       </c>
       <c r="AB105" s="27" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="106" spans="1:28" ht="24">
@@ -17936,7 +17946,7 @@
         <v>1800</v>
       </c>
       <c r="T106" s="12" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="U106" s="7" t="s">
         <v>701</v>
@@ -17958,7 +17968,7 @@
         <v>0</v>
       </c>
       <c r="AB106" s="27" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="107" spans="1:28" ht="24">
@@ -18022,7 +18032,7 @@
         <v>1800</v>
       </c>
       <c r="T107" s="12" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="U107" s="7" t="s">
         <v>560</v>
@@ -18044,7 +18054,7 @@
         <v>0</v>
       </c>
       <c r="AB107" s="27" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="108" spans="1:28" ht="120">
@@ -18108,7 +18118,7 @@
         <v>1700</v>
       </c>
       <c r="T108" s="12" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="U108" s="7" t="s">
         <v>527</v>
@@ -18130,7 +18140,7 @@
         <v>0</v>
       </c>
       <c r="AB108" s="27" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="109" spans="1:28" ht="24">
@@ -18216,7 +18226,7 @@
         <v>0</v>
       </c>
       <c r="AB109" s="27" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="110" spans="1:28" ht="36">
@@ -18302,7 +18312,7 @@
         <v>0</v>
       </c>
       <c r="AB110" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="111" spans="1:28" ht="48">
@@ -18366,7 +18376,7 @@
         <v>1600</v>
       </c>
       <c r="T111" s="12" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="U111" s="7" t="s">
         <v>541</v>
@@ -18388,7 +18398,7 @@
         <v>0</v>
       </c>
       <c r="AB111" s="27" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="112" spans="1:28" ht="24">
@@ -18474,7 +18484,7 @@
         <v>0</v>
       </c>
       <c r="AB112" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="113" spans="1:28" ht="24">
@@ -18538,7 +18548,7 @@
         <v>1400</v>
       </c>
       <c r="T113" s="12" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="U113" s="7" t="s">
         <v>709</v>
@@ -18560,7 +18570,7 @@
         <v>0</v>
       </c>
       <c r="AB113" s="27" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="114" spans="1:28" ht="24">
@@ -18646,7 +18656,7 @@
         <v>0</v>
       </c>
       <c r="AB114" s="27" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="115" spans="1:28" ht="36">
@@ -18732,7 +18742,7 @@
         <v>0</v>
       </c>
       <c r="AB115" s="27" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="116" spans="1:28" ht="36">
@@ -18818,7 +18828,7 @@
         <v>0</v>
       </c>
       <c r="AB116" s="27" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="117" spans="1:28" ht="48">
@@ -18904,7 +18914,7 @@
         <v>0</v>
       </c>
       <c r="AB117" s="27" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="118" spans="1:28" ht="48">
@@ -18990,7 +19000,7 @@
         <v>0</v>
       </c>
       <c r="AB118" s="27" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="119" spans="1:28" ht="48">
@@ -19076,7 +19086,7 @@
         <v>0</v>
       </c>
       <c r="AB119" s="27" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="120" spans="1:28" ht="48">
@@ -19162,7 +19172,7 @@
         <v>0</v>
       </c>
       <c r="AB120" s="27" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="121" spans="1:28" ht="48">
@@ -19248,7 +19258,7 @@
         <v>0</v>
       </c>
       <c r="AB121" s="27" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="122" spans="1:28" ht="48">
@@ -19334,7 +19344,7 @@
         <v>0</v>
       </c>
       <c r="AB122" s="27" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="123" spans="1:28" ht="48">
@@ -19420,7 +19430,7 @@
         <v>0</v>
       </c>
       <c r="AB123" s="27" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="124" spans="1:28" ht="48">
@@ -19506,7 +19516,7 @@
         <v>0</v>
       </c>
       <c r="AB124" s="27" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="125" spans="1:28" ht="48">
@@ -19592,7 +19602,7 @@
         <v>0</v>
       </c>
       <c r="AB125" s="27" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="126" spans="1:28" ht="72">
@@ -19656,16 +19666,16 @@
         <v>2200</v>
       </c>
       <c r="T126" s="12" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="U126" s="7" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="V126" s="1" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="W126" s="1" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="X126" s="1">
         <v>4</v>
@@ -19680,7 +19690,7 @@
         <v>1</v>
       </c>
       <c r="AB126" s="27" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="127" spans="1:28" ht="48">
@@ -19744,7 +19754,7 @@
         <v>3000</v>
       </c>
       <c r="T127" s="12" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="U127" s="7" t="s">
         <v>569</v>
@@ -19768,7 +19778,7 @@
         <v>1</v>
       </c>
       <c r="AB127" s="27" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="128" spans="1:28" ht="36">
@@ -19854,7 +19864,7 @@
         <v>1</v>
       </c>
       <c r="AB128" s="27" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
   </sheetData>
@@ -20017,7 +20027,7 @@
         <v>214</v>
       </c>
       <c r="H1" s="40" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>490</v>
@@ -20041,7 +20051,7 @@
         <v>504</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="Q1" s="14" t="s">
         <v>487</v>
@@ -20062,7 +20072,7 @@
         <v>656</v>
       </c>
       <c r="W1" s="14" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="X1" s="14" t="s">
         <v>215</v>
@@ -20127,7 +20137,7 @@
         <v>491</v>
       </c>
       <c r="P2" s="19" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>488</v>
@@ -20148,7 +20158,7 @@
         <v>201</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="X2" s="4" t="s">
         <v>200</v>
@@ -20189,7 +20199,7 @@
         <v>206</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>492</v>
@@ -20213,7 +20223,7 @@
         <v>506</v>
       </c>
       <c r="P3" s="42" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>489</v>
@@ -20234,7 +20244,7 @@
         <v>494</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="X3" s="2" t="s">
         <v>208</v>
@@ -20709,7 +20719,7 @@
         <v>-1</v>
       </c>
       <c r="T9" s="12" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="U9" s="7" t="s">
         <v>639</v>
@@ -20875,7 +20885,7 @@
         <v>214</v>
       </c>
       <c r="H1" s="40" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>490</v>
@@ -20899,7 +20909,7 @@
         <v>504</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="Q1" s="14" t="s">
         <v>487</v>
@@ -20920,7 +20930,7 @@
         <v>656</v>
       </c>
       <c r="W1" s="14" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="X1" s="14" t="s">
         <v>215</v>
@@ -20985,7 +20995,7 @@
         <v>491</v>
       </c>
       <c r="P2" s="19" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>488</v>
@@ -21006,7 +21016,7 @@
         <v>201</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="X2" s="4" t="s">
         <v>200</v>
@@ -21047,7 +21057,7 @@
         <v>206</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>492</v>
@@ -21071,7 +21081,7 @@
         <v>506</v>
       </c>
       <c r="P3" s="42" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>489</v>
@@ -21092,7 +21102,7 @@
         <v>494</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="X3" s="2" t="s">
         <v>208</v>
@@ -21115,13 +21125,13 @@
         <v>53200100</v>
       </c>
       <c r="B4" s="24" t="s">
+        <v>745</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>746</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="D4" s="8" t="s">
         <v>747</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>748</v>
       </c>
       <c r="E4" s="16">
         <v>3</v>
@@ -21171,7 +21181,7 @@
         <v>2300</v>
       </c>
       <c r="T4" s="12" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="U4" s="7" t="s">
         <v>644</v>
@@ -21193,7 +21203,7 @@
         <v>0</v>
       </c>
       <c r="AB4" s="27" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="24">
@@ -21201,13 +21211,13 @@
         <v>53200101</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>736</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>737</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="8" t="s">
         <v>738</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>739</v>
       </c>
       <c r="E5" s="16">
         <v>3</v>
@@ -21257,7 +21267,7 @@
         <v>1800</v>
       </c>
       <c r="T5" s="12" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="U5" s="7" t="s">
         <v>654</v>
@@ -21279,7 +21289,7 @@
         <v>0</v>
       </c>
       <c r="AB5" s="27" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="40.5">
@@ -21287,13 +21297,13 @@
         <v>53200102</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>748</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>749</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="8" t="s">
         <v>750</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>751</v>
       </c>
       <c r="E6" s="16">
         <v>3</v>
@@ -21343,10 +21353,10 @@
         <v>2300</v>
       </c>
       <c r="T6" s="12" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="U6" s="34" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="V6" s="1" t="s">
         <v>53</v>
@@ -21365,7 +21375,7 @@
         <v>0</v>
       </c>
       <c r="AB6" s="27" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="14.25">
@@ -21373,13 +21383,13 @@
         <v>53200103</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>740</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>741</v>
       </c>
       <c r="E7" s="16">
         <v>3</v>
@@ -21430,7 +21440,7 @@
       </c>
       <c r="T7" s="12"/>
       <c r="U7" s="34" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="V7" s="1" t="s">
         <v>52</v>
@@ -21449,7 +21459,7 @@
         <v>0</v>
       </c>
       <c r="AB7" s="27" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="60">
@@ -21457,13 +21467,13 @@
         <v>53200104</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>756</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>757</v>
       </c>
       <c r="E8" s="16">
         <v>3</v>
@@ -21513,16 +21523,16 @@
         <v>1800</v>
       </c>
       <c r="T8" s="12" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="U8" s="7" t="s">
         <v>666</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="X8" s="1">
         <v>4</v>
@@ -21537,7 +21547,7 @@
         <v>0</v>
       </c>
       <c r="AB8" s="27" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="9" spans="1:28" ht="24">
@@ -21545,13 +21555,13 @@
         <v>53200105</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>758</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>759</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="8" t="s">
         <v>760</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>761</v>
       </c>
       <c r="E9" s="16">
         <v>3</v>
@@ -21601,7 +21611,7 @@
         <v>8000</v>
       </c>
       <c r="T9" s="12" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="U9" s="7" t="s">
         <v>509</v>
@@ -21623,7 +21633,7 @@
         <v>0</v>
       </c>
       <c r="AB9" s="27" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
   </sheetData>
@@ -21795,12 +21805,12 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B2">
         <f>COUNTIF(标准!AB:AB,"*单伤*")</f>
@@ -21809,7 +21819,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B3">
         <f>COUNTIF(标准!AB:AB,"*群伤*")</f>
@@ -21818,7 +21828,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B4">
         <f>COUNTIF(标准!AB:AB,"*单治*")</f>
@@ -21827,7 +21837,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B5">
         <f>COUNTIF(标准!AB:AB,"*群治*")</f>
@@ -21836,7 +21846,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B6">
         <f>COUNTIF(标准!AB:AB,"*正状*")</f>
@@ -21845,7 +21855,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B7">
         <f>COUNTIF(标准!AB:AB,"*负状*")</f>
@@ -21854,7 +21864,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B8">
         <f>COUNTIF(标准!AB:AB,"*手牌*")</f>
@@ -21863,7 +21873,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B9">
         <f>COUNTIF(标准!AB:AB,"*过牌*")</f>
@@ -21872,7 +21882,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="B10">
         <f>COUNTIF(标准!AB:AB,"*陷阱*")</f>
@@ -21881,7 +21891,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B11">
         <f>COUNTIF(标准!AB:AB,"*地形*")</f>
@@ -21890,7 +21900,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B12">
         <f>COUNTIF(标准!AB:AB,"*属性*")</f>

</xml_diff>

<commit_message>
fix a bug of passive and active skill
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388" activeTab="2"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
   </bookViews>
   <sheets>
     <sheet name="标准" sheetId="1" r:id="rId1"/>
@@ -4348,509 +4348,6 @@
   <dxfs count="147">
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <name val="Courier New"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10.5"/>
-        <color rgb="FF000000"/>
-        <name val="Courier New"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <name val="Courier New"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -5469,6 +4966,20 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <name val="Courier New"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -5592,6 +5103,99 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -6215,6 +5819,19 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <name val="Courier New"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -6349,6 +5966,194 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -6972,6 +6777,19 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <name val="Courier New"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -7106,6 +6924,188 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -7283,11 +7283,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="432773040"/>
-        <c:axId val="432773600"/>
+        <c:axId val="47494032"/>
+        <c:axId val="47499632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="432773040"/>
+        <c:axId val="47494032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7330,7 +7330,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="432773600"/>
+        <c:crossAx val="47499632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7338,7 +7338,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="432773600"/>
+        <c:axId val="47499632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7389,7 +7389,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="432773040"/>
+        <c:crossAx val="47494032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8017,129 +8017,129 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AA125" totalsRowShown="0" headerRowDxfId="146" dataDxfId="145" tableBorderDxfId="144">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AA125" totalsRowShown="0" headerRowDxfId="123" dataDxfId="122" tableBorderDxfId="121">
   <autoFilter ref="A3:AA125"/>
   <sortState ref="A4:Y128">
     <sortCondition ref="A3:A128"/>
   </sortState>
   <tableColumns count="27">
-    <tableColumn id="1" name="Id" dataDxfId="143"/>
-    <tableColumn id="2" name="Name" dataDxfId="142"/>
-    <tableColumn id="20" name="Ename" dataDxfId="141"/>
-    <tableColumn id="21" name="Remark" dataDxfId="60"/>
-    <tableColumn id="3" name="Star" dataDxfId="140"/>
-    <tableColumn id="4" name="Type" dataDxfId="139"/>
-    <tableColumn id="5" name="Attr" dataDxfId="138"/>
-    <tableColumn id="8" name="Quality" dataDxfId="137">
+    <tableColumn id="1" name="Id" dataDxfId="120"/>
+    <tableColumn id="2" name="Name" dataDxfId="119"/>
+    <tableColumn id="20" name="Ename" dataDxfId="118"/>
+    <tableColumn id="21" name="Remark" dataDxfId="117"/>
+    <tableColumn id="3" name="Star" dataDxfId="116"/>
+    <tableColumn id="4" name="Type" dataDxfId="115"/>
+    <tableColumn id="5" name="Attr" dataDxfId="114"/>
+    <tableColumn id="8" name="Quality" dataDxfId="113">
       <calculatedColumnFormula>IF(AND(P4&gt;=13,P4&lt;=16),5,IF(AND(P4&gt;=9,P4&lt;=12),4,IF(AND(P4&gt;=5,P4&lt;=8),3,IF(AND(P4&gt;=1,P4&lt;=4),2,IF(AND(P4&gt;=-3,P4&lt;=0),1,IF(AND(P4&gt;=-5,P4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="136"/>
-    <tableColumn id="9" name="Damage" dataDxfId="135"/>
-    <tableColumn id="10" name="Cure" dataDxfId="134"/>
-    <tableColumn id="11" name="Time" dataDxfId="133"/>
-    <tableColumn id="13" name="Help" dataDxfId="132"/>
-    <tableColumn id="16" name="Rate" dataDxfId="131"/>
-    <tableColumn id="12" name="Modify" dataDxfId="130"/>
-    <tableColumn id="27" name="Sum" dataDxfId="129">
+    <tableColumn id="7" name="Cost" dataDxfId="112"/>
+    <tableColumn id="9" name="Damage" dataDxfId="111"/>
+    <tableColumn id="10" name="Cure" dataDxfId="110"/>
+    <tableColumn id="11" name="Time" dataDxfId="109"/>
+    <tableColumn id="13" name="Help" dataDxfId="108"/>
+    <tableColumn id="16" name="Rate" dataDxfId="107"/>
+    <tableColumn id="12" name="Modify" dataDxfId="106"/>
+    <tableColumn id="27" name="Sum" dataDxfId="105">
       <calculatedColumnFormula>(S4-2000)/20+O4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="128"/>
-    <tableColumn id="15" name="Target" dataDxfId="127"/>
-    <tableColumn id="25" name="Mark" dataDxfId="126"/>
-    <tableColumn id="22" name="Effect" dataDxfId="125"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="124"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="123"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="122"/>
-    <tableColumn id="18" name="Res" dataDxfId="121"/>
-    <tableColumn id="19" name="Icon" dataDxfId="120"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="119"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="118"/>
+    <tableColumn id="6" name="Range" dataDxfId="104"/>
+    <tableColumn id="15" name="Target" dataDxfId="103"/>
+    <tableColumn id="25" name="Mark" dataDxfId="102"/>
+    <tableColumn id="22" name="Effect" dataDxfId="101"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="100"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="99"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="98"/>
+    <tableColumn id="18" name="Res" dataDxfId="97"/>
+    <tableColumn id="19" name="Icon" dataDxfId="96"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="95"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="94"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AA9" totalsRowShown="0" headerRowDxfId="117" dataDxfId="116" tableBorderDxfId="115">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AA9" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69" tableBorderDxfId="68">
   <autoFilter ref="A3:AA9"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="27">
-    <tableColumn id="1" name="Id" dataDxfId="114"/>
-    <tableColumn id="2" name="Name" dataDxfId="113"/>
-    <tableColumn id="20" name="Ename" dataDxfId="112"/>
-    <tableColumn id="21" name="Remark" dataDxfId="59"/>
-    <tableColumn id="3" name="Star" dataDxfId="111"/>
-    <tableColumn id="4" name="Type" dataDxfId="110"/>
-    <tableColumn id="5" name="Attr" dataDxfId="109"/>
-    <tableColumn id="8" name="Quality" dataDxfId="108">
+    <tableColumn id="1" name="Id" dataDxfId="67"/>
+    <tableColumn id="2" name="Name" dataDxfId="66"/>
+    <tableColumn id="20" name="Ename" dataDxfId="65"/>
+    <tableColumn id="21" name="Remark" dataDxfId="64"/>
+    <tableColumn id="3" name="Star" dataDxfId="63"/>
+    <tableColumn id="4" name="Type" dataDxfId="62"/>
+    <tableColumn id="5" name="Attr" dataDxfId="61"/>
+    <tableColumn id="8" name="Quality" dataDxfId="60">
       <calculatedColumnFormula>IF(AND(P4&gt;=13,P4&lt;=16),5,IF(AND(P4&gt;=9,P4&lt;=12),4,IF(AND(P4&gt;=5,P4&lt;=8),3,IF(AND(P4&gt;=1,P4&lt;=4),2,IF(AND(P4&gt;=-3,P4&lt;=0),1,IF(AND(P4&gt;=-5,P4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="107"/>
-    <tableColumn id="9" name="Damage" dataDxfId="106"/>
-    <tableColumn id="10" name="Cure" dataDxfId="105"/>
-    <tableColumn id="11" name="Time" dataDxfId="104"/>
-    <tableColumn id="13" name="Help" dataDxfId="103"/>
-    <tableColumn id="16" name="Rate" dataDxfId="102"/>
-    <tableColumn id="12" name="Modify" dataDxfId="101"/>
-    <tableColumn id="27" name="Sum" dataDxfId="100">
+    <tableColumn id="7" name="Cost" dataDxfId="59"/>
+    <tableColumn id="9" name="Damage" dataDxfId="58"/>
+    <tableColumn id="10" name="Cure" dataDxfId="57"/>
+    <tableColumn id="11" name="Time" dataDxfId="56"/>
+    <tableColumn id="13" name="Help" dataDxfId="55"/>
+    <tableColumn id="16" name="Rate" dataDxfId="54"/>
+    <tableColumn id="12" name="Modify" dataDxfId="53"/>
+    <tableColumn id="27" name="Sum" dataDxfId="52">
       <calculatedColumnFormula>(S4-2000)/20+O4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="99"/>
-    <tableColumn id="15" name="Target" dataDxfId="98"/>
-    <tableColumn id="25" name="Mark" dataDxfId="97"/>
-    <tableColumn id="22" name="Effect" dataDxfId="96"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="95"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="94"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="93"/>
-    <tableColumn id="18" name="Res" dataDxfId="92"/>
-    <tableColumn id="19" name="Icon" dataDxfId="91"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="90"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="89"/>
+    <tableColumn id="6" name="Range" dataDxfId="51"/>
+    <tableColumn id="15" name="Target" dataDxfId="50"/>
+    <tableColumn id="25" name="Mark" dataDxfId="49"/>
+    <tableColumn id="22" name="Effect" dataDxfId="48"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="47"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="46"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="45"/>
+    <tableColumn id="18" name="Res" dataDxfId="44"/>
+    <tableColumn id="19" name="Icon" dataDxfId="43"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="42"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_35" displayName="表1_35" ref="A3:AA9" totalsRowShown="0" headerRowDxfId="88" tableBorderDxfId="87">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_35" displayName="表1_35" ref="A3:AA9" totalsRowShown="0" headerRowDxfId="28" tableBorderDxfId="27">
   <autoFilter ref="A3:AA9"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="27">
-    <tableColumn id="1" name="Id" dataDxfId="86"/>
-    <tableColumn id="2" name="Name" dataDxfId="85"/>
-    <tableColumn id="20" name="Ename" dataDxfId="84"/>
-    <tableColumn id="21" name="Remark" dataDxfId="58"/>
-    <tableColumn id="3" name="Star" dataDxfId="83"/>
-    <tableColumn id="4" name="Type" dataDxfId="82"/>
-    <tableColumn id="5" name="Attr" dataDxfId="81"/>
-    <tableColumn id="8" name="Quality" dataDxfId="80">
+    <tableColumn id="1" name="Id" dataDxfId="26"/>
+    <tableColumn id="2" name="Name" dataDxfId="25"/>
+    <tableColumn id="20" name="Ename" dataDxfId="24"/>
+    <tableColumn id="21" name="Remark" dataDxfId="23"/>
+    <tableColumn id="3" name="Star" dataDxfId="22"/>
+    <tableColumn id="4" name="Type" dataDxfId="21"/>
+    <tableColumn id="5" name="Attr" dataDxfId="20"/>
+    <tableColumn id="8" name="Quality" dataDxfId="19">
       <calculatedColumnFormula>IF(AND(P4&gt;=13,P4&lt;=16),5,IF(AND(P4&gt;=9,P4&lt;=12),4,IF(AND(P4&gt;=5,P4&lt;=8),3,IF(AND(P4&gt;=1,P4&lt;=4),2,IF(AND(P4&gt;=-3,P4&lt;=0),1,IF(AND(P4&gt;=-5,P4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="79"/>
-    <tableColumn id="9" name="Damage" dataDxfId="78"/>
-    <tableColumn id="10" name="Cure" dataDxfId="77"/>
-    <tableColumn id="11" name="Time" dataDxfId="76"/>
-    <tableColumn id="13" name="Help" dataDxfId="75"/>
-    <tableColumn id="16" name="Rate" dataDxfId="74"/>
-    <tableColumn id="12" name="Modify" dataDxfId="73"/>
-    <tableColumn id="27" name="Sum" dataDxfId="72">
+    <tableColumn id="7" name="Cost" dataDxfId="18"/>
+    <tableColumn id="9" name="Damage" dataDxfId="17"/>
+    <tableColumn id="10" name="Cure" dataDxfId="16"/>
+    <tableColumn id="11" name="Time" dataDxfId="15"/>
+    <tableColumn id="13" name="Help" dataDxfId="14"/>
+    <tableColumn id="16" name="Rate" dataDxfId="13"/>
+    <tableColumn id="12" name="Modify" dataDxfId="12"/>
+    <tableColumn id="27" name="Sum" dataDxfId="11">
       <calculatedColumnFormula>(S4-2000)/20+O4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="71"/>
-    <tableColumn id="15" name="Target" dataDxfId="70"/>
-    <tableColumn id="25" name="Mark" dataDxfId="69"/>
-    <tableColumn id="22" name="Effect" dataDxfId="68"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="67"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="66"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="65"/>
-    <tableColumn id="18" name="Res" dataDxfId="64"/>
-    <tableColumn id="19" name="Icon" dataDxfId="63"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="62"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="61"/>
+    <tableColumn id="6" name="Range" dataDxfId="10"/>
+    <tableColumn id="15" name="Target" dataDxfId="9"/>
+    <tableColumn id="25" name="Mark" dataDxfId="8"/>
+    <tableColumn id="22" name="Effect" dataDxfId="7"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="6"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="5"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="4"/>
+    <tableColumn id="18" name="Res" dataDxfId="3"/>
+    <tableColumn id="19" name="Icon" dataDxfId="2"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="1"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8434,11 +8434,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA125"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AB1" sqref="AB1:AB1048576"/>
+      <selection pane="bottomRight" activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -18874,81 +18874,81 @@
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I70:I114 I38:I68 I120:I124 I4:I15 I17:I35">
-    <cfRule type="cellIs" dxfId="57" priority="54" operator="notEqual">
+    <cfRule type="cellIs" dxfId="146" priority="54" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J125:P125 J38:P68 J4:O4 J70:P123 J5:P15 J17:P35">
-    <cfRule type="cellIs" dxfId="56" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="53" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I124">
-    <cfRule type="cellIs" dxfId="55" priority="51" operator="notEqual">
+    <cfRule type="cellIs" dxfId="144" priority="51" operator="notEqual">
       <formula>$E124</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I115:I119">
-    <cfRule type="cellIs" dxfId="54" priority="49" operator="notEqual">
+    <cfRule type="cellIs" dxfId="143" priority="49" operator="notEqual">
       <formula>$E115</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I125">
-    <cfRule type="cellIs" dxfId="53" priority="48" operator="notEqual">
+    <cfRule type="cellIs" dxfId="142" priority="48" operator="notEqual">
       <formula>$E125</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J125:P125">
-    <cfRule type="cellIs" dxfId="52" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="47" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J124:P124">
-    <cfRule type="cellIs" dxfId="51" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="33" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I69">
-    <cfRule type="cellIs" dxfId="50" priority="18" operator="notEqual">
+    <cfRule type="cellIs" dxfId="139" priority="18" operator="notEqual">
       <formula>$E69</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J69:P69">
-    <cfRule type="cellIs" dxfId="49" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="17" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36">
-    <cfRule type="cellIs" dxfId="48" priority="16" operator="notEqual">
+    <cfRule type="cellIs" dxfId="137" priority="16" operator="notEqual">
       <formula>$E36</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J36:P36">
-    <cfRule type="cellIs" dxfId="47" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="15" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37">
-    <cfRule type="cellIs" dxfId="46" priority="14" operator="notEqual">
+    <cfRule type="cellIs" dxfId="135" priority="14" operator="notEqual">
       <formula>$E37</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J37:P37">
-    <cfRule type="cellIs" dxfId="45" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="13" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H15 H17:H125">
-    <cfRule type="cellIs" dxfId="44" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="9" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="10" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="11" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="12" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="130" priority="12" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18965,26 +18965,26 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="cellIs" dxfId="40" priority="6" operator="notEqual">
+    <cfRule type="cellIs" dxfId="129" priority="6" operator="notEqual">
       <formula>$E16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:P16">
-    <cfRule type="cellIs" dxfId="39" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="cellIs" dxfId="38" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="2" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="124" priority="4" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19766,105 +19766,105 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="J4:P9">
-    <cfRule type="cellIs" dxfId="34" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="39" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:P8">
-    <cfRule type="cellIs" dxfId="33" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="35" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:P4">
-    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="34" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="31" priority="33" operator="notEqual">
+    <cfRule type="cellIs" dxfId="90" priority="33" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:P4">
-    <cfRule type="cellIs" dxfId="30" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="32" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="29" priority="31" operator="notEqual">
+    <cfRule type="cellIs" dxfId="88" priority="31" operator="notEqual">
       <formula>$E5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:P5">
-    <cfRule type="cellIs" dxfId="28" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="30" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" dxfId="27" priority="29" operator="notEqual">
+    <cfRule type="cellIs" dxfId="86" priority="29" operator="notEqual">
       <formula>$E6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:P6">
-    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="28" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="25" priority="27" operator="notEqual">
+    <cfRule type="cellIs" dxfId="84" priority="27" operator="notEqual">
       <formula>$E7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:P7">
-    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="26" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="23" priority="25" operator="notEqual">
+    <cfRule type="cellIs" dxfId="82" priority="25" operator="notEqual">
       <formula>$E8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:P8">
-    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="24" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="cellIs" dxfId="21" priority="23" operator="notEqual">
+    <cfRule type="cellIs" dxfId="80" priority="23" operator="notEqual">
       <formula>$E9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:P9">
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="22" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H9">
-    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="6" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="7" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="75" priority="8" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="2" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="71" priority="4" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19881,7 +19881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -20660,50 +20660,50 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I4:I9">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="notEqual">
+    <cfRule type="cellIs" dxfId="40" priority="12" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:P7">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:P9">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:P8">
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H9">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="6" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="7" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="33" priority="8" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="29" priority="4" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
new rebel effect spell
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="标准" sheetId="1" r:id="rId1"/>
@@ -717,7 +717,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="748">
   <si>
     <t>慈悲</t>
   </si>
@@ -3349,6 +3349,18 @@
   </si>
   <si>
     <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse)) im.AddBuff(56000001,lv,s.Time);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>{4:0.0}%几率策反目标敌方怪物</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>单负</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>t.Rebel();</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -7283,11 +7295,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="47494032"/>
-        <c:axId val="47499632"/>
+        <c:axId val="895218240"/>
+        <c:axId val="895212800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="47494032"/>
+        <c:axId val="895218240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7330,7 +7342,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47499632"/>
+        <c:crossAx val="895212800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7338,7 +7350,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47499632"/>
+        <c:axId val="895212800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7389,7 +7401,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47494032"/>
+        <c:crossAx val="895218240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8435,29 +8447,29 @@
   <dimension ref="A1:AA125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C75" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D75" sqref="D75"/>
+      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
-    <col min="2" max="3" width="7.88671875" customWidth="1"/>
-    <col min="5" max="5" width="3.109375" customWidth="1"/>
-    <col min="6" max="6" width="3.6640625" customWidth="1"/>
-    <col min="7" max="9" width="3.109375" customWidth="1"/>
-    <col min="10" max="10" width="3.88671875" customWidth="1"/>
+    <col min="1" max="1" width="9.125" customWidth="1"/>
+    <col min="2" max="3" width="7.875" customWidth="1"/>
+    <col min="5" max="5" width="3.125" customWidth="1"/>
+    <col min="6" max="6" width="3.625" customWidth="1"/>
+    <col min="7" max="9" width="3.125" customWidth="1"/>
+    <col min="10" max="10" width="3.875" customWidth="1"/>
     <col min="11" max="11" width="4" customWidth="1"/>
-    <col min="12" max="15" width="3.109375" customWidth="1"/>
-    <col min="16" max="16" width="5.21875" customWidth="1"/>
-    <col min="17" max="17" width="3.109375" customWidth="1"/>
-    <col min="18" max="18" width="5.33203125" customWidth="1"/>
-    <col min="19" max="19" width="5.77734375" customWidth="1"/>
-    <col min="20" max="20" width="23.44140625" customWidth="1"/>
-    <col min="21" max="21" width="24.33203125" customWidth="1"/>
-    <col min="22" max="23" width="7.88671875" customWidth="1"/>
+    <col min="12" max="15" width="3.125" customWidth="1"/>
+    <col min="16" max="16" width="5.25" customWidth="1"/>
+    <col min="17" max="17" width="3.125" customWidth="1"/>
+    <col min="18" max="18" width="5.375" customWidth="1"/>
+    <col min="19" max="19" width="5.75" customWidth="1"/>
+    <col min="20" max="20" width="23.5" customWidth="1"/>
+    <col min="21" max="21" width="24.375" customWidth="1"/>
+    <col min="22" max="23" width="7.875" customWidth="1"/>
     <col min="24" max="27" width="4" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8710,7 +8722,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="48">
+    <row r="4" spans="1:27" ht="36">
       <c r="A4">
         <v>53000001</v>
       </c>
@@ -9125,7 +9137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="60">
+    <row r="9" spans="1:27" ht="48">
       <c r="A9">
         <v>53000006</v>
       </c>
@@ -9208,7 +9220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="60">
+    <row r="10" spans="1:27" ht="48">
       <c r="A10">
         <v>53000007</v>
       </c>
@@ -9291,7 +9303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="60">
+    <row r="11" spans="1:27" ht="48">
       <c r="A11">
         <v>53000008</v>
       </c>
@@ -9374,7 +9386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="60">
+    <row r="12" spans="1:27" ht="48">
       <c r="A12">
         <v>53000009</v>
       </c>
@@ -9457,7 +9469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="60">
+    <row r="13" spans="1:27" ht="48">
       <c r="A13">
         <v>53000010</v>
       </c>
@@ -9540,7 +9552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="60">
+    <row r="14" spans="1:27" ht="48">
       <c r="A14">
         <v>53000011</v>
       </c>
@@ -9623,7 +9635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="60">
+    <row r="15" spans="1:27" ht="48">
       <c r="A15">
         <v>53000012</v>
       </c>
@@ -9955,18 +9967,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:27" ht="24">
+    <row r="19" spans="1:27">
       <c r="A19">
         <v>53000017</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>246</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>675</v>
+        <v>746</v>
       </c>
       <c r="E19" s="1">
         <v>5</v>
@@ -9979,7 +9991,7 @@
       </c>
       <c r="H19" s="1">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I19" s="1">
         <v>5</v>
@@ -9997,14 +10009,14 @@
         <v>0</v>
       </c>
       <c r="N19" s="1">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="O19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P19" s="42">
         <f t="shared" si="1"/>
-        <v>301</v>
+        <v>0</v>
       </c>
       <c r="Q19" s="1">
         <v>0</v>
@@ -10013,13 +10025,13 @@
         <v>6</v>
       </c>
       <c r="S19" s="1">
-        <v>8000</v>
+        <v>2000</v>
       </c>
       <c r="T19" s="11" t="s">
-        <v>653</v>
+        <v>747</v>
       </c>
       <c r="U19" s="7" t="s">
-        <v>378</v>
+        <v>745</v>
       </c>
       <c r="V19" s="1" t="s">
         <v>24</v>
@@ -11285,7 +11297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:27" ht="48">
+    <row r="35" spans="1:27" ht="36">
       <c r="A35">
         <v>53000036</v>
       </c>
@@ -12029,7 +12041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:27" ht="72">
+    <row r="44" spans="1:27" ht="60">
       <c r="A44">
         <v>53000045</v>
       </c>
@@ -12113,7 +12125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:27" ht="60">
+    <row r="45" spans="1:27" ht="48">
       <c r="A45">
         <v>53000046</v>
       </c>
@@ -12364,7 +12376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:27" ht="72">
+    <row r="48" spans="1:27" ht="60">
       <c r="A48">
         <v>53000049</v>
       </c>
@@ -12449,7 +12461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:27" ht="84">
+    <row r="49" spans="1:27" ht="72">
       <c r="A49">
         <v>53000050</v>
       </c>
@@ -12781,7 +12793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:27" ht="60">
+    <row r="53" spans="1:27" ht="48">
       <c r="A53">
         <v>53000054</v>
       </c>
@@ -12947,7 +12959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:27" ht="48">
+    <row r="55" spans="1:27" ht="36">
       <c r="A55">
         <v>53000056</v>
       </c>
@@ -13030,7 +13042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:27" ht="36">
+    <row r="56" spans="1:27" ht="24">
       <c r="A56">
         <v>53000057</v>
       </c>
@@ -13196,7 +13208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:27" ht="36">
+    <row r="58" spans="1:27" ht="24">
       <c r="A58">
         <v>53000059</v>
       </c>
@@ -13279,7 +13291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:27" ht="48">
+    <row r="59" spans="1:27" ht="36">
       <c r="A59">
         <v>53000060</v>
       </c>
@@ -13362,7 +13374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:27" ht="60">
+    <row r="60" spans="1:27" ht="48">
       <c r="A60">
         <v>53000061</v>
       </c>
@@ -13943,7 +13955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:27" ht="72">
+    <row r="67" spans="1:27" ht="60">
       <c r="A67">
         <v>53000068</v>
       </c>
@@ -14192,7 +14204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:27" ht="84">
+    <row r="70" spans="1:27" ht="72">
       <c r="A70">
         <v>53000071</v>
       </c>
@@ -14277,7 +14289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:27" ht="60">
+    <row r="71" spans="1:27" ht="48">
       <c r="A71">
         <v>53000072</v>
       </c>
@@ -14526,7 +14538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:27" ht="132">
+    <row r="74" spans="1:27" ht="108">
       <c r="A74">
         <v>53000075</v>
       </c>
@@ -14609,7 +14621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:27" ht="72">
+    <row r="75" spans="1:27" ht="60">
       <c r="A75">
         <v>53000076</v>
       </c>
@@ -14945,7 +14957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:27" ht="72">
+    <row r="79" spans="1:27" ht="60">
       <c r="A79">
         <v>53000080</v>
       </c>
@@ -15364,7 +15376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:27" ht="84">
+    <row r="84" spans="1:27" ht="60">
       <c r="A84">
         <v>53000085</v>
       </c>
@@ -16204,7 +16216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:27" ht="60">
+    <row r="94" spans="1:27" ht="48">
       <c r="A94">
         <v>53000095</v>
       </c>
@@ -16372,7 +16384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:27" ht="72">
+    <row r="96" spans="1:27" ht="60">
       <c r="A96">
         <v>53000097</v>
       </c>
@@ -16457,7 +16469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:27" ht="36">
+    <row r="97" spans="1:27" ht="24">
       <c r="A97">
         <v>53000098</v>
       </c>
@@ -16540,7 +16552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:27" ht="36">
+    <row r="98" spans="1:27" ht="24">
       <c r="A98">
         <v>53000099</v>
       </c>
@@ -16872,7 +16884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:27" ht="72">
+    <row r="102" spans="1:27" ht="60">
       <c r="A102">
         <v>53000103</v>
       </c>
@@ -17038,7 +17050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:27" ht="60">
+    <row r="104" spans="1:27" ht="36">
       <c r="A104">
         <v>53000105</v>
       </c>
@@ -17287,7 +17299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:27" ht="144">
+    <row r="107" spans="1:27" ht="120">
       <c r="A107">
         <v>53000108</v>
       </c>
@@ -17453,7 +17465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:27" ht="48">
+    <row r="109" spans="1:27" ht="36">
       <c r="A109">
         <v>53000110</v>
       </c>
@@ -17536,7 +17548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:27" ht="60">
+    <row r="110" spans="1:27" ht="48">
       <c r="A110">
         <v>53000111</v>
       </c>
@@ -17951,7 +17963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:27" ht="60">
+    <row r="115" spans="1:27" ht="36">
       <c r="A115">
         <v>53000116</v>
       </c>
@@ -18034,7 +18046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:27" ht="60">
+    <row r="116" spans="1:27" ht="48">
       <c r="A116">
         <v>53000117</v>
       </c>
@@ -18117,7 +18129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:27" ht="60">
+    <row r="117" spans="1:27" ht="48">
       <c r="A117">
         <v>53000118</v>
       </c>
@@ -18200,7 +18212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:27" ht="60">
+    <row r="118" spans="1:27" ht="48">
       <c r="A118">
         <v>53000119</v>
       </c>
@@ -18283,7 +18295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:27" ht="60">
+    <row r="119" spans="1:27" ht="48">
       <c r="A119">
         <v>53000120</v>
       </c>
@@ -18366,7 +18378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:27" ht="60">
+    <row r="120" spans="1:27" ht="48">
       <c r="A120">
         <v>53000121</v>
       </c>
@@ -18449,7 +18461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:27" ht="60">
+    <row r="121" spans="1:27" ht="48">
       <c r="A121">
         <v>53000122</v>
       </c>
@@ -18532,7 +18544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:27" ht="60">
+    <row r="122" spans="1:27" ht="48">
       <c r="A122">
         <v>53000125</v>
       </c>
@@ -18615,7 +18627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:27" ht="84">
+    <row r="123" spans="1:27" ht="72">
       <c r="A123">
         <v>53000126</v>
       </c>
@@ -18700,7 +18712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:27" ht="60">
+    <row r="124" spans="1:27" ht="48">
       <c r="A124">
         <v>53000127</v>
       </c>
@@ -19020,23 +19032,23 @@
       <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="3" width="7.88671875" customWidth="1"/>
-    <col min="5" max="5" width="3.109375" customWidth="1"/>
-    <col min="6" max="6" width="4.6640625" customWidth="1"/>
-    <col min="7" max="9" width="3.109375" customWidth="1"/>
-    <col min="10" max="10" width="3.88671875" customWidth="1"/>
+    <col min="2" max="3" width="7.875" customWidth="1"/>
+    <col min="5" max="5" width="3.125" customWidth="1"/>
+    <col min="6" max="6" width="4.625" customWidth="1"/>
+    <col min="7" max="9" width="3.125" customWidth="1"/>
+    <col min="10" max="10" width="3.875" customWidth="1"/>
     <col min="11" max="11" width="4" customWidth="1"/>
-    <col min="12" max="15" width="3.109375" customWidth="1"/>
-    <col min="16" max="16" width="5.109375" customWidth="1"/>
-    <col min="17" max="17" width="3.109375" customWidth="1"/>
-    <col min="18" max="18" width="5.33203125" customWidth="1"/>
-    <col min="19" max="19" width="5.77734375" customWidth="1"/>
-    <col min="20" max="20" width="23.44140625" customWidth="1"/>
-    <col min="21" max="21" width="27.21875" customWidth="1"/>
-    <col min="22" max="23" width="7.88671875" customWidth="1"/>
+    <col min="12" max="15" width="3.125" customWidth="1"/>
+    <col min="16" max="16" width="5.125" customWidth="1"/>
+    <col min="17" max="17" width="3.125" customWidth="1"/>
+    <col min="18" max="18" width="5.375" customWidth="1"/>
+    <col min="19" max="19" width="5.75" customWidth="1"/>
+    <col min="20" max="20" width="23.5" customWidth="1"/>
+    <col min="21" max="21" width="27.25" customWidth="1"/>
+    <col min="22" max="23" width="7.875" customWidth="1"/>
     <col min="24" max="27" width="4" customWidth="1"/>
   </cols>
   <sheetData>
@@ -19447,7 +19459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="36">
+    <row r="6" spans="1:27" ht="24">
       <c r="A6">
         <v>53100002</v>
       </c>
@@ -19888,23 +19900,23 @@
       <selection pane="bottomRight" activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" customWidth="1"/>
-    <col min="2" max="3" width="7.88671875" customWidth="1"/>
-    <col min="5" max="5" width="3.109375" customWidth="1"/>
-    <col min="6" max="6" width="4.33203125" customWidth="1"/>
-    <col min="7" max="9" width="3.109375" customWidth="1"/>
-    <col min="10" max="10" width="3.88671875" customWidth="1"/>
+    <col min="1" max="1" width="10.75" customWidth="1"/>
+    <col min="2" max="3" width="7.875" customWidth="1"/>
+    <col min="5" max="5" width="3.125" customWidth="1"/>
+    <col min="6" max="6" width="4.375" customWidth="1"/>
+    <col min="7" max="9" width="3.125" customWidth="1"/>
+    <col min="10" max="10" width="3.875" customWidth="1"/>
     <col min="11" max="11" width="4" customWidth="1"/>
-    <col min="12" max="15" width="3.109375" customWidth="1"/>
-    <col min="16" max="16" width="5.21875" customWidth="1"/>
-    <col min="17" max="17" width="3.109375" customWidth="1"/>
-    <col min="18" max="18" width="5.33203125" customWidth="1"/>
-    <col min="19" max="19" width="5.77734375" customWidth="1"/>
-    <col min="20" max="20" width="23.44140625" customWidth="1"/>
-    <col min="21" max="21" width="27.21875" customWidth="1"/>
-    <col min="22" max="23" width="7.88671875" customWidth="1"/>
+    <col min="12" max="15" width="3.125" customWidth="1"/>
+    <col min="16" max="16" width="5.25" customWidth="1"/>
+    <col min="17" max="17" width="3.125" customWidth="1"/>
+    <col min="18" max="18" width="5.375" customWidth="1"/>
+    <col min="19" max="19" width="5.75" customWidth="1"/>
+    <col min="20" max="20" width="23.5" customWidth="1"/>
+    <col min="21" max="21" width="27.25" customWidth="1"/>
+    <col min="22" max="23" width="7.875" customWidth="1"/>
     <col min="24" max="24" width="4" customWidth="1"/>
     <col min="25" max="25" width="5" customWidth="1"/>
     <col min="26" max="27" width="4" customWidth="1"/>
@@ -20325,7 +20337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="43.2">
+    <row r="6" spans="1:27" ht="40.5">
       <c r="A6">
         <v>53200102</v>
       </c>
@@ -20724,7 +20736,7 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -20773,7 +20785,7 @@
         <v>2.3345235059857505</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" ht="15">
       <c r="A5" s="31" t="s">
         <v>518</v>
       </c>
@@ -20850,7 +20862,7 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" t="s">

</xml_diff>

<commit_message>
fix some cure spell
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -2073,14 +2073,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>立刻获得{3:0}的金币</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>p.AddResource(0, (int)s.Help);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>对敌方单体造成{0}点魔法伤害</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -2491,9 +2483,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>未完成，单治</t>
-  </si>
-  <si>
     <t>未完成，群伤</t>
   </si>
   <si>
@@ -2515,9 +2504,6 @@
     <t>未完成，单伤，负状</t>
   </si>
   <si>
-    <t>未完成，群治</t>
-  </si>
-  <si>
     <t>未完成，卡牌</t>
   </si>
   <si>
@@ -2577,10 +2563,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse))im.AddHp(s.Cure);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse))im.AddBuff(56000017,lv,s.Time);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -2745,10 +2727,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>t.OnMagicDamage(s.Damage,s.Attr);if(t.Star&lt;6&amp;&amp;MathTool.GetRandom(100)&lt;s.Rate)t.SuddenDeath();</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>t.OnMagicDamage(t.IsHero?s.Damage*3/2:s.Damage,s.Attr);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -2858,10 +2836,6 @@
   </si>
   <si>
     <t>群伤</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>未完成</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -3342,10 +3316,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>回复1.5卡片距离内我方单位{1}点生命</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>对敌我所有3星以下单位造成{0}点魔法伤害</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3428,6 +3398,38 @@
   </si>
   <si>
     <t>t.AddBuff(56000019,lv,s.Time);if(MathTool.GetRandom(100)&lt;s.Rate&amp;&amp;!t.ResistBuffType(2))t.Transform(51000001);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster im in m.GetAllMonster(mouse))im.AddHp(s.Cure);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NAA</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>回复敌我所有单位{1}点生命</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>群治</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>回复1.5卡片距离内我方单位{1}点生命，抽一张牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>群治</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>t.OnMagicDamage(s.Damage,s.Attr);if(t.Star&lt;6&amp;&amp;MathTool.GetRandom(100)&lt;s.Rate)t.SuddenDeath();</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse))im.AddHp(s.Cure);p.GetNextNCard(1);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -7400,10 +7402,10 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>12</c:v>
@@ -8175,13 +8177,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AB116" totalsRowShown="0" headerRowDxfId="126" dataDxfId="125" tableBorderDxfId="124">
-  <autoFilter ref="A3:AB116">
-    <filterColumn colId="19">
-      <customFilters>
-        <customFilter val="*trans*"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A3:AB116"/>
   <sortState ref="A4:AB116">
     <sortCondition ref="A3:A116"/>
   </sortState>
@@ -8601,10 +8597,10 @@
   <dimension ref="A1:AB116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C95" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="T74" sqref="T74"/>
+      <selection pane="bottomRight" activeCell="T98" sqref="T98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8640,7 +8636,7 @@
         <v>203</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>198</v>
@@ -8652,7 +8648,7 @@
         <v>200</v>
       </c>
       <c r="H1" s="38" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="I1" s="13" t="s">
         <v>337</v>
@@ -8676,7 +8672,7 @@
         <v>351</v>
       </c>
       <c r="P1" s="16" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="Q1" s="13" t="s">
         <v>334</v>
@@ -8685,7 +8681,7 @@
         <v>333</v>
       </c>
       <c r="S1" s="13" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="T1" s="13" t="s">
         <v>382</v>
@@ -8694,13 +8690,13 @@
         <v>319</v>
       </c>
       <c r="V1" s="13" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="W1" s="13" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="X1" s="44" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="Y1" s="13" t="s">
         <v>201</v>
@@ -8762,7 +8758,7 @@
         <v>352</v>
       </c>
       <c r="P2" s="18" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>335</v>
@@ -8771,10 +8767,10 @@
         <v>187</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="U2" s="10" t="s">
         <v>187</v>
@@ -8783,10 +8779,10 @@
         <v>187</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="X2" s="45" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="Y2" s="4" t="s">
         <v>186</v>
@@ -8812,7 +8808,7 @@
         <v>204</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>190</v>
@@ -8824,7 +8820,7 @@
         <v>192</v>
       </c>
       <c r="H3" s="39" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>339</v>
@@ -8848,31 +8844,31 @@
         <v>353</v>
       </c>
       <c r="P3" s="40" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>336</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="U3" s="6" t="s">
         <v>320</v>
       </c>
       <c r="V3" s="6" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="X3" s="46" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="Y3" s="2" t="s">
         <v>194</v>
@@ -8887,7 +8883,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="48" hidden="1">
+    <row r="4" spans="1:28" ht="48">
       <c r="A4">
         <v>53000001</v>
       </c>
@@ -8898,7 +8894,7 @@
         <v>221</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>662</v>
+        <v>655</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
@@ -8948,7 +8944,7 @@
         <v>85.2</v>
       </c>
       <c r="T4" s="11" t="s">
-        <v>633</v>
+        <v>626</v>
       </c>
       <c r="U4" s="32" t="s">
         <v>401</v>
@@ -8971,7 +8967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:28" hidden="1">
+    <row r="5" spans="1:28">
       <c r="A5">
         <v>53000002</v>
       </c>
@@ -8982,7 +8978,7 @@
         <v>222</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>704</v>
+        <v>697</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -9032,10 +9028,10 @@
         <v>80</v>
       </c>
       <c r="T5" s="11" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>698</v>
+        <v>691</v>
       </c>
       <c r="V5" s="1" t="s">
         <v>4</v>
@@ -9055,7 +9051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="24" hidden="1">
+    <row r="6" spans="1:28" ht="24">
       <c r="A6">
         <v>53000003</v>
       </c>
@@ -9066,7 +9062,7 @@
         <v>223</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>638</v>
+        <v>631</v>
       </c>
       <c r="E6" s="1">
         <v>2</v>
@@ -9116,10 +9112,10 @@
         <v>100</v>
       </c>
       <c r="T6" s="11" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="V6" s="1" t="s">
         <v>7</v>
@@ -9139,7 +9135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="36" hidden="1">
+    <row r="7" spans="1:28" ht="36">
       <c r="A7">
         <v>53000004</v>
       </c>
@@ -9150,7 +9146,7 @@
         <v>224</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
@@ -9200,10 +9196,10 @@
         <v>100</v>
       </c>
       <c r="T7" s="11" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="U7" s="7" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="V7" s="1" t="s">
         <v>9</v>
@@ -9225,7 +9221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="72" hidden="1">
+    <row r="8" spans="1:28" ht="72">
       <c r="A8">
         <v>53000005</v>
       </c>
@@ -9236,7 +9232,7 @@
         <v>225</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="E8" s="1">
         <v>3</v>
@@ -9280,13 +9276,13 @@
         <v>25</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="S8">
         <v>100</v>
       </c>
       <c r="T8" s="11" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="U8" s="7" t="s">
         <v>381</v>
@@ -9311,7 +9307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="48" hidden="1">
+    <row r="9" spans="1:28" ht="48">
       <c r="A9">
         <v>53000006</v>
       </c>
@@ -9322,7 +9318,7 @@
         <v>310</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>639</v>
+        <v>632</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
@@ -9372,10 +9368,10 @@
         <v>90</v>
       </c>
       <c r="T9" s="11" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
       <c r="U9" s="7" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="V9" s="1" t="s">
         <v>2</v>
@@ -9395,7 +9391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="48" hidden="1">
+    <row r="10" spans="1:28" ht="48">
       <c r="A10">
         <v>53000007</v>
       </c>
@@ -9406,7 +9402,7 @@
         <v>311</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>639</v>
+        <v>632</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -9456,10 +9452,10 @@
         <v>90</v>
       </c>
       <c r="T10" s="11" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="U10" s="7" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="V10" s="1" t="s">
         <v>2</v>
@@ -9479,7 +9475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="48" hidden="1">
+    <row r="11" spans="1:28" ht="48">
       <c r="A11">
         <v>53000008</v>
       </c>
@@ -9490,7 +9486,7 @@
         <v>312</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>639</v>
+        <v>632</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -9540,10 +9536,10 @@
         <v>90</v>
       </c>
       <c r="T11" s="11" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="U11" s="7" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="V11" s="1" t="s">
         <v>2</v>
@@ -9563,7 +9559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="48" hidden="1">
+    <row r="12" spans="1:28" ht="48">
       <c r="A12">
         <v>53000009</v>
       </c>
@@ -9574,7 +9570,7 @@
         <v>313</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>639</v>
+        <v>632</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
@@ -9624,10 +9620,10 @@
         <v>90</v>
       </c>
       <c r="T12" s="11" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="U12" s="7" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="V12" s="1" t="s">
         <v>2</v>
@@ -9647,7 +9643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="48" hidden="1">
+    <row r="13" spans="1:28" ht="48">
       <c r="A13">
         <v>53000010</v>
       </c>
@@ -9658,7 +9654,7 @@
         <v>226</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>639</v>
+        <v>632</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
@@ -9708,10 +9704,10 @@
         <v>90</v>
       </c>
       <c r="T13" s="11" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="U13" s="7" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="V13" s="1" t="s">
         <v>2</v>
@@ -9731,7 +9727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="48" hidden="1">
+    <row r="14" spans="1:28" ht="48">
       <c r="A14">
         <v>53000011</v>
       </c>
@@ -9742,7 +9738,7 @@
         <v>220</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>639</v>
+        <v>632</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
@@ -9792,10 +9788,10 @@
         <v>90</v>
       </c>
       <c r="T14" s="11" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="U14" s="7" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="V14" s="1" t="s">
         <v>2</v>
@@ -9815,7 +9811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="48" hidden="1">
+    <row r="15" spans="1:28" ht="48">
       <c r="A15">
         <v>53000012</v>
       </c>
@@ -9826,7 +9822,7 @@
         <v>227</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>639</v>
+        <v>632</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
@@ -9876,10 +9872,10 @@
         <v>90</v>
       </c>
       <c r="T15" s="11" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="U15" s="7" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="V15" s="1" t="s">
         <v>2</v>
@@ -9910,7 +9906,7 @@
         <v>418</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>636</v>
+        <v>629</v>
       </c>
       <c r="E16" s="15">
         <v>4</v>
@@ -9960,10 +9956,10 @@
         <v>100</v>
       </c>
       <c r="T16" s="11" t="s">
-        <v>766</v>
+        <v>758</v>
       </c>
       <c r="U16" s="7" t="s">
-        <v>635</v>
+        <v>628</v>
       </c>
       <c r="V16" s="1" t="s">
         <v>109</v>
@@ -9985,18 +9981,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="72" hidden="1">
+    <row r="17" spans="1:28" ht="72">
       <c r="A17">
         <v>53000014</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="E17" s="1">
         <v>2</v>
@@ -10040,19 +10036,19 @@
         <v>30</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="S17">
         <v>100</v>
       </c>
       <c r="T17" s="11" t="s">
-        <v>676</v>
+        <v>669</v>
       </c>
       <c r="U17" s="7" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="W17" s="1"/>
       <c r="X17" s="1">
@@ -10071,7 +10067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28" hidden="1">
+    <row r="18" spans="1:28">
       <c r="A18">
         <v>53000015</v>
       </c>
@@ -10082,7 +10078,7 @@
         <v>228</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="E18" s="1">
         <v>1</v>
@@ -10132,7 +10128,7 @@
         <v>75</v>
       </c>
       <c r="T18" s="11" t="s">
-        <v>643</v>
+        <v>636</v>
       </c>
       <c r="U18" s="7" t="s">
         <v>354</v>
@@ -10157,7 +10153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="24" hidden="1">
+    <row r="19" spans="1:28" ht="24">
       <c r="A19">
         <v>53000016</v>
       </c>
@@ -10168,7 +10164,7 @@
         <v>229</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="E19" s="1">
         <v>3</v>
@@ -10218,7 +10214,7 @@
         <v>75</v>
       </c>
       <c r="T19" s="11" t="s">
-        <v>632</v>
+        <v>625</v>
       </c>
       <c r="U19" s="7" t="s">
         <v>355</v>
@@ -10243,7 +10239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" hidden="1">
+    <row r="20" spans="1:28">
       <c r="A20">
         <v>53000017</v>
       </c>
@@ -10254,7 +10250,7 @@
         <v>230</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="E20" s="1">
         <v>5</v>
@@ -10304,10 +10300,10 @@
         <v>100</v>
       </c>
       <c r="T20" s="11" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="U20" s="7" t="s">
-        <v>634</v>
+        <v>627</v>
       </c>
       <c r="V20" s="1" t="s">
         <v>19</v>
@@ -10329,7 +10325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="60" hidden="1">
+    <row r="21" spans="1:28" ht="60">
       <c r="A21">
         <v>53000018</v>
       </c>
@@ -10340,7 +10336,7 @@
         <v>231</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="E21" s="1">
         <v>3</v>
@@ -10390,10 +10386,10 @@
         <v>102</v>
       </c>
       <c r="T21" s="11" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="U21" s="7" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="V21" s="1" t="s">
         <v>21</v>
@@ -10415,7 +10411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="24" hidden="1">
+    <row r="22" spans="1:28" ht="24">
       <c r="A22">
         <v>53000019</v>
       </c>
@@ -10426,7 +10422,7 @@
         <v>232</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="E22" s="1">
         <v>4</v>
@@ -10476,10 +10472,10 @@
         <v>100</v>
       </c>
       <c r="T22" s="11" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
       <c r="U22" s="7" t="s">
-        <v>682</v>
+        <v>675</v>
       </c>
       <c r="V22" s="1" t="s">
         <v>23</v>
@@ -10503,7 +10499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="24" hidden="1">
+    <row r="23" spans="1:28" ht="24">
       <c r="A23">
         <v>53000020</v>
       </c>
@@ -10514,7 +10510,7 @@
         <v>233</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>679</v>
+        <v>672</v>
       </c>
       <c r="E23" s="1">
         <v>3</v>
@@ -10564,16 +10560,16 @@
         <v>100</v>
       </c>
       <c r="T23" s="11" t="s">
-        <v>681</v>
+        <v>674</v>
       </c>
       <c r="U23" s="7" t="s">
-        <v>677</v>
+        <v>670</v>
       </c>
       <c r="V23" s="1" t="s">
-        <v>678</v>
+        <v>671</v>
       </c>
       <c r="W23" s="1" t="s">
-        <v>678</v>
+        <v>671</v>
       </c>
       <c r="X23" s="1">
         <v>11000007</v>
@@ -10591,7 +10587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="24" hidden="1">
+    <row r="24" spans="1:28" ht="24">
       <c r="A24">
         <v>53000021</v>
       </c>
@@ -10602,7 +10598,7 @@
         <v>234</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>685</v>
+        <v>678</v>
       </c>
       <c r="E24" s="1">
         <v>3</v>
@@ -10652,10 +10648,10 @@
         <v>100</v>
       </c>
       <c r="T24" s="11" t="s">
-        <v>683</v>
+        <v>676</v>
       </c>
       <c r="U24" s="7" t="s">
-        <v>684</v>
+        <v>677</v>
       </c>
       <c r="V24" s="1" t="s">
         <v>26</v>
@@ -10679,7 +10675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="24" hidden="1">
+    <row r="25" spans="1:28" ht="24">
       <c r="A25">
         <v>53000022</v>
       </c>
@@ -10690,7 +10686,7 @@
         <v>235</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>717</v>
+        <v>710</v>
       </c>
       <c r="E25" s="1">
         <v>4</v>
@@ -10740,10 +10736,10 @@
         <v>107</v>
       </c>
       <c r="T25" s="11" t="s">
-        <v>716</v>
+        <v>709</v>
       </c>
       <c r="U25" s="7" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="V25" s="1" t="s">
         <v>29</v>
@@ -10765,7 +10761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="24" hidden="1">
+    <row r="26" spans="1:28" ht="24">
       <c r="A26">
         <v>53000023</v>
       </c>
@@ -10776,7 +10772,7 @@
         <v>236</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="E26" s="1">
         <v>3</v>
@@ -10826,10 +10822,10 @@
         <v>100</v>
       </c>
       <c r="T26" s="11" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="U26" s="22" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="V26" s="1" t="s">
         <v>2</v>
@@ -10849,7 +10845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="24" hidden="1">
+    <row r="27" spans="1:28" ht="24">
       <c r="A27">
         <v>53000024</v>
       </c>
@@ -10860,7 +10856,7 @@
         <v>237</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="E27" s="1">
         <v>3</v>
@@ -10910,10 +10906,10 @@
         <v>90</v>
       </c>
       <c r="T27" s="11" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="U27" s="7" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="V27" s="1" t="s">
         <v>29</v>
@@ -10935,7 +10931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="60" hidden="1">
+    <row r="28" spans="1:28" ht="60">
       <c r="A28">
         <v>53000025</v>
       </c>
@@ -10946,7 +10942,7 @@
         <v>238</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="E28" s="1">
         <v>3</v>
@@ -10996,10 +10992,10 @@
         <v>100</v>
       </c>
       <c r="T28" s="11" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="U28" s="7" t="s">
-        <v>646</v>
+        <v>639</v>
       </c>
       <c r="V28" s="1" t="s">
         <v>33</v>
@@ -11021,7 +11017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="24" hidden="1">
+    <row r="29" spans="1:28" ht="24">
       <c r="A29">
         <v>53000026</v>
       </c>
@@ -11032,7 +11028,7 @@
         <v>239</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>686</v>
+        <v>679</v>
       </c>
       <c r="E29" s="1">
         <v>4</v>
@@ -11082,10 +11078,10 @@
         <v>100</v>
       </c>
       <c r="T29" s="11" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="U29" s="7" t="s">
-        <v>640</v>
+        <v>633</v>
       </c>
       <c r="V29" s="1" t="s">
         <v>36</v>
@@ -11107,7 +11103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:28" hidden="1">
+    <row r="30" spans="1:28">
       <c r="A30">
         <v>53000027</v>
       </c>
@@ -11118,7 +11114,7 @@
         <v>240</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
       <c r="E30" s="1">
         <v>1</v>
@@ -11168,10 +11164,10 @@
         <v>96</v>
       </c>
       <c r="T30" s="11" t="s">
-        <v>653</v>
+        <v>646</v>
       </c>
       <c r="U30" s="7" t="s">
-        <v>655</v>
+        <v>648</v>
       </c>
       <c r="V30" s="1" t="s">
         <v>39</v>
@@ -11191,7 +11187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:28" hidden="1">
+    <row r="31" spans="1:28">
       <c r="A31">
         <v>53000028</v>
       </c>
@@ -11202,7 +11198,7 @@
         <v>241</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>658</v>
+        <v>651</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
@@ -11252,10 +11248,10 @@
         <v>96</v>
       </c>
       <c r="T31" s="11" t="s">
-        <v>654</v>
+        <v>647</v>
       </c>
       <c r="U31" s="7" t="s">
-        <v>656</v>
+        <v>649</v>
       </c>
       <c r="V31" s="1" t="s">
         <v>41</v>
@@ -11275,7 +11271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:28" ht="24" hidden="1">
+    <row r="32" spans="1:28" ht="24">
       <c r="A32">
         <v>53000029</v>
       </c>
@@ -11286,7 +11282,7 @@
         <v>242</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>637</v>
+        <v>630</v>
       </c>
       <c r="E32" s="1">
         <v>4</v>
@@ -11336,7 +11332,7 @@
         <v>100</v>
       </c>
       <c r="T32" s="11" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="U32" s="22" t="s">
         <v>378</v>
@@ -11359,18 +11355,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:28" ht="24" hidden="1">
+    <row r="33" spans="1:28" ht="24">
       <c r="A33">
         <v>53000030</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
       <c r="E33" s="1">
         <v>1</v>
@@ -11420,10 +11416,10 @@
         <v>100</v>
       </c>
       <c r="T33" s="11" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="U33" s="1" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="V33" s="1" t="s">
         <v>4</v>
@@ -11445,18 +11441,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:28" ht="24" hidden="1">
+    <row r="34" spans="1:28" ht="24">
       <c r="A34">
         <v>53000031</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
       <c r="E34" s="1">
         <v>2</v>
@@ -11506,10 +11502,10 @@
         <v>100</v>
       </c>
       <c r="T34" s="11" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="U34" s="1" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="V34" s="1" t="s">
         <v>4</v>
@@ -11531,7 +11527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:28" ht="96" hidden="1">
+    <row r="35" spans="1:28" ht="96">
       <c r="A35">
         <v>53000032</v>
       </c>
@@ -11542,7 +11538,7 @@
         <v>314</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>692</v>
+        <v>685</v>
       </c>
       <c r="E35" s="1">
         <v>3</v>
@@ -11592,16 +11588,16 @@
         <v>100</v>
       </c>
       <c r="T35" s="11" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="U35" s="7" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="V35" s="1" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="W35" s="1" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="X35" s="1">
         <v>11000009</v>
@@ -11619,7 +11615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:28" ht="60" hidden="1">
+    <row r="36" spans="1:28" ht="60">
       <c r="A36">
         <v>53000033</v>
       </c>
@@ -11630,10 +11626,10 @@
         <v>315</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>543</v>
+        <v>765</v>
       </c>
       <c r="E36" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F36">
         <v>201</v>
@@ -11646,7 +11642,7 @@
         <v>6</v>
       </c>
       <c r="I36" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J36" s="1">
         <v>0</v>
@@ -11680,7 +11676,7 @@
         <v>150</v>
       </c>
       <c r="T36" s="11" t="s">
-        <v>631</v>
+        <v>624</v>
       </c>
       <c r="U36" s="7" t="s">
         <v>392</v>
@@ -11691,7 +11687,9 @@
       <c r="W36" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="X36" s="1"/>
+      <c r="X36" s="1">
+        <v>11000007</v>
+      </c>
       <c r="Y36" s="1">
         <v>4</v>
       </c>
@@ -11705,7 +11703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:28" ht="60" hidden="1">
+    <row r="37" spans="1:28" ht="60">
       <c r="A37">
         <v>53000034</v>
       </c>
@@ -11716,7 +11714,7 @@
         <v>309</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>674</v>
+        <v>667</v>
       </c>
       <c r="E37" s="1">
         <v>1</v>
@@ -11791,7 +11789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:28" ht="60" hidden="1">
+    <row r="38" spans="1:28" ht="60">
       <c r="A38">
         <v>53000035</v>
       </c>
@@ -11802,7 +11800,7 @@
         <v>243</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E38" s="1">
         <v>3</v>
@@ -11852,7 +11850,7 @@
         <v>100</v>
       </c>
       <c r="T38" s="11" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="U38" s="7" t="s">
         <v>357</v>
@@ -11875,7 +11873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:28" ht="48" hidden="1">
+    <row r="39" spans="1:28" ht="48">
       <c r="A39">
         <v>53000036</v>
       </c>
@@ -11886,7 +11884,7 @@
         <v>244</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="E39" s="1">
         <v>2</v>
@@ -11937,10 +11935,10 @@
         <v>61</v>
       </c>
       <c r="T39" s="11" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
       <c r="U39" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="V39" s="1" t="s">
         <v>52</v>
@@ -11960,7 +11958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:28" ht="24" hidden="1">
+    <row r="40" spans="1:28" ht="24">
       <c r="A40">
         <v>53000037</v>
       </c>
@@ -11971,7 +11969,7 @@
         <v>245</v>
       </c>
       <c r="D40" s="26" t="s">
-        <v>649</v>
+        <v>642</v>
       </c>
       <c r="E40" s="1">
         <v>1</v>
@@ -12021,10 +12019,10 @@
         <v>100</v>
       </c>
       <c r="T40" s="11" t="s">
-        <v>644</v>
+        <v>637</v>
       </c>
       <c r="U40" s="7" t="s">
-        <v>647</v>
+        <v>640</v>
       </c>
       <c r="V40" s="1" t="s">
         <v>54</v>
@@ -12044,7 +12042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:28" ht="36" hidden="1">
+    <row r="41" spans="1:28" ht="36">
       <c r="A41">
         <v>53000038</v>
       </c>
@@ -12055,7 +12053,7 @@
         <v>246</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>650</v>
+        <v>643</v>
       </c>
       <c r="E41" s="1">
         <v>2</v>
@@ -12105,10 +12103,10 @@
         <v>100</v>
       </c>
       <c r="T41" s="11" t="s">
-        <v>645</v>
+        <v>638</v>
       </c>
       <c r="U41" s="7" t="s">
-        <v>648</v>
+        <v>641</v>
       </c>
       <c r="V41" s="1" t="s">
         <v>56</v>
@@ -12130,18 +12128,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:28" ht="24" hidden="1">
+    <row r="42" spans="1:28" ht="24">
       <c r="A42">
         <v>53000039</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D42" s="26" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="E42" s="1">
         <v>1</v>
@@ -12191,10 +12189,10 @@
         <v>85</v>
       </c>
       <c r="T42" s="11" t="s">
-        <v>642</v>
+        <v>635</v>
       </c>
       <c r="U42" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="V42" s="1" t="s">
         <v>4</v>
@@ -12216,18 +12214,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:28" ht="24" hidden="1">
+    <row r="43" spans="1:28" ht="24">
       <c r="A43">
         <v>53000040</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>247</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="E43" s="1">
         <v>2</v>
@@ -12277,10 +12275,10 @@
         <v>100</v>
       </c>
       <c r="T43" s="11" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="U43" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="V43" s="1" t="s">
         <v>4</v>
@@ -12302,7 +12300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:28" ht="24" hidden="1">
+    <row r="44" spans="1:28" ht="24">
       <c r="A44">
         <v>53000041</v>
       </c>
@@ -12313,7 +12311,7 @@
         <v>248</v>
       </c>
       <c r="D44" s="26" t="s">
-        <v>749</v>
+        <v>741</v>
       </c>
       <c r="E44" s="1">
         <v>2</v>
@@ -12366,7 +12364,7 @@
         <v>398</v>
       </c>
       <c r="U44" s="7" t="s">
-        <v>750</v>
+        <v>742</v>
       </c>
       <c r="V44" s="1" t="s">
         <v>58</v>
@@ -12386,7 +12384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:28" ht="60" hidden="1">
+    <row r="45" spans="1:28" ht="60">
       <c r="A45">
         <v>53000042</v>
       </c>
@@ -12397,7 +12395,7 @@
         <v>249</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E45" s="1">
         <v>3</v>
@@ -12447,7 +12445,7 @@
         <v>100</v>
       </c>
       <c r="T45" s="11" t="s">
-        <v>651</v>
+        <v>644</v>
       </c>
       <c r="U45" s="1" t="s">
         <v>358</v>
@@ -12470,7 +12468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:28" ht="24" hidden="1">
+    <row r="46" spans="1:28" ht="24">
       <c r="A46">
         <v>53000043</v>
       </c>
@@ -12481,7 +12479,7 @@
         <v>250</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>700</v>
+        <v>693</v>
       </c>
       <c r="E46" s="1">
         <v>2</v>
@@ -12531,10 +12529,10 @@
         <v>100</v>
       </c>
       <c r="T46" s="11" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="U46" s="1" t="s">
-        <v>699</v>
+        <v>692</v>
       </c>
       <c r="V46" s="1" t="s">
         <v>4</v>
@@ -12556,18 +12554,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:28" ht="24" hidden="1">
+    <row r="47" spans="1:28" ht="24">
       <c r="A47">
         <v>53000044</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>251</v>
       </c>
       <c r="D47" s="26" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
       <c r="E47" s="1">
         <v>3</v>
@@ -12617,10 +12615,10 @@
         <v>95</v>
       </c>
       <c r="T47" s="11" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="U47" s="1" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="V47" s="1" t="s">
         <v>4</v>
@@ -12642,7 +12640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:28" ht="72" hidden="1">
+    <row r="48" spans="1:28" ht="72">
       <c r="A48">
         <v>53000045</v>
       </c>
@@ -12653,7 +12651,7 @@
         <v>252</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>660</v>
+        <v>653</v>
       </c>
       <c r="E48" s="1">
         <v>2</v>
@@ -12703,10 +12701,10 @@
         <v>100</v>
       </c>
       <c r="T48" s="11" t="s">
-        <v>661</v>
+        <v>654</v>
       </c>
       <c r="U48" s="1" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
       <c r="V48" s="1" t="s">
         <v>342</v>
@@ -12728,7 +12726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:28" ht="60" hidden="1">
+    <row r="49" spans="1:28" ht="60">
       <c r="A49">
         <v>53000046</v>
       </c>
@@ -12739,7 +12737,7 @@
         <v>253</v>
       </c>
       <c r="D49" s="26" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E49" s="1">
         <v>5</v>
@@ -12789,7 +12787,7 @@
         <v>100</v>
       </c>
       <c r="T49" s="11" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="U49" s="7" t="s">
         <v>368</v>
@@ -12812,7 +12810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:28" ht="72" hidden="1">
+    <row r="50" spans="1:28" ht="72">
       <c r="A50">
         <v>53000047</v>
       </c>
@@ -12823,7 +12821,7 @@
         <v>254</v>
       </c>
       <c r="D50" s="26" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E50" s="1">
         <v>5</v>
@@ -12873,7 +12871,7 @@
         <v>110</v>
       </c>
       <c r="T50" s="11" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="U50" s="7" t="s">
         <v>369</v>
@@ -12898,7 +12896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:28" ht="60" hidden="1">
+    <row r="51" spans="1:28" ht="60">
       <c r="A51">
         <v>53000048</v>
       </c>
@@ -12909,7 +12907,7 @@
         <v>255</v>
       </c>
       <c r="D51" s="26" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E51" s="1">
         <v>3</v>
@@ -12959,10 +12957,10 @@
         <v>100</v>
       </c>
       <c r="T51" s="11" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="U51" s="1" t="s">
-        <v>751</v>
+        <v>743</v>
       </c>
       <c r="V51" s="1" t="s">
         <v>21</v>
@@ -12982,7 +12980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:28" ht="72" hidden="1">
+    <row r="52" spans="1:28" ht="72">
       <c r="A52">
         <v>53000049</v>
       </c>
@@ -12993,7 +12991,7 @@
         <v>256</v>
       </c>
       <c r="D52" s="26" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E52" s="1">
         <v>3</v>
@@ -13043,7 +13041,7 @@
         <v>110</v>
       </c>
       <c r="T52" s="11" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="U52" s="7" t="s">
         <v>370</v>
@@ -13068,7 +13066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:28" ht="84" hidden="1">
+    <row r="53" spans="1:28" ht="84">
       <c r="A53">
         <v>53000050</v>
       </c>
@@ -13079,7 +13077,7 @@
         <v>257</v>
       </c>
       <c r="D53" s="26" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E53" s="1">
         <v>4</v>
@@ -13123,16 +13121,16 @@
         <v>0</v>
       </c>
       <c r="R53" s="7" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="S53">
         <v>90</v>
       </c>
       <c r="T53" s="11" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="U53" s="7" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="V53" s="1" t="s">
         <v>71</v>
@@ -13152,7 +13150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:28" ht="60" hidden="1">
+    <row r="54" spans="1:28" ht="60">
       <c r="A54">
         <v>53000051</v>
       </c>
@@ -13163,7 +13161,7 @@
         <v>258</v>
       </c>
       <c r="D54" s="26" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E54" s="1">
         <v>3</v>
@@ -13213,7 +13211,7 @@
         <v>100</v>
       </c>
       <c r="T54" s="11" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="U54" s="1" t="s">
         <v>359</v>
@@ -13236,7 +13234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:28" ht="60" hidden="1">
+    <row r="55" spans="1:28" ht="60">
       <c r="A55">
         <v>53000052</v>
       </c>
@@ -13247,7 +13245,7 @@
         <v>259</v>
       </c>
       <c r="D55" s="26" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E55" s="1">
         <v>3</v>
@@ -13297,7 +13295,7 @@
         <v>100</v>
       </c>
       <c r="T55" s="11" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="U55" s="1" t="s">
         <v>360</v>
@@ -13320,7 +13318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:28" ht="60" hidden="1">
+    <row r="56" spans="1:28" ht="60">
       <c r="A56">
         <v>53000053</v>
       </c>
@@ -13331,7 +13329,7 @@
         <v>260</v>
       </c>
       <c r="D56" s="26" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E56" s="1">
         <v>3</v>
@@ -13381,7 +13379,7 @@
         <v>100</v>
       </c>
       <c r="T56" s="11" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="U56" s="1" t="s">
         <v>361</v>
@@ -13404,7 +13402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:28" ht="60" hidden="1">
+    <row r="57" spans="1:28" ht="60">
       <c r="A57">
         <v>53000054</v>
       </c>
@@ -13415,7 +13413,7 @@
         <v>207</v>
       </c>
       <c r="D57" s="26" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E57" s="1">
         <v>3</v>
@@ -13465,7 +13463,7 @@
         <v>83.5</v>
       </c>
       <c r="T57" s="11" t="s">
-        <v>641</v>
+        <v>634</v>
       </c>
       <c r="U57" s="7" t="s">
         <v>403</v>
@@ -13488,7 +13486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:28" ht="36" hidden="1">
+    <row r="58" spans="1:28" ht="36">
       <c r="A58">
         <v>53000055</v>
       </c>
@@ -13499,7 +13497,7 @@
         <v>261</v>
       </c>
       <c r="D58" s="26" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
       <c r="E58" s="1">
         <v>3</v>
@@ -13549,10 +13547,10 @@
         <v>100</v>
       </c>
       <c r="T58" s="11" t="s">
-        <v>701</v>
+        <v>694</v>
       </c>
       <c r="U58" s="1" t="s">
-        <v>702</v>
+        <v>695</v>
       </c>
       <c r="V58" s="1" t="s">
         <v>2</v>
@@ -13574,7 +13572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:28" ht="48" hidden="1">
+    <row r="59" spans="1:28" ht="48">
       <c r="A59">
         <v>53000056</v>
       </c>
@@ -13585,7 +13583,7 @@
         <v>262</v>
       </c>
       <c r="D59" s="26" t="s">
-        <v>697</v>
+        <v>690</v>
       </c>
       <c r="E59" s="1">
         <v>2</v>
@@ -13635,10 +13633,10 @@
         <v>100</v>
       </c>
       <c r="T59" s="11" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="U59" s="1" t="s">
-        <v>715</v>
+        <v>708</v>
       </c>
       <c r="V59" s="1" t="s">
         <v>82</v>
@@ -13660,7 +13658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:28" ht="24" hidden="1">
+    <row r="60" spans="1:28" ht="24">
       <c r="A60">
         <v>53000057</v>
       </c>
@@ -13671,7 +13669,7 @@
         <v>317</v>
       </c>
       <c r="D60" s="26" t="s">
-        <v>694</v>
+        <v>687</v>
       </c>
       <c r="E60" s="1">
         <v>1</v>
@@ -13715,19 +13713,19 @@
         <v>3</v>
       </c>
       <c r="R60" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="S60">
         <v>100</v>
       </c>
       <c r="T60" s="11" t="s">
-        <v>695</v>
+        <v>688</v>
       </c>
       <c r="U60" s="1" t="s">
-        <v>696</v>
+        <v>689</v>
       </c>
       <c r="V60" s="1" t="s">
-        <v>693</v>
+        <v>686</v>
       </c>
       <c r="W60" s="1"/>
       <c r="X60" s="1">
@@ -13746,7 +13744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:28" ht="24" hidden="1">
+    <row r="61" spans="1:28" ht="24">
       <c r="A61">
         <v>53000058</v>
       </c>
@@ -13757,7 +13755,7 @@
         <v>263</v>
       </c>
       <c r="D61" s="26" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="E61" s="1">
         <v>1</v>
@@ -13807,7 +13805,7 @@
         <v>90</v>
       </c>
       <c r="T61" s="11" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="U61" s="7" t="s">
         <v>362</v>
@@ -13830,7 +13828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:28" ht="36" hidden="1">
+    <row r="62" spans="1:28" ht="36">
       <c r="A62">
         <v>53000059</v>
       </c>
@@ -13841,7 +13839,7 @@
         <v>264</v>
       </c>
       <c r="D62" s="26" t="s">
-        <v>667</v>
+        <v>660</v>
       </c>
       <c r="E62" s="1">
         <v>2</v>
@@ -13891,7 +13889,7 @@
         <v>100</v>
       </c>
       <c r="T62" s="11" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="U62" s="7" t="s">
         <v>399</v>
@@ -13916,7 +13914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:28" ht="48" hidden="1">
+    <row r="63" spans="1:28" ht="48">
       <c r="A63">
         <v>53000060</v>
       </c>
@@ -13927,7 +13925,7 @@
         <v>265</v>
       </c>
       <c r="D63" s="26" t="s">
-        <v>666</v>
+        <v>659</v>
       </c>
       <c r="E63" s="1">
         <v>1</v>
@@ -13977,10 +13975,10 @@
         <v>100</v>
       </c>
       <c r="T63" s="11" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="U63" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="V63" s="1" t="s">
         <v>87</v>
@@ -14002,7 +14000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:28" ht="60" hidden="1">
+    <row r="64" spans="1:28" ht="60">
       <c r="A64">
         <v>53000061</v>
       </c>
@@ -14013,7 +14011,7 @@
         <v>266</v>
       </c>
       <c r="D64" s="26" t="s">
-        <v>663</v>
+        <v>656</v>
       </c>
       <c r="E64" s="1">
         <v>4</v>
@@ -14063,7 +14061,7 @@
         <v>100</v>
       </c>
       <c r="T64" s="11" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="U64" s="7" t="s">
         <v>393</v>
@@ -14088,7 +14086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:28" ht="24" hidden="1">
+    <row r="65" spans="1:28" ht="24">
       <c r="A65">
         <v>53000062</v>
       </c>
@@ -14099,7 +14097,7 @@
         <v>267</v>
       </c>
       <c r="D65" s="26" t="s">
-        <v>665</v>
+        <v>658</v>
       </c>
       <c r="E65" s="1">
         <v>1</v>
@@ -14149,7 +14147,7 @@
         <v>100</v>
       </c>
       <c r="T65" s="11" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
       <c r="U65" s="7" t="s">
         <v>363</v>
@@ -14174,7 +14172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:28" hidden="1">
+    <row r="66" spans="1:28">
       <c r="A66">
         <v>53000063</v>
       </c>
@@ -14185,7 +14183,7 @@
         <v>268</v>
       </c>
       <c r="D66" s="26" t="s">
-        <v>705</v>
+        <v>698</v>
       </c>
       <c r="E66" s="1">
         <v>1</v>
@@ -14235,10 +14233,10 @@
         <v>100</v>
       </c>
       <c r="T66" s="11" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="U66" s="7" t="s">
-        <v>706</v>
+        <v>699</v>
       </c>
       <c r="V66" s="1" t="s">
         <v>94</v>
@@ -14260,7 +14258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:28" ht="24" hidden="1">
+    <row r="67" spans="1:28" ht="24">
       <c r="A67">
         <v>53000064</v>
       </c>
@@ -14271,7 +14269,7 @@
         <v>269</v>
       </c>
       <c r="D67" s="26" t="s">
-        <v>700</v>
+        <v>693</v>
       </c>
       <c r="E67" s="1">
         <v>2</v>
@@ -14321,10 +14319,10 @@
         <v>100</v>
       </c>
       <c r="T67" s="11" t="s">
-        <v>708</v>
+        <v>701</v>
       </c>
       <c r="U67" s="1" t="s">
-        <v>707</v>
+        <v>700</v>
       </c>
       <c r="V67" s="1" t="s">
         <v>96</v>
@@ -14346,7 +14344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:28" ht="60" hidden="1">
+    <row r="68" spans="1:28" ht="60">
       <c r="A68">
         <v>53000065</v>
       </c>
@@ -14357,7 +14355,7 @@
         <v>209</v>
       </c>
       <c r="D68" s="26" t="s">
-        <v>664</v>
+        <v>657</v>
       </c>
       <c r="E68" s="1">
         <v>6</v>
@@ -14407,10 +14405,10 @@
         <v>100</v>
       </c>
       <c r="T68" s="11" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
       <c r="U68" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="V68" s="1" t="s">
         <v>97</v>
@@ -14432,7 +14430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:28" ht="24" hidden="1">
+    <row r="69" spans="1:28" ht="24">
       <c r="A69">
         <v>53000066</v>
       </c>
@@ -14443,7 +14441,7 @@
         <v>270</v>
       </c>
       <c r="D69" s="26" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="E69" s="1">
         <v>2</v>
@@ -14493,10 +14491,10 @@
         <v>85</v>
       </c>
       <c r="T69" s="11" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
       <c r="U69" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="V69" s="1" t="s">
         <v>4</v>
@@ -14518,7 +14516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:28" ht="36" hidden="1">
+    <row r="70" spans="1:28" ht="36">
       <c r="A70">
         <v>53000067</v>
       </c>
@@ -14529,7 +14527,7 @@
         <v>271</v>
       </c>
       <c r="D70" s="26" t="s">
-        <v>670</v>
+        <v>663</v>
       </c>
       <c r="E70" s="1">
         <v>3</v>
@@ -14579,10 +14577,10 @@
         <v>100</v>
       </c>
       <c r="T70" s="11" t="s">
-        <v>669</v>
+        <v>662</v>
       </c>
       <c r="U70" s="7" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="V70" s="1" t="s">
         <v>99</v>
@@ -14604,7 +14602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:28" ht="72" hidden="1">
+    <row r="71" spans="1:28" ht="72">
       <c r="A71">
         <v>53000068</v>
       </c>
@@ -14615,7 +14613,7 @@
         <v>272</v>
       </c>
       <c r="D71" s="26" t="s">
-        <v>720</v>
+        <v>713</v>
       </c>
       <c r="E71" s="1">
         <v>2</v>
@@ -14665,10 +14663,10 @@
         <v>100</v>
       </c>
       <c r="T71" s="11" t="s">
-        <v>718</v>
+        <v>711</v>
       </c>
       <c r="U71" s="7" t="s">
-        <v>719</v>
+        <v>712</v>
       </c>
       <c r="V71" s="1" t="s">
         <v>101</v>
@@ -14692,7 +14690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:28" ht="60" hidden="1">
+    <row r="72" spans="1:28" ht="60">
       <c r="A72">
         <v>53000069</v>
       </c>
@@ -14703,7 +14701,7 @@
         <v>212</v>
       </c>
       <c r="D72" s="26" t="s">
-        <v>724</v>
+        <v>717</v>
       </c>
       <c r="E72" s="1">
         <v>2</v>
@@ -14753,10 +14751,10 @@
         <v>100</v>
       </c>
       <c r="T72" s="11" t="s">
-        <v>725</v>
+        <v>718</v>
       </c>
       <c r="U72" s="7" t="s">
-        <v>723</v>
+        <v>716</v>
       </c>
       <c r="V72" s="1" t="s">
         <v>103</v>
@@ -14778,7 +14776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:28" ht="36" hidden="1">
+    <row r="73" spans="1:28" ht="36">
       <c r="A73">
         <v>53000070</v>
       </c>
@@ -14789,7 +14787,7 @@
         <v>214</v>
       </c>
       <c r="D73" s="26" t="s">
-        <v>724</v>
+        <v>717</v>
       </c>
       <c r="E73" s="1">
         <v>2</v>
@@ -14839,10 +14837,10 @@
         <v>100</v>
       </c>
       <c r="T73" s="11" t="s">
-        <v>729</v>
+        <v>722</v>
       </c>
       <c r="U73" s="7" t="s">
-        <v>730</v>
+        <v>723</v>
       </c>
       <c r="V73" s="1" t="s">
         <v>105</v>
@@ -14875,7 +14873,7 @@
         <v>211</v>
       </c>
       <c r="D74" s="26" t="s">
-        <v>761</v>
+        <v>753</v>
       </c>
       <c r="E74" s="1">
         <v>4</v>
@@ -14925,10 +14923,10 @@
         <v>103</v>
       </c>
       <c r="T74" s="11" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="U74" s="7" t="s">
-        <v>764</v>
+        <v>756</v>
       </c>
       <c r="V74" s="1" t="s">
         <v>107</v>
@@ -14963,7 +14961,7 @@
         <v>273</v>
       </c>
       <c r="D75" s="26" t="s">
-        <v>761</v>
+        <v>753</v>
       </c>
       <c r="E75" s="1">
         <v>3</v>
@@ -15013,10 +15011,10 @@
         <v>102</v>
       </c>
       <c r="T75" s="11" t="s">
-        <v>767</v>
+        <v>759</v>
       </c>
       <c r="U75" s="1" t="s">
-        <v>763</v>
+        <v>755</v>
       </c>
       <c r="V75" s="1" t="s">
         <v>109</v>
@@ -15038,7 +15036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:28" ht="48" hidden="1">
+    <row r="76" spans="1:28" ht="48">
       <c r="A76">
         <v>53000073</v>
       </c>
@@ -15049,7 +15047,7 @@
         <v>274</v>
       </c>
       <c r="D76" s="26" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="E76" s="1">
         <v>3</v>
@@ -15099,10 +15097,10 @@
         <v>95</v>
       </c>
       <c r="T76" s="11" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="U76" s="7" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="V76" s="1" t="s">
         <v>111</v>
@@ -15122,7 +15120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:28" ht="36" hidden="1">
+    <row r="77" spans="1:28" ht="36">
       <c r="A77">
         <v>53000074</v>
       </c>
@@ -15133,7 +15131,7 @@
         <v>316</v>
       </c>
       <c r="D77" s="26" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="E77" s="1">
         <v>4</v>
@@ -15206,7 +15204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:28" ht="132" hidden="1">
+    <row r="78" spans="1:28" ht="132">
       <c r="A78">
         <v>53000075</v>
       </c>
@@ -15217,7 +15215,7 @@
         <v>275</v>
       </c>
       <c r="D78" s="26" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="E78" s="1">
         <v>4</v>
@@ -15267,7 +15265,7 @@
         <v>180</v>
       </c>
       <c r="T78" s="11" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="U78" s="7" t="s">
         <v>364</v>
@@ -15290,7 +15288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:28" ht="72" hidden="1">
+    <row r="79" spans="1:28" ht="72">
       <c r="A79">
         <v>53000076</v>
       </c>
@@ -15301,7 +15299,7 @@
         <v>276</v>
       </c>
       <c r="D79" s="26" t="s">
-        <v>738</v>
+        <v>731</v>
       </c>
       <c r="E79" s="1">
         <v>3</v>
@@ -15351,10 +15349,10 @@
         <v>100</v>
       </c>
       <c r="T79" s="11" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="U79" s="7" t="s">
-        <v>739</v>
+        <v>732</v>
       </c>
       <c r="V79" s="1" t="s">
         <v>117</v>
@@ -15378,7 +15376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:28" ht="48" hidden="1">
+    <row r="80" spans="1:28" ht="48">
       <c r="A80">
         <v>53000077</v>
       </c>
@@ -15389,7 +15387,7 @@
         <v>277</v>
       </c>
       <c r="D80" s="26" t="s">
-        <v>738</v>
+        <v>731</v>
       </c>
       <c r="E80" s="1">
         <v>3</v>
@@ -15439,7 +15437,7 @@
         <v>107</v>
       </c>
       <c r="T80" s="11" t="s">
-        <v>671</v>
+        <v>664</v>
       </c>
       <c r="U80" s="7" t="s">
         <v>365</v>
@@ -15464,7 +15462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:28" hidden="1">
+    <row r="81" spans="1:28">
       <c r="A81">
         <v>53000078</v>
       </c>
@@ -15475,7 +15473,7 @@
         <v>278</v>
       </c>
       <c r="D81" s="26" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="E81" s="1">
         <v>1</v>
@@ -15519,16 +15517,16 @@
         <v>0</v>
       </c>
       <c r="R81" s="1" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="S81">
         <v>50</v>
       </c>
       <c r="T81" s="43" t="s">
-        <v>672</v>
+        <v>665</v>
       </c>
       <c r="U81" s="7" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="V81" s="1" t="s">
         <v>97</v>
@@ -15548,7 +15546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:28" ht="72" hidden="1">
+    <row r="82" spans="1:28" ht="72">
       <c r="A82">
         <v>53000079</v>
       </c>
@@ -15559,7 +15557,7 @@
         <v>279</v>
       </c>
       <c r="D82" s="26" t="s">
-        <v>737</v>
+        <v>730</v>
       </c>
       <c r="E82" s="1">
         <v>3</v>
@@ -15609,10 +15607,10 @@
         <v>100</v>
       </c>
       <c r="T82" s="11" t="s">
-        <v>742</v>
+        <v>735</v>
       </c>
       <c r="U82" s="7" t="s">
-        <v>740</v>
+        <v>733</v>
       </c>
       <c r="V82" s="1" t="s">
         <v>121</v>
@@ -15636,7 +15634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:28" ht="72" hidden="1">
+    <row r="83" spans="1:28" ht="72">
       <c r="A83">
         <v>53000080</v>
       </c>
@@ -15647,7 +15645,7 @@
         <v>280</v>
       </c>
       <c r="D83" s="26" t="s">
-        <v>738</v>
+        <v>731</v>
       </c>
       <c r="E83" s="1">
         <v>2</v>
@@ -15697,7 +15695,7 @@
         <v>100</v>
       </c>
       <c r="T83" s="11" t="s">
-        <v>741</v>
+        <v>734</v>
       </c>
       <c r="U83" s="7" t="s">
         <v>366</v>
@@ -15724,7 +15722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:28" ht="72" hidden="1">
+    <row r="84" spans="1:28" ht="72">
       <c r="A84">
         <v>53000081</v>
       </c>
@@ -15735,7 +15733,7 @@
         <v>281</v>
       </c>
       <c r="D84" s="26" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E84" s="1">
         <v>3</v>
@@ -15785,7 +15783,7 @@
         <v>90</v>
       </c>
       <c r="T84" s="11" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="U84" s="7" t="s">
         <v>371</v>
@@ -15810,7 +15808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:28" ht="24" hidden="1">
+    <row r="85" spans="1:28" ht="24">
       <c r="A85">
         <v>53000082</v>
       </c>
@@ -15821,7 +15819,7 @@
         <v>282</v>
       </c>
       <c r="D85" s="26" t="s">
-        <v>727</v>
+        <v>720</v>
       </c>
       <c r="E85" s="1">
         <v>3</v>
@@ -15871,10 +15869,10 @@
         <v>100</v>
       </c>
       <c r="T85" s="11" t="s">
-        <v>726</v>
+        <v>719</v>
       </c>
       <c r="U85" s="7" t="s">
-        <v>728</v>
+        <v>721</v>
       </c>
       <c r="V85" s="1" t="s">
         <v>126</v>
@@ -15896,18 +15894,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:28" ht="24" hidden="1">
+    <row r="86" spans="1:28" ht="24">
       <c r="A86" s="42">
         <v>53000083</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>283</v>
       </c>
       <c r="D86" s="26" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="E86" s="1">
         <v>2</v>
@@ -15957,13 +15955,13 @@
         <v>60</v>
       </c>
       <c r="T86" s="11" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="U86" s="7" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="V86" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="W86" s="1"/>
       <c r="X86" s="1"/>
@@ -15980,7 +15978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:28" ht="24" hidden="1">
+    <row r="87" spans="1:28" ht="24">
       <c r="A87">
         <v>53000084</v>
       </c>
@@ -15991,7 +15989,7 @@
         <v>213</v>
       </c>
       <c r="D87" s="26" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="E87" s="1">
         <v>3</v>
@@ -16041,13 +16039,13 @@
         <v>40</v>
       </c>
       <c r="T87" s="11" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="U87" s="7" t="s">
         <v>391</v>
       </c>
       <c r="V87" s="1" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="W87" s="1"/>
       <c r="X87" s="1"/>
@@ -16064,7 +16062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:28" ht="84" hidden="1">
+    <row r="88" spans="1:28" ht="84">
       <c r="A88">
         <v>53000085</v>
       </c>
@@ -16075,7 +16073,7 @@
         <v>215</v>
       </c>
       <c r="D88" s="26" t="s">
-        <v>745</v>
+        <v>738</v>
       </c>
       <c r="E88" s="1">
         <v>3</v>
@@ -16119,16 +16117,16 @@
         <v>20</v>
       </c>
       <c r="R88" s="1" t="s">
-        <v>743</v>
+        <v>736</v>
       </c>
       <c r="S88">
         <v>100</v>
       </c>
       <c r="T88" s="11" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="U88" s="7" t="s">
-        <v>744</v>
+        <v>737</v>
       </c>
       <c r="V88" s="1" t="s">
         <v>127</v>
@@ -16152,7 +16150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:28" ht="60" hidden="1">
+    <row r="89" spans="1:28" ht="60">
       <c r="A89">
         <v>53000086</v>
       </c>
@@ -16163,7 +16161,7 @@
         <v>216</v>
       </c>
       <c r="D89" s="26" t="s">
-        <v>733</v>
+        <v>726</v>
       </c>
       <c r="E89" s="1">
         <v>2</v>
@@ -16213,10 +16211,10 @@
         <v>102</v>
       </c>
       <c r="T89" s="11" t="s">
-        <v>732</v>
+        <v>725</v>
       </c>
       <c r="U89" s="7" t="s">
-        <v>731</v>
+        <v>724</v>
       </c>
       <c r="V89" s="1" t="s">
         <v>2</v>
@@ -16238,7 +16236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:28" ht="72" hidden="1">
+    <row r="90" spans="1:28" ht="72">
       <c r="A90">
         <v>53000087</v>
       </c>
@@ -16249,7 +16247,7 @@
         <v>217</v>
       </c>
       <c r="D90" s="26" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E90" s="1">
         <v>3</v>
@@ -16299,10 +16297,10 @@
         <v>75</v>
       </c>
       <c r="T90" s="11" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="U90" s="7" t="s">
-        <v>652</v>
+        <v>645</v>
       </c>
       <c r="V90" s="1" t="s">
         <v>60</v>
@@ -16324,7 +16322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:28" ht="72" hidden="1">
+    <row r="91" spans="1:28" ht="72">
       <c r="A91">
         <v>53000088</v>
       </c>
@@ -16335,7 +16333,7 @@
         <v>284</v>
       </c>
       <c r="D91" s="26" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="E91" s="1">
         <v>3</v>
@@ -16385,7 +16383,7 @@
         <v>100</v>
       </c>
       <c r="T91" s="11" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="U91" s="7" t="s">
         <v>372</v>
@@ -16412,7 +16410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:28" ht="60" hidden="1">
+    <row r="92" spans="1:28" ht="60">
       <c r="A92">
         <v>53000089</v>
       </c>
@@ -16423,7 +16421,7 @@
         <v>285</v>
       </c>
       <c r="D92" s="26" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E92" s="1">
         <v>4</v>
@@ -16473,13 +16471,13 @@
         <v>90</v>
       </c>
       <c r="T92" s="11" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="U92" s="7" t="s">
         <v>369</v>
       </c>
       <c r="V92" s="1" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="W92" s="1" t="s">
         <v>135</v>
@@ -16498,7 +16496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:28" ht="72" hidden="1">
+    <row r="93" spans="1:28" ht="72">
       <c r="A93">
         <v>53000090</v>
       </c>
@@ -16509,7 +16507,7 @@
         <v>286</v>
       </c>
       <c r="D93" s="26" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E93" s="1">
         <v>4</v>
@@ -16559,10 +16557,10 @@
         <v>82.5</v>
       </c>
       <c r="T93" s="11" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="U93" s="7" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="V93" s="1" t="s">
         <v>21</v>
@@ -16584,7 +16582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:28" ht="36" hidden="1">
+    <row r="94" spans="1:28" ht="36">
       <c r="A94">
         <v>53000091</v>
       </c>
@@ -16595,7 +16593,7 @@
         <v>287</v>
       </c>
       <c r="D94" s="26" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="E94" s="1">
         <v>2</v>
@@ -16645,7 +16643,7 @@
         <v>100</v>
       </c>
       <c r="T94" s="11" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="U94" s="7" t="s">
         <v>373</v>
@@ -16668,7 +16666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:28" ht="72" hidden="1">
+    <row r="95" spans="1:28" ht="72">
       <c r="A95">
         <v>53000092</v>
       </c>
@@ -16679,7 +16677,7 @@
         <v>288</v>
       </c>
       <c r="D95" s="26" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E95" s="1">
         <v>3</v>
@@ -16729,7 +16727,7 @@
         <v>75</v>
       </c>
       <c r="T95" s="11" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="U95" s="7" t="s">
         <v>374</v>
@@ -16754,7 +16752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:28" ht="60" hidden="1">
+    <row r="96" spans="1:28" ht="60">
       <c r="A96">
         <v>53000093</v>
       </c>
@@ -16765,7 +16763,7 @@
         <v>289</v>
       </c>
       <c r="D96" s="26" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="E96" s="1">
         <v>3</v>
@@ -16815,7 +16813,7 @@
         <v>125</v>
       </c>
       <c r="T96" s="11" t="s">
-        <v>601</v>
+        <v>766</v>
       </c>
       <c r="U96" s="7" t="s">
         <v>388</v>
@@ -16838,7 +16836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:28" ht="36" hidden="1">
+    <row r="97" spans="1:28" ht="36">
       <c r="A97">
         <v>53000094</v>
       </c>
@@ -16849,7 +16847,7 @@
         <v>290</v>
       </c>
       <c r="D97" s="26" t="s">
-        <v>713</v>
+        <v>706</v>
       </c>
       <c r="E97" s="1">
         <v>2</v>
@@ -16899,10 +16897,10 @@
         <v>25</v>
       </c>
       <c r="T97" s="11" t="s">
-        <v>710</v>
+        <v>703</v>
       </c>
       <c r="U97" s="1" t="s">
-        <v>709</v>
+        <v>702</v>
       </c>
       <c r="V97" s="1" t="s">
         <v>143</v>
@@ -16924,7 +16922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:28" ht="60" hidden="1">
+    <row r="98" spans="1:28" ht="72">
       <c r="A98">
         <v>53000095</v>
       </c>
@@ -16935,7 +16933,7 @@
         <v>291</v>
       </c>
       <c r="D98" s="26" t="s">
-        <v>535</v>
+        <v>765</v>
       </c>
       <c r="E98" s="1">
         <v>2</v>
@@ -16957,7 +16955,7 @@
         <v>0</v>
       </c>
       <c r="K98" s="1">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="L98" s="1">
         <v>0</v>
@@ -16985,10 +16983,10 @@
         <v>80</v>
       </c>
       <c r="T98" s="11" t="s">
-        <v>559</v>
+        <v>767</v>
       </c>
       <c r="U98" s="7" t="s">
-        <v>746</v>
+        <v>764</v>
       </c>
       <c r="V98" s="1" t="s">
         <v>145</v>
@@ -16996,7 +16994,9 @@
       <c r="W98" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="X98" s="1"/>
+      <c r="X98" s="1">
+        <v>11000008</v>
+      </c>
       <c r="Y98" s="1">
         <v>4</v>
       </c>
@@ -17010,21 +17010,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:28" ht="24" hidden="1">
+    <row r="99" spans="1:28" ht="36">
       <c r="A99">
         <v>53000096</v>
       </c>
-      <c r="B99" s="34" t="s">
+      <c r="B99" s="8" t="s">
         <v>146</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>292</v>
       </c>
       <c r="D99" s="26" t="s">
-        <v>630</v>
+        <v>763</v>
       </c>
       <c r="E99" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F99">
         <v>202</v>
@@ -17034,16 +17034,16 @@
       </c>
       <c r="H99" s="1">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I99" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J99" s="1">
         <v>0</v>
       </c>
       <c r="K99" s="1">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="L99" s="1">
         <v>0</v>
@@ -17059,28 +17059,30 @@
       </c>
       <c r="P99" s="41">
         <f t="shared" si="5"/>
-        <v>-51</v>
+        <v>3</v>
       </c>
       <c r="Q99" s="1">
         <v>200</v>
       </c>
       <c r="R99" s="1" t="s">
-        <v>1</v>
+        <v>761</v>
       </c>
       <c r="S99">
-        <v>50</v>
+        <v>104</v>
       </c>
       <c r="T99" s="11" t="s">
-        <v>430</v>
+        <v>760</v>
       </c>
       <c r="U99" s="1" t="s">
-        <v>429</v>
+        <v>762</v>
       </c>
       <c r="V99" s="1" t="s">
         <v>29</v>
       </c>
       <c r="W99" s="1"/>
-      <c r="X99" s="1"/>
+      <c r="X99" s="1">
+        <v>11000008</v>
+      </c>
       <c r="Y99" s="1">
         <v>4</v>
       </c>
@@ -17094,7 +17096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:28" ht="72" hidden="1">
+    <row r="100" spans="1:28" ht="72">
       <c r="A100">
         <v>53000097</v>
       </c>
@@ -17105,7 +17107,7 @@
         <v>293</v>
       </c>
       <c r="D100" s="26" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="E100" s="1">
         <v>2</v>
@@ -17155,7 +17157,7 @@
         <v>45</v>
       </c>
       <c r="T100" s="11" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="U100" s="7" t="s">
         <v>367</v>
@@ -17180,7 +17182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:28" ht="36" hidden="1">
+    <row r="101" spans="1:28" ht="36">
       <c r="A101">
         <v>53000098</v>
       </c>
@@ -17191,7 +17193,7 @@
         <v>294</v>
       </c>
       <c r="D101" s="26" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="E101" s="1">
         <v>4</v>
@@ -17241,7 +17243,7 @@
         <v>110</v>
       </c>
       <c r="T101" s="11" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="U101" s="7" t="s">
         <v>376</v>
@@ -17264,7 +17266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:28" ht="36" hidden="1">
+    <row r="102" spans="1:28" ht="36">
       <c r="A102">
         <v>53000099</v>
       </c>
@@ -17275,7 +17277,7 @@
         <v>295</v>
       </c>
       <c r="D102" s="26" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="E102" s="1">
         <v>2</v>
@@ -17325,7 +17327,7 @@
         <v>95</v>
       </c>
       <c r="T102" s="11" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="U102" s="7" t="s">
         <v>375</v>
@@ -17348,7 +17350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:28" ht="24" hidden="1">
+    <row r="103" spans="1:28" ht="24">
       <c r="A103">
         <v>53000100</v>
       </c>
@@ -17359,7 +17361,7 @@
         <v>296</v>
       </c>
       <c r="D103" s="26" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="E103" s="1">
         <v>3</v>
@@ -17432,7 +17434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:28" ht="24" hidden="1">
+    <row r="104" spans="1:28" ht="24">
       <c r="A104">
         <v>53000101</v>
       </c>
@@ -17443,7 +17445,7 @@
         <v>308</v>
       </c>
       <c r="D104" s="26" t="s">
-        <v>675</v>
+        <v>668</v>
       </c>
       <c r="E104" s="1">
         <v>2</v>
@@ -17516,7 +17518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:28" ht="24" hidden="1">
+    <row r="105" spans="1:28" ht="24">
       <c r="A105">
         <v>53000102</v>
       </c>
@@ -17527,7 +17529,7 @@
         <v>297</v>
       </c>
       <c r="D105" s="26" t="s">
-        <v>762</v>
+        <v>754</v>
       </c>
       <c r="E105" s="1">
         <v>3</v>
@@ -17577,7 +17579,7 @@
         <v>100</v>
       </c>
       <c r="T105" s="11" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="U105" s="7" t="s">
         <v>377</v>
@@ -17602,7 +17604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:28" ht="72" hidden="1">
+    <row r="106" spans="1:28" ht="72">
       <c r="A106">
         <v>53000103</v>
       </c>
@@ -17613,7 +17615,7 @@
         <v>298</v>
       </c>
       <c r="D106" s="26" t="s">
-        <v>733</v>
+        <v>726</v>
       </c>
       <c r="E106" s="1">
         <v>3</v>
@@ -17663,10 +17665,10 @@
         <v>105</v>
       </c>
       <c r="T106" s="11" t="s">
-        <v>734</v>
+        <v>727</v>
       </c>
       <c r="U106" s="7" t="s">
-        <v>735</v>
+        <v>728</v>
       </c>
       <c r="V106" s="1" t="s">
         <v>154</v>
@@ -17690,7 +17692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:28" ht="60" hidden="1">
+    <row r="107" spans="1:28" ht="60">
       <c r="A107">
         <v>53000104</v>
       </c>
@@ -17701,7 +17703,7 @@
         <v>299</v>
       </c>
       <c r="D107" s="26" t="s">
-        <v>724</v>
+        <v>717</v>
       </c>
       <c r="E107" s="1">
         <v>3</v>
@@ -17751,10 +17753,10 @@
         <v>105</v>
       </c>
       <c r="T107" s="11" t="s">
-        <v>736</v>
+        <v>729</v>
       </c>
       <c r="U107" s="7" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="V107" s="1" t="s">
         <v>156</v>
@@ -17776,7 +17778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:28" ht="60" hidden="1">
+    <row r="108" spans="1:28" ht="60">
       <c r="A108">
         <v>53000105</v>
       </c>
@@ -17787,7 +17789,7 @@
         <v>219</v>
       </c>
       <c r="D108" s="26" t="s">
-        <v>714</v>
+        <v>707</v>
       </c>
       <c r="E108" s="1">
         <v>3</v>
@@ -17837,10 +17839,10 @@
         <v>25</v>
       </c>
       <c r="T108" s="11" t="s">
-        <v>712</v>
+        <v>705</v>
       </c>
       <c r="U108" s="1" t="s">
-        <v>711</v>
+        <v>704</v>
       </c>
       <c r="V108" s="1" t="s">
         <v>158</v>
@@ -17862,7 +17864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:28" ht="24" hidden="1">
+    <row r="109" spans="1:28" ht="24">
       <c r="A109">
         <v>53000106</v>
       </c>
@@ -17873,7 +17875,7 @@
         <v>300</v>
       </c>
       <c r="D109" s="26" t="s">
-        <v>737</v>
+        <v>730</v>
       </c>
       <c r="E109" s="1">
         <v>1</v>
@@ -17923,10 +17925,10 @@
         <v>100</v>
       </c>
       <c r="T109" s="11" t="s">
-        <v>721</v>
+        <v>714</v>
       </c>
       <c r="U109" s="7" t="s">
-        <v>722</v>
+        <v>715</v>
       </c>
       <c r="V109" s="1" t="s">
         <v>160</v>
@@ -17948,7 +17950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:28" ht="24" hidden="1">
+    <row r="110" spans="1:28" ht="24">
       <c r="A110">
         <v>53000107</v>
       </c>
@@ -17959,7 +17961,7 @@
         <v>301</v>
       </c>
       <c r="D110" s="26" t="s">
-        <v>738</v>
+        <v>731</v>
       </c>
       <c r="E110" s="1">
         <v>1</v>
@@ -18009,10 +18011,10 @@
         <v>100</v>
       </c>
       <c r="T110" s="11" t="s">
-        <v>673</v>
+        <v>666</v>
       </c>
       <c r="U110" s="7" t="s">
-        <v>755</v>
+        <v>747</v>
       </c>
       <c r="V110" s="1" t="s">
         <v>162</v>
@@ -18034,7 +18036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:28" ht="144" hidden="1">
+    <row r="111" spans="1:28" ht="144">
       <c r="A111">
         <v>53000108</v>
       </c>
@@ -18045,7 +18047,7 @@
         <v>302</v>
       </c>
       <c r="D111" s="26" t="s">
-        <v>761</v>
+        <v>753</v>
       </c>
       <c r="E111" s="1">
         <v>2</v>
@@ -18095,10 +18097,10 @@
         <v>100</v>
       </c>
       <c r="T111" s="11" t="s">
-        <v>759</v>
+        <v>751</v>
       </c>
       <c r="U111" s="7" t="s">
-        <v>760</v>
+        <v>752</v>
       </c>
       <c r="V111" s="1" t="s">
         <v>164</v>
@@ -18120,7 +18122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:28" ht="36" hidden="1">
+    <row r="112" spans="1:28" ht="36">
       <c r="A112">
         <v>53000109</v>
       </c>
@@ -18131,7 +18133,7 @@
         <v>303</v>
       </c>
       <c r="D112" s="26" t="s">
-        <v>758</v>
+        <v>750</v>
       </c>
       <c r="E112" s="1">
         <v>2</v>
@@ -18181,10 +18183,10 @@
         <v>100</v>
       </c>
       <c r="T112" s="11" t="s">
-        <v>757</v>
+        <v>749</v>
       </c>
       <c r="U112" s="7" t="s">
-        <v>756</v>
+        <v>748</v>
       </c>
       <c r="V112" s="1" t="s">
         <v>166</v>
@@ -18206,7 +18208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:28" ht="48" hidden="1">
+    <row r="113" spans="1:28" ht="48">
       <c r="A113">
         <v>53000110</v>
       </c>
@@ -18217,7 +18219,7 @@
         <v>304</v>
       </c>
       <c r="D113" s="26" t="s">
-        <v>754</v>
+        <v>746</v>
       </c>
       <c r="E113" s="1">
         <v>3</v>
@@ -18267,10 +18269,10 @@
         <v>103</v>
       </c>
       <c r="T113" s="11" t="s">
-        <v>752</v>
+        <v>744</v>
       </c>
       <c r="U113" s="7" t="s">
-        <v>753</v>
+        <v>745</v>
       </c>
       <c r="V113" s="1" t="s">
         <v>29</v>
@@ -18292,7 +18294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:28" ht="60" hidden="1">
+    <row r="114" spans="1:28" ht="60">
       <c r="A114">
         <v>53000111</v>
       </c>
@@ -18303,7 +18305,7 @@
         <v>305</v>
       </c>
       <c r="D114" s="26" t="s">
-        <v>748</v>
+        <v>740</v>
       </c>
       <c r="E114" s="1">
         <v>3</v>
@@ -18353,10 +18355,10 @@
         <v>100</v>
       </c>
       <c r="T114" s="11" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="U114" s="7" t="s">
-        <v>747</v>
+        <v>739</v>
       </c>
       <c r="V114" s="1" t="s">
         <v>169</v>
@@ -18378,7 +18380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:28" ht="24" hidden="1">
+    <row r="115" spans="1:28" ht="24">
       <c r="A115">
         <v>53000112</v>
       </c>
@@ -18389,7 +18391,7 @@
         <v>306</v>
       </c>
       <c r="D115" s="26" t="s">
-        <v>754</v>
+        <v>746</v>
       </c>
       <c r="E115" s="1">
         <v>2</v>
@@ -18464,7 +18466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:28" ht="24" hidden="1">
+    <row r="116" spans="1:28" ht="24">
       <c r="A116">
         <v>53000113</v>
       </c>
@@ -18475,7 +18477,7 @@
         <v>307</v>
       </c>
       <c r="D116" s="26" t="s">
-        <v>749</v>
+        <v>741</v>
       </c>
       <c r="E116" s="1">
         <v>1</v>
@@ -18525,10 +18527,10 @@
         <v>100</v>
       </c>
       <c r="T116" s="11" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="U116" s="7" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="V116" s="1" t="s">
         <v>173</v>
@@ -18689,7 +18691,7 @@
         <v>203</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>198</v>
@@ -18701,7 +18703,7 @@
         <v>200</v>
       </c>
       <c r="H1" s="38" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="I1" s="13" t="s">
         <v>337</v>
@@ -18725,7 +18727,7 @@
         <v>351</v>
       </c>
       <c r="P1" s="16" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="Q1" s="13" t="s">
         <v>334</v>
@@ -18734,7 +18736,7 @@
         <v>333</v>
       </c>
       <c r="S1" s="13" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="T1" s="13" t="s">
         <v>382</v>
@@ -18743,13 +18745,13 @@
         <v>319</v>
       </c>
       <c r="V1" s="13" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="W1" s="13" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="X1" s="44" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="Y1" s="13" t="s">
         <v>201</v>
@@ -18811,7 +18813,7 @@
         <v>338</v>
       </c>
       <c r="P2" s="18" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>335</v>
@@ -18820,10 +18822,10 @@
         <v>187</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>689</v>
+        <v>682</v>
       </c>
       <c r="U2" s="10" t="s">
         <v>187</v>
@@ -18832,10 +18834,10 @@
         <v>187</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="X2" s="45" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="Y2" s="4" t="s">
         <v>186</v>
@@ -18861,7 +18863,7 @@
         <v>204</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>190</v>
@@ -18873,7 +18875,7 @@
         <v>192</v>
       </c>
       <c r="H3" s="39" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>339</v>
@@ -18897,7 +18899,7 @@
         <v>353</v>
       </c>
       <c r="P3" s="40" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>336</v>
@@ -18906,7 +18908,7 @@
         <v>193</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="T3" s="6" t="s">
         <v>318</v>
@@ -18918,10 +18920,10 @@
         <v>341</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="X3" s="46" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="Y3" s="2" t="s">
         <v>194</v>
@@ -19233,7 +19235,7 @@
         <v>-1</v>
       </c>
       <c r="T7" s="11" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="U7" s="7" t="s">
         <v>427</v>
@@ -19393,7 +19395,7 @@
         <v>-1</v>
       </c>
       <c r="T9" s="11" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="U9" s="7" t="s">
         <v>420</v>
@@ -19421,7 +19423,7 @@
         <v>53100006</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>687</v>
+        <v>680</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="37"/>
@@ -19467,16 +19469,16 @@
         <v>1</v>
       </c>
       <c r="R10" s="15" t="s">
-        <v>688</v>
+        <v>681</v>
       </c>
       <c r="S10" s="1">
         <v>0</v>
       </c>
       <c r="T10" s="11" t="s">
-        <v>691</v>
+        <v>684</v>
       </c>
       <c r="U10" s="7" t="s">
-        <v>690</v>
+        <v>683</v>
       </c>
       <c r="V10" s="15" t="s">
         <v>2</v>
@@ -19654,7 +19656,7 @@
         <v>203</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>198</v>
@@ -19666,7 +19668,7 @@
         <v>200</v>
       </c>
       <c r="H1" s="38" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="I1" s="13" t="s">
         <v>337</v>
@@ -19690,7 +19692,7 @@
         <v>351</v>
       </c>
       <c r="P1" s="16" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="Q1" s="13" t="s">
         <v>334</v>
@@ -19699,7 +19701,7 @@
         <v>333</v>
       </c>
       <c r="S1" s="13" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="T1" s="13" t="s">
         <v>382</v>
@@ -19708,13 +19710,13 @@
         <v>319</v>
       </c>
       <c r="V1" s="13" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="W1" s="13" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="X1" s="44" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="Y1" s="13" t="s">
         <v>201</v>
@@ -19776,7 +19778,7 @@
         <v>338</v>
       </c>
       <c r="P2" s="18" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>335</v>
@@ -19785,7 +19787,7 @@
         <v>187</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
       <c r="T2" s="4" t="s">
         <v>340</v>
@@ -19797,10 +19799,10 @@
         <v>187</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="X2" s="45" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="Y2" s="4" t="s">
         <v>186</v>
@@ -19826,7 +19828,7 @@
         <v>204</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>190</v>
@@ -19838,7 +19840,7 @@
         <v>192</v>
       </c>
       <c r="H3" s="39" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>339</v>
@@ -19862,7 +19864,7 @@
         <v>353</v>
       </c>
       <c r="P3" s="40" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="Q3" s="6" t="s">
         <v>336</v>
@@ -19871,7 +19873,7 @@
         <v>193</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="T3" s="6" t="s">
         <v>318</v>
@@ -19883,10 +19885,10 @@
         <v>341</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="X3" s="46" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="Y3" s="2" t="s">
         <v>194</v>
@@ -19906,13 +19908,13 @@
         <v>53200100</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E4" s="15">
         <v>3</v>
@@ -19962,7 +19964,7 @@
         <v>115</v>
       </c>
       <c r="T4" s="11" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="U4" s="7" t="s">
         <v>425</v>
@@ -19990,13 +19992,13 @@
         <v>53200101</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="E5" s="15">
         <v>3</v>
@@ -20046,10 +20048,10 @@
         <v>90</v>
       </c>
       <c r="T5" s="11" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="V5" s="1" t="s">
         <v>44</v>
@@ -20074,13 +20076,13 @@
         <v>53200102</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E6" s="15">
         <v>3</v>
@@ -20130,10 +20132,10 @@
         <v>115</v>
       </c>
       <c r="T6" s="11" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="U6" s="33" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="V6" s="1" t="s">
         <v>46</v>
@@ -20158,13 +20160,13 @@
         <v>53200103</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="E7" s="15">
         <v>3</v>
@@ -20215,7 +20217,7 @@
       </c>
       <c r="T7" s="11"/>
       <c r="U7" s="33" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="V7" s="1" t="s">
         <v>45</v>
@@ -20240,13 +20242,13 @@
         <v>53200104</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>494</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>498</v>
-      </c>
       <c r="D8" s="26" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E8" s="15">
         <v>3</v>
@@ -20296,16 +20298,16 @@
         <v>90</v>
       </c>
       <c r="T8" s="11" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="U8" s="7" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="X8" s="1"/>
       <c r="Y8" s="1">
@@ -20326,13 +20328,13 @@
         <v>53200105</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>498</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="D9" s="26" t="s">
         <v>500</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>502</v>
       </c>
       <c r="E9" s="15">
         <v>3</v>
@@ -20382,7 +20384,7 @@
         <v>400</v>
       </c>
       <c r="T9" s="11" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="U9" s="7" t="s">
         <v>356</v>
@@ -20476,7 +20478,7 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -20513,7 +20515,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B4">
         <f>SQRT((B3 + 5) / 6)</f>
@@ -20558,7 +20560,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="31" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B5">
         <f>SQRT((B3 + 5) / 6)</f>
@@ -20603,7 +20605,7 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B6">
         <f>SQRT((B3 + 7) / 8)</f>
@@ -20648,15 +20650,15 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B10" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
   </sheetData>
@@ -20677,12 +20679,12 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B2">
         <f>COUNTIF(标准!D:D,"*单伤*")</f>
@@ -20691,7 +20693,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B3">
         <f>COUNTIF(标准!D:D,"*群伤*")</f>
@@ -20700,25 +20702,25 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B4">
         <f>COUNTIF(标准!D:D,"*单治*")</f>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B5">
         <f>COUNTIF(标准!D:D,"*群治*")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B6">
         <f>COUNTIF(标准!D:D,"*正状*")</f>
@@ -20727,7 +20729,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B7">
         <f>COUNTIF(标准!D:D,"*负状*")</f>
@@ -20736,7 +20738,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B8">
         <f>COUNTIF(标准!D:D,"*手牌*")</f>
@@ -20745,7 +20747,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B9">
         <f>COUNTIF(标准!D:D,"*陷阱*")</f>
@@ -20754,7 +20756,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B10">
         <f>COUNTIF(标准!D:D,"*地形*")</f>
@@ -20763,7 +20765,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B11">
         <f>COUNTIF(标准!D:D,"*属性*")</f>
@@ -20772,7 +20774,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>660</v>
+        <v>653</v>
       </c>
       <c r="B12">
         <f>COUNTIF(标准!D:D,"*位移*")</f>

</xml_diff>

<commit_message>
fix 2 random damage spell bug
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -3222,18 +3222,10 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse))im.OnMagicDamage(s.Damage*MathTool.GetRandom(70,130),s.Attr);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>群伤</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>t.OnMagicDamage(s.Damage*MathTool.GetRandom(85,115),s.Attr);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>单伤</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3513,6 +3505,14 @@
   </si>
   <si>
     <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse))im.OnMagicDamage(s.Damage*MathTool.GetRandom(75,125)/100,s.Attr);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>t.OnMagicDamage(s.Damage*MathTool.GetRandom(85,115)/100,s.Attr);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse))im.OnMagicDamage(s.Damage*MathTool.GetRandom(70,130)/100,s.Attr);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -7516,11 +7516,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="392409920"/>
-        <c:axId val="392405568"/>
+        <c:axId val="1628999856"/>
+        <c:axId val="1629000400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="392409920"/>
+        <c:axId val="1628999856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7563,7 +7563,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="392405568"/>
+        <c:crossAx val="1629000400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7571,7 +7571,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="392405568"/>
+        <c:axId val="1629000400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7622,7 +7622,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="392409920"/>
+        <c:crossAx val="1628999856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8671,10 +8671,10 @@
   <dimension ref="A1:AB113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C103" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R105" sqref="R105"/>
+      <selection pane="bottomRight" activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -9018,10 +9018,10 @@
         <v>95</v>
       </c>
       <c r="T4" s="11" t="s">
+        <v>744</v>
+      </c>
+      <c r="U4" s="7" t="s">
         <v>746</v>
-      </c>
-      <c r="U4" s="7" t="s">
-        <v>748</v>
       </c>
       <c r="V4" s="1" t="s">
         <v>2</v>
@@ -10460,10 +10460,10 @@
         <v>102</v>
       </c>
       <c r="T21" s="11" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="U21" s="7" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="V21" s="1" t="s">
         <v>21</v>
@@ -10540,7 +10540,7 @@
         <v>40</v>
       </c>
       <c r="R22" s="7" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="S22">
         <v>100</v>
@@ -10628,7 +10628,7 @@
         <v>60</v>
       </c>
       <c r="R23" s="7" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="S23">
         <v>100</v>
@@ -10716,7 +10716,7 @@
         <v>90</v>
       </c>
       <c r="R24" s="7" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="S24">
         <v>100</v>
@@ -11874,7 +11874,7 @@
         <v>235</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="E38" s="1">
         <v>3</v>
@@ -11918,16 +11918,16 @@
         <v>15</v>
       </c>
       <c r="R38" s="1" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="S38">
         <v>100</v>
       </c>
       <c r="T38" s="11" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="U38" s="7" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="V38" s="1" t="s">
         <v>49</v>
@@ -11962,7 +11962,7 @@
         <v>236</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="E39" s="1">
         <v>3</v>
@@ -12006,16 +12006,16 @@
         <v>12</v>
       </c>
       <c r="R39" s="1" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="S39">
         <v>100</v>
       </c>
       <c r="T39" s="11" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="U39" s="1" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="V39" s="1" t="s">
         <v>51</v>
@@ -12182,7 +12182,7 @@
         <v>100</v>
       </c>
       <c r="T41" s="11" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="U41" s="7" t="s">
         <v>566</v>
@@ -12474,7 +12474,7 @@
         <v>241</v>
       </c>
       <c r="D45" s="25" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="E45" s="1">
         <v>3</v>
@@ -12524,7 +12524,7 @@
         <v>110</v>
       </c>
       <c r="T45" s="11" t="s">
-        <v>716</v>
+        <v>789</v>
       </c>
       <c r="U45" s="7" t="s">
         <v>714</v>
@@ -12778,7 +12778,7 @@
         <v>30</v>
       </c>
       <c r="R48" s="7" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="S48">
         <v>100</v>
@@ -12787,7 +12787,7 @@
         <v>715</v>
       </c>
       <c r="U48" s="1" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="V48" s="1" t="s">
         <v>324</v>
@@ -12906,7 +12906,7 @@
         <v>246</v>
       </c>
       <c r="D50" s="25" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="E50" s="1">
         <v>5</v>
@@ -12959,7 +12959,7 @@
         <v>523</v>
       </c>
       <c r="U50" s="7" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="V50" s="1" t="s">
         <v>65</v>
@@ -12994,7 +12994,7 @@
         <v>247</v>
       </c>
       <c r="D51" s="25" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="E51" s="1">
         <v>5</v>
@@ -13044,10 +13044,10 @@
         <v>100</v>
       </c>
       <c r="T51" s="11" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="U51" s="1" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="V51" s="1" t="s">
         <v>21</v>
@@ -13133,7 +13133,7 @@
         <v>524</v>
       </c>
       <c r="U52" s="7" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="V52" s="1" t="s">
         <v>68</v>
@@ -13254,7 +13254,7 @@
         <v>250</v>
       </c>
       <c r="D54" s="25" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="E54" s="1">
         <v>3</v>
@@ -13304,10 +13304,10 @@
         <v>100</v>
       </c>
       <c r="T54" s="11" t="s">
+        <v>727</v>
+      </c>
+      <c r="U54" s="1" t="s">
         <v>729</v>
-      </c>
-      <c r="U54" s="1" t="s">
-        <v>731</v>
       </c>
       <c r="V54" s="1" t="s">
         <v>72</v>
@@ -13336,13 +13336,13 @@
         <v>53000052</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="D55" s="25" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E55" s="1">
         <v>2</v>
@@ -13386,22 +13386,22 @@
         <v>12</v>
       </c>
       <c r="R55" s="1" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="S55">
         <v>95</v>
       </c>
       <c r="T55" s="11" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="U55" s="7" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="V55" s="1" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="W55" s="1" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="X55" s="1">
         <v>11000002</v>
@@ -13430,7 +13430,7 @@
         <v>251</v>
       </c>
       <c r="D56" s="25" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E56" s="1">
         <v>3</v>
@@ -13474,7 +13474,7 @@
         <v>20</v>
       </c>
       <c r="R56" s="1" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="S56">
         <v>100</v>
@@ -13483,7 +13483,7 @@
         <v>523</v>
       </c>
       <c r="U56" s="7" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="V56" s="1" t="s">
         <v>74</v>
@@ -13516,7 +13516,7 @@
         <v>199</v>
       </c>
       <c r="D57" s="25" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="E57" s="1">
         <v>3</v>
@@ -13566,10 +13566,10 @@
         <v>100</v>
       </c>
       <c r="T57" s="11" t="s">
-        <v>718</v>
+        <v>788</v>
       </c>
       <c r="U57" s="7" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="V57" s="1" t="s">
         <v>76</v>
@@ -13602,7 +13602,7 @@
         <v>252</v>
       </c>
       <c r="D58" s="25" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="E58" s="1">
         <v>4</v>
@@ -13854,10 +13854,10 @@
         <v>53000058</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="D61" s="25" t="s">
         <v>429</v>
@@ -13904,16 +13904,16 @@
         <v>12</v>
       </c>
       <c r="R61" s="1" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="S61">
         <v>100</v>
       </c>
       <c r="T61" s="11" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="U61" s="7" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="V61" s="1" t="s">
         <v>15</v>
@@ -15326,7 +15326,7 @@
         <v>265</v>
       </c>
       <c r="D78" s="25" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="E78" s="1">
         <v>4</v>
@@ -15586,7 +15586,7 @@
         <v>268</v>
       </c>
       <c r="D81" s="25" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="E81" s="1">
         <v>1</v>
@@ -15636,10 +15636,10 @@
         <v>100</v>
       </c>
       <c r="T81" s="39" t="s">
+        <v>745</v>
+      </c>
+      <c r="U81" s="7" t="s">
         <v>747</v>
-      </c>
-      <c r="U81" s="7" t="s">
-        <v>749</v>
       </c>
       <c r="V81" s="1" t="s">
         <v>93</v>
@@ -15802,7 +15802,7 @@
         <v>30</v>
       </c>
       <c r="R83" s="7" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="S83">
         <v>100</v>
@@ -15811,7 +15811,7 @@
         <v>650</v>
       </c>
       <c r="U83" s="7" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="V83" s="1" t="s">
         <v>81</v>
@@ -15846,7 +15846,7 @@
         <v>271</v>
       </c>
       <c r="D84" s="25" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="E84" s="1">
         <v>2</v>
@@ -15890,16 +15890,16 @@
         <v>30</v>
       </c>
       <c r="R84" s="7" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="S84">
         <v>100</v>
       </c>
       <c r="T84" s="11" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="U84" s="7" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="V84" s="1" t="s">
         <v>51</v>
@@ -16368,7 +16368,7 @@
         <v>209</v>
       </c>
       <c r="D90" s="25" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="E90" s="1">
         <v>3</v>
@@ -16412,16 +16412,16 @@
         <v>40</v>
       </c>
       <c r="R90" s="7" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="S90">
         <v>100</v>
       </c>
       <c r="T90" s="11" t="s">
+        <v>720</v>
+      </c>
+      <c r="U90" s="7" t="s">
         <v>722</v>
-      </c>
-      <c r="U90" s="7" t="s">
-        <v>724</v>
       </c>
       <c r="V90" s="1" t="s">
         <v>59</v>
@@ -16798,13 +16798,13 @@
         <v>53000092</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="C95" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="D95" s="25" t="s">
         <v>774</v>
-      </c>
-      <c r="D95" s="25" t="s">
-        <v>776</v>
       </c>
       <c r="E95" s="1">
         <v>3</v>
@@ -16848,19 +16848,19 @@
         <v>0</v>
       </c>
       <c r="R95" s="7" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="S95">
         <v>100</v>
       </c>
       <c r="T95" s="11" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="U95" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="V95" s="1" t="s">
         <v>778</v>
-      </c>
-      <c r="V95" s="1" t="s">
-        <v>780</v>
       </c>
       <c r="W95" s="1"/>
       <c r="X95" s="1">
@@ -17115,7 +17115,7 @@
         <v>680</v>
       </c>
       <c r="U98" s="7" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="V98" s="1" t="s">
         <v>139</v>
@@ -17544,7 +17544,7 @@
         <v>100</v>
       </c>
       <c r="T103" s="11" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="U103" s="1" t="s">
         <v>683</v>
@@ -17580,7 +17580,7 @@
         <v>294</v>
       </c>
       <c r="D104" s="25" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="E104" s="1">
         <v>3</v>
@@ -17624,16 +17624,16 @@
         <v>0</v>
       </c>
       <c r="R104" s="1" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="S104">
         <v>100</v>
       </c>
       <c r="T104" s="11" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="U104" s="1" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="V104" s="1" t="s">
         <v>168</v>

</xml_diff>

<commit_message>
fix a spell bug
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="标准" sheetId="1" r:id="rId1"/>
@@ -639,7 +639,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="790">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="791">
   <si>
     <t>慈悲</t>
   </si>
@@ -3513,6 +3513,10 @@
   </si>
   <si>
     <t>m.ReviveUnit(p,mouse,s.Cure);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>UES</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -7516,11 +7520,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="791097888"/>
-        <c:axId val="791098448"/>
+        <c:axId val="1578624464"/>
+        <c:axId val="1578627184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="791097888"/>
+        <c:axId val="1578624464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7563,7 +7567,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="791098448"/>
+        <c:crossAx val="1578627184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7571,7 +7575,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="791098448"/>
+        <c:axId val="1578627184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7622,7 +7626,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="791097888"/>
+        <c:crossAx val="1578624464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8671,31 +8675,31 @@
   <dimension ref="A1:AB113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="T29" sqref="T29"/>
+      <selection pane="bottomRight" activeCell="T51" sqref="T51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
-    <col min="2" max="3" width="7.88671875" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" customWidth="1"/>
-    <col min="5" max="5" width="3.109375" customWidth="1"/>
-    <col min="6" max="6" width="3.6640625" customWidth="1"/>
-    <col min="7" max="9" width="3.109375" customWidth="1"/>
-    <col min="10" max="10" width="3.88671875" customWidth="1"/>
+    <col min="1" max="1" width="9.125" customWidth="1"/>
+    <col min="2" max="3" width="7.875" customWidth="1"/>
+    <col min="4" max="4" width="10.875" customWidth="1"/>
+    <col min="5" max="5" width="3.125" customWidth="1"/>
+    <col min="6" max="6" width="3.625" customWidth="1"/>
+    <col min="7" max="9" width="3.125" customWidth="1"/>
+    <col min="10" max="10" width="3.875" customWidth="1"/>
     <col min="11" max="11" width="4" customWidth="1"/>
-    <col min="12" max="15" width="3.109375" customWidth="1"/>
-    <col min="16" max="16" width="5.21875" customWidth="1"/>
-    <col min="17" max="17" width="3.109375" customWidth="1"/>
-    <col min="18" max="18" width="5.33203125" customWidth="1"/>
-    <col min="19" max="19" width="5.77734375" customWidth="1"/>
-    <col min="20" max="20" width="23.44140625" customWidth="1"/>
-    <col min="21" max="21" width="24.33203125" customWidth="1"/>
-    <col min="22" max="23" width="7.88671875" customWidth="1"/>
-    <col min="24" max="24" width="9.109375" customWidth="1"/>
+    <col min="12" max="15" width="3.125" customWidth="1"/>
+    <col min="16" max="16" width="5.25" customWidth="1"/>
+    <col min="17" max="17" width="3.125" customWidth="1"/>
+    <col min="18" max="18" width="5.375" customWidth="1"/>
+    <col min="19" max="19" width="5.75" customWidth="1"/>
+    <col min="20" max="20" width="23.5" customWidth="1"/>
+    <col min="21" max="21" width="24.375" customWidth="1"/>
+    <col min="22" max="23" width="7.875" customWidth="1"/>
+    <col min="24" max="24" width="9.125" customWidth="1"/>
     <col min="25" max="28" width="4" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8957,7 +8961,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="48">
+    <row r="4" spans="1:28" ht="36">
       <c r="A4">
         <v>53000001</v>
       </c>
@@ -9969,7 +9973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="60">
+    <row r="16" spans="1:28" ht="48">
       <c r="A16">
         <v>53000013</v>
       </c>
@@ -10399,7 +10403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="60">
+    <row r="21" spans="1:28" ht="48">
       <c r="A21">
         <v>53000018</v>
       </c>
@@ -11005,7 +11009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="60">
+    <row r="28" spans="1:28" ht="48">
       <c r="A28">
         <v>53000025</v>
       </c>
@@ -11601,7 +11605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:28" ht="96">
+    <row r="35" spans="1:28" ht="72">
       <c r="A35">
         <v>53000032</v>
       </c>
@@ -11689,7 +11693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:28" ht="60">
+    <row r="36" spans="1:28" ht="48">
       <c r="A36">
         <v>53000033</v>
       </c>
@@ -11777,7 +11781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:28" ht="60">
+    <row r="37" spans="1:28" ht="36">
       <c r="A37">
         <v>53000034</v>
       </c>
@@ -11863,7 +11867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:28" ht="72">
+    <row r="38" spans="1:28" ht="60">
       <c r="A38">
         <v>53000035</v>
       </c>
@@ -11951,7 +11955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:28" ht="48">
+    <row r="39" spans="1:28" ht="36">
       <c r="A39">
         <v>53000036</v>
       </c>
@@ -12121,7 +12125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:28" ht="36">
+    <row r="41" spans="1:28" ht="24">
       <c r="A41">
         <v>53000038</v>
       </c>
@@ -12463,7 +12467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:28" ht="84">
+    <row r="45" spans="1:28" ht="72">
       <c r="A45">
         <v>53000042</v>
       </c>
@@ -12723,7 +12727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:28" ht="72">
+    <row r="48" spans="1:28" ht="60">
       <c r="A48">
         <v>53000045</v>
       </c>
@@ -12809,7 +12813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:28" ht="60">
+    <row r="49" spans="1:28" ht="48">
       <c r="A49">
         <v>53000046</v>
       </c>
@@ -12895,7 +12899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:28" ht="72">
+    <row r="50" spans="1:28" ht="60">
       <c r="A50">
         <v>53000047</v>
       </c>
@@ -13038,7 +13042,7 @@
         <v>0</v>
       </c>
       <c r="R51" s="1" t="s">
-        <v>48</v>
+        <v>790</v>
       </c>
       <c r="S51">
         <v>100</v>
@@ -13243,7 +13247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:28" ht="84">
+    <row r="54" spans="1:28" ht="72">
       <c r="A54">
         <v>53000051</v>
       </c>
@@ -13331,7 +13335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:28" ht="156">
+    <row r="55" spans="1:28" ht="132">
       <c r="A55">
         <v>53000052</v>
       </c>
@@ -13419,7 +13423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:28" ht="72">
+    <row r="56" spans="1:28" ht="60">
       <c r="A56">
         <v>53000053</v>
       </c>
@@ -13591,7 +13595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:28" ht="36">
+    <row r="58" spans="1:28" ht="24">
       <c r="A58">
         <v>53000055</v>
       </c>
@@ -13677,7 +13681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:28" ht="48">
+    <row r="59" spans="1:28" ht="36">
       <c r="A59">
         <v>53000056</v>
       </c>
@@ -13935,7 +13939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:28" ht="36">
+    <row r="62" spans="1:28" ht="24">
       <c r="A62">
         <v>53000059</v>
       </c>
@@ -14021,7 +14025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:28" ht="48">
+    <row r="63" spans="1:28" ht="36">
       <c r="A63">
         <v>53000060</v>
       </c>
@@ -14107,7 +14111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:28" ht="60">
+    <row r="64" spans="1:28" ht="48">
       <c r="A64">
         <v>53000061</v>
       </c>
@@ -14451,7 +14455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:28" ht="60">
+    <row r="68" spans="1:28" ht="48">
       <c r="A68">
         <v>53000065</v>
       </c>
@@ -14623,7 +14627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:28" ht="36">
+    <row r="70" spans="1:28" ht="24">
       <c r="A70">
         <v>53000067</v>
       </c>
@@ -14709,7 +14713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:28" ht="72">
+    <row r="71" spans="1:28" ht="60">
       <c r="A71">
         <v>53000068</v>
       </c>
@@ -14797,7 +14801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:28" ht="60">
+    <row r="72" spans="1:28" ht="48">
       <c r="A72">
         <v>53000069</v>
       </c>
@@ -14969,7 +14973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:28" ht="96">
+    <row r="74" spans="1:28" ht="84">
       <c r="A74">
         <v>53000071</v>
       </c>
@@ -15229,7 +15233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:28" ht="48">
+    <row r="77" spans="1:28" ht="36">
       <c r="A77">
         <v>53000074</v>
       </c>
@@ -15315,7 +15319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:28" ht="132">
+    <row r="78" spans="1:28" ht="108">
       <c r="A78">
         <v>53000075</v>
       </c>
@@ -15401,7 +15405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:28" ht="72">
+    <row r="79" spans="1:28" ht="60">
       <c r="A79">
         <v>53000076</v>
       </c>
@@ -15575,7 +15579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:28" ht="48">
+    <row r="81" spans="1:28" ht="36">
       <c r="A81">
         <v>53000078</v>
       </c>
@@ -15659,7 +15663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:28" ht="72">
+    <row r="82" spans="1:28" ht="60">
       <c r="A82">
         <v>53000079</v>
       </c>
@@ -15747,7 +15751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:28" ht="72">
+    <row r="83" spans="1:28" ht="60">
       <c r="A83">
         <v>53000080</v>
       </c>
@@ -15835,7 +15839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:28" ht="84">
+    <row r="84" spans="1:28" ht="72">
       <c r="A84">
         <v>53000081</v>
       </c>
@@ -16009,7 +16013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:28" ht="60">
+    <row r="86" spans="1:28" ht="48">
       <c r="A86">
         <v>53000083</v>
       </c>
@@ -16183,7 +16187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:28" ht="84">
+    <row r="88" spans="1:28" ht="60">
       <c r="A88">
         <v>53000085</v>
       </c>
@@ -16357,7 +16361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:28" ht="60">
+    <row r="90" spans="1:28" ht="48">
       <c r="A90">
         <v>53000087</v>
       </c>
@@ -16445,7 +16449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:28" ht="72">
+    <row r="91" spans="1:28" ht="60">
       <c r="A91">
         <v>53000088</v>
       </c>
@@ -16533,7 +16537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:28" ht="72">
+    <row r="92" spans="1:28" ht="60">
       <c r="A92">
         <v>53000089</v>
       </c>
@@ -17051,7 +17055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:28" ht="72">
+    <row r="98" spans="1:28" ht="60">
       <c r="A98">
         <v>53000095</v>
       </c>
@@ -17225,7 +17229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:28" ht="72">
+    <row r="100" spans="1:28" ht="60">
       <c r="A100">
         <v>53000097</v>
       </c>
@@ -17397,7 +17401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:28" ht="36">
+    <row r="102" spans="1:28" ht="24">
       <c r="A102">
         <v>53000099</v>
       </c>
@@ -17483,7 +17487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:28" ht="84">
+    <row r="103" spans="1:28" ht="72">
       <c r="A103">
         <v>53000100</v>
       </c>
@@ -17915,7 +17919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:28" ht="60">
+    <row r="108" spans="1:28" ht="36">
       <c r="A108">
         <v>53000105</v>
       </c>
@@ -18173,7 +18177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:28" ht="144">
+    <row r="111" spans="1:28" ht="120">
       <c r="A111">
         <v>53000108</v>
       </c>
@@ -18259,7 +18263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:28" ht="36">
+    <row r="112" spans="1:28" ht="24">
       <c r="A112">
         <v>53000109</v>
       </c>
@@ -18345,7 +18349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:28" ht="48">
+    <row r="113" spans="1:28" ht="36">
       <c r="A113">
         <v>53000110</v>
       </c>
@@ -18539,23 +18543,23 @@
       <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="3" width="7.88671875" customWidth="1"/>
-    <col min="5" max="5" width="3.109375" customWidth="1"/>
-    <col min="6" max="6" width="4.6640625" customWidth="1"/>
-    <col min="7" max="9" width="3.109375" customWidth="1"/>
-    <col min="10" max="10" width="3.88671875" customWidth="1"/>
+    <col min="2" max="3" width="7.875" customWidth="1"/>
+    <col min="5" max="5" width="3.125" customWidth="1"/>
+    <col min="6" max="6" width="4.625" customWidth="1"/>
+    <col min="7" max="9" width="3.125" customWidth="1"/>
+    <col min="10" max="10" width="3.875" customWidth="1"/>
     <col min="11" max="11" width="4" customWidth="1"/>
-    <col min="12" max="15" width="3.109375" customWidth="1"/>
-    <col min="16" max="16" width="5.109375" customWidth="1"/>
-    <col min="17" max="17" width="3.109375" customWidth="1"/>
-    <col min="18" max="18" width="5.33203125" customWidth="1"/>
-    <col min="19" max="19" width="5.77734375" customWidth="1"/>
-    <col min="20" max="20" width="23.44140625" customWidth="1"/>
-    <col min="21" max="21" width="27.21875" customWidth="1"/>
-    <col min="22" max="24" width="7.88671875" customWidth="1"/>
+    <col min="12" max="15" width="3.125" customWidth="1"/>
+    <col min="16" max="16" width="5.125" customWidth="1"/>
+    <col min="17" max="17" width="3.125" customWidth="1"/>
+    <col min="18" max="18" width="5.375" customWidth="1"/>
+    <col min="19" max="19" width="5.75" customWidth="1"/>
+    <col min="20" max="20" width="23.5" customWidth="1"/>
+    <col min="21" max="21" width="27.25" customWidth="1"/>
+    <col min="22" max="24" width="7.875" customWidth="1"/>
     <col min="25" max="28" width="4" customWidth="1"/>
   </cols>
   <sheetData>
@@ -18977,7 +18981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="36">
+    <row r="6" spans="1:28" ht="24">
       <c r="A6">
         <v>53100002</v>
       </c>
@@ -19587,23 +19591,23 @@
       <selection pane="bottomRight" activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" customWidth="1"/>
-    <col min="2" max="3" width="7.88671875" customWidth="1"/>
-    <col min="5" max="5" width="3.109375" customWidth="1"/>
-    <col min="6" max="6" width="4.33203125" customWidth="1"/>
-    <col min="7" max="9" width="3.109375" customWidth="1"/>
-    <col min="10" max="10" width="3.88671875" customWidth="1"/>
+    <col min="1" max="1" width="10.75" customWidth="1"/>
+    <col min="2" max="3" width="7.875" customWidth="1"/>
+    <col min="5" max="5" width="3.125" customWidth="1"/>
+    <col min="6" max="6" width="4.375" customWidth="1"/>
+    <col min="7" max="9" width="3.125" customWidth="1"/>
+    <col min="10" max="10" width="3.875" customWidth="1"/>
     <col min="11" max="11" width="4" customWidth="1"/>
-    <col min="12" max="15" width="3.109375" customWidth="1"/>
-    <col min="16" max="16" width="5.21875" customWidth="1"/>
-    <col min="17" max="17" width="3.109375" customWidth="1"/>
-    <col min="18" max="18" width="5.33203125" customWidth="1"/>
-    <col min="19" max="19" width="5.77734375" customWidth="1"/>
-    <col min="20" max="20" width="23.44140625" customWidth="1"/>
-    <col min="21" max="21" width="27.21875" customWidth="1"/>
-    <col min="22" max="24" width="7.88671875" customWidth="1"/>
+    <col min="12" max="15" width="3.125" customWidth="1"/>
+    <col min="16" max="16" width="5.25" customWidth="1"/>
+    <col min="17" max="17" width="3.125" customWidth="1"/>
+    <col min="18" max="18" width="5.375" customWidth="1"/>
+    <col min="19" max="19" width="5.75" customWidth="1"/>
+    <col min="20" max="20" width="23.5" customWidth="1"/>
+    <col min="21" max="21" width="27.25" customWidth="1"/>
+    <col min="22" max="24" width="7.875" customWidth="1"/>
     <col min="25" max="25" width="4" customWidth="1"/>
     <col min="26" max="26" width="5" customWidth="1"/>
     <col min="27" max="28" width="4" customWidth="1"/>
@@ -20035,7 +20039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="43.2">
+    <row r="6" spans="1:28" ht="40.5">
       <c r="A6">
         <v>53200102</v>
       </c>
@@ -20438,7 +20442,7 @@
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
@@ -20522,7 +20526,7 @@
         <v>1.5811388300841898</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" ht="15">
       <c r="A5" s="30" t="s">
         <v>395</v>
       </c>
@@ -20639,7 +20643,7 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" t="s">

</xml_diff>

<commit_message>
#71 add a silent card
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -2873,15 +2873,7 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>永久降低敌方单体{3:0.0}%攻击和最大生命</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>负状</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>t.Atk.Source*=(1-s.Help/100);t.AddMaxHp(-s.Help/100*t.MaxHp.Source);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -3545,6 +3537,14 @@
   </si>
   <si>
     <t>question</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>t.Atk.Source*=(1-s.Help/100);t.AddMaxHp(-s.Help/100*t.MaxHp.Source);t.Silent();</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>沉默目标，并降低敌方单体{3:0.0}%攻击和最大生命</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -4547,59 +4547,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="154">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="147">
     <dxf>
       <font>
         <b/>
@@ -8334,132 +8282,132 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AB114" totalsRowShown="0" headerRowDxfId="153" dataDxfId="152" tableBorderDxfId="151">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AB114" totalsRowShown="0" headerRowDxfId="146" dataDxfId="145" tableBorderDxfId="144">
   <autoFilter ref="A3:AB114"/>
   <sortState ref="A4:AB113">
     <sortCondition ref="A3:A113"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="150"/>
-    <tableColumn id="2" name="Name" dataDxfId="149"/>
-    <tableColumn id="20" name="Ename" dataDxfId="148"/>
-    <tableColumn id="21" name="Remark" dataDxfId="147"/>
-    <tableColumn id="3" name="Star" dataDxfId="146"/>
-    <tableColumn id="4" name="Type" dataDxfId="145"/>
-    <tableColumn id="5" name="Attr" dataDxfId="144"/>
-    <tableColumn id="8" name="Quality" dataDxfId="143">
+    <tableColumn id="1" name="Id" dataDxfId="143"/>
+    <tableColumn id="2" name="Name" dataDxfId="142"/>
+    <tableColumn id="20" name="Ename" dataDxfId="141"/>
+    <tableColumn id="21" name="Remark" dataDxfId="140"/>
+    <tableColumn id="3" name="Star" dataDxfId="139"/>
+    <tableColumn id="4" name="Type" dataDxfId="138"/>
+    <tableColumn id="5" name="Attr" dataDxfId="137"/>
+    <tableColumn id="8" name="Quality" dataDxfId="136">
       <calculatedColumnFormula>IF(AND(P4&gt;=13,P4&lt;=16),5,IF(AND(P4&gt;=9,P4&lt;=12),4,IF(AND(P4&gt;=5,P4&lt;=8),3,IF(AND(P4&gt;=1,P4&lt;=4),2,IF(AND(P4&gt;=-3,P4&lt;=0),1,IF(AND(P4&gt;=-5,P4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="142"/>
-    <tableColumn id="9" name="Damage" dataDxfId="141"/>
-    <tableColumn id="10" name="Cure" dataDxfId="140"/>
-    <tableColumn id="11" name="Time" dataDxfId="139"/>
-    <tableColumn id="13" name="Help" dataDxfId="138"/>
-    <tableColumn id="16" name="Rate" dataDxfId="137"/>
-    <tableColumn id="12" name="Modify" dataDxfId="136"/>
-    <tableColumn id="27" name="Sum" dataDxfId="135">
+    <tableColumn id="7" name="Cost" dataDxfId="135"/>
+    <tableColumn id="9" name="Damage" dataDxfId="134"/>
+    <tableColumn id="10" name="Cure" dataDxfId="133"/>
+    <tableColumn id="11" name="Time" dataDxfId="132"/>
+    <tableColumn id="13" name="Help" dataDxfId="131"/>
+    <tableColumn id="16" name="Rate" dataDxfId="130"/>
+    <tableColumn id="12" name="Modify" dataDxfId="129"/>
+    <tableColumn id="27" name="Sum" dataDxfId="128">
       <calculatedColumnFormula>S4-100+O4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="134"/>
-    <tableColumn id="15" name="Target" dataDxfId="133"/>
-    <tableColumn id="25" name="Mark" dataDxfId="132"/>
-    <tableColumn id="22" name="Effect" dataDxfId="131"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="130"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="129"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="128"/>
-    <tableColumn id="26" name="JobId" dataDxfId="127"/>
-    <tableColumn id="18" name="Res" dataDxfId="126"/>
-    <tableColumn id="19" name="Icon" dataDxfId="125"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="124"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="123"/>
+    <tableColumn id="6" name="Range" dataDxfId="127"/>
+    <tableColumn id="15" name="Target" dataDxfId="126"/>
+    <tableColumn id="25" name="Mark" dataDxfId="125"/>
+    <tableColumn id="22" name="Effect" dataDxfId="124"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="123"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="122"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="121"/>
+    <tableColumn id="26" name="JobId" dataDxfId="120"/>
+    <tableColumn id="18" name="Res" dataDxfId="119"/>
+    <tableColumn id="19" name="Icon" dataDxfId="118"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="117"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="116"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AB11" totalsRowShown="0" headerRowDxfId="122" dataDxfId="121" tableBorderDxfId="120">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AB11" totalsRowShown="0" headerRowDxfId="115" dataDxfId="114" tableBorderDxfId="113">
   <autoFilter ref="A3:AB11"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="119"/>
-    <tableColumn id="2" name="Name" dataDxfId="118"/>
-    <tableColumn id="20" name="Ename" dataDxfId="117"/>
-    <tableColumn id="21" name="Remark" dataDxfId="116"/>
-    <tableColumn id="3" name="Star" dataDxfId="115"/>
-    <tableColumn id="4" name="Type" dataDxfId="114"/>
-    <tableColumn id="5" name="Attr" dataDxfId="113"/>
-    <tableColumn id="8" name="Quality" dataDxfId="112">
+    <tableColumn id="1" name="Id" dataDxfId="112"/>
+    <tableColumn id="2" name="Name" dataDxfId="111"/>
+    <tableColumn id="20" name="Ename" dataDxfId="110"/>
+    <tableColumn id="21" name="Remark" dataDxfId="109"/>
+    <tableColumn id="3" name="Star" dataDxfId="108"/>
+    <tableColumn id="4" name="Type" dataDxfId="107"/>
+    <tableColumn id="5" name="Attr" dataDxfId="106"/>
+    <tableColumn id="8" name="Quality" dataDxfId="105">
       <calculatedColumnFormula>IF(AND(P4&gt;=13,P4&lt;=16),5,IF(AND(P4&gt;=9,P4&lt;=12),4,IF(AND(P4&gt;=5,P4&lt;=8),3,IF(AND(P4&gt;=1,P4&lt;=4),2,IF(AND(P4&gt;=-3,P4&lt;=0),1,IF(AND(P4&gt;=-5,P4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="111"/>
-    <tableColumn id="9" name="Damage" dataDxfId="110"/>
-    <tableColumn id="10" name="Cure" dataDxfId="109"/>
-    <tableColumn id="11" name="Time" dataDxfId="108"/>
-    <tableColumn id="13" name="Help" dataDxfId="107"/>
-    <tableColumn id="16" name="Rate" dataDxfId="106"/>
-    <tableColumn id="12" name="Modify" dataDxfId="105"/>
-    <tableColumn id="27" name="Sum" dataDxfId="104">
+    <tableColumn id="7" name="Cost" dataDxfId="104"/>
+    <tableColumn id="9" name="Damage" dataDxfId="103"/>
+    <tableColumn id="10" name="Cure" dataDxfId="102"/>
+    <tableColumn id="11" name="Time" dataDxfId="101"/>
+    <tableColumn id="13" name="Help" dataDxfId="100"/>
+    <tableColumn id="16" name="Rate" dataDxfId="99"/>
+    <tableColumn id="12" name="Modify" dataDxfId="98"/>
+    <tableColumn id="27" name="Sum" dataDxfId="97">
       <calculatedColumnFormula>S4-100+O4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="103"/>
-    <tableColumn id="15" name="Target" dataDxfId="102"/>
-    <tableColumn id="25" name="Mark" dataDxfId="101"/>
-    <tableColumn id="22" name="Effect" dataDxfId="100"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="99"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="98"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="97"/>
-    <tableColumn id="26" name="JobId" dataDxfId="96"/>
-    <tableColumn id="18" name="Res" dataDxfId="95"/>
-    <tableColumn id="19" name="Icon" dataDxfId="94"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="93"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="92"/>
+    <tableColumn id="6" name="Range" dataDxfId="96"/>
+    <tableColumn id="15" name="Target" dataDxfId="95"/>
+    <tableColumn id="25" name="Mark" dataDxfId="94"/>
+    <tableColumn id="22" name="Effect" dataDxfId="93"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="92"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="91"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="90"/>
+    <tableColumn id="26" name="JobId" dataDxfId="89"/>
+    <tableColumn id="18" name="Res" dataDxfId="88"/>
+    <tableColumn id="19" name="Icon" dataDxfId="87"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="86"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="85"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_35" displayName="表1_35" ref="A3:AB9" totalsRowShown="0" headerRowDxfId="91" tableBorderDxfId="90">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_35" displayName="表1_35" ref="A3:AB9" totalsRowShown="0" headerRowDxfId="84" tableBorderDxfId="83">
   <autoFilter ref="A3:AB9"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="89"/>
-    <tableColumn id="2" name="Name" dataDxfId="88"/>
-    <tableColumn id="20" name="Ename" dataDxfId="87"/>
-    <tableColumn id="21" name="Remark" dataDxfId="86"/>
-    <tableColumn id="3" name="Star" dataDxfId="85"/>
-    <tableColumn id="4" name="Type" dataDxfId="84"/>
-    <tableColumn id="5" name="Attr" dataDxfId="83"/>
-    <tableColumn id="8" name="Quality" dataDxfId="82">
+    <tableColumn id="1" name="Id" dataDxfId="82"/>
+    <tableColumn id="2" name="Name" dataDxfId="81"/>
+    <tableColumn id="20" name="Ename" dataDxfId="80"/>
+    <tableColumn id="21" name="Remark" dataDxfId="79"/>
+    <tableColumn id="3" name="Star" dataDxfId="78"/>
+    <tableColumn id="4" name="Type" dataDxfId="77"/>
+    <tableColumn id="5" name="Attr" dataDxfId="76"/>
+    <tableColumn id="8" name="Quality" dataDxfId="75">
       <calculatedColumnFormula>IF(AND(P4&gt;=13,P4&lt;=16),5,IF(AND(P4&gt;=9,P4&lt;=12),4,IF(AND(P4&gt;=5,P4&lt;=8),3,IF(AND(P4&gt;=1,P4&lt;=4),2,IF(AND(P4&gt;=-3,P4&lt;=0),1,IF(AND(P4&gt;=-5,P4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="81"/>
-    <tableColumn id="9" name="Damage" dataDxfId="80"/>
-    <tableColumn id="10" name="Cure" dataDxfId="79"/>
-    <tableColumn id="11" name="Time" dataDxfId="78"/>
-    <tableColumn id="13" name="Help" dataDxfId="77"/>
-    <tableColumn id="16" name="Rate" dataDxfId="76"/>
-    <tableColumn id="12" name="Modify" dataDxfId="75"/>
-    <tableColumn id="27" name="Sum" dataDxfId="74">
+    <tableColumn id="7" name="Cost" dataDxfId="74"/>
+    <tableColumn id="9" name="Damage" dataDxfId="73"/>
+    <tableColumn id="10" name="Cure" dataDxfId="72"/>
+    <tableColumn id="11" name="Time" dataDxfId="71"/>
+    <tableColumn id="13" name="Help" dataDxfId="70"/>
+    <tableColumn id="16" name="Rate" dataDxfId="69"/>
+    <tableColumn id="12" name="Modify" dataDxfId="68"/>
+    <tableColumn id="27" name="Sum" dataDxfId="67">
       <calculatedColumnFormula>S4-100+O4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="73"/>
-    <tableColumn id="15" name="Target" dataDxfId="72"/>
-    <tableColumn id="25" name="Mark" dataDxfId="71"/>
-    <tableColumn id="22" name="Effect" dataDxfId="70"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="69"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="68"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="67"/>
-    <tableColumn id="26" name="JobId" dataDxfId="66"/>
-    <tableColumn id="18" name="Res" dataDxfId="65"/>
-    <tableColumn id="19" name="Icon" dataDxfId="64"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="63"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="62"/>
+    <tableColumn id="6" name="Range" dataDxfId="66"/>
+    <tableColumn id="15" name="Target" dataDxfId="65"/>
+    <tableColumn id="25" name="Mark" dataDxfId="64"/>
+    <tableColumn id="22" name="Effect" dataDxfId="63"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="62"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="61"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="60"/>
+    <tableColumn id="26" name="JobId" dataDxfId="59"/>
+    <tableColumn id="18" name="Res" dataDxfId="58"/>
+    <tableColumn id="19" name="Icon" dataDxfId="57"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="56"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8755,10 +8703,10 @@
   <dimension ref="A1:AB114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C111" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W114" sqref="W114"/>
+      <selection pane="bottomRight" activeCell="U72" sqref="U72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -9017,7 +8965,7 @@
         <v>490</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="V3" s="6" t="s">
         <v>500</v>
@@ -9052,7 +9000,7 @@
         <v>213</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
@@ -9102,10 +9050,10 @@
         <v>95</v>
       </c>
       <c r="T4" s="11" t="s">
+        <v>736</v>
+      </c>
+      <c r="U4" s="7" t="s">
         <v>738</v>
-      </c>
-      <c r="U4" s="7" t="s">
-        <v>740</v>
       </c>
       <c r="V4" s="1" t="s">
         <v>2</v>
@@ -9136,7 +9084,7 @@
         <v>214</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -10114,7 +10062,7 @@
         <v>100</v>
       </c>
       <c r="T16" s="11" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="U16" s="7" t="s">
         <v>553</v>
@@ -10544,10 +10492,10 @@
         <v>102</v>
       </c>
       <c r="T21" s="11" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="U21" s="7" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="V21" s="1" t="s">
         <v>21</v>
@@ -10624,7 +10572,7 @@
         <v>40</v>
       </c>
       <c r="R22" s="7" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="S22">
         <v>100</v>
@@ -10712,7 +10660,7 @@
         <v>60</v>
       </c>
       <c r="R23" s="7" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="S23">
         <v>100</v>
@@ -10800,7 +10748,7 @@
         <v>90</v>
       </c>
       <c r="R24" s="7" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="S24">
         <v>100</v>
@@ -11236,7 +11184,7 @@
         <v>100</v>
       </c>
       <c r="T29" s="11" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="U29" s="7" t="s">
         <v>558</v>
@@ -11784,7 +11732,7 @@
         <v>301</v>
       </c>
       <c r="D36" s="25" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="E36" s="1">
         <v>4</v>
@@ -11958,7 +11906,7 @@
         <v>235</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="E38" s="1">
         <v>3</v>
@@ -12002,16 +11950,16 @@
         <v>15</v>
       </c>
       <c r="R38" s="1" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="S38">
         <v>100</v>
       </c>
       <c r="T38" s="11" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="U38" s="7" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="V38" s="1" t="s">
         <v>49</v>
@@ -12046,7 +11994,7 @@
         <v>236</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="E39" s="1">
         <v>3</v>
@@ -12090,16 +12038,16 @@
         <v>12</v>
       </c>
       <c r="R39" s="1" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="S39">
         <v>100</v>
       </c>
       <c r="T39" s="11" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="U39" s="1" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="V39" s="1" t="s">
         <v>51</v>
@@ -12266,7 +12214,7 @@
         <v>100</v>
       </c>
       <c r="T41" s="11" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="U41" s="7" t="s">
         <v>564</v>
@@ -12474,7 +12422,7 @@
         <v>240</v>
       </c>
       <c r="D44" s="25" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="E44" s="1">
         <v>2</v>
@@ -12527,7 +12475,7 @@
         <v>359</v>
       </c>
       <c r="U44" s="7" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="V44" s="1" t="s">
         <v>57</v>
@@ -12558,7 +12506,7 @@
         <v>241</v>
       </c>
       <c r="D45" s="25" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="E45" s="1">
         <v>3</v>
@@ -12608,10 +12556,10 @@
         <v>110</v>
       </c>
       <c r="T45" s="11" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="U45" s="7" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="V45" s="1" t="s">
         <v>59</v>
@@ -12862,16 +12810,16 @@
         <v>30</v>
       </c>
       <c r="R48" s="7" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="S48">
         <v>100</v>
       </c>
       <c r="T48" s="11" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="U48" s="1" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="V48" s="1" t="s">
         <v>324</v>
@@ -12904,7 +12852,7 @@
         <v>245</v>
       </c>
       <c r="D49" s="25" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="E49" s="1">
         <v>5</v>
@@ -12954,10 +12902,10 @@
         <v>100</v>
       </c>
       <c r="T49" s="11" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="U49" s="7" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="V49" s="1" t="s">
         <v>63</v>
@@ -12990,7 +12938,7 @@
         <v>246</v>
       </c>
       <c r="D50" s="25" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="E50" s="1">
         <v>5</v>
@@ -13043,7 +12991,7 @@
         <v>522</v>
       </c>
       <c r="U50" s="7" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="V50" s="1" t="s">
         <v>65</v>
@@ -13078,7 +13026,7 @@
         <v>247</v>
       </c>
       <c r="D51" s="25" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="E51" s="1">
         <v>5</v>
@@ -13122,16 +13070,16 @@
         <v>0</v>
       </c>
       <c r="R51" s="1" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="S51">
         <v>100</v>
       </c>
       <c r="T51" s="11" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="U51" s="1" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="V51" s="1" t="s">
         <v>21</v>
@@ -13164,7 +13112,7 @@
         <v>248</v>
       </c>
       <c r="D52" s="25" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="E52" s="1">
         <v>3</v>
@@ -13217,7 +13165,7 @@
         <v>523</v>
       </c>
       <c r="U52" s="7" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="V52" s="1" t="s">
         <v>68</v>
@@ -13252,7 +13200,7 @@
         <v>249</v>
       </c>
       <c r="D53" s="25" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="E53" s="1">
         <v>4</v>
@@ -13302,10 +13250,10 @@
         <v>95</v>
       </c>
       <c r="T53" s="11" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="U53" s="7" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="V53" s="1" t="s">
         <v>70</v>
@@ -13338,7 +13286,7 @@
         <v>250</v>
       </c>
       <c r="D54" s="25" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="E54" s="1">
         <v>3</v>
@@ -13388,10 +13336,10 @@
         <v>100</v>
       </c>
       <c r="T54" s="11" t="s">
+        <v>719</v>
+      </c>
+      <c r="U54" s="1" t="s">
         <v>721</v>
-      </c>
-      <c r="U54" s="1" t="s">
-        <v>723</v>
       </c>
       <c r="V54" s="1" t="s">
         <v>72</v>
@@ -13420,13 +13368,13 @@
         <v>53000052</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="D55" s="25" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="E55" s="1">
         <v>2</v>
@@ -13470,22 +13418,22 @@
         <v>12</v>
       </c>
       <c r="R55" s="1" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="S55">
         <v>95</v>
       </c>
       <c r="T55" s="11" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="U55" s="7" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="V55" s="1" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="W55" s="1" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="X55" s="1">
         <v>11000002</v>
@@ -13514,7 +13462,7 @@
         <v>251</v>
       </c>
       <c r="D56" s="25" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="E56" s="1">
         <v>3</v>
@@ -13558,7 +13506,7 @@
         <v>20</v>
       </c>
       <c r="R56" s="1" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="S56">
         <v>100</v>
@@ -13567,7 +13515,7 @@
         <v>522</v>
       </c>
       <c r="U56" s="7" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="V56" s="1" t="s">
         <v>74</v>
@@ -13600,7 +13548,7 @@
         <v>199</v>
       </c>
       <c r="D57" s="25" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E57" s="1">
         <v>3</v>
@@ -13650,10 +13598,10 @@
         <v>100</v>
       </c>
       <c r="T57" s="11" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="U57" s="7" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="V57" s="1" t="s">
         <v>76</v>
@@ -13686,7 +13634,7 @@
         <v>252</v>
       </c>
       <c r="D58" s="25" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="E58" s="1">
         <v>4</v>
@@ -13938,10 +13886,10 @@
         <v>53000058</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="D61" s="25" t="s">
         <v>428</v>
@@ -13988,16 +13936,16 @@
         <v>12</v>
       </c>
       <c r="R61" s="1" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="S61">
         <v>100</v>
       </c>
       <c r="T61" s="11" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="U61" s="7" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="V61" s="1" t="s">
         <v>15</v>
@@ -14252,7 +14200,7 @@
         <v>100</v>
       </c>
       <c r="T64" s="11" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="U64" s="7" t="s">
         <v>356</v>
@@ -14768,10 +14716,10 @@
         <v>100</v>
       </c>
       <c r="T70" s="11" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="U70" s="7" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="V70" s="1" t="s">
         <v>95</v>
@@ -14892,7 +14840,7 @@
         <v>204</v>
       </c>
       <c r="D72" s="25" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="E72" s="1">
         <v>2</v>
@@ -14920,7 +14868,7 @@
         <v>0</v>
       </c>
       <c r="M72" s="1">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="N72" s="1">
         <v>0</v>
@@ -14942,10 +14890,10 @@
         <v>100</v>
       </c>
       <c r="T72" s="11" t="s">
-        <v>631</v>
+        <v>796</v>
       </c>
       <c r="U72" s="7" t="s">
-        <v>629</v>
+        <v>797</v>
       </c>
       <c r="V72" s="1" t="s">
         <v>99</v>
@@ -14978,7 +14926,7 @@
         <v>206</v>
       </c>
       <c r="D73" s="25" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="E73" s="1">
         <v>2</v>
@@ -15028,10 +14976,10 @@
         <v>100</v>
       </c>
       <c r="T73" s="11" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="U73" s="7" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="V73" s="1" t="s">
         <v>101</v>
@@ -15064,7 +15012,7 @@
         <v>203</v>
       </c>
       <c r="D74" s="25" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="E74" s="1">
         <v>4</v>
@@ -15114,10 +15062,10 @@
         <v>103</v>
       </c>
       <c r="T74" s="11" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="U74" s="7" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="V74" s="1" t="s">
         <v>103</v>
@@ -15152,7 +15100,7 @@
         <v>263</v>
       </c>
       <c r="D75" s="25" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="E75" s="1">
         <v>3</v>
@@ -15202,10 +15150,10 @@
         <v>102</v>
       </c>
       <c r="T75" s="11" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="U75" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="V75" s="1" t="s">
         <v>105</v>
@@ -15238,7 +15186,7 @@
         <v>264</v>
       </c>
       <c r="D76" s="25" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="E76" s="1">
         <v>3</v>
@@ -15324,7 +15272,7 @@
         <v>302</v>
       </c>
       <c r="D77" s="25" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E77" s="1">
         <v>3</v>
@@ -15374,10 +15322,10 @@
         <v>103</v>
       </c>
       <c r="T77" s="11" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="U77" s="7" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="V77" s="1" t="s">
         <v>109</v>
@@ -15410,7 +15358,7 @@
         <v>265</v>
       </c>
       <c r="D78" s="25" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="E78" s="1">
         <v>4</v>
@@ -15496,7 +15444,7 @@
         <v>266</v>
       </c>
       <c r="D79" s="25" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="E79" s="1">
         <v>3</v>
@@ -15549,7 +15497,7 @@
         <v>492</v>
       </c>
       <c r="U79" s="7" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="V79" s="1" t="s">
         <v>113</v>
@@ -15584,7 +15532,7 @@
         <v>267</v>
       </c>
       <c r="D80" s="25" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="E80" s="1">
         <v>3</v>
@@ -15670,7 +15618,7 @@
         <v>268</v>
       </c>
       <c r="D81" s="25" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="E81" s="1">
         <v>1</v>
@@ -15720,10 +15668,10 @@
         <v>100</v>
       </c>
       <c r="T81" s="39" t="s">
+        <v>737</v>
+      </c>
+      <c r="U81" s="7" t="s">
         <v>739</v>
-      </c>
-      <c r="U81" s="7" t="s">
-        <v>741</v>
       </c>
       <c r="V81" s="1" t="s">
         <v>93</v>
@@ -15754,7 +15702,7 @@
         <v>269</v>
       </c>
       <c r="D82" s="25" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="E82" s="1">
         <v>3</v>
@@ -15804,10 +15752,10 @@
         <v>100</v>
       </c>
       <c r="T82" s="11" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="U82" s="7" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="V82" s="1" t="s">
         <v>117</v>
@@ -15842,7 +15790,7 @@
         <v>270</v>
       </c>
       <c r="D83" s="25" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="E83" s="1">
         <v>2</v>
@@ -15886,16 +15834,16 @@
         <v>30</v>
       </c>
       <c r="R83" s="7" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="S83">
         <v>100</v>
       </c>
       <c r="T83" s="11" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="U83" s="7" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="V83" s="1" t="s">
         <v>81</v>
@@ -15930,7 +15878,7 @@
         <v>271</v>
       </c>
       <c r="D84" s="25" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="E84" s="1">
         <v>2</v>
@@ -15974,16 +15922,16 @@
         <v>30</v>
       </c>
       <c r="R84" s="7" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="S84">
         <v>100</v>
       </c>
       <c r="T84" s="11" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="U84" s="7" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="V84" s="1" t="s">
         <v>51</v>
@@ -16018,7 +15966,7 @@
         <v>272</v>
       </c>
       <c r="D85" s="25" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="E85" s="1">
         <v>3</v>
@@ -16068,10 +16016,10 @@
         <v>100</v>
       </c>
       <c r="T85" s="11" t="s">
+        <v>630</v>
+      </c>
+      <c r="U85" s="7" t="s">
         <v>632</v>
-      </c>
-      <c r="U85" s="7" t="s">
-        <v>634</v>
       </c>
       <c r="V85" s="1" t="s">
         <v>122</v>
@@ -16104,7 +16052,7 @@
         <v>291</v>
       </c>
       <c r="D86" s="25" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="E86" s="1">
         <v>3</v>
@@ -16157,7 +16105,7 @@
         <v>525</v>
       </c>
       <c r="U86" s="7" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="V86" s="1" t="s">
         <v>162</v>
@@ -16190,7 +16138,7 @@
         <v>205</v>
       </c>
       <c r="D87" s="25" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="E87" s="1">
         <v>4</v>
@@ -16234,16 +16182,16 @@
         <v>15</v>
       </c>
       <c r="R87" s="1" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="S87">
         <v>100</v>
       </c>
       <c r="T87" s="11" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="U87" s="7" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="V87" s="1" t="s">
         <v>469</v>
@@ -16278,7 +16226,7 @@
         <v>207</v>
       </c>
       <c r="D88" s="25" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="E88" s="1">
         <v>3</v>
@@ -16322,7 +16270,7 @@
         <v>20</v>
       </c>
       <c r="R88" s="1" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="S88">
         <v>100</v>
@@ -16331,7 +16279,7 @@
         <v>493</v>
       </c>
       <c r="U88" s="7" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="V88" s="1" t="s">
         <v>123</v>
@@ -16366,7 +16314,7 @@
         <v>208</v>
       </c>
       <c r="D89" s="25" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="E89" s="1">
         <v>2</v>
@@ -16416,10 +16364,10 @@
         <v>102</v>
       </c>
       <c r="T89" s="11" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="U89" s="7" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="V89" s="1" t="s">
         <v>2</v>
@@ -16452,7 +16400,7 @@
         <v>209</v>
       </c>
       <c r="D90" s="25" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="E90" s="1">
         <v>3</v>
@@ -16496,16 +16444,16 @@
         <v>40</v>
       </c>
       <c r="R90" s="7" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="S90">
         <v>100</v>
       </c>
       <c r="T90" s="11" t="s">
+        <v>712</v>
+      </c>
+      <c r="U90" s="7" t="s">
         <v>714</v>
-      </c>
-      <c r="U90" s="7" t="s">
-        <v>716</v>
       </c>
       <c r="V90" s="1" t="s">
         <v>59</v>
@@ -16628,7 +16576,7 @@
         <v>274</v>
       </c>
       <c r="D92" s="25" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="E92" s="1">
         <v>4</v>
@@ -16678,10 +16626,10 @@
         <v>100</v>
       </c>
       <c r="T92" s="11" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="U92" s="7" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="V92" s="1" t="s">
         <v>489</v>
@@ -16716,7 +16664,7 @@
         <v>292</v>
       </c>
       <c r="D93" s="25" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="E93" s="1">
         <v>2</v>
@@ -16802,7 +16750,7 @@
         <v>275</v>
       </c>
       <c r="D94" s="25" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="E94" s="1">
         <v>2</v>
@@ -16882,13 +16830,13 @@
         <v>53000092</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="C95" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="D95" s="25" t="s">
         <v>766</v>
-      </c>
-      <c r="D95" s="25" t="s">
-        <v>768</v>
       </c>
       <c r="E95" s="1">
         <v>3</v>
@@ -16932,19 +16880,19 @@
         <v>0</v>
       </c>
       <c r="R95" s="7" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="S95">
         <v>100</v>
       </c>
       <c r="T95" s="11" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="U95" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V95" s="1" t="s">
         <v>770</v>
-      </c>
-      <c r="V95" s="1" t="s">
-        <v>772</v>
       </c>
       <c r="W95" s="1"/>
       <c r="X95" s="1">
@@ -16974,7 +16922,7 @@
         <v>276</v>
       </c>
       <c r="D96" s="25" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E96" s="1">
         <v>2</v>
@@ -17024,10 +16972,10 @@
         <v>100</v>
       </c>
       <c r="T96" s="11" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="U96" s="7" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="V96" s="1" t="s">
         <v>134</v>
@@ -17146,7 +17094,7 @@
         <v>278</v>
       </c>
       <c r="D98" s="25" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="E98" s="1">
         <v>2</v>
@@ -17196,10 +17144,10 @@
         <v>100</v>
       </c>
       <c r="T98" s="11" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="U98" s="7" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="V98" s="1" t="s">
         <v>139</v>
@@ -17234,7 +17182,7 @@
         <v>279</v>
       </c>
       <c r="D99" s="25" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="E99" s="1">
         <v>3</v>
@@ -17278,16 +17226,16 @@
         <v>200</v>
       </c>
       <c r="R99" s="1" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="S99">
         <v>104</v>
       </c>
       <c r="T99" s="11" t="s">
+        <v>667</v>
+      </c>
+      <c r="U99" s="1" t="s">
         <v>669</v>
-      </c>
-      <c r="U99" s="1" t="s">
-        <v>671</v>
       </c>
       <c r="V99" s="1" t="s">
         <v>29</v>
@@ -17320,7 +17268,7 @@
         <v>280</v>
       </c>
       <c r="D100" s="25" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="E100" s="1">
         <v>2</v>
@@ -17370,10 +17318,10 @@
         <v>100</v>
       </c>
       <c r="T100" s="11" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="U100" s="7" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="V100" s="1" t="s">
         <v>81</v>
@@ -17406,7 +17354,7 @@
         <v>293</v>
       </c>
       <c r="D101" s="25" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="E101" s="1">
         <v>1</v>
@@ -17492,7 +17440,7 @@
         <v>281</v>
       </c>
       <c r="D102" s="25" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="E102" s="1">
         <v>1</v>
@@ -17542,10 +17490,10 @@
         <v>100</v>
       </c>
       <c r="T102" s="11" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="U102" s="7" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="V102" s="1" t="s">
         <v>97</v>
@@ -17578,7 +17526,7 @@
         <v>282</v>
       </c>
       <c r="D103" s="25" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="E103" s="1">
         <v>4</v>
@@ -17622,16 +17570,16 @@
         <v>0</v>
       </c>
       <c r="R103" s="1" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="S103">
         <v>100</v>
       </c>
       <c r="T103" s="11" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="U103" s="1" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="V103" s="1" t="s">
         <v>144</v>
@@ -17664,7 +17612,7 @@
         <v>294</v>
       </c>
       <c r="D104" s="25" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="E104" s="1">
         <v>3</v>
@@ -17708,16 +17656,16 @@
         <v>0</v>
       </c>
       <c r="R104" s="1" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="S104">
         <v>100</v>
       </c>
       <c r="T104" s="11" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="U104" s="1" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="V104" s="1" t="s">
         <v>168</v>
@@ -17750,7 +17698,7 @@
         <v>283</v>
       </c>
       <c r="D105" s="25" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="E105" s="1">
         <v>3</v>
@@ -17836,7 +17784,7 @@
         <v>284</v>
       </c>
       <c r="D106" s="25" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="E106" s="1">
         <v>3</v>
@@ -17886,10 +17834,10 @@
         <v>105</v>
       </c>
       <c r="T106" s="11" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="U106" s="7" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="V106" s="1" t="s">
         <v>147</v>
@@ -17924,7 +17872,7 @@
         <v>285</v>
       </c>
       <c r="D107" s="25" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="E107" s="1">
         <v>3</v>
@@ -17974,7 +17922,7 @@
         <v>105</v>
       </c>
       <c r="T107" s="11" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="U107" s="7" t="s">
         <v>415</v>
@@ -18096,7 +18044,7 @@
         <v>286</v>
       </c>
       <c r="D109" s="25" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="E109" s="1">
         <v>1</v>
@@ -18182,7 +18130,7 @@
         <v>287</v>
       </c>
       <c r="D110" s="25" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="E110" s="1">
         <v>1</v>
@@ -18235,7 +18183,7 @@
         <v>582</v>
       </c>
       <c r="U110" s="7" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="V110" s="1" t="s">
         <v>155</v>
@@ -18268,7 +18216,7 @@
         <v>288</v>
       </c>
       <c r="D111" s="25" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="E111" s="1">
         <v>2</v>
@@ -18318,10 +18266,10 @@
         <v>100</v>
       </c>
       <c r="T111" s="11" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="U111" s="7" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="V111" s="1" t="s">
         <v>157</v>
@@ -18354,7 +18302,7 @@
         <v>289</v>
       </c>
       <c r="D112" s="25" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="E112" s="1">
         <v>2</v>
@@ -18404,10 +18352,10 @@
         <v>100</v>
       </c>
       <c r="T112" s="11" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="U112" s="7" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="V112" s="1" t="s">
         <v>159</v>
@@ -18440,7 +18388,7 @@
         <v>290</v>
       </c>
       <c r="D113" s="25" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="E113" s="1">
         <v>3</v>
@@ -18490,10 +18438,10 @@
         <v>103</v>
       </c>
       <c r="T113" s="11" t="s">
+        <v>791</v>
+      </c>
+      <c r="U113" s="7" t="s">
         <v>793</v>
-      </c>
-      <c r="U113" s="7" t="s">
-        <v>795</v>
       </c>
       <c r="V113" s="1" t="s">
         <v>29</v>
@@ -18520,13 +18468,13 @@
         <v>53000111</v>
       </c>
       <c r="B114" s="8" t="s">
+        <v>786</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="D114" s="25" t="s">
         <v>788</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>789</v>
-      </c>
-      <c r="D114" s="25" t="s">
-        <v>790</v>
       </c>
       <c r="E114" s="1">
         <v>3</v>
@@ -18570,22 +18518,22 @@
         <v>20</v>
       </c>
       <c r="R114" s="1" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="S114">
         <v>100</v>
       </c>
       <c r="T114" s="11" t="s">
+        <v>792</v>
+      </c>
+      <c r="U114" s="7" t="s">
         <v>794</v>
       </c>
-      <c r="U114" s="7" t="s">
-        <v>796</v>
-      </c>
       <c r="V114" s="1" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="W114" s="1" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="X114" s="1">
         <v>11000007</v>
@@ -18609,85 +18557,85 @@
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I38:I68 I17:I35 I4:I15 I70:I114">
-    <cfRule type="cellIs" dxfId="61" priority="55" operator="notEqual">
+    <cfRule type="cellIs" dxfId="54" priority="55" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:O4 J17:P35 J5:P15 J38:P68 J70:P114">
-    <cfRule type="cellIs" dxfId="60" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="54" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I69">
-    <cfRule type="cellIs" dxfId="59" priority="19" operator="notEqual">
+    <cfRule type="cellIs" dxfId="52" priority="19" operator="notEqual">
       <formula>$E69</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J69:P69">
-    <cfRule type="cellIs" dxfId="58" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="18" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36">
-    <cfRule type="cellIs" dxfId="57" priority="17" operator="notEqual">
+    <cfRule type="cellIs" dxfId="50" priority="17" operator="notEqual">
       <formula>$E36</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J36:P36">
-    <cfRule type="cellIs" dxfId="56" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="16" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37">
-    <cfRule type="cellIs" dxfId="55" priority="15" operator="notEqual">
+    <cfRule type="cellIs" dxfId="48" priority="15" operator="notEqual">
       <formula>$E37</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J37:P37">
-    <cfRule type="cellIs" dxfId="54" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="14" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H15 H17:H114">
-    <cfRule type="cellIs" dxfId="53" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="10" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="11" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="12" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="13" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="43" priority="13" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="cellIs" dxfId="49" priority="7" operator="notEqual">
+    <cfRule type="cellIs" dxfId="42" priority="7" operator="notEqual">
       <formula>$E16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:P16">
-    <cfRule type="cellIs" dxfId="48" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="cellIs" dxfId="47" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="4" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="37" priority="5" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="43" priority="1" operator="containsText" text="未完成">
+    <cfRule type="containsText" dxfId="36" priority="1" operator="containsText" text="未完成">
       <formula>NOT(ISERROR(SEARCH("未完成",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19554,7 +19502,7 @@
         <v>53100007</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="34"/>
@@ -19600,16 +19548,16 @@
         <v>0</v>
       </c>
       <c r="R11" s="15" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="S11" s="1">
         <v>-1</v>
       </c>
       <c r="T11" s="11" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="U11" s="7" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="V11" s="15" t="s">
         <v>2</v>
@@ -19632,110 +19580,110 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="J4:P11">
-    <cfRule type="cellIs" dxfId="42" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="40" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:P8">
-    <cfRule type="cellIs" dxfId="41" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="36" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:P4">
-    <cfRule type="cellIs" dxfId="40" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="35" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="39" priority="34" operator="notEqual">
+    <cfRule type="cellIs" dxfId="32" priority="34" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:P4">
-    <cfRule type="cellIs" dxfId="38" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="33" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="37" priority="32" operator="notEqual">
+    <cfRule type="cellIs" dxfId="30" priority="32" operator="notEqual">
       <formula>$E5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:P5">
-    <cfRule type="cellIs" dxfId="36" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" dxfId="35" priority="30" operator="notEqual">
+    <cfRule type="cellIs" dxfId="28" priority="30" operator="notEqual">
       <formula>$E6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:P6">
-    <cfRule type="cellIs" dxfId="34" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="29" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="33" priority="28" operator="notEqual">
+    <cfRule type="cellIs" dxfId="26" priority="28" operator="notEqual">
       <formula>$E7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:P7">
-    <cfRule type="cellIs" dxfId="32" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="31" priority="26" operator="notEqual">
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="notEqual">
       <formula>$E8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:P8">
-    <cfRule type="cellIs" dxfId="30" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I11">
-    <cfRule type="cellIs" dxfId="29" priority="24" operator="notEqual">
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="notEqual">
       <formula>$E9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:P11">
-    <cfRule type="cellIs" dxfId="28" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H11">
-    <cfRule type="cellIs" dxfId="27" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="17" priority="9" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10:L11">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20546,50 +20494,50 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I4:I9">
-    <cfRule type="cellIs" dxfId="18" priority="12" operator="notEqual">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:P7">
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:P9">
-    <cfRule type="cellIs" dxfId="16" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:P8">
-    <cfRule type="cellIs" dxfId="15" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H9">
-    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
magicbook/card add ele and typesub info
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -7572,11 +7572,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2019059472"/>
-        <c:axId val="-2019058928"/>
+        <c:axId val="-263593856"/>
+        <c:axId val="-263597664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2019059472"/>
+        <c:axId val="-263593856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7619,7 +7619,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2019058928"/>
+        <c:crossAx val="-263597664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7627,7 +7627,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2019058928"/>
+        <c:axId val="-263597664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7678,7 +7678,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2019059472"/>
+        <c:crossAx val="-263593856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8307,13 +8307,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AB115" totalsRowShown="0" headerRowDxfId="127" dataDxfId="126" tableBorderDxfId="125">
-  <autoFilter ref="A3:AB115">
-    <filterColumn colId="17">
-      <customFilters>
-        <customFilter val="T*"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A3:AB115"/>
   <sortState ref="A4:AB113">
     <sortCondition ref="A3:A113"/>
   </sortState>
@@ -8736,7 +8730,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F115" sqref="F115"/>
+      <selection pane="bottomRight" activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -9019,7 +9013,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="36" hidden="1">
+    <row r="4" spans="1:28" ht="36">
       <c r="A4">
         <v>53000001</v>
       </c>
@@ -9103,7 +9097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:28" hidden="1">
+    <row r="5" spans="1:28">
       <c r="A5">
         <v>53000002</v>
       </c>
@@ -9187,7 +9181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="24" hidden="1">
+    <row r="6" spans="1:28" ht="24">
       <c r="A6">
         <v>53000003</v>
       </c>
@@ -9271,7 +9265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="36" hidden="1">
+    <row r="7" spans="1:28" ht="36">
       <c r="A7">
         <v>53000004</v>
       </c>
@@ -9357,7 +9351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="72" hidden="1">
+    <row r="8" spans="1:28" ht="72">
       <c r="A8">
         <v>53000005</v>
       </c>
@@ -9443,7 +9437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="48" hidden="1">
+    <row r="9" spans="1:28" ht="48">
       <c r="A9">
         <v>53000006</v>
       </c>
@@ -9527,7 +9521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="48" hidden="1">
+    <row r="10" spans="1:28" ht="48">
       <c r="A10">
         <v>53000007</v>
       </c>
@@ -9611,7 +9605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="48" hidden="1">
+    <row r="11" spans="1:28" ht="48">
       <c r="A11">
         <v>53000008</v>
       </c>
@@ -9695,7 +9689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="48" hidden="1">
+    <row r="12" spans="1:28" ht="48">
       <c r="A12">
         <v>53000009</v>
       </c>
@@ -9779,7 +9773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="48" hidden="1">
+    <row r="13" spans="1:28" ht="48">
       <c r="A13">
         <v>53000010</v>
       </c>
@@ -9863,7 +9857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="48" hidden="1">
+    <row r="14" spans="1:28" ht="48">
       <c r="A14">
         <v>53000011</v>
       </c>
@@ -9947,7 +9941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="48" hidden="1">
+    <row r="15" spans="1:28" ht="48">
       <c r="A15">
         <v>53000012</v>
       </c>
@@ -10031,7 +10025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="48" hidden="1">
+    <row r="16" spans="1:28" ht="48">
       <c r="A16">
         <v>53000013</v>
       </c>
@@ -10117,7 +10111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="72" hidden="1">
+    <row r="17" spans="1:28" ht="72">
       <c r="A17">
         <v>53000014</v>
       </c>
@@ -10203,7 +10197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28" hidden="1">
+    <row r="18" spans="1:28">
       <c r="A18">
         <v>53000015</v>
       </c>
@@ -10289,7 +10283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="24" hidden="1">
+    <row r="19" spans="1:28" ht="24">
       <c r="A19">
         <v>53000016</v>
       </c>
@@ -10375,7 +10369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" hidden="1">
+    <row r="20" spans="1:28">
       <c r="A20">
         <v>53000017</v>
       </c>
@@ -10461,7 +10455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="48" hidden="1">
+    <row r="21" spans="1:28" ht="48">
       <c r="A21">
         <v>53000018</v>
       </c>
@@ -10547,7 +10541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="24" hidden="1">
+    <row r="22" spans="1:28" ht="24">
       <c r="A22">
         <v>53000019</v>
       </c>
@@ -10635,7 +10629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="24" hidden="1">
+    <row r="23" spans="1:28" ht="24">
       <c r="A23">
         <v>53000020</v>
       </c>
@@ -10723,7 +10717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="24" hidden="1">
+    <row r="24" spans="1:28" ht="24">
       <c r="A24">
         <v>53000021</v>
       </c>
@@ -10811,7 +10805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="24" hidden="1">
+    <row r="25" spans="1:28" ht="24">
       <c r="A25">
         <v>53000022</v>
       </c>
@@ -10897,7 +10891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="24" hidden="1">
+    <row r="26" spans="1:28" ht="24">
       <c r="A26">
         <v>53000023</v>
       </c>
@@ -10981,7 +10975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="24" hidden="1">
+    <row r="27" spans="1:28" ht="24">
       <c r="A27">
         <v>53000024</v>
       </c>
@@ -11067,7 +11061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="48" hidden="1">
+    <row r="28" spans="1:28" ht="48">
       <c r="A28">
         <v>53000025</v>
       </c>
@@ -11239,7 +11233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:28" hidden="1">
+    <row r="30" spans="1:28">
       <c r="A30">
         <v>53000027</v>
       </c>
@@ -11323,7 +11317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:28" hidden="1">
+    <row r="31" spans="1:28">
       <c r="A31">
         <v>53000028</v>
       </c>
@@ -11407,7 +11401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:28" ht="24" hidden="1">
+    <row r="32" spans="1:28" ht="24">
       <c r="A32">
         <v>53000029</v>
       </c>
@@ -11491,7 +11485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:28" ht="24" hidden="1">
+    <row r="33" spans="1:28" ht="24">
       <c r="A33">
         <v>53000030</v>
       </c>
@@ -11577,7 +11571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:28" ht="24" hidden="1">
+    <row r="34" spans="1:28" ht="24">
       <c r="A34">
         <v>53000031</v>
       </c>
@@ -11751,7 +11745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:28" ht="48" hidden="1">
+    <row r="36" spans="1:28" ht="48">
       <c r="A36">
         <v>53000033</v>
       </c>
@@ -11775,7 +11769,7 @@
       </c>
       <c r="H36" s="1">
         <f t="shared" ref="H36:H67" si="2">IF(AND(P36&gt;=13,P36&lt;=16),5,IF(AND(P36&gt;=9,P36&lt;=12),4,IF(AND(P36&gt;=5,P36&lt;=8),3,IF(AND(P36&gt;=1,P36&lt;=4),2,IF(AND(P36&gt;=-3,P36&lt;=0),1,IF(AND(P36&gt;=-5,P36&lt;=-4),0,6))))))</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I36" s="1">
         <v>4</v>
@@ -11784,7 +11778,7 @@
         <v>0</v>
       </c>
       <c r="K36" s="1">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="L36" s="1">
         <v>0</v>
@@ -11800,7 +11794,7 @@
       </c>
       <c r="P36" s="38">
         <f t="shared" ref="P36:P67" si="3">S36-100+O36</f>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="Q36" s="1">
         <v>12</v>
@@ -11809,7 +11803,7 @@
         <v>118</v>
       </c>
       <c r="S36">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="T36" s="11" t="s">
         <v>548</v>
@@ -11839,7 +11833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:28" ht="36" hidden="1">
+    <row r="37" spans="1:28" ht="36">
       <c r="A37">
         <v>53000034</v>
       </c>
@@ -11925,7 +11919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:28" ht="60" hidden="1">
+    <row r="38" spans="1:28" ht="60">
       <c r="A38">
         <v>53000035</v>
       </c>
@@ -12013,7 +12007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:28" ht="36" hidden="1">
+    <row r="39" spans="1:28" ht="36">
       <c r="A39">
         <v>53000036</v>
       </c>
@@ -12099,7 +12093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:28" ht="24" hidden="1">
+    <row r="40" spans="1:28" ht="24">
       <c r="A40">
         <v>53000037</v>
       </c>
@@ -12183,7 +12177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:28" ht="24" hidden="1">
+    <row r="41" spans="1:28" ht="24">
       <c r="A41">
         <v>53000038</v>
       </c>
@@ -12269,7 +12263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:28" ht="24" hidden="1">
+    <row r="42" spans="1:28" ht="24">
       <c r="A42">
         <v>53000039</v>
       </c>
@@ -12355,7 +12349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:28" ht="24" hidden="1">
+    <row r="43" spans="1:28" ht="24">
       <c r="A43">
         <v>53000040</v>
       </c>
@@ -12441,7 +12435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:28" ht="24" hidden="1">
+    <row r="44" spans="1:28" ht="24">
       <c r="A44">
         <v>53000041</v>
       </c>
@@ -12525,7 +12519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:28" ht="72" hidden="1">
+    <row r="45" spans="1:28" ht="72">
       <c r="A45">
         <v>53000042</v>
       </c>
@@ -12613,7 +12607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:28" ht="24" hidden="1">
+    <row r="46" spans="1:28" ht="24">
       <c r="A46">
         <v>53000043</v>
       </c>
@@ -12699,7 +12693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:28" ht="24" hidden="1">
+    <row r="47" spans="1:28" ht="24">
       <c r="A47">
         <v>53000044</v>
       </c>
@@ -12785,7 +12779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:28" ht="60" hidden="1">
+    <row r="48" spans="1:28" ht="60">
       <c r="A48">
         <v>53000045</v>
       </c>
@@ -12871,7 +12865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:28" ht="48" hidden="1">
+    <row r="49" spans="1:28" ht="48">
       <c r="A49">
         <v>53000046</v>
       </c>
@@ -12957,7 +12951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:28" ht="60" hidden="1">
+    <row r="50" spans="1:28" ht="60">
       <c r="A50">
         <v>53000047</v>
       </c>
@@ -13045,7 +13039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:28" ht="24" hidden="1">
+    <row r="51" spans="1:28" ht="24">
       <c r="A51">
         <v>53000048</v>
       </c>
@@ -13131,7 +13125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:28" ht="72" hidden="1">
+    <row r="52" spans="1:28" ht="72">
       <c r="A52">
         <v>53000049</v>
       </c>
@@ -13219,7 +13213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:28" ht="60" hidden="1">
+    <row r="53" spans="1:28" ht="60">
       <c r="A53">
         <v>53000050</v>
       </c>
@@ -13305,7 +13299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:28" ht="72" hidden="1">
+    <row r="54" spans="1:28" ht="72">
       <c r="A54">
         <v>53000051</v>
       </c>
@@ -13393,7 +13387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:28" ht="132" hidden="1">
+    <row r="55" spans="1:28" ht="132">
       <c r="A55">
         <v>53000052</v>
       </c>
@@ -13481,7 +13475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:28" ht="60" hidden="1">
+    <row r="56" spans="1:28" ht="60">
       <c r="A56">
         <v>53000053</v>
       </c>
@@ -13567,7 +13561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:28" ht="36" hidden="1">
+    <row r="57" spans="1:28" ht="36">
       <c r="A57">
         <v>53000054</v>
       </c>
@@ -13653,7 +13647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:28" ht="24" hidden="1">
+    <row r="58" spans="1:28" ht="24">
       <c r="A58">
         <v>53000055</v>
       </c>
@@ -13739,7 +13733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:28" ht="36" hidden="1">
+    <row r="59" spans="1:28" ht="36">
       <c r="A59">
         <v>53000056</v>
       </c>
@@ -13825,7 +13819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:28" ht="24" hidden="1">
+    <row r="60" spans="1:28" ht="24">
       <c r="A60">
         <v>53000057</v>
       </c>
@@ -13911,7 +13905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:28" ht="60" hidden="1">
+    <row r="61" spans="1:28" ht="60">
       <c r="A61">
         <v>53000058</v>
       </c>
@@ -13997,7 +13991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:28" ht="24" hidden="1">
+    <row r="62" spans="1:28" ht="24">
       <c r="A62">
         <v>53000059</v>
       </c>
@@ -14083,7 +14077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:28" ht="36" hidden="1">
+    <row r="63" spans="1:28" ht="36">
       <c r="A63">
         <v>53000060</v>
       </c>
@@ -14169,7 +14163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:28" ht="48" hidden="1">
+    <row r="64" spans="1:28" ht="48">
       <c r="A64">
         <v>53000061</v>
       </c>
@@ -14255,7 +14249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:28" ht="24" hidden="1">
+    <row r="65" spans="1:28" ht="24">
       <c r="A65">
         <v>53000062</v>
       </c>
@@ -14341,7 +14335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:28" hidden="1">
+    <row r="66" spans="1:28">
       <c r="A66">
         <v>53000063</v>
       </c>
@@ -14427,7 +14421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:28" ht="24" hidden="1">
+    <row r="67" spans="1:28" ht="24">
       <c r="A67">
         <v>53000064</v>
       </c>
@@ -14513,7 +14507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:28" ht="48" hidden="1">
+    <row r="68" spans="1:28" ht="48">
       <c r="A68">
         <v>53000065</v>
       </c>
@@ -14599,7 +14593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:28" ht="24" hidden="1">
+    <row r="69" spans="1:28" ht="24">
       <c r="A69">
         <v>53000066</v>
       </c>
@@ -14685,7 +14679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:28" ht="24" hidden="1">
+    <row r="70" spans="1:28" ht="24">
       <c r="A70">
         <v>53000067</v>
       </c>
@@ -14771,7 +14765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:28" ht="60" hidden="1">
+    <row r="71" spans="1:28" ht="60">
       <c r="A71">
         <v>53000068</v>
       </c>
@@ -14859,7 +14853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:28" ht="48" hidden="1">
+    <row r="72" spans="1:28" ht="48">
       <c r="A72">
         <v>53000069</v>
       </c>
@@ -14945,7 +14939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:28" ht="36" hidden="1">
+    <row r="73" spans="1:28" ht="36">
       <c r="A73">
         <v>53000070</v>
       </c>
@@ -15031,7 +15025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:28" ht="84" hidden="1">
+    <row r="74" spans="1:28" ht="84">
       <c r="A74">
         <v>53000071</v>
       </c>
@@ -15119,7 +15113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:28" ht="60" hidden="1">
+    <row r="75" spans="1:28" ht="60">
       <c r="A75">
         <v>53000072</v>
       </c>
@@ -15205,7 +15199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:28" ht="48" hidden="1">
+    <row r="76" spans="1:28" ht="48">
       <c r="A76">
         <v>53000073</v>
       </c>
@@ -15291,7 +15285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:28" ht="36" hidden="1">
+    <row r="77" spans="1:28" ht="36">
       <c r="A77">
         <v>53000074</v>
       </c>
@@ -15377,7 +15371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:28" ht="108" hidden="1">
+    <row r="78" spans="1:28" ht="108">
       <c r="A78">
         <v>53000075</v>
       </c>
@@ -15463,7 +15457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:28" ht="60" hidden="1">
+    <row r="79" spans="1:28" ht="60">
       <c r="A79">
         <v>53000076</v>
       </c>
@@ -15551,7 +15545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:28" ht="48" hidden="1">
+    <row r="80" spans="1:28" ht="48">
       <c r="A80">
         <v>53000077</v>
       </c>
@@ -15637,7 +15631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:28" ht="36" hidden="1">
+    <row r="81" spans="1:28" ht="36">
       <c r="A81">
         <v>53000078</v>
       </c>
@@ -15721,7 +15715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:28" ht="60" hidden="1">
+    <row r="82" spans="1:28" ht="60">
       <c r="A82">
         <v>53000079</v>
       </c>
@@ -15809,7 +15803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:28" ht="60" hidden="1">
+    <row r="83" spans="1:28" ht="60">
       <c r="A83">
         <v>53000080</v>
       </c>
@@ -15897,7 +15891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:28" ht="72" hidden="1">
+    <row r="84" spans="1:28" ht="72">
       <c r="A84">
         <v>53000081</v>
       </c>
@@ -15985,7 +15979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:28" ht="24" hidden="1">
+    <row r="85" spans="1:28" ht="24">
       <c r="A85">
         <v>53000082</v>
       </c>
@@ -16071,7 +16065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:28" ht="48" hidden="1">
+    <row r="86" spans="1:28" ht="48">
       <c r="A86">
         <v>53000083</v>
       </c>
@@ -16157,7 +16151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:28" ht="60" hidden="1">
+    <row r="87" spans="1:28" ht="60">
       <c r="A87">
         <v>53000084</v>
       </c>
@@ -16333,7 +16327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:28" ht="60" hidden="1">
+    <row r="89" spans="1:28" ht="60">
       <c r="A89">
         <v>53000086</v>
       </c>
@@ -16419,7 +16413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:28" ht="48" hidden="1">
+    <row r="90" spans="1:28" ht="48">
       <c r="A90">
         <v>53000087</v>
       </c>
@@ -16507,7 +16501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:28" ht="60" hidden="1">
+    <row r="91" spans="1:28" ht="60">
       <c r="A91">
         <v>53000088</v>
       </c>
@@ -16595,7 +16589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:28" ht="60" hidden="1">
+    <row r="92" spans="1:28" ht="60">
       <c r="A92">
         <v>53000089</v>
       </c>
@@ -16683,7 +16677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:28" ht="24" hidden="1">
+    <row r="93" spans="1:28" ht="24">
       <c r="A93">
         <v>53000090</v>
       </c>
@@ -16769,7 +16763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:28" ht="36" hidden="1">
+    <row r="94" spans="1:28" ht="36">
       <c r="A94">
         <v>53000091</v>
       </c>
@@ -16855,7 +16849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:28" ht="24" hidden="1">
+    <row r="95" spans="1:28" ht="24">
       <c r="A95">
         <v>53000092</v>
       </c>
@@ -16941,7 +16935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:28" ht="60" hidden="1">
+    <row r="96" spans="1:28" ht="60">
       <c r="A96">
         <v>53000093</v>
       </c>
@@ -17027,7 +17021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:28" ht="36" hidden="1">
+    <row r="97" spans="1:28" ht="36">
       <c r="A97">
         <v>53000094</v>
       </c>
@@ -17051,7 +17045,7 @@
       </c>
       <c r="H97" s="1">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I97" s="1">
         <v>2</v>
@@ -17076,7 +17070,7 @@
       </c>
       <c r="P97" s="38">
         <f t="shared" si="5"/>
-        <v>-75</v>
+        <v>0</v>
       </c>
       <c r="Q97" s="1">
         <v>200</v>
@@ -17085,7 +17079,7 @@
         <v>136</v>
       </c>
       <c r="S97">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="T97" s="11" t="s">
         <v>613</v>
@@ -17113,7 +17107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:28" ht="60" hidden="1">
+    <row r="98" spans="1:28" ht="60">
       <c r="A98">
         <v>53000095</v>
       </c>
@@ -17201,7 +17195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:28" ht="36" hidden="1">
+    <row r="99" spans="1:28" ht="36">
       <c r="A99">
         <v>53000096</v>
       </c>
@@ -17287,7 +17281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:28" ht="60" hidden="1">
+    <row r="100" spans="1:28" ht="60">
       <c r="A100">
         <v>53000097</v>
       </c>
@@ -17373,7 +17367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:28" ht="24" hidden="1">
+    <row r="101" spans="1:28" ht="24">
       <c r="A101">
         <v>53000098</v>
       </c>
@@ -17459,7 +17453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:28" ht="24" hidden="1">
+    <row r="102" spans="1:28" ht="24">
       <c r="A102">
         <v>53000099</v>
       </c>
@@ -17545,7 +17539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:28" ht="72" hidden="1">
+    <row r="103" spans="1:28" ht="72">
       <c r="A103">
         <v>53000100</v>
       </c>
@@ -17631,7 +17625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:28" ht="24" hidden="1">
+    <row r="104" spans="1:28" ht="24">
       <c r="A104">
         <v>53000101</v>
       </c>
@@ -17717,7 +17711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:28" ht="24" hidden="1">
+    <row r="105" spans="1:28" ht="24">
       <c r="A105">
         <v>53000102</v>
       </c>
@@ -17803,7 +17797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:28" ht="72" hidden="1">
+    <row r="106" spans="1:28" ht="72">
       <c r="A106">
         <v>53000103</v>
       </c>
@@ -17891,7 +17885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:28" ht="60" hidden="1">
+    <row r="107" spans="1:28" ht="60">
       <c r="A107">
         <v>53000104</v>
       </c>
@@ -17977,7 +17971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:28" ht="36" hidden="1">
+    <row r="108" spans="1:28" ht="36">
       <c r="A108">
         <v>53000105</v>
       </c>
@@ -18001,7 +17995,7 @@
       </c>
       <c r="H108" s="1">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I108" s="1">
         <v>3</v>
@@ -18022,11 +18016,11 @@
         <v>0</v>
       </c>
       <c r="O108" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P108" s="38">
         <f t="shared" si="7"/>
-        <v>-75</v>
+        <v>2</v>
       </c>
       <c r="Q108" s="1">
         <v>10</v>
@@ -18035,7 +18029,7 @@
         <v>136</v>
       </c>
       <c r="S108">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="T108" s="11" t="s">
         <v>615</v>
@@ -18063,7 +18057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:28" ht="24" hidden="1">
+    <row r="109" spans="1:28" ht="24">
       <c r="A109">
         <v>53000106</v>
       </c>
@@ -18149,7 +18143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:28" ht="24" hidden="1">
+    <row r="110" spans="1:28" ht="24">
       <c r="A110">
         <v>53000107</v>
       </c>
@@ -18235,7 +18229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:28" ht="120" hidden="1">
+    <row r="111" spans="1:28" ht="120">
       <c r="A111">
         <v>53000108</v>
       </c>
@@ -18321,7 +18315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:28" ht="24" hidden="1">
+    <row r="112" spans="1:28" ht="24">
       <c r="A112">
         <v>53000109</v>
       </c>
@@ -18407,7 +18401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:28" ht="36" hidden="1">
+    <row r="113" spans="1:28" ht="36">
       <c r="A113">
         <v>53000110</v>
       </c>
@@ -18493,7 +18487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:28" ht="72" hidden="1">
+    <row r="114" spans="1:28" ht="72">
       <c r="A114">
         <v>53000111</v>
       </c>

</xml_diff>

<commit_message>
# new card Sprint
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -639,7 +639,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="801">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="807">
   <si>
     <t>慈悲</t>
   </si>
@@ -2720,10 +2720,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>破坏所有敌方单位的武器，{4:0.0}%几率抽取额外1张卡牌</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse))im.AddBuff(56000011,lv,s.Time);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -2852,14 +2848,6 @@
   </si>
   <si>
     <t>将我方单位变换为随机怪物，并回复{1}点生命</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>抽取1张卡片,{4:0.0}%几率抽取额外1张卡牌</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>下一张使用的怪物卡消耗为0,{4:0.0}%几率抽取额外1张卡牌</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -3357,10 +3345,6 @@
   </si>
   <si>
     <t>Shiv</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>p.GetNextNCard(null,1);if(MathTool.GetRandom(100)&lt;s.Rate) p.GetNextNCard(null,1);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -3522,6 +3506,42 @@
   </si>
   <si>
     <t>策反目标敌方怪物，并回复其{1}点生命</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprint</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>疾跑</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>p.GetNextNCard(null,1);if(MathTool.GetRandom(100)&lt;s.Rate) p.GetNextNCard(null,1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(MathTool.GetRandom(100)&lt;s.Rate) p.GetNextNCard(null,3);else p.GetNextNCard(null,4);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>抽1张卡片,{4:0.0}%几率抽额外1张卡牌</t>
+  </si>
+  <si>
+    <t>下一张使用的怪物卡消耗为0,{4:0.0}%几率抽额外1张卡牌</t>
+  </si>
+  <si>
+    <t>破坏所有敌方单位的武器，{4:0.0}%几率抽额外1张卡牌</t>
+  </si>
+  <si>
+    <t>抽3张卡片,{4:0.0}%几率抽额外1张卡牌</t>
+  </si>
+  <si>
+    <t>yellowflash</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NFO</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -4524,54 +4544,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="150">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="148">
     <dxf>
       <font>
         <b/>
@@ -5020,6 +4993,33 @@
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -8289,132 +8289,132 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AB120" totalsRowShown="0" headerRowDxfId="149" dataDxfId="148" tableBorderDxfId="147">
-  <autoFilter ref="A3:AB120"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AB121" totalsRowShown="0" headerRowDxfId="147" dataDxfId="146" tableBorderDxfId="145">
+  <autoFilter ref="A3:AB121"/>
   <sortState ref="A4:AB113">
     <sortCondition ref="A3:A113"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="146"/>
-    <tableColumn id="2" name="Name" dataDxfId="145"/>
-    <tableColumn id="20" name="Ename" dataDxfId="144"/>
-    <tableColumn id="21" name="Remark" dataDxfId="143"/>
-    <tableColumn id="3" name="Star" dataDxfId="142"/>
-    <tableColumn id="4" name="Type" dataDxfId="141"/>
-    <tableColumn id="5" name="Attr" dataDxfId="140"/>
-    <tableColumn id="8" name="Quality" dataDxfId="139">
+    <tableColumn id="1" name="Id" dataDxfId="144"/>
+    <tableColumn id="2" name="Name" dataDxfId="143"/>
+    <tableColumn id="20" name="Ename" dataDxfId="142"/>
+    <tableColumn id="21" name="Remark" dataDxfId="141"/>
+    <tableColumn id="3" name="Star" dataDxfId="140"/>
+    <tableColumn id="4" name="Type" dataDxfId="139"/>
+    <tableColumn id="5" name="Attr" dataDxfId="138"/>
+    <tableColumn id="8" name="Quality" dataDxfId="137">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="138"/>
-    <tableColumn id="9" name="Damage" dataDxfId="137"/>
-    <tableColumn id="10" name="Cure" dataDxfId="136"/>
-    <tableColumn id="11" name="Time" dataDxfId="135"/>
-    <tableColumn id="13" name="Help" dataDxfId="134"/>
-    <tableColumn id="16" name="Rate" dataDxfId="133"/>
-    <tableColumn id="18" name="Atk" dataDxfId="60"/>
-    <tableColumn id="12" name="Modify" dataDxfId="132"/>
-    <tableColumn id="27" name="Sum" dataDxfId="131">
+    <tableColumn id="7" name="Cost" dataDxfId="136"/>
+    <tableColumn id="9" name="Damage" dataDxfId="135"/>
+    <tableColumn id="10" name="Cure" dataDxfId="134"/>
+    <tableColumn id="11" name="Time" dataDxfId="133"/>
+    <tableColumn id="13" name="Help" dataDxfId="132"/>
+    <tableColumn id="16" name="Rate" dataDxfId="131"/>
+    <tableColumn id="18" name="Atk" dataDxfId="58"/>
+    <tableColumn id="12" name="Modify" dataDxfId="130"/>
+    <tableColumn id="27" name="Sum" dataDxfId="129">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="130"/>
-    <tableColumn id="15" name="Target" dataDxfId="129"/>
-    <tableColumn id="25" name="Mark" dataDxfId="128"/>
-    <tableColumn id="22" name="Effect" dataDxfId="127"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="126"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="125"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="124"/>
-    <tableColumn id="26" name="JobId" dataDxfId="123"/>
-    <tableColumn id="19" name="Icon" dataDxfId="122"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="121"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="120"/>
+    <tableColumn id="6" name="Range" dataDxfId="128"/>
+    <tableColumn id="15" name="Target" dataDxfId="127"/>
+    <tableColumn id="25" name="Mark" dataDxfId="126"/>
+    <tableColumn id="22" name="Effect" dataDxfId="125"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="124"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="123"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="122"/>
+    <tableColumn id="26" name="JobId" dataDxfId="121"/>
+    <tableColumn id="19" name="Icon" dataDxfId="120"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="119"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="118"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AB11" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118" tableBorderDxfId="117">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AB11" totalsRowShown="0" headerRowDxfId="117" dataDxfId="116" tableBorderDxfId="115">
   <autoFilter ref="A3:AB11"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="116"/>
-    <tableColumn id="2" name="Name" dataDxfId="115"/>
-    <tableColumn id="20" name="Ename" dataDxfId="114"/>
-    <tableColumn id="21" name="Remark" dataDxfId="113"/>
-    <tableColumn id="3" name="Star" dataDxfId="112"/>
-    <tableColumn id="4" name="Type" dataDxfId="111"/>
-    <tableColumn id="5" name="Attr" dataDxfId="110"/>
-    <tableColumn id="8" name="Quality" dataDxfId="109">
+    <tableColumn id="1" name="Id" dataDxfId="114"/>
+    <tableColumn id="2" name="Name" dataDxfId="113"/>
+    <tableColumn id="20" name="Ename" dataDxfId="112"/>
+    <tableColumn id="21" name="Remark" dataDxfId="111"/>
+    <tableColumn id="3" name="Star" dataDxfId="110"/>
+    <tableColumn id="4" name="Type" dataDxfId="109"/>
+    <tableColumn id="5" name="Attr" dataDxfId="108"/>
+    <tableColumn id="8" name="Quality" dataDxfId="107">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="108"/>
-    <tableColumn id="9" name="Damage" dataDxfId="107"/>
-    <tableColumn id="10" name="Cure" dataDxfId="106"/>
-    <tableColumn id="11" name="Time" dataDxfId="105"/>
-    <tableColumn id="13" name="Help" dataDxfId="104"/>
-    <tableColumn id="16" name="Rate" dataDxfId="103"/>
-    <tableColumn id="18" name="Atk" dataDxfId="59"/>
-    <tableColumn id="12" name="Modify" dataDxfId="102"/>
-    <tableColumn id="27" name="Sum" dataDxfId="101">
+    <tableColumn id="7" name="Cost" dataDxfId="106"/>
+    <tableColumn id="9" name="Damage" dataDxfId="105"/>
+    <tableColumn id="10" name="Cure" dataDxfId="104"/>
+    <tableColumn id="11" name="Time" dataDxfId="103"/>
+    <tableColumn id="13" name="Help" dataDxfId="102"/>
+    <tableColumn id="16" name="Rate" dataDxfId="101"/>
+    <tableColumn id="18" name="Atk" dataDxfId="57"/>
+    <tableColumn id="12" name="Modify" dataDxfId="100"/>
+    <tableColumn id="27" name="Sum" dataDxfId="99">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="100"/>
-    <tableColumn id="15" name="Target" dataDxfId="99"/>
-    <tableColumn id="25" name="Mark" dataDxfId="98"/>
-    <tableColumn id="22" name="Effect" dataDxfId="97"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="96"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="95"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="94"/>
-    <tableColumn id="26" name="JobId" dataDxfId="93"/>
-    <tableColumn id="19" name="Icon" dataDxfId="92"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="91"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="90"/>
+    <tableColumn id="6" name="Range" dataDxfId="98"/>
+    <tableColumn id="15" name="Target" dataDxfId="97"/>
+    <tableColumn id="25" name="Mark" dataDxfId="96"/>
+    <tableColumn id="22" name="Effect" dataDxfId="95"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="94"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="93"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="92"/>
+    <tableColumn id="26" name="JobId" dataDxfId="91"/>
+    <tableColumn id="19" name="Icon" dataDxfId="90"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="89"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="88"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_35" displayName="表1_35" ref="A3:AB9" totalsRowShown="0" headerRowDxfId="89" tableBorderDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_35" displayName="表1_35" ref="A3:AB9" totalsRowShown="0" headerRowDxfId="87" tableBorderDxfId="86">
   <autoFilter ref="A3:AB9"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="87"/>
-    <tableColumn id="2" name="Name" dataDxfId="86"/>
-    <tableColumn id="20" name="Ename" dataDxfId="85"/>
-    <tableColumn id="21" name="Remark" dataDxfId="84"/>
-    <tableColumn id="3" name="Star" dataDxfId="83"/>
-    <tableColumn id="4" name="Type" dataDxfId="82"/>
-    <tableColumn id="5" name="Attr" dataDxfId="81"/>
-    <tableColumn id="8" name="Quality" dataDxfId="80">
+    <tableColumn id="1" name="Id" dataDxfId="85"/>
+    <tableColumn id="2" name="Name" dataDxfId="84"/>
+    <tableColumn id="20" name="Ename" dataDxfId="83"/>
+    <tableColumn id="21" name="Remark" dataDxfId="82"/>
+    <tableColumn id="3" name="Star" dataDxfId="81"/>
+    <tableColumn id="4" name="Type" dataDxfId="80"/>
+    <tableColumn id="5" name="Attr" dataDxfId="79"/>
+    <tableColumn id="8" name="Quality" dataDxfId="78">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="79"/>
-    <tableColumn id="9" name="Damage" dataDxfId="78"/>
-    <tableColumn id="10" name="Cure" dataDxfId="77"/>
-    <tableColumn id="11" name="Time" dataDxfId="76"/>
-    <tableColumn id="13" name="Help" dataDxfId="75"/>
-    <tableColumn id="16" name="Rate" dataDxfId="74"/>
-    <tableColumn id="18" name="Atk" dataDxfId="2"/>
-    <tableColumn id="12" name="Modify" dataDxfId="73"/>
-    <tableColumn id="27" name="Sum" dataDxfId="72">
+    <tableColumn id="7" name="Cost" dataDxfId="77"/>
+    <tableColumn id="9" name="Damage" dataDxfId="76"/>
+    <tableColumn id="10" name="Cure" dataDxfId="75"/>
+    <tableColumn id="11" name="Time" dataDxfId="74"/>
+    <tableColumn id="13" name="Help" dataDxfId="73"/>
+    <tableColumn id="16" name="Rate" dataDxfId="72"/>
+    <tableColumn id="18" name="Atk" dataDxfId="56"/>
+    <tableColumn id="12" name="Modify" dataDxfId="71"/>
+    <tableColumn id="27" name="Sum" dataDxfId="70">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="71"/>
-    <tableColumn id="15" name="Target" dataDxfId="70"/>
-    <tableColumn id="25" name="Mark" dataDxfId="69"/>
-    <tableColumn id="22" name="Effect" dataDxfId="68"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="67"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="66"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="65"/>
-    <tableColumn id="26" name="JobId" dataDxfId="64"/>
-    <tableColumn id="19" name="Icon" dataDxfId="63"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="62"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="61"/>
+    <tableColumn id="6" name="Range" dataDxfId="69"/>
+    <tableColumn id="15" name="Target" dataDxfId="68"/>
+    <tableColumn id="25" name="Mark" dataDxfId="67"/>
+    <tableColumn id="22" name="Effect" dataDxfId="66"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="65"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="64"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="63"/>
+    <tableColumn id="26" name="JobId" dataDxfId="62"/>
+    <tableColumn id="19" name="Icon" dataDxfId="61"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="60"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8707,13 +8707,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB120"/>
+  <dimension ref="A1:AB121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C117" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="V20" sqref="V20"/>
+      <selection pane="bottomRight" activeCell="S121" sqref="S121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8782,7 +8782,7 @@
         <v>349</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="P1" s="17" t="s">
         <v>331</v>
@@ -8868,7 +8868,7 @@
         <v>350</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>332</v>
@@ -8886,7 +8886,7 @@
         <v>502</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="V2" s="10" t="s">
         <v>179</v>
@@ -8954,7 +8954,7 @@
         <v>351</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="P3" s="20" t="s">
         <v>333</v>
@@ -8975,7 +8975,7 @@
         <v>475</v>
       </c>
       <c r="V3" s="6" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="W3" s="6" t="s">
         <v>482</v>
@@ -9007,7 +9007,7 @@
         <v>211</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
@@ -9060,10 +9060,10 @@
         <v>95</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>765</v>
+        <v>799</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>629</v>
+        <v>801</v>
       </c>
       <c r="W4" s="1" t="s">
         <v>2</v>
@@ -9091,7 +9091,7 @@
         <v>212</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -9175,7 +9175,7 @@
         <v>213</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="E6" s="1">
         <v>2</v>
@@ -9228,7 +9228,7 @@
         <v>100</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="V6" s="7" t="s">
         <v>380</v>
@@ -9259,7 +9259,7 @@
         <v>214</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
@@ -9312,7 +9312,7 @@
         <v>100</v>
       </c>
       <c r="U7" s="11" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="V7" s="7" t="s">
         <v>381</v>
@@ -9345,7 +9345,7 @@
         <v>215</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="E8" s="1">
         <v>3</v>
@@ -9431,7 +9431,7 @@
         <v>294</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
@@ -9515,7 +9515,7 @@
         <v>295</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -9599,7 +9599,7 @@
         <v>296</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -9683,7 +9683,7 @@
         <v>297</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
@@ -9767,7 +9767,7 @@
         <v>216</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
@@ -9851,7 +9851,7 @@
         <v>210</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
@@ -9935,7 +9935,7 @@
         <v>217</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
@@ -10019,7 +10019,7 @@
         <v>372</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="E16" s="15">
         <v>4</v>
@@ -10105,7 +10105,7 @@
         <v>480</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="E17" s="1">
         <v>2</v>
@@ -10191,7 +10191,7 @@
         <v>218</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="E18" s="1">
         <v>1</v>
@@ -10244,10 +10244,10 @@
         <v>75</v>
       </c>
       <c r="U18" s="11" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="V18" s="7" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="W18" s="1" t="s">
         <v>15</v>
@@ -10277,7 +10277,7 @@
         <v>219</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="E19" s="1">
         <v>3</v>
@@ -10363,7 +10363,7 @@
         <v>220</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="E20" s="1">
         <v>7</v>
@@ -10416,13 +10416,13 @@
         <v>100</v>
       </c>
       <c r="U20" s="11" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="V20" s="7" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="X20" s="1"/>
       <c r="Y20" s="1">
@@ -10449,7 +10449,7 @@
         <v>221</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="E21" s="1">
         <v>3</v>
@@ -10502,10 +10502,10 @@
         <v>102</v>
       </c>
       <c r="U21" s="11" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="V21" s="7" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="W21" s="1" t="s">
         <v>21</v>
@@ -10535,7 +10535,7 @@
         <v>222</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="E22" s="1">
         <v>4</v>
@@ -10582,13 +10582,13 @@
         <v>40</v>
       </c>
       <c r="S22" s="7" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="T22">
         <v>100</v>
       </c>
       <c r="U22" s="11" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="V22" s="7" t="s">
         <v>536</v>
@@ -10623,7 +10623,7 @@
         <v>223</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="E23" s="1">
         <v>3</v>
@@ -10670,7 +10670,7 @@
         <v>60</v>
       </c>
       <c r="S23" s="7" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="T23">
         <v>100</v>
@@ -10711,7 +10711,7 @@
         <v>224</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="E24" s="1">
         <v>3</v>
@@ -10758,7 +10758,7 @@
         <v>90</v>
       </c>
       <c r="S24" s="7" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="T24">
         <v>100</v>
@@ -11022,7 +11022,7 @@
         <v>90</v>
       </c>
       <c r="U27" s="11" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="V27" s="7" t="s">
         <v>395</v>
@@ -11055,7 +11055,7 @@
         <v>228</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="E28" s="1">
         <v>3</v>
@@ -11108,7 +11108,7 @@
         <v>100</v>
       </c>
       <c r="U28" s="11" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="V28" s="7" t="s">
         <v>522</v>
@@ -11141,7 +11141,7 @@
         <v>229</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="E29" s="1">
         <v>4</v>
@@ -11194,7 +11194,7 @@
         <v>100</v>
       </c>
       <c r="U29" s="11" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="V29" s="7" t="s">
         <v>519</v>
@@ -11227,7 +11227,7 @@
         <v>230</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E30" s="1">
         <v>1</v>
@@ -11311,7 +11311,7 @@
         <v>231</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
@@ -11395,7 +11395,7 @@
         <v>232</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="E32" s="1">
         <v>4</v>
@@ -11448,7 +11448,7 @@
         <v>100</v>
       </c>
       <c r="U32" s="11" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="V32" s="21" t="s">
         <v>343</v>
@@ -11651,7 +11651,7 @@
         <v>298</v>
       </c>
       <c r="D35" s="25" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="E35" s="1">
         <v>3</v>
@@ -11704,7 +11704,7 @@
         <v>100</v>
       </c>
       <c r="U35" s="11" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="V35" s="7" t="s">
         <v>420</v>
@@ -11739,7 +11739,7 @@
         <v>299</v>
       </c>
       <c r="D36" s="25" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="E36" s="1">
         <v>4</v>
@@ -11880,7 +11880,7 @@
         <v>100</v>
       </c>
       <c r="U37" s="11" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="V37" s="7" t="s">
         <v>357</v>
@@ -11913,7 +11913,7 @@
         <v>233</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="E38" s="1">
         <v>3</v>
@@ -11960,16 +11960,16 @@
         <v>15</v>
       </c>
       <c r="S38" s="1" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="T38">
         <v>100</v>
       </c>
       <c r="U38" s="11" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="V38" s="7" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="W38" s="1" t="s">
         <v>49</v>
@@ -12001,7 +12001,7 @@
         <v>234</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="E39" s="1">
         <v>3</v>
@@ -12048,16 +12048,16 @@
         <v>12</v>
       </c>
       <c r="S39" s="1" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="T39">
         <v>100</v>
       </c>
       <c r="U39" s="11" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="V39" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="W39" s="1" t="s">
         <v>51</v>
@@ -12087,7 +12087,7 @@
         <v>235</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="E40" s="1">
         <v>1</v>
@@ -12171,7 +12171,7 @@
         <v>236</v>
       </c>
       <c r="D41" s="25" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="E41" s="1">
         <v>2</v>
@@ -12224,7 +12224,7 @@
         <v>100</v>
       </c>
       <c r="U41" s="11" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="V41" s="7" t="s">
         <v>524</v>
@@ -12482,7 +12482,7 @@
         <v>100</v>
       </c>
       <c r="U44" s="11" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="V44" s="7" t="s">
         <v>580</v>
@@ -12513,7 +12513,7 @@
         <v>239</v>
       </c>
       <c r="D45" s="25" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="E45" s="1">
         <v>3</v>
@@ -12566,10 +12566,10 @@
         <v>110</v>
       </c>
       <c r="U45" s="11" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="V45" s="7" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="W45" s="1" t="s">
         <v>59</v>
@@ -12820,16 +12820,16 @@
         <v>30</v>
       </c>
       <c r="S48" s="7" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="T48">
         <v>100</v>
       </c>
       <c r="U48" s="11" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="V48" s="1" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="W48" s="1" t="s">
         <v>322</v>
@@ -12859,7 +12859,7 @@
         <v>243</v>
       </c>
       <c r="D49" s="25" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="E49" s="1">
         <v>5</v>
@@ -12912,10 +12912,10 @@
         <v>100</v>
       </c>
       <c r="U49" s="11" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="V49" s="7" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="W49" s="1" t="s">
         <v>63</v>
@@ -12945,7 +12945,7 @@
         <v>244</v>
       </c>
       <c r="D50" s="25" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="E50" s="1">
         <v>5</v>
@@ -12998,10 +12998,10 @@
         <v>100</v>
       </c>
       <c r="U50" s="11" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="V50" s="7" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="W50" s="1" t="s">
         <v>65</v>
@@ -13033,7 +13033,7 @@
         <v>245</v>
       </c>
       <c r="D51" s="25" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="E51" s="1">
         <v>5</v>
@@ -13080,16 +13080,16 @@
         <v>0</v>
       </c>
       <c r="S51" s="1" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="T51">
         <v>100</v>
       </c>
       <c r="U51" s="11" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="V51" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="W51" s="1" t="s">
         <v>21</v>
@@ -13119,7 +13119,7 @@
         <v>246</v>
       </c>
       <c r="D52" s="25" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="E52" s="1">
         <v>3</v>
@@ -13172,10 +13172,10 @@
         <v>105</v>
       </c>
       <c r="U52" s="11" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="V52" s="7" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="W52" s="1" t="s">
         <v>68</v>
@@ -13207,7 +13207,7 @@
         <v>247</v>
       </c>
       <c r="D53" s="25" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="E53" s="1">
         <v>4</v>
@@ -13260,10 +13260,10 @@
         <v>95</v>
       </c>
       <c r="U53" s="11" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="V53" s="7" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="W53" s="1" t="s">
         <v>70</v>
@@ -13293,7 +13293,7 @@
         <v>248</v>
       </c>
       <c r="D54" s="25" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="E54" s="1">
         <v>3</v>
@@ -13346,10 +13346,10 @@
         <v>100</v>
       </c>
       <c r="U54" s="11" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="V54" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="W54" s="1" t="s">
         <v>72</v>
@@ -13375,13 +13375,13 @@
         <v>53000052</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="D55" s="25" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="E55" s="1">
         <v>2</v>
@@ -13428,22 +13428,22 @@
         <v>12</v>
       </c>
       <c r="S55" s="1" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="T55">
         <v>95</v>
       </c>
       <c r="U55" s="11" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="V55" s="7" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="W55" s="1" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="X55" s="1" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="Y55" s="1">
         <v>11000002</v>
@@ -13469,7 +13469,7 @@
         <v>249</v>
       </c>
       <c r="D56" s="25" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="E56" s="1">
         <v>3</v>
@@ -13516,16 +13516,16 @@
         <v>20</v>
       </c>
       <c r="S56" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="T56">
         <v>100</v>
       </c>
       <c r="U56" s="11" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="V56" s="7" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="W56" s="1" t="s">
         <v>74</v>
@@ -13555,7 +13555,7 @@
         <v>197</v>
       </c>
       <c r="D57" s="25" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="E57" s="1">
         <v>3</v>
@@ -13608,10 +13608,10 @@
         <v>100</v>
       </c>
       <c r="U57" s="11" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="V57" s="7" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="W57" s="1" t="s">
         <v>76</v>
@@ -13641,7 +13641,7 @@
         <v>250</v>
       </c>
       <c r="D58" s="25" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="E58" s="1">
         <v>4</v>
@@ -13694,7 +13694,7 @@
         <v>100</v>
       </c>
       <c r="U58" s="11" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="V58" s="1" t="s">
         <v>552</v>
@@ -13893,10 +13893,10 @@
         <v>53000058</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="D61" s="25" t="s">
         <v>417</v>
@@ -13946,16 +13946,16 @@
         <v>12</v>
       </c>
       <c r="S61" s="1" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="T61">
         <v>100</v>
       </c>
       <c r="U61" s="11" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="V61" s="7" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="W61" s="1" t="s">
         <v>15</v>
@@ -13985,7 +13985,7 @@
         <v>252</v>
       </c>
       <c r="D62" s="25" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="E62" s="1">
         <v>2</v>
@@ -14038,10 +14038,10 @@
         <v>100</v>
       </c>
       <c r="U62" s="11" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="V62" s="7" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="W62" s="1" t="s">
         <v>83</v>
@@ -14071,7 +14071,7 @@
         <v>253</v>
       </c>
       <c r="D63" s="25" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="E63" s="1">
         <v>1</v>
@@ -14124,7 +14124,7 @@
         <v>100</v>
       </c>
       <c r="U63" s="11" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="V63" s="1" t="s">
         <v>397</v>
@@ -14157,7 +14157,7 @@
         <v>254</v>
       </c>
       <c r="D64" s="25" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="E64" s="1">
         <v>4</v>
@@ -14243,7 +14243,7 @@
         <v>255</v>
       </c>
       <c r="D65" s="25" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="E65" s="1">
         <v>1</v>
@@ -14501,7 +14501,7 @@
         <v>199</v>
       </c>
       <c r="D68" s="25" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="E68" s="1">
         <v>6</v>
@@ -14554,7 +14554,7 @@
         <v>100</v>
       </c>
       <c r="U68" s="11" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="V68" s="1" t="s">
         <v>407</v>
@@ -14673,7 +14673,7 @@
         <v>259</v>
       </c>
       <c r="D70" s="25" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="E70" s="1">
         <v>3</v>
@@ -14726,10 +14726,10 @@
         <v>100</v>
       </c>
       <c r="U70" s="11" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="V70" s="7" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="W70" s="1" t="s">
         <v>95</v>
@@ -14759,7 +14759,7 @@
         <v>260</v>
       </c>
       <c r="D71" s="25" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="E71" s="1">
         <v>2</v>
@@ -14847,7 +14847,7 @@
         <v>202</v>
       </c>
       <c r="D72" s="25" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="E72" s="1">
         <v>2</v>
@@ -14900,13 +14900,13 @@
         <v>100</v>
       </c>
       <c r="U72" s="11" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="V72" s="7" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="W72" s="1" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="X72" s="1"/>
       <c r="Y72" s="1">
@@ -14933,7 +14933,7 @@
         <v>204</v>
       </c>
       <c r="D73" s="25" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="E73" s="1">
         <v>2</v>
@@ -15019,7 +15019,7 @@
         <v>201</v>
       </c>
       <c r="D74" s="25" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="E74" s="1">
         <v>4</v>
@@ -15107,7 +15107,7 @@
         <v>261</v>
       </c>
       <c r="D75" s="25" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="E75" s="1">
         <v>3</v>
@@ -15193,7 +15193,7 @@
         <v>262</v>
       </c>
       <c r="D76" s="25" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="E76" s="1">
         <v>3</v>
@@ -15279,7 +15279,7 @@
         <v>300</v>
       </c>
       <c r="D77" s="25" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="E77" s="1">
         <v>3</v>
@@ -15332,10 +15332,10 @@
         <v>103</v>
       </c>
       <c r="U77" s="11" t="s">
+        <v>601</v>
+      </c>
+      <c r="V77" s="7" t="s">
         <v>602</v>
-      </c>
-      <c r="V77" s="7" t="s">
-        <v>603</v>
       </c>
       <c r="W77" s="1" t="s">
         <v>109</v>
@@ -15365,7 +15365,7 @@
         <v>263</v>
       </c>
       <c r="D78" s="25" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="E78" s="1">
         <v>4</v>
@@ -15451,7 +15451,7 @@
         <v>264</v>
       </c>
       <c r="D79" s="25" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="E79" s="1">
         <v>3</v>
@@ -15539,7 +15539,7 @@
         <v>265</v>
       </c>
       <c r="D80" s="25" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="E80" s="1">
         <v>3</v>
@@ -15625,7 +15625,7 @@
         <v>266</v>
       </c>
       <c r="D81" s="25" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="E81" s="1">
         <v>1</v>
@@ -15678,10 +15678,10 @@
         <v>100</v>
       </c>
       <c r="U81" s="39" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="V81" s="7" t="s">
-        <v>630</v>
+        <v>802</v>
       </c>
       <c r="W81" s="1" t="s">
         <v>93</v>
@@ -15709,7 +15709,7 @@
         <v>267</v>
       </c>
       <c r="D82" s="25" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="E82" s="1">
         <v>3</v>
@@ -15797,7 +15797,7 @@
         <v>268</v>
       </c>
       <c r="D83" s="25" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="E83" s="1">
         <v>2</v>
@@ -15844,7 +15844,7 @@
         <v>30</v>
       </c>
       <c r="S83" s="7" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="T83">
         <v>100</v>
@@ -15853,7 +15853,7 @@
         <v>574</v>
       </c>
       <c r="V83" s="7" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="W83" s="1" t="s">
         <v>81</v>
@@ -15885,7 +15885,7 @@
         <v>269</v>
       </c>
       <c r="D84" s="25" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="E84" s="1">
         <v>2</v>
@@ -15932,16 +15932,16 @@
         <v>30</v>
       </c>
       <c r="S84" s="7" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="T84">
         <v>100</v>
       </c>
       <c r="U84" s="11" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="V84" s="7" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="W84" s="1" t="s">
         <v>51</v>
@@ -15973,7 +15973,7 @@
         <v>270</v>
       </c>
       <c r="D85" s="25" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="E85" s="1">
         <v>3</v>
@@ -16026,10 +16026,10 @@
         <v>100</v>
       </c>
       <c r="U85" s="11" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="V85" s="7" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="W85" s="1" t="s">
         <v>122</v>
@@ -16059,7 +16059,7 @@
         <v>289</v>
       </c>
       <c r="D86" s="25" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="E86" s="1">
         <v>3</v>
@@ -16112,7 +16112,7 @@
         <v>100</v>
       </c>
       <c r="U86" s="11" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="V86" s="7" t="s">
         <v>578</v>
@@ -16145,7 +16145,7 @@
         <v>203</v>
       </c>
       <c r="D87" s="25" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="E87" s="1">
         <v>4</v>
@@ -16192,16 +16192,16 @@
         <v>15</v>
       </c>
       <c r="S87" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="T87">
         <v>100</v>
       </c>
       <c r="U87" s="11" t="s">
+        <v>599</v>
+      </c>
+      <c r="V87" s="7" t="s">
         <v>600</v>
-      </c>
-      <c r="V87" s="7" t="s">
-        <v>601</v>
       </c>
       <c r="W87" s="1" t="s">
         <v>455</v>
@@ -16233,7 +16233,7 @@
         <v>205</v>
       </c>
       <c r="D88" s="25" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="E88" s="1">
         <v>3</v>
@@ -16286,7 +16286,7 @@
         <v>100</v>
       </c>
       <c r="U88" s="11" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="V88" s="7" t="s">
         <v>577</v>
@@ -16321,7 +16321,7 @@
         <v>206</v>
       </c>
       <c r="D89" s="25" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="E89" s="1">
         <v>2</v>
@@ -16407,7 +16407,7 @@
         <v>207</v>
       </c>
       <c r="D90" s="25" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="E90" s="1">
         <v>3</v>
@@ -16454,16 +16454,16 @@
         <v>40</v>
       </c>
       <c r="S90" s="7" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="T90">
         <v>100</v>
       </c>
       <c r="U90" s="11" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="V90" s="7" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="W90" s="1" t="s">
         <v>59</v>
@@ -16495,7 +16495,7 @@
         <v>271</v>
       </c>
       <c r="D91" s="25" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="E91" s="1">
         <v>3</v>
@@ -16548,7 +16548,7 @@
         <v>100</v>
       </c>
       <c r="U91" s="11" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="V91" s="7" t="s">
         <v>340</v>
@@ -16583,7 +16583,7 @@
         <v>272</v>
       </c>
       <c r="D92" s="25" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="E92" s="1">
         <v>4</v>
@@ -16636,10 +16636,10 @@
         <v>100</v>
       </c>
       <c r="U92" s="11" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="V92" s="7" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="W92" s="1" t="s">
         <v>474</v>
@@ -16757,7 +16757,7 @@
         <v>273</v>
       </c>
       <c r="D94" s="25" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="E94" s="1">
         <v>2</v>
@@ -16810,7 +16810,7 @@
         <v>100</v>
       </c>
       <c r="U94" s="11" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="V94" s="7" t="s">
         <v>341</v>
@@ -16837,13 +16837,13 @@
         <v>53000092</v>
       </c>
       <c r="B95" s="8" t="s">
+        <v>645</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="D95" s="25" t="s">
         <v>648</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>649</v>
-      </c>
-      <c r="D95" s="25" t="s">
-        <v>651</v>
       </c>
       <c r="E95" s="1">
         <v>3</v>
@@ -16890,19 +16890,19 @@
         <v>0</v>
       </c>
       <c r="S95" s="7" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="T95">
         <v>100</v>
       </c>
       <c r="U95" s="11" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="V95" s="1" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="W95" s="1" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="X95" s="1"/>
       <c r="Y95" s="1">
@@ -16929,7 +16929,7 @@
         <v>274</v>
       </c>
       <c r="D96" s="25" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="E96" s="1">
         <v>2</v>
@@ -16982,10 +16982,10 @@
         <v>100</v>
       </c>
       <c r="U96" s="11" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="V96" s="7" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="W96" s="1" t="s">
         <v>134</v>
@@ -17101,7 +17101,7 @@
         <v>276</v>
       </c>
       <c r="D98" s="25" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="E98" s="1">
         <v>2</v>
@@ -17154,10 +17154,10 @@
         <v>100</v>
       </c>
       <c r="U98" s="11" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="V98" s="7" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="W98" s="1" t="s">
         <v>139</v>
@@ -17189,7 +17189,7 @@
         <v>277</v>
       </c>
       <c r="D99" s="25" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="E99" s="1">
         <v>3</v>
@@ -17275,7 +17275,7 @@
         <v>278</v>
       </c>
       <c r="D100" s="25" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="E100" s="1">
         <v>2</v>
@@ -17328,10 +17328,10 @@
         <v>100</v>
       </c>
       <c r="U100" s="11" t="s">
+        <v>595</v>
+      </c>
+      <c r="V100" s="7" t="s">
         <v>596</v>
-      </c>
-      <c r="V100" s="7" t="s">
-        <v>597</v>
       </c>
       <c r="W100" s="1" t="s">
         <v>81</v>
@@ -17447,7 +17447,7 @@
         <v>279</v>
       </c>
       <c r="D102" s="25" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="E102" s="1">
         <v>1</v>
@@ -17500,10 +17500,10 @@
         <v>100</v>
       </c>
       <c r="U102" s="11" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="V102" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="W102" s="1" t="s">
         <v>97</v>
@@ -17533,7 +17533,7 @@
         <v>280</v>
       </c>
       <c r="D103" s="25" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="E103" s="1">
         <v>4</v>
@@ -17586,10 +17586,10 @@
         <v>100</v>
       </c>
       <c r="U103" s="11" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="V103" s="1" t="s">
-        <v>595</v>
+        <v>803</v>
       </c>
       <c r="W103" s="1" t="s">
         <v>144</v>
@@ -17619,7 +17619,7 @@
         <v>292</v>
       </c>
       <c r="D104" s="25" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="E104" s="1">
         <v>3</v>
@@ -17666,16 +17666,16 @@
         <v>0</v>
       </c>
       <c r="S104" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="T104">
         <v>100</v>
       </c>
       <c r="U104" s="11" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="V104" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="W104" s="1" t="s">
         <v>168</v>
@@ -17705,7 +17705,7 @@
         <v>281</v>
       </c>
       <c r="D105" s="25" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="E105" s="1">
         <v>3</v>
@@ -17758,7 +17758,7 @@
         <v>100</v>
       </c>
       <c r="U105" s="11" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="V105" s="7" t="s">
         <v>342</v>
@@ -17791,7 +17791,7 @@
         <v>282</v>
       </c>
       <c r="D106" s="25" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="E106" s="1">
         <v>3</v>
@@ -17844,10 +17844,10 @@
         <v>105</v>
       </c>
       <c r="U106" s="11" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="V106" s="7" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="W106" s="1" t="s">
         <v>147</v>
@@ -17879,7 +17879,7 @@
         <v>283</v>
       </c>
       <c r="D107" s="25" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="E107" s="1">
         <v>3</v>
@@ -17932,10 +17932,10 @@
         <v>105</v>
       </c>
       <c r="U107" s="11" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="V107" s="7" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="W107" s="1" t="s">
         <v>149</v>
@@ -18051,7 +18051,7 @@
         <v>284</v>
       </c>
       <c r="D109" s="25" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="E109" s="1">
         <v>1</v>
@@ -18104,10 +18104,10 @@
         <v>100</v>
       </c>
       <c r="U109" s="11" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="V109" s="7" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="W109" s="1" t="s">
         <v>153</v>
@@ -18137,7 +18137,7 @@
         <v>285</v>
       </c>
       <c r="D110" s="25" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="E110" s="1">
         <v>1</v>
@@ -18190,10 +18190,10 @@
         <v>100</v>
       </c>
       <c r="U110" s="11" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="V110" s="7" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="W110" s="1" t="s">
         <v>155</v>
@@ -18223,7 +18223,7 @@
         <v>286</v>
       </c>
       <c r="D111" s="25" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="E111" s="1">
         <v>2</v>
@@ -18276,7 +18276,7 @@
         <v>100</v>
       </c>
       <c r="U111" s="11" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="V111" s="7" t="s">
         <v>584</v>
@@ -18309,7 +18309,7 @@
         <v>287</v>
       </c>
       <c r="D112" s="25" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="E112" s="1">
         <v>2</v>
@@ -18448,10 +18448,10 @@
         <v>103</v>
       </c>
       <c r="U113" s="11" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="V113" s="7" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="W113" s="1" t="s">
         <v>29</v>
@@ -18475,13 +18475,13 @@
         <v>53000111</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="D114" s="25" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="E114" s="1">
         <v>3</v>
@@ -18528,22 +18528,22 @@
         <v>20</v>
       </c>
       <c r="S114" s="1" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="T114">
         <v>100</v>
       </c>
       <c r="U114" s="11" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="V114" s="7" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="W114" s="1" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="X114" s="1" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="Y114" s="1">
         <v>11000007</v>
@@ -18563,13 +18563,13 @@
         <v>53000112</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="D115" s="25" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="E115" s="1">
         <v>3</v>
@@ -18616,16 +18616,16 @@
         <v>100</v>
       </c>
       <c r="S115" s="1" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="T115">
         <v>100</v>
       </c>
       <c r="U115" s="11" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="V115" s="7" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="W115" s="1" t="s">
         <v>123</v>
@@ -18651,10 +18651,10 @@
         <v>53000113</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="D116" s="25"/>
       <c r="E116" s="1">
@@ -18702,22 +18702,22 @@
         <v>0</v>
       </c>
       <c r="S116" s="1" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="T116">
         <v>100</v>
       </c>
       <c r="U116" s="11" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="V116" s="7" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="W116" s="1" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="X116" s="1" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="Y116" s="1">
         <v>11000003</v>
@@ -18737,10 +18737,10 @@
         <v>53000114</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="D117" s="25"/>
       <c r="E117" s="1">
@@ -18788,16 +18788,16 @@
         <v>0</v>
       </c>
       <c r="S117" s="1" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="T117">
         <v>101</v>
       </c>
       <c r="U117" s="11" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="V117" s="7" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="W117" s="1" t="s">
         <v>99</v>
@@ -18823,10 +18823,10 @@
         <v>53000115</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="D118" s="25"/>
       <c r="E118" s="1">
@@ -18874,16 +18874,16 @@
         <v>0</v>
       </c>
       <c r="S118" s="1" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="T118">
         <v>100</v>
       </c>
       <c r="U118" s="11" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="V118" s="7" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="W118" s="1" t="s">
         <v>99</v>
@@ -18909,13 +18909,13 @@
         <v>53000116</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="D119" s="25" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="E119" s="1">
         <v>2</v>
@@ -18968,10 +18968,10 @@
         <v>101</v>
       </c>
       <c r="U119" s="11" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="V119" s="7" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="W119" s="1" t="s">
         <v>99</v>
@@ -18997,13 +18997,13 @@
         <v>53000117</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="D120" s="25" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="E120" s="1">
         <v>1</v>
@@ -19050,16 +19050,16 @@
         <v>0</v>
       </c>
       <c r="S120" s="1" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="T120">
         <v>100</v>
       </c>
       <c r="U120" s="11" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="V120" s="7" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="W120" s="1" t="s">
         <v>99</v>
@@ -19077,6 +19077,92 @@
         <v>0</v>
       </c>
       <c r="AB120" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:28" ht="72">
+      <c r="A121">
+        <v>53000118</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>798</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="D121" s="25"/>
+      <c r="E121" s="1">
+        <v>6</v>
+      </c>
+      <c r="F121">
+        <v>202</v>
+      </c>
+      <c r="G121" s="1">
+        <v>0</v>
+      </c>
+      <c r="H121" s="1">
+        <f t="shared" ref="H121" si="22">IF(AND(Q121&gt;=13,Q121&lt;=16),5,IF(AND(Q121&gt;=9,Q121&lt;=12),4,IF(AND(Q121&gt;=5,Q121&lt;=8),3,IF(AND(Q121&gt;=1,Q121&lt;=4),2,IF(AND(Q121&gt;=-3,Q121&lt;=0),1,IF(AND(Q121&gt;=-5,Q121&lt;=-4),0,6))))))</f>
+        <v>1</v>
+      </c>
+      <c r="I121" s="1">
+        <v>6</v>
+      </c>
+      <c r="J121" s="1">
+        <v>0</v>
+      </c>
+      <c r="K121" s="1">
+        <v>0</v>
+      </c>
+      <c r="L121" s="1">
+        <v>0</v>
+      </c>
+      <c r="M121" s="1">
+        <v>0</v>
+      </c>
+      <c r="N121" s="1">
+        <v>25</v>
+      </c>
+      <c r="O121" s="1">
+        <v>0</v>
+      </c>
+      <c r="P121" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q121" s="38">
+        <f t="shared" ref="Q121" si="23">T121-100+P121</f>
+        <v>0</v>
+      </c>
+      <c r="R121" s="1">
+        <v>0</v>
+      </c>
+      <c r="S121" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="T121">
+        <v>100</v>
+      </c>
+      <c r="U121" s="11" t="s">
+        <v>800</v>
+      </c>
+      <c r="V121" s="7" t="s">
+        <v>804</v>
+      </c>
+      <c r="W121" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="X121" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="Y121" s="1">
+        <v>11000003</v>
+      </c>
+      <c r="Z121" s="1">
+        <v>118</v>
+      </c>
+      <c r="AA121" s="27">
+        <v>0</v>
+      </c>
+      <c r="AB121" s="25">
         <v>1</v>
       </c>
     </row>
@@ -19085,91 +19171,91 @@
     <sortCondition ref="E1"/>
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="I38:I68 I17:I35 I4:I15 I70:I120">
-    <cfRule type="cellIs" dxfId="58" priority="56" operator="notEqual">
+  <conditionalFormatting sqref="I38:I68 I17:I35 I4:I15 I70:I121">
+    <cfRule type="cellIs" dxfId="55" priority="56" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J17:N35 J4:N15 J38:N68 P70:Q120 P38:Q68 P5:Q15 P17:Q35 P4 J70:N120">
-    <cfRule type="cellIs" dxfId="57" priority="55" operator="equal">
+  <conditionalFormatting sqref="J17:N35 J4:N15 J38:N68 P38:Q68 P5:Q15 P17:Q35 P4 P70:Q121 J70:N121">
+    <cfRule type="cellIs" dxfId="54" priority="55" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I69">
-    <cfRule type="cellIs" dxfId="56" priority="20" operator="notEqual">
+    <cfRule type="cellIs" dxfId="53" priority="20" operator="notEqual">
       <formula>$E69</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J69:N69 P69:Q69">
-    <cfRule type="cellIs" dxfId="55" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="19" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36">
-    <cfRule type="cellIs" dxfId="54" priority="18" operator="notEqual">
+    <cfRule type="cellIs" dxfId="51" priority="18" operator="notEqual">
       <formula>$E36</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J36:N36 P36:Q36">
-    <cfRule type="cellIs" dxfId="53" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="17" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37">
-    <cfRule type="cellIs" dxfId="52" priority="16" operator="notEqual">
+    <cfRule type="cellIs" dxfId="49" priority="16" operator="notEqual">
       <formula>$E37</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J37:N37 P37:Q37">
-    <cfRule type="cellIs" dxfId="51" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="15" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:H15 H17:H120">
-    <cfRule type="cellIs" dxfId="50" priority="11" operator="equal">
+  <conditionalFormatting sqref="H4:H15 H17:H121">
+    <cfRule type="cellIs" dxfId="47" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="12" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="13" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="14" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="44" priority="14" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="cellIs" dxfId="46" priority="8" operator="notEqual">
+    <cfRule type="cellIs" dxfId="43" priority="8" operator="notEqual">
       <formula>$E16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:N16 P16:Q16">
-    <cfRule type="cellIs" dxfId="45" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="cellIs" dxfId="44" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="5" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="38" priority="6" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="40" priority="2" operator="containsText" text="未完成">
+    <cfRule type="containsText" dxfId="37" priority="2" operator="containsText" text="未完成">
       <formula>NOT(ISERROR(SEARCH("未完成",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O4:O120">
-    <cfRule type="cellIs" dxfId="39" priority="1" operator="equal">
+  <conditionalFormatting sqref="O4:O121">
+    <cfRule type="cellIs" dxfId="36" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19257,7 +19343,7 @@
         <v>349</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="P1" s="17" t="s">
         <v>331</v>
@@ -19343,7 +19429,7 @@
         <v>348</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>318</v>
@@ -19429,7 +19515,7 @@
         <v>351</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="P3" s="20" t="s">
         <v>333</v>
@@ -19531,7 +19617,7 @@
         <v>-1</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="V4" s="7" t="s">
         <v>342</v>
@@ -19691,7 +19777,7 @@
         <v>-1</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="V6" s="7" t="s">
         <v>377</v>
@@ -19851,7 +19937,7 @@
         <v>-1</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="V8" s="7" t="s">
         <v>379</v>
@@ -20036,7 +20122,7 @@
         <v>53100007</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="34"/>
@@ -20085,16 +20171,16 @@
         <v>0</v>
       </c>
       <c r="S11" s="15" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="T11" s="1">
         <v>-1</v>
       </c>
       <c r="U11" s="11" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="V11" s="7" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="W11" s="15" t="s">
         <v>2</v>
@@ -20114,110 +20200,110 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="J4:Q11">
-    <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="40" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:Q8">
-    <cfRule type="cellIs" dxfId="37" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="36" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:Q4 O4:O11">
-    <cfRule type="cellIs" dxfId="36" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="35" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="35" priority="34" operator="notEqual">
+    <cfRule type="cellIs" dxfId="32" priority="34" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:Q4 O4:O11">
-    <cfRule type="cellIs" dxfId="34" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="33" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="33" priority="32" operator="notEqual">
+    <cfRule type="cellIs" dxfId="30" priority="32" operator="notEqual">
       <formula>$E5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:Q5">
-    <cfRule type="cellIs" dxfId="32" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" dxfId="31" priority="30" operator="notEqual">
+    <cfRule type="cellIs" dxfId="28" priority="30" operator="notEqual">
       <formula>$E6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:Q6">
-    <cfRule type="cellIs" dxfId="30" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="29" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="29" priority="28" operator="notEqual">
+    <cfRule type="cellIs" dxfId="26" priority="28" operator="notEqual">
       <formula>$E7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:Q7">
-    <cfRule type="cellIs" dxfId="28" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="27" priority="26" operator="notEqual">
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="notEqual">
       <formula>$E8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:Q8">
-    <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I11">
-    <cfRule type="cellIs" dxfId="25" priority="24" operator="notEqual">
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="notEqual">
       <formula>$E9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:Q11">
-    <cfRule type="cellIs" dxfId="24" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H11">
-    <cfRule type="cellIs" dxfId="23" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="17" priority="9" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10:L11">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20306,7 +20392,7 @@
         <v>349</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="P1" s="17" t="s">
         <v>331</v>
@@ -20392,7 +20478,7 @@
         <v>348</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>318</v>
@@ -20478,7 +20564,7 @@
         <v>351</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="P3" s="20" t="s">
         <v>333</v>
@@ -20584,7 +20670,7 @@
         <v>115</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="V4" s="7" t="s">
         <v>376</v>
@@ -20668,7 +20754,7 @@
         <v>90</v>
       </c>
       <c r="U5" s="11" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="V5" s="7" t="s">
         <v>380</v>
@@ -20918,7 +21004,7 @@
         <v>90</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="V8" s="7" t="s">
         <v>390</v>
@@ -21027,50 +21113,50 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I4:I9">
-    <cfRule type="cellIs" dxfId="14" priority="12" operator="notEqual">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:Q7 O4:O9">
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:Q9">
-    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:Q8">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H9">
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
remove the id in activecard
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -2672,10 +2672,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>t.AddMaxHp(t.MaxHp*s.Help/100);t.AddHp(s.Cure);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>使敌方单体随机获得晕眩，诅咒，致盲中一种状态{2:0.0}回合，使用后返回手牌</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -2908,10 +2904,6 @@
   </si>
   <si>
     <t>降低1.5卡片范围内所有单位{3:0}%生命上限</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse))im.AddMaxHp(-im.MaxHp*s.Help/100);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -3542,6 +3534,14 @@
   </si>
   <si>
     <t>NFO</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>t.AddMaxHp(t.MaxHp.Source*s.Help/100);t.AddHp(s.Cure);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse))im.AddMaxHp(-im.MaxHp.Source*s.Help/100);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -4547,536 +4547,6 @@
   <dxfs count="148">
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -5600,6 +5070,33 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -5832,6 +5329,99 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -6362,6 +5952,33 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -6602,6 +6219,204 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -7132,6 +6947,33 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -7373,6 +7215,164 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -7555,11 +7555,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="214538848"/>
-        <c:axId val="214539408"/>
+        <c:axId val="268612720"/>
+        <c:axId val="268613280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="214538848"/>
+        <c:axId val="268612720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7602,7 +7602,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="214539408"/>
+        <c:crossAx val="268613280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7610,7 +7610,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="214539408"/>
+        <c:axId val="268613280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7661,7 +7661,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="214538848"/>
+        <c:crossAx val="268612720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8289,132 +8289,132 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AB121" totalsRowShown="0" headerRowDxfId="147" dataDxfId="146" tableBorderDxfId="145">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AB121" totalsRowShown="0" headerRowDxfId="127" dataDxfId="126" tableBorderDxfId="125">
   <autoFilter ref="A3:AB121"/>
   <sortState ref="A4:AB113">
     <sortCondition ref="A3:A113"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="144"/>
-    <tableColumn id="2" name="Name" dataDxfId="143"/>
-    <tableColumn id="20" name="Ename" dataDxfId="142"/>
-    <tableColumn id="21" name="Remark" dataDxfId="141"/>
-    <tableColumn id="3" name="Star" dataDxfId="140"/>
-    <tableColumn id="4" name="Type" dataDxfId="139"/>
-    <tableColumn id="5" name="Attr" dataDxfId="138"/>
-    <tableColumn id="8" name="Quality" dataDxfId="137">
+    <tableColumn id="1" name="Id" dataDxfId="124"/>
+    <tableColumn id="2" name="Name" dataDxfId="123"/>
+    <tableColumn id="20" name="Ename" dataDxfId="122"/>
+    <tableColumn id="21" name="Remark" dataDxfId="121"/>
+    <tableColumn id="3" name="Star" dataDxfId="120"/>
+    <tableColumn id="4" name="Type" dataDxfId="119"/>
+    <tableColumn id="5" name="Attr" dataDxfId="118"/>
+    <tableColumn id="8" name="Quality" dataDxfId="117">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="136"/>
-    <tableColumn id="9" name="Damage" dataDxfId="135"/>
-    <tableColumn id="10" name="Cure" dataDxfId="134"/>
-    <tableColumn id="11" name="Time" dataDxfId="133"/>
-    <tableColumn id="13" name="Help" dataDxfId="132"/>
-    <tableColumn id="16" name="Rate" dataDxfId="131"/>
-    <tableColumn id="18" name="Atk" dataDxfId="58"/>
-    <tableColumn id="12" name="Modify" dataDxfId="130"/>
-    <tableColumn id="27" name="Sum" dataDxfId="129">
+    <tableColumn id="7" name="Cost" dataDxfId="116"/>
+    <tableColumn id="9" name="Damage" dataDxfId="115"/>
+    <tableColumn id="10" name="Cure" dataDxfId="114"/>
+    <tableColumn id="11" name="Time" dataDxfId="113"/>
+    <tableColumn id="13" name="Help" dataDxfId="112"/>
+    <tableColumn id="16" name="Rate" dataDxfId="111"/>
+    <tableColumn id="18" name="Atk" dataDxfId="110"/>
+    <tableColumn id="12" name="Modify" dataDxfId="109"/>
+    <tableColumn id="27" name="Sum" dataDxfId="108">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="128"/>
-    <tableColumn id="15" name="Target" dataDxfId="127"/>
-    <tableColumn id="25" name="Mark" dataDxfId="126"/>
-    <tableColumn id="22" name="Effect" dataDxfId="125"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="124"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="123"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="122"/>
-    <tableColumn id="26" name="JobId" dataDxfId="121"/>
-    <tableColumn id="19" name="Icon" dataDxfId="120"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="119"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="118"/>
+    <tableColumn id="6" name="Range" dataDxfId="107"/>
+    <tableColumn id="15" name="Target" dataDxfId="106"/>
+    <tableColumn id="25" name="Mark" dataDxfId="105"/>
+    <tableColumn id="22" name="Effect" dataDxfId="104"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="103"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="102"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="101"/>
+    <tableColumn id="26" name="JobId" dataDxfId="100"/>
+    <tableColumn id="19" name="Icon" dataDxfId="99"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="98"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="97"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AB11" totalsRowShown="0" headerRowDxfId="117" dataDxfId="116" tableBorderDxfId="115">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AB11" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71" tableBorderDxfId="70">
   <autoFilter ref="A3:AB11"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="114"/>
-    <tableColumn id="2" name="Name" dataDxfId="113"/>
-    <tableColumn id="20" name="Ename" dataDxfId="112"/>
-    <tableColumn id="21" name="Remark" dataDxfId="111"/>
-    <tableColumn id="3" name="Star" dataDxfId="110"/>
-    <tableColumn id="4" name="Type" dataDxfId="109"/>
-    <tableColumn id="5" name="Attr" dataDxfId="108"/>
-    <tableColumn id="8" name="Quality" dataDxfId="107">
+    <tableColumn id="1" name="Id" dataDxfId="69"/>
+    <tableColumn id="2" name="Name" dataDxfId="68"/>
+    <tableColumn id="20" name="Ename" dataDxfId="67"/>
+    <tableColumn id="21" name="Remark" dataDxfId="66"/>
+    <tableColumn id="3" name="Star" dataDxfId="65"/>
+    <tableColumn id="4" name="Type" dataDxfId="64"/>
+    <tableColumn id="5" name="Attr" dataDxfId="63"/>
+    <tableColumn id="8" name="Quality" dataDxfId="62">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="106"/>
-    <tableColumn id="9" name="Damage" dataDxfId="105"/>
-    <tableColumn id="10" name="Cure" dataDxfId="104"/>
-    <tableColumn id="11" name="Time" dataDxfId="103"/>
-    <tableColumn id="13" name="Help" dataDxfId="102"/>
-    <tableColumn id="16" name="Rate" dataDxfId="101"/>
-    <tableColumn id="18" name="Atk" dataDxfId="57"/>
-    <tableColumn id="12" name="Modify" dataDxfId="100"/>
-    <tableColumn id="27" name="Sum" dataDxfId="99">
+    <tableColumn id="7" name="Cost" dataDxfId="61"/>
+    <tableColumn id="9" name="Damage" dataDxfId="60"/>
+    <tableColumn id="10" name="Cure" dataDxfId="59"/>
+    <tableColumn id="11" name="Time" dataDxfId="58"/>
+    <tableColumn id="13" name="Help" dataDxfId="57"/>
+    <tableColumn id="16" name="Rate" dataDxfId="56"/>
+    <tableColumn id="18" name="Atk" dataDxfId="55"/>
+    <tableColumn id="12" name="Modify" dataDxfId="54"/>
+    <tableColumn id="27" name="Sum" dataDxfId="53">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="98"/>
-    <tableColumn id="15" name="Target" dataDxfId="97"/>
-    <tableColumn id="25" name="Mark" dataDxfId="96"/>
-    <tableColumn id="22" name="Effect" dataDxfId="95"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="94"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="93"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="92"/>
-    <tableColumn id="26" name="JobId" dataDxfId="91"/>
-    <tableColumn id="19" name="Icon" dataDxfId="90"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="89"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="88"/>
+    <tableColumn id="6" name="Range" dataDxfId="52"/>
+    <tableColumn id="15" name="Target" dataDxfId="51"/>
+    <tableColumn id="25" name="Mark" dataDxfId="50"/>
+    <tableColumn id="22" name="Effect" dataDxfId="49"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="48"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="47"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="46"/>
+    <tableColumn id="26" name="JobId" dataDxfId="45"/>
+    <tableColumn id="19" name="Icon" dataDxfId="44"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="43"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_35" displayName="表1_35" ref="A3:AB9" totalsRowShown="0" headerRowDxfId="87" tableBorderDxfId="86">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_35" displayName="表1_35" ref="A3:AB9" totalsRowShown="0" headerRowDxfId="29" tableBorderDxfId="28">
   <autoFilter ref="A3:AB9"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="85"/>
-    <tableColumn id="2" name="Name" dataDxfId="84"/>
-    <tableColumn id="20" name="Ename" dataDxfId="83"/>
-    <tableColumn id="21" name="Remark" dataDxfId="82"/>
-    <tableColumn id="3" name="Star" dataDxfId="81"/>
-    <tableColumn id="4" name="Type" dataDxfId="80"/>
-    <tableColumn id="5" name="Attr" dataDxfId="79"/>
-    <tableColumn id="8" name="Quality" dataDxfId="78">
+    <tableColumn id="1" name="Id" dataDxfId="27"/>
+    <tableColumn id="2" name="Name" dataDxfId="26"/>
+    <tableColumn id="20" name="Ename" dataDxfId="25"/>
+    <tableColumn id="21" name="Remark" dataDxfId="24"/>
+    <tableColumn id="3" name="Star" dataDxfId="23"/>
+    <tableColumn id="4" name="Type" dataDxfId="22"/>
+    <tableColumn id="5" name="Attr" dataDxfId="21"/>
+    <tableColumn id="8" name="Quality" dataDxfId="20">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="77"/>
-    <tableColumn id="9" name="Damage" dataDxfId="76"/>
-    <tableColumn id="10" name="Cure" dataDxfId="75"/>
-    <tableColumn id="11" name="Time" dataDxfId="74"/>
-    <tableColumn id="13" name="Help" dataDxfId="73"/>
-    <tableColumn id="16" name="Rate" dataDxfId="72"/>
-    <tableColumn id="18" name="Atk" dataDxfId="56"/>
-    <tableColumn id="12" name="Modify" dataDxfId="71"/>
-    <tableColumn id="27" name="Sum" dataDxfId="70">
+    <tableColumn id="7" name="Cost" dataDxfId="19"/>
+    <tableColumn id="9" name="Damage" dataDxfId="18"/>
+    <tableColumn id="10" name="Cure" dataDxfId="17"/>
+    <tableColumn id="11" name="Time" dataDxfId="16"/>
+    <tableColumn id="13" name="Help" dataDxfId="15"/>
+    <tableColumn id="16" name="Rate" dataDxfId="14"/>
+    <tableColumn id="18" name="Atk" dataDxfId="13"/>
+    <tableColumn id="12" name="Modify" dataDxfId="12"/>
+    <tableColumn id="27" name="Sum" dataDxfId="11">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="69"/>
-    <tableColumn id="15" name="Target" dataDxfId="68"/>
-    <tableColumn id="25" name="Mark" dataDxfId="67"/>
-    <tableColumn id="22" name="Effect" dataDxfId="66"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="65"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="64"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="63"/>
-    <tableColumn id="26" name="JobId" dataDxfId="62"/>
-    <tableColumn id="19" name="Icon" dataDxfId="61"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="60"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="59"/>
+    <tableColumn id="6" name="Range" dataDxfId="10"/>
+    <tableColumn id="15" name="Target" dataDxfId="9"/>
+    <tableColumn id="25" name="Mark" dataDxfId="8"/>
+    <tableColumn id="22" name="Effect" dataDxfId="7"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="6"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="5"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="4"/>
+    <tableColumn id="26" name="JobId" dataDxfId="3"/>
+    <tableColumn id="19" name="Icon" dataDxfId="2"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="1"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8710,10 +8710,10 @@
   <dimension ref="A1:AB121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C117" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="S121" sqref="S121"/>
+      <selection pane="bottomRight" activeCell="U38" sqref="U38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8782,7 +8782,7 @@
         <v>349</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="P1" s="17" t="s">
         <v>331</v>
@@ -8868,7 +8868,7 @@
         <v>350</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>332</v>
@@ -8886,7 +8886,7 @@
         <v>502</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="V2" s="10" t="s">
         <v>179</v>
@@ -8954,7 +8954,7 @@
         <v>351</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="P3" s="20" t="s">
         <v>333</v>
@@ -8975,7 +8975,7 @@
         <v>475</v>
       </c>
       <c r="V3" s="6" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="W3" s="6" t="s">
         <v>482</v>
@@ -9007,7 +9007,7 @@
         <v>211</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
@@ -9060,10 +9060,10 @@
         <v>95</v>
       </c>
       <c r="U4" s="11" t="s">
+        <v>797</v>
+      </c>
+      <c r="V4" s="7" t="s">
         <v>799</v>
-      </c>
-      <c r="V4" s="7" t="s">
-        <v>801</v>
       </c>
       <c r="W4" s="1" t="s">
         <v>2</v>
@@ -9091,7 +9091,7 @@
         <v>212</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -9175,7 +9175,7 @@
         <v>213</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="E6" s="1">
         <v>2</v>
@@ -9228,7 +9228,7 @@
         <v>100</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="V6" s="7" t="s">
         <v>380</v>
@@ -9259,7 +9259,7 @@
         <v>214</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
@@ -9312,7 +9312,7 @@
         <v>100</v>
       </c>
       <c r="U7" s="11" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="V7" s="7" t="s">
         <v>381</v>
@@ -9345,7 +9345,7 @@
         <v>215</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="E8" s="1">
         <v>3</v>
@@ -9431,7 +9431,7 @@
         <v>294</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
@@ -9515,7 +9515,7 @@
         <v>295</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -9599,7 +9599,7 @@
         <v>296</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -9683,7 +9683,7 @@
         <v>297</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
@@ -9767,7 +9767,7 @@
         <v>216</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
@@ -9851,7 +9851,7 @@
         <v>210</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
@@ -9935,7 +9935,7 @@
         <v>217</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
@@ -10019,7 +10019,7 @@
         <v>372</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="E16" s="15">
         <v>4</v>
@@ -10072,7 +10072,7 @@
         <v>100</v>
       </c>
       <c r="U16" s="11" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="V16" s="7" t="s">
         <v>518</v>
@@ -10105,7 +10105,7 @@
         <v>480</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E17" s="1">
         <v>2</v>
@@ -10191,7 +10191,7 @@
         <v>218</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="E18" s="1">
         <v>1</v>
@@ -10244,10 +10244,10 @@
         <v>75</v>
       </c>
       <c r="U18" s="11" t="s">
+        <v>791</v>
+      </c>
+      <c r="V18" s="7" t="s">
         <v>793</v>
-      </c>
-      <c r="V18" s="7" t="s">
-        <v>795</v>
       </c>
       <c r="W18" s="1" t="s">
         <v>15</v>
@@ -10277,7 +10277,7 @@
         <v>219</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="E19" s="1">
         <v>3</v>
@@ -10363,7 +10363,7 @@
         <v>220</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="E20" s="1">
         <v>7</v>
@@ -10416,13 +10416,13 @@
         <v>100</v>
       </c>
       <c r="U20" s="11" t="s">
+        <v>792</v>
+      </c>
+      <c r="V20" s="7" t="s">
         <v>794</v>
       </c>
-      <c r="V20" s="7" t="s">
-        <v>796</v>
-      </c>
       <c r="W20" s="1" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="X20" s="1"/>
       <c r="Y20" s="1">
@@ -10449,7 +10449,7 @@
         <v>221</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="E21" s="1">
         <v>3</v>
@@ -10502,10 +10502,10 @@
         <v>102</v>
       </c>
       <c r="U21" s="11" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="V21" s="7" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="W21" s="1" t="s">
         <v>21</v>
@@ -10535,7 +10535,7 @@
         <v>222</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E22" s="1">
         <v>4</v>
@@ -10582,13 +10582,13 @@
         <v>40</v>
       </c>
       <c r="S22" s="7" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="T22">
         <v>100</v>
       </c>
       <c r="U22" s="11" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="V22" s="7" t="s">
         <v>536</v>
@@ -10623,7 +10623,7 @@
         <v>223</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E23" s="1">
         <v>3</v>
@@ -10670,7 +10670,7 @@
         <v>60</v>
       </c>
       <c r="S23" s="7" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="T23">
         <v>100</v>
@@ -10711,7 +10711,7 @@
         <v>224</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E24" s="1">
         <v>3</v>
@@ -10758,7 +10758,7 @@
         <v>90</v>
       </c>
       <c r="S24" s="7" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="T24">
         <v>100</v>
@@ -11022,7 +11022,7 @@
         <v>90</v>
       </c>
       <c r="U27" s="11" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="V27" s="7" t="s">
         <v>395</v>
@@ -11055,7 +11055,7 @@
         <v>228</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="E28" s="1">
         <v>3</v>
@@ -11108,7 +11108,7 @@
         <v>100</v>
       </c>
       <c r="U28" s="11" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="V28" s="7" t="s">
         <v>522</v>
@@ -11141,7 +11141,7 @@
         <v>229</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="E29" s="1">
         <v>4</v>
@@ -11194,7 +11194,7 @@
         <v>100</v>
       </c>
       <c r="U29" s="11" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="V29" s="7" t="s">
         <v>519</v>
@@ -11227,7 +11227,7 @@
         <v>230</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="E30" s="1">
         <v>1</v>
@@ -11311,7 +11311,7 @@
         <v>231</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
@@ -11395,7 +11395,7 @@
         <v>232</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="E32" s="1">
         <v>4</v>
@@ -11448,7 +11448,7 @@
         <v>100</v>
       </c>
       <c r="U32" s="11" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="V32" s="21" t="s">
         <v>343</v>
@@ -11651,7 +11651,7 @@
         <v>298</v>
       </c>
       <c r="D35" s="25" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E35" s="1">
         <v>3</v>
@@ -11704,7 +11704,7 @@
         <v>100</v>
       </c>
       <c r="U35" s="11" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="V35" s="7" t="s">
         <v>420</v>
@@ -11739,7 +11739,7 @@
         <v>299</v>
       </c>
       <c r="D36" s="25" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="E36" s="1">
         <v>4</v>
@@ -11880,7 +11880,7 @@
         <v>100</v>
       </c>
       <c r="U37" s="11" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="V37" s="7" t="s">
         <v>357</v>
@@ -11902,7 +11902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:28" ht="72">
+    <row r="38" spans="1:28" ht="84">
       <c r="A38">
         <v>53000035</v>
       </c>
@@ -11913,7 +11913,7 @@
         <v>233</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E38" s="1">
         <v>3</v>
@@ -11960,16 +11960,16 @@
         <v>15</v>
       </c>
       <c r="S38" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="T38">
         <v>100</v>
       </c>
       <c r="U38" s="11" t="s">
-        <v>643</v>
+        <v>806</v>
       </c>
       <c r="V38" s="7" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="W38" s="1" t="s">
         <v>49</v>
@@ -12001,7 +12001,7 @@
         <v>234</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="E39" s="1">
         <v>3</v>
@@ -12048,16 +12048,16 @@
         <v>12</v>
       </c>
       <c r="S39" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="T39">
         <v>100</v>
       </c>
       <c r="U39" s="11" t="s">
+        <v>636</v>
+      </c>
+      <c r="V39" s="1" t="s">
         <v>637</v>
-      </c>
-      <c r="V39" s="1" t="s">
-        <v>638</v>
       </c>
       <c r="W39" s="1" t="s">
         <v>51</v>
@@ -12087,7 +12087,7 @@
         <v>235</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="E40" s="1">
         <v>1</v>
@@ -12171,7 +12171,7 @@
         <v>236</v>
       </c>
       <c r="D41" s="25" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="E41" s="1">
         <v>2</v>
@@ -12224,7 +12224,7 @@
         <v>100</v>
       </c>
       <c r="U41" s="11" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="V41" s="7" t="s">
         <v>524</v>
@@ -12482,7 +12482,7 @@
         <v>100</v>
       </c>
       <c r="U44" s="11" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="V44" s="7" t="s">
         <v>580</v>
@@ -12513,7 +12513,7 @@
         <v>239</v>
       </c>
       <c r="D45" s="25" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E45" s="1">
         <v>3</v>
@@ -12566,10 +12566,10 @@
         <v>110</v>
       </c>
       <c r="U45" s="11" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="V45" s="7" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="W45" s="1" t="s">
         <v>59</v>
@@ -12820,16 +12820,16 @@
         <v>30</v>
       </c>
       <c r="S48" s="7" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="T48">
         <v>100</v>
       </c>
       <c r="U48" s="11" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="V48" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="W48" s="1" t="s">
         <v>322</v>
@@ -12859,7 +12859,7 @@
         <v>243</v>
       </c>
       <c r="D49" s="25" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E49" s="1">
         <v>5</v>
@@ -12912,10 +12912,10 @@
         <v>100</v>
       </c>
       <c r="U49" s="11" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="V49" s="7" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="W49" s="1" t="s">
         <v>63</v>
@@ -12945,7 +12945,7 @@
         <v>244</v>
       </c>
       <c r="D50" s="25" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E50" s="1">
         <v>5</v>
@@ -12998,10 +12998,10 @@
         <v>100</v>
       </c>
       <c r="U50" s="11" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="V50" s="7" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="W50" s="1" t="s">
         <v>65</v>
@@ -13033,7 +13033,7 @@
         <v>245</v>
       </c>
       <c r="D51" s="25" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="E51" s="1">
         <v>5</v>
@@ -13080,16 +13080,16 @@
         <v>0</v>
       </c>
       <c r="S51" s="1" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="T51">
         <v>100</v>
       </c>
       <c r="U51" s="11" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="V51" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="W51" s="1" t="s">
         <v>21</v>
@@ -13119,7 +13119,7 @@
         <v>246</v>
       </c>
       <c r="D52" s="25" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E52" s="1">
         <v>3</v>
@@ -13172,10 +13172,10 @@
         <v>105</v>
       </c>
       <c r="U52" s="11" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="V52" s="7" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="W52" s="1" t="s">
         <v>68</v>
@@ -13207,7 +13207,7 @@
         <v>247</v>
       </c>
       <c r="D53" s="25" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E53" s="1">
         <v>4</v>
@@ -13260,10 +13260,10 @@
         <v>95</v>
       </c>
       <c r="U53" s="11" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="V53" s="7" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="W53" s="1" t="s">
         <v>70</v>
@@ -13293,7 +13293,7 @@
         <v>248</v>
       </c>
       <c r="D54" s="25" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="E54" s="1">
         <v>3</v>
@@ -13346,10 +13346,10 @@
         <v>100</v>
       </c>
       <c r="U54" s="11" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="V54" s="1" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="W54" s="1" t="s">
         <v>72</v>
@@ -13375,13 +13375,13 @@
         <v>53000052</v>
       </c>
       <c r="B55" s="8" t="s">
+        <v>630</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>631</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>632</v>
-      </c>
       <c r="D55" s="25" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E55" s="1">
         <v>2</v>
@@ -13428,22 +13428,22 @@
         <v>12</v>
       </c>
       <c r="S55" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="T55">
         <v>95</v>
       </c>
       <c r="U55" s="11" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="V55" s="7" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="W55" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="X55" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="Y55" s="1">
         <v>11000002</v>
@@ -13469,7 +13469,7 @@
         <v>249</v>
       </c>
       <c r="D56" s="25" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E56" s="1">
         <v>3</v>
@@ -13516,16 +13516,16 @@
         <v>20</v>
       </c>
       <c r="S56" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="T56">
         <v>100</v>
       </c>
       <c r="U56" s="11" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="V56" s="7" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="W56" s="1" t="s">
         <v>74</v>
@@ -13555,7 +13555,7 @@
         <v>197</v>
       </c>
       <c r="D57" s="25" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="E57" s="1">
         <v>3</v>
@@ -13608,10 +13608,10 @@
         <v>100</v>
       </c>
       <c r="U57" s="11" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="V57" s="7" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="W57" s="1" t="s">
         <v>76</v>
@@ -13641,7 +13641,7 @@
         <v>250</v>
       </c>
       <c r="D58" s="25" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="E58" s="1">
         <v>4</v>
@@ -13694,7 +13694,7 @@
         <v>100</v>
       </c>
       <c r="U58" s="11" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="V58" s="1" t="s">
         <v>552</v>
@@ -13893,10 +13893,10 @@
         <v>53000058</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D61" s="25" t="s">
         <v>417</v>
@@ -13946,16 +13946,16 @@
         <v>12</v>
       </c>
       <c r="S61" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="T61">
         <v>100</v>
       </c>
       <c r="U61" s="11" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="V61" s="7" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="W61" s="1" t="s">
         <v>15</v>
@@ -13985,7 +13985,7 @@
         <v>252</v>
       </c>
       <c r="D62" s="25" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="E62" s="1">
         <v>2</v>
@@ -14038,10 +14038,10 @@
         <v>100</v>
       </c>
       <c r="U62" s="11" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="V62" s="7" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="W62" s="1" t="s">
         <v>83</v>
@@ -14071,7 +14071,7 @@
         <v>253</v>
       </c>
       <c r="D63" s="25" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="E63" s="1">
         <v>1</v>
@@ -14124,7 +14124,7 @@
         <v>100</v>
       </c>
       <c r="U63" s="11" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="V63" s="1" t="s">
         <v>397</v>
@@ -14157,7 +14157,7 @@
         <v>254</v>
       </c>
       <c r="D64" s="25" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="E64" s="1">
         <v>4</v>
@@ -14210,7 +14210,7 @@
         <v>100</v>
       </c>
       <c r="U64" s="11" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="V64" s="7" t="s">
         <v>354</v>
@@ -14243,7 +14243,7 @@
         <v>255</v>
       </c>
       <c r="D65" s="25" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="E65" s="1">
         <v>1</v>
@@ -14501,7 +14501,7 @@
         <v>199</v>
       </c>
       <c r="D68" s="25" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E68" s="1">
         <v>6</v>
@@ -14554,7 +14554,7 @@
         <v>100</v>
       </c>
       <c r="U68" s="11" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="V68" s="1" t="s">
         <v>407</v>
@@ -14673,7 +14673,7 @@
         <v>259</v>
       </c>
       <c r="D70" s="25" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="E70" s="1">
         <v>3</v>
@@ -14726,10 +14726,10 @@
         <v>100</v>
       </c>
       <c r="U70" s="11" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="V70" s="7" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="W70" s="1" t="s">
         <v>95</v>
@@ -14759,7 +14759,7 @@
         <v>260</v>
       </c>
       <c r="D71" s="25" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="E71" s="1">
         <v>2</v>
@@ -14847,7 +14847,7 @@
         <v>202</v>
       </c>
       <c r="D72" s="25" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="E72" s="1">
         <v>2</v>
@@ -14900,13 +14900,13 @@
         <v>100</v>
       </c>
       <c r="U72" s="11" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="V72" s="7" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="W72" s="1" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="X72" s="1"/>
       <c r="Y72" s="1">
@@ -14933,7 +14933,7 @@
         <v>204</v>
       </c>
       <c r="D73" s="25" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="E73" s="1">
         <v>2</v>
@@ -15019,7 +15019,7 @@
         <v>201</v>
       </c>
       <c r="D74" s="25" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="E74" s="1">
         <v>4</v>
@@ -15072,10 +15072,10 @@
         <v>103</v>
       </c>
       <c r="U74" s="11" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="V74" s="7" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="W74" s="1" t="s">
         <v>103</v>
@@ -15107,7 +15107,7 @@
         <v>261</v>
       </c>
       <c r="D75" s="25" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="E75" s="1">
         <v>3</v>
@@ -15160,10 +15160,10 @@
         <v>102</v>
       </c>
       <c r="U75" s="11" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="V75" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="W75" s="1" t="s">
         <v>105</v>
@@ -15193,7 +15193,7 @@
         <v>262</v>
       </c>
       <c r="D76" s="25" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="E76" s="1">
         <v>3</v>
@@ -15279,7 +15279,7 @@
         <v>300</v>
       </c>
       <c r="D77" s="25" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="E77" s="1">
         <v>3</v>
@@ -15332,10 +15332,10 @@
         <v>103</v>
       </c>
       <c r="U77" s="11" t="s">
+        <v>600</v>
+      </c>
+      <c r="V77" s="7" t="s">
         <v>601</v>
-      </c>
-      <c r="V77" s="7" t="s">
-        <v>602</v>
       </c>
       <c r="W77" s="1" t="s">
         <v>109</v>
@@ -15365,7 +15365,7 @@
         <v>263</v>
       </c>
       <c r="D78" s="25" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="E78" s="1">
         <v>4</v>
@@ -15451,7 +15451,7 @@
         <v>264</v>
       </c>
       <c r="D79" s="25" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="E79" s="1">
         <v>3</v>
@@ -15539,7 +15539,7 @@
         <v>265</v>
       </c>
       <c r="D80" s="25" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="E80" s="1">
         <v>3</v>
@@ -15625,7 +15625,7 @@
         <v>266</v>
       </c>
       <c r="D81" s="25" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="E81" s="1">
         <v>1</v>
@@ -15678,10 +15678,10 @@
         <v>100</v>
       </c>
       <c r="U81" s="39" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="V81" s="7" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="W81" s="1" t="s">
         <v>93</v>
@@ -15709,7 +15709,7 @@
         <v>267</v>
       </c>
       <c r="D82" s="25" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="E82" s="1">
         <v>3</v>
@@ -15797,7 +15797,7 @@
         <v>268</v>
       </c>
       <c r="D83" s="25" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="E83" s="1">
         <v>2</v>
@@ -15844,7 +15844,7 @@
         <v>30</v>
       </c>
       <c r="S83" s="7" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="T83">
         <v>100</v>
@@ -15853,7 +15853,7 @@
         <v>574</v>
       </c>
       <c r="V83" s="7" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="W83" s="1" t="s">
         <v>81</v>
@@ -15885,7 +15885,7 @@
         <v>269</v>
       </c>
       <c r="D84" s="25" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E84" s="1">
         <v>2</v>
@@ -15932,16 +15932,16 @@
         <v>30</v>
       </c>
       <c r="S84" s="7" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="T84">
         <v>100</v>
       </c>
       <c r="U84" s="11" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="V84" s="7" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="W84" s="1" t="s">
         <v>51</v>
@@ -15973,7 +15973,7 @@
         <v>270</v>
       </c>
       <c r="D85" s="25" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="E85" s="1">
         <v>3</v>
@@ -16026,10 +16026,10 @@
         <v>100</v>
       </c>
       <c r="U85" s="11" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="V85" s="7" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="W85" s="1" t="s">
         <v>122</v>
@@ -16059,7 +16059,7 @@
         <v>289</v>
       </c>
       <c r="D86" s="25" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E86" s="1">
         <v>3</v>
@@ -16112,7 +16112,7 @@
         <v>100</v>
       </c>
       <c r="U86" s="11" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="V86" s="7" t="s">
         <v>578</v>
@@ -16145,7 +16145,7 @@
         <v>203</v>
       </c>
       <c r="D87" s="25" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="E87" s="1">
         <v>4</v>
@@ -16192,16 +16192,16 @@
         <v>15</v>
       </c>
       <c r="S87" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="T87">
         <v>100</v>
       </c>
       <c r="U87" s="11" t="s">
+        <v>598</v>
+      </c>
+      <c r="V87" s="7" t="s">
         <v>599</v>
-      </c>
-      <c r="V87" s="7" t="s">
-        <v>600</v>
       </c>
       <c r="W87" s="1" t="s">
         <v>455</v>
@@ -16233,7 +16233,7 @@
         <v>205</v>
       </c>
       <c r="D88" s="25" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="E88" s="1">
         <v>3</v>
@@ -16286,7 +16286,7 @@
         <v>100</v>
       </c>
       <c r="U88" s="11" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="V88" s="7" t="s">
         <v>577</v>
@@ -16321,7 +16321,7 @@
         <v>206</v>
       </c>
       <c r="D89" s="25" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="E89" s="1">
         <v>2</v>
@@ -16407,7 +16407,7 @@
         <v>207</v>
       </c>
       <c r="D90" s="25" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="E90" s="1">
         <v>3</v>
@@ -16454,16 +16454,16 @@
         <v>40</v>
       </c>
       <c r="S90" s="7" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="T90">
         <v>100</v>
       </c>
       <c r="U90" s="11" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="V90" s="7" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="W90" s="1" t="s">
         <v>59</v>
@@ -16495,7 +16495,7 @@
         <v>271</v>
       </c>
       <c r="D91" s="25" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E91" s="1">
         <v>3</v>
@@ -16548,7 +16548,7 @@
         <v>100</v>
       </c>
       <c r="U91" s="11" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="V91" s="7" t="s">
         <v>340</v>
@@ -16583,7 +16583,7 @@
         <v>272</v>
       </c>
       <c r="D92" s="25" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E92" s="1">
         <v>4</v>
@@ -16636,10 +16636,10 @@
         <v>100</v>
       </c>
       <c r="U92" s="11" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="V92" s="7" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="W92" s="1" t="s">
         <v>474</v>
@@ -16757,7 +16757,7 @@
         <v>273</v>
       </c>
       <c r="D94" s="25" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="E94" s="1">
         <v>2</v>
@@ -16810,7 +16810,7 @@
         <v>100</v>
       </c>
       <c r="U94" s="11" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="V94" s="7" t="s">
         <v>341</v>
@@ -16837,13 +16837,13 @@
         <v>53000092</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C95" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="D95" s="25" t="s">
         <v>646</v>
-      </c>
-      <c r="D95" s="25" t="s">
-        <v>648</v>
       </c>
       <c r="E95" s="1">
         <v>3</v>
@@ -16890,19 +16890,19 @@
         <v>0</v>
       </c>
       <c r="S95" s="7" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="T95">
         <v>100</v>
       </c>
       <c r="U95" s="11" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="V95" s="1" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="W95" s="1" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="X95" s="1"/>
       <c r="Y95" s="1">
@@ -16929,7 +16929,7 @@
         <v>274</v>
       </c>
       <c r="D96" s="25" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="E96" s="1">
         <v>2</v>
@@ -16982,10 +16982,10 @@
         <v>100</v>
       </c>
       <c r="U96" s="11" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="V96" s="7" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="W96" s="1" t="s">
         <v>134</v>
@@ -17101,7 +17101,7 @@
         <v>276</v>
       </c>
       <c r="D98" s="25" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="E98" s="1">
         <v>2</v>
@@ -17154,10 +17154,10 @@
         <v>100</v>
       </c>
       <c r="U98" s="11" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="V98" s="7" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="W98" s="1" t="s">
         <v>139</v>
@@ -17189,7 +17189,7 @@
         <v>277</v>
       </c>
       <c r="D99" s="25" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="E99" s="1">
         <v>3</v>
@@ -17236,16 +17236,16 @@
         <v>200</v>
       </c>
       <c r="S99" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="T99">
         <v>104</v>
       </c>
       <c r="U99" s="11" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="V99" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="W99" s="1" t="s">
         <v>29</v>
@@ -17275,7 +17275,7 @@
         <v>278</v>
       </c>
       <c r="D100" s="25" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="E100" s="1">
         <v>2</v>
@@ -17328,10 +17328,10 @@
         <v>100</v>
       </c>
       <c r="U100" s="11" t="s">
+        <v>594</v>
+      </c>
+      <c r="V100" s="7" t="s">
         <v>595</v>
-      </c>
-      <c r="V100" s="7" t="s">
-        <v>596</v>
       </c>
       <c r="W100" s="1" t="s">
         <v>81</v>
@@ -17447,7 +17447,7 @@
         <v>279</v>
       </c>
       <c r="D102" s="25" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="E102" s="1">
         <v>1</v>
@@ -17500,10 +17500,10 @@
         <v>100</v>
       </c>
       <c r="U102" s="11" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="V102" s="7" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="W102" s="1" t="s">
         <v>97</v>
@@ -17533,7 +17533,7 @@
         <v>280</v>
       </c>
       <c r="D103" s="25" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="E103" s="1">
         <v>4</v>
@@ -17580,16 +17580,16 @@
         <v>0</v>
       </c>
       <c r="S103" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="T103">
         <v>100</v>
       </c>
       <c r="U103" s="11" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="V103" s="1" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="W103" s="1" t="s">
         <v>144</v>
@@ -17619,7 +17619,7 @@
         <v>292</v>
       </c>
       <c r="D104" s="25" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="E104" s="1">
         <v>3</v>
@@ -17666,16 +17666,16 @@
         <v>0</v>
       </c>
       <c r="S104" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="T104">
         <v>100</v>
       </c>
       <c r="U104" s="11" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="V104" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="W104" s="1" t="s">
         <v>168</v>
@@ -17705,7 +17705,7 @@
         <v>281</v>
       </c>
       <c r="D105" s="25" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="E105" s="1">
         <v>3</v>
@@ -17758,7 +17758,7 @@
         <v>100</v>
       </c>
       <c r="U105" s="11" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="V105" s="7" t="s">
         <v>342</v>
@@ -17791,7 +17791,7 @@
         <v>282</v>
       </c>
       <c r="D106" s="25" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="E106" s="1">
         <v>3</v>
@@ -17844,10 +17844,10 @@
         <v>105</v>
       </c>
       <c r="U106" s="11" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="V106" s="7" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="W106" s="1" t="s">
         <v>147</v>
@@ -17879,7 +17879,7 @@
         <v>283</v>
       </c>
       <c r="D107" s="25" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="E107" s="1">
         <v>3</v>
@@ -17932,10 +17932,10 @@
         <v>105</v>
       </c>
       <c r="U107" s="11" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="V107" s="7" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="W107" s="1" t="s">
         <v>149</v>
@@ -18051,7 +18051,7 @@
         <v>284</v>
       </c>
       <c r="D109" s="25" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="E109" s="1">
         <v>1</v>
@@ -18104,10 +18104,10 @@
         <v>100</v>
       </c>
       <c r="U109" s="11" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="V109" s="7" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="W109" s="1" t="s">
         <v>153</v>
@@ -18137,7 +18137,7 @@
         <v>285</v>
       </c>
       <c r="D110" s="25" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="E110" s="1">
         <v>1</v>
@@ -18190,10 +18190,10 @@
         <v>100</v>
       </c>
       <c r="U110" s="11" t="s">
+        <v>777</v>
+      </c>
+      <c r="V110" s="7" t="s">
         <v>779</v>
-      </c>
-      <c r="V110" s="7" t="s">
-        <v>781</v>
       </c>
       <c r="W110" s="1" t="s">
         <v>155</v>
@@ -18223,7 +18223,7 @@
         <v>286</v>
       </c>
       <c r="D111" s="25" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="E111" s="1">
         <v>2</v>
@@ -18276,10 +18276,10 @@
         <v>100</v>
       </c>
       <c r="U111" s="11" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="V111" s="7" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="W111" s="1" t="s">
         <v>157</v>
@@ -18309,7 +18309,7 @@
         <v>287</v>
       </c>
       <c r="D112" s="25" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="E112" s="1">
         <v>2</v>
@@ -18362,7 +18362,7 @@
         <v>100</v>
       </c>
       <c r="U112" s="11" t="s">
-        <v>583</v>
+        <v>805</v>
       </c>
       <c r="V112" s="7" t="s">
         <v>582</v>
@@ -18448,10 +18448,10 @@
         <v>103</v>
       </c>
       <c r="U113" s="11" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="V113" s="7" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="W113" s="1" t="s">
         <v>29</v>
@@ -18475,13 +18475,13 @@
         <v>53000111</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="D114" s="25" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="E114" s="1">
         <v>3</v>
@@ -18528,22 +18528,22 @@
         <v>20</v>
       </c>
       <c r="S114" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="T114">
         <v>100</v>
       </c>
       <c r="U114" s="11" t="s">
+        <v>663</v>
+      </c>
+      <c r="V114" s="7" t="s">
+        <v>664</v>
+      </c>
+      <c r="W114" s="1" t="s">
         <v>665</v>
       </c>
-      <c r="V114" s="7" t="s">
-        <v>666</v>
-      </c>
-      <c r="W114" s="1" t="s">
-        <v>667</v>
-      </c>
       <c r="X114" s="1" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="Y114" s="1">
         <v>11000007</v>
@@ -18563,13 +18563,13 @@
         <v>53000112</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="D115" s="25" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="E115" s="1">
         <v>3</v>
@@ -18616,16 +18616,16 @@
         <v>100</v>
       </c>
       <c r="S115" s="1" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="T115">
         <v>100</v>
       </c>
       <c r="U115" s="11" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="V115" s="7" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="W115" s="1" t="s">
         <v>123</v>
@@ -18651,10 +18651,10 @@
         <v>53000113</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="D116" s="25"/>
       <c r="E116" s="1">
@@ -18702,22 +18702,22 @@
         <v>0</v>
       </c>
       <c r="S116" s="1" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="T116">
         <v>100</v>
       </c>
       <c r="U116" s="11" t="s">
+        <v>749</v>
+      </c>
+      <c r="V116" s="7" t="s">
         <v>751</v>
       </c>
-      <c r="V116" s="7" t="s">
-        <v>753</v>
-      </c>
       <c r="W116" s="1" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="X116" s="1" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="Y116" s="1">
         <v>11000003</v>
@@ -18737,10 +18737,10 @@
         <v>53000114</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="D117" s="25"/>
       <c r="E117" s="1">
@@ -18788,16 +18788,16 @@
         <v>0</v>
       </c>
       <c r="S117" s="1" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="T117">
         <v>101</v>
       </c>
       <c r="U117" s="11" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="V117" s="7" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="W117" s="1" t="s">
         <v>99</v>
@@ -18823,10 +18823,10 @@
         <v>53000115</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="D118" s="25"/>
       <c r="E118" s="1">
@@ -18874,16 +18874,16 @@
         <v>0</v>
       </c>
       <c r="S118" s="1" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="T118">
         <v>100</v>
       </c>
       <c r="U118" s="11" t="s">
+        <v>761</v>
+      </c>
+      <c r="V118" s="7" t="s">
         <v>763</v>
-      </c>
-      <c r="V118" s="7" t="s">
-        <v>765</v>
       </c>
       <c r="W118" s="1" t="s">
         <v>99</v>
@@ -18909,13 +18909,13 @@
         <v>53000116</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="D119" s="25" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="E119" s="1">
         <v>2</v>
@@ -18968,10 +18968,10 @@
         <v>101</v>
       </c>
       <c r="U119" s="11" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="V119" s="7" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="W119" s="1" t="s">
         <v>99</v>
@@ -18997,13 +18997,13 @@
         <v>53000117</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="D120" s="25" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="E120" s="1">
         <v>1</v>
@@ -19050,16 +19050,16 @@
         <v>0</v>
       </c>
       <c r="S120" s="1" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="T120">
         <v>100</v>
       </c>
       <c r="U120" s="11" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="V120" s="7" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="W120" s="1" t="s">
         <v>99</v>
@@ -19085,10 +19085,10 @@
         <v>53000118</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="D121" s="25"/>
       <c r="E121" s="1">
@@ -19136,22 +19136,22 @@
         <v>0</v>
       </c>
       <c r="S121" s="1" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="T121">
         <v>100</v>
       </c>
       <c r="U121" s="11" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="V121" s="7" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="W121" s="1" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="X121" s="1" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="Y121" s="1">
         <v>11000003</v>
@@ -19172,90 +19172,90 @@
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I38:I68 I17:I35 I4:I15 I70:I121">
-    <cfRule type="cellIs" dxfId="55" priority="56" operator="notEqual">
+    <cfRule type="cellIs" dxfId="147" priority="56" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J17:N35 J4:N15 J38:N68 P38:Q68 P5:Q15 P17:Q35 P4 P70:Q121 J70:N121">
-    <cfRule type="cellIs" dxfId="54" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="55" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I69">
-    <cfRule type="cellIs" dxfId="53" priority="20" operator="notEqual">
+    <cfRule type="cellIs" dxfId="145" priority="20" operator="notEqual">
       <formula>$E69</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J69:N69 P69:Q69">
-    <cfRule type="cellIs" dxfId="52" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="19" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36">
-    <cfRule type="cellIs" dxfId="51" priority="18" operator="notEqual">
+    <cfRule type="cellIs" dxfId="143" priority="18" operator="notEqual">
       <formula>$E36</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J36:N36 P36:Q36">
-    <cfRule type="cellIs" dxfId="50" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="17" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37">
-    <cfRule type="cellIs" dxfId="49" priority="16" operator="notEqual">
+    <cfRule type="cellIs" dxfId="141" priority="16" operator="notEqual">
       <formula>$E37</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J37:N37 P37:Q37">
-    <cfRule type="cellIs" dxfId="48" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="15" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H15 H17:H121">
-    <cfRule type="cellIs" dxfId="47" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="12" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="13" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="14" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="136" priority="14" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="cellIs" dxfId="43" priority="8" operator="notEqual">
+    <cfRule type="cellIs" dxfId="135" priority="8" operator="notEqual">
       <formula>$E16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:N16 P16:Q16">
-    <cfRule type="cellIs" dxfId="42" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="cellIs" dxfId="41" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="5" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="130" priority="6" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="37" priority="2" operator="containsText" text="未完成">
+    <cfRule type="containsText" dxfId="129" priority="2" operator="containsText" text="未完成">
       <formula>NOT(ISERROR(SEARCH("未完成",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:O121">
-    <cfRule type="cellIs" dxfId="36" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19343,7 +19343,7 @@
         <v>349</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="P1" s="17" t="s">
         <v>331</v>
@@ -19429,7 +19429,7 @@
         <v>348</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>318</v>
@@ -19515,7 +19515,7 @@
         <v>351</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="P3" s="20" t="s">
         <v>333</v>
@@ -19617,7 +19617,7 @@
         <v>-1</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="V4" s="7" t="s">
         <v>342</v>
@@ -19777,7 +19777,7 @@
         <v>-1</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="V6" s="7" t="s">
         <v>377</v>
@@ -19937,7 +19937,7 @@
         <v>-1</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="V8" s="7" t="s">
         <v>379</v>
@@ -20122,7 +20122,7 @@
         <v>53100007</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="34"/>
@@ -20171,16 +20171,16 @@
         <v>0</v>
       </c>
       <c r="S11" s="15" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="T11" s="1">
         <v>-1</v>
       </c>
       <c r="U11" s="11" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="V11" s="7" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="W11" s="15" t="s">
         <v>2</v>
@@ -20200,110 +20200,110 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="J4:Q11">
-    <cfRule type="cellIs" dxfId="35" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="40" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:Q8">
-    <cfRule type="cellIs" dxfId="34" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="36" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:Q4 O4:O11">
-    <cfRule type="cellIs" dxfId="33" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="35" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="32" priority="34" operator="notEqual">
+    <cfRule type="cellIs" dxfId="93" priority="34" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:Q4 O4:O11">
-    <cfRule type="cellIs" dxfId="31" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="33" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="30" priority="32" operator="notEqual">
+    <cfRule type="cellIs" dxfId="91" priority="32" operator="notEqual">
       <formula>$E5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:Q5">
-    <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="31" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" dxfId="28" priority="30" operator="notEqual">
+    <cfRule type="cellIs" dxfId="89" priority="30" operator="notEqual">
       <formula>$E6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:Q6">
-    <cfRule type="cellIs" dxfId="27" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="29" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="26" priority="28" operator="notEqual">
+    <cfRule type="cellIs" dxfId="87" priority="28" operator="notEqual">
       <formula>$E7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:Q7">
-    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="27" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="24" priority="26" operator="notEqual">
+    <cfRule type="cellIs" dxfId="85" priority="26" operator="notEqual">
       <formula>$E8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:Q8">
-    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="25" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I11">
-    <cfRule type="cellIs" dxfId="22" priority="24" operator="notEqual">
+    <cfRule type="cellIs" dxfId="83" priority="24" operator="notEqual">
       <formula>$E9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:Q11">
-    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="23" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H11">
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="7" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="8" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="78" priority="9" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="4" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="74" priority="5" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10:L11">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20392,7 +20392,7 @@
         <v>349</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="P1" s="17" t="s">
         <v>331</v>
@@ -20478,7 +20478,7 @@
         <v>348</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>318</v>
@@ -20564,7 +20564,7 @@
         <v>351</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="P3" s="20" t="s">
         <v>333</v>
@@ -20670,7 +20670,7 @@
         <v>115</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="V4" s="7" t="s">
         <v>376</v>
@@ -20754,7 +20754,7 @@
         <v>90</v>
       </c>
       <c r="U5" s="11" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="V5" s="7" t="s">
         <v>380</v>
@@ -21004,7 +21004,7 @@
         <v>90</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="V8" s="7" t="s">
         <v>390</v>
@@ -21113,50 +21113,50 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I4:I9">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="notEqual">
+    <cfRule type="cellIs" dxfId="41" priority="12" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:Q7 O4:O9">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:Q9">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:Q8">
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H9">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="6" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="34" priority="8" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="30" priority="4" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
#58 2 new cards for warrior
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -639,7 +639,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="831">
   <si>
     <t>慈悲</t>
   </si>
@@ -3586,6 +3586,58 @@
   </si>
   <si>
     <t>Shadowstep</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>旋风斩</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Whirl Wind</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>范围</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NAR</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse)){im.OnMagicDamage(null, s.Damage,s.Attr);}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对3卡片距离内敌我单位造成{0}点魔法伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hit1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>斩杀</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Execute</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>直伤</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>UES</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(t.Hp&lt;=s.Damage&amp;&amp;t.HpRate&lt;100)t.SuddenDeath();</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>直接斩杀生命值低于{0}且生命未满的敌方单位</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -4591,76 +4643,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="157">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="156">
     <dxf>
       <font>
         <b/>
@@ -4949,6 +4932,68 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7671,11 +7716,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="725470816"/>
-        <c:axId val="725471376"/>
+        <c:axId val="467440464"/>
+        <c:axId val="467439904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="725470816"/>
+        <c:axId val="467440464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7718,7 +7763,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="725471376"/>
+        <c:crossAx val="467439904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7726,7 +7771,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="725471376"/>
+        <c:axId val="467439904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7777,7 +7822,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="725470816"/>
+        <c:crossAx val="467440464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8405,132 +8450,132 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AB123" totalsRowShown="0" headerRowDxfId="156" dataDxfId="155" tableBorderDxfId="154">
-  <autoFilter ref="A3:AB123"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AB125" totalsRowShown="0" headerRowDxfId="155" dataDxfId="154" tableBorderDxfId="153">
+  <autoFilter ref="A3:AB125"/>
   <sortState ref="A4:AB113">
     <sortCondition ref="A3:A113"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="153"/>
-    <tableColumn id="2" name="Name" dataDxfId="152"/>
-    <tableColumn id="20" name="Ename" dataDxfId="151"/>
-    <tableColumn id="21" name="Remark" dataDxfId="150"/>
-    <tableColumn id="3" name="Star" dataDxfId="149"/>
-    <tableColumn id="4" name="Type" dataDxfId="148"/>
-    <tableColumn id="5" name="Attr" dataDxfId="147"/>
-    <tableColumn id="8" name="Quality" dataDxfId="146">
+    <tableColumn id="1" name="Id" dataDxfId="152"/>
+    <tableColumn id="2" name="Name" dataDxfId="151"/>
+    <tableColumn id="20" name="Ename" dataDxfId="150"/>
+    <tableColumn id="21" name="Remark" dataDxfId="149"/>
+    <tableColumn id="3" name="Star" dataDxfId="148"/>
+    <tableColumn id="4" name="Type" dataDxfId="147"/>
+    <tableColumn id="5" name="Attr" dataDxfId="146"/>
+    <tableColumn id="8" name="Quality" dataDxfId="145">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="145"/>
-    <tableColumn id="9" name="Damage" dataDxfId="144"/>
-    <tableColumn id="10" name="Cure" dataDxfId="143"/>
-    <tableColumn id="11" name="Time" dataDxfId="142"/>
-    <tableColumn id="13" name="Help" dataDxfId="141"/>
-    <tableColumn id="16" name="Rate" dataDxfId="140"/>
-    <tableColumn id="18" name="Atk" dataDxfId="139"/>
-    <tableColumn id="12" name="Modify" dataDxfId="138"/>
-    <tableColumn id="27" name="Sum" dataDxfId="137">
+    <tableColumn id="7" name="Cost" dataDxfId="144"/>
+    <tableColumn id="9" name="Damage" dataDxfId="143"/>
+    <tableColumn id="10" name="Cure" dataDxfId="142"/>
+    <tableColumn id="11" name="Time" dataDxfId="141"/>
+    <tableColumn id="13" name="Help" dataDxfId="140"/>
+    <tableColumn id="16" name="Rate" dataDxfId="139"/>
+    <tableColumn id="18" name="Atk" dataDxfId="138"/>
+    <tableColumn id="12" name="Modify" dataDxfId="137"/>
+    <tableColumn id="27" name="Sum" dataDxfId="136">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="136"/>
-    <tableColumn id="15" name="Target" dataDxfId="135"/>
-    <tableColumn id="25" name="Mark" dataDxfId="134"/>
-    <tableColumn id="22" name="Effect" dataDxfId="133"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="132"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="131"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="130"/>
-    <tableColumn id="26" name="JobId" dataDxfId="129"/>
-    <tableColumn id="19" name="Icon" dataDxfId="128"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="127"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="126"/>
+    <tableColumn id="6" name="Range" dataDxfId="135"/>
+    <tableColumn id="15" name="Target" dataDxfId="134"/>
+    <tableColumn id="25" name="Mark" dataDxfId="133"/>
+    <tableColumn id="22" name="Effect" dataDxfId="132"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="131"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="130"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="129"/>
+    <tableColumn id="26" name="JobId" dataDxfId="128"/>
+    <tableColumn id="19" name="Icon" dataDxfId="127"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="126"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="125"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AB11" totalsRowShown="0" headerRowDxfId="125" dataDxfId="124" tableBorderDxfId="123">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AB11" totalsRowShown="0" headerRowDxfId="124" dataDxfId="123" tableBorderDxfId="122">
   <autoFilter ref="A3:AB11"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="122"/>
-    <tableColumn id="2" name="Name" dataDxfId="121"/>
-    <tableColumn id="20" name="Ename" dataDxfId="120"/>
-    <tableColumn id="21" name="Remark" dataDxfId="119"/>
-    <tableColumn id="3" name="Star" dataDxfId="118"/>
-    <tableColumn id="4" name="Type" dataDxfId="117"/>
-    <tableColumn id="5" name="Attr" dataDxfId="116"/>
-    <tableColumn id="8" name="Quality" dataDxfId="115">
+    <tableColumn id="1" name="Id" dataDxfId="121"/>
+    <tableColumn id="2" name="Name" dataDxfId="120"/>
+    <tableColumn id="20" name="Ename" dataDxfId="119"/>
+    <tableColumn id="21" name="Remark" dataDxfId="118"/>
+    <tableColumn id="3" name="Star" dataDxfId="117"/>
+    <tableColumn id="4" name="Type" dataDxfId="116"/>
+    <tableColumn id="5" name="Attr" dataDxfId="115"/>
+    <tableColumn id="8" name="Quality" dataDxfId="114">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="114"/>
-    <tableColumn id="9" name="Damage" dataDxfId="113"/>
-    <tableColumn id="10" name="Cure" dataDxfId="112"/>
-    <tableColumn id="11" name="Time" dataDxfId="111"/>
-    <tableColumn id="13" name="Help" dataDxfId="110"/>
-    <tableColumn id="16" name="Rate" dataDxfId="109"/>
-    <tableColumn id="18" name="Atk" dataDxfId="108"/>
-    <tableColumn id="12" name="Modify" dataDxfId="107"/>
-    <tableColumn id="27" name="Sum" dataDxfId="106">
+    <tableColumn id="7" name="Cost" dataDxfId="113"/>
+    <tableColumn id="9" name="Damage" dataDxfId="112"/>
+    <tableColumn id="10" name="Cure" dataDxfId="111"/>
+    <tableColumn id="11" name="Time" dataDxfId="110"/>
+    <tableColumn id="13" name="Help" dataDxfId="109"/>
+    <tableColumn id="16" name="Rate" dataDxfId="108"/>
+    <tableColumn id="18" name="Atk" dataDxfId="107"/>
+    <tableColumn id="12" name="Modify" dataDxfId="106"/>
+    <tableColumn id="27" name="Sum" dataDxfId="105">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="105"/>
-    <tableColumn id="15" name="Target" dataDxfId="104"/>
-    <tableColumn id="25" name="Mark" dataDxfId="103"/>
-    <tableColumn id="22" name="Effect" dataDxfId="102"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="101"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="100"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="99"/>
-    <tableColumn id="26" name="JobId" dataDxfId="98"/>
-    <tableColumn id="19" name="Icon" dataDxfId="97"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="96"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="95"/>
+    <tableColumn id="6" name="Range" dataDxfId="104"/>
+    <tableColumn id="15" name="Target" dataDxfId="103"/>
+    <tableColumn id="25" name="Mark" dataDxfId="102"/>
+    <tableColumn id="22" name="Effect" dataDxfId="101"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="100"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="99"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="98"/>
+    <tableColumn id="26" name="JobId" dataDxfId="97"/>
+    <tableColumn id="19" name="Icon" dataDxfId="96"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="95"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="94"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_35" displayName="表1_35" ref="A3:AB9" totalsRowShown="0" headerRowDxfId="94" tableBorderDxfId="93">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_35" displayName="表1_35" ref="A3:AB9" totalsRowShown="0" headerRowDxfId="93" tableBorderDxfId="92">
   <autoFilter ref="A3:AB9"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="92"/>
-    <tableColumn id="2" name="Name" dataDxfId="91"/>
-    <tableColumn id="20" name="Ename" dataDxfId="90"/>
-    <tableColumn id="21" name="Remark" dataDxfId="89"/>
-    <tableColumn id="3" name="Star" dataDxfId="88"/>
-    <tableColumn id="4" name="Type" dataDxfId="87"/>
-    <tableColumn id="5" name="Attr" dataDxfId="86"/>
-    <tableColumn id="8" name="Quality" dataDxfId="85">
+    <tableColumn id="1" name="Id" dataDxfId="91"/>
+    <tableColumn id="2" name="Name" dataDxfId="90"/>
+    <tableColumn id="20" name="Ename" dataDxfId="89"/>
+    <tableColumn id="21" name="Remark" dataDxfId="88"/>
+    <tableColumn id="3" name="Star" dataDxfId="87"/>
+    <tableColumn id="4" name="Type" dataDxfId="86"/>
+    <tableColumn id="5" name="Attr" dataDxfId="85"/>
+    <tableColumn id="8" name="Quality" dataDxfId="84">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="84"/>
-    <tableColumn id="9" name="Damage" dataDxfId="83"/>
-    <tableColumn id="10" name="Cure" dataDxfId="82"/>
-    <tableColumn id="11" name="Time" dataDxfId="81"/>
-    <tableColumn id="13" name="Help" dataDxfId="80"/>
-    <tableColumn id="16" name="Rate" dataDxfId="79"/>
-    <tableColumn id="18" name="Atk" dataDxfId="78"/>
-    <tableColumn id="12" name="Modify" dataDxfId="77"/>
-    <tableColumn id="27" name="Sum" dataDxfId="76">
+    <tableColumn id="7" name="Cost" dataDxfId="83"/>
+    <tableColumn id="9" name="Damage" dataDxfId="82"/>
+    <tableColumn id="10" name="Cure" dataDxfId="81"/>
+    <tableColumn id="11" name="Time" dataDxfId="80"/>
+    <tableColumn id="13" name="Help" dataDxfId="79"/>
+    <tableColumn id="16" name="Rate" dataDxfId="78"/>
+    <tableColumn id="18" name="Atk" dataDxfId="77"/>
+    <tableColumn id="12" name="Modify" dataDxfId="76"/>
+    <tableColumn id="27" name="Sum" dataDxfId="75">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="75"/>
-    <tableColumn id="15" name="Target" dataDxfId="74"/>
-    <tableColumn id="25" name="Mark" dataDxfId="73"/>
-    <tableColumn id="22" name="Effect" dataDxfId="72"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="71"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="70"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="69"/>
-    <tableColumn id="26" name="JobId" dataDxfId="68"/>
-    <tableColumn id="19" name="Icon" dataDxfId="67"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="66"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="65"/>
+    <tableColumn id="6" name="Range" dataDxfId="74"/>
+    <tableColumn id="15" name="Target" dataDxfId="73"/>
+    <tableColumn id="25" name="Mark" dataDxfId="72"/>
+    <tableColumn id="22" name="Effect" dataDxfId="71"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="70"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="69"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="68"/>
+    <tableColumn id="26" name="JobId" dataDxfId="67"/>
+    <tableColumn id="19" name="Icon" dataDxfId="66"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="65"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8823,13 +8868,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB123"/>
+  <dimension ref="A1:AB125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C120" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C121" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P122" sqref="P122"/>
+      <selection pane="bottomRight" activeCell="V123" sqref="V123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -19193,7 +19238,7 @@
         <v>0</v>
       </c>
       <c r="AB120" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:28" ht="72">
@@ -19451,6 +19496,182 @@
         <v>0</v>
       </c>
       <c r="AB123" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:28" ht="72">
+      <c r="A124">
+        <v>53000121</v>
+      </c>
+      <c r="B124" s="22" t="s">
+        <v>818</v>
+      </c>
+      <c r="C124" s="15" t="s">
+        <v>819</v>
+      </c>
+      <c r="D124" s="25" t="s">
+        <v>820</v>
+      </c>
+      <c r="E124" s="15">
+        <v>1</v>
+      </c>
+      <c r="F124" s="15">
+        <v>201</v>
+      </c>
+      <c r="G124" s="15">
+        <v>2</v>
+      </c>
+      <c r="H124" s="43">
+        <f t="shared" ref="H124" si="26">IF(AND(Q124&gt;=13,Q124&lt;=16),5,IF(AND(Q124&gt;=9,Q124&lt;=12),4,IF(AND(Q124&gt;=5,Q124&lt;=8),3,IF(AND(Q124&gt;=1,Q124&lt;=4),2,IF(AND(Q124&gt;=-3,Q124&lt;=0),1,IF(AND(Q124&gt;=-5,Q124&lt;=-4),0,6))))))</f>
+        <v>1</v>
+      </c>
+      <c r="I124" s="15">
+        <v>1</v>
+      </c>
+      <c r="J124" s="15">
+        <v>45</v>
+      </c>
+      <c r="K124" s="15">
+        <v>0</v>
+      </c>
+      <c r="L124" s="15">
+        <v>0</v>
+      </c>
+      <c r="M124" s="15">
+        <v>0</v>
+      </c>
+      <c r="N124" s="15">
+        <v>0</v>
+      </c>
+      <c r="O124" s="15">
+        <v>0</v>
+      </c>
+      <c r="P124" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q124" s="43">
+        <f t="shared" ref="Q124" si="27">T124-100+P124</f>
+        <v>0</v>
+      </c>
+      <c r="R124" s="15">
+        <v>30</v>
+      </c>
+      <c r="S124" s="7" t="s">
+        <v>821</v>
+      </c>
+      <c r="T124">
+        <v>100</v>
+      </c>
+      <c r="U124" s="11" t="s">
+        <v>822</v>
+      </c>
+      <c r="V124" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="W124" s="15" t="s">
+        <v>824</v>
+      </c>
+      <c r="X124" s="15" t="s">
+        <v>824</v>
+      </c>
+      <c r="Y124" s="1">
+        <v>11000001</v>
+      </c>
+      <c r="Z124" s="15">
+        <v>121</v>
+      </c>
+      <c r="AA124" s="27">
+        <v>0</v>
+      </c>
+      <c r="AB124" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:28" ht="36">
+      <c r="A125">
+        <v>53000122</v>
+      </c>
+      <c r="B125" s="22" t="s">
+        <v>825</v>
+      </c>
+      <c r="C125" s="15" t="s">
+        <v>826</v>
+      </c>
+      <c r="D125" s="25" t="s">
+        <v>827</v>
+      </c>
+      <c r="E125" s="15">
+        <v>1</v>
+      </c>
+      <c r="F125" s="15">
+        <v>200</v>
+      </c>
+      <c r="G125" s="15">
+        <v>2</v>
+      </c>
+      <c r="H125" s="43">
+        <f t="shared" ref="H125" si="28">IF(AND(Q125&gt;=13,Q125&lt;=16),5,IF(AND(Q125&gt;=9,Q125&lt;=12),4,IF(AND(Q125&gt;=5,Q125&lt;=8),3,IF(AND(Q125&gt;=1,Q125&lt;=4),2,IF(AND(Q125&gt;=-3,Q125&lt;=0),1,IF(AND(Q125&gt;=-5,Q125&lt;=-4),0,6))))))</f>
+        <v>1</v>
+      </c>
+      <c r="I125" s="15">
+        <v>1</v>
+      </c>
+      <c r="J125" s="15">
+        <v>200</v>
+      </c>
+      <c r="K125" s="15">
+        <v>0</v>
+      </c>
+      <c r="L125" s="15">
+        <v>0</v>
+      </c>
+      <c r="M125" s="15">
+        <v>0</v>
+      </c>
+      <c r="N125" s="15">
+        <v>0</v>
+      </c>
+      <c r="O125" s="15">
+        <v>0</v>
+      </c>
+      <c r="P125" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q125" s="43">
+        <f t="shared" ref="Q125" si="29">T125-100+P125</f>
+        <v>0</v>
+      </c>
+      <c r="R125" s="15">
+        <v>0</v>
+      </c>
+      <c r="S125" s="7" t="s">
+        <v>828</v>
+      </c>
+      <c r="T125">
+        <v>100</v>
+      </c>
+      <c r="U125" s="11" t="s">
+        <v>829</v>
+      </c>
+      <c r="V125" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="W125" s="15" t="s">
+        <v>824</v>
+      </c>
+      <c r="X125" s="15" t="s">
+        <v>824</v>
+      </c>
+      <c r="Y125" s="1">
+        <v>11000001</v>
+      </c>
+      <c r="Z125" s="15">
+        <v>122</v>
+      </c>
+      <c r="AA125" s="27">
+        <v>0</v>
+      </c>
+      <c r="AB125" s="25">
         <v>1</v>
       </c>
     </row>
@@ -19460,124 +19681,124 @@
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I38:I68 I17:I35 I4:I15 I70:I122">
-    <cfRule type="cellIs" dxfId="64" priority="65" operator="notEqual">
+    <cfRule type="cellIs" dxfId="63" priority="65" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J17:N35 J4:N15 J38:N68 P38:Q68 P5:Q15 P17:Q35 P4 P70:Q122 J70:N122">
-    <cfRule type="cellIs" dxfId="63" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="64" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I69">
-    <cfRule type="cellIs" dxfId="62" priority="29" operator="notEqual">
+    <cfRule type="cellIs" dxfId="61" priority="29" operator="notEqual">
       <formula>$E69</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J69:N69 P69:Q69">
-    <cfRule type="cellIs" dxfId="61" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="28" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36">
-    <cfRule type="cellIs" dxfId="60" priority="27" operator="notEqual">
+    <cfRule type="cellIs" dxfId="59" priority="27" operator="notEqual">
       <formula>$E36</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J36:N36 P36:Q36">
-    <cfRule type="cellIs" dxfId="59" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="26" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37">
-    <cfRule type="cellIs" dxfId="58" priority="25" operator="notEqual">
+    <cfRule type="cellIs" dxfId="57" priority="25" operator="notEqual">
       <formula>$E37</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J37:N37 P37:Q37">
-    <cfRule type="cellIs" dxfId="57" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="24" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H15 H17:H122">
-    <cfRule type="cellIs" dxfId="56" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="20" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="21" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="22" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="23" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="52" priority="23" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="cellIs" dxfId="52" priority="17" operator="notEqual">
+    <cfRule type="cellIs" dxfId="51" priority="17" operator="notEqual">
       <formula>$E16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:N16 P16:Q16">
-    <cfRule type="cellIs" dxfId="51" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="16" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="cellIs" dxfId="50" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="12" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="13" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="14" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="15" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="46" priority="15" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D122 D124:D1048576">
-    <cfRule type="containsText" dxfId="46" priority="11" operator="containsText" text="未完成">
+  <conditionalFormatting sqref="D1:D122 D126:D1048576">
+    <cfRule type="containsText" dxfId="45" priority="11" operator="containsText" text="未完成">
       <formula>NOT(ISERROR(SEARCH("未完成",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O4:O123">
-    <cfRule type="cellIs" dxfId="45" priority="10" operator="equal">
+  <conditionalFormatting sqref="O4:O125">
+    <cfRule type="cellIs" dxfId="44" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I123">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="notEqual">
+  <conditionalFormatting sqref="I123:I125">
+    <cfRule type="cellIs" dxfId="43" priority="9" operator="notEqual">
       <formula>$E123</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J123:N123 P123:Q123">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+  <conditionalFormatting sqref="J123:N125 P123:Q125">
+    <cfRule type="cellIs" dxfId="42" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H123">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+  <conditionalFormatting sqref="H123:H125">
+    <cfRule type="cellIs" dxfId="41" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="5" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="6" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="38" priority="7" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O123">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+  <conditionalFormatting sqref="O123:O125">
+    <cfRule type="cellIs" dxfId="37" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D123">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="未完成">
+  <conditionalFormatting sqref="D123:D125">
+    <cfRule type="containsText" dxfId="36" priority="1" operator="containsText" text="未完成">
       <formula>NOT(ISERROR(SEARCH("未完成",D123)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20522,110 +20743,110 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="J4:Q11">
-    <cfRule type="cellIs" dxfId="44" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="40" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:Q8">
-    <cfRule type="cellIs" dxfId="43" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="36" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:Q4 O4:O11">
-    <cfRule type="cellIs" dxfId="42" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="35" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="41" priority="34" operator="notEqual">
+    <cfRule type="cellIs" dxfId="32" priority="34" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:Q4 O4:O11">
-    <cfRule type="cellIs" dxfId="40" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="33" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="39" priority="32" operator="notEqual">
+    <cfRule type="cellIs" dxfId="30" priority="32" operator="notEqual">
       <formula>$E5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:Q5">
-    <cfRule type="cellIs" dxfId="38" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" dxfId="37" priority="30" operator="notEqual">
+    <cfRule type="cellIs" dxfId="28" priority="30" operator="notEqual">
       <formula>$E6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:Q6">
-    <cfRule type="cellIs" dxfId="36" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="29" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="35" priority="28" operator="notEqual">
+    <cfRule type="cellIs" dxfId="26" priority="28" operator="notEqual">
       <formula>$E7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:Q7">
-    <cfRule type="cellIs" dxfId="34" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="33" priority="26" operator="notEqual">
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="notEqual">
       <formula>$E8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:Q8">
-    <cfRule type="cellIs" dxfId="32" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I11">
-    <cfRule type="cellIs" dxfId="31" priority="24" operator="notEqual">
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="notEqual">
       <formula>$E9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:Q11">
-    <cfRule type="cellIs" dxfId="30" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H11">
-    <cfRule type="cellIs" dxfId="29" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="17" priority="9" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="25" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10:L11">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21435,50 +21656,50 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I4:I9">
-    <cfRule type="cellIs" dxfId="20" priority="12" operator="notEqual">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:Q7 O4:O9">
-    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:Q9">
-    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:Q8">
-    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H9">
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
new warrior card charge
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -639,7 +639,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="861">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="862">
   <si>
     <t>慈悲</t>
   </si>
@@ -3709,54 +3709,59 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>Upgrade</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>升级</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>光剑</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Light Sword</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NER</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对1.5卡片距离内敌方单位造成{0}点魔法伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NFR</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>群体，状态</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Charge</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>冲锋</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>if(t.WeaponType==0)t.AddWeapon(52100000,lv);else if(t.WeaponType==1)t.LevelUpWeapon((int)s.Help);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse)){im.SetToPosition("come",(int)s.Help);}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>修复友方目标手中武器，并提升{3:0}级。如果目标没有武器，则给予铁锤</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Upgrade</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>升级</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>光剑</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Light Sword</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>NER</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对1.5卡片距离内敌方单位造成{0}点魔法伤害</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对1.5卡片距离内敌方单位造成{1}点魔法伤害</t>
-  </si>
-  <si>
-    <t>NFR</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>群体，状态</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Charge</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>冲锋</t>
+    <t>范围内的友方单位向前移动{3:0}格</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -4762,79 +4767,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="165">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="156">
     <dxf>
       <font>
         <b/>
@@ -8641,132 +8574,132 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AB131" totalsRowShown="0" headerRowDxfId="164" dataDxfId="163" tableBorderDxfId="162">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AB131" totalsRowShown="0" headerRowDxfId="155" dataDxfId="154" tableBorderDxfId="153">
   <autoFilter ref="A3:AB131"/>
   <sortState ref="A4:AB113">
     <sortCondition ref="A3:A113"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="161"/>
-    <tableColumn id="2" name="Name" dataDxfId="160"/>
-    <tableColumn id="20" name="Ename" dataDxfId="159"/>
-    <tableColumn id="21" name="Remark" dataDxfId="158"/>
-    <tableColumn id="3" name="Star" dataDxfId="157"/>
-    <tableColumn id="4" name="Type" dataDxfId="156"/>
-    <tableColumn id="5" name="Attr" dataDxfId="155"/>
-    <tableColumn id="8" name="Quality" dataDxfId="154">
+    <tableColumn id="1" name="Id" dataDxfId="152"/>
+    <tableColumn id="2" name="Name" dataDxfId="151"/>
+    <tableColumn id="20" name="Ename" dataDxfId="150"/>
+    <tableColumn id="21" name="Remark" dataDxfId="149"/>
+    <tableColumn id="3" name="Star" dataDxfId="148"/>
+    <tableColumn id="4" name="Type" dataDxfId="147"/>
+    <tableColumn id="5" name="Attr" dataDxfId="146"/>
+    <tableColumn id="8" name="Quality" dataDxfId="145">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="153"/>
-    <tableColumn id="9" name="Damage" dataDxfId="152"/>
-    <tableColumn id="10" name="Cure" dataDxfId="151"/>
-    <tableColumn id="11" name="Time" dataDxfId="150"/>
-    <tableColumn id="13" name="Help" dataDxfId="149"/>
-    <tableColumn id="16" name="Rate" dataDxfId="148"/>
-    <tableColumn id="18" name="Atk" dataDxfId="147"/>
-    <tableColumn id="12" name="Modify" dataDxfId="146"/>
-    <tableColumn id="27" name="Sum" dataDxfId="145">
+    <tableColumn id="7" name="Cost" dataDxfId="144"/>
+    <tableColumn id="9" name="Damage" dataDxfId="143"/>
+    <tableColumn id="10" name="Cure" dataDxfId="142"/>
+    <tableColumn id="11" name="Time" dataDxfId="141"/>
+    <tableColumn id="13" name="Help" dataDxfId="140"/>
+    <tableColumn id="16" name="Rate" dataDxfId="139"/>
+    <tableColumn id="18" name="Atk" dataDxfId="138"/>
+    <tableColumn id="12" name="Modify" dataDxfId="137"/>
+    <tableColumn id="27" name="Sum" dataDxfId="136">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="144"/>
-    <tableColumn id="15" name="Target" dataDxfId="143"/>
-    <tableColumn id="25" name="Mark" dataDxfId="142"/>
-    <tableColumn id="22" name="Effect" dataDxfId="141"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="140"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="139"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="138"/>
-    <tableColumn id="26" name="JobId" dataDxfId="137"/>
-    <tableColumn id="19" name="Icon" dataDxfId="136"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="135"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="134"/>
+    <tableColumn id="6" name="Range" dataDxfId="135"/>
+    <tableColumn id="15" name="Target" dataDxfId="134"/>
+    <tableColumn id="25" name="Mark" dataDxfId="133"/>
+    <tableColumn id="22" name="Effect" dataDxfId="132"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="131"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="130"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="129"/>
+    <tableColumn id="26" name="JobId" dataDxfId="128"/>
+    <tableColumn id="19" name="Icon" dataDxfId="127"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="126"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="125"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AB11" totalsRowShown="0" headerRowDxfId="133" dataDxfId="132" tableBorderDxfId="131">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AB11" totalsRowShown="0" headerRowDxfId="124" dataDxfId="123" tableBorderDxfId="122">
   <autoFilter ref="A3:AB11"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="130"/>
-    <tableColumn id="2" name="Name" dataDxfId="129"/>
-    <tableColumn id="20" name="Ename" dataDxfId="128"/>
-    <tableColumn id="21" name="Remark" dataDxfId="127"/>
-    <tableColumn id="3" name="Star" dataDxfId="126"/>
-    <tableColumn id="4" name="Type" dataDxfId="125"/>
-    <tableColumn id="5" name="Attr" dataDxfId="124"/>
-    <tableColumn id="8" name="Quality" dataDxfId="123">
+    <tableColumn id="1" name="Id" dataDxfId="121"/>
+    <tableColumn id="2" name="Name" dataDxfId="120"/>
+    <tableColumn id="20" name="Ename" dataDxfId="119"/>
+    <tableColumn id="21" name="Remark" dataDxfId="118"/>
+    <tableColumn id="3" name="Star" dataDxfId="117"/>
+    <tableColumn id="4" name="Type" dataDxfId="116"/>
+    <tableColumn id="5" name="Attr" dataDxfId="115"/>
+    <tableColumn id="8" name="Quality" dataDxfId="114">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="122"/>
-    <tableColumn id="9" name="Damage" dataDxfId="121"/>
-    <tableColumn id="10" name="Cure" dataDxfId="120"/>
-    <tableColumn id="11" name="Time" dataDxfId="119"/>
-    <tableColumn id="13" name="Help" dataDxfId="118"/>
-    <tableColumn id="16" name="Rate" dataDxfId="117"/>
-    <tableColumn id="18" name="Atk" dataDxfId="116"/>
-    <tableColumn id="12" name="Modify" dataDxfId="115"/>
-    <tableColumn id="27" name="Sum" dataDxfId="114">
+    <tableColumn id="7" name="Cost" dataDxfId="113"/>
+    <tableColumn id="9" name="Damage" dataDxfId="112"/>
+    <tableColumn id="10" name="Cure" dataDxfId="111"/>
+    <tableColumn id="11" name="Time" dataDxfId="110"/>
+    <tableColumn id="13" name="Help" dataDxfId="109"/>
+    <tableColumn id="16" name="Rate" dataDxfId="108"/>
+    <tableColumn id="18" name="Atk" dataDxfId="107"/>
+    <tableColumn id="12" name="Modify" dataDxfId="106"/>
+    <tableColumn id="27" name="Sum" dataDxfId="105">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="113"/>
-    <tableColumn id="15" name="Target" dataDxfId="112"/>
-    <tableColumn id="25" name="Mark" dataDxfId="111"/>
-    <tableColumn id="22" name="Effect" dataDxfId="110"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="109"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="108"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="107"/>
-    <tableColumn id="26" name="JobId" dataDxfId="106"/>
-    <tableColumn id="19" name="Icon" dataDxfId="105"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="104"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="103"/>
+    <tableColumn id="6" name="Range" dataDxfId="104"/>
+    <tableColumn id="15" name="Target" dataDxfId="103"/>
+    <tableColumn id="25" name="Mark" dataDxfId="102"/>
+    <tableColumn id="22" name="Effect" dataDxfId="101"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="100"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="99"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="98"/>
+    <tableColumn id="26" name="JobId" dataDxfId="97"/>
+    <tableColumn id="19" name="Icon" dataDxfId="96"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="95"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="94"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_35" displayName="表1_35" ref="A3:AB9" totalsRowShown="0" headerRowDxfId="102" tableBorderDxfId="101">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_35" displayName="表1_35" ref="A3:AB9" totalsRowShown="0" headerRowDxfId="93" tableBorderDxfId="92">
   <autoFilter ref="A3:AB9"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="100"/>
-    <tableColumn id="2" name="Name" dataDxfId="99"/>
-    <tableColumn id="20" name="Ename" dataDxfId="98"/>
-    <tableColumn id="21" name="Remark" dataDxfId="97"/>
-    <tableColumn id="3" name="Star" dataDxfId="96"/>
-    <tableColumn id="4" name="Type" dataDxfId="95"/>
-    <tableColumn id="5" name="Attr" dataDxfId="94"/>
-    <tableColumn id="8" name="Quality" dataDxfId="93">
+    <tableColumn id="1" name="Id" dataDxfId="91"/>
+    <tableColumn id="2" name="Name" dataDxfId="90"/>
+    <tableColumn id="20" name="Ename" dataDxfId="89"/>
+    <tableColumn id="21" name="Remark" dataDxfId="88"/>
+    <tableColumn id="3" name="Star" dataDxfId="87"/>
+    <tableColumn id="4" name="Type" dataDxfId="86"/>
+    <tableColumn id="5" name="Attr" dataDxfId="85"/>
+    <tableColumn id="8" name="Quality" dataDxfId="84">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="92"/>
-    <tableColumn id="9" name="Damage" dataDxfId="91"/>
-    <tableColumn id="10" name="Cure" dataDxfId="90"/>
-    <tableColumn id="11" name="Time" dataDxfId="89"/>
-    <tableColumn id="13" name="Help" dataDxfId="88"/>
-    <tableColumn id="16" name="Rate" dataDxfId="87"/>
-    <tableColumn id="18" name="Atk" dataDxfId="86"/>
-    <tableColumn id="12" name="Modify" dataDxfId="85"/>
-    <tableColumn id="27" name="Sum" dataDxfId="84">
+    <tableColumn id="7" name="Cost" dataDxfId="83"/>
+    <tableColumn id="9" name="Damage" dataDxfId="82"/>
+    <tableColumn id="10" name="Cure" dataDxfId="81"/>
+    <tableColumn id="11" name="Time" dataDxfId="80"/>
+    <tableColumn id="13" name="Help" dataDxfId="79"/>
+    <tableColumn id="16" name="Rate" dataDxfId="78"/>
+    <tableColumn id="18" name="Atk" dataDxfId="77"/>
+    <tableColumn id="12" name="Modify" dataDxfId="76"/>
+    <tableColumn id="27" name="Sum" dataDxfId="75">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="83"/>
-    <tableColumn id="15" name="Target" dataDxfId="82"/>
-    <tableColumn id="25" name="Mark" dataDxfId="81"/>
-    <tableColumn id="22" name="Effect" dataDxfId="80"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="79"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="78"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="77"/>
-    <tableColumn id="26" name="JobId" dataDxfId="76"/>
-    <tableColumn id="19" name="Icon" dataDxfId="75"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="74"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="73"/>
+    <tableColumn id="6" name="Range" dataDxfId="74"/>
+    <tableColumn id="15" name="Target" dataDxfId="73"/>
+    <tableColumn id="25" name="Mark" dataDxfId="72"/>
+    <tableColumn id="22" name="Effect" dataDxfId="71"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="70"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="69"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="68"/>
+    <tableColumn id="26" name="JobId" dataDxfId="67"/>
+    <tableColumn id="19" name="Icon" dataDxfId="66"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="65"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9065,7 +8998,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C128" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Z131" sqref="Z131"/>
+      <selection pane="bottomRight" activeCell="D129" sqref="D129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -20135,10 +20068,10 @@
         <v>53000126</v>
       </c>
       <c r="B129" s="22" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="C129" s="15" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="D129" s="25"/>
       <c r="E129" s="15">
@@ -20192,10 +20125,10 @@
         <v>100</v>
       </c>
       <c r="U129" s="11" t="s">
-        <v>848</v>
+        <v>858</v>
       </c>
       <c r="V129" s="1" t="s">
-        <v>849</v>
+        <v>860</v>
       </c>
       <c r="W129" s="1" t="s">
         <v>796</v>
@@ -20221,10 +20154,10 @@
         <v>53000127</v>
       </c>
       <c r="B130" s="22" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="C130" s="15" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="D130" s="25"/>
       <c r="E130" s="15">
@@ -20272,7 +20205,7 @@
         <v>15</v>
       </c>
       <c r="S130" s="7" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="T130">
         <v>103</v>
@@ -20281,7 +20214,7 @@
         <v>825</v>
       </c>
       <c r="V130" s="1" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="W130" s="1" t="s">
         <v>796</v>
@@ -20307,41 +20240,41 @@
         <v>53000128</v>
       </c>
       <c r="B131" s="22" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="D131" s="25" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="E131" s="15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F131" s="15">
         <v>201</v>
       </c>
       <c r="G131" s="15">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H131" s="43">
         <f t="shared" ref="H131" si="40">IF(AND(Q131&gt;=13,Q131&lt;=16),5,IF(AND(Q131&gt;=9,Q131&lt;=12),4,IF(AND(Q131&gt;=5,Q131&lt;=8),3,IF(AND(Q131&gt;=1,Q131&lt;=4),2,IF(AND(Q131&gt;=-3,Q131&lt;=0),1,IF(AND(Q131&gt;=-5,Q131&lt;=-4),0,6))))))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I131" s="15">
+        <v>1</v>
+      </c>
+      <c r="J131" s="15">
+        <v>0</v>
+      </c>
+      <c r="K131" s="15">
+        <v>0</v>
+      </c>
+      <c r="L131" s="15">
+        <v>0</v>
+      </c>
+      <c r="M131" s="15">
         <v>4</v>
-      </c>
-      <c r="J131" s="15">
-        <v>60</v>
-      </c>
-      <c r="K131" s="15">
-        <v>0</v>
-      </c>
-      <c r="L131" s="15">
-        <v>0</v>
-      </c>
-      <c r="M131" s="15">
-        <v>0</v>
       </c>
       <c r="N131" s="15">
         <v>0</v>
@@ -20354,22 +20287,22 @@
       </c>
       <c r="Q131" s="43">
         <f t="shared" ref="Q131" si="41">T131-100+P131</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="R131" s="15">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="S131" s="7" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
       <c r="T131">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="U131" s="11" t="s">
-        <v>825</v>
+        <v>859</v>
       </c>
       <c r="V131" s="1" t="s">
-        <v>856</v>
+        <v>861</v>
       </c>
       <c r="W131" s="1" t="s">
         <v>796</v>
@@ -20396,124 +20329,124 @@
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I38:I68 I17:I35 I4:I15 I70:I122">
-    <cfRule type="cellIs" dxfId="72" priority="65" operator="notEqual">
+    <cfRule type="cellIs" dxfId="63" priority="65" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J17:N35 J4:N15 J38:N68 P38:Q68 P5:Q15 P17:Q35 P4 P70:Q122 J70:N122">
-    <cfRule type="cellIs" dxfId="71" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="64" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I69">
-    <cfRule type="cellIs" dxfId="70" priority="29" operator="notEqual">
+    <cfRule type="cellIs" dxfId="61" priority="29" operator="notEqual">
       <formula>$E69</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J69:N69 P69:Q69">
-    <cfRule type="cellIs" dxfId="69" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="28" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36">
-    <cfRule type="cellIs" dxfId="68" priority="27" operator="notEqual">
+    <cfRule type="cellIs" dxfId="59" priority="27" operator="notEqual">
       <formula>$E36</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J36:N36 P36:Q36">
-    <cfRule type="cellIs" dxfId="67" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="26" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37">
-    <cfRule type="cellIs" dxfId="66" priority="25" operator="notEqual">
+    <cfRule type="cellIs" dxfId="57" priority="25" operator="notEqual">
       <formula>$E37</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J37:N37 P37:Q37">
-    <cfRule type="cellIs" dxfId="65" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="24" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H15 H17:H122">
-    <cfRule type="cellIs" dxfId="64" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="20" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="21" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="22" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="23" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="52" priority="23" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="cellIs" dxfId="60" priority="17" operator="notEqual">
+    <cfRule type="cellIs" dxfId="51" priority="17" operator="notEqual">
       <formula>$E16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:N16 P16:Q16">
-    <cfRule type="cellIs" dxfId="59" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="16" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="cellIs" dxfId="58" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="12" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="13" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="14" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="15" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="46" priority="15" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D122 D132:D1048576">
-    <cfRule type="containsText" dxfId="54" priority="11" operator="containsText" text="未完成">
+    <cfRule type="containsText" dxfId="45" priority="11" operator="containsText" text="未完成">
       <formula>NOT(ISERROR(SEARCH("未完成",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:O131">
-    <cfRule type="cellIs" dxfId="53" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I123:I131">
-    <cfRule type="cellIs" dxfId="52" priority="9" operator="notEqual">
+    <cfRule type="cellIs" dxfId="43" priority="9" operator="notEqual">
       <formula>$E123</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J123:N131 P123:Q131">
-    <cfRule type="cellIs" dxfId="51" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H123:H131">
-    <cfRule type="cellIs" dxfId="50" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="5" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="6" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="7" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="38" priority="7" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O123:O131">
-    <cfRule type="cellIs" dxfId="46" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123:D131">
-    <cfRule type="containsText" dxfId="45" priority="1" operator="containsText" text="未完成">
+    <cfRule type="containsText" dxfId="36" priority="1" operator="containsText" text="未完成">
       <formula>NOT(ISERROR(SEARCH("未完成",D123)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21458,110 +21391,110 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="J4:Q11">
-    <cfRule type="cellIs" dxfId="44" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="40" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:Q8">
-    <cfRule type="cellIs" dxfId="43" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="36" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:Q4 O4:O11">
-    <cfRule type="cellIs" dxfId="42" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="35" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="41" priority="34" operator="notEqual">
+    <cfRule type="cellIs" dxfId="32" priority="34" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:Q4 O4:O11">
-    <cfRule type="cellIs" dxfId="40" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="33" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="39" priority="32" operator="notEqual">
+    <cfRule type="cellIs" dxfId="30" priority="32" operator="notEqual">
       <formula>$E5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:Q5">
-    <cfRule type="cellIs" dxfId="38" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" dxfId="37" priority="30" operator="notEqual">
+    <cfRule type="cellIs" dxfId="28" priority="30" operator="notEqual">
       <formula>$E6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:Q6">
-    <cfRule type="cellIs" dxfId="36" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="29" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="35" priority="28" operator="notEqual">
+    <cfRule type="cellIs" dxfId="26" priority="28" operator="notEqual">
       <formula>$E7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:Q7">
-    <cfRule type="cellIs" dxfId="34" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="33" priority="26" operator="notEqual">
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="notEqual">
       <formula>$E8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:Q8">
-    <cfRule type="cellIs" dxfId="32" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I11">
-    <cfRule type="cellIs" dxfId="31" priority="24" operator="notEqual">
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="notEqual">
       <formula>$E9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:Q11">
-    <cfRule type="cellIs" dxfId="30" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H11">
-    <cfRule type="cellIs" dxfId="29" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="17" priority="9" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="25" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10:L11">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22371,50 +22304,50 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I4:I9">
-    <cfRule type="cellIs" dxfId="20" priority="12" operator="notEqual">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:Q7 O4:O9">
-    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:Q9">
-    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:Q8">
-    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H9">
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
finish some new cards
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
   </bookViews>
   <sheets>
     <sheet name="标准" sheetId="1" r:id="rId1"/>
@@ -636,7 +636,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="880">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1321" uniqueCount="894">
   <si>
     <t>慈悲</t>
   </si>
@@ -3599,10 +3599,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>t.Atk.Source+=s.Atk;if(t.HpRate&gt;70)t.Def.Source-=3;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>猛击</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3831,6 +3827,66 @@
   </si>
   <si>
     <t>bluewing</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>持盾冲锋</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shield Rush</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>大反击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Counter Strike</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>群体，直伤</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>状态</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NEW</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse)){im.OnMagicDamage(null, s.Damage,s.Attr);}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对一行敌方单位造成{0}点魔法伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hit1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>t.Atk.Source+=s.Atk;if(t.Hp&gt;s.Damage)t.Def.Source-=3;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>t.Atk.Source+=s.Atk;if(t.HpRate&lt;50)t.Def.Source+=4;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>yellowflash</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>UFS</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>永久提高友方{5}点攻击，如果目标生命低于50%，则永久提高目标4点防御</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -4836,7 +4892,37 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="156">
+  <dxfs count="159">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -8643,132 +8729,132 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AB133" totalsRowShown="0" headerRowDxfId="155" dataDxfId="154" tableBorderDxfId="153">
-  <autoFilter ref="A3:AB133"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AB135" totalsRowShown="0" headerRowDxfId="158" dataDxfId="157" tableBorderDxfId="156">
+  <autoFilter ref="A3:AB135"/>
   <sortState ref="A4:AB113">
     <sortCondition ref="A3:A113"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="152"/>
-    <tableColumn id="2" name="Name" dataDxfId="151"/>
-    <tableColumn id="20" name="Ename" dataDxfId="150"/>
-    <tableColumn id="21" name="Remark" dataDxfId="149"/>
-    <tableColumn id="3" name="Star" dataDxfId="148"/>
-    <tableColumn id="4" name="Type" dataDxfId="147"/>
-    <tableColumn id="5" name="Attr" dataDxfId="146"/>
-    <tableColumn id="8" name="Quality" dataDxfId="145">
+    <tableColumn id="1" name="Id" dataDxfId="155"/>
+    <tableColumn id="2" name="Name" dataDxfId="154"/>
+    <tableColumn id="20" name="Ename" dataDxfId="153"/>
+    <tableColumn id="21" name="Remark" dataDxfId="152"/>
+    <tableColumn id="3" name="Star" dataDxfId="151"/>
+    <tableColumn id="4" name="Type" dataDxfId="150"/>
+    <tableColumn id="5" name="Attr" dataDxfId="149"/>
+    <tableColumn id="8" name="Quality" dataDxfId="148">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="144"/>
-    <tableColumn id="9" name="Damage" dataDxfId="143"/>
-    <tableColumn id="10" name="Cure" dataDxfId="142"/>
-    <tableColumn id="11" name="Time" dataDxfId="141"/>
-    <tableColumn id="13" name="Help" dataDxfId="140"/>
-    <tableColumn id="16" name="Rate" dataDxfId="139"/>
-    <tableColumn id="18" name="Atk" dataDxfId="138"/>
-    <tableColumn id="12" name="Modify" dataDxfId="137"/>
-    <tableColumn id="27" name="Sum" dataDxfId="136">
+    <tableColumn id="7" name="Cost" dataDxfId="147"/>
+    <tableColumn id="9" name="Damage" dataDxfId="146"/>
+    <tableColumn id="10" name="Cure" dataDxfId="145"/>
+    <tableColumn id="11" name="Time" dataDxfId="144"/>
+    <tableColumn id="13" name="Help" dataDxfId="143"/>
+    <tableColumn id="16" name="Rate" dataDxfId="142"/>
+    <tableColumn id="18" name="Atk" dataDxfId="141"/>
+    <tableColumn id="12" name="Modify" dataDxfId="140"/>
+    <tableColumn id="27" name="Sum" dataDxfId="139">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="135"/>
-    <tableColumn id="15" name="Target" dataDxfId="134"/>
-    <tableColumn id="25" name="Mark" dataDxfId="133"/>
-    <tableColumn id="22" name="Effect" dataDxfId="132"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="131"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="130"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="129"/>
-    <tableColumn id="26" name="JobId" dataDxfId="128"/>
-    <tableColumn id="19" name="Icon" dataDxfId="127"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="126"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="125"/>
+    <tableColumn id="6" name="Range" dataDxfId="138"/>
+    <tableColumn id="15" name="Target" dataDxfId="137"/>
+    <tableColumn id="25" name="Mark" dataDxfId="136"/>
+    <tableColumn id="22" name="Effect" dataDxfId="135"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="134"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="133"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="132"/>
+    <tableColumn id="26" name="JobId" dataDxfId="131"/>
+    <tableColumn id="19" name="Icon" dataDxfId="130"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="129"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="128"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AB12" totalsRowShown="0" headerRowDxfId="124" dataDxfId="123" tableBorderDxfId="122">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AB12" totalsRowShown="0" headerRowDxfId="127" dataDxfId="126" tableBorderDxfId="125">
   <autoFilter ref="A3:AB12"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="121"/>
-    <tableColumn id="2" name="Name" dataDxfId="120"/>
-    <tableColumn id="20" name="Ename" dataDxfId="119"/>
-    <tableColumn id="21" name="Remark" dataDxfId="118"/>
-    <tableColumn id="3" name="Star" dataDxfId="117"/>
-    <tableColumn id="4" name="Type" dataDxfId="116"/>
-    <tableColumn id="5" name="Attr" dataDxfId="115"/>
-    <tableColumn id="8" name="Quality" dataDxfId="114">
+    <tableColumn id="1" name="Id" dataDxfId="124"/>
+    <tableColumn id="2" name="Name" dataDxfId="123"/>
+    <tableColumn id="20" name="Ename" dataDxfId="122"/>
+    <tableColumn id="21" name="Remark" dataDxfId="121"/>
+    <tableColumn id="3" name="Star" dataDxfId="120"/>
+    <tableColumn id="4" name="Type" dataDxfId="119"/>
+    <tableColumn id="5" name="Attr" dataDxfId="118"/>
+    <tableColumn id="8" name="Quality" dataDxfId="117">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="113"/>
-    <tableColumn id="9" name="Damage" dataDxfId="112"/>
-    <tableColumn id="10" name="Cure" dataDxfId="111"/>
-    <tableColumn id="11" name="Time" dataDxfId="110"/>
-    <tableColumn id="13" name="Help" dataDxfId="109"/>
-    <tableColumn id="16" name="Rate" dataDxfId="108"/>
-    <tableColumn id="18" name="Atk" dataDxfId="107"/>
-    <tableColumn id="12" name="Modify" dataDxfId="106"/>
-    <tableColumn id="27" name="Sum" dataDxfId="105">
+    <tableColumn id="7" name="Cost" dataDxfId="116"/>
+    <tableColumn id="9" name="Damage" dataDxfId="115"/>
+    <tableColumn id="10" name="Cure" dataDxfId="114"/>
+    <tableColumn id="11" name="Time" dataDxfId="113"/>
+    <tableColumn id="13" name="Help" dataDxfId="112"/>
+    <tableColumn id="16" name="Rate" dataDxfId="111"/>
+    <tableColumn id="18" name="Atk" dataDxfId="110"/>
+    <tableColumn id="12" name="Modify" dataDxfId="109"/>
+    <tableColumn id="27" name="Sum" dataDxfId="108">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="104"/>
-    <tableColumn id="15" name="Target" dataDxfId="103"/>
-    <tableColumn id="25" name="Mark" dataDxfId="102"/>
-    <tableColumn id="22" name="Effect" dataDxfId="101"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="100"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="99"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="98"/>
-    <tableColumn id="26" name="JobId" dataDxfId="97"/>
-    <tableColumn id="19" name="Icon" dataDxfId="96"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="95"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="94"/>
+    <tableColumn id="6" name="Range" dataDxfId="107"/>
+    <tableColumn id="15" name="Target" dataDxfId="106"/>
+    <tableColumn id="25" name="Mark" dataDxfId="105"/>
+    <tableColumn id="22" name="Effect" dataDxfId="104"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="103"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="102"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="101"/>
+    <tableColumn id="26" name="JobId" dataDxfId="100"/>
+    <tableColumn id="19" name="Icon" dataDxfId="99"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="98"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="97"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_35" displayName="表1_35" ref="A3:AB9" totalsRowShown="0" headerRowDxfId="93" tableBorderDxfId="92">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_35" displayName="表1_35" ref="A3:AB9" totalsRowShown="0" headerRowDxfId="96" tableBorderDxfId="95">
   <autoFilter ref="A3:AB9"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="91"/>
-    <tableColumn id="2" name="Name" dataDxfId="90"/>
-    <tableColumn id="20" name="Ename" dataDxfId="89"/>
-    <tableColumn id="21" name="Remark" dataDxfId="88"/>
-    <tableColumn id="3" name="Star" dataDxfId="87"/>
-    <tableColumn id="4" name="Type" dataDxfId="86"/>
-    <tableColumn id="5" name="Attr" dataDxfId="85"/>
-    <tableColumn id="8" name="Quality" dataDxfId="84">
+    <tableColumn id="1" name="Id" dataDxfId="94"/>
+    <tableColumn id="2" name="Name" dataDxfId="93"/>
+    <tableColumn id="20" name="Ename" dataDxfId="92"/>
+    <tableColumn id="21" name="Remark" dataDxfId="91"/>
+    <tableColumn id="3" name="Star" dataDxfId="90"/>
+    <tableColumn id="4" name="Type" dataDxfId="89"/>
+    <tableColumn id="5" name="Attr" dataDxfId="88"/>
+    <tableColumn id="8" name="Quality" dataDxfId="87">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="83"/>
-    <tableColumn id="9" name="Damage" dataDxfId="82"/>
-    <tableColumn id="10" name="Cure" dataDxfId="81"/>
-    <tableColumn id="11" name="Time" dataDxfId="80"/>
-    <tableColumn id="13" name="Help" dataDxfId="79"/>
-    <tableColumn id="16" name="Rate" dataDxfId="78"/>
-    <tableColumn id="18" name="Atk" dataDxfId="77"/>
-    <tableColumn id="12" name="Modify" dataDxfId="76"/>
-    <tableColumn id="27" name="Sum" dataDxfId="75">
+    <tableColumn id="7" name="Cost" dataDxfId="86"/>
+    <tableColumn id="9" name="Damage" dataDxfId="85"/>
+    <tableColumn id="10" name="Cure" dataDxfId="84"/>
+    <tableColumn id="11" name="Time" dataDxfId="83"/>
+    <tableColumn id="13" name="Help" dataDxfId="82"/>
+    <tableColumn id="16" name="Rate" dataDxfId="81"/>
+    <tableColumn id="18" name="Atk" dataDxfId="80"/>
+    <tableColumn id="12" name="Modify" dataDxfId="79"/>
+    <tableColumn id="27" name="Sum" dataDxfId="78">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="74"/>
-    <tableColumn id="15" name="Target" dataDxfId="73"/>
-    <tableColumn id="25" name="Mark" dataDxfId="72"/>
-    <tableColumn id="22" name="Effect" dataDxfId="71"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="70"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="69"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="68"/>
-    <tableColumn id="26" name="JobId" dataDxfId="67"/>
-    <tableColumn id="19" name="Icon" dataDxfId="66"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="65"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="64"/>
+    <tableColumn id="6" name="Range" dataDxfId="77"/>
+    <tableColumn id="15" name="Target" dataDxfId="76"/>
+    <tableColumn id="25" name="Mark" dataDxfId="75"/>
+    <tableColumn id="22" name="Effect" dataDxfId="74"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="73"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="72"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="71"/>
+    <tableColumn id="26" name="JobId" dataDxfId="70"/>
+    <tableColumn id="19" name="Icon" dataDxfId="69"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="68"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9061,13 +9147,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB133"/>
+  <dimension ref="A1:AB135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C130" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C132" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="V132" sqref="V132"/>
+      <selection pane="bottomRight" activeCell="V134" sqref="V134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -9666,10 +9752,10 @@
         <v>100</v>
       </c>
       <c r="U7" s="11" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="V7" s="7" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="W7" s="1" t="s">
         <v>9</v>
@@ -11206,10 +11292,10 @@
         <v>107</v>
       </c>
       <c r="U25" s="11" t="s">
+        <v>829</v>
+      </c>
+      <c r="V25" s="7" t="s">
         <v>830</v>
-      </c>
-      <c r="V25" s="7" t="s">
-        <v>831</v>
       </c>
       <c r="W25" s="1" t="s">
         <v>29</v>
@@ -12320,7 +12406,7 @@
         <v>100</v>
       </c>
       <c r="U38" s="11" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="V38" s="7" t="s">
         <v>630</v>
@@ -12525,7 +12611,7 @@
         <v>236</v>
       </c>
       <c r="D41" s="25" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="E41" s="1">
         <v>2</v>
@@ -12572,16 +12658,16 @@
         <v>12</v>
       </c>
       <c r="S41" s="1" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="T41">
         <v>100</v>
       </c>
       <c r="U41" s="11" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="V41" s="7" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="W41" s="1" t="s">
         <v>55</v>
@@ -13185,7 +13271,7 @@
         <v>700</v>
       </c>
       <c r="V48" s="1" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="W48" s="1" t="s">
         <v>322</v>
@@ -13784,16 +13870,16 @@
         <v>0</v>
       </c>
       <c r="S55" s="1" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="T55">
         <v>95</v>
       </c>
       <c r="U55" s="11" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="V55" s="7" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="W55" s="1" t="s">
         <v>624</v>
@@ -14300,16 +14386,16 @@
         <v>0</v>
       </c>
       <c r="S61" s="1" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="T61">
         <v>100</v>
       </c>
       <c r="U61" s="11" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="V61" s="7" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="W61" s="1" t="s">
         <v>15</v>
@@ -15340,7 +15426,7 @@
         <v>100</v>
       </c>
       <c r="U73" s="11" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="V73" s="7" t="s">
         <v>563</v>
@@ -19932,7 +20018,7 @@
         <v>100</v>
       </c>
       <c r="U126" s="11" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="V126" s="1" t="s">
         <v>814</v>
@@ -20020,7 +20106,7 @@
         <v>101</v>
       </c>
       <c r="U127" s="11" t="s">
-        <v>821</v>
+        <v>889</v>
       </c>
       <c r="V127" s="1" t="s">
         <v>820</v>
@@ -20049,13 +20135,13 @@
         <v>53000125</v>
       </c>
       <c r="B128" s="22" t="s">
+        <v>821</v>
+      </c>
+      <c r="C128" s="15" t="s">
         <v>822</v>
       </c>
-      <c r="C128" s="15" t="s">
+      <c r="D128" s="25" t="s">
         <v>823</v>
-      </c>
-      <c r="D128" s="25" t="s">
-        <v>824</v>
       </c>
       <c r="E128" s="15">
         <v>2</v>
@@ -20102,22 +20188,22 @@
         <v>0</v>
       </c>
       <c r="S128" s="7" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="T128">
         <v>100</v>
       </c>
       <c r="U128" s="11" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="V128" s="1" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="W128" s="15" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="X128" s="15" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="Y128" s="1">
         <v>11000002</v>
@@ -20137,10 +20223,10 @@
         <v>53000126</v>
       </c>
       <c r="B129" s="22" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="C129" s="15" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="D129" s="25"/>
       <c r="E129" s="15">
@@ -20188,16 +20274,16 @@
         <v>0</v>
       </c>
       <c r="S129" s="7" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="T129">
         <v>100</v>
       </c>
       <c r="U129" s="11" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="V129" s="1" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="W129" s="1" t="s">
         <v>782</v>
@@ -20223,10 +20309,10 @@
         <v>53000127</v>
       </c>
       <c r="B130" s="22" t="s">
+        <v>833</v>
+      </c>
+      <c r="C130" s="15" t="s">
         <v>834</v>
-      </c>
-      <c r="C130" s="15" t="s">
-        <v>835</v>
       </c>
       <c r="D130" s="25"/>
       <c r="E130" s="15">
@@ -20274,7 +20360,7 @@
         <v>15</v>
       </c>
       <c r="S130" s="7" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="T130">
         <v>103</v>
@@ -20283,7 +20369,7 @@
         <v>810</v>
       </c>
       <c r="V130" s="1" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="W130" s="1" t="s">
         <v>782</v>
@@ -20309,13 +20395,13 @@
         <v>53000128</v>
       </c>
       <c r="B131" s="22" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="D131" s="25" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="E131" s="15">
         <v>1</v>
@@ -20362,16 +20448,16 @@
         <v>25</v>
       </c>
       <c r="S131" s="7" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="T131">
         <v>100</v>
       </c>
       <c r="U131" s="11" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="V131" s="1" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="W131" s="1" t="s">
         <v>782</v>
@@ -20397,13 +20483,13 @@
         <v>53000129</v>
       </c>
       <c r="B132" s="22" t="s">
+        <v>862</v>
+      </c>
+      <c r="C132" s="15" t="s">
+        <v>861</v>
+      </c>
+      <c r="D132" s="25" t="s">
         <v>863</v>
-      </c>
-      <c r="C132" s="15" t="s">
-        <v>862</v>
-      </c>
-      <c r="D132" s="25" t="s">
-        <v>864</v>
       </c>
       <c r="E132" s="15">
         <v>3</v>
@@ -20450,22 +20536,22 @@
         <v>0</v>
       </c>
       <c r="S132" s="7" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="T132">
         <v>103</v>
       </c>
       <c r="U132" s="11" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="V132" s="1" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="W132" s="1" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="X132" s="1" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="Y132" s="1">
         <v>11000002</v>
@@ -20485,13 +20571,13 @@
         <v>53000130</v>
       </c>
       <c r="B133" s="22" t="s">
+        <v>872</v>
+      </c>
+      <c r="C133" s="15" t="s">
         <v>873</v>
       </c>
-      <c r="C133" s="15" t="s">
-        <v>874</v>
-      </c>
       <c r="D133" s="25" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="E133" s="15">
         <v>5</v>
@@ -20538,22 +20624,22 @@
         <v>25</v>
       </c>
       <c r="S133" s="7" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="T133">
         <v>107</v>
       </c>
       <c r="U133" s="11" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="V133" s="1" t="s">
+        <v>877</v>
+      </c>
+      <c r="W133" s="1" t="s">
         <v>878</v>
       </c>
-      <c r="W133" s="1" t="s">
-        <v>879</v>
-      </c>
       <c r="X133" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="Y133" s="1">
         <v>11000002</v>
@@ -20565,6 +20651,182 @@
         <v>0</v>
       </c>
       <c r="AB133" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:28" ht="72">
+      <c r="A134">
+        <v>53000131</v>
+      </c>
+      <c r="B134" s="22" t="s">
+        <v>879</v>
+      </c>
+      <c r="C134" s="15" t="s">
+        <v>880</v>
+      </c>
+      <c r="D134" s="25" t="s">
+        <v>883</v>
+      </c>
+      <c r="E134" s="15">
+        <v>2</v>
+      </c>
+      <c r="F134" s="15">
+        <v>201</v>
+      </c>
+      <c r="G134" s="15">
+        <v>0</v>
+      </c>
+      <c r="H134" s="43">
+        <f t="shared" ref="H134:H135" si="46">IF(AND(Q134&gt;=13,Q134&lt;=16),5,IF(AND(Q134&gt;=9,Q134&lt;=12),4,IF(AND(Q134&gt;=5,Q134&lt;=8),3,IF(AND(Q134&gt;=1,Q134&lt;=4),2,IF(AND(Q134&gt;=-3,Q134&lt;=0),1,IF(AND(Q134&gt;=-5,Q134&lt;=-4),0,6))))))</f>
+        <v>1</v>
+      </c>
+      <c r="I134" s="15">
+        <v>2</v>
+      </c>
+      <c r="J134" s="15">
+        <v>40</v>
+      </c>
+      <c r="K134" s="15">
+        <v>0</v>
+      </c>
+      <c r="L134" s="15">
+        <v>1</v>
+      </c>
+      <c r="M134" s="15">
+        <v>0</v>
+      </c>
+      <c r="N134" s="15">
+        <v>0</v>
+      </c>
+      <c r="O134" s="15">
+        <v>0</v>
+      </c>
+      <c r="P134" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q134" s="43">
+        <f t="shared" ref="Q134:Q135" si="47">T134-100+P134</f>
+        <v>0</v>
+      </c>
+      <c r="R134" s="15">
+        <v>30</v>
+      </c>
+      <c r="S134" s="7" t="s">
+        <v>885</v>
+      </c>
+      <c r="T134">
+        <v>100</v>
+      </c>
+      <c r="U134" s="11" t="s">
+        <v>886</v>
+      </c>
+      <c r="V134" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="W134" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="X134" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="Y134" s="1">
+        <v>11000002</v>
+      </c>
+      <c r="Z134" s="15">
+        <v>131</v>
+      </c>
+      <c r="AA134" s="27">
+        <v>0</v>
+      </c>
+      <c r="AB134" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:28" ht="36">
+      <c r="A135">
+        <v>53000132</v>
+      </c>
+      <c r="B135" s="22" t="s">
+        <v>881</v>
+      </c>
+      <c r="C135" s="15" t="s">
+        <v>882</v>
+      </c>
+      <c r="D135" s="25" t="s">
+        <v>884</v>
+      </c>
+      <c r="E135" s="15">
+        <v>3</v>
+      </c>
+      <c r="F135" s="15">
+        <v>201</v>
+      </c>
+      <c r="G135" s="15">
+        <v>0</v>
+      </c>
+      <c r="H135" s="43">
+        <f t="shared" si="46"/>
+        <v>2</v>
+      </c>
+      <c r="I135" s="15">
+        <v>3</v>
+      </c>
+      <c r="J135" s="15">
+        <v>0</v>
+      </c>
+      <c r="K135" s="15">
+        <v>0</v>
+      </c>
+      <c r="L135" s="15">
+        <v>0</v>
+      </c>
+      <c r="M135" s="15">
+        <v>0</v>
+      </c>
+      <c r="N135" s="15">
+        <v>0</v>
+      </c>
+      <c r="O135" s="15">
+        <v>200</v>
+      </c>
+      <c r="P135" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q135" s="43">
+        <f t="shared" si="47"/>
+        <v>2</v>
+      </c>
+      <c r="R135" s="15">
+        <v>0</v>
+      </c>
+      <c r="S135" s="7" t="s">
+        <v>892</v>
+      </c>
+      <c r="T135">
+        <v>102</v>
+      </c>
+      <c r="U135" s="11" t="s">
+        <v>890</v>
+      </c>
+      <c r="V135" s="1" t="s">
+        <v>893</v>
+      </c>
+      <c r="W135" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="X135" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="Y135" s="1">
+        <v>11000002</v>
+      </c>
+      <c r="Z135" s="15">
+        <v>132</v>
+      </c>
+      <c r="AA135" s="27">
+        <v>0</v>
+      </c>
+      <c r="AB135" s="25">
         <v>1</v>
       </c>
     </row>
@@ -20574,125 +20836,140 @@
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I38:I68 I17:I35 I4:I15 I70:I122">
-    <cfRule type="cellIs" dxfId="63" priority="65" operator="notEqual">
+    <cfRule type="cellIs" dxfId="66" priority="68" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J17:N35 J4:N15 J38:N68 P38:Q68 P5:Q15 P17:Q35 P4 P70:Q122 J70:N122">
-    <cfRule type="cellIs" dxfId="62" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="67" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I69">
-    <cfRule type="cellIs" dxfId="61" priority="29" operator="notEqual">
+    <cfRule type="cellIs" dxfId="64" priority="32" operator="notEqual">
       <formula>$E69</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J69:N69 P69:Q69">
-    <cfRule type="cellIs" dxfId="60" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="31" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36">
-    <cfRule type="cellIs" dxfId="59" priority="27" operator="notEqual">
+    <cfRule type="cellIs" dxfId="62" priority="30" operator="notEqual">
       <formula>$E36</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J36:N36 P36:Q36">
-    <cfRule type="cellIs" dxfId="58" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="29" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37">
-    <cfRule type="cellIs" dxfId="57" priority="25" operator="notEqual">
+    <cfRule type="cellIs" dxfId="60" priority="28" operator="notEqual">
       <formula>$E37</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J37:N37 P37:Q37">
-    <cfRule type="cellIs" dxfId="56" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="27" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H15 H17:H122">
-    <cfRule type="cellIs" dxfId="55" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="23" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="24" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="25" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="23" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="55" priority="26" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="cellIs" dxfId="51" priority="17" operator="notEqual">
+    <cfRule type="cellIs" dxfId="54" priority="20" operator="notEqual">
       <formula>$E16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:N16 P16:Q16">
-    <cfRule type="cellIs" dxfId="50" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="19" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="cellIs" dxfId="49" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="15" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="16" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="17" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="15" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="49" priority="18" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D122 D134:D1048576">
-    <cfRule type="containsText" dxfId="45" priority="11" operator="containsText" text="未完成">
+  <conditionalFormatting sqref="D1:D122 D136:D1048576">
+    <cfRule type="containsText" dxfId="48" priority="14" operator="containsText" text="未完成">
       <formula>NOT(ISERROR(SEARCH("未完成",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O4:O133">
-    <cfRule type="cellIs" dxfId="44" priority="10" operator="equal">
+  <conditionalFormatting sqref="O4:O134">
+    <cfRule type="cellIs" dxfId="47" priority="13" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I123:I133">
-    <cfRule type="cellIs" dxfId="43" priority="9" operator="notEqual">
+  <conditionalFormatting sqref="I123:I135">
+    <cfRule type="cellIs" dxfId="46" priority="12" operator="notEqual">
       <formula>$E123</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J123:N133 P123:Q133">
-    <cfRule type="cellIs" dxfId="42" priority="8" operator="equal">
+  <conditionalFormatting sqref="J123:N134 P123:Q134">
+    <cfRule type="cellIs" dxfId="45" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H123:H133">
-    <cfRule type="cellIs" dxfId="41" priority="4" operator="equal">
+  <conditionalFormatting sqref="H123:H135">
+    <cfRule type="cellIs" dxfId="44" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="8" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="9" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="7" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="41" priority="10" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O123:O133">
-    <cfRule type="cellIs" dxfId="37" priority="2" operator="equal">
+  <conditionalFormatting sqref="O123:O134">
+    <cfRule type="cellIs" dxfId="40" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D123:D133">
-    <cfRule type="containsText" dxfId="36" priority="1" operator="containsText" text="未完成">
+  <conditionalFormatting sqref="D123:D135">
+    <cfRule type="containsText" dxfId="39" priority="4" operator="containsText" text="未完成">
       <formula>NOT(ISERROR(SEARCH("未完成",D123)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O135">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J135:N135 P135:Q135">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O135">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21207,16 +21484,16 @@
         <v>0</v>
       </c>
       <c r="S6" s="15" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="T6" s="1">
         <v>-1</v>
       </c>
       <c r="U6" s="11" t="s">
+        <v>859</v>
+      </c>
+      <c r="V6" s="7" t="s">
         <v>860</v>
-      </c>
-      <c r="V6" s="7" t="s">
-        <v>861</v>
       </c>
       <c r="W6" s="15" t="s">
         <v>365</v>
@@ -21638,7 +21915,7 @@
         <v>53100008</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="34"/>
@@ -21687,16 +21964,16 @@
         <v>0</v>
       </c>
       <c r="S12" s="15" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="T12" s="1">
         <v>-1</v>
       </c>
       <c r="U12" s="11" t="s">
+        <v>847</v>
+      </c>
+      <c r="V12" s="7" t="s">
         <v>848</v>
-      </c>
-      <c r="V12" s="7" t="s">
-        <v>849</v>
       </c>
       <c r="W12" s="15" t="s">
         <v>2</v>
@@ -21716,110 +21993,110 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="J4:Q12">
-    <cfRule type="cellIs" dxfId="35" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:Q8">
-    <cfRule type="cellIs" dxfId="34" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="36" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:Q4 O4:O12">
-    <cfRule type="cellIs" dxfId="33" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="35" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="32" priority="34" operator="notEqual">
+    <cfRule type="cellIs" dxfId="35" priority="34" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:Q4 O4:O12">
-    <cfRule type="cellIs" dxfId="31" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="33" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="30" priority="32" operator="notEqual">
+    <cfRule type="cellIs" dxfId="33" priority="32" operator="notEqual">
       <formula>$E5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:Q5">
-    <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="31" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" dxfId="28" priority="30" operator="notEqual">
+    <cfRule type="cellIs" dxfId="31" priority="30" operator="notEqual">
       <formula>$E6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:Q6">
-    <cfRule type="cellIs" dxfId="27" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="29" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="26" priority="28" operator="notEqual">
+    <cfRule type="cellIs" dxfId="29" priority="28" operator="notEqual">
       <formula>$E7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:Q7">
-    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="27" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="24" priority="26" operator="notEqual">
+    <cfRule type="cellIs" dxfId="27" priority="26" operator="notEqual">
       <formula>$E8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:Q8">
-    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I12">
-    <cfRule type="cellIs" dxfId="22" priority="24" operator="notEqual">
+    <cfRule type="cellIs" dxfId="25" priority="24" operator="notEqual">
       <formula>$E9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:Q12">
-    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="23" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H12">
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="7" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="20" priority="9" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10:L12">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22629,50 +22906,50 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I4:I9">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="notEqual">
+    <cfRule type="cellIs" dxfId="14" priority="12" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:Q7 O4:O9">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:Q9">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:Q8">
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H9">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
now trap must would be triggered, and part of mana will be substruct when triggered
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17766"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="标准" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="~评分" sheetId="2" r:id="rId4"/>
     <sheet name="~类型统计" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -3823,30 +3823,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>陷阱：对方召唤时，冰冻目标5回合。触发几率{4:0.0}%</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>陷阱：对方召唤时，对目标造成{0}点魔法伤害。触发几率{4:0.0}%</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>陷阱：对方使用的卡牌时，额外消耗1倍费用。触发几率{4:0.0}%</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>陷阱：对方使用的下张魔法卡无效。触发几率{4:0.0}%</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>陷阱：对方使用的下张卡牌无效。触发几率{4:0.0}%</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>陷阱：对方使用的下张武器卡无效。触发几率{4:0.0}%</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Freezing Trap</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3859,10 +3835,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>陷阱：对方召唤时，将目标移回手牌，并提升{3}点费用。触发几率{4:0.0}%</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>p.AddTrap(54000005,lv,s.Rate,0,0);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3903,10 +3875,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>陷阱：对方召唤时，如果目标星级低于3，使目标反叛。触发几率{4:0.0}%</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>p.AddPp(s.Help);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -4000,14 +3968,46 @@
   </si>
   <si>
     <t>NEO</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>陷阱：对方召唤时，冰冻目标5回合。触发需求MP:1，{4:0.0}%不消耗MP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>陷阱：对方使用卡牌时，额外消耗1倍费用。触发需求MP:1，{4:0.0}%不消耗MP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>陷阱：对方召唤时，对目标造成{0}点魔法伤害。触发需求MP:1，{4:0.0}%不消耗MP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>陷阱：对方使用的下张魔法卡无效。触发需求MP:1，{4:0.0}%不消耗MP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>陷阱：对方使用的下张卡牌无效。触发需求MP:3，{4:0.0}%不消耗MP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>陷阱：对方使用的下张武器卡无效。触发需求MP:1，{4:0.0}%不消耗MP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>陷阱：对方召唤时，将目标移回手牌，并提升{3}点费用。触发需求MP:1，{4:0.0}%不消耗MP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>陷阱：对方召唤时，如果目标星级低于3，使目标反叛。触发需求MP:1，{4:0.0}%不消耗MP</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="33">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5005,7 +5005,14 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="167">
+  <dxfs count="168">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -7679,6 +7686,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -7965,13 +7979,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
@@ -8002,7 +8009,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
@@ -8159,6 +8166,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CA22-4075-A404-74AE8324B43F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -8885,7 +8897,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="图表 3"/>
+        <xdr:cNvPr id="4" name="图表 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8904,139 +8922,139 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AB140" totalsRowShown="0" headerRowDxfId="127" dataDxfId="126" tableBorderDxfId="125">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AB140" totalsRowShown="0" headerRowDxfId="128" dataDxfId="127" tableBorderDxfId="126">
   <autoFilter ref="A3:AB140"/>
   <sortState ref="A4:AB113">
     <sortCondition ref="A3:A113"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="124"/>
-    <tableColumn id="2" name="Name" dataDxfId="123"/>
-    <tableColumn id="20" name="Ename" dataDxfId="122"/>
-    <tableColumn id="21" name="Remark" dataDxfId="121"/>
-    <tableColumn id="3" name="Star" dataDxfId="120"/>
-    <tableColumn id="4" name="Type" dataDxfId="119"/>
-    <tableColumn id="5" name="Attr" dataDxfId="118"/>
-    <tableColumn id="8" name="Quality" dataDxfId="117">
+    <tableColumn id="1" name="Id" dataDxfId="125"/>
+    <tableColumn id="2" name="Name" dataDxfId="124"/>
+    <tableColumn id="20" name="Ename" dataDxfId="123"/>
+    <tableColumn id="21" name="Remark" dataDxfId="122"/>
+    <tableColumn id="3" name="Star" dataDxfId="121"/>
+    <tableColumn id="4" name="Type" dataDxfId="120"/>
+    <tableColumn id="5" name="Attr" dataDxfId="119"/>
+    <tableColumn id="8" name="Quality" dataDxfId="118">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="116"/>
-    <tableColumn id="9" name="Damage" dataDxfId="115"/>
-    <tableColumn id="10" name="Cure" dataDxfId="114"/>
-    <tableColumn id="11" name="Time" dataDxfId="113"/>
-    <tableColumn id="13" name="Help" dataDxfId="112"/>
-    <tableColumn id="16" name="Rate" dataDxfId="111"/>
-    <tableColumn id="18" name="Atk" dataDxfId="110"/>
-    <tableColumn id="12" name="Modify" dataDxfId="109"/>
-    <tableColumn id="27" name="Sum" dataDxfId="108">
+    <tableColumn id="7" name="Cost" dataDxfId="117"/>
+    <tableColumn id="9" name="Damage" dataDxfId="116"/>
+    <tableColumn id="10" name="Cure" dataDxfId="115"/>
+    <tableColumn id="11" name="Time" dataDxfId="114"/>
+    <tableColumn id="13" name="Help" dataDxfId="113"/>
+    <tableColumn id="16" name="Rate" dataDxfId="112"/>
+    <tableColumn id="18" name="Atk" dataDxfId="111"/>
+    <tableColumn id="12" name="Modify" dataDxfId="110"/>
+    <tableColumn id="27" name="Sum" dataDxfId="109">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="107"/>
-    <tableColumn id="15" name="Target" dataDxfId="106"/>
-    <tableColumn id="25" name="Mark" dataDxfId="105"/>
-    <tableColumn id="22" name="Effect" dataDxfId="104"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="103"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="102"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="101"/>
-    <tableColumn id="26" name="JobId" dataDxfId="100"/>
-    <tableColumn id="19" name="Icon" dataDxfId="99"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="98"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="97"/>
+    <tableColumn id="6" name="Range" dataDxfId="108"/>
+    <tableColumn id="15" name="Target" dataDxfId="107"/>
+    <tableColumn id="25" name="Mark" dataDxfId="106"/>
+    <tableColumn id="22" name="Effect" dataDxfId="105"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="104"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="103"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="102"/>
+    <tableColumn id="26" name="JobId" dataDxfId="101"/>
+    <tableColumn id="19" name="Icon" dataDxfId="100"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="99"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="98"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AB12" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71" tableBorderDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AB12" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72" tableBorderDxfId="71">
   <autoFilter ref="A3:AB12"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="69"/>
-    <tableColumn id="2" name="Name" dataDxfId="68"/>
-    <tableColumn id="20" name="Ename" dataDxfId="67"/>
-    <tableColumn id="21" name="Remark" dataDxfId="66"/>
-    <tableColumn id="3" name="Star" dataDxfId="65"/>
-    <tableColumn id="4" name="Type" dataDxfId="64"/>
-    <tableColumn id="5" name="Attr" dataDxfId="63"/>
-    <tableColumn id="8" name="Quality" dataDxfId="62">
+    <tableColumn id="1" name="Id" dataDxfId="70"/>
+    <tableColumn id="2" name="Name" dataDxfId="69"/>
+    <tableColumn id="20" name="Ename" dataDxfId="68"/>
+    <tableColumn id="21" name="Remark" dataDxfId="67"/>
+    <tableColumn id="3" name="Star" dataDxfId="66"/>
+    <tableColumn id="4" name="Type" dataDxfId="65"/>
+    <tableColumn id="5" name="Attr" dataDxfId="64"/>
+    <tableColumn id="8" name="Quality" dataDxfId="63">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="61"/>
-    <tableColumn id="9" name="Damage" dataDxfId="60"/>
-    <tableColumn id="10" name="Cure" dataDxfId="59"/>
-    <tableColumn id="11" name="Time" dataDxfId="58"/>
-    <tableColumn id="13" name="Help" dataDxfId="57"/>
-    <tableColumn id="16" name="Rate" dataDxfId="56"/>
-    <tableColumn id="18" name="Atk" dataDxfId="55"/>
-    <tableColumn id="12" name="Modify" dataDxfId="54"/>
-    <tableColumn id="27" name="Sum" dataDxfId="53">
+    <tableColumn id="7" name="Cost" dataDxfId="62"/>
+    <tableColumn id="9" name="Damage" dataDxfId="61"/>
+    <tableColumn id="10" name="Cure" dataDxfId="60"/>
+    <tableColumn id="11" name="Time" dataDxfId="59"/>
+    <tableColumn id="13" name="Help" dataDxfId="58"/>
+    <tableColumn id="16" name="Rate" dataDxfId="57"/>
+    <tableColumn id="18" name="Atk" dataDxfId="56"/>
+    <tableColumn id="12" name="Modify" dataDxfId="55"/>
+    <tableColumn id="27" name="Sum" dataDxfId="54">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="52"/>
-    <tableColumn id="15" name="Target" dataDxfId="51"/>
-    <tableColumn id="25" name="Mark" dataDxfId="50"/>
-    <tableColumn id="22" name="Effect" dataDxfId="49"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="48"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="47"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="46"/>
-    <tableColumn id="26" name="JobId" dataDxfId="45"/>
-    <tableColumn id="19" name="Icon" dataDxfId="44"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="43"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="42"/>
+    <tableColumn id="6" name="Range" dataDxfId="53"/>
+    <tableColumn id="15" name="Target" dataDxfId="52"/>
+    <tableColumn id="25" name="Mark" dataDxfId="51"/>
+    <tableColumn id="22" name="Effect" dataDxfId="50"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="49"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="48"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="47"/>
+    <tableColumn id="26" name="JobId" dataDxfId="46"/>
+    <tableColumn id="19" name="Icon" dataDxfId="45"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="44"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_35" displayName="表1_35" ref="A3:AB9" totalsRowShown="0" headerRowDxfId="29" tableBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_35" displayName="表1_35" ref="A3:AB9" totalsRowShown="0" headerRowDxfId="30" tableBorderDxfId="29">
   <autoFilter ref="A3:AB9"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="27"/>
-    <tableColumn id="2" name="Name" dataDxfId="26"/>
-    <tableColumn id="20" name="Ename" dataDxfId="25"/>
-    <tableColumn id="21" name="Remark" dataDxfId="24"/>
-    <tableColumn id="3" name="Star" dataDxfId="23"/>
-    <tableColumn id="4" name="Type" dataDxfId="22"/>
-    <tableColumn id="5" name="Attr" dataDxfId="21"/>
-    <tableColumn id="8" name="Quality" dataDxfId="20">
+    <tableColumn id="1" name="Id" dataDxfId="28"/>
+    <tableColumn id="2" name="Name" dataDxfId="27"/>
+    <tableColumn id="20" name="Ename" dataDxfId="26"/>
+    <tableColumn id="21" name="Remark" dataDxfId="25"/>
+    <tableColumn id="3" name="Star" dataDxfId="24"/>
+    <tableColumn id="4" name="Type" dataDxfId="23"/>
+    <tableColumn id="5" name="Attr" dataDxfId="22"/>
+    <tableColumn id="8" name="Quality" dataDxfId="21">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="19"/>
-    <tableColumn id="9" name="Damage" dataDxfId="18"/>
-    <tableColumn id="10" name="Cure" dataDxfId="17"/>
-    <tableColumn id="11" name="Time" dataDxfId="16"/>
-    <tableColumn id="13" name="Help" dataDxfId="15"/>
-    <tableColumn id="16" name="Rate" dataDxfId="14"/>
-    <tableColumn id="18" name="Atk" dataDxfId="13"/>
-    <tableColumn id="12" name="Modify" dataDxfId="12"/>
-    <tableColumn id="27" name="Sum" dataDxfId="11">
+    <tableColumn id="7" name="Cost" dataDxfId="20"/>
+    <tableColumn id="9" name="Damage" dataDxfId="19"/>
+    <tableColumn id="10" name="Cure" dataDxfId="18"/>
+    <tableColumn id="11" name="Time" dataDxfId="17"/>
+    <tableColumn id="13" name="Help" dataDxfId="16"/>
+    <tableColumn id="16" name="Rate" dataDxfId="15"/>
+    <tableColumn id="18" name="Atk" dataDxfId="14"/>
+    <tableColumn id="12" name="Modify" dataDxfId="13"/>
+    <tableColumn id="27" name="Sum" dataDxfId="12">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="10"/>
-    <tableColumn id="15" name="Target" dataDxfId="9"/>
-    <tableColumn id="25" name="Mark" dataDxfId="8"/>
-    <tableColumn id="22" name="Effect" dataDxfId="7"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="6"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="5"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="4"/>
-    <tableColumn id="26" name="JobId" dataDxfId="3"/>
-    <tableColumn id="19" name="Icon" dataDxfId="2"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="1"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="0"/>
+    <tableColumn id="6" name="Range" dataDxfId="11"/>
+    <tableColumn id="15" name="Target" dataDxfId="10"/>
+    <tableColumn id="25" name="Mark" dataDxfId="9"/>
+    <tableColumn id="22" name="Effect" dataDxfId="8"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="7"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="6"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="5"/>
+    <tableColumn id="26" name="JobId" dataDxfId="4"/>
+    <tableColumn id="19" name="Icon" dataDxfId="3"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="2"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -9111,6 +9129,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -9146,6 +9181,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -9325,35 +9377,35 @@
   <dimension ref="A1:AB140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C79" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D81" sqref="D81"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
-    <col min="2" max="3" width="7.88671875" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" customWidth="1"/>
-    <col min="5" max="5" width="3.109375" customWidth="1"/>
-    <col min="6" max="6" width="3.6640625" customWidth="1"/>
-    <col min="7" max="9" width="3.109375" customWidth="1"/>
-    <col min="10" max="10" width="3.88671875" customWidth="1"/>
+    <col min="1" max="1" width="9.125" customWidth="1"/>
+    <col min="2" max="3" width="7.875" customWidth="1"/>
+    <col min="4" max="4" width="10.875" customWidth="1"/>
+    <col min="5" max="5" width="3.125" customWidth="1"/>
+    <col min="6" max="6" width="3.625" customWidth="1"/>
+    <col min="7" max="9" width="3.125" customWidth="1"/>
+    <col min="10" max="10" width="3.875" customWidth="1"/>
     <col min="11" max="11" width="4" customWidth="1"/>
-    <col min="12" max="16" width="3.109375" customWidth="1"/>
-    <col min="17" max="17" width="5.21875" customWidth="1"/>
-    <col min="18" max="18" width="3.109375" customWidth="1"/>
-    <col min="19" max="19" width="5.33203125" customWidth="1"/>
-    <col min="20" max="20" width="5.77734375" customWidth="1"/>
-    <col min="21" max="21" width="23.44140625" customWidth="1"/>
-    <col min="22" max="22" width="24.33203125" customWidth="1"/>
-    <col min="23" max="24" width="7.88671875" customWidth="1"/>
-    <col min="25" max="25" width="9.109375" customWidth="1"/>
+    <col min="12" max="16" width="3.125" customWidth="1"/>
+    <col min="17" max="17" width="5.25" customWidth="1"/>
+    <col min="18" max="18" width="3.125" customWidth="1"/>
+    <col min="19" max="19" width="5.375" customWidth="1"/>
+    <col min="20" max="20" width="5.75" customWidth="1"/>
+    <col min="21" max="21" width="23.5" customWidth="1"/>
+    <col min="22" max="22" width="58.125" customWidth="1"/>
+    <col min="23" max="24" width="7.875" customWidth="1"/>
+    <col min="25" max="25" width="9.125" customWidth="1"/>
     <col min="26" max="28" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="65.25" customHeight="1">
+    <row r="1" spans="1:28" ht="65.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>187</v>
       </c>
@@ -9439,7 +9491,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>178</v>
       </c>
@@ -9525,7 +9577,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>180</v>
       </c>
@@ -9611,7 +9663,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="60">
+    <row r="4" spans="1:28" ht="48" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>53000001</v>
       </c>
@@ -9675,10 +9727,10 @@
         <v>95</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>912</v>
+        <v>904</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>914</v>
+        <v>906</v>
       </c>
       <c r="W4" s="1" t="s">
         <v>2</v>
@@ -9695,7 +9747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>53000002</v>
       </c>
@@ -9779,7 +9831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="24">
+    <row r="6" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>53000003</v>
       </c>
@@ -9863,7 +9915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="48">
+    <row r="7" spans="1:28" ht="36" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>53000004</v>
       </c>
@@ -9949,7 +10001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="72">
+    <row r="8" spans="1:28" ht="72" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>53000005</v>
       </c>
@@ -10035,7 +10087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="48">
+    <row r="9" spans="1:28" ht="48" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>53000006</v>
       </c>
@@ -10119,7 +10171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="48">
+    <row r="10" spans="1:28" ht="48" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>53000007</v>
       </c>
@@ -10203,7 +10255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="48">
+    <row r="11" spans="1:28" ht="48" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>53000008</v>
       </c>
@@ -10287,7 +10339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="48">
+    <row r="12" spans="1:28" ht="48" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>53000009</v>
       </c>
@@ -10371,7 +10423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="48">
+    <row r="13" spans="1:28" ht="48" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>53000010</v>
       </c>
@@ -10455,7 +10507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="48">
+    <row r="14" spans="1:28" ht="48" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>53000011</v>
       </c>
@@ -10539,7 +10591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="48">
+    <row r="15" spans="1:28" ht="48" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>53000012</v>
       </c>
@@ -10623,7 +10675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="60">
+    <row r="16" spans="1:28" ht="48" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>53000013</v>
       </c>
@@ -10709,7 +10761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="72">
+    <row r="17" spans="1:28" ht="72" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>53000014</v>
       </c>
@@ -10795,7 +10847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>53000015</v>
       </c>
@@ -10881,7 +10933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="24">
+    <row r="19" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>53000016</v>
       </c>
@@ -10967,7 +11019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="24">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>53000017</v>
       </c>
@@ -11053,7 +11105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="60">
+    <row r="21" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>53000018</v>
       </c>
@@ -11139,7 +11191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="24">
+    <row r="22" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>53000019</v>
       </c>
@@ -11227,7 +11279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="24">
+    <row r="23" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>53000020</v>
       </c>
@@ -11315,7 +11367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="24">
+    <row r="24" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>53000021</v>
       </c>
@@ -11403,7 +11455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="24">
+    <row r="25" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>53000022</v>
       </c>
@@ -11489,7 +11541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="24">
+    <row r="26" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>53000023</v>
       </c>
@@ -11573,7 +11625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="24">
+    <row r="27" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>53000024</v>
       </c>
@@ -11659,7 +11711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="60">
+    <row r="28" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>53000025</v>
       </c>
@@ -11745,7 +11797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="24">
+    <row r="29" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>53000026</v>
       </c>
@@ -11831,7 +11883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:28">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>53000027</v>
       </c>
@@ -11915,7 +11967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:28">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>53000028</v>
       </c>
@@ -11999,7 +12051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:28" ht="24">
+    <row r="32" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>53000029</v>
       </c>
@@ -12083,7 +12135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:28" ht="24">
+    <row r="33" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>53000030</v>
       </c>
@@ -12125,7 +12177,7 @@
         <v>0</v>
       </c>
       <c r="N33" s="1">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="O33" s="1">
         <v>0</v>
@@ -12147,10 +12199,10 @@
         <v>100</v>
       </c>
       <c r="U33" s="11" t="s">
-        <v>887</v>
+        <v>880</v>
       </c>
       <c r="V33" s="1" t="s">
-        <v>877</v>
+        <v>914</v>
       </c>
       <c r="W33" s="1" t="s">
         <v>4</v>
@@ -12169,7 +12221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:28" ht="24">
+    <row r="34" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>53000031</v>
       </c>
@@ -12196,7 +12248,7 @@
         <v>1</v>
       </c>
       <c r="I34" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J34" s="1">
         <v>100</v>
@@ -12211,7 +12263,7 @@
         <v>0</v>
       </c>
       <c r="N34" s="1">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="O34" s="1">
         <v>0</v>
@@ -12233,10 +12285,10 @@
         <v>100</v>
       </c>
       <c r="U34" s="11" t="s">
-        <v>888</v>
+        <v>881</v>
       </c>
       <c r="V34" s="1" t="s">
-        <v>878</v>
+        <v>916</v>
       </c>
       <c r="W34" s="1" t="s">
         <v>4</v>
@@ -12255,7 +12307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:28" ht="84">
+    <row r="35" spans="1:28" ht="72" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>53000032</v>
       </c>
@@ -12343,7 +12395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:28" ht="60">
+    <row r="36" spans="1:28" ht="48" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>53000033</v>
       </c>
@@ -12431,7 +12483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:28" ht="60">
+    <row r="37" spans="1:28" ht="48" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>53000034</v>
       </c>
@@ -12517,7 +12569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:28" ht="84">
+    <row r="38" spans="1:28" ht="72" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>53000035</v>
       </c>
@@ -12605,7 +12657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:28" ht="48">
+    <row r="39" spans="1:28" ht="36" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>53000036</v>
       </c>
@@ -12691,7 +12743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:28" ht="24">
+    <row r="40" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>53000037</v>
       </c>
@@ -12775,7 +12827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:28" ht="60">
+    <row r="41" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>53000038</v>
       </c>
@@ -12863,7 +12915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:28" ht="24">
+    <row r="42" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>53000039</v>
       </c>
@@ -12905,7 +12957,7 @@
         <v>0</v>
       </c>
       <c r="N42" s="1">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="O42" s="1">
         <v>0</v>
@@ -12927,10 +12979,10 @@
         <v>85</v>
       </c>
       <c r="U42" s="11" t="s">
-        <v>889</v>
+        <v>882</v>
       </c>
       <c r="V42" s="1" t="s">
-        <v>879</v>
+        <v>915</v>
       </c>
       <c r="W42" s="1" t="s">
         <v>4</v>
@@ -12949,7 +13001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:28" ht="24">
+    <row r="43" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>53000040</v>
       </c>
@@ -12976,7 +13028,7 @@
         <v>1</v>
       </c>
       <c r="I43" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J43" s="1">
         <v>0</v>
@@ -12991,7 +13043,7 @@
         <v>0</v>
       </c>
       <c r="N43" s="1">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="O43" s="1">
         <v>0</v>
@@ -13013,10 +13065,10 @@
         <v>100</v>
       </c>
       <c r="U43" s="11" t="s">
-        <v>890</v>
+        <v>883</v>
       </c>
       <c r="V43" s="1" t="s">
-        <v>880</v>
+        <v>917</v>
       </c>
       <c r="W43" s="1" t="s">
         <v>4</v>
@@ -13035,7 +13087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:28" ht="36">
+    <row r="44" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>53000041</v>
       </c>
@@ -13119,7 +13171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:28" ht="96">
+    <row r="45" spans="1:28" ht="84" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>53000042</v>
       </c>
@@ -13207,7 +13259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:28" ht="24">
+    <row r="46" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>53000043</v>
       </c>
@@ -13293,7 +13345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:28" ht="24">
+    <row r="47" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>53000044</v>
       </c>
@@ -13320,7 +13372,7 @@
         <v>2</v>
       </c>
       <c r="I47" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J47" s="1">
         <v>0</v>
@@ -13335,7 +13387,7 @@
         <v>0</v>
       </c>
       <c r="N47" s="1">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="O47" s="1">
         <v>0</v>
@@ -13357,10 +13409,10 @@
         <v>95</v>
       </c>
       <c r="U47" s="11" t="s">
-        <v>891</v>
+        <v>884</v>
       </c>
       <c r="V47" s="1" t="s">
-        <v>881</v>
+        <v>918</v>
       </c>
       <c r="W47" s="1" t="s">
         <v>4</v>
@@ -13379,7 +13431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:28" ht="72">
+    <row r="48" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>53000045</v>
       </c>
@@ -13465,7 +13517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:28" ht="60">
+    <row r="49" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>53000046</v>
       </c>
@@ -13551,7 +13603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:28" ht="72">
+    <row r="50" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>53000047</v>
       </c>
@@ -13639,7 +13691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:28" ht="24">
+    <row r="51" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>53000048</v>
       </c>
@@ -13725,7 +13777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:28" ht="84">
+    <row r="52" spans="1:28" ht="72" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>53000049</v>
       </c>
@@ -13813,7 +13865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:28" ht="72">
+    <row r="53" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A53">
         <v>53000050</v>
       </c>
@@ -13899,7 +13951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:28" ht="96">
+    <row r="54" spans="1:28" ht="84" x14ac:dyDescent="0.15">
       <c r="A54">
         <v>53000051</v>
       </c>
@@ -13987,7 +14039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:28" ht="36">
+    <row r="55" spans="1:28" ht="36" x14ac:dyDescent="0.15">
       <c r="A55">
         <v>53000052</v>
       </c>
@@ -14073,7 +14125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:28" ht="72">
+    <row r="56" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A56">
         <v>53000053</v>
       </c>
@@ -14159,7 +14211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:28" ht="48">
+    <row r="57" spans="1:28" ht="36" x14ac:dyDescent="0.15">
       <c r="A57">
         <v>53000054</v>
       </c>
@@ -14245,7 +14297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:28" ht="36">
+    <row r="58" spans="1:28" ht="36" x14ac:dyDescent="0.15">
       <c r="A58">
         <v>53000055</v>
       </c>
@@ -14331,7 +14383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:28" ht="48">
+    <row r="59" spans="1:28" ht="36" x14ac:dyDescent="0.15">
       <c r="A59">
         <v>53000056</v>
       </c>
@@ -14417,7 +14469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:28" ht="24">
+    <row r="60" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A60">
         <v>53000057</v>
       </c>
@@ -14503,7 +14555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:28" ht="36">
+    <row r="61" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A61">
         <v>53000058</v>
       </c>
@@ -14589,7 +14641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:28" ht="24">
+    <row r="62" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A62">
         <v>53000059</v>
       </c>
@@ -14675,7 +14727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:28" ht="60">
+    <row r="63" spans="1:28" ht="48" x14ac:dyDescent="0.15">
       <c r="A63">
         <v>53000060</v>
       </c>
@@ -14761,7 +14813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:28" ht="60">
+    <row r="64" spans="1:28" ht="48" x14ac:dyDescent="0.15">
       <c r="A64">
         <v>53000061</v>
       </c>
@@ -14847,7 +14899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:28" ht="24">
+    <row r="65" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A65">
         <v>53000062</v>
       </c>
@@ -14933,7 +14985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:28">
+    <row r="66" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A66">
         <v>53000063</v>
       </c>
@@ -15019,7 +15071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:28" ht="24">
+    <row r="67" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A67">
         <v>53000064</v>
       </c>
@@ -15105,7 +15157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:28" ht="60">
+    <row r="68" spans="1:28" ht="48" x14ac:dyDescent="0.15">
       <c r="A68">
         <v>53000065</v>
       </c>
@@ -15191,7 +15243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:28" ht="24">
+    <row r="69" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A69">
         <v>53000066</v>
       </c>
@@ -15218,7 +15270,7 @@
         <v>1</v>
       </c>
       <c r="I69" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J69" s="1">
         <v>0</v>
@@ -15233,7 +15285,7 @@
         <v>0</v>
       </c>
       <c r="N69" s="1">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="O69" s="1">
         <v>0</v>
@@ -15255,10 +15307,10 @@
         <v>85</v>
       </c>
       <c r="U69" s="11" t="s">
-        <v>892</v>
+        <v>885</v>
       </c>
       <c r="V69" s="1" t="s">
-        <v>882</v>
+        <v>919</v>
       </c>
       <c r="W69" s="1" t="s">
         <v>4</v>
@@ -15277,7 +15329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:28" ht="36">
+    <row r="70" spans="1:28" ht="36" x14ac:dyDescent="0.15">
       <c r="A70">
         <v>53000067</v>
       </c>
@@ -15363,7 +15415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:28" ht="72">
+    <row r="71" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A71">
         <v>53000068</v>
       </c>
@@ -15451,7 +15503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:28" ht="48">
+    <row r="72" spans="1:28" ht="48" x14ac:dyDescent="0.15">
       <c r="A72">
         <v>53000069</v>
       </c>
@@ -15537,7 +15589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:28" ht="36">
+    <row r="73" spans="1:28" ht="36" x14ac:dyDescent="0.15">
       <c r="A73">
         <v>53000070</v>
       </c>
@@ -15623,7 +15675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:28" ht="96">
+    <row r="74" spans="1:28" ht="84" x14ac:dyDescent="0.15">
       <c r="A74">
         <v>53000071</v>
       </c>
@@ -15711,7 +15763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:28" ht="60">
+    <row r="75" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A75">
         <v>53000072</v>
       </c>
@@ -15797,7 +15849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:28" ht="48">
+    <row r="76" spans="1:28" ht="48" x14ac:dyDescent="0.15">
       <c r="A76">
         <v>53000073</v>
       </c>
@@ -15883,7 +15935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:28" ht="48">
+    <row r="77" spans="1:28" ht="36" x14ac:dyDescent="0.15">
       <c r="A77">
         <v>53000074</v>
       </c>
@@ -15969,7 +16021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:28" ht="132">
+    <row r="78" spans="1:28" ht="108" x14ac:dyDescent="0.15">
       <c r="A78">
         <v>53000075</v>
       </c>
@@ -16055,7 +16107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:28" ht="72">
+    <row r="79" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A79">
         <v>53000076</v>
       </c>
@@ -16143,7 +16195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:28" ht="48">
+    <row r="80" spans="1:28" ht="48" x14ac:dyDescent="0.15">
       <c r="A80">
         <v>53000077</v>
       </c>
@@ -16229,7 +16281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:28" ht="60">
+    <row r="81" spans="1:28" ht="48" x14ac:dyDescent="0.15">
       <c r="A81">
         <v>53000078</v>
       </c>
@@ -16313,7 +16365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:28" ht="72">
+    <row r="82" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A82">
         <v>53000079</v>
       </c>
@@ -16401,7 +16453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:28" ht="72">
+    <row r="83" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A83">
         <v>53000080</v>
       </c>
@@ -16489,7 +16541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:28" ht="96">
+    <row r="84" spans="1:28" ht="84" x14ac:dyDescent="0.15">
       <c r="A84">
         <v>53000081</v>
       </c>
@@ -16577,7 +16629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:28">
+    <row r="85" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A85">
         <v>53000082</v>
       </c>
@@ -16663,7 +16715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:28" ht="60">
+    <row r="86" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A86">
         <v>53000083</v>
       </c>
@@ -16749,7 +16801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:28" ht="60">
+    <row r="87" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A87">
         <v>53000084</v>
       </c>
@@ -16837,7 +16889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:28" ht="72">
+    <row r="88" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A88">
         <v>53000085</v>
       </c>
@@ -16925,7 +16977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:28" ht="60">
+    <row r="89" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A89">
         <v>53000086</v>
       </c>
@@ -17011,7 +17063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:28" ht="60">
+    <row r="90" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A90">
         <v>53000087</v>
       </c>
@@ -17099,7 +17151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:28" ht="72">
+    <row r="91" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A91">
         <v>53000088</v>
       </c>
@@ -17187,7 +17239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:28" ht="72">
+    <row r="92" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A92">
         <v>53000089</v>
       </c>
@@ -17275,7 +17327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:28" ht="24">
+    <row r="93" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A93">
         <v>53000090</v>
       </c>
@@ -17361,7 +17413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:28" ht="48">
+    <row r="94" spans="1:28" ht="36" x14ac:dyDescent="0.15">
       <c r="A94">
         <v>53000091</v>
       </c>
@@ -17447,7 +17499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:28" ht="24">
+    <row r="95" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A95">
         <v>53000092</v>
       </c>
@@ -17533,7 +17585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:28" ht="72">
+    <row r="96" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A96">
         <v>53000093</v>
       </c>
@@ -17619,7 +17671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:28" ht="36">
+    <row r="97" spans="1:28" ht="36" x14ac:dyDescent="0.15">
       <c r="A97">
         <v>53000094</v>
       </c>
@@ -17705,7 +17757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:28" ht="72">
+    <row r="98" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A98">
         <v>53000095</v>
       </c>
@@ -17793,7 +17845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:28" ht="36">
+    <row r="99" spans="1:28" ht="36" x14ac:dyDescent="0.15">
       <c r="A99">
         <v>53000096</v>
       </c>
@@ -17879,7 +17931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:28" ht="72">
+    <row r="100" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A100">
         <v>53000097</v>
       </c>
@@ -17965,7 +18017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:28" ht="24">
+    <row r="101" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A101">
         <v>53000098</v>
       </c>
@@ -18051,7 +18103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:28" ht="36">
+    <row r="102" spans="1:28" ht="36" x14ac:dyDescent="0.15">
       <c r="A102">
         <v>53000099</v>
       </c>
@@ -18137,7 +18189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:28" ht="96">
+    <row r="103" spans="1:28" ht="72" x14ac:dyDescent="0.15">
       <c r="A103">
         <v>53000100</v>
       </c>
@@ -18223,7 +18275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:28" ht="24">
+    <row r="104" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A104">
         <v>53000101</v>
       </c>
@@ -18309,7 +18361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:28" ht="24">
+    <row r="105" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A105">
         <v>53000102</v>
       </c>
@@ -18395,7 +18447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:28" ht="72">
+    <row r="106" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A106">
         <v>53000103</v>
       </c>
@@ -18483,7 +18535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:28" ht="60">
+    <row r="107" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A107">
         <v>53000104</v>
       </c>
@@ -18569,7 +18621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:28" ht="60">
+    <row r="108" spans="1:28" ht="36" x14ac:dyDescent="0.15">
       <c r="A108">
         <v>53000105</v>
       </c>
@@ -18655,7 +18707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:28">
+    <row r="109" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A109">
         <v>53000106</v>
       </c>
@@ -18741,7 +18793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:28">
+    <row r="110" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A110">
         <v>53000107</v>
       </c>
@@ -18827,7 +18879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:28" ht="144">
+    <row r="111" spans="1:28" ht="120" x14ac:dyDescent="0.15">
       <c r="A111">
         <v>53000108</v>
       </c>
@@ -18913,7 +18965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:28" ht="36">
+    <row r="112" spans="1:28" ht="36" x14ac:dyDescent="0.15">
       <c r="A112">
         <v>53000109</v>
       </c>
@@ -18999,7 +19051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:28" ht="48">
+    <row r="113" spans="1:28" ht="36" x14ac:dyDescent="0.15">
       <c r="A113">
         <v>53000110</v>
       </c>
@@ -19085,7 +19137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:28" ht="84">
+    <row r="114" spans="1:28" ht="72" x14ac:dyDescent="0.15">
       <c r="A114">
         <v>53000111</v>
       </c>
@@ -19173,7 +19225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:28" ht="60">
+    <row r="115" spans="1:28" ht="48" x14ac:dyDescent="0.15">
       <c r="A115">
         <v>53000112</v>
       </c>
@@ -19261,7 +19313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:28" ht="36">
+    <row r="116" spans="1:28" ht="36" x14ac:dyDescent="0.15">
       <c r="A116">
         <v>53000113</v>
       </c>
@@ -19347,7 +19399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:28" ht="72">
+    <row r="117" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A117">
         <v>53000114</v>
       </c>
@@ -19433,7 +19485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:28" ht="36">
+    <row r="118" spans="1:28" ht="36" x14ac:dyDescent="0.15">
       <c r="A118">
         <v>53000115</v>
       </c>
@@ -19519,7 +19571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:28" ht="72">
+    <row r="119" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A119">
         <v>53000116</v>
       </c>
@@ -19607,7 +19659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:28" ht="48">
+    <row r="120" spans="1:28" ht="36" x14ac:dyDescent="0.15">
       <c r="A120">
         <v>53000117</v>
       </c>
@@ -19695,7 +19747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:28" ht="72">
+    <row r="121" spans="1:28" ht="48" x14ac:dyDescent="0.15">
       <c r="A121">
         <v>53000118</v>
       </c>
@@ -19781,7 +19833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:28" ht="36">
+    <row r="122" spans="1:28" ht="36" x14ac:dyDescent="0.15">
       <c r="A122">
         <v>53000119</v>
       </c>
@@ -19867,7 +19919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:28" ht="24">
+    <row r="123" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A123">
         <v>53000120</v>
       </c>
@@ -19953,7 +20005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:28" ht="72">
+    <row r="124" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A124">
         <v>53000121</v>
       </c>
@@ -20041,7 +20093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:28" ht="36">
+    <row r="125" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A125">
         <v>53000122</v>
       </c>
@@ -20129,7 +20181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:28" ht="36">
+    <row r="126" spans="1:28" ht="36" x14ac:dyDescent="0.15">
       <c r="A126">
         <v>53000123</v>
       </c>
@@ -20217,7 +20269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:28" ht="36">
+    <row r="127" spans="1:28" ht="36" x14ac:dyDescent="0.15">
       <c r="A127">
         <v>53000124</v>
       </c>
@@ -20305,7 +20357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:28" ht="48">
+    <row r="128" spans="1:28" ht="48" x14ac:dyDescent="0.15">
       <c r="A128">
         <v>53000125</v>
       </c>
@@ -20393,7 +20445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:28" ht="72">
+    <row r="129" spans="1:28" ht="48" x14ac:dyDescent="0.15">
       <c r="A129">
         <v>53000126</v>
       </c>
@@ -20479,7 +20531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:28" ht="72">
+    <row r="130" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A130">
         <v>53000127</v>
       </c>
@@ -20565,7 +20617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:28" ht="72">
+    <row r="131" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A131">
         <v>53000128</v>
       </c>
@@ -20653,7 +20705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:28" ht="36">
+    <row r="132" spans="1:28" ht="36" x14ac:dyDescent="0.15">
       <c r="A132">
         <v>53000129</v>
       </c>
@@ -20741,7 +20793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:28" ht="96">
+    <row r="133" spans="1:28" ht="84" x14ac:dyDescent="0.15">
       <c r="A133">
         <v>53000130</v>
       </c>
@@ -20829,7 +20881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:28" ht="72">
+    <row r="134" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A134">
         <v>53000131</v>
       </c>
@@ -20917,7 +20969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:28" ht="36">
+    <row r="135" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A135">
         <v>53000132</v>
       </c>
@@ -21005,18 +21057,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:28" ht="24">
+    <row r="136" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A136">
         <v>53000133</v>
       </c>
       <c r="B136" s="22" t="s">
-        <v>884</v>
+        <v>878</v>
       </c>
       <c r="C136" s="15" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
       <c r="D136" s="25" t="s">
-        <v>885</v>
+        <v>879</v>
       </c>
       <c r="E136" s="15">
         <v>2</v>
@@ -21031,8 +21083,8 @@
         <f t="shared" si="46"/>
         <v>1</v>
       </c>
-      <c r="I136" s="15">
-        <v>2</v>
+      <c r="I136" s="1">
+        <v>1</v>
       </c>
       <c r="J136" s="15">
         <v>0</v>
@@ -21046,8 +21098,8 @@
       <c r="M136" s="15">
         <v>2</v>
       </c>
-      <c r="N136" s="15">
-        <v>30</v>
+      <c r="N136" s="1">
+        <v>20</v>
       </c>
       <c r="O136" s="15">
         <v>0</v>
@@ -21069,10 +21121,10 @@
         <v>100</v>
       </c>
       <c r="U136" s="11" t="s">
-        <v>893</v>
+        <v>886</v>
       </c>
       <c r="V136" s="1" t="s">
-        <v>886</v>
+        <v>920</v>
       </c>
       <c r="W136" s="15" t="s">
         <v>4</v>
@@ -21091,18 +21143,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:28" ht="24">
+    <row r="137" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A137">
         <v>53000134</v>
       </c>
       <c r="B137" s="22" t="s">
-        <v>895</v>
+        <v>888</v>
       </c>
       <c r="C137" s="15" t="s">
-        <v>894</v>
+        <v>887</v>
       </c>
       <c r="D137" s="25" t="s">
-        <v>885</v>
+        <v>879</v>
       </c>
       <c r="E137" s="15">
         <v>2</v>
@@ -21117,8 +21169,8 @@
         <f t="shared" ref="H137" si="48">IF(AND(Q137&gt;=13,Q137&lt;=16),5,IF(AND(Q137&gt;=9,Q137&lt;=12),4,IF(AND(Q137&gt;=5,Q137&lt;=8),3,IF(AND(Q137&gt;=1,Q137&lt;=4),2,IF(AND(Q137&gt;=-3,Q137&lt;=0),1,IF(AND(Q137&gt;=-5,Q137&lt;=-4),0,6))))))</f>
         <v>2</v>
       </c>
-      <c r="I137" s="15">
-        <v>2</v>
+      <c r="I137" s="1">
+        <v>1</v>
       </c>
       <c r="J137" s="15">
         <v>0</v>
@@ -21132,8 +21184,8 @@
       <c r="M137" s="15">
         <v>0</v>
       </c>
-      <c r="N137" s="15">
-        <v>60</v>
+      <c r="N137" s="1">
+        <v>20</v>
       </c>
       <c r="O137" s="15">
         <v>0</v>
@@ -21155,10 +21207,10 @@
         <v>103</v>
       </c>
       <c r="U137" s="11" t="s">
-        <v>896</v>
+        <v>889</v>
       </c>
       <c r="V137" s="1" t="s">
-        <v>897</v>
+        <v>921</v>
       </c>
       <c r="W137" s="15" t="s">
         <v>4</v>
@@ -21177,18 +21229,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:28" ht="96">
+    <row r="138" spans="1:28" ht="84" x14ac:dyDescent="0.15">
       <c r="A138">
         <v>53000135</v>
       </c>
       <c r="B138" s="22" t="s">
-        <v>900</v>
+        <v>892</v>
       </c>
       <c r="C138" s="15" t="s">
-        <v>901</v>
+        <v>893</v>
       </c>
       <c r="D138" s="25" t="s">
-        <v>905</v>
+        <v>897</v>
       </c>
       <c r="E138" s="15">
         <v>4</v>
@@ -21235,16 +21287,16 @@
         <v>20</v>
       </c>
       <c r="S138" s="15" t="s">
-        <v>906</v>
+        <v>898</v>
       </c>
       <c r="T138" s="15">
         <v>108</v>
       </c>
       <c r="U138" s="11" t="s">
-        <v>908</v>
+        <v>900</v>
       </c>
       <c r="V138" s="1" t="s">
-        <v>910</v>
+        <v>902</v>
       </c>
       <c r="W138" s="1" t="s">
         <v>871</v>
@@ -21263,18 +21315,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:28" ht="132">
+    <row r="139" spans="1:28" ht="108" x14ac:dyDescent="0.15">
       <c r="A139">
         <v>53000136</v>
       </c>
       <c r="B139" s="22" t="s">
-        <v>903</v>
+        <v>895</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>902</v>
+        <v>894</v>
       </c>
       <c r="D139" s="25" t="s">
-        <v>904</v>
+        <v>896</v>
       </c>
       <c r="E139" s="15">
         <v>4</v>
@@ -21321,16 +21373,16 @@
         <v>20</v>
       </c>
       <c r="S139" s="15" t="s">
-        <v>911</v>
+        <v>903</v>
       </c>
       <c r="T139" s="15">
         <v>100</v>
       </c>
       <c r="U139" s="11" t="s">
-        <v>913</v>
+        <v>905</v>
       </c>
       <c r="V139" s="1" t="s">
-        <v>915</v>
+        <v>907</v>
       </c>
       <c r="W139" s="15" t="s">
         <v>4</v>
@@ -21349,18 +21401,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:28" ht="60">
+    <row r="140" spans="1:28" ht="48" x14ac:dyDescent="0.15">
       <c r="A140">
         <v>53000137</v>
       </c>
       <c r="B140" s="22" t="s">
-        <v>916</v>
+        <v>908</v>
       </c>
       <c r="C140" s="15" t="s">
-        <v>917</v>
+        <v>909</v>
       </c>
       <c r="D140" s="25" t="s">
-        <v>918</v>
+        <v>910</v>
       </c>
       <c r="E140" s="15">
         <v>2</v>
@@ -21407,16 +21459,16 @@
         <v>0</v>
       </c>
       <c r="S140" s="15" t="s">
-        <v>921</v>
+        <v>913</v>
       </c>
       <c r="T140" s="15">
         <v>102</v>
       </c>
       <c r="U140" s="11" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
       <c r="V140" s="1" t="s">
-        <v>920</v>
+        <v>912</v>
       </c>
       <c r="W140" s="15" t="s">
         <v>4</v>
@@ -21440,126 +21492,131 @@
     <sortCondition ref="E1"/>
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="I38:I68 I17:I35 I4:I15 I70:I122">
-    <cfRule type="cellIs" dxfId="166" priority="77" operator="notEqual">
+  <conditionalFormatting sqref="I4:I15 I70:I122 I17:I35 I38:I68">
+    <cfRule type="cellIs" dxfId="167" priority="79" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J17:N35 J4:N15 J38:N68 P38:Q68 P5:Q15 P17:Q35 P4 P70:Q122 J70:N122">
-    <cfRule type="cellIs" dxfId="165" priority="76" operator="equal">
+  <conditionalFormatting sqref="J4:N15 P38:Q68 P5:Q15 P17:Q35 P4 P70:Q122 J70:N122 J17:N35 J38:N68 N69 N136:N137">
+    <cfRule type="cellIs" dxfId="166" priority="78" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I69">
-    <cfRule type="cellIs" dxfId="164" priority="41" operator="notEqual">
-      <formula>$E69</formula>
+  <conditionalFormatting sqref="J69:M69 P69:Q69">
+    <cfRule type="cellIs" dxfId="165" priority="42" operator="equal">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J69:N69 P69:Q69">
+  <conditionalFormatting sqref="I36">
+    <cfRule type="cellIs" dxfId="164" priority="41" operator="notEqual">
+      <formula>$E36</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J36:N36 P36:Q36">
     <cfRule type="cellIs" dxfId="163" priority="40" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I36">
+  <conditionalFormatting sqref="I37">
     <cfRule type="cellIs" dxfId="162" priority="39" operator="notEqual">
-      <formula>$E36</formula>
+      <formula>$E37</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J36:N36 P36:Q36">
+  <conditionalFormatting sqref="J37:N37 P37:Q37">
     <cfRule type="cellIs" dxfId="161" priority="38" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I37">
-    <cfRule type="cellIs" dxfId="160" priority="37" operator="notEqual">
-      <formula>$E37</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J37:N37 P37:Q37">
-    <cfRule type="cellIs" dxfId="159" priority="36" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H4:H15 H17:H122">
-    <cfRule type="cellIs" dxfId="158" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="34" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="35" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="36" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="155" priority="35" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="157" priority="37" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="cellIs" dxfId="154" priority="29" operator="notEqual">
+    <cfRule type="cellIs" dxfId="156" priority="31" operator="notEqual">
       <formula>$E16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:N16 P16:Q16">
-    <cfRule type="cellIs" dxfId="153" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="30" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="cellIs" dxfId="152" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="26" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="151" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="27" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="28" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="149" priority="27" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="151" priority="29" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D122 D141:D1048576">
-    <cfRule type="containsText" dxfId="148" priority="23" operator="containsText" text="未完成">
+    <cfRule type="containsText" dxfId="150" priority="25" operator="containsText" text="未完成">
       <formula>NOT(ISERROR(SEARCH("未完成",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:O134">
+    <cfRule type="cellIs" dxfId="149" priority="24" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I123:I135">
+    <cfRule type="cellIs" dxfId="148" priority="23" operator="notEqual">
+      <formula>$E123</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J123:N134 P123:Q134">
     <cfRule type="cellIs" dxfId="147" priority="22" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I123:I135">
-    <cfRule type="cellIs" dxfId="146" priority="21" operator="notEqual">
-      <formula>$E123</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J123:N134 P123:Q134">
-    <cfRule type="cellIs" dxfId="145" priority="20" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H123:H135">
-    <cfRule type="cellIs" dxfId="144" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="18" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="19" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="20" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="19" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="143" priority="21" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O123:O134">
+    <cfRule type="cellIs" dxfId="142" priority="16" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D123:D135">
+    <cfRule type="containsText" dxfId="141" priority="15" operator="containsText" text="未完成">
+      <formula>NOT(ISERROR(SEARCH("未完成",D123)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O135">
     <cfRule type="cellIs" dxfId="140" priority="14" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D123:D135">
-    <cfRule type="containsText" dxfId="139" priority="13" operator="containsText" text="未完成">
-      <formula>NOT(ISERROR(SEARCH("未完成",D123)))</formula>
+  <conditionalFormatting sqref="J135:N135 P135:Q135">
+    <cfRule type="cellIs" dxfId="139" priority="13" operator="equal">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O135">
@@ -21567,48 +21624,43 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J135:N135 P135:Q135">
-    <cfRule type="cellIs" dxfId="137" priority="11" operator="equal">
-      <formula>0</formula>
+  <conditionalFormatting sqref="I138:I140">
+    <cfRule type="cellIs" dxfId="137" priority="11" operator="notEqual">
+      <formula>$E138</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O135">
+  <conditionalFormatting sqref="J138:N140 P136:Q140 J136:M137">
     <cfRule type="cellIs" dxfId="136" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I136:I140">
-    <cfRule type="cellIs" dxfId="135" priority="9" operator="notEqual">
-      <formula>$E136</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J136:N140 P136:Q140">
-    <cfRule type="cellIs" dxfId="134" priority="8" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H136:H140">
-    <cfRule type="cellIs" dxfId="133" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="7" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="131" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="8" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="7" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="132" priority="9" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O136:O140">
-    <cfRule type="cellIs" dxfId="129" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136:D140">
-    <cfRule type="containsText" dxfId="128" priority="1" operator="containsText" text="未完成">
+    <cfRule type="containsText" dxfId="130" priority="3" operator="containsText" text="未完成">
       <formula>NOT(ISERROR(SEARCH("未完成",D136)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I136:I137 I69">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+      <formula>$E69</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21631,27 +21683,27 @@
       <selection pane="bottomRight" activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="3" width="7.88671875" customWidth="1"/>
-    <col min="5" max="5" width="3.109375" customWidth="1"/>
-    <col min="6" max="6" width="4.6640625" customWidth="1"/>
-    <col min="7" max="9" width="3.109375" customWidth="1"/>
-    <col min="10" max="10" width="3.88671875" customWidth="1"/>
+    <col min="2" max="3" width="7.875" customWidth="1"/>
+    <col min="5" max="5" width="3.125" customWidth="1"/>
+    <col min="6" max="6" width="4.625" customWidth="1"/>
+    <col min="7" max="9" width="3.125" customWidth="1"/>
+    <col min="10" max="10" width="3.875" customWidth="1"/>
     <col min="11" max="11" width="4" customWidth="1"/>
-    <col min="12" max="16" width="3.109375" customWidth="1"/>
-    <col min="17" max="17" width="5.109375" customWidth="1"/>
-    <col min="18" max="18" width="3.109375" customWidth="1"/>
-    <col min="19" max="19" width="5.33203125" customWidth="1"/>
-    <col min="20" max="20" width="5.77734375" customWidth="1"/>
-    <col min="21" max="21" width="23.44140625" customWidth="1"/>
-    <col min="22" max="22" width="27.21875" customWidth="1"/>
-    <col min="23" max="25" width="7.88671875" customWidth="1"/>
+    <col min="12" max="16" width="3.125" customWidth="1"/>
+    <col min="17" max="17" width="5.125" customWidth="1"/>
+    <col min="18" max="18" width="3.125" customWidth="1"/>
+    <col min="19" max="19" width="5.375" customWidth="1"/>
+    <col min="20" max="20" width="5.75" customWidth="1"/>
+    <col min="21" max="21" width="23.5" customWidth="1"/>
+    <col min="22" max="22" width="27.25" customWidth="1"/>
+    <col min="23" max="25" width="7.875" customWidth="1"/>
     <col min="26" max="28" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="65.25" customHeight="1">
+    <row r="1" spans="1:28" ht="65.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>187</v>
       </c>
@@ -21737,7 +21789,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>178</v>
       </c>
@@ -21823,7 +21875,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>180</v>
       </c>
@@ -21909,7 +21961,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="24">
+    <row r="4" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>53100000</v>
       </c>
@@ -21989,7 +22041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>53100001</v>
       </c>
@@ -22069,7 +22121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="24">
+    <row r="6" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>53100002</v>
       </c>
@@ -22129,10 +22181,10 @@
         <v>-1</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>907</v>
+        <v>899</v>
       </c>
       <c r="V6" s="7" t="s">
-        <v>909</v>
+        <v>901</v>
       </c>
       <c r="W6" s="15" t="s">
         <v>365</v>
@@ -22149,7 +22201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>53100003</v>
       </c>
@@ -22209,10 +22261,10 @@
         <v>-1</v>
       </c>
       <c r="U7" s="11" t="s">
-        <v>898</v>
+        <v>890</v>
       </c>
       <c r="V7" s="7" t="s">
-        <v>899</v>
+        <v>891</v>
       </c>
       <c r="W7" s="15" t="s">
         <v>2</v>
@@ -22229,7 +22281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="48">
+    <row r="8" spans="1:28" ht="36" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>53100004</v>
       </c>
@@ -22309,7 +22361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="24">
+    <row r="9" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>53100005</v>
       </c>
@@ -22389,7 +22441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="24">
+    <row r="10" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>53100006</v>
       </c>
@@ -22469,7 +22521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="24">
+    <row r="11" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>53100007</v>
       </c>
@@ -22549,7 +22601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="24">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>53100008</v>
       </c>
@@ -22632,110 +22684,110 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="J4:Q12">
-    <cfRule type="cellIs" dxfId="96" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="40" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:Q8">
-    <cfRule type="cellIs" dxfId="95" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="36" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:Q4 O4:O12">
-    <cfRule type="cellIs" dxfId="94" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="35" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="93" priority="34" operator="notEqual">
+    <cfRule type="cellIs" dxfId="94" priority="34" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:Q4 O4:O12">
-    <cfRule type="cellIs" dxfId="92" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="33" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="91" priority="32" operator="notEqual">
+    <cfRule type="cellIs" dxfId="92" priority="32" operator="notEqual">
       <formula>$E5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:Q5">
-    <cfRule type="cellIs" dxfId="90" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="31" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" dxfId="89" priority="30" operator="notEqual">
+    <cfRule type="cellIs" dxfId="90" priority="30" operator="notEqual">
       <formula>$E6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:Q6">
-    <cfRule type="cellIs" dxfId="88" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="29" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="87" priority="28" operator="notEqual">
+    <cfRule type="cellIs" dxfId="88" priority="28" operator="notEqual">
       <formula>$E7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:Q7">
-    <cfRule type="cellIs" dxfId="86" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="27" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="85" priority="26" operator="notEqual">
+    <cfRule type="cellIs" dxfId="86" priority="26" operator="notEqual">
       <formula>$E8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:Q8">
-    <cfRule type="cellIs" dxfId="84" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="25" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I12">
-    <cfRule type="cellIs" dxfId="83" priority="24" operator="notEqual">
+    <cfRule type="cellIs" dxfId="84" priority="24" operator="notEqual">
       <formula>$E9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:Q12">
-    <cfRule type="cellIs" dxfId="82" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="23" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H12">
-    <cfRule type="cellIs" dxfId="81" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="7" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="8" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="79" priority="9" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="77" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="4" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="75" priority="5" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10:L12">
-    <cfRule type="cellIs" dxfId="73" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22759,28 +22811,28 @@
       <selection pane="bottomRight" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" customWidth="1"/>
-    <col min="2" max="3" width="7.88671875" customWidth="1"/>
-    <col min="5" max="5" width="3.109375" customWidth="1"/>
-    <col min="6" max="6" width="4.33203125" customWidth="1"/>
-    <col min="7" max="9" width="3.109375" customWidth="1"/>
-    <col min="10" max="10" width="3.88671875" customWidth="1"/>
+    <col min="1" max="1" width="10.75" customWidth="1"/>
+    <col min="2" max="3" width="7.875" customWidth="1"/>
+    <col min="5" max="5" width="3.125" customWidth="1"/>
+    <col min="6" max="6" width="4.375" customWidth="1"/>
+    <col min="7" max="9" width="3.125" customWidth="1"/>
+    <col min="10" max="10" width="3.875" customWidth="1"/>
     <col min="11" max="11" width="4" customWidth="1"/>
-    <col min="12" max="16" width="3.109375" customWidth="1"/>
-    <col min="17" max="17" width="5.21875" customWidth="1"/>
-    <col min="18" max="18" width="3.109375" customWidth="1"/>
-    <col min="19" max="19" width="5.33203125" customWidth="1"/>
-    <col min="20" max="20" width="5.77734375" customWidth="1"/>
-    <col min="21" max="21" width="23.44140625" customWidth="1"/>
-    <col min="22" max="22" width="27.21875" customWidth="1"/>
-    <col min="23" max="25" width="7.88671875" customWidth="1"/>
+    <col min="12" max="16" width="3.125" customWidth="1"/>
+    <col min="17" max="17" width="5.25" customWidth="1"/>
+    <col min="18" max="18" width="3.125" customWidth="1"/>
+    <col min="19" max="19" width="5.375" customWidth="1"/>
+    <col min="20" max="20" width="5.75" customWidth="1"/>
+    <col min="21" max="21" width="23.5" customWidth="1"/>
+    <col min="22" max="22" width="27.25" customWidth="1"/>
+    <col min="23" max="25" width="7.875" customWidth="1"/>
     <col min="26" max="26" width="5" customWidth="1"/>
     <col min="27" max="28" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="65.25" customHeight="1">
+    <row r="1" spans="1:28" ht="65.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="12" t="s">
         <v>187</v>
       </c>
@@ -22866,7 +22918,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>178</v>
       </c>
@@ -22952,7 +23004,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>180</v>
       </c>
@@ -23038,7 +23090,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="48">
+    <row r="4" spans="1:28" ht="36" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>53200100</v>
       </c>
@@ -23122,7 +23174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="24">
+    <row r="5" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>53200101</v>
       </c>
@@ -23206,7 +23258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="43.2">
+    <row r="6" spans="1:28" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>53200102</v>
       </c>
@@ -23290,7 +23342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>53200103</v>
       </c>
@@ -23372,7 +23424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="72">
+    <row r="8" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>53200104</v>
       </c>
@@ -23458,7 +23510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="24">
+    <row r="9" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>53200105</v>
       </c>
@@ -23545,50 +23597,50 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I4:I9">
-    <cfRule type="cellIs" dxfId="41" priority="12" operator="notEqual">
+    <cfRule type="cellIs" dxfId="42" priority="12" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:Q7 O4:O9">
-    <cfRule type="cellIs" dxfId="40" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:Q9">
-    <cfRule type="cellIs" dxfId="39" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:Q8">
-    <cfRule type="cellIs" dxfId="38" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H9">
-    <cfRule type="cellIs" dxfId="37" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="6" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="7" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="35" priority="8" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="33" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="31" priority="4" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23609,14 +23661,17 @@
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B3">
         <v>1</v>
       </c>
@@ -23648,7 +23703,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>383</v>
       </c>
@@ -23693,7 +23748,7 @@
         <v>1.5811388300841898</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.15">
       <c r="A5" s="30" t="s">
         <v>384</v>
       </c>
@@ -23738,7 +23793,7 @@
         <v>1.5811388300841898</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>385</v>
       </c>
@@ -23783,12 +23838,12 @@
         <v>1.4577379737113252</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>388</v>
       </c>
@@ -23810,14 +23865,17 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B1" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>405</v>
       </c>
@@ -23826,7 +23884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>407</v>
       </c>
@@ -23835,7 +23893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>408</v>
       </c>
@@ -23844,7 +23902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>415</v>
       </c>
@@ -23853,7 +23911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>409</v>
       </c>
@@ -23862,7 +23920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>410</v>
       </c>
@@ -23871,7 +23929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>411</v>
       </c>
@@ -23880,7 +23938,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>439</v>
       </c>
@@ -23889,7 +23947,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>412</v>
       </c>
@@ -23898,7 +23956,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>413</v>
       </c>
@@ -23907,7 +23965,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>512</v>
       </c>

</xml_diff>

<commit_message>
optimise the cardflow. including death show and trap show
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -3835,34 +3835,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>p.AddTrap(54000005,lv,s.Rate,0,0);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>p.AddTrap(54000006,lv,s.Rate,s.Damage,0);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>p.AddTrap(54000004,lv,s.Rate,0,0);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>p.AddTrap(54000002,lv,s.Rate,0,0);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>p.AddTrap(54000003,lv,s.Rate,0,0);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>p.AddTrap(54000001,lv,s.Rate,0,0);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>p.AddTrap(54000007,lv,s.Rate,0,s.Help);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Misdirection</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3871,10 +3843,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>p.AddTrap(54000008,lv,s.Rate,0,0);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>p.AddPp(s.Help);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -4000,6 +3968,38 @@
   </si>
   <si>
     <t>陷阱：对方召唤时，如果目标星级低于3，使目标反叛。触发需求MP:1，{4:0.0}%不消耗MP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>p.AddTrap(54000005,s.Id,lv,s.Rate,0,0);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>p.AddTrap(54000006,s.Id,lv,s.Rate,s.Damage,0);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>p.AddTrap(54000004,s.Id,lv,s.Rate,0,0);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>p.AddTrap(54000002,s.Id,lv,s.Rate,0,0);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>p.AddTrap(54000003,s.Id,lv,s.Rate,0,0);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>p.AddTrap(54000001,s.Id,lv,s.Rate,0,0);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>p.AddTrap(54000007,s.Id,lv,s.Rate,0,s.Help);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>p.AddTrap(54000008,s.Id,lv,s.Rate,0,0);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -5005,14 +5005,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="168">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="167">
     <dxf>
       <font>
         <b val="0"/>
@@ -8922,132 +8915,132 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AB140" totalsRowShown="0" headerRowDxfId="128" dataDxfId="127" tableBorderDxfId="126">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AB140" totalsRowShown="0" headerRowDxfId="127" dataDxfId="126" tableBorderDxfId="125">
   <autoFilter ref="A3:AB140"/>
   <sortState ref="A4:AB113">
     <sortCondition ref="A3:A113"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="125"/>
-    <tableColumn id="2" name="Name" dataDxfId="124"/>
-    <tableColumn id="20" name="Ename" dataDxfId="123"/>
-    <tableColumn id="21" name="Remark" dataDxfId="122"/>
-    <tableColumn id="3" name="Star" dataDxfId="121"/>
-    <tableColumn id="4" name="Type" dataDxfId="120"/>
-    <tableColumn id="5" name="Attr" dataDxfId="119"/>
-    <tableColumn id="8" name="Quality" dataDxfId="118">
+    <tableColumn id="1" name="Id" dataDxfId="124"/>
+    <tableColumn id="2" name="Name" dataDxfId="123"/>
+    <tableColumn id="20" name="Ename" dataDxfId="122"/>
+    <tableColumn id="21" name="Remark" dataDxfId="121"/>
+    <tableColumn id="3" name="Star" dataDxfId="120"/>
+    <tableColumn id="4" name="Type" dataDxfId="119"/>
+    <tableColumn id="5" name="Attr" dataDxfId="118"/>
+    <tableColumn id="8" name="Quality" dataDxfId="117">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="117"/>
-    <tableColumn id="9" name="Damage" dataDxfId="116"/>
-    <tableColumn id="10" name="Cure" dataDxfId="115"/>
-    <tableColumn id="11" name="Time" dataDxfId="114"/>
-    <tableColumn id="13" name="Help" dataDxfId="113"/>
-    <tableColumn id="16" name="Rate" dataDxfId="112"/>
-    <tableColumn id="18" name="Atk" dataDxfId="111"/>
-    <tableColumn id="12" name="Modify" dataDxfId="110"/>
-    <tableColumn id="27" name="Sum" dataDxfId="109">
+    <tableColumn id="7" name="Cost" dataDxfId="116"/>
+    <tableColumn id="9" name="Damage" dataDxfId="115"/>
+    <tableColumn id="10" name="Cure" dataDxfId="114"/>
+    <tableColumn id="11" name="Time" dataDxfId="113"/>
+    <tableColumn id="13" name="Help" dataDxfId="112"/>
+    <tableColumn id="16" name="Rate" dataDxfId="111"/>
+    <tableColumn id="18" name="Atk" dataDxfId="110"/>
+    <tableColumn id="12" name="Modify" dataDxfId="109"/>
+    <tableColumn id="27" name="Sum" dataDxfId="108">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="108"/>
-    <tableColumn id="15" name="Target" dataDxfId="107"/>
-    <tableColumn id="25" name="Mark" dataDxfId="106"/>
-    <tableColumn id="22" name="Effect" dataDxfId="105"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="104"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="103"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="102"/>
-    <tableColumn id="26" name="JobId" dataDxfId="101"/>
-    <tableColumn id="19" name="Icon" dataDxfId="100"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="99"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="98"/>
+    <tableColumn id="6" name="Range" dataDxfId="107"/>
+    <tableColumn id="15" name="Target" dataDxfId="106"/>
+    <tableColumn id="25" name="Mark" dataDxfId="105"/>
+    <tableColumn id="22" name="Effect" dataDxfId="104"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="103"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="102"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="101"/>
+    <tableColumn id="26" name="JobId" dataDxfId="100"/>
+    <tableColumn id="19" name="Icon" dataDxfId="99"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="98"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="97"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AB12" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72" tableBorderDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AB12" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71" tableBorderDxfId="70">
   <autoFilter ref="A3:AB12"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="70"/>
-    <tableColumn id="2" name="Name" dataDxfId="69"/>
-    <tableColumn id="20" name="Ename" dataDxfId="68"/>
-    <tableColumn id="21" name="Remark" dataDxfId="67"/>
-    <tableColumn id="3" name="Star" dataDxfId="66"/>
-    <tableColumn id="4" name="Type" dataDxfId="65"/>
-    <tableColumn id="5" name="Attr" dataDxfId="64"/>
-    <tableColumn id="8" name="Quality" dataDxfId="63">
+    <tableColumn id="1" name="Id" dataDxfId="69"/>
+    <tableColumn id="2" name="Name" dataDxfId="68"/>
+    <tableColumn id="20" name="Ename" dataDxfId="67"/>
+    <tableColumn id="21" name="Remark" dataDxfId="66"/>
+    <tableColumn id="3" name="Star" dataDxfId="65"/>
+    <tableColumn id="4" name="Type" dataDxfId="64"/>
+    <tableColumn id="5" name="Attr" dataDxfId="63"/>
+    <tableColumn id="8" name="Quality" dataDxfId="62">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="62"/>
-    <tableColumn id="9" name="Damage" dataDxfId="61"/>
-    <tableColumn id="10" name="Cure" dataDxfId="60"/>
-    <tableColumn id="11" name="Time" dataDxfId="59"/>
-    <tableColumn id="13" name="Help" dataDxfId="58"/>
-    <tableColumn id="16" name="Rate" dataDxfId="57"/>
-    <tableColumn id="18" name="Atk" dataDxfId="56"/>
-    <tableColumn id="12" name="Modify" dataDxfId="55"/>
-    <tableColumn id="27" name="Sum" dataDxfId="54">
+    <tableColumn id="7" name="Cost" dataDxfId="61"/>
+    <tableColumn id="9" name="Damage" dataDxfId="60"/>
+    <tableColumn id="10" name="Cure" dataDxfId="59"/>
+    <tableColumn id="11" name="Time" dataDxfId="58"/>
+    <tableColumn id="13" name="Help" dataDxfId="57"/>
+    <tableColumn id="16" name="Rate" dataDxfId="56"/>
+    <tableColumn id="18" name="Atk" dataDxfId="55"/>
+    <tableColumn id="12" name="Modify" dataDxfId="54"/>
+    <tableColumn id="27" name="Sum" dataDxfId="53">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="53"/>
-    <tableColumn id="15" name="Target" dataDxfId="52"/>
-    <tableColumn id="25" name="Mark" dataDxfId="51"/>
-    <tableColumn id="22" name="Effect" dataDxfId="50"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="49"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="48"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="47"/>
-    <tableColumn id="26" name="JobId" dataDxfId="46"/>
-    <tableColumn id="19" name="Icon" dataDxfId="45"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="44"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="43"/>
+    <tableColumn id="6" name="Range" dataDxfId="52"/>
+    <tableColumn id="15" name="Target" dataDxfId="51"/>
+    <tableColumn id="25" name="Mark" dataDxfId="50"/>
+    <tableColumn id="22" name="Effect" dataDxfId="49"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="48"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="47"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="46"/>
+    <tableColumn id="26" name="JobId" dataDxfId="45"/>
+    <tableColumn id="19" name="Icon" dataDxfId="44"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="43"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_35" displayName="表1_35" ref="A3:AB9" totalsRowShown="0" headerRowDxfId="30" tableBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_35" displayName="表1_35" ref="A3:AB9" totalsRowShown="0" headerRowDxfId="29" tableBorderDxfId="28">
   <autoFilter ref="A3:AB9"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="28"/>
-    <tableColumn id="2" name="Name" dataDxfId="27"/>
-    <tableColumn id="20" name="Ename" dataDxfId="26"/>
-    <tableColumn id="21" name="Remark" dataDxfId="25"/>
-    <tableColumn id="3" name="Star" dataDxfId="24"/>
-    <tableColumn id="4" name="Type" dataDxfId="23"/>
-    <tableColumn id="5" name="Attr" dataDxfId="22"/>
-    <tableColumn id="8" name="Quality" dataDxfId="21">
+    <tableColumn id="1" name="Id" dataDxfId="27"/>
+    <tableColumn id="2" name="Name" dataDxfId="26"/>
+    <tableColumn id="20" name="Ename" dataDxfId="25"/>
+    <tableColumn id="21" name="Remark" dataDxfId="24"/>
+    <tableColumn id="3" name="Star" dataDxfId="23"/>
+    <tableColumn id="4" name="Type" dataDxfId="22"/>
+    <tableColumn id="5" name="Attr" dataDxfId="21"/>
+    <tableColumn id="8" name="Quality" dataDxfId="20">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="20"/>
-    <tableColumn id="9" name="Damage" dataDxfId="19"/>
-    <tableColumn id="10" name="Cure" dataDxfId="18"/>
-    <tableColumn id="11" name="Time" dataDxfId="17"/>
-    <tableColumn id="13" name="Help" dataDxfId="16"/>
-    <tableColumn id="16" name="Rate" dataDxfId="15"/>
-    <tableColumn id="18" name="Atk" dataDxfId="14"/>
-    <tableColumn id="12" name="Modify" dataDxfId="13"/>
-    <tableColumn id="27" name="Sum" dataDxfId="12">
+    <tableColumn id="7" name="Cost" dataDxfId="19"/>
+    <tableColumn id="9" name="Damage" dataDxfId="18"/>
+    <tableColumn id="10" name="Cure" dataDxfId="17"/>
+    <tableColumn id="11" name="Time" dataDxfId="16"/>
+    <tableColumn id="13" name="Help" dataDxfId="15"/>
+    <tableColumn id="16" name="Rate" dataDxfId="14"/>
+    <tableColumn id="18" name="Atk" dataDxfId="13"/>
+    <tableColumn id="12" name="Modify" dataDxfId="12"/>
+    <tableColumn id="27" name="Sum" dataDxfId="11">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="11"/>
-    <tableColumn id="15" name="Target" dataDxfId="10"/>
-    <tableColumn id="25" name="Mark" dataDxfId="9"/>
-    <tableColumn id="22" name="Effect" dataDxfId="8"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="7"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="6"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="5"/>
-    <tableColumn id="26" name="JobId" dataDxfId="4"/>
-    <tableColumn id="19" name="Icon" dataDxfId="3"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="2"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="1"/>
+    <tableColumn id="6" name="Range" dataDxfId="10"/>
+    <tableColumn id="15" name="Target" dataDxfId="9"/>
+    <tableColumn id="25" name="Mark" dataDxfId="8"/>
+    <tableColumn id="22" name="Effect" dataDxfId="7"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="6"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="5"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="4"/>
+    <tableColumn id="26" name="JobId" dataDxfId="3"/>
+    <tableColumn id="19" name="Icon" dataDxfId="2"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="1"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9380,7 +9373,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9727,10 +9720,10 @@
         <v>95</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>904</v>
+        <v>896</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>906</v>
+        <v>898</v>
       </c>
       <c r="W4" s="1" t="s">
         <v>2</v>
@@ -12199,10 +12192,10 @@
         <v>100</v>
       </c>
       <c r="U33" s="11" t="s">
-        <v>880</v>
+        <v>914</v>
       </c>
       <c r="V33" s="1" t="s">
-        <v>914</v>
+        <v>906</v>
       </c>
       <c r="W33" s="1" t="s">
         <v>4</v>
@@ -12285,10 +12278,10 @@
         <v>100</v>
       </c>
       <c r="U34" s="11" t="s">
-        <v>881</v>
+        <v>915</v>
       </c>
       <c r="V34" s="1" t="s">
-        <v>916</v>
+        <v>908</v>
       </c>
       <c r="W34" s="1" t="s">
         <v>4</v>
@@ -12979,10 +12972,10 @@
         <v>85</v>
       </c>
       <c r="U42" s="11" t="s">
-        <v>882</v>
+        <v>916</v>
       </c>
       <c r="V42" s="1" t="s">
-        <v>915</v>
+        <v>907</v>
       </c>
       <c r="W42" s="1" t="s">
         <v>4</v>
@@ -13065,10 +13058,10 @@
         <v>100</v>
       </c>
       <c r="U43" s="11" t="s">
-        <v>883</v>
+        <v>917</v>
       </c>
       <c r="V43" s="1" t="s">
-        <v>917</v>
+        <v>909</v>
       </c>
       <c r="W43" s="1" t="s">
         <v>4</v>
@@ -13409,10 +13402,10 @@
         <v>95</v>
       </c>
       <c r="U47" s="11" t="s">
-        <v>884</v>
+        <v>918</v>
       </c>
       <c r="V47" s="1" t="s">
-        <v>918</v>
+        <v>910</v>
       </c>
       <c r="W47" s="1" t="s">
         <v>4</v>
@@ -15307,10 +15300,10 @@
         <v>85</v>
       </c>
       <c r="U69" s="11" t="s">
-        <v>885</v>
+        <v>919</v>
       </c>
       <c r="V69" s="1" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
       <c r="W69" s="1" t="s">
         <v>4</v>
@@ -21121,10 +21114,10 @@
         <v>100</v>
       </c>
       <c r="U136" s="11" t="s">
-        <v>886</v>
+        <v>920</v>
       </c>
       <c r="V136" s="1" t="s">
-        <v>920</v>
+        <v>912</v>
       </c>
       <c r="W136" s="15" t="s">
         <v>4</v>
@@ -21148,10 +21141,10 @@
         <v>53000134</v>
       </c>
       <c r="B137" s="22" t="s">
-        <v>888</v>
+        <v>881</v>
       </c>
       <c r="C137" s="15" t="s">
-        <v>887</v>
+        <v>880</v>
       </c>
       <c r="D137" s="25" t="s">
         <v>879</v>
@@ -21207,10 +21200,10 @@
         <v>103</v>
       </c>
       <c r="U137" s="11" t="s">
-        <v>889</v>
+        <v>921</v>
       </c>
       <c r="V137" s="1" t="s">
-        <v>921</v>
+        <v>913</v>
       </c>
       <c r="W137" s="15" t="s">
         <v>4</v>
@@ -21234,13 +21227,13 @@
         <v>53000135</v>
       </c>
       <c r="B138" s="22" t="s">
-        <v>892</v>
+        <v>884</v>
       </c>
       <c r="C138" s="15" t="s">
-        <v>893</v>
+        <v>885</v>
       </c>
       <c r="D138" s="25" t="s">
-        <v>897</v>
+        <v>889</v>
       </c>
       <c r="E138" s="15">
         <v>4</v>
@@ -21287,16 +21280,16 @@
         <v>20</v>
       </c>
       <c r="S138" s="15" t="s">
-        <v>898</v>
+        <v>890</v>
       </c>
       <c r="T138" s="15">
         <v>108</v>
       </c>
       <c r="U138" s="11" t="s">
-        <v>900</v>
+        <v>892</v>
       </c>
       <c r="V138" s="1" t="s">
-        <v>902</v>
+        <v>894</v>
       </c>
       <c r="W138" s="1" t="s">
         <v>871</v>
@@ -21320,13 +21313,13 @@
         <v>53000136</v>
       </c>
       <c r="B139" s="22" t="s">
-        <v>895</v>
+        <v>887</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>894</v>
+        <v>886</v>
       </c>
       <c r="D139" s="25" t="s">
-        <v>896</v>
+        <v>888</v>
       </c>
       <c r="E139" s="15">
         <v>4</v>
@@ -21373,16 +21366,16 @@
         <v>20</v>
       </c>
       <c r="S139" s="15" t="s">
-        <v>903</v>
+        <v>895</v>
       </c>
       <c r="T139" s="15">
         <v>100</v>
       </c>
       <c r="U139" s="11" t="s">
-        <v>905</v>
+        <v>897</v>
       </c>
       <c r="V139" s="1" t="s">
-        <v>907</v>
+        <v>899</v>
       </c>
       <c r="W139" s="15" t="s">
         <v>4</v>
@@ -21406,13 +21399,13 @@
         <v>53000137</v>
       </c>
       <c r="B140" s="22" t="s">
-        <v>908</v>
+        <v>900</v>
       </c>
       <c r="C140" s="15" t="s">
-        <v>909</v>
+        <v>901</v>
       </c>
       <c r="D140" s="25" t="s">
-        <v>910</v>
+        <v>902</v>
       </c>
       <c r="E140" s="15">
         <v>2</v>
@@ -21459,16 +21452,16 @@
         <v>0</v>
       </c>
       <c r="S140" s="15" t="s">
-        <v>913</v>
+        <v>905</v>
       </c>
       <c r="T140" s="15">
         <v>102</v>
       </c>
       <c r="U140" s="11" t="s">
-        <v>911</v>
+        <v>903</v>
       </c>
       <c r="V140" s="1" t="s">
-        <v>912</v>
+        <v>904</v>
       </c>
       <c r="W140" s="15" t="s">
         <v>4</v>
@@ -21493,173 +21486,173 @@
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I4:I15 I70:I122 I17:I35 I38:I68">
-    <cfRule type="cellIs" dxfId="167" priority="79" operator="notEqual">
+    <cfRule type="cellIs" dxfId="166" priority="79" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:N15 P38:Q68 P5:Q15 P17:Q35 P4 P70:Q122 J70:N122 J17:N35 J38:N68 N69 N136:N137">
-    <cfRule type="cellIs" dxfId="166" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="78" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J69:M69 P69:Q69">
-    <cfRule type="cellIs" dxfId="165" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="42" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36">
-    <cfRule type="cellIs" dxfId="164" priority="41" operator="notEqual">
+    <cfRule type="cellIs" dxfId="163" priority="41" operator="notEqual">
       <formula>$E36</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J36:N36 P36:Q36">
-    <cfRule type="cellIs" dxfId="163" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="40" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37">
-    <cfRule type="cellIs" dxfId="162" priority="39" operator="notEqual">
+    <cfRule type="cellIs" dxfId="161" priority="39" operator="notEqual">
       <formula>$E37</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J37:N37 P37:Q37">
-    <cfRule type="cellIs" dxfId="161" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="38" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H15 H17:H122">
-    <cfRule type="cellIs" dxfId="160" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="34" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="159" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="35" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="36" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="37" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="156" priority="37" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="cellIs" dxfId="156" priority="31" operator="notEqual">
+    <cfRule type="cellIs" dxfId="155" priority="31" operator="notEqual">
       <formula>$E16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:N16 P16:Q16">
-    <cfRule type="cellIs" dxfId="155" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="30" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="cellIs" dxfId="154" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="26" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="153" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="27" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="28" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="151" priority="29" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="150" priority="29" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D122 D141:D1048576">
-    <cfRule type="containsText" dxfId="150" priority="25" operator="containsText" text="未完成">
+    <cfRule type="containsText" dxfId="149" priority="25" operator="containsText" text="未完成">
       <formula>NOT(ISERROR(SEARCH("未完成",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:O134">
-    <cfRule type="cellIs" dxfId="149" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="24" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I123:I135">
-    <cfRule type="cellIs" dxfId="148" priority="23" operator="notEqual">
+    <cfRule type="cellIs" dxfId="147" priority="23" operator="notEqual">
       <formula>$E123</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J123:N134 P123:Q134">
-    <cfRule type="cellIs" dxfId="147" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="22" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H123:H135">
-    <cfRule type="cellIs" dxfId="146" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="18" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="19" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="20" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="21" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="142" priority="21" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O123:O134">
-    <cfRule type="cellIs" dxfId="142" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="16" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123:D135">
-    <cfRule type="containsText" dxfId="141" priority="15" operator="containsText" text="未完成">
+    <cfRule type="containsText" dxfId="140" priority="15" operator="containsText" text="未完成">
       <formula>NOT(ISERROR(SEARCH("未完成",D123)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O135">
-    <cfRule type="cellIs" dxfId="140" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="14" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J135:N135 P135:Q135">
-    <cfRule type="cellIs" dxfId="139" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="13" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O135">
-    <cfRule type="cellIs" dxfId="138" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="12" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I138:I140">
-    <cfRule type="cellIs" dxfId="137" priority="11" operator="notEqual">
+    <cfRule type="cellIs" dxfId="136" priority="11" operator="notEqual">
       <formula>$E138</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J138:N140 P136:Q140 J136:M137">
-    <cfRule type="cellIs" dxfId="136" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H136:H140">
-    <cfRule type="cellIs" dxfId="135" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="7" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="8" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="131" priority="9" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O136:O140">
-    <cfRule type="cellIs" dxfId="131" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D136:D140">
-    <cfRule type="containsText" dxfId="130" priority="3" operator="containsText" text="未完成">
+    <cfRule type="containsText" dxfId="129" priority="3" operator="containsText" text="未完成">
       <formula>NOT(ISERROR(SEARCH("未完成",D136)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I136:I137 I69">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="128" priority="1" operator="notEqual">
       <formula>$E69</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22181,10 +22174,10 @@
         <v>-1</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>899</v>
+        <v>891</v>
       </c>
       <c r="V6" s="7" t="s">
-        <v>901</v>
+        <v>893</v>
       </c>
       <c r="W6" s="15" t="s">
         <v>365</v>
@@ -22261,10 +22254,10 @@
         <v>-1</v>
       </c>
       <c r="U7" s="11" t="s">
-        <v>890</v>
+        <v>882</v>
       </c>
       <c r="V7" s="7" t="s">
-        <v>891</v>
+        <v>883</v>
       </c>
       <c r="W7" s="15" t="s">
         <v>2</v>
@@ -22684,110 +22677,110 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="J4:Q12">
-    <cfRule type="cellIs" dxfId="97" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="40" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:Q8">
-    <cfRule type="cellIs" dxfId="96" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="36" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:Q4 O4:O12">
-    <cfRule type="cellIs" dxfId="95" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="35" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="94" priority="34" operator="notEqual">
+    <cfRule type="cellIs" dxfId="93" priority="34" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:Q4 O4:O12">
-    <cfRule type="cellIs" dxfId="93" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="33" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="92" priority="32" operator="notEqual">
+    <cfRule type="cellIs" dxfId="91" priority="32" operator="notEqual">
       <formula>$E5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:Q5">
-    <cfRule type="cellIs" dxfId="91" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="31" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" dxfId="90" priority="30" operator="notEqual">
+    <cfRule type="cellIs" dxfId="89" priority="30" operator="notEqual">
       <formula>$E6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:Q6">
-    <cfRule type="cellIs" dxfId="89" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="29" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="88" priority="28" operator="notEqual">
+    <cfRule type="cellIs" dxfId="87" priority="28" operator="notEqual">
       <formula>$E7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:Q7">
-    <cfRule type="cellIs" dxfId="87" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="27" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="86" priority="26" operator="notEqual">
+    <cfRule type="cellIs" dxfId="85" priority="26" operator="notEqual">
       <formula>$E8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:Q8">
-    <cfRule type="cellIs" dxfId="85" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="25" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I12">
-    <cfRule type="cellIs" dxfId="84" priority="24" operator="notEqual">
+    <cfRule type="cellIs" dxfId="83" priority="24" operator="notEqual">
       <formula>$E9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:Q12">
-    <cfRule type="cellIs" dxfId="83" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="23" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H12">
-    <cfRule type="cellIs" dxfId="82" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="7" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="8" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="78" priority="9" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="78" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="4" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="74" priority="5" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10:L12">
-    <cfRule type="cellIs" dxfId="74" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23597,50 +23590,50 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I4:I9">
-    <cfRule type="cellIs" dxfId="42" priority="12" operator="notEqual">
+    <cfRule type="cellIs" dxfId="41" priority="12" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:Q7 O4:O9">
-    <cfRule type="cellIs" dxfId="41" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:Q9">
-    <cfRule type="cellIs" dxfId="40" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:Q8">
-    <cfRule type="cellIs" dxfId="39" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H9">
-    <cfRule type="cellIs" dxfId="38" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="6" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="34" priority="8" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="34" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="30" priority="4" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
integegrade the discover with a spell
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -636,7 +636,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="922">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="925">
   <si>
     <t>慈悲</t>
   </si>
@@ -4000,6 +4000,18 @@
   </si>
   <si>
     <t>p.AddTrap(54000008,s.Id,lv,s.Rate,0,0);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>p.DiscoverCardType(null,3,lv);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>符文石</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>发现一张法术</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -8142,7 +8154,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>8</c:v>
@@ -8915,8 +8927,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AB140" totalsRowShown="0" headerRowDxfId="127" dataDxfId="126" tableBorderDxfId="125">
-  <autoFilter ref="A3:AB140"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AB141" totalsRowShown="0" headerRowDxfId="127" dataDxfId="126" tableBorderDxfId="125">
+  <autoFilter ref="A3:AB141"/>
   <sortState ref="A4:AB113">
     <sortCondition ref="A3:A113"/>
   </sortState>
@@ -9367,13 +9379,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB140"/>
+  <dimension ref="A1:AB141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C136" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="U7" sqref="U7"/>
+      <selection pane="bottomRight" activeCell="T139" sqref="T139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -21477,6 +21489,92 @@
         <v>0</v>
       </c>
       <c r="AB140" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:28" ht="24" x14ac:dyDescent="0.15">
+      <c r="A141">
+        <v>53000138</v>
+      </c>
+      <c r="B141" s="22" t="s">
+        <v>923</v>
+      </c>
+      <c r="C141" s="15" t="s">
+        <v>901</v>
+      </c>
+      <c r="D141" s="25" t="s">
+        <v>411</v>
+      </c>
+      <c r="E141" s="15">
+        <v>2</v>
+      </c>
+      <c r="F141" s="15">
+        <v>201</v>
+      </c>
+      <c r="G141" s="15">
+        <v>0</v>
+      </c>
+      <c r="H141" s="43">
+        <f t="shared" ref="H141" si="54">IF(AND(Q141&gt;=13,Q141&lt;=16),5,IF(AND(Q141&gt;=9,Q141&lt;=12),4,IF(AND(Q141&gt;=5,Q141&lt;=8),3,IF(AND(Q141&gt;=1,Q141&lt;=4),2,IF(AND(Q141&gt;=-3,Q141&lt;=0),1,IF(AND(Q141&gt;=-5,Q141&lt;=-4),0,6))))))</f>
+        <v>2</v>
+      </c>
+      <c r="I141" s="15">
+        <v>2</v>
+      </c>
+      <c r="J141" s="15">
+        <v>0</v>
+      </c>
+      <c r="K141" s="15">
+        <v>0</v>
+      </c>
+      <c r="L141" s="15">
+        <v>0</v>
+      </c>
+      <c r="M141" s="15">
+        <v>0</v>
+      </c>
+      <c r="N141" s="15">
+        <v>20</v>
+      </c>
+      <c r="O141" s="15">
+        <v>0</v>
+      </c>
+      <c r="P141" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q141" s="43">
+        <f t="shared" ref="Q141" si="55">T141-100+P141</f>
+        <v>3</v>
+      </c>
+      <c r="R141" s="15">
+        <v>1</v>
+      </c>
+      <c r="S141" s="15" t="s">
+        <v>768</v>
+      </c>
+      <c r="T141" s="15">
+        <v>103</v>
+      </c>
+      <c r="U141" s="11" t="s">
+        <v>922</v>
+      </c>
+      <c r="V141" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="W141" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="X141" s="15"/>
+      <c r="Y141" s="15">
+        <v>11000004</v>
+      </c>
+      <c r="Z141" s="15">
+        <v>137</v>
+      </c>
+      <c r="AA141" s="27">
+        <v>0</v>
+      </c>
+      <c r="AB141" s="25">
         <v>1</v>
       </c>
     </row>
@@ -21558,7 +21656,7 @@
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D122 D141:D1048576">
+  <conditionalFormatting sqref="D1:D122 D142:D1048576">
     <cfRule type="containsText" dxfId="149" priority="25" operator="containsText" text="未完成">
       <formula>NOT(ISERROR(SEARCH("未完成",D1)))</formula>
     </cfRule>
@@ -21617,17 +21715,17 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I138:I140">
+  <conditionalFormatting sqref="I138:I141">
     <cfRule type="cellIs" dxfId="136" priority="11" operator="notEqual">
       <formula>$E138</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J138:N140 P136:Q140 J136:M137">
+  <conditionalFormatting sqref="J136:M137 J138:N141 P136:Q141">
     <cfRule type="cellIs" dxfId="135" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H136:H140">
+  <conditionalFormatting sqref="H136:H141">
     <cfRule type="cellIs" dxfId="134" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
@@ -21641,12 +21739,12 @@
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O136:O140">
+  <conditionalFormatting sqref="O136:O141">
     <cfRule type="cellIs" dxfId="130" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D136:D140">
+  <conditionalFormatting sqref="D136:D141">
     <cfRule type="containsText" dxfId="129" priority="3" operator="containsText" text="未完成">
       <formula>NOT(ISERROR(SEARCH("未完成",D136)))</formula>
     </cfRule>
@@ -23928,7 +24026,7 @@
       </c>
       <c r="B8">
         <f>COUNTIF(标准!D:D,"*手牌*")</f>
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
optimise the feeling of select card
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -636,7 +636,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="925">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="926">
   <si>
     <t>慈悲</t>
   </si>
@@ -4007,11 +4007,15 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>符文石</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>发现一张法术</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>雕文石板</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Glyphic Tablet</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -9385,7 +9389,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C136" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="T139" sqref="T139"/>
+      <selection pane="bottomRight" activeCell="W141" sqref="W141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -19835,7 +19839,7 @@
         <v>0</v>
       </c>
       <c r="AB121" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:28" ht="36" x14ac:dyDescent="0.15">
@@ -19921,7 +19925,7 @@
         <v>0</v>
       </c>
       <c r="AB122" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:28" x14ac:dyDescent="0.15">
@@ -20007,7 +20011,7 @@
         <v>0</v>
       </c>
       <c r="AB123" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:28" ht="60" x14ac:dyDescent="0.15">
@@ -20095,7 +20099,7 @@
         <v>0</v>
       </c>
       <c r="AB124" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:28" ht="24" x14ac:dyDescent="0.15">
@@ -20183,7 +20187,7 @@
         <v>0</v>
       </c>
       <c r="AB125" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:28" ht="36" x14ac:dyDescent="0.15">
@@ -20271,7 +20275,7 @@
         <v>0</v>
       </c>
       <c r="AB126" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:28" ht="36" x14ac:dyDescent="0.15">
@@ -20359,7 +20363,7 @@
         <v>0</v>
       </c>
       <c r="AB127" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:28" ht="48" x14ac:dyDescent="0.15">
@@ -20447,7 +20451,7 @@
         <v>0</v>
       </c>
       <c r="AB128" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:28" ht="48" x14ac:dyDescent="0.15">
@@ -20533,7 +20537,7 @@
         <v>0</v>
       </c>
       <c r="AB129" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:28" ht="60" x14ac:dyDescent="0.15">
@@ -20619,7 +20623,7 @@
         <v>0</v>
       </c>
       <c r="AB130" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:28" ht="60" x14ac:dyDescent="0.15">
@@ -20707,7 +20711,7 @@
         <v>0</v>
       </c>
       <c r="AB131" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:28" ht="36" x14ac:dyDescent="0.15">
@@ -20795,7 +20799,7 @@
         <v>0</v>
       </c>
       <c r="AB132" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:28" ht="84" x14ac:dyDescent="0.15">
@@ -20883,7 +20887,7 @@
         <v>0</v>
       </c>
       <c r="AB133" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:28" ht="60" x14ac:dyDescent="0.15">
@@ -20971,7 +20975,7 @@
         <v>0</v>
       </c>
       <c r="AB134" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:28" ht="24" x14ac:dyDescent="0.15">
@@ -21497,10 +21501,10 @@
         <v>53000138</v>
       </c>
       <c r="B141" s="22" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>901</v>
+        <v>925</v>
       </c>
       <c r="D141" s="25" t="s">
         <v>411</v>
@@ -21559,17 +21563,15 @@
         <v>922</v>
       </c>
       <c r="V141" s="1" t="s">
-        <v>924</v>
-      </c>
-      <c r="W141" s="15" t="s">
-        <v>4</v>
+        <v>923</v>
+      </c>
+      <c r="W141" s="1" t="s">
+        <v>767</v>
       </c>
       <c r="X141" s="15"/>
-      <c r="Y141" s="15">
-        <v>11000004</v>
-      </c>
+      <c r="Y141" s="15"/>
       <c r="Z141" s="15">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AA141" s="27">
         <v>0</v>

</xml_diff>

<commit_message>
fix a bug of cardflow would show tip when not
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -3899,123 +3899,123 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>int count=2;if(MathTool.GetRandom(100)&lt;s.Rate)count=3;foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse).SortRandom().Top(count)){im.OnMagicDamage(null,s.Damage,s.Attr);}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>抽1张卡片,{4:0.0}%几率抽额外1张卡牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对范围内随机2-3个单位造成{0}点魔法伤害，{4:0.0}%几率造成3个单位受伤</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>照明弹</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flare</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>手牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>r.RemoveRandomTrap();if(MathTool.GetRandom(100)&lt;s.Rate)r.RemoveRandomTrap();p.GetNextNCard(null,1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>抽1张卡片，随机消除对方1-2个陷阱（{4:0.0}%几率消除2个）</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NEO</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>陷阱：对方召唤时，冰冻目标5回合。触发需求MP:1，{4:0.0}%不消耗MP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>陷阱：对方使用卡牌时，额外消耗1倍费用。触发需求MP:1，{4:0.0}%不消耗MP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>陷阱：对方召唤时，对目标造成{0}点魔法伤害。触发需求MP:1，{4:0.0}%不消耗MP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>陷阱：对方使用的下张魔法卡无效。触发需求MP:1，{4:0.0}%不消耗MP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>陷阱：对方使用的下张卡牌无效。触发需求MP:3，{4:0.0}%不消耗MP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>陷阱：对方使用的下张武器卡无效。触发需求MP:1，{4:0.0}%不消耗MP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>陷阱：对方召唤时，将目标移回手牌，并提升{3}点费用。触发需求MP:1，{4:0.0}%不消耗MP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>陷阱：对方召唤时，如果目标星级低于3，使目标反叛。触发需求MP:1，{4:0.0}%不消耗MP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>p.AddTrap(54000005,s.Id,lv,s.Rate,0,0);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>p.AddTrap(54000006,s.Id,lv,s.Rate,s.Damage,0);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>p.AddTrap(54000004,s.Id,lv,s.Rate,0,0);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>p.AddTrap(54000002,s.Id,lv,s.Rate,0,0);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>p.AddTrap(54000003,s.Id,lv,s.Rate,0,0);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>p.AddTrap(54000001,s.Id,lv,s.Rate,0,0);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>p.AddTrap(54000007,s.Id,lv,s.Rate,0,s.Help);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>p.AddTrap(54000008,s.Id,lv,s.Rate,0,0);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>雕文石板</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Glyphic Tablet</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>发现一张法术,{4:0.0}%几率发现的卡牌等级+1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>p.GetNextNCard(null,1);if(MathTool.GetRandom(100)&lt;s.Rate) p.GetNextNCard(null,1);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>int count=2;if(MathTool.GetRandom(100)&lt;s.Rate)count=3;foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse).SortRandom().Top(count)){im.OnMagicDamage(null,s.Damage,s.Attr);}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>抽1张卡片,{4:0.0}%几率抽额外1张卡牌</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对范围内随机2-3个单位造成{0}点魔法伤害，{4:0.0}%几率造成3个单位受伤</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>照明弹</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Flare</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>手牌</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>r.RemoveRandomTrap();if(MathTool.GetRandom(100)&lt;s.Rate)r.RemoveRandomTrap();p.GetNextNCard(null,1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>抽1张卡片，随机消除对方1-2个陷阱（{4:0.0}%几率消除2个）</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>NEO</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>陷阱：对方召唤时，冰冻目标5回合。触发需求MP:1，{4:0.0}%不消耗MP</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>陷阱：对方使用卡牌时，额外消耗1倍费用。触发需求MP:1，{4:0.0}%不消耗MP</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>陷阱：对方召唤时，对目标造成{0}点魔法伤害。触发需求MP:1，{4:0.0}%不消耗MP</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>陷阱：对方使用的下张魔法卡无效。触发需求MP:1，{4:0.0}%不消耗MP</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>陷阱：对方使用的下张卡牌无效。触发需求MP:3，{4:0.0}%不消耗MP</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>陷阱：对方使用的下张武器卡无效。触发需求MP:1，{4:0.0}%不消耗MP</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>陷阱：对方召唤时，将目标移回手牌，并提升{3}点费用。触发需求MP:1，{4:0.0}%不消耗MP</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>陷阱：对方召唤时，如果目标星级低于3，使目标反叛。触发需求MP:1，{4:0.0}%不消耗MP</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>p.AddTrap(54000005,s.Id,lv,s.Rate,0,0);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>p.AddTrap(54000006,s.Id,lv,s.Rate,s.Damage,0);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>p.AddTrap(54000004,s.Id,lv,s.Rate,0,0);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>p.AddTrap(54000002,s.Id,lv,s.Rate,0,0);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>p.AddTrap(54000003,s.Id,lv,s.Rate,0,0);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>p.AddTrap(54000001,s.Id,lv,s.Rate,0,0);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>p.AddTrap(54000007,s.Id,lv,s.Rate,0,s.Help);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>p.AddTrap(54000008,s.Id,lv,s.Rate,0,0);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>p.DiscoverCardType(null,3,lv);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>发现一张法术</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>雕文石板</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Glyphic Tablet</t>
+    <t>if(MathTool.GetRandom(100)&lt;s.Rate)lv++;p.DiscoverCardType(null,3,lv);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -9389,7 +9389,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C136" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W141" sqref="W141"/>
+      <selection pane="bottomRight" activeCell="U141" sqref="U141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9736,10 +9736,10 @@
         <v>95</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>896</v>
+        <v>924</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="W4" s="1" t="s">
         <v>2</v>
@@ -12208,10 +12208,10 @@
         <v>100</v>
       </c>
       <c r="U33" s="11" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="V33" s="1" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="W33" s="1" t="s">
         <v>4</v>
@@ -12294,10 +12294,10 @@
         <v>100</v>
       </c>
       <c r="U34" s="11" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="V34" s="1" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="W34" s="1" t="s">
         <v>4</v>
@@ -12988,10 +12988,10 @@
         <v>85</v>
       </c>
       <c r="U42" s="11" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="V42" s="1" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="W42" s="1" t="s">
         <v>4</v>
@@ -13074,10 +13074,10 @@
         <v>100</v>
       </c>
       <c r="U43" s="11" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="V43" s="1" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="W43" s="1" t="s">
         <v>4</v>
@@ -13418,10 +13418,10 @@
         <v>95</v>
       </c>
       <c r="U47" s="11" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="V47" s="1" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="W47" s="1" t="s">
         <v>4</v>
@@ -15316,10 +15316,10 @@
         <v>85</v>
       </c>
       <c r="U69" s="11" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="V69" s="1" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="W69" s="1" t="s">
         <v>4</v>
@@ -21130,10 +21130,10 @@
         <v>100</v>
       </c>
       <c r="U136" s="11" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="V136" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="W136" s="15" t="s">
         <v>4</v>
@@ -21216,10 +21216,10 @@
         <v>103</v>
       </c>
       <c r="U137" s="11" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="V137" s="1" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="W137" s="15" t="s">
         <v>4</v>
@@ -21388,10 +21388,10 @@
         <v>100</v>
       </c>
       <c r="U139" s="11" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="V139" s="1" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="W139" s="15" t="s">
         <v>4</v>
@@ -21415,13 +21415,13 @@
         <v>53000137</v>
       </c>
       <c r="B140" s="22" t="s">
+        <v>899</v>
+      </c>
+      <c r="C140" s="15" t="s">
         <v>900</v>
       </c>
-      <c r="C140" s="15" t="s">
+      <c r="D140" s="25" t="s">
         <v>901</v>
-      </c>
-      <c r="D140" s="25" t="s">
-        <v>902</v>
       </c>
       <c r="E140" s="15">
         <v>2</v>
@@ -21468,16 +21468,16 @@
         <v>0</v>
       </c>
       <c r="S140" s="15" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="T140" s="15">
         <v>102</v>
       </c>
       <c r="U140" s="11" t="s">
+        <v>902</v>
+      </c>
+      <c r="V140" s="1" t="s">
         <v>903</v>
-      </c>
-      <c r="V140" s="1" t="s">
-        <v>904</v>
       </c>
       <c r="W140" s="15" t="s">
         <v>4</v>
@@ -21496,15 +21496,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:28" ht="24" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:28" ht="36" x14ac:dyDescent="0.15">
       <c r="A141">
         <v>53000138</v>
       </c>
       <c r="B141" s="22" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
       <c r="D141" s="25" t="s">
         <v>411</v>
@@ -21513,14 +21513,14 @@
         <v>2</v>
       </c>
       <c r="F141" s="15">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G141" s="15">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H141" s="43">
         <f t="shared" ref="H141" si="54">IF(AND(Q141&gt;=13,Q141&lt;=16),5,IF(AND(Q141&gt;=9,Q141&lt;=12),4,IF(AND(Q141&gt;=5,Q141&lt;=8),3,IF(AND(Q141&gt;=1,Q141&lt;=4),2,IF(AND(Q141&gt;=-3,Q141&lt;=0),1,IF(AND(Q141&gt;=-5,Q141&lt;=-4),0,6))))))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I141" s="15">
         <v>2</v>
@@ -21548,7 +21548,7 @@
       </c>
       <c r="Q141" s="43">
         <f t="shared" ref="Q141" si="55">T141-100+P141</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R141" s="15">
         <v>1</v>
@@ -21557,10 +21557,10 @@
         <v>768</v>
       </c>
       <c r="T141" s="15">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="U141" s="11" t="s">
-        <v>922</v>
+        <v>925</v>
       </c>
       <c r="V141" s="1" t="s">
         <v>923</v>

</xml_diff>

<commit_message>
recalculate the def and mag effect of attr
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -3121,9 +3121,6 @@
     <t>t.OnMagicDamage(null, s.Damage*MathTool.GetRandom(85,115)/100,s.Attr);</t>
   </si>
   <si>
-    <t>foreach(IMonster im in m.GetAllMonster(mouse).FilterType(0))im.OnMagicDamage(null, s.Damage,s.Attr);</t>
-  </si>
-  <si>
     <t>t.OnMagicDamage(null, s.Damage,s.Attr);t.Silent();</t>
   </si>
   <si>
@@ -4056,6 +4053,10 @@
   </si>
   <si>
     <t>lockon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster im in m.GetAllMonster(mouse))im.OnMagicDamage(null, s.Damage,s.Attr);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -9419,10 +9420,10 @@
   <dimension ref="A1:AB143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C136" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C60" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W140" sqref="W140"/>
+      <selection pane="bottomRight" activeCell="U68" sqref="U68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9491,7 +9492,7 @@
         <v>349</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="P1" s="17" t="s">
         <v>331</v>
@@ -9577,7 +9578,7 @@
         <v>350</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>332</v>
@@ -9595,7 +9596,7 @@
         <v>490</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="V2" s="10" t="s">
         <v>179</v>
@@ -9663,7 +9664,7 @@
         <v>351</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="P3" s="20" t="s">
         <v>333</v>
@@ -9769,10 +9770,10 @@
         <v>95</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="W4" s="1" t="s">
         <v>2</v>
@@ -9937,7 +9938,7 @@
         <v>100</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="V6" s="7" t="s">
         <v>378</v>
@@ -10021,10 +10022,10 @@
         <v>100</v>
       </c>
       <c r="U7" s="11" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="V7" s="7" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="W7" s="1" t="s">
         <v>9</v>
@@ -10953,10 +10954,10 @@
         <v>75</v>
       </c>
       <c r="U18" s="11" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="V18" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="W18" s="1" t="s">
         <v>15</v>
@@ -11125,10 +11126,10 @@
         <v>100</v>
       </c>
       <c r="U20" s="11" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="V20" s="7" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="W20" s="1" t="s">
         <v>649</v>
@@ -11561,10 +11562,10 @@
         <v>107</v>
       </c>
       <c r="U25" s="11" t="s">
+        <v>813</v>
+      </c>
+      <c r="V25" s="7" t="s">
         <v>814</v>
-      </c>
-      <c r="V25" s="7" t="s">
-        <v>815</v>
       </c>
       <c r="W25" s="1" t="s">
         <v>29</v>
@@ -11731,7 +11732,7 @@
         <v>90</v>
       </c>
       <c r="U27" s="11" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="V27" s="7" t="s">
         <v>391</v>
@@ -12241,10 +12242,10 @@
         <v>100</v>
       </c>
       <c r="U33" s="11" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="V33" s="1" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="W33" s="1" t="s">
         <v>4</v>
@@ -12327,10 +12328,10 @@
         <v>100</v>
       </c>
       <c r="U34" s="11" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="V34" s="1" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="W34" s="1" t="s">
         <v>4</v>
@@ -12675,7 +12676,7 @@
         <v>100</v>
       </c>
       <c r="U38" s="11" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="V38" s="7" t="s">
         <v>617</v>
@@ -12880,7 +12881,7 @@
         <v>236</v>
       </c>
       <c r="D41" s="25" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="E41" s="1">
         <v>2</v>
@@ -12927,16 +12928,16 @@
         <v>12</v>
       </c>
       <c r="S41" s="1" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="T41">
         <v>100</v>
       </c>
       <c r="U41" s="11" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="V41" s="7" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="W41" s="1" t="s">
         <v>55</v>
@@ -13021,10 +13022,10 @@
         <v>85</v>
       </c>
       <c r="U42" s="11" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="V42" s="1" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="W42" s="1" t="s">
         <v>4</v>
@@ -13107,10 +13108,10 @@
         <v>100</v>
       </c>
       <c r="U43" s="11" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="V43" s="1" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="W43" s="1" t="s">
         <v>4</v>
@@ -13451,10 +13452,10 @@
         <v>95</v>
       </c>
       <c r="U47" s="11" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="V47" s="1" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="W47" s="1" t="s">
         <v>4</v>
@@ -13540,7 +13541,7 @@
         <v>687</v>
       </c>
       <c r="V48" s="1" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="W48" s="1" t="s">
         <v>322</v>
@@ -14139,16 +14140,16 @@
         <v>0</v>
       </c>
       <c r="S55" s="1" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="T55">
         <v>95</v>
       </c>
       <c r="U55" s="11" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="V55" s="7" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="W55" s="1" t="s">
         <v>611</v>
@@ -14655,16 +14656,16 @@
         <v>0</v>
       </c>
       <c r="S61" s="1" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="T61">
         <v>100</v>
       </c>
       <c r="U61" s="11" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="V61" s="7" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="W61" s="1" t="s">
         <v>15</v>
@@ -14747,10 +14748,10 @@
         <v>100</v>
       </c>
       <c r="U62" s="11" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="V62" s="7" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="W62" s="1" t="s">
         <v>83</v>
@@ -15263,7 +15264,7 @@
         <v>100</v>
       </c>
       <c r="U68" s="11" t="s">
-        <v>703</v>
+        <v>935</v>
       </c>
       <c r="V68" s="1" t="s">
         <v>403</v>
@@ -15349,10 +15350,10 @@
         <v>85</v>
       </c>
       <c r="U69" s="11" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="V69" s="1" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="W69" s="1" t="s">
         <v>4</v>
@@ -15435,7 +15436,7 @@
         <v>100</v>
       </c>
       <c r="U70" s="11" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="V70" s="7" t="s">
         <v>633</v>
@@ -15609,13 +15610,13 @@
         <v>100</v>
       </c>
       <c r="U72" s="11" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="V72" s="7" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="W72" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="X72" s="1"/>
       <c r="Y72" s="1">
@@ -15695,7 +15696,7 @@
         <v>100</v>
       </c>
       <c r="U73" s="11" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="V73" s="7" t="s">
         <v>550</v>
@@ -16390,7 +16391,7 @@
         <v>681</v>
       </c>
       <c r="V81" s="7" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="W81" s="1" t="s">
         <v>93</v>
@@ -16647,7 +16648,7 @@
         <v>100</v>
       </c>
       <c r="U84" s="11" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="V84" s="7" t="s">
         <v>594</v>
@@ -16735,10 +16736,10 @@
         <v>100</v>
       </c>
       <c r="U85" s="11" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="V85" s="7" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="W85" s="1" t="s">
         <v>122</v>
@@ -16821,7 +16822,7 @@
         <v>100</v>
       </c>
       <c r="U86" s="11" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="V86" s="7" t="s">
         <v>559</v>
@@ -17169,7 +17170,7 @@
         <v>100</v>
       </c>
       <c r="U90" s="11" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="V90" s="7" t="s">
         <v>596</v>
@@ -17519,7 +17520,7 @@
         <v>100</v>
       </c>
       <c r="U94" s="11" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="V94" s="7" t="s">
         <v>341</v>
@@ -17691,7 +17692,7 @@
         <v>100</v>
       </c>
       <c r="U96" s="11" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="V96" s="7" t="s">
         <v>583</v>
@@ -18209,7 +18210,7 @@
         <v>100</v>
       </c>
       <c r="U102" s="11" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="V102" s="7" t="s">
         <v>577</v>
@@ -18298,7 +18299,7 @@
         <v>684</v>
       </c>
       <c r="V103" s="1" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="W103" s="1" t="s">
         <v>144</v>
@@ -18553,10 +18554,10 @@
         <v>105</v>
       </c>
       <c r="U106" s="11" t="s">
+        <v>753</v>
+      </c>
+      <c r="V106" s="7" t="s">
         <v>754</v>
-      </c>
-      <c r="V106" s="7" t="s">
-        <v>755</v>
       </c>
       <c r="W106" s="1" t="s">
         <v>147</v>
@@ -18644,7 +18645,7 @@
         <v>636</v>
       </c>
       <c r="V107" s="7" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="W107" s="1" t="s">
         <v>149</v>
@@ -18813,10 +18814,10 @@
         <v>100</v>
       </c>
       <c r="U109" s="11" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="V109" s="7" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="W109" s="1" t="s">
         <v>153</v>
@@ -18899,10 +18900,10 @@
         <v>100</v>
       </c>
       <c r="U110" s="11" t="s">
+        <v>744</v>
+      </c>
+      <c r="V110" s="7" t="s">
         <v>745</v>
-      </c>
-      <c r="V110" s="7" t="s">
-        <v>746</v>
       </c>
       <c r="W110" s="1" t="s">
         <v>155</v>
@@ -19071,7 +19072,7 @@
         <v>100</v>
       </c>
       <c r="U112" s="11" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="V112" s="7" t="s">
         <v>563</v>
@@ -19157,10 +19158,10 @@
         <v>103</v>
       </c>
       <c r="U113" s="11" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="V113" s="7" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="W113" s="1" t="s">
         <v>29</v>
@@ -19360,10 +19361,10 @@
         <v>53000113</v>
       </c>
       <c r="B116" s="8" t="s">
+        <v>714</v>
+      </c>
+      <c r="C116" s="1" t="s">
         <v>715</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>716</v>
       </c>
       <c r="D116" s="25"/>
       <c r="E116" s="1">
@@ -19411,22 +19412,22 @@
         <v>0</v>
       </c>
       <c r="S116" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="T116">
         <v>100</v>
       </c>
       <c r="U116" s="11" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="V116" s="7" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="W116" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="X116" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="Y116" s="1">
         <v>11000003</v>
@@ -19446,10 +19447,10 @@
         <v>53000114</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D117" s="25"/>
       <c r="E117" s="1">
@@ -19497,16 +19498,16 @@
         <v>0</v>
       </c>
       <c r="S117" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="T117">
         <v>101</v>
       </c>
       <c r="U117" s="11" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="V117" s="7" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="W117" s="1" t="s">
         <v>99</v>
@@ -19532,10 +19533,10 @@
         <v>53000115</v>
       </c>
       <c r="B118" s="8" t="s">
+        <v>727</v>
+      </c>
+      <c r="C118" s="1" t="s">
         <v>728</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>729</v>
       </c>
       <c r="D118" s="25"/>
       <c r="E118" s="1">
@@ -19583,16 +19584,16 @@
         <v>0</v>
       </c>
       <c r="S118" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="T118">
         <v>100</v>
       </c>
       <c r="U118" s="11" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="V118" s="7" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="W118" s="1" t="s">
         <v>99</v>
@@ -19618,13 +19619,13 @@
         <v>53000116</v>
       </c>
       <c r="B119" s="8" t="s">
+        <v>733</v>
+      </c>
+      <c r="C119" s="1" t="s">
         <v>734</v>
       </c>
-      <c r="C119" s="1" t="s">
-        <v>735</v>
-      </c>
       <c r="D119" s="25" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="E119" s="1">
         <v>2</v>
@@ -19677,10 +19678,10 @@
         <v>101</v>
       </c>
       <c r="U119" s="11" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="V119" s="7" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="W119" s="1" t="s">
         <v>99</v>
@@ -19706,13 +19707,13 @@
         <v>53000117</v>
       </c>
       <c r="B120" s="8" t="s">
+        <v>737</v>
+      </c>
+      <c r="C120" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="C120" s="1" t="s">
-        <v>739</v>
-      </c>
       <c r="D120" s="25" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="E120" s="1">
         <v>1</v>
@@ -19759,16 +19760,16 @@
         <v>0</v>
       </c>
       <c r="S120" s="1" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="T120">
         <v>100</v>
       </c>
       <c r="U120" s="11" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="V120" s="7" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="W120" s="1" t="s">
         <v>99</v>
@@ -19794,10 +19795,10 @@
         <v>53000118</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="D121" s="25"/>
       <c r="E121" s="1">
@@ -19845,22 +19846,22 @@
         <v>0</v>
       </c>
       <c r="S121" s="1" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="T121">
         <v>100</v>
       </c>
       <c r="U121" s="11" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="V121" s="7" t="s">
+        <v>765</v>
+      </c>
+      <c r="W121" s="1" t="s">
         <v>766</v>
       </c>
-      <c r="W121" s="1" t="s">
-        <v>767</v>
-      </c>
       <c r="X121" s="1" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="Y121" s="1">
         <v>11000003</v>
@@ -19880,10 +19881,10 @@
         <v>53000119</v>
       </c>
       <c r="B122" s="8" t="s">
+        <v>769</v>
+      </c>
+      <c r="C122" s="1" t="s">
         <v>770</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>771</v>
       </c>
       <c r="D122" s="25"/>
       <c r="E122" s="1">
@@ -19931,22 +19932,22 @@
         <v>0</v>
       </c>
       <c r="S122" s="1" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="T122">
         <v>105</v>
       </c>
       <c r="U122" s="11" t="s">
+        <v>771</v>
+      </c>
+      <c r="V122" s="7" t="s">
         <v>772</v>
       </c>
-      <c r="V122" s="7" t="s">
+      <c r="W122" s="1" t="s">
         <v>773</v>
       </c>
-      <c r="W122" s="1" t="s">
-        <v>774</v>
-      </c>
       <c r="X122" s="1" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="Y122" s="1">
         <v>11000003</v>
@@ -19966,13 +19967,13 @@
         <v>53000120</v>
       </c>
       <c r="B123" s="22" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C123" s="15" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="D123" s="25" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="E123" s="15">
         <v>1</v>
@@ -20025,10 +20026,10 @@
         <v>100</v>
       </c>
       <c r="U123" s="11" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="V123" s="7" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="W123" s="15" t="s">
         <v>57</v>
@@ -20052,13 +20053,13 @@
         <v>53000121</v>
       </c>
       <c r="B124" s="22" t="s">
+        <v>781</v>
+      </c>
+      <c r="C124" s="15" t="s">
         <v>782</v>
       </c>
-      <c r="C124" s="15" t="s">
+      <c r="D124" s="25" t="s">
         <v>783</v>
-      </c>
-      <c r="D124" s="25" t="s">
-        <v>784</v>
       </c>
       <c r="E124" s="15">
         <v>1</v>
@@ -20105,22 +20106,22 @@
         <v>30</v>
       </c>
       <c r="S124" s="7" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="T124">
         <v>100</v>
       </c>
       <c r="U124" s="11" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="V124" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="W124" s="15" t="s">
         <v>786</v>
       </c>
-      <c r="W124" s="15" t="s">
-        <v>787</v>
-      </c>
       <c r="X124" s="15" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="Y124" s="1">
         <v>11000001</v>
@@ -20140,10 +20141,10 @@
         <v>53000122</v>
       </c>
       <c r="B125" s="22" t="s">
+        <v>787</v>
+      </c>
+      <c r="C125" s="15" t="s">
         <v>788</v>
-      </c>
-      <c r="C125" s="15" t="s">
-        <v>789</v>
       </c>
       <c r="D125" s="25" t="s">
         <v>669</v>
@@ -20193,22 +20194,22 @@
         <v>0</v>
       </c>
       <c r="S125" s="7" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="T125">
         <v>101</v>
       </c>
       <c r="U125" s="11" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="V125" s="1" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="W125" s="15" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="X125" s="15" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="Y125" s="1">
         <v>11000001</v>
@@ -20228,10 +20229,10 @@
         <v>53000123</v>
       </c>
       <c r="B126" s="22" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="C126" s="15" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="D126" s="25" t="s">
         <v>651</v>
@@ -20281,22 +20282,22 @@
         <v>0</v>
       </c>
       <c r="S126" s="7" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="T126">
         <v>100</v>
       </c>
       <c r="U126" s="11" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="V126" s="1" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="W126" s="15" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="X126" s="15" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="Y126" s="1">
         <v>11000001</v>
@@ -20316,13 +20317,13 @@
         <v>53000124</v>
       </c>
       <c r="B127" s="22" t="s">
+        <v>799</v>
+      </c>
+      <c r="C127" s="15" t="s">
         <v>800</v>
       </c>
-      <c r="C127" s="15" t="s">
+      <c r="D127" s="25" t="s">
         <v>801</v>
-      </c>
-      <c r="D127" s="25" t="s">
-        <v>802</v>
       </c>
       <c r="E127" s="15">
         <v>2</v>
@@ -20369,22 +20370,22 @@
         <v>0</v>
       </c>
       <c r="S127" s="7" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="T127">
         <v>101</v>
       </c>
       <c r="U127" s="11" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="V127" s="1" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="W127" s="15" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="X127" s="15" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="Y127" s="1">
         <v>11000001</v>
@@ -20404,13 +20405,13 @@
         <v>53000125</v>
       </c>
       <c r="B128" s="22" t="s">
+        <v>805</v>
+      </c>
+      <c r="C128" s="15" t="s">
         <v>806</v>
       </c>
-      <c r="C128" s="15" t="s">
+      <c r="D128" s="25" t="s">
         <v>807</v>
-      </c>
-      <c r="D128" s="25" t="s">
-        <v>808</v>
       </c>
       <c r="E128" s="15">
         <v>2</v>
@@ -20457,22 +20458,22 @@
         <v>0</v>
       </c>
       <c r="S128" s="7" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="T128">
         <v>100</v>
       </c>
       <c r="U128" s="11" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="V128" s="1" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="W128" s="15" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="X128" s="15" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="Y128" s="1">
         <v>11000002</v>
@@ -20492,10 +20493,10 @@
         <v>53000126</v>
       </c>
       <c r="B129" s="22" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C129" s="15" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D129" s="25"/>
       <c r="E129" s="15">
@@ -20543,22 +20544,22 @@
         <v>0</v>
       </c>
       <c r="S129" s="7" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="T129">
         <v>100</v>
       </c>
       <c r="U129" s="11" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="V129" s="1" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="W129" s="1" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="X129" s="1" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="Y129" s="1">
         <v>11000001</v>
@@ -20578,10 +20579,10 @@
         <v>53000127</v>
       </c>
       <c r="B130" s="22" t="s">
+        <v>817</v>
+      </c>
+      <c r="C130" s="15" t="s">
         <v>818</v>
-      </c>
-      <c r="C130" s="15" t="s">
-        <v>819</v>
       </c>
       <c r="D130" s="25"/>
       <c r="E130" s="15">
@@ -20629,22 +20630,22 @@
         <v>15</v>
       </c>
       <c r="S130" s="7" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="T130">
         <v>103</v>
       </c>
       <c r="U130" s="11" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="V130" s="1" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="W130" s="1" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="X130" s="1" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="Y130" s="1">
         <v>11000001</v>
@@ -20664,13 +20665,13 @@
         <v>53000128</v>
       </c>
       <c r="B131" s="22" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="D131" s="25" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="E131" s="15">
         <v>1</v>
@@ -20717,22 +20718,22 @@
         <v>25</v>
       </c>
       <c r="S131" s="7" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="T131">
         <v>100</v>
       </c>
       <c r="U131" s="11" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="V131" s="1" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="W131" s="1" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="X131" s="1" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="Y131" s="1">
         <v>11000001</v>
@@ -20752,13 +20753,13 @@
         <v>53000129</v>
       </c>
       <c r="B132" s="22" t="s">
+        <v>844</v>
+      </c>
+      <c r="C132" s="15" t="s">
+        <v>843</v>
+      </c>
+      <c r="D132" s="25" t="s">
         <v>845</v>
-      </c>
-      <c r="C132" s="15" t="s">
-        <v>844</v>
-      </c>
-      <c r="D132" s="25" t="s">
-        <v>846</v>
       </c>
       <c r="E132" s="15">
         <v>3</v>
@@ -20805,22 +20806,22 @@
         <v>0</v>
       </c>
       <c r="S132" s="7" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="T132">
         <v>103</v>
       </c>
       <c r="U132" s="11" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="V132" s="1" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="W132" s="1" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="X132" s="1" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="Y132" s="1">
         <v>11000002</v>
@@ -20840,13 +20841,13 @@
         <v>53000130</v>
       </c>
       <c r="B133" s="22" t="s">
+        <v>854</v>
+      </c>
+      <c r="C133" s="15" t="s">
         <v>855</v>
       </c>
-      <c r="C133" s="15" t="s">
-        <v>856</v>
-      </c>
       <c r="D133" s="25" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="E133" s="15">
         <v>5</v>
@@ -20893,22 +20894,22 @@
         <v>25</v>
       </c>
       <c r="S133" s="7" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="T133">
         <v>107</v>
       </c>
       <c r="U133" s="11" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="V133" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="W133" s="1" t="s">
         <v>860</v>
       </c>
-      <c r="W133" s="1" t="s">
-        <v>861</v>
-      </c>
       <c r="X133" s="1" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="Y133" s="1">
         <v>11000002</v>
@@ -20928,13 +20929,13 @@
         <v>53000131</v>
       </c>
       <c r="B134" s="22" t="s">
+        <v>861</v>
+      </c>
+      <c r="C134" s="15" t="s">
         <v>862</v>
       </c>
-      <c r="C134" s="15" t="s">
-        <v>863</v>
-      </c>
       <c r="D134" s="25" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="E134" s="15">
         <v>2</v>
@@ -20981,22 +20982,22 @@
         <v>30</v>
       </c>
       <c r="S134" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="T134">
         <v>100</v>
       </c>
       <c r="U134" s="11" t="s">
+        <v>868</v>
+      </c>
+      <c r="V134" s="1" t="s">
         <v>869</v>
       </c>
-      <c r="V134" s="1" t="s">
+      <c r="W134" s="1" t="s">
         <v>870</v>
       </c>
-      <c r="W134" s="1" t="s">
-        <v>871</v>
-      </c>
       <c r="X134" s="1" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="Y134" s="1">
         <v>11000002</v>
@@ -21016,13 +21017,13 @@
         <v>53000132</v>
       </c>
       <c r="B135" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="C135" s="15" t="s">
         <v>864</v>
       </c>
-      <c r="C135" s="15" t="s">
-        <v>865</v>
-      </c>
       <c r="D135" s="25" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="E135" s="15">
         <v>3</v>
@@ -21069,22 +21070,22 @@
         <v>0</v>
       </c>
       <c r="S135" s="7" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="T135">
         <v>102</v>
       </c>
       <c r="U135" s="11" t="s">
+        <v>872</v>
+      </c>
+      <c r="V135" s="1" t="s">
+        <v>875</v>
+      </c>
+      <c r="W135" s="1" t="s">
         <v>873</v>
       </c>
-      <c r="V135" s="1" t="s">
-        <v>876</v>
-      </c>
-      <c r="W135" s="1" t="s">
-        <v>874</v>
-      </c>
       <c r="X135" s="1" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="Y135" s="1">
         <v>11000002</v>
@@ -21104,13 +21105,13 @@
         <v>53000133</v>
       </c>
       <c r="B136" s="22" t="s">
+        <v>877</v>
+      </c>
+      <c r="C136" s="15" t="s">
+        <v>876</v>
+      </c>
+      <c r="D136" s="25" t="s">
         <v>878</v>
-      </c>
-      <c r="C136" s="15" t="s">
-        <v>877</v>
-      </c>
-      <c r="D136" s="25" t="s">
-        <v>879</v>
       </c>
       <c r="E136" s="15">
         <v>2</v>
@@ -21163,10 +21164,10 @@
         <v>100</v>
       </c>
       <c r="U136" s="11" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="V136" s="1" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="W136" s="15" t="s">
         <v>4</v>
@@ -21190,13 +21191,13 @@
         <v>53000134</v>
       </c>
       <c r="B137" s="22" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="C137" s="15" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="D137" s="25" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="E137" s="15">
         <v>2</v>
@@ -21249,10 +21250,10 @@
         <v>103</v>
       </c>
       <c r="U137" s="11" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="V137" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="W137" s="15" t="s">
         <v>4</v>
@@ -21276,13 +21277,13 @@
         <v>53000135</v>
       </c>
       <c r="B138" s="22" t="s">
+        <v>883</v>
+      </c>
+      <c r="C138" s="15" t="s">
         <v>884</v>
       </c>
-      <c r="C138" s="15" t="s">
-        <v>885</v>
-      </c>
       <c r="D138" s="25" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="E138" s="15">
         <v>4</v>
@@ -21329,19 +21330,19 @@
         <v>20</v>
       </c>
       <c r="S138" s="15" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="T138" s="15">
         <v>108</v>
       </c>
       <c r="U138" s="11" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="V138" s="1" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="W138" s="1" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="X138" s="15"/>
       <c r="Y138" s="15">
@@ -21362,13 +21363,13 @@
         <v>53000136</v>
       </c>
       <c r="B139" s="22" t="s">
+        <v>886</v>
+      </c>
+      <c r="C139" s="15" t="s">
+        <v>885</v>
+      </c>
+      <c r="D139" s="25" t="s">
         <v>887</v>
-      </c>
-      <c r="C139" s="15" t="s">
-        <v>886</v>
-      </c>
-      <c r="D139" s="25" t="s">
-        <v>888</v>
       </c>
       <c r="E139" s="15">
         <v>4</v>
@@ -21415,19 +21416,19 @@
         <v>20</v>
       </c>
       <c r="S139" s="15" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="T139" s="15">
         <v>100</v>
       </c>
       <c r="U139" s="11" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="V139" s="1" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="W139" s="15" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="X139" s="15"/>
       <c r="Y139" s="15">
@@ -21448,13 +21449,13 @@
         <v>53000137</v>
       </c>
       <c r="B140" s="22" t="s">
+        <v>898</v>
+      </c>
+      <c r="C140" s="15" t="s">
         <v>899</v>
       </c>
-      <c r="C140" s="15" t="s">
+      <c r="D140" s="25" t="s">
         <v>900</v>
-      </c>
-      <c r="D140" s="25" t="s">
-        <v>901</v>
       </c>
       <c r="E140" s="15">
         <v>2</v>
@@ -21501,16 +21502,16 @@
         <v>0</v>
       </c>
       <c r="S140" s="15" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="T140" s="15">
         <v>102</v>
       </c>
       <c r="U140" s="11" t="s">
+        <v>901</v>
+      </c>
+      <c r="V140" s="1" t="s">
         <v>902</v>
-      </c>
-      <c r="V140" s="1" t="s">
-        <v>903</v>
       </c>
       <c r="W140" s="15" t="s">
         <v>4</v>
@@ -21534,10 +21535,10 @@
         <v>53000138</v>
       </c>
       <c r="B141" s="22" t="s">
+        <v>920</v>
+      </c>
+      <c r="C141" s="15" t="s">
         <v>921</v>
-      </c>
-      <c r="C141" s="15" t="s">
-        <v>922</v>
       </c>
       <c r="D141" s="25" t="s">
         <v>411</v>
@@ -21587,19 +21588,19 @@
         <v>1</v>
       </c>
       <c r="S141" s="15" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="T141" s="15">
         <v>105</v>
       </c>
       <c r="U141" s="11" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="V141" s="1" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="W141" s="1" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="X141" s="15"/>
       <c r="Y141" s="15">
@@ -21620,10 +21621,10 @@
         <v>53000139</v>
       </c>
       <c r="B142" s="22" t="s">
+        <v>923</v>
+      </c>
+      <c r="C142" s="15" t="s">
         <v>924</v>
-      </c>
-      <c r="C142" s="15" t="s">
-        <v>925</v>
       </c>
       <c r="D142" s="25" t="s">
         <v>514</v>
@@ -21673,19 +21674,19 @@
         <v>2</v>
       </c>
       <c r="S142" s="15" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="T142" s="15">
         <v>103</v>
       </c>
       <c r="U142" s="11" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="V142" s="1" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="W142" s="15" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="X142" s="15"/>
       <c r="Y142" s="15">
@@ -21706,10 +21707,10 @@
         <v>53000140</v>
       </c>
       <c r="B143" s="22" t="s">
+        <v>926</v>
+      </c>
+      <c r="C143" s="15" t="s">
         <v>927</v>
-      </c>
-      <c r="C143" s="15" t="s">
-        <v>928</v>
       </c>
       <c r="D143" s="25" t="s">
         <v>411</v>
@@ -21759,19 +21760,19 @@
         <v>3</v>
       </c>
       <c r="S143" s="15" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="T143" s="15">
         <v>100</v>
       </c>
       <c r="U143" s="11" t="s">
+        <v>932</v>
+      </c>
+      <c r="V143" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="W143" s="15" t="s">
         <v>933</v>
-      </c>
-      <c r="V143" s="1" t="s">
-        <v>930</v>
-      </c>
-      <c r="W143" s="15" t="s">
-        <v>934</v>
       </c>
       <c r="X143" s="15"/>
       <c r="Y143" s="15">
@@ -22042,7 +22043,7 @@
         <v>349</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="P1" s="17" t="s">
         <v>331</v>
@@ -22128,7 +22129,7 @@
         <v>348</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>318</v>
@@ -22214,7 +22215,7 @@
         <v>351</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="P3" s="20" t="s">
         <v>333</v>
@@ -22316,7 +22317,7 @@
         <v>-1</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="V4" s="7" t="s">
         <v>342</v>
@@ -22470,16 +22471,16 @@
         <v>0</v>
       </c>
       <c r="S6" s="15" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="T6" s="1">
         <v>-1</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="V6" s="7" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="W6" s="15" t="s">
         <v>365</v>
@@ -22556,10 +22557,10 @@
         <v>-1</v>
       </c>
       <c r="U7" s="11" t="s">
+        <v>881</v>
+      </c>
+      <c r="V7" s="7" t="s">
         <v>882</v>
-      </c>
-      <c r="V7" s="7" t="s">
-        <v>883</v>
       </c>
       <c r="W7" s="15" t="s">
         <v>2</v>
@@ -22901,7 +22902,7 @@
         <v>53100008</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="34"/>
@@ -22950,16 +22951,16 @@
         <v>0</v>
       </c>
       <c r="S12" s="15" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="T12" s="1">
         <v>-1</v>
       </c>
       <c r="U12" s="11" t="s">
+        <v>831</v>
+      </c>
+      <c r="V12" s="7" t="s">
         <v>832</v>
-      </c>
-      <c r="V12" s="7" t="s">
-        <v>833</v>
       </c>
       <c r="W12" s="15" t="s">
         <v>2</v>
@@ -23171,7 +23172,7 @@
         <v>349</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="P1" s="17" t="s">
         <v>331</v>
@@ -23257,7 +23258,7 @@
         <v>348</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>318</v>
@@ -23343,7 +23344,7 @@
         <v>351</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="P3" s="20" t="s">
         <v>333</v>
@@ -23449,7 +23450,7 @@
         <v>115</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="V4" s="7" t="s">
         <v>376</v>
@@ -23533,7 +23534,7 @@
         <v>90</v>
       </c>
       <c r="U5" s="11" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="V5" s="7" t="s">
         <v>378</v>
@@ -23783,7 +23784,7 @@
         <v>90</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="V8" s="7" t="s">
         <v>387</v>

</xml_diff>

<commit_message>
dependent the spell damage and magic damage event; add a vibrate parameter to spell damage
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="标准" sheetId="1" r:id="rId1"/>
@@ -636,7 +636,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1393" uniqueCount="945">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1393" uniqueCount="942">
   <si>
     <t>慈悲</t>
   </si>
@@ -3051,73 +3051,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>t.OnMagicDamage(null, s.Damage,s.Attr);</t>
-  </si>
-  <si>
-    <t>t.OnMagicDamage(null, s.Damage,s.Attr);if(MathTool.GetRandom(100)&lt;s.Rate)t.AddBuff(56000010,lv,s.Time);</t>
-  </si>
-  <si>
-    <t>t.OnMagicDamage(null, s.Damage,s.Attr);if(MathTool.GetRandom(100)&lt;s.Rate)t.AddBuff(56000009,lv,s.Time);</t>
-  </si>
-  <si>
-    <t>m.RemoveTomb(mouse);foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse))im.OnMagicDamage(null, s.Damage,s.Attr);</t>
-  </si>
-  <si>
-    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse))im.OnMagicDamage(null, s.Damage*MathTool.GetRandom(70,130)/100,s.Attr);</t>
-  </si>
-  <si>
-    <t>foreach(IMonster im in m.GetAllMonster(mouse).FilterStar(1,5))im.OnMagicDamage(null, s.Damage,s.Attr);</t>
-  </si>
-  <si>
-    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse))im.OnMagicDamage(null, s.Damage,s.Attr);</t>
-  </si>
-  <si>
-    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse))if(im.HpRate&lt;1)im.OnMagicDamage(null, s.Damage,s.Attr);</t>
-  </si>
-  <si>
-    <t>foreach(IMonster im in m.GetAllMonster(mouse).FilterType(0))if(im.IsDefence)im.OnMagicDamage(null, s.Damage,s.Attr);</t>
-  </si>
-  <si>
-    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse)){im.OnMagicDamage(null, s.Damage,s.Attr);im.AddBuff(56000009,lv,s.Time);}</t>
-  </si>
-  <si>
-    <t>t.OnMagicDamage(null, s.Damage*MathTool.GetRandom(85,115)/100,s.Attr);</t>
-  </si>
-  <si>
-    <t>t.OnMagicDamage(null, s.Damage,s.Attr);t.Silent();</t>
-  </si>
-  <si>
-    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse))im.OnMagicDamage(null, s.Damage*MathTool.GetRandom(75,125)/100,s.Attr);</t>
-  </si>
-  <si>
-    <t>foreach(IMonster im in m.GetAllMonster(mouse).FilterStar(1,2))im.OnMagicDamage(null, s.Damage,s.Attr);</t>
-  </si>
-  <si>
-    <t>t.OnMagicDamage(null, s.Damage,s.Attr);if(MathTool.GetRandom(100)&lt;s.Rate)t.AddBuff(56000002,lv,s.Time);</t>
-  </si>
-  <si>
-    <t>t.OnMagicDamage(null, s.Damage,s.Attr);p.AddCard(null,s.Id, s.Level);</t>
-  </si>
-  <si>
-    <t>t.OnMagicDamage(null, s.Damage,s.Attr);if(MathTool.GetRandom(100)&lt;s.Rate&amp;&amp;!t.ResistBuffType(1))t.SuddenDeath();</t>
-  </si>
-  <si>
-    <t>t.OnMagicDamage(null, s.Damage,s.Attr);p.GetNextNCard(null,1);</t>
-  </si>
-  <si>
-    <t>t.OnMagicDamage(null,s.Damage,0);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>if(MathTool.GetRandom(100)&lt;s.Rate)t.OnMagicDamage(null, s.Damage,0);</t>
-  </si>
-  <si>
-    <t>t.OnMagicDamage(null, s.Damage,0);</t>
-  </si>
-  <si>
-    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse))im.OnMagicDamage(null, s.Damage,3);</t>
-  </si>
-  <si>
     <t>闷棍</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3162,10 +3095,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>t.OnMagicDamage(null, s.Damage,s.Attr);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>对敌方单体造成{0}点魔法伤害，对未受伤单位造成双倍伤害</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3182,10 +3111,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>t.OnMagicDamage(null, s.Damage,s.Attr);p.GetNextNCard(null,1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>连击</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3202,14 +3127,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>if(t.HpRate&gt;=100) t.OnMagicDamage(null, s.Damage*2,s.Attr);else t.OnMagicDamage(null, s.Damage,s.Attr);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>if(t.Owner.Combo) t.OnMagicDamage(null, s.Damage*2,s.Attr); else t.OnMagicDamage(null, s.Damage,s.Attr);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>冷血</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3391,10 +3308,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse)){im.OnMagicDamage(null, s.Damage,s.Attr);}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>永久提高单体{5}点攻击，连击造成双倍效果</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3451,10 +3364,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>t.OnMagicDamage(null, s.Damage,s.Attr);if(t.HpRate&gt;0)p.GetNextNCard(null,1);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>UFS</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3586,14 +3495,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>t.OnMagicDamage(null, p.Tower.GetPArmor()*s.Rate/100,s.Attr);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>p.Tower.AddPArmor(s.Cure);t.OnMagicDamage(null, s.Damage,s.Attr);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>使我方王塔获得{1}点物甲，抽一张牌</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3618,14 +3519,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>t.OnMagicDamage(null, s.Damage,s.Attr);t.AddBuff(56000007,lv,s.Time);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse)){im.OnMagicDamage(null, s.Damage,s.Attr);im.AddBuff(56000012,lv,s.Time);}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>对敌方单体造成{0}点魔法伤害，并使目标中毒{2:0.0}回合</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3662,10 +3555,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse)){im.OnMagicDamage(null, s.Damage,s.Attr);}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>对一行敌方单位造成{0}点魔法伤害</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3734,10 +3623,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse).SortRandom().Top(1)){im.SuddenDeath();im.Owner.Tower.OnMagicDamage(null,s.Damage,s.Attr);}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>对敌王塔造成{0}点魔法伤害</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3750,10 +3635,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>int count=2;if(MathTool.GetRandom(100)&lt;s.Rate)count=3;foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse).SortRandom().Top(count)){im.OnMagicDamage(null,s.Damage,s.Attr);}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>抽1张卡片,{4:0.0}%几率抽额外1张卡牌</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3907,10 +3788,6 @@
   </si>
   <si>
     <t>lockon</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreach(IMonster im in m.GetAllMonster(mouse))im.OnMagicDamage(null, s.Damage,s.Attr);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -3975,10 +3852,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>t.OnMagicDamage(null, s.Damage,s.Attr);t.Atk+=s.Atk;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>t.Atk+=s.Atk;if(t.Hp&gt;s.Damage)t.Def-=3;</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3987,10 +3860,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>r.Tower.OnMagicDamage(null,s.Damage,s.Attr);</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>t.AddMArmor(s.Cure);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -4091,6 +3960,112 @@
   <si>
     <t>范围，直伤</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>t.OnSpellDamage( s.Damage,s.Attr);</t>
+  </si>
+  <si>
+    <t>t.OnSpellDamage( s.Damage,s.Attr);t.AddBuff(56000007,lv,s.Time);</t>
+  </si>
+  <si>
+    <t>t.OnSpellDamage( s.Damage,s.Attr);if(MathTool.GetRandom(100)&lt;s.Rate)t.AddBuff(56000010,lv,s.Time);</t>
+  </si>
+  <si>
+    <t>t.OnSpellDamage( s.Damage,s.Attr);if(MathTool.GetRandom(100)&lt;s.Rate)t.AddBuff(56000009,lv,s.Time);</t>
+  </si>
+  <si>
+    <t>m.RemoveTomb(mouse);foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse))im.OnSpellDamage( s.Damage,s.Attr);</t>
+  </si>
+  <si>
+    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse))im.OnSpellDamage( s.Damage,s.Attr,0.3);</t>
+  </si>
+  <si>
+    <t>foreach(IMonster im in m.GetAllMonster(mouse).FilterStar(1,5))im.OnSpellDamage( s.Damage,s.Attr);</t>
+  </si>
+  <si>
+    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse))im.OnSpellDamage( s.Damage,s.Attr);</t>
+  </si>
+  <si>
+    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse))if(im.HpRate&lt;1)im.OnSpellDamage( s.Damage,s.Attr);</t>
+  </si>
+  <si>
+    <t>foreach(IMonster im in m.GetAllMonster(mouse).FilterType(0))if(im.IsDefence)im.OnSpellDamage( s.Damage,s.Attr);</t>
+  </si>
+  <si>
+    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse)){im.OnSpellDamage( s.Damage,s.Attr);im.AddBuff(56000009,lv,s.Time);}</t>
+  </si>
+  <si>
+    <t>t.OnSpellDamage( p.Tower.GetPArmor()*s.Rate/100,s.Attr);</t>
+  </si>
+  <si>
+    <t>t.OnSpellDamage( s.Damage,s.Attr,0.15);</t>
+  </si>
+  <si>
+    <t>foreach(IMonster im in m.GetAllMonster(mouse))im.OnSpellDamage( s.Damage,s.Attr);</t>
+  </si>
+  <si>
+    <t>t.OnSpellDamage( s.Damage,s.Attr);t.Silent();</t>
+  </si>
+  <si>
+    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse))im.OnSpellDamage( s.Damage,s.Attr,0.25);</t>
+  </si>
+  <si>
+    <t>foreach(IMonster im in m.GetAllMonster(mouse).FilterStar(1,2))im.OnSpellDamage( s.Damage,s.Attr);</t>
+  </si>
+  <si>
+    <t>t.OnSpellDamage( s.Damage,s.Attr);if(MathTool.GetRandom(100)&lt;s.Rate)t.AddBuff(56000002,lv,s.Time);</t>
+  </si>
+  <si>
+    <t>t.OnSpellDamage( s.Damage,s.Attr);p.AddCard(null,s.Id, s.Level);</t>
+  </si>
+  <si>
+    <t>t.OnSpellDamage( s.Damage,s.Attr);if(MathTool.GetRandom(100)&lt;s.Rate&amp;&amp;!t.ResistBuffType(1))t.SuddenDeath();</t>
+  </si>
+  <si>
+    <t>t.OnSpellDamage( s.Damage,s.Attr);p.GetNextNCard(null,1);</t>
+  </si>
+  <si>
+    <t>if(t.HpRate&gt;=100) t.OnSpellDamage( s.Damage*2,s.Attr);else t.OnSpellDamage( s.Damage,s.Attr);</t>
+  </si>
+  <si>
+    <t>if(t.Owner.Combo) t.OnSpellDamage( s.Damage*2,s.Attr); else t.OnSpellDamage( s.Damage,s.Attr);</t>
+  </si>
+  <si>
+    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse)){im.OnSpellDamage( s.Damage,s.Attr);}</t>
+  </si>
+  <si>
+    <t>t.OnSpellDamage( s.Damage,s.Attr);t.Atk+=s.Atk;</t>
+  </si>
+  <si>
+    <t>t.OnSpellDamage( s.Damage,s.Attr);if(t.HpRate&gt;0)p.GetNextNCard(null,1);</t>
+  </si>
+  <si>
+    <t>p.Tower.AddPArmor(s.Cure);t.OnSpellDamage( s.Damage,s.Attr);</t>
+  </si>
+  <si>
+    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse)){im.OnSpellDamage( s.Damage,s.Attr);im.AddBuff(56000012,lv,s.Time);}</t>
+  </si>
+  <si>
+    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse).SortRandom().Top(1)){im.SuddenDeath();im.Owner.Tower.OnSpellDamage(s.Damage,s.Attr);}</t>
+  </si>
+  <si>
+    <t>int count=2;if(MathTool.GetRandom(100)&lt;s.Rate)count=3;foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse).SortRandom().Top(count)){im.OnSpellDamage(s.Damage,s.Attr);}</t>
+  </si>
+  <si>
+    <t>t.OnSpellDamage(s.Damage,0);</t>
+  </si>
+  <si>
+    <t>r.Tower.OnSpellDamage(s.Damage,s.Attr);</t>
+  </si>
+  <si>
+    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,s.Target,s.Shape,s.Range,mouse))im.OnSpellDamage(s.Damage,3);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(MathTool.GetRandom(100)&lt;s.Rate)t.OnSpellDamage( s.Damage,0);</t>
+  </si>
+  <si>
+    <t>t.OnSpellDamage( s.Damage,0);</t>
   </si>
 </sst>
 </file>
@@ -5105,13 +5080,6 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="174">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -7840,6 +7808,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
@@ -9069,132 +9044,132 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AB143" totalsRowShown="0" headerRowDxfId="135" dataDxfId="134" tableBorderDxfId="133">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AB143" totalsRowShown="0" headerRowDxfId="134" dataDxfId="133" tableBorderDxfId="132">
   <autoFilter ref="A3:AB143"/>
   <sortState ref="A4:AB113">
     <sortCondition ref="A3:A113"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="132"/>
-    <tableColumn id="2" name="Name" dataDxfId="131"/>
-    <tableColumn id="20" name="Ename" dataDxfId="130"/>
-    <tableColumn id="21" name="Remark" dataDxfId="129"/>
-    <tableColumn id="3" name="Star" dataDxfId="128"/>
-    <tableColumn id="4" name="Type" dataDxfId="127"/>
-    <tableColumn id="5" name="Attr" dataDxfId="126"/>
-    <tableColumn id="8" name="Quality" dataDxfId="125">
+    <tableColumn id="1" name="Id" dataDxfId="131"/>
+    <tableColumn id="2" name="Name" dataDxfId="130"/>
+    <tableColumn id="20" name="Ename" dataDxfId="129"/>
+    <tableColumn id="21" name="Remark" dataDxfId="128"/>
+    <tableColumn id="3" name="Star" dataDxfId="127"/>
+    <tableColumn id="4" name="Type" dataDxfId="126"/>
+    <tableColumn id="5" name="Attr" dataDxfId="125"/>
+    <tableColumn id="8" name="Quality" dataDxfId="124">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="124"/>
-    <tableColumn id="9" name="Damage" dataDxfId="123"/>
-    <tableColumn id="10" name="Cure" dataDxfId="122"/>
-    <tableColumn id="11" name="Time" dataDxfId="121"/>
-    <tableColumn id="13" name="Help" dataDxfId="120"/>
-    <tableColumn id="16" name="Rate" dataDxfId="119"/>
-    <tableColumn id="18" name="Atk" dataDxfId="118"/>
-    <tableColumn id="12" name="Modify" dataDxfId="117"/>
-    <tableColumn id="27" name="Sum" dataDxfId="116">
+    <tableColumn id="7" name="Cost" dataDxfId="123"/>
+    <tableColumn id="9" name="Damage" dataDxfId="122"/>
+    <tableColumn id="10" name="Cure" dataDxfId="121"/>
+    <tableColumn id="11" name="Time" dataDxfId="120"/>
+    <tableColumn id="13" name="Help" dataDxfId="119"/>
+    <tableColumn id="16" name="Rate" dataDxfId="118"/>
+    <tableColumn id="18" name="Atk" dataDxfId="117"/>
+    <tableColumn id="12" name="Modify" dataDxfId="116"/>
+    <tableColumn id="27" name="Sum" dataDxfId="115">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="115"/>
-    <tableColumn id="15" name="Target" dataDxfId="114"/>
-    <tableColumn id="25" name="Mark" dataDxfId="113"/>
-    <tableColumn id="22" name="Effect" dataDxfId="112"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="111"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="110"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="109"/>
-    <tableColumn id="26" name="JobId" dataDxfId="108"/>
-    <tableColumn id="19" name="Icon" dataDxfId="107"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="106"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="105"/>
+    <tableColumn id="6" name="Range" dataDxfId="114"/>
+    <tableColumn id="15" name="Target" dataDxfId="113"/>
+    <tableColumn id="25" name="Mark" dataDxfId="112"/>
+    <tableColumn id="22" name="Effect" dataDxfId="111"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="110"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="109"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="108"/>
+    <tableColumn id="26" name="JobId" dataDxfId="107"/>
+    <tableColumn id="19" name="Icon" dataDxfId="106"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="105"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="104"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AB15" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72" tableBorderDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AB15" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71" tableBorderDxfId="70">
   <autoFilter ref="A3:AB15"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="70"/>
-    <tableColumn id="2" name="Name" dataDxfId="69"/>
-    <tableColumn id="20" name="Ename" dataDxfId="68"/>
-    <tableColumn id="21" name="Remark" dataDxfId="67"/>
-    <tableColumn id="3" name="Star" dataDxfId="66"/>
-    <tableColumn id="4" name="Type" dataDxfId="65"/>
-    <tableColumn id="5" name="Attr" dataDxfId="64"/>
-    <tableColumn id="8" name="Quality" dataDxfId="63">
+    <tableColumn id="1" name="Id" dataDxfId="69"/>
+    <tableColumn id="2" name="Name" dataDxfId="68"/>
+    <tableColumn id="20" name="Ename" dataDxfId="67"/>
+    <tableColumn id="21" name="Remark" dataDxfId="66"/>
+    <tableColumn id="3" name="Star" dataDxfId="65"/>
+    <tableColumn id="4" name="Type" dataDxfId="64"/>
+    <tableColumn id="5" name="Attr" dataDxfId="63"/>
+    <tableColumn id="8" name="Quality" dataDxfId="62">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="62"/>
-    <tableColumn id="9" name="Damage" dataDxfId="61"/>
-    <tableColumn id="10" name="Cure" dataDxfId="60"/>
-    <tableColumn id="11" name="Time" dataDxfId="59"/>
-    <tableColumn id="13" name="Help" dataDxfId="58"/>
-    <tableColumn id="16" name="Rate" dataDxfId="57"/>
-    <tableColumn id="18" name="Atk" dataDxfId="56"/>
-    <tableColumn id="12" name="Modify" dataDxfId="55"/>
-    <tableColumn id="27" name="Sum" dataDxfId="54">
+    <tableColumn id="7" name="Cost" dataDxfId="61"/>
+    <tableColumn id="9" name="Damage" dataDxfId="60"/>
+    <tableColumn id="10" name="Cure" dataDxfId="59"/>
+    <tableColumn id="11" name="Time" dataDxfId="58"/>
+    <tableColumn id="13" name="Help" dataDxfId="57"/>
+    <tableColumn id="16" name="Rate" dataDxfId="56"/>
+    <tableColumn id="18" name="Atk" dataDxfId="55"/>
+    <tableColumn id="12" name="Modify" dataDxfId="54"/>
+    <tableColumn id="27" name="Sum" dataDxfId="53">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="53"/>
-    <tableColumn id="15" name="Target" dataDxfId="52"/>
-    <tableColumn id="25" name="Mark" dataDxfId="51"/>
-    <tableColumn id="22" name="Effect" dataDxfId="50"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="49"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="48"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="47"/>
-    <tableColumn id="26" name="JobId" dataDxfId="46"/>
-    <tableColumn id="19" name="Icon" dataDxfId="45"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="44"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="43"/>
+    <tableColumn id="6" name="Range" dataDxfId="52"/>
+    <tableColumn id="15" name="Target" dataDxfId="51"/>
+    <tableColumn id="25" name="Mark" dataDxfId="50"/>
+    <tableColumn id="22" name="Effect" dataDxfId="49"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="48"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="47"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="46"/>
+    <tableColumn id="26" name="JobId" dataDxfId="45"/>
+    <tableColumn id="19" name="Icon" dataDxfId="44"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="43"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_35" displayName="表1_35" ref="A3:AB9" totalsRowShown="0" headerRowDxfId="30" tableBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_35" displayName="表1_35" ref="A3:AB9" totalsRowShown="0" headerRowDxfId="29" tableBorderDxfId="28">
   <autoFilter ref="A3:AB9"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" name="Id" dataDxfId="28"/>
-    <tableColumn id="2" name="Name" dataDxfId="27"/>
-    <tableColumn id="20" name="Ename" dataDxfId="26"/>
-    <tableColumn id="21" name="Remark" dataDxfId="25"/>
-    <tableColumn id="3" name="Star" dataDxfId="24"/>
-    <tableColumn id="4" name="Type" dataDxfId="23"/>
-    <tableColumn id="5" name="Attr" dataDxfId="22"/>
-    <tableColumn id="8" name="Quality" dataDxfId="21">
+    <tableColumn id="1" name="Id" dataDxfId="27"/>
+    <tableColumn id="2" name="Name" dataDxfId="26"/>
+    <tableColumn id="20" name="Ename" dataDxfId="25"/>
+    <tableColumn id="21" name="Remark" dataDxfId="24"/>
+    <tableColumn id="3" name="Star" dataDxfId="23"/>
+    <tableColumn id="4" name="Type" dataDxfId="22"/>
+    <tableColumn id="5" name="Attr" dataDxfId="21"/>
+    <tableColumn id="8" name="Quality" dataDxfId="20">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="20"/>
-    <tableColumn id="9" name="Damage" dataDxfId="19"/>
-    <tableColumn id="10" name="Cure" dataDxfId="18"/>
-    <tableColumn id="11" name="Time" dataDxfId="17"/>
-    <tableColumn id="13" name="Help" dataDxfId="16"/>
-    <tableColumn id="16" name="Rate" dataDxfId="15"/>
-    <tableColumn id="18" name="Atk" dataDxfId="14"/>
-    <tableColumn id="12" name="Modify" dataDxfId="13"/>
-    <tableColumn id="27" name="Sum" dataDxfId="12">
+    <tableColumn id="7" name="Cost" dataDxfId="19"/>
+    <tableColumn id="9" name="Damage" dataDxfId="18"/>
+    <tableColumn id="10" name="Cure" dataDxfId="17"/>
+    <tableColumn id="11" name="Time" dataDxfId="16"/>
+    <tableColumn id="13" name="Help" dataDxfId="15"/>
+    <tableColumn id="16" name="Rate" dataDxfId="14"/>
+    <tableColumn id="18" name="Atk" dataDxfId="13"/>
+    <tableColumn id="12" name="Modify" dataDxfId="12"/>
+    <tableColumn id="27" name="Sum" dataDxfId="11">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="11"/>
-    <tableColumn id="15" name="Target" dataDxfId="10"/>
-    <tableColumn id="25" name="Mark" dataDxfId="9"/>
-    <tableColumn id="22" name="Effect" dataDxfId="8"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="7"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="6"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="5"/>
-    <tableColumn id="26" name="JobId" dataDxfId="4"/>
-    <tableColumn id="19" name="Icon" dataDxfId="3"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="2"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="1"/>
+    <tableColumn id="6" name="Range" dataDxfId="10"/>
+    <tableColumn id="15" name="Target" dataDxfId="9"/>
+    <tableColumn id="25" name="Mark" dataDxfId="8"/>
+    <tableColumn id="22" name="Effect" dataDxfId="7"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="6"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="5"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="4"/>
+    <tableColumn id="26" name="JobId" dataDxfId="3"/>
+    <tableColumn id="19" name="Icon" dataDxfId="2"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="1"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9523,11 +9498,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C133" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D138" sqref="D138"/>
+      <selection pane="bottomRight" activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9596,7 +9571,7 @@
         <v>349</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>732</v>
+        <v>706</v>
       </c>
       <c r="P1" s="17" t="s">
         <v>331</v>
@@ -9682,7 +9657,7 @@
         <v>350</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>730</v>
+        <v>704</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>332</v>
@@ -9700,7 +9675,7 @@
         <v>490</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>729</v>
+        <v>703</v>
       </c>
       <c r="V2" s="10" t="s">
         <v>179</v>
@@ -9768,7 +9743,7 @@
         <v>351</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>731</v>
+        <v>705</v>
       </c>
       <c r="P3" s="20" t="s">
         <v>333</v>
@@ -9874,10 +9849,10 @@
         <v>95</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>890</v>
+        <v>855</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>864</v>
+        <v>829</v>
       </c>
       <c r="W4" s="1" t="s">
         <v>2</v>
@@ -10042,7 +10017,7 @@
         <v>100</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>715</v>
+        <v>907</v>
       </c>
       <c r="V6" s="7" t="s">
         <v>378</v>
@@ -10126,10 +10101,10 @@
         <v>100</v>
       </c>
       <c r="U7" s="11" t="s">
-        <v>830</v>
+        <v>908</v>
       </c>
       <c r="V7" s="7" t="s">
-        <v>832</v>
+        <v>800</v>
       </c>
       <c r="W7" s="1" t="s">
         <v>9</v>
@@ -10159,7 +10134,7 @@
         <v>215</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>937</v>
+        <v>899</v>
       </c>
       <c r="E8" s="1">
         <v>3</v>
@@ -10919,7 +10894,7 @@
         <v>468</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>938</v>
+        <v>900</v>
       </c>
       <c r="E17" s="1">
         <v>2</v>
@@ -11058,10 +11033,10 @@
         <v>75</v>
       </c>
       <c r="U18" s="11" t="s">
-        <v>739</v>
+        <v>713</v>
       </c>
       <c r="V18" s="7" t="s">
-        <v>741</v>
+        <v>715</v>
       </c>
       <c r="W18" s="1" t="s">
         <v>15</v>
@@ -11230,10 +11205,10 @@
         <v>100</v>
       </c>
       <c r="U20" s="11" t="s">
-        <v>740</v>
+        <v>714</v>
       </c>
       <c r="V20" s="7" t="s">
-        <v>742</v>
+        <v>716</v>
       </c>
       <c r="W20" s="1" t="s">
         <v>644</v>
@@ -11316,7 +11291,7 @@
         <v>102</v>
       </c>
       <c r="U21" s="11" t="s">
-        <v>683</v>
+        <v>909</v>
       </c>
       <c r="V21" s="7" t="s">
         <v>591</v>
@@ -11349,7 +11324,7 @@
         <v>222</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>938</v>
+        <v>900</v>
       </c>
       <c r="E22" s="1">
         <v>4</v>
@@ -11437,7 +11412,7 @@
         <v>223</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>938</v>
+        <v>900</v>
       </c>
       <c r="E23" s="1">
         <v>3</v>
@@ -11525,7 +11500,7 @@
         <v>224</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>938</v>
+        <v>900</v>
       </c>
       <c r="E24" s="1">
         <v>3</v>
@@ -11666,10 +11641,10 @@
         <v>107</v>
       </c>
       <c r="U25" s="11" t="s">
-        <v>790</v>
+        <v>762</v>
       </c>
       <c r="V25" s="7" t="s">
-        <v>791</v>
+        <v>763</v>
       </c>
       <c r="W25" s="1" t="s">
         <v>29</v>
@@ -11836,7 +11811,7 @@
         <v>90</v>
       </c>
       <c r="U27" s="11" t="s">
-        <v>711</v>
+        <v>689</v>
       </c>
       <c r="V27" s="7" t="s">
         <v>391</v>
@@ -11922,7 +11897,7 @@
         <v>100</v>
       </c>
       <c r="U28" s="11" t="s">
-        <v>684</v>
+        <v>910</v>
       </c>
       <c r="V28" s="7" t="s">
         <v>506</v>
@@ -12097,7 +12072,7 @@
         <v>508</v>
       </c>
       <c r="V30" s="7" t="s">
-        <v>928</v>
+        <v>890</v>
       </c>
       <c r="W30" s="1" t="s">
         <v>39</v>
@@ -12181,7 +12156,7 @@
         <v>509</v>
       </c>
       <c r="V31" s="7" t="s">
-        <v>929</v>
+        <v>891</v>
       </c>
       <c r="W31" s="1" t="s">
         <v>41</v>
@@ -12262,7 +12237,7 @@
         <v>100</v>
       </c>
       <c r="U32" s="11" t="s">
-        <v>682</v>
+        <v>907</v>
       </c>
       <c r="V32" s="21" t="s">
         <v>343</v>
@@ -12346,10 +12321,10 @@
         <v>100</v>
       </c>
       <c r="U33" s="11" t="s">
-        <v>880</v>
+        <v>845</v>
       </c>
       <c r="V33" s="1" t="s">
-        <v>872</v>
+        <v>837</v>
       </c>
       <c r="W33" s="1" t="s">
         <v>4</v>
@@ -12432,10 +12407,10 @@
         <v>100</v>
       </c>
       <c r="U34" s="11" t="s">
-        <v>881</v>
+        <v>846</v>
       </c>
       <c r="V34" s="1" t="s">
-        <v>874</v>
+        <v>839</v>
       </c>
       <c r="W34" s="1" t="s">
         <v>4</v>
@@ -12465,7 +12440,7 @@
         <v>298</v>
       </c>
       <c r="D35" s="25" t="s">
-        <v>938</v>
+        <v>900</v>
       </c>
       <c r="E35" s="1">
         <v>3</v>
@@ -12518,7 +12493,7 @@
         <v>100</v>
       </c>
       <c r="U35" s="11" t="s">
-        <v>685</v>
+        <v>911</v>
       </c>
       <c r="V35" s="7" t="s">
         <v>416</v>
@@ -12727,7 +12702,7 @@
         <v>233</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>938</v>
+        <v>900</v>
       </c>
       <c r="E38" s="1">
         <v>3</v>
@@ -12780,7 +12755,7 @@
         <v>100</v>
       </c>
       <c r="U38" s="11" t="s">
-        <v>809</v>
+        <v>781</v>
       </c>
       <c r="V38" s="7" t="s">
         <v>613</v>
@@ -12985,7 +12960,7 @@
         <v>236</v>
       </c>
       <c r="D41" s="25" t="s">
-        <v>939</v>
+        <v>901</v>
       </c>
       <c r="E41" s="1">
         <v>2</v>
@@ -13032,16 +13007,16 @@
         <v>12</v>
       </c>
       <c r="S41" s="1" t="s">
-        <v>811</v>
+        <v>783</v>
       </c>
       <c r="T41">
         <v>100</v>
       </c>
       <c r="U41" s="11" t="s">
-        <v>810</v>
+        <v>782</v>
       </c>
       <c r="V41" s="7" t="s">
-        <v>812</v>
+        <v>784</v>
       </c>
       <c r="W41" s="1" t="s">
         <v>55</v>
@@ -13126,10 +13101,10 @@
         <v>85</v>
       </c>
       <c r="U42" s="11" t="s">
-        <v>882</v>
+        <v>847</v>
       </c>
       <c r="V42" s="1" t="s">
-        <v>873</v>
+        <v>838</v>
       </c>
       <c r="W42" s="1" t="s">
         <v>4</v>
@@ -13212,10 +13187,10 @@
         <v>100</v>
       </c>
       <c r="U43" s="11" t="s">
-        <v>883</v>
+        <v>848</v>
       </c>
       <c r="V43" s="1" t="s">
-        <v>875</v>
+        <v>840</v>
       </c>
       <c r="W43" s="1" t="s">
         <v>4</v>
@@ -13318,7 +13293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:28" ht="84" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>53000042</v>
       </c>
@@ -13329,7 +13304,7 @@
         <v>239</v>
       </c>
       <c r="D45" s="25" t="s">
-        <v>938</v>
+        <v>900</v>
       </c>
       <c r="E45" s="1">
         <v>3</v>
@@ -13382,7 +13357,7 @@
         <v>110</v>
       </c>
       <c r="U45" s="11" t="s">
-        <v>686</v>
+        <v>912</v>
       </c>
       <c r="V45" s="7" t="s">
         <v>588</v>
@@ -13556,10 +13531,10 @@
         <v>95</v>
       </c>
       <c r="U47" s="11" t="s">
-        <v>884</v>
+        <v>849</v>
       </c>
       <c r="V47" s="1" t="s">
-        <v>876</v>
+        <v>841</v>
       </c>
       <c r="W47" s="1" t="s">
         <v>4</v>
@@ -13645,7 +13620,7 @@
         <v>677</v>
       </c>
       <c r="V48" s="1" t="s">
-        <v>814</v>
+        <v>786</v>
       </c>
       <c r="W48" s="1" t="s">
         <v>322</v>
@@ -13675,7 +13650,7 @@
         <v>243</v>
       </c>
       <c r="D49" s="25" t="s">
-        <v>938</v>
+        <v>900</v>
       </c>
       <c r="E49" s="1">
         <v>5</v>
@@ -13728,7 +13703,7 @@
         <v>100</v>
       </c>
       <c r="U49" s="11" t="s">
-        <v>687</v>
+        <v>913</v>
       </c>
       <c r="V49" s="7" t="s">
         <v>582</v>
@@ -13761,7 +13736,7 @@
         <v>244</v>
       </c>
       <c r="D50" s="25" t="s">
-        <v>938</v>
+        <v>900</v>
       </c>
       <c r="E50" s="1">
         <v>5</v>
@@ -13814,7 +13789,7 @@
         <v>100</v>
       </c>
       <c r="U50" s="11" t="s">
-        <v>688</v>
+        <v>914</v>
       </c>
       <c r="V50" s="7" t="s">
         <v>614</v>
@@ -13902,7 +13877,7 @@
         <v>100</v>
       </c>
       <c r="U51" s="11" t="s">
-        <v>682</v>
+        <v>907</v>
       </c>
       <c r="V51" s="1" t="s">
         <v>596</v>
@@ -13935,7 +13910,7 @@
         <v>246</v>
       </c>
       <c r="D52" s="25" t="s">
-        <v>938</v>
+        <v>900</v>
       </c>
       <c r="E52" s="1">
         <v>3</v>
@@ -13988,7 +13963,7 @@
         <v>105</v>
       </c>
       <c r="U52" s="11" t="s">
-        <v>689</v>
+        <v>915</v>
       </c>
       <c r="V52" s="7" t="s">
         <v>593</v>
@@ -14023,7 +13998,7 @@
         <v>247</v>
       </c>
       <c r="D53" s="25" t="s">
-        <v>938</v>
+        <v>900</v>
       </c>
       <c r="E53" s="1">
         <v>4</v>
@@ -14076,7 +14051,7 @@
         <v>95</v>
       </c>
       <c r="U53" s="11" t="s">
-        <v>690</v>
+        <v>916</v>
       </c>
       <c r="V53" s="7" t="s">
         <v>581</v>
@@ -14109,7 +14084,7 @@
         <v>248</v>
       </c>
       <c r="D54" s="25" t="s">
-        <v>940</v>
+        <v>902</v>
       </c>
       <c r="E54" s="1">
         <v>3</v>
@@ -14162,7 +14137,7 @@
         <v>100</v>
       </c>
       <c r="U54" s="11" t="s">
-        <v>691</v>
+        <v>917</v>
       </c>
       <c r="V54" s="1" t="s">
         <v>594</v>
@@ -14197,7 +14172,7 @@
         <v>605</v>
       </c>
       <c r="D55" s="25" t="s">
-        <v>938</v>
+        <v>900</v>
       </c>
       <c r="E55" s="1">
         <v>1</v>
@@ -14244,16 +14219,16 @@
         <v>0</v>
       </c>
       <c r="S55" s="1" t="s">
-        <v>813</v>
+        <v>785</v>
       </c>
       <c r="T55">
         <v>95</v>
       </c>
       <c r="U55" s="11" t="s">
-        <v>822</v>
+        <v>918</v>
       </c>
       <c r="V55" s="7" t="s">
-        <v>815</v>
+        <v>787</v>
       </c>
       <c r="W55" s="1" t="s">
         <v>607</v>
@@ -14283,7 +14258,7 @@
         <v>249</v>
       </c>
       <c r="D56" s="25" t="s">
-        <v>938</v>
+        <v>900</v>
       </c>
       <c r="E56" s="1">
         <v>3</v>
@@ -14336,7 +14311,7 @@
         <v>100</v>
       </c>
       <c r="U56" s="11" t="s">
-        <v>688</v>
+        <v>914</v>
       </c>
       <c r="V56" s="7" t="s">
         <v>598</v>
@@ -14358,7 +14333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:28" ht="36" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:28" ht="24" x14ac:dyDescent="0.15">
       <c r="A57">
         <v>53000054</v>
       </c>
@@ -14422,7 +14397,7 @@
         <v>100</v>
       </c>
       <c r="U57" s="11" t="s">
-        <v>692</v>
+        <v>919</v>
       </c>
       <c r="V57" s="7" t="s">
         <v>595</v>
@@ -14760,16 +14735,16 @@
         <v>0</v>
       </c>
       <c r="S61" s="1" t="s">
-        <v>806</v>
+        <v>778</v>
       </c>
       <c r="T61">
         <v>100</v>
       </c>
       <c r="U61" s="11" t="s">
-        <v>821</v>
+        <v>793</v>
       </c>
       <c r="V61" s="7" t="s">
-        <v>824</v>
+        <v>794</v>
       </c>
       <c r="W61" s="1" t="s">
         <v>15</v>
@@ -14852,10 +14827,10 @@
         <v>100</v>
       </c>
       <c r="U62" s="11" t="s">
-        <v>904</v>
+        <v>868</v>
       </c>
       <c r="V62" s="7" t="s">
-        <v>738</v>
+        <v>712</v>
       </c>
       <c r="W62" s="1" t="s">
         <v>83</v>
@@ -15315,7 +15290,7 @@
         <v>199</v>
       </c>
       <c r="D68" s="25" t="s">
-        <v>938</v>
+        <v>900</v>
       </c>
       <c r="E68" s="1">
         <v>6</v>
@@ -15368,7 +15343,7 @@
         <v>100</v>
       </c>
       <c r="U68" s="11" t="s">
-        <v>903</v>
+        <v>920</v>
       </c>
       <c r="V68" s="1" t="s">
         <v>403</v>
@@ -15454,10 +15429,10 @@
         <v>85</v>
       </c>
       <c r="U69" s="11" t="s">
-        <v>885</v>
+        <v>850</v>
       </c>
       <c r="V69" s="1" t="s">
-        <v>877</v>
+        <v>842</v>
       </c>
       <c r="W69" s="1" t="s">
         <v>4</v>
@@ -15540,7 +15515,7 @@
         <v>100</v>
       </c>
       <c r="U70" s="11" t="s">
-        <v>693</v>
+        <v>921</v>
       </c>
       <c r="V70" s="7" t="s">
         <v>629</v>
@@ -15573,7 +15548,7 @@
         <v>260</v>
       </c>
       <c r="D71" s="25" t="s">
-        <v>940</v>
+        <v>902</v>
       </c>
       <c r="E71" s="1">
         <v>2</v>
@@ -15714,13 +15689,13 @@
         <v>100</v>
       </c>
       <c r="U72" s="11" t="s">
-        <v>905</v>
+        <v>869</v>
       </c>
       <c r="V72" s="7" t="s">
-        <v>737</v>
+        <v>711</v>
       </c>
       <c r="W72" s="1" t="s">
-        <v>712</v>
+        <v>690</v>
       </c>
       <c r="X72" s="1"/>
       <c r="Y72" s="1">
@@ -15800,7 +15775,7 @@
         <v>100</v>
       </c>
       <c r="U73" s="11" t="s">
-        <v>805</v>
+        <v>777</v>
       </c>
       <c r="V73" s="7" t="s">
         <v>548</v>
@@ -15833,7 +15808,7 @@
         <v>201</v>
       </c>
       <c r="D74" s="25" t="s">
-        <v>941</v>
+        <v>903</v>
       </c>
       <c r="E74" s="1">
         <v>4</v>
@@ -16007,7 +15982,7 @@
         <v>262</v>
       </c>
       <c r="D76" s="25" t="s">
-        <v>941</v>
+        <v>903</v>
       </c>
       <c r="E76" s="1">
         <v>3</v>
@@ -16495,7 +16470,7 @@
         <v>671</v>
       </c>
       <c r="V81" s="7" t="s">
-        <v>746</v>
+        <v>720</v>
       </c>
       <c r="W81" s="1" t="s">
         <v>93</v>
@@ -16688,7 +16663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:28" ht="84" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A84">
         <v>53000081</v>
       </c>
@@ -16699,7 +16674,7 @@
         <v>269</v>
       </c>
       <c r="D84" s="25" t="s">
-        <v>938</v>
+        <v>900</v>
       </c>
       <c r="E84" s="1">
         <v>2</v>
@@ -16752,7 +16727,7 @@
         <v>100</v>
       </c>
       <c r="U84" s="11" t="s">
-        <v>694</v>
+        <v>922</v>
       </c>
       <c r="V84" s="7" t="s">
         <v>590</v>
@@ -16840,10 +16815,10 @@
         <v>100</v>
       </c>
       <c r="U85" s="11" t="s">
-        <v>906</v>
+        <v>870</v>
       </c>
       <c r="V85" s="7" t="s">
-        <v>736</v>
+        <v>710</v>
       </c>
       <c r="W85" s="1" t="s">
         <v>122</v>
@@ -16873,7 +16848,7 @@
         <v>289</v>
       </c>
       <c r="D86" s="25" t="s">
-        <v>938</v>
+        <v>900</v>
       </c>
       <c r="E86" s="1">
         <v>3</v>
@@ -16926,7 +16901,7 @@
         <v>100</v>
       </c>
       <c r="U86" s="11" t="s">
-        <v>695</v>
+        <v>923</v>
       </c>
       <c r="V86" s="7" t="s">
         <v>555</v>
@@ -17188,10 +17163,10 @@
         <v>102</v>
       </c>
       <c r="U89" s="11" t="s">
-        <v>907</v>
+        <v>871</v>
       </c>
       <c r="V89" s="7" t="s">
-        <v>932</v>
+        <v>894</v>
       </c>
       <c r="W89" s="1" t="s">
         <v>2</v>
@@ -17274,7 +17249,7 @@
         <v>100</v>
       </c>
       <c r="U90" s="11" t="s">
-        <v>696</v>
+        <v>924</v>
       </c>
       <c r="V90" s="7" t="s">
         <v>592</v>
@@ -17309,7 +17284,7 @@
         <v>271</v>
       </c>
       <c r="D91" s="25" t="s">
-        <v>938</v>
+        <v>900</v>
       </c>
       <c r="E91" s="1">
         <v>3</v>
@@ -17362,7 +17337,7 @@
         <v>100</v>
       </c>
       <c r="U91" s="11" t="s">
-        <v>688</v>
+        <v>914</v>
       </c>
       <c r="V91" s="7" t="s">
         <v>340</v>
@@ -17397,7 +17372,7 @@
         <v>272</v>
       </c>
       <c r="D92" s="25" t="s">
-        <v>938</v>
+        <v>900</v>
       </c>
       <c r="E92" s="1">
         <v>4</v>
@@ -17450,7 +17425,7 @@
         <v>100</v>
       </c>
       <c r="U92" s="11" t="s">
-        <v>688</v>
+        <v>914</v>
       </c>
       <c r="V92" s="7" t="s">
         <v>580</v>
@@ -17624,7 +17599,7 @@
         <v>100</v>
       </c>
       <c r="U94" s="11" t="s">
-        <v>697</v>
+        <v>925</v>
       </c>
       <c r="V94" s="7" t="s">
         <v>341</v>
@@ -17796,7 +17771,7 @@
         <v>100</v>
       </c>
       <c r="U96" s="11" t="s">
-        <v>698</v>
+        <v>926</v>
       </c>
       <c r="V96" s="7" t="s">
         <v>579</v>
@@ -18314,7 +18289,7 @@
         <v>100</v>
       </c>
       <c r="U102" s="11" t="s">
-        <v>699</v>
+        <v>927</v>
       </c>
       <c r="V102" s="7" t="s">
         <v>573</v>
@@ -18403,7 +18378,7 @@
         <v>674</v>
       </c>
       <c r="V103" s="1" t="s">
-        <v>747</v>
+        <v>721</v>
       </c>
       <c r="W103" s="1" t="s">
         <v>144</v>
@@ -18572,7 +18547,7 @@
         <v>100</v>
       </c>
       <c r="U105" s="11" t="s">
-        <v>682</v>
+        <v>907</v>
       </c>
       <c r="V105" s="7" t="s">
         <v>342</v>
@@ -18658,10 +18633,10 @@
         <v>105</v>
       </c>
       <c r="U106" s="11" t="s">
-        <v>908</v>
+        <v>872</v>
       </c>
       <c r="V106" s="7" t="s">
-        <v>930</v>
+        <v>892</v>
       </c>
       <c r="W106" s="1" t="s">
         <v>147</v>
@@ -18746,10 +18721,10 @@
         <v>105</v>
       </c>
       <c r="U107" s="11" t="s">
-        <v>909</v>
+        <v>873</v>
       </c>
       <c r="V107" s="7" t="s">
-        <v>931</v>
+        <v>893</v>
       </c>
       <c r="W107" s="1" t="s">
         <v>149</v>
@@ -18918,10 +18893,10 @@
         <v>100</v>
       </c>
       <c r="U109" s="11" t="s">
-        <v>911</v>
+        <v>875</v>
       </c>
       <c r="V109" s="7" t="s">
-        <v>735</v>
+        <v>709</v>
       </c>
       <c r="W109" s="1" t="s">
         <v>153</v>
@@ -19004,10 +18979,10 @@
         <v>100</v>
       </c>
       <c r="U110" s="11" t="s">
-        <v>910</v>
+        <v>874</v>
       </c>
       <c r="V110" s="7" t="s">
-        <v>734</v>
+        <v>708</v>
       </c>
       <c r="W110" s="1" t="s">
         <v>155</v>
@@ -19176,7 +19151,7 @@
         <v>100</v>
       </c>
       <c r="U112" s="11" t="s">
-        <v>912</v>
+        <v>876</v>
       </c>
       <c r="V112" s="7" t="s">
         <v>559</v>
@@ -19262,10 +19237,10 @@
         <v>103</v>
       </c>
       <c r="U113" s="11" t="s">
-        <v>708</v>
+        <v>686</v>
       </c>
       <c r="V113" s="7" t="s">
-        <v>707</v>
+        <v>685</v>
       </c>
       <c r="W113" s="1" t="s">
         <v>29</v>
@@ -19465,10 +19440,10 @@
         <v>53000113</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>704</v>
+        <v>682</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>705</v>
+        <v>683</v>
       </c>
       <c r="D116" s="25"/>
       <c r="E116" s="1">
@@ -19516,22 +19491,22 @@
         <v>0</v>
       </c>
       <c r="S116" s="1" t="s">
-        <v>706</v>
+        <v>684</v>
       </c>
       <c r="T116">
         <v>100</v>
       </c>
       <c r="U116" s="11" t="s">
-        <v>934</v>
+        <v>896</v>
       </c>
       <c r="V116" s="7" t="s">
-        <v>710</v>
+        <v>688</v>
       </c>
       <c r="W116" s="1" t="s">
-        <v>709</v>
+        <v>687</v>
       </c>
       <c r="X116" s="1" t="s">
-        <v>709</v>
+        <v>687</v>
       </c>
       <c r="Y116" s="1">
         <v>11000003</v>
@@ -19551,10 +19526,10 @@
         <v>53000114</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>714</v>
+        <v>692</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>713</v>
+        <v>691</v>
       </c>
       <c r="D117" s="25"/>
       <c r="E117" s="1">
@@ -19602,16 +19577,16 @@
         <v>0</v>
       </c>
       <c r="S117" s="1" t="s">
-        <v>706</v>
+        <v>684</v>
       </c>
       <c r="T117">
         <v>101</v>
       </c>
       <c r="U117" s="11" t="s">
-        <v>725</v>
+        <v>928</v>
       </c>
       <c r="V117" s="7" t="s">
-        <v>716</v>
+        <v>693</v>
       </c>
       <c r="W117" s="1" t="s">
         <v>99</v>
@@ -19637,10 +19612,10 @@
         <v>53000115</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>717</v>
+        <v>694</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>718</v>
+        <v>695</v>
       </c>
       <c r="D118" s="25"/>
       <c r="E118" s="1">
@@ -19688,16 +19663,16 @@
         <v>0</v>
       </c>
       <c r="S118" s="1" t="s">
-        <v>719</v>
+        <v>696</v>
       </c>
       <c r="T118">
         <v>100</v>
       </c>
       <c r="U118" s="11" t="s">
-        <v>720</v>
+        <v>927</v>
       </c>
       <c r="V118" s="7" t="s">
-        <v>722</v>
+        <v>698</v>
       </c>
       <c r="W118" s="1" t="s">
         <v>99</v>
@@ -19723,13 +19698,13 @@
         <v>53000116</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>723</v>
+        <v>699</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>724</v>
+        <v>700</v>
       </c>
       <c r="D119" s="25" t="s">
-        <v>721</v>
+        <v>697</v>
       </c>
       <c r="E119" s="1">
         <v>2</v>
@@ -19782,10 +19757,10 @@
         <v>101</v>
       </c>
       <c r="U119" s="11" t="s">
-        <v>726</v>
+        <v>929</v>
       </c>
       <c r="V119" s="7" t="s">
-        <v>776</v>
+        <v>749</v>
       </c>
       <c r="W119" s="1" t="s">
         <v>99</v>
@@ -19811,13 +19786,13 @@
         <v>53000117</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>727</v>
+        <v>701</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>728</v>
+        <v>702</v>
       </c>
       <c r="D120" s="25" t="s">
-        <v>721</v>
+        <v>697</v>
       </c>
       <c r="E120" s="1">
         <v>1</v>
@@ -19864,16 +19839,16 @@
         <v>0</v>
       </c>
       <c r="S120" s="1" t="s">
-        <v>733</v>
+        <v>707</v>
       </c>
       <c r="T120">
         <v>100</v>
       </c>
       <c r="U120" s="11" t="s">
-        <v>913</v>
+        <v>877</v>
       </c>
       <c r="V120" s="7" t="s">
-        <v>774</v>
+        <v>747</v>
       </c>
       <c r="W120" s="1" t="s">
         <v>99</v>
@@ -19899,10 +19874,10 @@
         <v>53000118</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>744</v>
+        <v>718</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>743</v>
+        <v>717</v>
       </c>
       <c r="D121" s="25"/>
       <c r="E121" s="1">
@@ -19950,22 +19925,22 @@
         <v>0</v>
       </c>
       <c r="S121" s="1" t="s">
-        <v>750</v>
+        <v>724</v>
       </c>
       <c r="T121">
         <v>100</v>
       </c>
       <c r="U121" s="11" t="s">
-        <v>745</v>
+        <v>719</v>
       </c>
       <c r="V121" s="7" t="s">
-        <v>748</v>
+        <v>722</v>
       </c>
       <c r="W121" s="1" t="s">
-        <v>749</v>
+        <v>723</v>
       </c>
       <c r="X121" s="1" t="s">
-        <v>749</v>
+        <v>723</v>
       </c>
       <c r="Y121" s="1">
         <v>11000003</v>
@@ -19985,10 +19960,10 @@
         <v>53000119</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>751</v>
+        <v>725</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>752</v>
+        <v>726</v>
       </c>
       <c r="D122" s="25"/>
       <c r="E122" s="1">
@@ -20036,22 +20011,22 @@
         <v>0</v>
       </c>
       <c r="S122" s="1" t="s">
-        <v>756</v>
+        <v>730</v>
       </c>
       <c r="T122">
         <v>105</v>
       </c>
       <c r="U122" s="11" t="s">
-        <v>753</v>
+        <v>727</v>
       </c>
       <c r="V122" s="7" t="s">
-        <v>754</v>
+        <v>728</v>
       </c>
       <c r="W122" s="1" t="s">
-        <v>755</v>
+        <v>729</v>
       </c>
       <c r="X122" s="1" t="s">
-        <v>755</v>
+        <v>729</v>
       </c>
       <c r="Y122" s="1">
         <v>11000003</v>
@@ -20071,13 +20046,13 @@
         <v>53000120</v>
       </c>
       <c r="B123" s="22" t="s">
-        <v>758</v>
+        <v>732</v>
       </c>
       <c r="C123" s="15" t="s">
-        <v>761</v>
+        <v>735</v>
       </c>
       <c r="D123" s="25" t="s">
-        <v>757</v>
+        <v>731</v>
       </c>
       <c r="E123" s="15">
         <v>1</v>
@@ -20130,10 +20105,10 @@
         <v>100</v>
       </c>
       <c r="U123" s="11" t="s">
-        <v>760</v>
+        <v>734</v>
       </c>
       <c r="V123" s="7" t="s">
-        <v>759</v>
+        <v>733</v>
       </c>
       <c r="W123" s="15" t="s">
         <v>57</v>
@@ -20157,13 +20132,13 @@
         <v>53000121</v>
       </c>
       <c r="B124" s="22" t="s">
-        <v>762</v>
+        <v>736</v>
       </c>
       <c r="C124" s="15" t="s">
-        <v>763</v>
+        <v>737</v>
       </c>
       <c r="D124" s="25" t="s">
-        <v>943</v>
+        <v>905</v>
       </c>
       <c r="E124" s="15">
         <v>1</v>
@@ -20210,22 +20185,22 @@
         <v>30</v>
       </c>
       <c r="S124" s="7" t="s">
-        <v>764</v>
+        <v>738</v>
       </c>
       <c r="T124">
         <v>100</v>
       </c>
       <c r="U124" s="11" t="s">
-        <v>773</v>
+        <v>930</v>
       </c>
       <c r="V124" s="1" t="s">
-        <v>765</v>
+        <v>739</v>
       </c>
       <c r="W124" s="15" t="s">
-        <v>766</v>
+        <v>740</v>
       </c>
       <c r="X124" s="15" t="s">
-        <v>766</v>
+        <v>740</v>
       </c>
       <c r="Y124" s="1">
         <v>11000001</v>
@@ -20245,13 +20220,13 @@
         <v>53000122</v>
       </c>
       <c r="B125" s="22" t="s">
-        <v>767</v>
+        <v>741</v>
       </c>
       <c r="C125" s="15" t="s">
-        <v>768</v>
+        <v>742</v>
       </c>
       <c r="D125" s="25" t="s">
-        <v>942</v>
+        <v>904</v>
       </c>
       <c r="E125" s="15">
         <v>1</v>
@@ -20298,22 +20273,22 @@
         <v>0</v>
       </c>
       <c r="S125" s="7" t="s">
-        <v>769</v>
+        <v>743</v>
       </c>
       <c r="T125">
         <v>101</v>
       </c>
       <c r="U125" s="11" t="s">
-        <v>770</v>
+        <v>744</v>
       </c>
       <c r="V125" s="1" t="s">
-        <v>781</v>
+        <v>754</v>
       </c>
       <c r="W125" s="15" t="s">
-        <v>766</v>
+        <v>740</v>
       </c>
       <c r="X125" s="15" t="s">
-        <v>766</v>
+        <v>740</v>
       </c>
       <c r="Y125" s="1">
         <v>11000001</v>
@@ -20333,10 +20308,10 @@
         <v>53000123</v>
       </c>
       <c r="B126" s="22" t="s">
-        <v>772</v>
+        <v>746</v>
       </c>
       <c r="C126" s="15" t="s">
-        <v>771</v>
+        <v>745</v>
       </c>
       <c r="D126" s="25" t="s">
         <v>646</v>
@@ -20386,22 +20361,22 @@
         <v>0</v>
       </c>
       <c r="S126" s="7" t="s">
-        <v>775</v>
+        <v>748</v>
       </c>
       <c r="T126">
         <v>100</v>
       </c>
       <c r="U126" s="11" t="s">
-        <v>914</v>
+        <v>931</v>
       </c>
       <c r="V126" s="1" t="s">
-        <v>777</v>
+        <v>750</v>
       </c>
       <c r="W126" s="15" t="s">
-        <v>766</v>
+        <v>740</v>
       </c>
       <c r="X126" s="15" t="s">
-        <v>766</v>
+        <v>740</v>
       </c>
       <c r="Y126" s="1">
         <v>11000001</v>
@@ -20421,13 +20396,13 @@
         <v>53000124</v>
       </c>
       <c r="B127" s="22" t="s">
-        <v>778</v>
+        <v>751</v>
       </c>
       <c r="C127" s="15" t="s">
-        <v>779</v>
+        <v>752</v>
       </c>
       <c r="D127" s="25" t="s">
-        <v>780</v>
+        <v>753</v>
       </c>
       <c r="E127" s="15">
         <v>2</v>
@@ -20474,22 +20449,22 @@
         <v>0</v>
       </c>
       <c r="S127" s="7" t="s">
-        <v>719</v>
+        <v>696</v>
       </c>
       <c r="T127">
         <v>101</v>
       </c>
       <c r="U127" s="11" t="s">
-        <v>915</v>
+        <v>878</v>
       </c>
       <c r="V127" s="1" t="s">
-        <v>782</v>
+        <v>755</v>
       </c>
       <c r="W127" s="15" t="s">
-        <v>766</v>
+        <v>740</v>
       </c>
       <c r="X127" s="15" t="s">
-        <v>766</v>
+        <v>740</v>
       </c>
       <c r="Y127" s="1">
         <v>11000001</v>
@@ -20509,13 +20484,13 @@
         <v>53000125</v>
       </c>
       <c r="B128" s="22" t="s">
-        <v>783</v>
+        <v>756</v>
       </c>
       <c r="C128" s="15" t="s">
-        <v>784</v>
+        <v>757</v>
       </c>
       <c r="D128" s="25" t="s">
-        <v>785</v>
+        <v>758</v>
       </c>
       <c r="E128" s="15">
         <v>2</v>
@@ -20562,22 +20537,22 @@
         <v>0</v>
       </c>
       <c r="S128" s="7" t="s">
-        <v>786</v>
+        <v>759</v>
       </c>
       <c r="T128">
         <v>100</v>
       </c>
       <c r="U128" s="11" t="s">
-        <v>788</v>
+        <v>932</v>
       </c>
       <c r="V128" s="1" t="s">
-        <v>825</v>
+        <v>795</v>
       </c>
       <c r="W128" s="15" t="s">
-        <v>787</v>
+        <v>760</v>
       </c>
       <c r="X128" s="15" t="s">
-        <v>787</v>
+        <v>760</v>
       </c>
       <c r="Y128" s="1">
         <v>11000002</v>
@@ -20597,10 +20572,10 @@
         <v>53000126</v>
       </c>
       <c r="B129" s="22" t="s">
-        <v>793</v>
+        <v>765</v>
       </c>
       <c r="C129" s="15" t="s">
-        <v>792</v>
+        <v>764</v>
       </c>
       <c r="D129" s="25"/>
       <c r="E129" s="15">
@@ -20648,22 +20623,22 @@
         <v>0</v>
       </c>
       <c r="S129" s="7" t="s">
-        <v>789</v>
+        <v>761</v>
       </c>
       <c r="T129">
         <v>100</v>
       </c>
       <c r="U129" s="11" t="s">
-        <v>801</v>
+        <v>773</v>
       </c>
       <c r="V129" s="1" t="s">
-        <v>803</v>
+        <v>775</v>
       </c>
       <c r="W129" s="1" t="s">
-        <v>844</v>
+        <v>811</v>
       </c>
       <c r="X129" s="1" t="s">
-        <v>749</v>
+        <v>723</v>
       </c>
       <c r="Y129" s="1">
         <v>11000001</v>
@@ -20683,13 +20658,13 @@
         <v>53000127</v>
       </c>
       <c r="B130" s="22" t="s">
-        <v>794</v>
+        <v>766</v>
       </c>
       <c r="C130" s="15" t="s">
-        <v>795</v>
+        <v>767</v>
       </c>
       <c r="D130" s="25" t="s">
-        <v>944</v>
+        <v>906</v>
       </c>
       <c r="E130" s="15">
         <v>4</v>
@@ -20736,22 +20711,22 @@
         <v>15</v>
       </c>
       <c r="S130" s="7" t="s">
-        <v>796</v>
+        <v>768</v>
       </c>
       <c r="T130">
         <v>103</v>
       </c>
       <c r="U130" s="11" t="s">
-        <v>773</v>
+        <v>930</v>
       </c>
       <c r="V130" s="1" t="s">
-        <v>797</v>
+        <v>769</v>
       </c>
       <c r="W130" s="1" t="s">
-        <v>749</v>
+        <v>723</v>
       </c>
       <c r="X130" s="1" t="s">
-        <v>749</v>
+        <v>723</v>
       </c>
       <c r="Y130" s="1">
         <v>11000001</v>
@@ -20771,13 +20746,13 @@
         <v>53000128</v>
       </c>
       <c r="B131" s="22" t="s">
-        <v>800</v>
+        <v>772</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>799</v>
+        <v>771</v>
       </c>
       <c r="D131" s="25" t="s">
-        <v>939</v>
+        <v>901</v>
       </c>
       <c r="E131" s="15">
         <v>1</v>
@@ -20824,22 +20799,22 @@
         <v>25</v>
       </c>
       <c r="S131" s="7" t="s">
-        <v>798</v>
+        <v>770</v>
       </c>
       <c r="T131">
         <v>100</v>
       </c>
       <c r="U131" s="11" t="s">
-        <v>802</v>
+        <v>774</v>
       </c>
       <c r="V131" s="1" t="s">
-        <v>804</v>
+        <v>776</v>
       </c>
       <c r="W131" s="1" t="s">
-        <v>749</v>
+        <v>723</v>
       </c>
       <c r="X131" s="1" t="s">
-        <v>749</v>
+        <v>723</v>
       </c>
       <c r="Y131" s="1">
         <v>11000001</v>
@@ -20859,13 +20834,13 @@
         <v>53000129</v>
       </c>
       <c r="B132" s="22" t="s">
-        <v>818</v>
+        <v>790</v>
       </c>
       <c r="C132" s="15" t="s">
-        <v>817</v>
+        <v>789</v>
       </c>
       <c r="D132" s="25" t="s">
-        <v>819</v>
+        <v>791</v>
       </c>
       <c r="E132" s="15">
         <v>3</v>
@@ -20912,22 +20887,22 @@
         <v>0</v>
       </c>
       <c r="S132" s="7" t="s">
-        <v>827</v>
+        <v>797</v>
       </c>
       <c r="T132">
         <v>103</v>
       </c>
       <c r="U132" s="11" t="s">
-        <v>823</v>
+        <v>933</v>
       </c>
       <c r="V132" s="1" t="s">
-        <v>826</v>
+        <v>796</v>
       </c>
       <c r="W132" s="1" t="s">
-        <v>820</v>
+        <v>792</v>
       </c>
       <c r="X132" s="1" t="s">
-        <v>820</v>
+        <v>792</v>
       </c>
       <c r="Y132" s="1">
         <v>11000002</v>
@@ -20947,13 +20922,13 @@
         <v>53000130</v>
       </c>
       <c r="B133" s="22" t="s">
-        <v>828</v>
+        <v>798</v>
       </c>
       <c r="C133" s="15" t="s">
-        <v>829</v>
+        <v>799</v>
       </c>
       <c r="D133" s="25" t="s">
-        <v>939</v>
+        <v>901</v>
       </c>
       <c r="E133" s="15">
         <v>5</v>
@@ -21000,22 +20975,22 @@
         <v>25</v>
       </c>
       <c r="S133" s="7" t="s">
-        <v>796</v>
+        <v>768</v>
       </c>
       <c r="T133">
         <v>107</v>
       </c>
       <c r="U133" s="11" t="s">
-        <v>831</v>
+        <v>934</v>
       </c>
       <c r="V133" s="1" t="s">
-        <v>833</v>
+        <v>801</v>
       </c>
       <c r="W133" s="1" t="s">
-        <v>834</v>
+        <v>802</v>
       </c>
       <c r="X133" s="1" t="s">
-        <v>834</v>
+        <v>802</v>
       </c>
       <c r="Y133" s="1">
         <v>11000002</v>
@@ -21035,13 +21010,13 @@
         <v>53000131</v>
       </c>
       <c r="B134" s="22" t="s">
-        <v>835</v>
+        <v>803</v>
       </c>
       <c r="C134" s="15" t="s">
-        <v>836</v>
+        <v>804</v>
       </c>
       <c r="D134" s="25" t="s">
-        <v>938</v>
+        <v>900</v>
       </c>
       <c r="E134" s="15">
         <v>2</v>
@@ -21088,22 +21063,22 @@
         <v>30</v>
       </c>
       <c r="S134" s="7" t="s">
-        <v>840</v>
+        <v>808</v>
       </c>
       <c r="T134">
         <v>100</v>
       </c>
       <c r="U134" s="11" t="s">
-        <v>841</v>
+        <v>930</v>
       </c>
       <c r="V134" s="1" t="s">
-        <v>842</v>
+        <v>809</v>
       </c>
       <c r="W134" s="1" t="s">
-        <v>843</v>
+        <v>810</v>
       </c>
       <c r="X134" s="1" t="s">
-        <v>843</v>
+        <v>810</v>
       </c>
       <c r="Y134" s="1">
         <v>11000002</v>
@@ -21123,13 +21098,13 @@
         <v>53000132</v>
       </c>
       <c r="B135" s="22" t="s">
-        <v>837</v>
+        <v>805</v>
       </c>
       <c r="C135" s="15" t="s">
-        <v>838</v>
+        <v>806</v>
       </c>
       <c r="D135" s="25" t="s">
-        <v>839</v>
+        <v>807</v>
       </c>
       <c r="E135" s="15">
         <v>3</v>
@@ -21176,22 +21151,22 @@
         <v>0</v>
       </c>
       <c r="S135" s="7" t="s">
-        <v>845</v>
+        <v>812</v>
       </c>
       <c r="T135">
         <v>102</v>
       </c>
       <c r="U135" s="11" t="s">
-        <v>916</v>
+        <v>879</v>
       </c>
       <c r="V135" s="1" t="s">
-        <v>846</v>
+        <v>813</v>
       </c>
       <c r="W135" s="1" t="s">
-        <v>844</v>
+        <v>811</v>
       </c>
       <c r="X135" s="1" t="s">
-        <v>844</v>
+        <v>811</v>
       </c>
       <c r="Y135" s="1">
         <v>11000002</v>
@@ -21211,13 +21186,13 @@
         <v>53000133</v>
       </c>
       <c r="B136" s="22" t="s">
-        <v>848</v>
+        <v>815</v>
       </c>
       <c r="C136" s="15" t="s">
-        <v>847</v>
+        <v>814</v>
       </c>
       <c r="D136" s="25" t="s">
-        <v>849</v>
+        <v>816</v>
       </c>
       <c r="E136" s="15">
         <v>2</v>
@@ -21270,10 +21245,10 @@
         <v>100</v>
       </c>
       <c r="U136" s="11" t="s">
-        <v>886</v>
+        <v>851</v>
       </c>
       <c r="V136" s="1" t="s">
-        <v>878</v>
+        <v>843</v>
       </c>
       <c r="W136" s="15" t="s">
         <v>4</v>
@@ -21297,13 +21272,13 @@
         <v>53000134</v>
       </c>
       <c r="B137" s="22" t="s">
-        <v>851</v>
+        <v>818</v>
       </c>
       <c r="C137" s="15" t="s">
-        <v>850</v>
+        <v>817</v>
       </c>
       <c r="D137" s="25" t="s">
-        <v>849</v>
+        <v>816</v>
       </c>
       <c r="E137" s="15">
         <v>2</v>
@@ -21356,10 +21331,10 @@
         <v>103</v>
       </c>
       <c r="U137" s="11" t="s">
-        <v>887</v>
+        <v>852</v>
       </c>
       <c r="V137" s="1" t="s">
-        <v>879</v>
+        <v>844</v>
       </c>
       <c r="W137" s="15" t="s">
         <v>4</v>
@@ -21383,13 +21358,13 @@
         <v>53000135</v>
       </c>
       <c r="B138" s="22" t="s">
-        <v>854</v>
+        <v>821</v>
       </c>
       <c r="C138" s="15" t="s">
-        <v>855</v>
+        <v>822</v>
       </c>
       <c r="D138" s="25" t="s">
-        <v>938</v>
+        <v>900</v>
       </c>
       <c r="E138" s="15">
         <v>4</v>
@@ -21436,19 +21411,19 @@
         <v>20</v>
       </c>
       <c r="S138" s="15" t="s">
-        <v>858</v>
+        <v>825</v>
       </c>
       <c r="T138" s="15">
         <v>108</v>
       </c>
       <c r="U138" s="11" t="s">
-        <v>859</v>
+        <v>935</v>
       </c>
       <c r="V138" s="1" t="s">
-        <v>861</v>
+        <v>827</v>
       </c>
       <c r="W138" s="1" t="s">
-        <v>843</v>
+        <v>810</v>
       </c>
       <c r="X138" s="15"/>
       <c r="Y138" s="15">
@@ -21469,13 +21444,13 @@
         <v>53000136</v>
       </c>
       <c r="B139" s="22" t="s">
-        <v>857</v>
+        <v>824</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>856</v>
+        <v>823</v>
       </c>
       <c r="D139" s="25" t="s">
-        <v>938</v>
+        <v>900</v>
       </c>
       <c r="E139" s="15">
         <v>4</v>
@@ -21522,19 +21497,19 @@
         <v>20</v>
       </c>
       <c r="S139" s="15" t="s">
-        <v>862</v>
+        <v>828</v>
       </c>
       <c r="T139" s="15">
         <v>100</v>
       </c>
       <c r="U139" s="11" t="s">
-        <v>863</v>
+        <v>936</v>
       </c>
       <c r="V139" s="1" t="s">
-        <v>865</v>
+        <v>830</v>
       </c>
       <c r="W139" s="15" t="s">
-        <v>902</v>
+        <v>867</v>
       </c>
       <c r="X139" s="15"/>
       <c r="Y139" s="15">
@@ -21555,13 +21530,13 @@
         <v>53000137</v>
       </c>
       <c r="B140" s="22" t="s">
-        <v>866</v>
+        <v>831</v>
       </c>
       <c r="C140" s="15" t="s">
-        <v>867</v>
+        <v>832</v>
       </c>
       <c r="D140" s="25" t="s">
-        <v>868</v>
+        <v>833</v>
       </c>
       <c r="E140" s="15">
         <v>2</v>
@@ -21608,16 +21583,16 @@
         <v>0</v>
       </c>
       <c r="S140" s="15" t="s">
-        <v>871</v>
+        <v>836</v>
       </c>
       <c r="T140" s="15">
         <v>102</v>
       </c>
       <c r="U140" s="11" t="s">
-        <v>869</v>
+        <v>834</v>
       </c>
       <c r="V140" s="1" t="s">
-        <v>870</v>
+        <v>835</v>
       </c>
       <c r="W140" s="15" t="s">
         <v>4</v>
@@ -21641,10 +21616,10 @@
         <v>53000138</v>
       </c>
       <c r="B141" s="22" t="s">
-        <v>888</v>
+        <v>853</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>889</v>
+        <v>854</v>
       </c>
       <c r="D141" s="25" t="s">
         <v>411</v>
@@ -21694,19 +21669,19 @@
         <v>1</v>
       </c>
       <c r="S141" s="15" t="s">
-        <v>750</v>
+        <v>724</v>
       </c>
       <c r="T141" s="15">
         <v>105</v>
       </c>
       <c r="U141" s="11" t="s">
-        <v>899</v>
+        <v>864</v>
       </c>
       <c r="V141" s="1" t="s">
-        <v>896</v>
+        <v>861</v>
       </c>
       <c r="W141" s="1" t="s">
-        <v>749</v>
+        <v>723</v>
       </c>
       <c r="X141" s="15"/>
       <c r="Y141" s="15">
@@ -21727,10 +21702,10 @@
         <v>53000139</v>
       </c>
       <c r="B142" s="22" t="s">
-        <v>891</v>
+        <v>856</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>892</v>
+        <v>857</v>
       </c>
       <c r="D142" s="25" t="s">
         <v>512</v>
@@ -21780,19 +21755,19 @@
         <v>2</v>
       </c>
       <c r="S142" s="15" t="s">
-        <v>871</v>
+        <v>836</v>
       </c>
       <c r="T142" s="15">
         <v>103</v>
       </c>
       <c r="U142" s="11" t="s">
-        <v>898</v>
+        <v>863</v>
       </c>
       <c r="V142" s="1" t="s">
-        <v>893</v>
+        <v>858</v>
       </c>
       <c r="W142" s="15" t="s">
-        <v>901</v>
+        <v>866</v>
       </c>
       <c r="X142" s="15"/>
       <c r="Y142" s="15">
@@ -21813,10 +21788,10 @@
         <v>53000140</v>
       </c>
       <c r="B143" s="22" t="s">
-        <v>894</v>
+        <v>859</v>
       </c>
       <c r="C143" s="15" t="s">
-        <v>895</v>
+        <v>860</v>
       </c>
       <c r="D143" s="25" t="s">
         <v>411</v>
@@ -21866,19 +21841,19 @@
         <v>3</v>
       </c>
       <c r="S143" s="15" t="s">
-        <v>871</v>
+        <v>836</v>
       </c>
       <c r="T143" s="15">
         <v>100</v>
       </c>
       <c r="U143" s="11" t="s">
-        <v>900</v>
+        <v>865</v>
       </c>
       <c r="V143" s="1" t="s">
-        <v>897</v>
+        <v>862</v>
       </c>
       <c r="W143" s="15" t="s">
-        <v>901</v>
+        <v>866</v>
       </c>
       <c r="X143" s="15"/>
       <c r="Y143" s="15">
@@ -22066,7 +22041,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="未完成">
+    <cfRule type="containsText" dxfId="135" priority="1" operator="containsText" text="未完成">
       <formula>NOT(ISERROR(SEARCH("未完成",D138)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22087,7 +22062,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomRight" activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -22154,7 +22129,7 @@
         <v>349</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>732</v>
+        <v>706</v>
       </c>
       <c r="P1" s="17" t="s">
         <v>331</v>
@@ -22240,7 +22215,7 @@
         <v>348</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>730</v>
+        <v>704</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>318</v>
@@ -22326,7 +22301,7 @@
         <v>351</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>731</v>
+        <v>705</v>
       </c>
       <c r="P3" s="20" t="s">
         <v>333</v>
@@ -22428,7 +22403,7 @@
         <v>-1</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>700</v>
+        <v>937</v>
       </c>
       <c r="V4" s="7" t="s">
         <v>342</v>
@@ -22582,16 +22557,16 @@
         <v>0</v>
       </c>
       <c r="S6" s="15" t="s">
-        <v>816</v>
+        <v>788</v>
       </c>
       <c r="T6" s="1">
         <v>-1</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>917</v>
+        <v>938</v>
       </c>
       <c r="V6" s="7" t="s">
-        <v>860</v>
+        <v>826</v>
       </c>
       <c r="W6" s="15" t="s">
         <v>365</v>
@@ -22668,10 +22643,10 @@
         <v>-1</v>
       </c>
       <c r="U7" s="11" t="s">
-        <v>852</v>
+        <v>819</v>
       </c>
       <c r="V7" s="7" t="s">
-        <v>853</v>
+        <v>820</v>
       </c>
       <c r="W7" s="15" t="s">
         <v>2</v>
@@ -23013,7 +22988,7 @@
         <v>53100008</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>808</v>
+        <v>780</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="34"/>
@@ -23062,16 +23037,16 @@
         <v>0</v>
       </c>
       <c r="S12" s="15" t="s">
-        <v>806</v>
+        <v>778</v>
       </c>
       <c r="T12" s="1">
         <v>-1</v>
       </c>
       <c r="U12" s="11" t="s">
-        <v>807</v>
+        <v>779</v>
       </c>
       <c r="V12" s="7" t="s">
-        <v>924</v>
+        <v>886</v>
       </c>
       <c r="W12" s="15" t="s">
         <v>2</v>
@@ -23093,7 +23068,7 @@
         <v>53200001</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>921</v>
+        <v>883</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="34"/>
@@ -23142,19 +23117,19 @@
         <v>0</v>
       </c>
       <c r="S13" s="15" t="s">
-        <v>920</v>
+        <v>882</v>
       </c>
       <c r="T13" s="1">
         <v>-1</v>
       </c>
       <c r="U13" s="11" t="s">
-        <v>918</v>
+        <v>880</v>
       </c>
       <c r="V13" s="7" t="s">
-        <v>925</v>
+        <v>887</v>
       </c>
       <c r="W13" s="15" t="s">
-        <v>919</v>
+        <v>881</v>
       </c>
       <c r="X13" s="15"/>
       <c r="Y13" s="15"/>
@@ -23173,7 +23148,7 @@
         <v>53200002</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>926</v>
+        <v>888</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="44"/>
@@ -23222,16 +23197,16 @@
         <v>0</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>927</v>
+        <v>889</v>
       </c>
       <c r="T14">
         <v>-1</v>
       </c>
       <c r="U14" s="11" t="s">
-        <v>922</v>
+        <v>884</v>
       </c>
       <c r="V14" s="7" t="s">
-        <v>923</v>
+        <v>885</v>
       </c>
       <c r="W14" s="15" t="s">
         <v>2</v>
@@ -23253,7 +23228,7 @@
         <v>53200003</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>936</v>
+        <v>898</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="34"/>
@@ -23308,10 +23283,10 @@
         <v>-1</v>
       </c>
       <c r="U15" s="11" t="s">
-        <v>935</v>
+        <v>897</v>
       </c>
       <c r="V15" s="7" t="s">
-        <v>933</v>
+        <v>895</v>
       </c>
       <c r="W15" s="15" t="s">
         <v>2</v>
@@ -23331,139 +23306,139 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="J4:Q13 J15:Q15">
-    <cfRule type="cellIs" dxfId="104" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="52" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:Q8">
-    <cfRule type="cellIs" dxfId="103" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="48" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:Q4 O4:O13 O15">
-    <cfRule type="cellIs" dxfId="102" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="47" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="101" priority="46" operator="notEqual">
+    <cfRule type="cellIs" dxfId="100" priority="46" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:Q4 O4:O13 O15">
-    <cfRule type="cellIs" dxfId="100" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="45" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="99" priority="44" operator="notEqual">
+    <cfRule type="cellIs" dxfId="98" priority="44" operator="notEqual">
       <formula>$E5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:Q5">
-    <cfRule type="cellIs" dxfId="98" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="43" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" dxfId="97" priority="42" operator="notEqual">
+    <cfRule type="cellIs" dxfId="96" priority="42" operator="notEqual">
       <formula>$E6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:Q6">
-    <cfRule type="cellIs" dxfId="96" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="41" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="95" priority="40" operator="notEqual">
+    <cfRule type="cellIs" dxfId="94" priority="40" operator="notEqual">
       <formula>$E7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:Q7">
-    <cfRule type="cellIs" dxfId="94" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="39" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="93" priority="38" operator="notEqual">
+    <cfRule type="cellIs" dxfId="92" priority="38" operator="notEqual">
       <formula>$E8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:Q8">
-    <cfRule type="cellIs" dxfId="92" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="37" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I13 I15">
-    <cfRule type="cellIs" dxfId="91" priority="36" operator="notEqual">
+    <cfRule type="cellIs" dxfId="90" priority="36" operator="notEqual">
       <formula>$E9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:Q13 J15:Q15">
-    <cfRule type="cellIs" dxfId="90" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="35" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H13 H15">
-    <cfRule type="cellIs" dxfId="89" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="18" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="19" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="20" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="21" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="85" priority="21" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="85" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="14" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="15" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="16" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="17" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="81" priority="17" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10:L13 L15">
-    <cfRule type="cellIs" dxfId="81" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="13" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="80" priority="9" operator="notEqual">
+    <cfRule type="cellIs" dxfId="79" priority="9" operator="notEqual">
       <formula>$E14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="cellIs" dxfId="79" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="5" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="6" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="7" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="75" priority="7" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P14:Q14 J14:N14">
-    <cfRule type="cellIs" dxfId="75" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O14">
-    <cfRule type="cellIs" dxfId="74" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23480,11 +23455,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L1" sqref="L1"/>
+      <selection pane="bottomRight" activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -23552,7 +23527,7 @@
         <v>349</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>732</v>
+        <v>706</v>
       </c>
       <c r="P1" s="17" t="s">
         <v>331</v>
@@ -23638,7 +23613,7 @@
         <v>348</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>730</v>
+        <v>704</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>318</v>
@@ -23724,7 +23699,7 @@
         <v>351</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>731</v>
+        <v>705</v>
       </c>
       <c r="P3" s="20" t="s">
         <v>333</v>
@@ -23830,7 +23805,7 @@
         <v>115</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>701</v>
+        <v>940</v>
       </c>
       <c r="V4" s="7" t="s">
         <v>376</v>
@@ -23914,7 +23889,7 @@
         <v>90</v>
       </c>
       <c r="U5" s="11" t="s">
-        <v>702</v>
+        <v>941</v>
       </c>
       <c r="V5" s="7" t="s">
         <v>378</v>
@@ -24164,7 +24139,7 @@
         <v>90</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>703</v>
+        <v>939</v>
       </c>
       <c r="V8" s="7" t="s">
         <v>387</v>
@@ -24273,50 +24248,50 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I4:I9">
-    <cfRule type="cellIs" dxfId="42" priority="12" operator="notEqual">
+    <cfRule type="cellIs" dxfId="41" priority="12" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:Q7 O4:O9">
-    <cfRule type="cellIs" dxfId="41" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:Q9">
-    <cfRule type="cellIs" dxfId="40" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:Q8">
-    <cfRule type="cellIs" dxfId="39" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H9">
-    <cfRule type="cellIs" dxfId="38" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="6" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="34" priority="8" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="34" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="30" priority="4" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
grave monster skill implement
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="标准" sheetId="1" r:id="rId1"/>
@@ -636,7 +636,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1393" uniqueCount="935">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1393" uniqueCount="934">
   <si>
     <t>慈悲</t>
   </si>
@@ -2290,21 +2290,37 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>召唤师回复{3:0.0}点MP</t>
+  </si>
+  <si>
+    <t>夺取对方召唤师{3:0.0}点MP</t>
+  </si>
+  <si>
     <t>属性</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>召唤师回复{3:0.0}点MP</t>
-  </si>
-  <si>
-    <t>夺取对方召唤师{3:0.0}点MP</t>
+    <t>回复召唤师{3:0.0}点LP和MP，并抽一张牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>属性</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>回复召唤师{3:0.0}点LP和MP，并抽一张牌</t>
+    <t>召唤师回复{3:0.0}点PP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>消耗召唤师所有PP，回复{3:0.0}倍的MP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>回复双方召唤师{3:0.0}点LP和PP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>减少双方召唤师{3:0.0}点LP和MP</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -2312,34 +2328,10 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>召唤师回复{3:0.0}点PP</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>消耗召唤师所有PP，回复{3:0.0}倍的MP</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>回复双方召唤师{3:0.0}点LP和PP</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>减少双方召唤师{3:0.0}点LP和MP</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>属性</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>属性</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>2/3机率减少对方召唤师{3:0.0}点MP，否则减少自身{3:0.0}点MP</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>手牌</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -2448,10 +2440,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>DNS</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>GetDescript</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3567,9 +3555,6 @@
     <t>p.AddMp(spl.Help);p.AddLp(spl.Help);p.Action.GetNextNCard(null,1);</t>
   </si>
   <si>
-    <t>if(MathTool.GetRandom(3)==0)p.AddMp(-spl.Help);else r.AddMp(-spl.Help);</t>
-  </si>
-  <si>
     <t>p.AddLp(spl.Help);t.Action.SuddenDeath();</t>
   </si>
   <si>
@@ -3745,9 +3730,6 @@
   </si>
   <si>
     <t>p.Action.AddTrap(54000006,spl.Id,spl.Level,spl.Rate,spl.Damage,0);</t>
-  </si>
-  <si>
-    <t>p.Action.AddMonster(MathTool.GetRandom(51000001,51000300),spl.Level,m.GetRandomPoint());</t>
   </si>
   <si>
     <t>p.Action.AddTrap(54000004,spl.Id,spl.Level,spl.Rate,0,0);</t>
@@ -3940,6 +3922,22 @@
   </si>
   <si>
     <t>对范围内3个随机敌人造成{0}点魔法伤害</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>p.Action.AddMonster(MathTool.GetRandom(51000001,51000300),spl.Level,m.GetRandomPoint());</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>在指定位置召唤一个我方死亡的随机怪物</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int monId=p.Action.GetGraveMonsterId();if(monId&gt;0)p.Action.AddMonster(monId,spl.Level,mouse);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>DNG</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -7733,7 +7731,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1</c:v>
@@ -8951,11 +8949,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="V18" sqref="V18"/>
+      <selection pane="bottomRight" activeCell="S59" sqref="S59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9024,7 +9022,7 @@
         <v>344</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="P1" s="17" t="s">
         <v>327</v>
@@ -9110,7 +9108,7 @@
         <v>345</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>328</v>
@@ -9196,7 +9194,7 @@
         <v>346</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="P3" s="20" t="s">
         <v>329</v>
@@ -9217,7 +9215,7 @@
         <v>443</v>
       </c>
       <c r="V3" s="6" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="W3" s="6" t="s">
         <v>317</v>
@@ -9249,7 +9247,7 @@
         <v>209</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
@@ -9302,10 +9300,10 @@
         <v>95</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="W4" s="1" t="s">
         <v>2</v>
@@ -9333,7 +9331,7 @@
         <v>210</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -9386,10 +9384,10 @@
         <v>80</v>
       </c>
       <c r="U5" s="11" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="V5" s="7" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="W5" s="1" t="s">
         <v>4</v>
@@ -9417,7 +9415,7 @@
         <v>211</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="E6" s="1">
         <v>2</v>
@@ -9470,7 +9468,7 @@
         <v>100</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="V6" s="7" t="s">
         <v>371</v>
@@ -9501,7 +9499,7 @@
         <v>212</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
@@ -9554,10 +9552,10 @@
         <v>100</v>
       </c>
       <c r="U7" s="11" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="V7" s="7" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="W7" s="1" t="s">
         <v>9</v>
@@ -9587,7 +9585,7 @@
         <v>213</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="E8" s="1">
         <v>3</v>
@@ -9640,7 +9638,7 @@
         <v>100</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="V8" s="7" t="s">
         <v>341</v>
@@ -9673,7 +9671,7 @@
         <v>290</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
@@ -9726,7 +9724,7 @@
         <v>90</v>
       </c>
       <c r="U9" s="11" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="V9" s="7" t="s">
         <v>452</v>
@@ -9757,7 +9755,7 @@
         <v>291</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -9810,7 +9808,7 @@
         <v>90</v>
       </c>
       <c r="U10" s="11" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="V10" s="7" t="s">
         <v>451</v>
@@ -9841,7 +9839,7 @@
         <v>292</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -9894,7 +9892,7 @@
         <v>90</v>
       </c>
       <c r="U11" s="11" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="V11" s="7" t="s">
         <v>453</v>
@@ -9925,7 +9923,7 @@
         <v>293</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
@@ -9978,7 +9976,7 @@
         <v>90</v>
       </c>
       <c r="U12" s="11" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="V12" s="7" t="s">
         <v>454</v>
@@ -10009,7 +10007,7 @@
         <v>214</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
@@ -10062,7 +10060,7 @@
         <v>90</v>
       </c>
       <c r="U13" s="11" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="V13" s="7" t="s">
         <v>455</v>
@@ -10093,7 +10091,7 @@
         <v>208</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
@@ -10146,7 +10144,7 @@
         <v>90</v>
       </c>
       <c r="U14" s="11" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="V14" s="7" t="s">
         <v>456</v>
@@ -10177,7 +10175,7 @@
         <v>215</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
@@ -10230,7 +10228,7 @@
         <v>90</v>
       </c>
       <c r="U15" s="11" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="V15" s="7" t="s">
         <v>457</v>
@@ -10261,7 +10259,7 @@
         <v>366</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="E16" s="15">
         <v>4</v>
@@ -10314,7 +10312,7 @@
         <v>100</v>
       </c>
       <c r="U16" s="11" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="V16" s="7" t="s">
         <v>469</v>
@@ -10347,7 +10345,7 @@
         <v>447</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="E17" s="1">
         <v>2</v>
@@ -10400,10 +10398,10 @@
         <v>100</v>
       </c>
       <c r="U17" s="11" t="s">
-        <v>910</v>
+        <v>905</v>
       </c>
       <c r="V17" s="7" t="s">
-        <v>934</v>
+        <v>929</v>
       </c>
       <c r="W17" s="1" t="s">
         <v>449</v>
@@ -10433,7 +10431,7 @@
         <v>216</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="E18" s="1">
         <v>1</v>
@@ -10486,10 +10484,10 @@
         <v>75</v>
       </c>
       <c r="U18" s="11" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="V18" s="7" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="W18" s="1" t="s">
         <v>15</v>
@@ -10519,7 +10517,7 @@
         <v>217</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="E19" s="1">
         <v>3</v>
@@ -10572,7 +10570,7 @@
         <v>75</v>
       </c>
       <c r="U19" s="11" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="V19" s="7" t="s">
         <v>330</v>
@@ -10605,7 +10603,7 @@
         <v>218</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="E20" s="1">
         <v>7</v>
@@ -10658,13 +10656,13 @@
         <v>100</v>
       </c>
       <c r="U20" s="11" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="V20" s="7" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="X20" s="1"/>
       <c r="Y20" s="1">
@@ -10691,7 +10689,7 @@
         <v>219</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="E21" s="1">
         <v>3</v>
@@ -10744,10 +10742,10 @@
         <v>102</v>
       </c>
       <c r="U21" s="11" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
       <c r="V21" s="7" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="W21" s="1" t="s">
         <v>21</v>
@@ -10777,7 +10775,7 @@
         <v>220</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="E22" s="1">
         <v>4</v>
@@ -10824,13 +10822,13 @@
         <v>40</v>
       </c>
       <c r="S22" s="7" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="T22">
         <v>100</v>
       </c>
       <c r="U22" s="11" t="s">
-        <v>907</v>
+        <v>902</v>
       </c>
       <c r="V22" s="7" t="s">
         <v>477</v>
@@ -10865,7 +10863,7 @@
         <v>221</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="E23" s="1">
         <v>3</v>
@@ -10912,13 +10910,13 @@
         <v>60</v>
       </c>
       <c r="S23" s="7" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="T23">
         <v>100</v>
       </c>
       <c r="U23" s="11" t="s">
-        <v>908</v>
+        <v>903</v>
       </c>
       <c r="V23" s="7" t="s">
         <v>475</v>
@@ -10953,7 +10951,7 @@
         <v>222</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="E24" s="1">
         <v>3</v>
@@ -11000,13 +10998,13 @@
         <v>90</v>
       </c>
       <c r="S24" s="7" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="T24">
         <v>100</v>
       </c>
       <c r="U24" s="11" t="s">
-        <v>909</v>
+        <v>904</v>
       </c>
       <c r="V24" s="7" t="s">
         <v>478</v>
@@ -11041,7 +11039,7 @@
         <v>223</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E25" s="1">
         <v>4</v>
@@ -11094,10 +11092,10 @@
         <v>107</v>
       </c>
       <c r="U25" s="11" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="V25" s="7" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="W25" s="1" t="s">
         <v>29</v>
@@ -11180,7 +11178,7 @@
         <v>100</v>
       </c>
       <c r="U26" s="11" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="V26" s="21" t="s">
         <v>383</v>
@@ -11264,7 +11262,7 @@
         <v>90</v>
       </c>
       <c r="U27" s="11" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="V27" s="7" t="s">
         <v>384</v>
@@ -11297,7 +11295,7 @@
         <v>226</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="E28" s="1">
         <v>3</v>
@@ -11350,7 +11348,7 @@
         <v>100</v>
       </c>
       <c r="U28" s="11" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
       <c r="V28" s="7" t="s">
         <v>471</v>
@@ -11383,7 +11381,7 @@
         <v>227</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="E29" s="1">
         <v>4</v>
@@ -11436,7 +11434,7 @@
         <v>100</v>
       </c>
       <c r="U29" s="11" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="V29" s="7" t="s">
         <v>470</v>
@@ -11469,7 +11467,7 @@
         <v>228</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="E30" s="1">
         <v>1</v>
@@ -11522,10 +11520,10 @@
         <v>96</v>
       </c>
       <c r="U30" s="11" t="s">
-        <v>917</v>
+        <v>912</v>
       </c>
       <c r="V30" s="7" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="W30" s="1" t="s">
         <v>39</v>
@@ -11553,7 +11551,7 @@
         <v>229</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
@@ -11606,10 +11604,10 @@
         <v>96</v>
       </c>
       <c r="U31" s="11" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
       <c r="V31" s="7" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="W31" s="1" t="s">
         <v>41</v>
@@ -11637,7 +11635,7 @@
         <v>230</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="E32" s="1">
         <v>4</v>
@@ -11690,7 +11688,7 @@
         <v>100</v>
       </c>
       <c r="U32" s="11" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="V32" s="21" t="s">
         <v>338</v>
@@ -11774,10 +11772,10 @@
         <v>100</v>
       </c>
       <c r="U33" s="11" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="V33" s="1" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="W33" s="1" t="s">
         <v>4</v>
@@ -11860,10 +11858,10 @@
         <v>100</v>
       </c>
       <c r="U34" s="11" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="V34" s="1" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="W34" s="1" t="s">
         <v>4</v>
@@ -11893,7 +11891,7 @@
         <v>294</v>
       </c>
       <c r="D35" s="25" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="E35" s="1">
         <v>3</v>
@@ -11946,7 +11944,7 @@
         <v>100</v>
       </c>
       <c r="U35" s="11" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="V35" s="7" t="s">
         <v>404</v>
@@ -11981,7 +11979,7 @@
         <v>295</v>
       </c>
       <c r="D36" s="25" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="E36" s="1">
         <v>4</v>
@@ -12034,7 +12032,7 @@
         <v>100</v>
       </c>
       <c r="U36" s="11" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="V36" s="7" t="s">
         <v>348</v>
@@ -12122,7 +12120,7 @@
         <v>100</v>
       </c>
       <c r="U37" s="11" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="V37" s="7" t="s">
         <v>351</v>
@@ -12155,7 +12153,7 @@
         <v>231</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="E38" s="1">
         <v>3</v>
@@ -12202,16 +12200,16 @@
         <v>15</v>
       </c>
       <c r="S38" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="T38">
         <v>100</v>
       </c>
       <c r="U38" s="11" t="s">
-        <v>929</v>
+        <v>924</v>
       </c>
       <c r="V38" s="7" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="W38" s="1" t="s">
         <v>49</v>
@@ -12243,7 +12241,7 @@
         <v>232</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="E39" s="1">
         <v>3</v>
@@ -12290,16 +12288,16 @@
         <v>12</v>
       </c>
       <c r="S39" s="1" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="T39">
         <v>100</v>
       </c>
       <c r="U39" s="11" t="s">
-        <v>880</v>
+        <v>930</v>
       </c>
       <c r="V39" s="1" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="W39" s="1" t="s">
         <v>51</v>
@@ -12329,7 +12327,7 @@
         <v>233</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="E40" s="1">
         <v>1</v>
@@ -12382,7 +12380,7 @@
         <v>100</v>
       </c>
       <c r="U40" s="11" t="s">
-        <v>913</v>
+        <v>908</v>
       </c>
       <c r="V40" s="7" t="s">
         <v>472</v>
@@ -12413,7 +12411,7 @@
         <v>234</v>
       </c>
       <c r="D41" s="25" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="E41" s="1">
         <v>2</v>
@@ -12460,16 +12458,16 @@
         <v>12</v>
       </c>
       <c r="S41" s="1" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="T41">
         <v>100</v>
       </c>
       <c r="U41" s="11" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="V41" s="7" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="W41" s="1" t="s">
         <v>55</v>
@@ -12554,10 +12552,10 @@
         <v>85</v>
       </c>
       <c r="U42" s="11" t="s">
-        <v>881</v>
+        <v>876</v>
       </c>
       <c r="V42" s="1" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="W42" s="1" t="s">
         <v>4</v>
@@ -12640,10 +12638,10 @@
         <v>100</v>
       </c>
       <c r="U43" s="11" t="s">
-        <v>882</v>
+        <v>877</v>
       </c>
       <c r="V43" s="1" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="W43" s="1" t="s">
         <v>4</v>
@@ -12670,10 +12668,10 @@
         <v>56</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="D44" s="25" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E44" s="1">
         <v>2</v>
@@ -12726,10 +12724,10 @@
         <v>100</v>
       </c>
       <c r="U44" s="11" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="V44" s="7" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="W44" s="1" t="s">
         <v>57</v>
@@ -12757,7 +12755,7 @@
         <v>236</v>
       </c>
       <c r="D45" s="25" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="E45" s="1">
         <v>3</v>
@@ -12810,10 +12808,10 @@
         <v>110</v>
       </c>
       <c r="U45" s="11" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="V45" s="7" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="W45" s="1" t="s">
         <v>59</v>
@@ -12845,7 +12843,7 @@
         <v>237</v>
       </c>
       <c r="D46" s="25" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E46" s="1">
         <v>2</v>
@@ -12898,10 +12896,10 @@
         <v>100</v>
       </c>
       <c r="U46" s="11" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="V46" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="W46" s="1" t="s">
         <v>4</v>
@@ -12984,10 +12982,10 @@
         <v>95</v>
       </c>
       <c r="U47" s="11" t="s">
-        <v>883</v>
+        <v>878</v>
       </c>
       <c r="V47" s="1" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="W47" s="1" t="s">
         <v>4</v>
@@ -13064,16 +13062,16 @@
         <v>30</v>
       </c>
       <c r="S48" s="7" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="T48">
         <v>100</v>
       </c>
       <c r="U48" s="11" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="V48" s="1" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="W48" s="1" t="s">
         <v>318</v>
@@ -13103,7 +13101,7 @@
         <v>240</v>
       </c>
       <c r="D49" s="25" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="E49" s="1">
         <v>5</v>
@@ -13156,10 +13154,10 @@
         <v>100</v>
       </c>
       <c r="U49" s="11" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
       <c r="V49" s="7" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="W49" s="1" t="s">
         <v>63</v>
@@ -13189,7 +13187,7 @@
         <v>241</v>
       </c>
       <c r="D50" s="25" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="E50" s="1">
         <v>5</v>
@@ -13242,10 +13240,10 @@
         <v>100</v>
       </c>
       <c r="U50" s="11" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="V50" s="7" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="W50" s="1" t="s">
         <v>65</v>
@@ -13277,7 +13275,7 @@
         <v>242</v>
       </c>
       <c r="D51" s="25" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="E51" s="1">
         <v>5</v>
@@ -13324,16 +13322,16 @@
         <v>0</v>
       </c>
       <c r="S51" s="1" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="T51">
         <v>100</v>
       </c>
       <c r="U51" s="11" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="V51" s="1" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="W51" s="1" t="s">
         <v>21</v>
@@ -13363,7 +13361,7 @@
         <v>243</v>
       </c>
       <c r="D52" s="25" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="E52" s="1">
         <v>3</v>
@@ -13416,10 +13414,10 @@
         <v>105</v>
       </c>
       <c r="U52" s="11" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="V52" s="7" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="W52" s="1" t="s">
         <v>68</v>
@@ -13451,7 +13449,7 @@
         <v>244</v>
       </c>
       <c r="D53" s="25" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="E53" s="1">
         <v>4</v>
@@ -13504,10 +13502,10 @@
         <v>95</v>
       </c>
       <c r="U53" s="11" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="V53" s="7" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="W53" s="1" t="s">
         <v>70</v>
@@ -13537,7 +13535,7 @@
         <v>245</v>
       </c>
       <c r="D54" s="25" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="E54" s="1">
         <v>3</v>
@@ -13590,10 +13588,10 @@
         <v>100</v>
       </c>
       <c r="U54" s="11" t="s">
-        <v>884</v>
+        <v>879</v>
       </c>
       <c r="V54" s="1" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="W54" s="1" t="s">
         <v>72</v>
@@ -13619,13 +13617,13 @@
         <v>53000052</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="D55" s="25" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="E55" s="1">
         <v>1</v>
@@ -13672,19 +13670,19 @@
         <v>0</v>
       </c>
       <c r="S55" s="1" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="T55">
         <v>95</v>
       </c>
       <c r="U55" s="11" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="V55" s="7" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="W55" s="1" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="X55" s="1"/>
       <c r="Y55" s="1">
@@ -13711,7 +13709,7 @@
         <v>246</v>
       </c>
       <c r="D56" s="25" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="E56" s="1">
         <v>3</v>
@@ -13758,16 +13756,16 @@
         <v>20</v>
       </c>
       <c r="S56" s="1" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="T56">
         <v>100</v>
       </c>
       <c r="U56" s="11" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="V56" s="7" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="W56" s="1" t="s">
         <v>74</v>
@@ -13797,7 +13795,7 @@
         <v>195</v>
       </c>
       <c r="D57" s="25" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="E57" s="1">
         <v>3</v>
@@ -13850,10 +13848,10 @@
         <v>100</v>
       </c>
       <c r="U57" s="11" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
       <c r="V57" s="7" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="W57" s="1" t="s">
         <v>76</v>
@@ -13883,7 +13881,7 @@
         <v>247</v>
       </c>
       <c r="D58" s="25" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="E58" s="1">
         <v>4</v>
@@ -13936,10 +13934,10 @@
         <v>100</v>
       </c>
       <c r="U58" s="11" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="V58" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="W58" s="1" t="s">
         <v>2</v>
@@ -13958,7 +13956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:28" ht="36" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:28" ht="60" x14ac:dyDescent="0.15">
       <c r="A59">
         <v>53000056</v>
       </c>
@@ -13969,7 +13967,7 @@
         <v>248</v>
       </c>
       <c r="D59" s="25" t="s">
-        <v>486</v>
+        <v>545</v>
       </c>
       <c r="E59" s="1">
         <v>2</v>
@@ -13997,7 +13995,7 @@
         <v>0</v>
       </c>
       <c r="M59" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N59" s="1">
         <v>0</v>
@@ -14015,17 +14013,17 @@
       <c r="R59" s="1">
         <v>0</v>
       </c>
-      <c r="S59" s="1" t="s">
-        <v>28</v>
+      <c r="S59" s="15" t="s">
+        <v>933</v>
       </c>
       <c r="T59">
         <v>100</v>
       </c>
       <c r="U59" s="11" t="s">
-        <v>820</v>
+        <v>932</v>
       </c>
       <c r="V59" s="1" t="s">
-        <v>498</v>
+        <v>931</v>
       </c>
       <c r="W59" s="1" t="s">
         <v>79</v>
@@ -14108,7 +14106,7 @@
         <v>100</v>
       </c>
       <c r="U60" s="11" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="V60" s="1" t="s">
         <v>485</v>
@@ -14135,10 +14133,10 @@
         <v>53000058</v>
       </c>
       <c r="B61" s="8" t="s">
+        <v>539</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>542</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>545</v>
       </c>
       <c r="D61" s="25" t="s">
         <v>401</v>
@@ -14188,16 +14186,16 @@
         <v>0</v>
       </c>
       <c r="S61" s="1" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="T61">
         <v>100</v>
       </c>
       <c r="U61" s="11" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="V61" s="7" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="W61" s="1" t="s">
         <v>15</v>
@@ -14227,7 +14225,7 @@
         <v>249</v>
       </c>
       <c r="D62" s="25" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="E62" s="1">
         <v>2</v>
@@ -14280,10 +14278,10 @@
         <v>100</v>
       </c>
       <c r="U62" s="11" t="s">
-        <v>902</v>
+        <v>897</v>
       </c>
       <c r="V62" s="7" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="W62" s="1" t="s">
         <v>83</v>
@@ -14313,7 +14311,7 @@
         <v>250</v>
       </c>
       <c r="D63" s="25" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="E63" s="1">
         <v>1</v>
@@ -14366,7 +14364,7 @@
         <v>100</v>
       </c>
       <c r="U63" s="11" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="V63" s="1" t="s">
         <v>385</v>
@@ -14399,7 +14397,7 @@
         <v>251</v>
       </c>
       <c r="D64" s="25" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="E64" s="1">
         <v>4</v>
@@ -14452,7 +14450,7 @@
         <v>100</v>
       </c>
       <c r="U64" s="11" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="V64" s="7" t="s">
         <v>349</v>
@@ -14485,7 +14483,7 @@
         <v>252</v>
       </c>
       <c r="D65" s="25" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="E65" s="1">
         <v>1</v>
@@ -14538,7 +14536,7 @@
         <v>100</v>
       </c>
       <c r="U65" s="11" t="s">
-        <v>885</v>
+        <v>880</v>
       </c>
       <c r="V65" s="7" t="s">
         <v>332</v>
@@ -14571,7 +14569,7 @@
         <v>253</v>
       </c>
       <c r="D66" s="25" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E66" s="1">
         <v>1</v>
@@ -14624,10 +14622,10 @@
         <v>100</v>
       </c>
       <c r="U66" s="11" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="V66" s="7" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="W66" s="1" t="s">
         <v>90</v>
@@ -14657,7 +14655,7 @@
         <v>254</v>
       </c>
       <c r="D67" s="25" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E67" s="1">
         <v>2</v>
@@ -14710,10 +14708,10 @@
         <v>100</v>
       </c>
       <c r="U67" s="11" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="V67" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="W67" s="1" t="s">
         <v>92</v>
@@ -14743,7 +14741,7 @@
         <v>197</v>
       </c>
       <c r="D68" s="25" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="E68" s="1">
         <v>6</v>
@@ -14796,7 +14794,7 @@
         <v>100</v>
       </c>
       <c r="U68" s="11" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="V68" s="1" t="s">
         <v>391</v>
@@ -14882,10 +14880,10 @@
         <v>85</v>
       </c>
       <c r="U69" s="11" t="s">
-        <v>886</v>
+        <v>881</v>
       </c>
       <c r="V69" s="1" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="W69" s="1" t="s">
         <v>4</v>
@@ -14915,7 +14913,7 @@
         <v>256</v>
       </c>
       <c r="D70" s="25" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="E70" s="1">
         <v>3</v>
@@ -14968,10 +14966,10 @@
         <v>100</v>
       </c>
       <c r="U70" s="11" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="V70" s="7" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="W70" s="1" t="s">
         <v>95</v>
@@ -15001,7 +14999,7 @@
         <v>257</v>
       </c>
       <c r="D71" s="25" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="E71" s="1">
         <v>2</v>
@@ -15054,10 +15052,10 @@
         <v>100</v>
       </c>
       <c r="U71" s="11" t="s">
-        <v>887</v>
+        <v>882</v>
       </c>
       <c r="V71" s="7" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="W71" s="1" t="s">
         <v>97</v>
@@ -15089,7 +15087,7 @@
         <v>200</v>
       </c>
       <c r="D72" s="25" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="E72" s="1">
         <v>2</v>
@@ -15142,13 +15140,13 @@
         <v>100</v>
       </c>
       <c r="U72" s="11" t="s">
-        <v>930</v>
+        <v>925</v>
       </c>
       <c r="V72" s="7" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="W72" s="1" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="X72" s="1"/>
       <c r="Y72" s="1">
@@ -15175,7 +15173,7 @@
         <v>202</v>
       </c>
       <c r="D73" s="25" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="E73" s="1">
         <v>2</v>
@@ -15228,10 +15226,10 @@
         <v>100</v>
       </c>
       <c r="U73" s="11" t="s">
-        <v>931</v>
+        <v>926</v>
       </c>
       <c r="V73" s="7" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="W73" s="1" t="s">
         <v>101</v>
@@ -15261,7 +15259,7 @@
         <v>199</v>
       </c>
       <c r="D74" s="25" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="E74" s="1">
         <v>4</v>
@@ -15314,10 +15312,10 @@
         <v>103</v>
       </c>
       <c r="U74" s="11" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="V74" s="7" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="W74" s="1" t="s">
         <v>103</v>
@@ -15349,7 +15347,7 @@
         <v>258</v>
       </c>
       <c r="D75" s="25" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="E75" s="1">
         <v>3</v>
@@ -15402,10 +15400,10 @@
         <v>102</v>
       </c>
       <c r="U75" s="11" t="s">
-        <v>888</v>
+        <v>883</v>
       </c>
       <c r="V75" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="W75" s="1" t="s">
         <v>105</v>
@@ -15435,7 +15433,7 @@
         <v>259</v>
       </c>
       <c r="D76" s="25" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="E76" s="1">
         <v>3</v>
@@ -15488,7 +15486,7 @@
         <v>100</v>
       </c>
       <c r="U76" s="11" t="s">
-        <v>889</v>
+        <v>884</v>
       </c>
       <c r="V76" s="7" t="s">
         <v>468</v>
@@ -15521,7 +15519,7 @@
         <v>296</v>
       </c>
       <c r="D77" s="25" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="E77" s="1">
         <v>3</v>
@@ -15574,10 +15572,10 @@
         <v>103</v>
       </c>
       <c r="U77" s="11" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
       <c r="V77" s="7" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="W77" s="1" t="s">
         <v>109</v>
@@ -15607,7 +15605,7 @@
         <v>260</v>
       </c>
       <c r="D78" s="25" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="E78" s="1">
         <v>4</v>
@@ -15660,7 +15658,7 @@
         <v>95</v>
       </c>
       <c r="U78" s="11" t="s">
-        <v>923</v>
+        <v>918</v>
       </c>
       <c r="V78" s="7" t="s">
         <v>333</v>
@@ -15693,7 +15691,7 @@
         <v>261</v>
       </c>
       <c r="D79" s="25" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="E79" s="1">
         <v>3</v>
@@ -15746,10 +15744,10 @@
         <v>100</v>
       </c>
       <c r="U79" s="11" t="s">
-        <v>890</v>
+        <v>885</v>
       </c>
       <c r="V79" s="7" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="W79" s="1" t="s">
         <v>113</v>
@@ -15781,7 +15779,7 @@
         <v>262</v>
       </c>
       <c r="D80" s="25" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="E80" s="1">
         <v>3</v>
@@ -15834,7 +15832,7 @@
         <v>107</v>
       </c>
       <c r="U80" s="11" t="s">
-        <v>891</v>
+        <v>886</v>
       </c>
       <c r="V80" s="7" t="s">
         <v>334</v>
@@ -15867,7 +15865,7 @@
         <v>263</v>
       </c>
       <c r="D81" s="25" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="E81" s="1">
         <v>1</v>
@@ -15920,10 +15918,10 @@
         <v>100</v>
       </c>
       <c r="U81" s="39" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="V81" s="7" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="W81" s="1" t="s">
         <v>93</v>
@@ -15951,7 +15949,7 @@
         <v>264</v>
       </c>
       <c r="D82" s="25" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="E82" s="1">
         <v>3</v>
@@ -16004,10 +16002,10 @@
         <v>100</v>
       </c>
       <c r="U82" s="11" t="s">
-        <v>924</v>
+        <v>919</v>
       </c>
       <c r="V82" s="7" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="W82" s="1" t="s">
         <v>117</v>
@@ -16039,7 +16037,7 @@
         <v>265</v>
       </c>
       <c r="D83" s="25" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="E83" s="1">
         <v>2</v>
@@ -16086,16 +16084,16 @@
         <v>30</v>
       </c>
       <c r="S83" s="7" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="T83">
         <v>100</v>
       </c>
       <c r="U83" s="11" t="s">
-        <v>892</v>
+        <v>887</v>
       </c>
       <c r="V83" s="7" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="W83" s="1" t="s">
         <v>81</v>
@@ -16127,7 +16125,7 @@
         <v>266</v>
       </c>
       <c r="D84" s="25" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="E84" s="1">
         <v>2</v>
@@ -16174,16 +16172,16 @@
         <v>30</v>
       </c>
       <c r="S84" s="7" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="T84">
         <v>100</v>
       </c>
       <c r="U84" s="11" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="V84" s="7" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="W84" s="1" t="s">
         <v>51</v>
@@ -16215,7 +16213,7 @@
         <v>267</v>
       </c>
       <c r="D85" s="25" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="E85" s="1">
         <v>3</v>
@@ -16268,10 +16266,10 @@
         <v>100</v>
       </c>
       <c r="U85" s="11" t="s">
-        <v>903</v>
+        <v>898</v>
       </c>
       <c r="V85" s="7" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="W85" s="1" t="s">
         <v>122</v>
@@ -16298,10 +16296,10 @@
         <v>160</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>893</v>
+        <v>888</v>
       </c>
       <c r="D86" s="25" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="E86" s="1">
         <v>3</v>
@@ -16354,13 +16352,13 @@
         <v>100</v>
       </c>
       <c r="U86" s="11" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
       <c r="V86" s="7" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="W86" s="1" t="s">
-        <v>894</v>
+        <v>889</v>
       </c>
       <c r="X86" s="1"/>
       <c r="Y86" s="1">
@@ -16387,7 +16385,7 @@
         <v>201</v>
       </c>
       <c r="D87" s="25" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="E87" s="1">
         <v>4</v>
@@ -16434,22 +16432,22 @@
         <v>15</v>
       </c>
       <c r="S87" s="1" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="T87">
         <v>100</v>
       </c>
       <c r="U87" s="11" t="s">
-        <v>895</v>
+        <v>890</v>
       </c>
       <c r="V87" s="7" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="W87" s="1" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="X87" s="1" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="Y87" s="1">
         <v>11000008</v>
@@ -16475,7 +16473,7 @@
         <v>203</v>
       </c>
       <c r="D88" s="25" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="E88" s="1">
         <v>3</v>
@@ -16522,22 +16520,22 @@
         <v>20</v>
       </c>
       <c r="S88" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="T88">
         <v>100</v>
       </c>
       <c r="U88" s="11" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="V88" s="7" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="W88" s="1" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="X88" s="1" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="Y88" s="1">
         <v>11000009</v>
@@ -16563,7 +16561,7 @@
         <v>204</v>
       </c>
       <c r="D89" s="25" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="E89" s="1">
         <v>2</v>
@@ -16616,10 +16614,10 @@
         <v>102</v>
       </c>
       <c r="U89" s="11" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="V89" s="7" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="W89" s="1" t="s">
         <v>2</v>
@@ -16649,7 +16647,7 @@
         <v>205</v>
       </c>
       <c r="D90" s="25" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="E90" s="1">
         <v>3</v>
@@ -16696,16 +16694,16 @@
         <v>40</v>
       </c>
       <c r="S90" s="7" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="T90">
         <v>100</v>
       </c>
       <c r="U90" s="11" t="s">
-        <v>920</v>
+        <v>915</v>
       </c>
       <c r="V90" s="7" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="W90" s="1" t="s">
         <v>59</v>
@@ -16737,7 +16735,7 @@
         <v>268</v>
       </c>
       <c r="D91" s="25" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="E91" s="1">
         <v>3</v>
@@ -16790,7 +16788,7 @@
         <v>100</v>
       </c>
       <c r="U91" s="11" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="V91" s="7" t="s">
         <v>335</v>
@@ -16825,7 +16823,7 @@
         <v>269</v>
       </c>
       <c r="D92" s="25" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="E92" s="1">
         <v>4</v>
@@ -16878,10 +16876,10 @@
         <v>100</v>
       </c>
       <c r="U92" s="11" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="V92" s="7" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="W92" s="1" t="s">
         <v>442</v>
@@ -16913,7 +16911,7 @@
         <v>286</v>
       </c>
       <c r="D93" s="25" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="E93" s="1">
         <v>2</v>
@@ -16966,7 +16964,7 @@
         <v>100</v>
       </c>
       <c r="U93" s="11" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="V93" s="1" t="s">
         <v>350</v>
@@ -16999,7 +16997,7 @@
         <v>270</v>
       </c>
       <c r="D94" s="25" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="E94" s="1">
         <v>2</v>
@@ -17052,7 +17050,7 @@
         <v>100</v>
       </c>
       <c r="U94" s="11" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="V94" s="7" t="s">
         <v>336</v>
@@ -17079,13 +17077,13 @@
         <v>53000092</v>
       </c>
       <c r="B95" s="8" t="s">
+        <v>550</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="D95" s="25" t="s">
         <v>553</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>554</v>
-      </c>
-      <c r="D95" s="25" t="s">
-        <v>556</v>
       </c>
       <c r="E95" s="1">
         <v>3</v>
@@ -17132,19 +17130,19 @@
         <v>0</v>
       </c>
       <c r="S95" s="7" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="T95">
         <v>100</v>
       </c>
       <c r="U95" s="11" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="V95" s="1" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="W95" s="1" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="X95" s="1"/>
       <c r="Y95" s="1">
@@ -17171,7 +17169,7 @@
         <v>271</v>
       </c>
       <c r="D96" s="25" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="E96" s="1">
         <v>2</v>
@@ -17224,10 +17222,10 @@
         <v>100</v>
       </c>
       <c r="U96" s="11" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
       <c r="V96" s="7" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="W96" s="1" t="s">
         <v>133</v>
@@ -17257,7 +17255,7 @@
         <v>272</v>
       </c>
       <c r="D97" s="25" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E97" s="1">
         <v>2</v>
@@ -17310,10 +17308,10 @@
         <v>100</v>
       </c>
       <c r="U97" s="11" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="V97" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="W97" s="1" t="s">
         <v>136</v>
@@ -17343,7 +17341,7 @@
         <v>273</v>
       </c>
       <c r="D98" s="25" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E98" s="1">
         <v>2</v>
@@ -17396,10 +17394,10 @@
         <v>100</v>
       </c>
       <c r="U98" s="11" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="V98" s="7" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="W98" s="1" t="s">
         <v>138</v>
@@ -17431,7 +17429,7 @@
         <v>274</v>
       </c>
       <c r="D99" s="25" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E99" s="1">
         <v>3</v>
@@ -17478,16 +17476,16 @@
         <v>200</v>
       </c>
       <c r="S99" s="1" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="T99">
         <v>104</v>
       </c>
       <c r="U99" s="11" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
       <c r="V99" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="W99" s="1" t="s">
         <v>29</v>
@@ -17517,7 +17515,7 @@
         <v>275</v>
       </c>
       <c r="D100" s="25" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="E100" s="1">
         <v>2</v>
@@ -17570,10 +17568,10 @@
         <v>100</v>
       </c>
       <c r="U100" s="11" t="s">
-        <v>890</v>
+        <v>885</v>
       </c>
       <c r="V100" s="7" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="W100" s="1" t="s">
         <v>81</v>
@@ -17603,7 +17601,7 @@
         <v>287</v>
       </c>
       <c r="D101" s="25" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E101" s="1">
         <v>1</v>
@@ -17656,7 +17654,7 @@
         <v>100</v>
       </c>
       <c r="U101" s="11" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
       <c r="V101" s="7" t="s">
         <v>390</v>
@@ -17689,7 +17687,7 @@
         <v>276</v>
       </c>
       <c r="D102" s="25" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="E102" s="1">
         <v>1</v>
@@ -17742,10 +17740,10 @@
         <v>100</v>
       </c>
       <c r="U102" s="11" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="V102" s="7" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="W102" s="1" t="s">
         <v>97</v>
@@ -17775,7 +17773,7 @@
         <v>277</v>
       </c>
       <c r="D103" s="25" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="E103" s="1">
         <v>4</v>
@@ -17822,16 +17820,16 @@
         <v>0</v>
       </c>
       <c r="S103" s="1" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="T103">
         <v>100</v>
       </c>
       <c r="U103" s="11" t="s">
-        <v>844</v>
+        <v>840</v>
       </c>
       <c r="V103" s="1" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="W103" s="1" t="s">
         <v>143</v>
@@ -17861,7 +17859,7 @@
         <v>288</v>
       </c>
       <c r="D104" s="25" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="E104" s="1">
         <v>3</v>
@@ -17908,16 +17906,16 @@
         <v>0</v>
       </c>
       <c r="S104" s="1" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="T104">
         <v>100</v>
       </c>
       <c r="U104" s="11" t="s">
-        <v>896</v>
+        <v>891</v>
       </c>
       <c r="V104" s="1" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="W104" s="1" t="s">
         <v>166</v>
@@ -17947,7 +17945,7 @@
         <v>278</v>
       </c>
       <c r="D105" s="25" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="E105" s="1">
         <v>1</v>
@@ -18000,7 +17998,7 @@
         <v>100</v>
       </c>
       <c r="U105" s="11" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="V105" s="7" t="s">
         <v>337</v>
@@ -18033,7 +18031,7 @@
         <v>279</v>
       </c>
       <c r="D106" s="25" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="E106" s="1">
         <v>3</v>
@@ -18086,10 +18084,10 @@
         <v>105</v>
       </c>
       <c r="U106" s="11" t="s">
-        <v>921</v>
+        <v>916</v>
       </c>
       <c r="V106" s="7" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="W106" s="1" t="s">
         <v>146</v>
@@ -18121,7 +18119,7 @@
         <v>280</v>
       </c>
       <c r="D107" s="25" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="E107" s="1">
         <v>3</v>
@@ -18174,10 +18172,10 @@
         <v>105</v>
       </c>
       <c r="U107" s="11" t="s">
-        <v>922</v>
+        <v>917</v>
       </c>
       <c r="V107" s="7" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="W107" s="1" t="s">
         <v>148</v>
@@ -18207,7 +18205,7 @@
         <v>207</v>
       </c>
       <c r="D108" s="25" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E108" s="1">
         <v>3</v>
@@ -18260,10 +18258,10 @@
         <v>100</v>
       </c>
       <c r="U108" s="11" t="s">
-        <v>845</v>
+        <v>841</v>
       </c>
       <c r="V108" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="W108" s="1" t="s">
         <v>150</v>
@@ -18293,7 +18291,7 @@
         <v>281</v>
       </c>
       <c r="D109" s="25" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="E109" s="1">
         <v>1</v>
@@ -18346,10 +18344,10 @@
         <v>100</v>
       </c>
       <c r="U109" s="11" t="s">
-        <v>903</v>
+        <v>898</v>
       </c>
       <c r="V109" s="7" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="W109" s="1" t="s">
         <v>152</v>
@@ -18379,7 +18377,7 @@
         <v>282</v>
       </c>
       <c r="D110" s="25" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="E110" s="1">
         <v>1</v>
@@ -18432,10 +18430,10 @@
         <v>100</v>
       </c>
       <c r="U110" s="11" t="s">
-        <v>904</v>
+        <v>899</v>
       </c>
       <c r="V110" s="7" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="W110" s="1" t="s">
         <v>154</v>
@@ -18465,7 +18463,7 @@
         <v>283</v>
       </c>
       <c r="D111" s="25" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="E111" s="1">
         <v>2</v>
@@ -18518,10 +18516,10 @@
         <v>100</v>
       </c>
       <c r="U111" s="11" t="s">
-        <v>925</v>
+        <v>920</v>
       </c>
       <c r="V111" s="7" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="W111" s="1" t="s">
         <v>156</v>
@@ -18551,7 +18549,7 @@
         <v>284</v>
       </c>
       <c r="D112" s="25" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="E112" s="1">
         <v>2</v>
@@ -18604,10 +18602,10 @@
         <v>100</v>
       </c>
       <c r="U112" s="11" t="s">
-        <v>933</v>
+        <v>928</v>
       </c>
       <c r="V112" s="7" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="W112" s="1" t="s">
         <v>158</v>
@@ -18637,7 +18635,7 @@
         <v>285</v>
       </c>
       <c r="D113" s="25" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="E113" s="1">
         <v>3</v>
@@ -18690,10 +18688,10 @@
         <v>103</v>
       </c>
       <c r="U113" s="11" t="s">
-        <v>846</v>
+        <v>842</v>
       </c>
       <c r="V113" s="7" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="W113" s="1" t="s">
         <v>29</v>
@@ -18717,13 +18715,13 @@
         <v>53000111</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="D114" s="25" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="E114" s="1">
         <v>3</v>
@@ -18770,22 +18768,22 @@
         <v>20</v>
       </c>
       <c r="S114" s="1" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="T114">
         <v>100</v>
       </c>
       <c r="U114" s="11" t="s">
-        <v>847</v>
+        <v>843</v>
       </c>
       <c r="V114" s="7" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="W114" s="1" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="X114" s="1" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="Y114" s="1">
         <v>11000007</v>
@@ -18805,13 +18803,13 @@
         <v>53000112</v>
       </c>
       <c r="B115" s="8" t="s">
+        <v>569</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="D115" s="25" t="s">
         <v>572</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>787</v>
-      </c>
-      <c r="D115" s="25" t="s">
-        <v>575</v>
       </c>
       <c r="E115" s="1">
         <v>3</v>
@@ -18858,22 +18856,22 @@
         <v>100</v>
       </c>
       <c r="S115" s="1" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="T115">
         <v>100</v>
       </c>
       <c r="U115" s="11" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
       <c r="V115" s="7" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="W115" s="1" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="X115" s="1" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="Y115" s="1">
         <v>11000009</v>
@@ -18893,10 +18891,10 @@
         <v>53000113</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="D116" s="25"/>
       <c r="E116" s="1">
@@ -18944,22 +18942,22 @@
         <v>0</v>
       </c>
       <c r="S116" s="1" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="T116">
         <v>100</v>
       </c>
       <c r="U116" s="11" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="V116" s="7" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="W116" s="1" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="X116" s="1" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="Y116" s="1">
         <v>11000003</v>
@@ -18979,10 +18977,10 @@
         <v>53000114</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="D117" s="25"/>
       <c r="E117" s="1">
@@ -19030,16 +19028,16 @@
         <v>0</v>
       </c>
       <c r="S117" s="1" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="T117">
         <v>101</v>
       </c>
       <c r="U117" s="11" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="V117" s="7" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="W117" s="1" t="s">
         <v>99</v>
@@ -19065,10 +19063,10 @@
         <v>53000115</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="D118" s="25"/>
       <c r="E118" s="1">
@@ -19116,16 +19114,16 @@
         <v>0</v>
       </c>
       <c r="S118" s="1" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="T118">
         <v>100</v>
       </c>
       <c r="U118" s="11" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="V118" s="7" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="W118" s="1" t="s">
         <v>99</v>
@@ -19151,13 +19149,13 @@
         <v>53000116</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="D119" s="25" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="E119" s="1">
         <v>2</v>
@@ -19210,10 +19208,10 @@
         <v>101</v>
       </c>
       <c r="U119" s="11" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="V119" s="7" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="W119" s="1" t="s">
         <v>99</v>
@@ -19239,13 +19237,13 @@
         <v>53000117</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="D120" s="25" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="E120" s="1">
         <v>1</v>
@@ -19292,16 +19290,16 @@
         <v>0</v>
       </c>
       <c r="S120" s="1" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="T120">
         <v>100</v>
       </c>
       <c r="U120" s="11" t="s">
-        <v>905</v>
+        <v>900</v>
       </c>
       <c r="V120" s="7" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="W120" s="1" t="s">
         <v>99</v>
@@ -19327,10 +19325,10 @@
         <v>53000118</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="D121" s="25"/>
       <c r="E121" s="1">
@@ -19378,22 +19376,22 @@
         <v>0</v>
       </c>
       <c r="S121" s="1" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="T121">
         <v>100</v>
       </c>
       <c r="U121" s="11" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
       <c r="V121" s="7" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="W121" s="1" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="X121" s="1" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="Y121" s="1">
         <v>11000003</v>
@@ -19413,10 +19411,10 @@
         <v>53000119</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="D122" s="25"/>
       <c r="E122" s="1">
@@ -19464,22 +19462,22 @@
         <v>0</v>
       </c>
       <c r="S122" s="1" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="T122">
         <v>105</v>
       </c>
       <c r="U122" s="11" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
       <c r="V122" s="7" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="W122" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="X122" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="Y122" s="1">
         <v>11000003</v>
@@ -19499,13 +19497,13 @@
         <v>53000120</v>
       </c>
       <c r="B123" s="22" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="C123" s="15" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="D123" s="25" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="E123" s="15">
         <v>1</v>
@@ -19558,10 +19556,10 @@
         <v>100</v>
       </c>
       <c r="U123" s="11" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="V123" s="7" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="W123" s="15" t="s">
         <v>57</v>
@@ -19585,13 +19583,13 @@
         <v>53000121</v>
       </c>
       <c r="B124" s="22" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="C124" s="15" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="D124" s="25" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="E124" s="15">
         <v>1</v>
@@ -19638,22 +19636,22 @@
         <v>30</v>
       </c>
       <c r="S124" s="7" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="T124">
         <v>100</v>
       </c>
       <c r="U124" s="11" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="V124" s="1" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="W124" s="15" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="X124" s="15" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="Y124" s="1">
         <v>11000001</v>
@@ -19673,13 +19671,13 @@
         <v>53000122</v>
       </c>
       <c r="B125" s="22" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="C125" s="15" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="D125" s="25" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="E125" s="15">
         <v>1</v>
@@ -19726,22 +19724,22 @@
         <v>0</v>
       </c>
       <c r="S125" s="7" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="T125">
         <v>101</v>
       </c>
       <c r="U125" s="11" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
       <c r="V125" s="1" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="W125" s="15" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="X125" s="15" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="Y125" s="1">
         <v>11000001</v>
@@ -19761,13 +19759,13 @@
         <v>53000123</v>
       </c>
       <c r="B126" s="22" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="C126" s="15" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="D126" s="25" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="E126" s="15">
         <v>1</v>
@@ -19814,22 +19812,22 @@
         <v>0</v>
       </c>
       <c r="S126" s="7" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="T126">
         <v>100</v>
       </c>
       <c r="U126" s="11" t="s">
-        <v>906</v>
+        <v>901</v>
       </c>
       <c r="V126" s="1" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="W126" s="15" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="X126" s="15" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="Y126" s="1">
         <v>11000001</v>
@@ -19849,13 +19847,13 @@
         <v>53000124</v>
       </c>
       <c r="B127" s="22" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="C127" s="15" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="D127" s="25" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="E127" s="15">
         <v>2</v>
@@ -19902,22 +19900,22 @@
         <v>0</v>
       </c>
       <c r="S127" s="7" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="T127">
         <v>101</v>
       </c>
       <c r="U127" s="11" t="s">
-        <v>912</v>
+        <v>907</v>
       </c>
       <c r="V127" s="1" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="W127" s="15" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="X127" s="15" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="Y127" s="1">
         <v>11000001</v>
@@ -19937,13 +19935,13 @@
         <v>53000125</v>
       </c>
       <c r="B128" s="22" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="C128" s="15" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="D128" s="25" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="E128" s="15">
         <v>2</v>
@@ -19990,22 +19988,22 @@
         <v>0</v>
       </c>
       <c r="S128" s="7" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="T128">
         <v>100</v>
       </c>
       <c r="U128" s="11" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="V128" s="1" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="W128" s="15" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="X128" s="15" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="Y128" s="1">
         <v>11000002</v>
@@ -20025,10 +20023,10 @@
         <v>53000126</v>
       </c>
       <c r="B129" s="22" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="C129" s="15" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="D129" s="25"/>
       <c r="E129" s="15">
@@ -20076,22 +20074,22 @@
         <v>0</v>
       </c>
       <c r="S129" s="7" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="T129">
         <v>100</v>
       </c>
       <c r="U129" s="11" t="s">
-        <v>897</v>
+        <v>892</v>
       </c>
       <c r="V129" s="1" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="W129" s="1" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="X129" s="1" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="Y129" s="1">
         <v>11000001</v>
@@ -20111,13 +20109,13 @@
         <v>53000127</v>
       </c>
       <c r="B130" s="22" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="C130" s="15" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="D130" s="25" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="E130" s="15">
         <v>4</v>
@@ -20164,22 +20162,22 @@
         <v>15</v>
       </c>
       <c r="S130" s="7" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="T130">
         <v>103</v>
       </c>
       <c r="U130" s="11" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="V130" s="1" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="W130" s="1" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="X130" s="1" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="Y130" s="1">
         <v>11000001</v>
@@ -20199,13 +20197,13 @@
         <v>53000128</v>
       </c>
       <c r="B131" s="22" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="D131" s="25" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="E131" s="15">
         <v>1</v>
@@ -20252,22 +20250,22 @@
         <v>25</v>
       </c>
       <c r="S131" s="7" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="T131">
         <v>100</v>
       </c>
       <c r="U131" s="11" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="V131" s="1" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="W131" s="1" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="X131" s="1" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="Y131" s="1">
         <v>11000001</v>
@@ -20287,13 +20285,13 @@
         <v>53000129</v>
       </c>
       <c r="B132" s="22" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="C132" s="15" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="D132" s="25" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="E132" s="15">
         <v>3</v>
@@ -20340,22 +20338,22 @@
         <v>0</v>
       </c>
       <c r="S132" s="7" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="T132">
         <v>103</v>
       </c>
       <c r="U132" s="11" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="V132" s="1" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="W132" s="1" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="X132" s="1" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="Y132" s="1">
         <v>11000002</v>
@@ -20375,13 +20373,13 @@
         <v>53000130</v>
       </c>
       <c r="B133" s="22" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="C133" s="15" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="D133" s="25" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="E133" s="15">
         <v>5</v>
@@ -20428,22 +20426,22 @@
         <v>25</v>
       </c>
       <c r="S133" s="7" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="T133">
         <v>107</v>
       </c>
       <c r="U133" s="11" t="s">
-        <v>898</v>
+        <v>893</v>
       </c>
       <c r="V133" s="1" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="W133" s="1" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="X133" s="1" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="Y133" s="1">
         <v>11000002</v>
@@ -20463,13 +20461,13 @@
         <v>53000131</v>
       </c>
       <c r="B134" s="22" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="C134" s="15" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="D134" s="25" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="E134" s="15">
         <v>2</v>
@@ -20516,22 +20514,22 @@
         <v>30</v>
       </c>
       <c r="S134" s="7" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="T134">
         <v>100</v>
       </c>
       <c r="U134" s="11" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="V134" s="1" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="W134" s="1" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="X134" s="1" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="Y134" s="1">
         <v>11000002</v>
@@ -20551,13 +20549,13 @@
         <v>53000132</v>
       </c>
       <c r="B135" s="22" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="C135" s="15" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="D135" s="25" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="E135" s="15">
         <v>3</v>
@@ -20604,22 +20602,22 @@
         <v>0</v>
       </c>
       <c r="S135" s="7" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="T135">
         <v>102</v>
       </c>
       <c r="U135" s="11" t="s">
-        <v>911</v>
+        <v>906</v>
       </c>
       <c r="V135" s="1" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="W135" s="1" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="X135" s="1" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="Y135" s="1">
         <v>11000002</v>
@@ -20639,13 +20637,13 @@
         <v>53000133</v>
       </c>
       <c r="B136" s="22" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="C136" s="15" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="D136" s="25" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="E136" s="15">
         <v>2</v>
@@ -20698,10 +20696,10 @@
         <v>100</v>
       </c>
       <c r="U136" s="11" t="s">
-        <v>899</v>
+        <v>894</v>
       </c>
       <c r="V136" s="1" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="W136" s="15" t="s">
         <v>4</v>
@@ -20725,13 +20723,13 @@
         <v>53000134</v>
       </c>
       <c r="B137" s="22" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="C137" s="15" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="D137" s="25" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="E137" s="15">
         <v>2</v>
@@ -20784,10 +20782,10 @@
         <v>103</v>
       </c>
       <c r="U137" s="11" t="s">
-        <v>900</v>
+        <v>895</v>
       </c>
       <c r="V137" s="1" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="W137" s="15" t="s">
         <v>4</v>
@@ -20811,13 +20809,13 @@
         <v>53000135</v>
       </c>
       <c r="B138" s="22" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="C138" s="15" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="D138" s="25" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="E138" s="15">
         <v>4</v>
@@ -20864,19 +20862,19 @@
         <v>20</v>
       </c>
       <c r="S138" s="15" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="T138" s="15">
         <v>108</v>
       </c>
       <c r="U138" s="11" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
       <c r="V138" s="1" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="W138" s="1" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="X138" s="15"/>
       <c r="Y138" s="15">
@@ -20897,13 +20895,13 @@
         <v>53000136</v>
       </c>
       <c r="B139" s="22" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="D139" s="25" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="E139" s="15">
         <v>4</v>
@@ -20950,19 +20948,19 @@
         <v>20</v>
       </c>
       <c r="S139" s="15" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="T139" s="15">
         <v>100</v>
       </c>
       <c r="U139" s="11" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="V139" s="1" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="W139" s="15" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="X139" s="15"/>
       <c r="Y139" s="15">
@@ -20983,13 +20981,13 @@
         <v>53000137</v>
       </c>
       <c r="B140" s="22" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="C140" s="15" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="D140" s="25" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="E140" s="15">
         <v>2</v>
@@ -21036,16 +21034,16 @@
         <v>0</v>
       </c>
       <c r="S140" s="15" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="T140" s="15">
         <v>102</v>
       </c>
       <c r="U140" s="11" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="V140" s="1" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="W140" s="15" t="s">
         <v>4</v>
@@ -21069,10 +21067,10 @@
         <v>53000138</v>
       </c>
       <c r="B141" s="22" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="D141" s="25" t="s">
         <v>399</v>
@@ -21122,19 +21120,19 @@
         <v>1</v>
       </c>
       <c r="S141" s="15" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="T141" s="15">
         <v>105</v>
       </c>
       <c r="U141" s="11" t="s">
-        <v>926</v>
+        <v>921</v>
       </c>
       <c r="V141" s="1" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="W141" s="1" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="X141" s="15"/>
       <c r="Y141" s="15">
@@ -21155,10 +21153,10 @@
         <v>53000139</v>
       </c>
       <c r="B142" s="22" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="D142" s="25" t="s">
         <v>474</v>
@@ -21208,19 +21206,19 @@
         <v>2</v>
       </c>
       <c r="S142" s="15" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="T142" s="15">
         <v>103</v>
       </c>
       <c r="U142" s="11" t="s">
-        <v>901</v>
+        <v>896</v>
       </c>
       <c r="V142" s="1" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="W142" s="15" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="X142" s="15"/>
       <c r="Y142" s="15">
@@ -21241,10 +21239,10 @@
         <v>53000140</v>
       </c>
       <c r="B143" s="22" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="C143" s="15" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="D143" s="25" t="s">
         <v>399</v>
@@ -21294,19 +21292,19 @@
         <v>3</v>
       </c>
       <c r="S143" s="15" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="T143" s="15">
         <v>100</v>
       </c>
       <c r="U143" s="11" t="s">
-        <v>927</v>
+        <v>922</v>
       </c>
       <c r="V143" s="1" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="W143" s="15" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="X143" s="15"/>
       <c r="Y143" s="15">
@@ -21364,11 +21362,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="U14" sqref="U14"/>
+      <selection pane="bottomRight" activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -21435,7 +21433,7 @@
         <v>344</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="P1" s="17" t="s">
         <v>327</v>
@@ -21521,7 +21519,7 @@
         <v>343</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>314</v>
@@ -21607,7 +21605,7 @@
         <v>346</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="P3" s="20" t="s">
         <v>329</v>
@@ -21709,7 +21707,7 @@
         <v>-1</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="V4" s="7" t="s">
         <v>337</v>
@@ -21789,10 +21787,10 @@
         <v>-1</v>
       </c>
       <c r="U5" s="11" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="V5" s="7" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="W5" s="1" t="s">
         <v>15</v>
@@ -21863,16 +21861,16 @@
         <v>0</v>
       </c>
       <c r="S6" s="15" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="T6" s="1">
         <v>-1</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
       <c r="V6" s="7" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="W6" s="15" t="s">
         <v>359</v>
@@ -21949,10 +21947,10 @@
         <v>-1</v>
       </c>
       <c r="U7" s="11" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="V7" s="7" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="W7" s="15" t="s">
         <v>2</v>
@@ -22029,7 +22027,7 @@
         <v>-1</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="V8" s="7" t="s">
         <v>370</v>
@@ -22109,7 +22107,7 @@
         <v>-1</v>
       </c>
       <c r="U9" s="11" t="s">
-        <v>914</v>
+        <v>909</v>
       </c>
       <c r="V9" s="7" t="s">
         <v>368</v>
@@ -22189,7 +22187,7 @@
         <v>-1</v>
       </c>
       <c r="U10" s="11" t="s">
-        <v>915</v>
+        <v>910</v>
       </c>
       <c r="V10" s="7" t="s">
         <v>482</v>
@@ -22214,7 +22212,7 @@
         <v>53100007</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="34"/>
@@ -22263,16 +22261,16 @@
         <v>0</v>
       </c>
       <c r="S11" s="15" t="s">
-        <v>526</v>
+        <v>933</v>
       </c>
       <c r="T11" s="1">
         <v>-1</v>
       </c>
       <c r="U11" s="11" t="s">
-        <v>916</v>
+        <v>911</v>
       </c>
       <c r="V11" s="7" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="W11" s="15" t="s">
         <v>2</v>
@@ -22294,7 +22292,7 @@
         <v>53100008</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="34"/>
@@ -22343,16 +22341,16 @@
         <v>0</v>
       </c>
       <c r="S12" s="15" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="T12" s="1">
         <v>-1</v>
       </c>
       <c r="U12" s="11" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="V12" s="7" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="W12" s="15" t="s">
         <v>2</v>
@@ -22374,7 +22372,7 @@
         <v>53200001</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="34"/>
@@ -22423,19 +22421,19 @@
         <v>0</v>
       </c>
       <c r="S13" s="15" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="T13" s="1">
         <v>-1</v>
       </c>
       <c r="U13" s="11" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="V13" s="7" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="W13" s="15" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="X13" s="15"/>
       <c r="Y13" s="15"/>
@@ -22454,7 +22452,7 @@
         <v>53200002</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="44"/>
@@ -22503,16 +22501,16 @@
         <v>0</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="T14">
         <v>-1</v>
       </c>
       <c r="U14" s="11" t="s">
-        <v>932</v>
+        <v>927</v>
       </c>
       <c r="V14" s="7" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="W14" s="15" t="s">
         <v>2</v>
@@ -22534,7 +22532,7 @@
         <v>53200003</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="34"/>
@@ -22583,16 +22581,16 @@
         <v>0</v>
       </c>
       <c r="S15" s="15" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="T15" s="1">
         <v>-1</v>
       </c>
       <c r="U15" s="11" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="V15" s="7" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="W15" s="15" t="s">
         <v>2</v>
@@ -22722,7 +22720,7 @@
         <v>344</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="P1" s="17" t="s">
         <v>327</v>
@@ -22808,7 +22806,7 @@
         <v>343</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>314</v>
@@ -22894,7 +22892,7 @@
         <v>346</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="P3" s="20" t="s">
         <v>329</v>
@@ -23000,7 +22998,7 @@
         <v>115</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="V4" s="7" t="s">
         <v>369</v>
@@ -23084,7 +23082,7 @@
         <v>90</v>
       </c>
       <c r="U5" s="11" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="V5" s="7" t="s">
         <v>371</v>
@@ -23168,7 +23166,7 @@
         <v>115</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="V6" s="31" t="s">
         <v>410</v>
@@ -23334,7 +23332,7 @@
         <v>90</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
       <c r="V8" s="7" t="s">
         <v>380</v>
@@ -23420,7 +23418,7 @@
         <v>400</v>
       </c>
       <c r="U9" s="11" t="s">
-        <v>928</v>
+        <v>923</v>
       </c>
       <c r="V9" s="7" t="s">
         <v>331</v>
@@ -23784,7 +23782,7 @@
       </c>
       <c r="B11">
         <f>COUNTIF(标准!D:D,"*属性*")</f>
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
rearrange the code the carddeck
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -3497,9 +3497,6 @@
     <t>r.Action.ConvertCard(2,51000019,(int)-spl.Help);</t>
   </si>
   <si>
-    <t>p.Action.CardLevelUp((int)spl.Help, 0);</t>
-  </si>
-  <si>
     <t>r.Action.DeleteRandomCardFor(p,(int)spl.Help);</t>
   </si>
   <si>
@@ -3591,9 +3588,6 @@
   </si>
   <si>
     <t>m.RemoveTomb(mouse);foreach(IMonster im in m.GetRangeMonster(p.IsLeft,spl.Target,spl.Shape,spl.Range,mouse))im.AddHp(spl.Cure);</t>
-  </si>
-  <si>
-    <t>r.Action.CardLevelUp(-(int)spl.Help,3);</t>
   </si>
   <si>
     <t>t.OnSpellDamage( spl.Damage,spl.Attr);p.Action.AddCard(null,spl.Id, spl.Level);</t>
@@ -3946,6 +3940,14 @@
   </si>
   <si>
     <t>IsNew</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>p.Action.CardLevelUp((int)spl.Help,0,false);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>r.Action.CardLevelUp(-(int)spl.Help,3,false);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -4974,186 +4976,8 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -5174,43 +4998,6 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -5982,6 +5769,71 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -6006,6 +5858,26 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -6779,6 +6651,51 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -6803,6 +6720,26 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -7573,6 +7510,71 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -8569,135 +8571,135 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AC143" totalsRowShown="0" headerRowDxfId="112" dataDxfId="111" tableBorderDxfId="110">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AC143" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105" tableBorderDxfId="104">
   <autoFilter ref="A3:AC143"/>
   <sortState ref="A4:AC113">
     <sortCondition ref="A3:A113"/>
   </sortState>
   <tableColumns count="29">
-    <tableColumn id="1" name="Id" dataDxfId="109"/>
-    <tableColumn id="2" name="Name" dataDxfId="108"/>
-    <tableColumn id="20" name="Ename" dataDxfId="107"/>
-    <tableColumn id="21" name="Remark" dataDxfId="106"/>
-    <tableColumn id="3" name="Star" dataDxfId="105"/>
-    <tableColumn id="4" name="Type" dataDxfId="104"/>
-    <tableColumn id="5" name="Attr" dataDxfId="103"/>
-    <tableColumn id="8" name="Quality" dataDxfId="102">
+    <tableColumn id="1" name="Id" dataDxfId="103"/>
+    <tableColumn id="2" name="Name" dataDxfId="102"/>
+    <tableColumn id="20" name="Ename" dataDxfId="101"/>
+    <tableColumn id="21" name="Remark" dataDxfId="100"/>
+    <tableColumn id="3" name="Star" dataDxfId="99"/>
+    <tableColumn id="4" name="Type" dataDxfId="98"/>
+    <tableColumn id="5" name="Attr" dataDxfId="97"/>
+    <tableColumn id="8" name="Quality" dataDxfId="96">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="101"/>
-    <tableColumn id="9" name="Damage" dataDxfId="100"/>
-    <tableColumn id="10" name="Cure" dataDxfId="99"/>
-    <tableColumn id="11" name="Time" dataDxfId="98"/>
-    <tableColumn id="13" name="Help" dataDxfId="97"/>
-    <tableColumn id="16" name="Rate" dataDxfId="96"/>
-    <tableColumn id="18" name="Atk" dataDxfId="95"/>
-    <tableColumn id="12" name="Modify" dataDxfId="94"/>
-    <tableColumn id="27" name="Sum" dataDxfId="93">
+    <tableColumn id="7" name="Cost" dataDxfId="95"/>
+    <tableColumn id="9" name="Damage" dataDxfId="94"/>
+    <tableColumn id="10" name="Cure" dataDxfId="93"/>
+    <tableColumn id="11" name="Time" dataDxfId="92"/>
+    <tableColumn id="13" name="Help" dataDxfId="91"/>
+    <tableColumn id="16" name="Rate" dataDxfId="90"/>
+    <tableColumn id="18" name="Atk" dataDxfId="89"/>
+    <tableColumn id="12" name="Modify" dataDxfId="88"/>
+    <tableColumn id="27" name="Sum" dataDxfId="87">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="92"/>
-    <tableColumn id="15" name="Target" dataDxfId="91"/>
-    <tableColumn id="25" name="Mark" dataDxfId="90"/>
-    <tableColumn id="22" name="Effect" dataDxfId="89"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="88"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="87"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="86"/>
-    <tableColumn id="26" name="JobId" dataDxfId="85"/>
-    <tableColumn id="19" name="Icon" dataDxfId="84"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="83"/>
-    <tableColumn id="29" name="IsHeroCard" dataDxfId="0"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="82"/>
+    <tableColumn id="6" name="Range" dataDxfId="86"/>
+    <tableColumn id="15" name="Target" dataDxfId="85"/>
+    <tableColumn id="25" name="Mark" dataDxfId="84"/>
+    <tableColumn id="22" name="Effect" dataDxfId="83"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="82"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="81"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="80"/>
+    <tableColumn id="26" name="JobId" dataDxfId="79"/>
+    <tableColumn id="19" name="Icon" dataDxfId="78"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="77"/>
+    <tableColumn id="29" name="IsHeroCard" dataDxfId="76"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="75"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AC15" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80" tableBorderDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AC15" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67" tableBorderDxfId="66">
   <autoFilter ref="A3:AC15"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="29">
-    <tableColumn id="1" name="Id" dataDxfId="78"/>
-    <tableColumn id="2" name="Name" dataDxfId="77"/>
-    <tableColumn id="20" name="Ename" dataDxfId="76"/>
-    <tableColumn id="21" name="Remark" dataDxfId="75"/>
-    <tableColumn id="3" name="Star" dataDxfId="74"/>
-    <tableColumn id="4" name="Type" dataDxfId="73"/>
-    <tableColumn id="5" name="Attr" dataDxfId="72"/>
-    <tableColumn id="8" name="Quality" dataDxfId="71">
+    <tableColumn id="1" name="Id" dataDxfId="65"/>
+    <tableColumn id="2" name="Name" dataDxfId="64"/>
+    <tableColumn id="20" name="Ename" dataDxfId="63"/>
+    <tableColumn id="21" name="Remark" dataDxfId="62"/>
+    <tableColumn id="3" name="Star" dataDxfId="61"/>
+    <tableColumn id="4" name="Type" dataDxfId="60"/>
+    <tableColumn id="5" name="Attr" dataDxfId="59"/>
+    <tableColumn id="8" name="Quality" dataDxfId="58">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="70"/>
-    <tableColumn id="9" name="Damage" dataDxfId="69"/>
-    <tableColumn id="10" name="Cure" dataDxfId="68"/>
-    <tableColumn id="11" name="Time" dataDxfId="67"/>
-    <tableColumn id="13" name="Help" dataDxfId="66"/>
-    <tableColumn id="16" name="Rate" dataDxfId="65"/>
-    <tableColumn id="18" name="Atk" dataDxfId="64"/>
-    <tableColumn id="12" name="Modify" dataDxfId="63"/>
-    <tableColumn id="27" name="Sum" dataDxfId="62">
+    <tableColumn id="7" name="Cost" dataDxfId="57"/>
+    <tableColumn id="9" name="Damage" dataDxfId="56"/>
+    <tableColumn id="10" name="Cure" dataDxfId="55"/>
+    <tableColumn id="11" name="Time" dataDxfId="54"/>
+    <tableColumn id="13" name="Help" dataDxfId="53"/>
+    <tableColumn id="16" name="Rate" dataDxfId="52"/>
+    <tableColumn id="18" name="Atk" dataDxfId="51"/>
+    <tableColumn id="12" name="Modify" dataDxfId="50"/>
+    <tableColumn id="27" name="Sum" dataDxfId="49">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="61"/>
-    <tableColumn id="15" name="Target" dataDxfId="60"/>
-    <tableColumn id="25" name="Mark" dataDxfId="59"/>
-    <tableColumn id="22" name="Effect" dataDxfId="58"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="57"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="56"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="55"/>
-    <tableColumn id="26" name="JobId" dataDxfId="54"/>
-    <tableColumn id="19" name="Icon" dataDxfId="53"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="52"/>
-    <tableColumn id="29" name="IsHeroCard" dataDxfId="20"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="51"/>
+    <tableColumn id="6" name="Range" dataDxfId="48"/>
+    <tableColumn id="15" name="Target" dataDxfId="47"/>
+    <tableColumn id="25" name="Mark" dataDxfId="46"/>
+    <tableColumn id="22" name="Effect" dataDxfId="45"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="44"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="43"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="42"/>
+    <tableColumn id="26" name="JobId" dataDxfId="41"/>
+    <tableColumn id="19" name="Icon" dataDxfId="40"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="39"/>
+    <tableColumn id="29" name="IsHeroCard" dataDxfId="38"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_35" displayName="表1_35" ref="A3:AC9" totalsRowShown="0" headerRowDxfId="50" tableBorderDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_35" displayName="表1_35" ref="A3:AC9" totalsRowShown="0" headerRowDxfId="30" tableBorderDxfId="29">
   <autoFilter ref="A3:AC9"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="29">
-    <tableColumn id="1" name="Id" dataDxfId="48"/>
-    <tableColumn id="2" name="Name" dataDxfId="47"/>
-    <tableColumn id="20" name="Ename" dataDxfId="46"/>
-    <tableColumn id="21" name="Remark" dataDxfId="45"/>
-    <tableColumn id="3" name="Star" dataDxfId="44"/>
-    <tableColumn id="4" name="Type" dataDxfId="43"/>
-    <tableColumn id="5" name="Attr" dataDxfId="42"/>
-    <tableColumn id="8" name="Quality" dataDxfId="41">
+    <tableColumn id="1" name="Id" dataDxfId="28"/>
+    <tableColumn id="2" name="Name" dataDxfId="27"/>
+    <tableColumn id="20" name="Ename" dataDxfId="26"/>
+    <tableColumn id="21" name="Remark" dataDxfId="25"/>
+    <tableColumn id="3" name="Star" dataDxfId="24"/>
+    <tableColumn id="4" name="Type" dataDxfId="23"/>
+    <tableColumn id="5" name="Attr" dataDxfId="22"/>
+    <tableColumn id="8" name="Quality" dataDxfId="21">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="40"/>
-    <tableColumn id="9" name="Damage" dataDxfId="39"/>
-    <tableColumn id="10" name="Cure" dataDxfId="38"/>
-    <tableColumn id="11" name="Time" dataDxfId="37"/>
-    <tableColumn id="13" name="Help" dataDxfId="36"/>
-    <tableColumn id="16" name="Rate" dataDxfId="35"/>
-    <tableColumn id="18" name="Atk" dataDxfId="34"/>
-    <tableColumn id="12" name="Modify" dataDxfId="33"/>
-    <tableColumn id="27" name="Sum" dataDxfId="32">
+    <tableColumn id="7" name="Cost" dataDxfId="20"/>
+    <tableColumn id="9" name="Damage" dataDxfId="19"/>
+    <tableColumn id="10" name="Cure" dataDxfId="18"/>
+    <tableColumn id="11" name="Time" dataDxfId="17"/>
+    <tableColumn id="13" name="Help" dataDxfId="16"/>
+    <tableColumn id="16" name="Rate" dataDxfId="15"/>
+    <tableColumn id="18" name="Atk" dataDxfId="14"/>
+    <tableColumn id="12" name="Modify" dataDxfId="13"/>
+    <tableColumn id="27" name="Sum" dataDxfId="12">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="31"/>
-    <tableColumn id="15" name="Target" dataDxfId="30"/>
-    <tableColumn id="25" name="Mark" dataDxfId="29"/>
-    <tableColumn id="22" name="Effect" dataDxfId="28"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="27"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="26"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="25"/>
-    <tableColumn id="26" name="JobId" dataDxfId="24"/>
-    <tableColumn id="19" name="Icon" dataDxfId="23"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="22"/>
-    <tableColumn id="29" name="IsHeroCard" dataDxfId="19"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="21"/>
+    <tableColumn id="6" name="Range" dataDxfId="11"/>
+    <tableColumn id="15" name="Target" dataDxfId="10"/>
+    <tableColumn id="25" name="Mark" dataDxfId="9"/>
+    <tableColumn id="22" name="Effect" dataDxfId="8"/>
+    <tableColumn id="24" name="GetDescript" dataDxfId="7"/>
+    <tableColumn id="17" name="UnitEffect" dataDxfId="6"/>
+    <tableColumn id="28" name="AreaEffect" dataDxfId="5"/>
+    <tableColumn id="26" name="JobId" dataDxfId="4"/>
+    <tableColumn id="19" name="Icon" dataDxfId="3"/>
+    <tableColumn id="14" name="IsSpecial" dataDxfId="2"/>
+    <tableColumn id="29" name="IsHeroCard" dataDxfId="1"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9027,10 +9029,10 @@
   <dimension ref="A1:AC143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="J88" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Y4" sqref="Y4"/>
+      <selection pane="bottomRight" activeCell="U93" sqref="U93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9138,7 +9140,7 @@
         <v>352</v>
       </c>
       <c r="AB1" s="23" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="AC1" s="23" t="s">
         <v>355</v>
@@ -9316,10 +9318,10 @@
         <v>353</v>
       </c>
       <c r="AB3" s="43" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="AC3" s="43" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="60" x14ac:dyDescent="0.15">
@@ -9647,7 +9649,7 @@
         <v>100</v>
       </c>
       <c r="U7" s="11" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="V7" s="7" t="s">
         <v>698</v>
@@ -9736,7 +9738,7 @@
         <v>100</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="V8" s="7" t="s">
         <v>341</v>
@@ -10523,10 +10525,10 @@
         <v>100</v>
       </c>
       <c r="U17" s="11" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="V17" s="7" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="W17" s="1" t="s">
         <v>448</v>
@@ -10701,7 +10703,7 @@
         <v>75</v>
       </c>
       <c r="U19" s="11" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="V19" s="7" t="s">
         <v>330</v>
@@ -10879,7 +10881,7 @@
         <v>102</v>
       </c>
       <c r="U21" s="11" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="V21" s="7" t="s">
         <v>527</v>
@@ -10968,7 +10970,7 @@
         <v>100</v>
       </c>
       <c r="U22" s="11" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="V22" s="7" t="s">
         <v>476</v>
@@ -11059,7 +11061,7 @@
         <v>100</v>
       </c>
       <c r="U23" s="11" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="V23" s="7" t="s">
         <v>474</v>
@@ -11150,7 +11152,7 @@
         <v>100</v>
       </c>
       <c r="U24" s="11" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="V24" s="7" t="s">
         <v>477</v>
@@ -11330,7 +11332,7 @@
         <v>100</v>
       </c>
       <c r="U26" s="11" t="s">
-        <v>798</v>
+        <v>934</v>
       </c>
       <c r="V26" s="21" t="s">
         <v>382</v>
@@ -11417,7 +11419,7 @@
         <v>90</v>
       </c>
       <c r="U27" s="11" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="V27" s="7" t="s">
         <v>383</v>
@@ -11506,7 +11508,7 @@
         <v>100</v>
       </c>
       <c r="U28" s="11" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="V28" s="7" t="s">
         <v>470</v>
@@ -11595,7 +11597,7 @@
         <v>100</v>
       </c>
       <c r="U29" s="11" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="V29" s="7" t="s">
         <v>469</v>
@@ -11684,7 +11686,7 @@
         <v>96</v>
       </c>
       <c r="U30" s="11" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="V30" s="7" t="s">
         <v>760</v>
@@ -11771,7 +11773,7 @@
         <v>96</v>
       </c>
       <c r="U31" s="11" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="V31" s="7" t="s">
         <v>761</v>
@@ -11945,7 +11947,7 @@
         <v>100</v>
       </c>
       <c r="U33" s="11" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="V33" s="1" t="s">
         <v>733</v>
@@ -12034,7 +12036,7 @@
         <v>100</v>
       </c>
       <c r="U34" s="11" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="V34" s="1" t="s">
         <v>735</v>
@@ -12123,7 +12125,7 @@
         <v>100</v>
       </c>
       <c r="U35" s="11" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="V35" s="7" t="s">
         <v>403</v>
@@ -12214,7 +12216,7 @@
         <v>100</v>
       </c>
       <c r="U36" s="11" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="V36" s="7" t="s">
         <v>348</v>
@@ -12305,7 +12307,7 @@
         <v>100</v>
       </c>
       <c r="U37" s="11" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="V37" s="7" t="s">
         <v>351</v>
@@ -12394,7 +12396,7 @@
         <v>100</v>
       </c>
       <c r="U38" s="11" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="V38" s="7" t="s">
         <v>547</v>
@@ -12485,7 +12487,7 @@
         <v>100</v>
       </c>
       <c r="U39" s="11" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="V39" s="1" t="s">
         <v>543</v>
@@ -12574,7 +12576,7 @@
         <v>100</v>
       </c>
       <c r="U40" s="11" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="V40" s="7" t="s">
         <v>471</v>
@@ -12661,7 +12663,7 @@
         <v>100</v>
       </c>
       <c r="U41" s="11" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="V41" s="7" t="s">
         <v>683</v>
@@ -12752,7 +12754,7 @@
         <v>85</v>
       </c>
       <c r="U42" s="11" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="V42" s="1" t="s">
         <v>734</v>
@@ -12841,7 +12843,7 @@
         <v>100</v>
       </c>
       <c r="U43" s="11" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="V43" s="1" t="s">
         <v>736</v>
@@ -12930,7 +12932,7 @@
         <v>100</v>
       </c>
       <c r="U44" s="11" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="V44" s="7" t="s">
         <v>504</v>
@@ -13017,7 +13019,7 @@
         <v>110</v>
       </c>
       <c r="U45" s="11" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="V45" s="7" t="s">
         <v>524</v>
@@ -13108,7 +13110,7 @@
         <v>100</v>
       </c>
       <c r="U46" s="11" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="V46" s="1" t="s">
         <v>486</v>
@@ -13197,7 +13199,7 @@
         <v>95</v>
       </c>
       <c r="U47" s="11" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="V47" s="1" t="s">
         <v>737</v>
@@ -13286,7 +13288,7 @@
         <v>100</v>
       </c>
       <c r="U48" s="11" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="V48" s="1" t="s">
         <v>685</v>
@@ -13375,7 +13377,7 @@
         <v>100</v>
       </c>
       <c r="U49" s="11" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="V49" s="7" t="s">
         <v>520</v>
@@ -13464,7 +13466,7 @@
         <v>100</v>
       </c>
       <c r="U50" s="11" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="V50" s="7" t="s">
         <v>548</v>
@@ -13644,7 +13646,7 @@
         <v>105</v>
       </c>
       <c r="U52" s="11" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="V52" s="7" t="s">
         <v>529</v>
@@ -13735,7 +13737,7 @@
         <v>95</v>
       </c>
       <c r="U53" s="11" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="V53" s="7" t="s">
         <v>519</v>
@@ -13824,7 +13826,7 @@
         <v>100</v>
       </c>
       <c r="U54" s="11" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="V54" s="1" t="s">
         <v>530</v>
@@ -13915,7 +13917,7 @@
         <v>95</v>
       </c>
       <c r="U55" s="11" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="V55" s="7" t="s">
         <v>686</v>
@@ -14004,7 +14006,7 @@
         <v>100</v>
       </c>
       <c r="U56" s="11" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="V56" s="7" t="s">
         <v>534</v>
@@ -14093,7 +14095,7 @@
         <v>100</v>
       </c>
       <c r="U57" s="11" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="V57" s="7" t="s">
         <v>531</v>
@@ -14182,7 +14184,7 @@
         <v>100</v>
       </c>
       <c r="U58" s="11" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="V58" s="1" t="s">
         <v>488</v>
@@ -14265,16 +14267,16 @@
         <v>0</v>
       </c>
       <c r="S59" s="15" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="T59">
         <v>100</v>
       </c>
       <c r="U59" s="11" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="V59" s="1" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="W59" s="1" t="s">
         <v>79</v>
@@ -14360,7 +14362,7 @@
         <v>100</v>
       </c>
       <c r="U60" s="11" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="V60" s="1" t="s">
         <v>484</v>
@@ -14449,7 +14451,7 @@
         <v>100</v>
       </c>
       <c r="U61" s="11" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="V61" s="7" t="s">
         <v>692</v>
@@ -14538,7 +14540,7 @@
         <v>100</v>
       </c>
       <c r="U62" s="11" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="V62" s="7" t="s">
         <v>625</v>
@@ -14627,7 +14629,7 @@
         <v>100</v>
       </c>
       <c r="U63" s="11" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="V63" s="1" t="s">
         <v>384</v>
@@ -14716,7 +14718,7 @@
         <v>100</v>
       </c>
       <c r="U64" s="11" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="V64" s="7" t="s">
         <v>349</v>
@@ -14805,7 +14807,7 @@
         <v>100</v>
       </c>
       <c r="U65" s="11" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="V65" s="7" t="s">
         <v>332</v>
@@ -14894,7 +14896,7 @@
         <v>100</v>
       </c>
       <c r="U66" s="11" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="V66" s="7" t="s">
         <v>490</v>
@@ -14983,7 +14985,7 @@
         <v>100</v>
       </c>
       <c r="U67" s="11" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="V67" s="1" t="s">
         <v>491</v>
@@ -15072,7 +15074,7 @@
         <v>100</v>
       </c>
       <c r="U68" s="11" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="V68" s="1" t="s">
         <v>390</v>
@@ -15161,7 +15163,7 @@
         <v>85</v>
       </c>
       <c r="U69" s="11" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="V69" s="1" t="s">
         <v>738</v>
@@ -15250,7 +15252,7 @@
         <v>100</v>
       </c>
       <c r="U70" s="11" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="V70" s="7" t="s">
         <v>563</v>
@@ -15339,7 +15341,7 @@
         <v>100</v>
       </c>
       <c r="U71" s="11" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="V71" s="7" t="s">
         <v>497</v>
@@ -15430,7 +15432,7 @@
         <v>100</v>
       </c>
       <c r="U72" s="11" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="V72" s="7" t="s">
         <v>624</v>
@@ -15519,7 +15521,7 @@
         <v>100</v>
       </c>
       <c r="U73" s="11" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="V73" s="7" t="s">
         <v>498</v>
@@ -15608,7 +15610,7 @@
         <v>103</v>
       </c>
       <c r="U74" s="11" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="V74" s="7" t="s">
         <v>508</v>
@@ -15699,7 +15701,7 @@
         <v>102</v>
       </c>
       <c r="U75" s="11" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="V75" s="1" t="s">
         <v>507</v>
@@ -15788,7 +15790,7 @@
         <v>100</v>
       </c>
       <c r="U76" s="11" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="V76" s="7" t="s">
         <v>467</v>
@@ -15877,7 +15879,7 @@
         <v>103</v>
       </c>
       <c r="U77" s="11" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="V77" s="7" t="s">
         <v>516</v>
@@ -15966,7 +15968,7 @@
         <v>95</v>
       </c>
       <c r="U78" s="11" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="V78" s="7" t="s">
         <v>333</v>
@@ -16055,7 +16057,7 @@
         <v>100</v>
       </c>
       <c r="U79" s="11" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="V79" s="7" t="s">
         <v>499</v>
@@ -16146,7 +16148,7 @@
         <v>107</v>
       </c>
       <c r="U80" s="11" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="V80" s="7" t="s">
         <v>334</v>
@@ -16235,7 +16237,7 @@
         <v>100</v>
       </c>
       <c r="U81" s="37" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="V81" s="7" t="s">
         <v>629</v>
@@ -16322,7 +16324,7 @@
         <v>100</v>
       </c>
       <c r="U82" s="11" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="V82" s="7" t="s">
         <v>500</v>
@@ -16413,7 +16415,7 @@
         <v>100</v>
       </c>
       <c r="U83" s="11" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="V83" s="7" t="s">
         <v>525</v>
@@ -16504,7 +16506,7 @@
         <v>100</v>
       </c>
       <c r="U84" s="11" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="V84" s="7" t="s">
         <v>526</v>
@@ -16595,7 +16597,7 @@
         <v>100</v>
       </c>
       <c r="U85" s="11" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="V85" s="7" t="s">
         <v>623</v>
@@ -16628,7 +16630,7 @@
         <v>160</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="D86" s="25" t="s">
         <v>768</v>
@@ -16684,13 +16686,13 @@
         <v>100</v>
       </c>
       <c r="U86" s="11" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="V86" s="7" t="s">
         <v>502</v>
       </c>
       <c r="W86" s="1" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="X86" s="1"/>
       <c r="Y86" s="1">
@@ -16773,7 +16775,7 @@
         <v>100</v>
       </c>
       <c r="U87" s="11" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="V87" s="7" t="s">
         <v>515</v>
@@ -16864,7 +16866,7 @@
         <v>100</v>
       </c>
       <c r="U88" s="11" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="V88" s="7" t="s">
         <v>777</v>
@@ -16955,7 +16957,7 @@
         <v>102</v>
       </c>
       <c r="U89" s="11" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="V89" s="7" t="s">
         <v>764</v>
@@ -17044,7 +17046,7 @@
         <v>100</v>
       </c>
       <c r="U90" s="11" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="V90" s="7" t="s">
         <v>528</v>
@@ -17135,7 +17137,7 @@
         <v>100</v>
       </c>
       <c r="U91" s="11" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="V91" s="7" t="s">
         <v>335</v>
@@ -17226,7 +17228,7 @@
         <v>100</v>
       </c>
       <c r="U92" s="11" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="V92" s="7" t="s">
         <v>518</v>
@@ -17317,7 +17319,7 @@
         <v>100</v>
       </c>
       <c r="U93" s="11" t="s">
-        <v>830</v>
+        <v>935</v>
       </c>
       <c r="V93" s="1" t="s">
         <v>350</v>
@@ -17406,7 +17408,7 @@
         <v>100</v>
       </c>
       <c r="U94" s="11" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="V94" s="7" t="s">
         <v>336</v>
@@ -17495,7 +17497,7 @@
         <v>100</v>
       </c>
       <c r="U95" s="11" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="V95" s="1" t="s">
         <v>553</v>
@@ -17584,7 +17586,7 @@
         <v>100</v>
       </c>
       <c r="U96" s="11" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="V96" s="7" t="s">
         <v>517</v>
@@ -17673,7 +17675,7 @@
         <v>100</v>
       </c>
       <c r="U97" s="11" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="V97" s="1" t="s">
         <v>492</v>
@@ -17762,7 +17764,7 @@
         <v>100</v>
       </c>
       <c r="U98" s="11" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="V98" s="7" t="s">
         <v>535</v>
@@ -17853,7 +17855,7 @@
         <v>104</v>
       </c>
       <c r="U99" s="11" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="V99" s="1" t="s">
         <v>510</v>
@@ -17942,7 +17944,7 @@
         <v>100</v>
       </c>
       <c r="U100" s="11" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="V100" s="7" t="s">
         <v>512</v>
@@ -18031,7 +18033,7 @@
         <v>100</v>
       </c>
       <c r="U101" s="11" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="V101" s="7" t="s">
         <v>389</v>
@@ -18120,7 +18122,7 @@
         <v>100</v>
       </c>
       <c r="U102" s="11" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="V102" s="7" t="s">
         <v>513</v>
@@ -18209,7 +18211,7 @@
         <v>100</v>
       </c>
       <c r="U103" s="11" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="V103" s="1" t="s">
         <v>630</v>
@@ -18298,7 +18300,7 @@
         <v>100</v>
       </c>
       <c r="U104" s="11" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="V104" s="1" t="s">
         <v>537</v>
@@ -18476,7 +18478,7 @@
         <v>105</v>
       </c>
       <c r="U106" s="11" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="V106" s="7" t="s">
         <v>762</v>
@@ -18567,7 +18569,7 @@
         <v>105</v>
       </c>
       <c r="U107" s="11" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="V107" s="7" t="s">
         <v>763</v>
@@ -18656,7 +18658,7 @@
         <v>100</v>
       </c>
       <c r="U108" s="11" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="V108" s="1" t="s">
         <v>493</v>
@@ -18745,7 +18747,7 @@
         <v>100</v>
       </c>
       <c r="U109" s="11" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="V109" s="7" t="s">
         <v>622</v>
@@ -18834,7 +18836,7 @@
         <v>100</v>
       </c>
       <c r="U110" s="11" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="V110" s="7" t="s">
         <v>621</v>
@@ -18923,7 +18925,7 @@
         <v>100</v>
       </c>
       <c r="U111" s="11" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="V111" s="7" t="s">
         <v>506</v>
@@ -19012,7 +19014,7 @@
         <v>100</v>
       </c>
       <c r="U112" s="11" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="V112" s="7" t="s">
         <v>778</v>
@@ -19101,7 +19103,7 @@
         <v>103</v>
       </c>
       <c r="U113" s="11" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="V113" s="7" t="s">
         <v>601</v>
@@ -19190,7 +19192,7 @@
         <v>100</v>
       </c>
       <c r="U114" s="11" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="V114" s="7" t="s">
         <v>567</v>
@@ -19281,7 +19283,7 @@
         <v>100</v>
       </c>
       <c r="U115" s="11" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="V115" s="7" t="s">
         <v>570</v>
@@ -19370,7 +19372,7 @@
         <v>100</v>
       </c>
       <c r="U116" s="11" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="V116" s="7" t="s">
         <v>603</v>
@@ -19459,7 +19461,7 @@
         <v>101</v>
       </c>
       <c r="U117" s="11" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="V117" s="7" t="s">
         <v>607</v>
@@ -19548,7 +19550,7 @@
         <v>100</v>
       </c>
       <c r="U118" s="11" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="V118" s="7" t="s">
         <v>612</v>
@@ -19639,7 +19641,7 @@
         <v>101</v>
       </c>
       <c r="U119" s="11" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="V119" s="7" t="s">
         <v>655</v>
@@ -19730,7 +19732,7 @@
         <v>100</v>
       </c>
       <c r="U120" s="11" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="V120" s="7" t="s">
         <v>653</v>
@@ -19819,7 +19821,7 @@
         <v>100</v>
       </c>
       <c r="U121" s="11" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="V121" s="7" t="s">
         <v>631</v>
@@ -19908,7 +19910,7 @@
         <v>105</v>
       </c>
       <c r="U122" s="11" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="V122" s="7" t="s">
         <v>636</v>
@@ -19999,7 +20001,7 @@
         <v>100</v>
       </c>
       <c r="U123" s="11" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="V123" s="7" t="s">
         <v>641</v>
@@ -20088,7 +20090,7 @@
         <v>100</v>
       </c>
       <c r="U124" s="11" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="V124" s="1" t="s">
         <v>646</v>
@@ -20179,7 +20181,7 @@
         <v>101</v>
       </c>
       <c r="U125" s="11" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="V125" s="1" t="s">
         <v>660</v>
@@ -20270,7 +20272,7 @@
         <v>100</v>
       </c>
       <c r="U126" s="11" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="V126" s="1" t="s">
         <v>656</v>
@@ -20361,7 +20363,7 @@
         <v>101</v>
       </c>
       <c r="U127" s="11" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="V127" s="1" t="s">
         <v>661</v>
@@ -20452,7 +20454,7 @@
         <v>100</v>
       </c>
       <c r="U128" s="11" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="V128" s="1" t="s">
         <v>693</v>
@@ -20541,7 +20543,7 @@
         <v>100</v>
       </c>
       <c r="U129" s="11" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="V129" s="1" t="s">
         <v>678</v>
@@ -20632,7 +20634,7 @@
         <v>103</v>
       </c>
       <c r="U130" s="11" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="V130" s="1" t="s">
         <v>674</v>
@@ -20723,7 +20725,7 @@
         <v>100</v>
       </c>
       <c r="U131" s="11" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="V131" s="1" t="s">
         <v>679</v>
@@ -20814,7 +20816,7 @@
         <v>103</v>
       </c>
       <c r="U132" s="11" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="V132" s="1" t="s">
         <v>694</v>
@@ -20905,7 +20907,7 @@
         <v>107</v>
       </c>
       <c r="U133" s="11" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="V133" s="1" t="s">
         <v>699</v>
@@ -20996,7 +20998,7 @@
         <v>100</v>
       </c>
       <c r="U134" s="11" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="V134" s="1" t="s">
         <v>707</v>
@@ -21087,7 +21089,7 @@
         <v>102</v>
       </c>
       <c r="U135" s="11" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="V135" s="1" t="s">
         <v>711</v>
@@ -21178,7 +21180,7 @@
         <v>100</v>
       </c>
       <c r="U136" s="11" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="V136" s="1" t="s">
         <v>739</v>
@@ -21267,7 +21269,7 @@
         <v>103</v>
       </c>
       <c r="U137" s="11" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="V137" s="1" t="s">
         <v>740</v>
@@ -21356,7 +21358,7 @@
         <v>108</v>
       </c>
       <c r="U138" s="11" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="V138" s="1" t="s">
         <v>724</v>
@@ -21445,7 +21447,7 @@
         <v>100</v>
       </c>
       <c r="U139" s="11" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="V139" s="1" t="s">
         <v>727</v>
@@ -21534,7 +21536,7 @@
         <v>102</v>
       </c>
       <c r="U140" s="11" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="V140" s="1" t="s">
         <v>731</v>
@@ -21623,7 +21625,7 @@
         <v>105</v>
       </c>
       <c r="U141" s="11" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="V141" s="1" t="s">
         <v>748</v>
@@ -21712,7 +21714,7 @@
         <v>103</v>
       </c>
       <c r="U142" s="11" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="V142" s="1" t="s">
         <v>745</v>
@@ -21801,7 +21803,7 @@
         <v>100</v>
       </c>
       <c r="U143" s="11" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="V143" s="1" t="s">
         <v>749</v>
@@ -21832,26 +21834,26 @@
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I4:I143">
-    <cfRule type="cellIs" dxfId="18" priority="80" operator="notEqual">
+    <cfRule type="cellIs" dxfId="112" priority="80" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:P143">
-    <cfRule type="cellIs" dxfId="17" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="79" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H143">
-    <cfRule type="cellIs" dxfId="16" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="35" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="36" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="37" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="38" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="107" priority="38" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21978,7 +21980,7 @@
         <v>352</v>
       </c>
       <c r="AB1" s="23" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="AC1" s="23" t="s">
         <v>355</v>
@@ -22156,10 +22158,10 @@
         <v>353</v>
       </c>
       <c r="AB3" s="43" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="AC3" s="43" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="24" x14ac:dyDescent="0.15">
@@ -22222,7 +22224,7 @@
         <v>-1</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="V4" s="7" t="s">
         <v>337</v>
@@ -22388,7 +22390,7 @@
         <v>-1</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="V6" s="7" t="s">
         <v>723</v>
@@ -22471,7 +22473,7 @@
         <v>-1</v>
       </c>
       <c r="U7" s="11" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="V7" s="7" t="s">
         <v>717</v>
@@ -22554,7 +22556,7 @@
         <v>-1</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="V8" s="7" t="s">
         <v>369</v>
@@ -22637,7 +22639,7 @@
         <v>-1</v>
       </c>
       <c r="U9" s="11" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="V9" s="7" t="s">
         <v>367</v>
@@ -22720,7 +22722,7 @@
         <v>-1</v>
       </c>
       <c r="U10" s="11" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="V10" s="7" t="s">
         <v>481</v>
@@ -22797,13 +22799,13 @@
         <v>0</v>
       </c>
       <c r="S11" s="15" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="T11" s="1">
         <v>-1</v>
       </c>
       <c r="U11" s="11" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="V11" s="7" t="s">
         <v>522</v>
@@ -22886,7 +22888,7 @@
         <v>-1</v>
       </c>
       <c r="U12" s="11" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="V12" s="7" t="s">
         <v>756</v>
@@ -22969,7 +22971,7 @@
         <v>-1</v>
       </c>
       <c r="U13" s="11" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="V13" s="7" t="s">
         <v>757</v>
@@ -23052,7 +23054,7 @@
         <v>-1</v>
       </c>
       <c r="U14" s="11" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="V14" s="7" t="s">
         <v>755</v>
@@ -23161,28 +23163,28 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I4:I15">
-    <cfRule type="cellIs" dxfId="12" priority="9" operator="notEqual">
+    <cfRule type="cellIs" dxfId="74" priority="9" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="73" priority="7" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:O15">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H15">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="5" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="6" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23310,7 +23312,7 @@
         <v>352</v>
       </c>
       <c r="AB1" s="23" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="AC1" s="23" t="s">
         <v>355</v>
@@ -23488,10 +23490,10 @@
         <v>353</v>
       </c>
       <c r="AB3" s="43" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="AC3" s="43" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="36" x14ac:dyDescent="0.15">
@@ -23558,7 +23560,7 @@
         <v>115</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="V4" s="7" t="s">
         <v>368</v>
@@ -23645,7 +23647,7 @@
         <v>90</v>
       </c>
       <c r="U5" s="11" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="V5" s="7" t="s">
         <v>370</v>
@@ -23732,7 +23734,7 @@
         <v>115</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="V6" s="29" t="s">
         <v>409</v>
@@ -23904,7 +23906,7 @@
         <v>90</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="V8" s="7" t="s">
         <v>379</v>
@@ -23993,7 +23995,7 @@
         <v>400</v>
       </c>
       <c r="U9" s="11" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="V9" s="7" t="s">
         <v>331</v>
@@ -24019,26 +24021,26 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I4:I9">
-    <cfRule type="cellIs" dxfId="6" priority="12" operator="notEqual">
+    <cfRule type="cellIs" dxfId="36" priority="12" operator="notEqual">
       <formula>$E4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:P9">
-    <cfRule type="cellIs" dxfId="5" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H9">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="6" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="7" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="31" priority="8" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
optimise some spell interface
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{207C1C66-2C55-4505-9E75-549B7AAC1B58}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="标准" sheetId="1" r:id="rId1"/>
@@ -23,13 +24,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>real</author>
     <author>Real</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -56,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -83,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -109,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -135,7 +136,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -161,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0">
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -187,7 +188,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U2" authorId="1" shapeId="0">
+    <comment ref="U2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -206,13 +207,13 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>real</author>
     <author>Real</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -239,7 +240,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -266,7 +267,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -292,7 +293,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -318,7 +319,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -344,7 +345,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U2" authorId="1" shapeId="0">
+    <comment ref="U2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -421,13 +422,13 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>real</author>
     <author>Real</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -454,7 +455,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -481,7 +482,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -507,7 +508,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -533,7 +534,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
       <text>
         <r>
           <rPr>
@@ -559,7 +560,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U2" authorId="1" shapeId="0">
+    <comment ref="U2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
       <text>
         <r>
           <rPr>
@@ -636,7 +637,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="936">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="937">
   <si>
     <t>慈悲</t>
   </si>
@@ -3518,18 +3519,9 @@
     <t>p.Action.AddCard(null,t.CardId, t.Level+(int)spl.Help);</t>
   </si>
   <si>
-    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,spl.Target,spl.Shape,spl.Range,mouse))im.OnSpellDamage( spl.Damage,spl.Attr,0.3);</t>
-  </si>
-  <si>
     <t>p.AddMp(spl.Help);r.AddMp(-spl.Help);</t>
   </si>
   <si>
-    <t>m.SetRowUnitPosition(mouse.Y,p.IsLeft,"siden");if(MathTool.GetRandom(100)&lt;spl.Rate) p.Action.AddCard(null,spl.Id, spl.Level);</t>
-  </si>
-  <si>
-    <t>foreach(IMonster im in m.GetAllMonster(mouse).FilterStar(1,5))im.OnSpellDamage( spl.Damage,spl.Attr);</t>
-  </si>
-  <si>
     <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,spl.Target,spl.Shape,spl.Range,mouse))im.OnSpellDamage( spl.Damage,spl.Attr);</t>
   </si>
   <si>
@@ -3756,9 +3748,6 @@
   </si>
   <si>
     <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,spl.Target,spl.Shape,spl.Range,mouse))im.Action.AddBuff(56000003,spl.Level,spl.Time);</t>
-  </si>
-  <si>
-    <t>Sispl.Leveler Light</t>
   </si>
   <si>
     <t>sispl.Levelerlight</t>
@@ -3948,13 +3937,33 @@
   </si>
   <si>
     <t>r.Action.CardLevelUp(-(int)spl.Help,3,false);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Silver Light</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster im in m.GetAllMonster(mouse).FilterStar(1,5))im.OnSpellDamage(spl.Damage,spl.Attr);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,spl.Target,spl.Shape,spl.Range,mouse))im.OnSpellDamage(spl.Damage,spl.Attr);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,spl.Target,spl.Shape,spl.Range,mouse))im.OnSpellDamage( spl.Damage,spl.Attr,0.3);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,spl.Target,spl.Shape,spl.Range,mouse))im.Action.SetToPosition("side",1);if(MathTool.GetRandom(100)&lt;spl.Rate) p.Action.AddCard(null,spl.Id, spl.Level);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -7578,74 +7587,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -8571,135 +8512,135 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AC143" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105" tableBorderDxfId="104">
-  <autoFilter ref="A3:AC143"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:AC143" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105" tableBorderDxfId="104">
+  <autoFilter ref="A3:AC143" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A4:AC113">
     <sortCondition ref="A3:A113"/>
   </sortState>
   <tableColumns count="29">
-    <tableColumn id="1" name="Id" dataDxfId="103"/>
-    <tableColumn id="2" name="Name" dataDxfId="102"/>
-    <tableColumn id="20" name="Ename" dataDxfId="101"/>
-    <tableColumn id="21" name="Remark" dataDxfId="100"/>
-    <tableColumn id="3" name="Star" dataDxfId="99"/>
-    <tableColumn id="4" name="Type" dataDxfId="98"/>
-    <tableColumn id="5" name="Attr" dataDxfId="97"/>
-    <tableColumn id="8" name="Quality" dataDxfId="96">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="103"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="102"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Ename" dataDxfId="101"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Remark" dataDxfId="100"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Star" dataDxfId="99"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Type" dataDxfId="98"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Attr" dataDxfId="97"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Quality" dataDxfId="96">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="95"/>
-    <tableColumn id="9" name="Damage" dataDxfId="94"/>
-    <tableColumn id="10" name="Cure" dataDxfId="93"/>
-    <tableColumn id="11" name="Time" dataDxfId="92"/>
-    <tableColumn id="13" name="Help" dataDxfId="91"/>
-    <tableColumn id="16" name="Rate" dataDxfId="90"/>
-    <tableColumn id="18" name="Atk" dataDxfId="89"/>
-    <tableColumn id="12" name="Modify" dataDxfId="88"/>
-    <tableColumn id="27" name="Sum" dataDxfId="87">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Cost" dataDxfId="95"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Damage" dataDxfId="94"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Cure" dataDxfId="93"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Time" dataDxfId="92"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Help" dataDxfId="91"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Rate" dataDxfId="90"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Atk" dataDxfId="89"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Modify" dataDxfId="88"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Sum" dataDxfId="87">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="86"/>
-    <tableColumn id="15" name="Target" dataDxfId="85"/>
-    <tableColumn id="25" name="Mark" dataDxfId="84"/>
-    <tableColumn id="22" name="Effect" dataDxfId="83"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="82"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="81"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="80"/>
-    <tableColumn id="26" name="JobId" dataDxfId="79"/>
-    <tableColumn id="19" name="Icon" dataDxfId="78"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="77"/>
-    <tableColumn id="29" name="IsHeroCard" dataDxfId="76"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="75"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Range" dataDxfId="86"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Target" dataDxfId="85"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Mark" dataDxfId="84"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Effect" dataDxfId="83"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="GetDescript" dataDxfId="82"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="UnitEffect" dataDxfId="81"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="AreaEffect" dataDxfId="80"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="JobId" dataDxfId="79"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Icon" dataDxfId="78"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="IsSpecial" dataDxfId="77"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="IsHeroCard" dataDxfId="76"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="IsNew" dataDxfId="75"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AC15" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67" tableBorderDxfId="66">
-  <autoFilter ref="A3:AC15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表1_3" displayName="表1_3" ref="A3:AC15" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67" tableBorderDxfId="66">
+  <autoFilter ref="A3:AC15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="29">
-    <tableColumn id="1" name="Id" dataDxfId="65"/>
-    <tableColumn id="2" name="Name" dataDxfId="64"/>
-    <tableColumn id="20" name="Ename" dataDxfId="63"/>
-    <tableColumn id="21" name="Remark" dataDxfId="62"/>
-    <tableColumn id="3" name="Star" dataDxfId="61"/>
-    <tableColumn id="4" name="Type" dataDxfId="60"/>
-    <tableColumn id="5" name="Attr" dataDxfId="59"/>
-    <tableColumn id="8" name="Quality" dataDxfId="58">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id" dataDxfId="65"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="64"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="Ename" dataDxfId="63"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="Remark" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Star" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Type" dataDxfId="60"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Attr" dataDxfId="59"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Quality" dataDxfId="58">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="57"/>
-    <tableColumn id="9" name="Damage" dataDxfId="56"/>
-    <tableColumn id="10" name="Cure" dataDxfId="55"/>
-    <tableColumn id="11" name="Time" dataDxfId="54"/>
-    <tableColumn id="13" name="Help" dataDxfId="53"/>
-    <tableColumn id="16" name="Rate" dataDxfId="52"/>
-    <tableColumn id="18" name="Atk" dataDxfId="51"/>
-    <tableColumn id="12" name="Modify" dataDxfId="50"/>
-    <tableColumn id="27" name="Sum" dataDxfId="49">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Cost" dataDxfId="57"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Damage" dataDxfId="56"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Cure" dataDxfId="55"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Time" dataDxfId="54"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Help" dataDxfId="53"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Rate" dataDxfId="52"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Atk" dataDxfId="51"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Modify" dataDxfId="50"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0100-00001B000000}" name="Sum" dataDxfId="49">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="48"/>
-    <tableColumn id="15" name="Target" dataDxfId="47"/>
-    <tableColumn id="25" name="Mark" dataDxfId="46"/>
-    <tableColumn id="22" name="Effect" dataDxfId="45"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="44"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="43"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="42"/>
-    <tableColumn id="26" name="JobId" dataDxfId="41"/>
-    <tableColumn id="19" name="Icon" dataDxfId="40"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="39"/>
-    <tableColumn id="29" name="IsHeroCard" dataDxfId="38"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Range" dataDxfId="48"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Target" dataDxfId="47"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0100-000019000000}" name="Mark" dataDxfId="46"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="Effect" dataDxfId="45"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0100-000018000000}" name="GetDescript" dataDxfId="44"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="UnitEffect" dataDxfId="43"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0100-00001C000000}" name="AreaEffect" dataDxfId="42"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0100-00001A000000}" name="JobId" dataDxfId="41"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="Icon" dataDxfId="40"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="IsSpecial" dataDxfId="39"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0100-00001D000000}" name="IsHeroCard" dataDxfId="38"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="IsNew" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_35" displayName="表1_35" ref="A3:AC9" totalsRowShown="0" headerRowDxfId="30" tableBorderDxfId="29">
-  <autoFilter ref="A3:AC9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="表1_35" displayName="表1_35" ref="A3:AC9" totalsRowShown="0" headerRowDxfId="30" tableBorderDxfId="29">
+  <autoFilter ref="A3:AC9" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="29">
-    <tableColumn id="1" name="Id" dataDxfId="28"/>
-    <tableColumn id="2" name="Name" dataDxfId="27"/>
-    <tableColumn id="20" name="Ename" dataDxfId="26"/>
-    <tableColumn id="21" name="Remark" dataDxfId="25"/>
-    <tableColumn id="3" name="Star" dataDxfId="24"/>
-    <tableColumn id="4" name="Type" dataDxfId="23"/>
-    <tableColumn id="5" name="Attr" dataDxfId="22"/>
-    <tableColumn id="8" name="Quality" dataDxfId="21">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Id" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="27"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0200-000014000000}" name="Ename" dataDxfId="26"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0200-000015000000}" name="Remark" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Star" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Type" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Attr" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Quality" dataDxfId="21">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="20"/>
-    <tableColumn id="9" name="Damage" dataDxfId="19"/>
-    <tableColumn id="10" name="Cure" dataDxfId="18"/>
-    <tableColumn id="11" name="Time" dataDxfId="17"/>
-    <tableColumn id="13" name="Help" dataDxfId="16"/>
-    <tableColumn id="16" name="Rate" dataDxfId="15"/>
-    <tableColumn id="18" name="Atk" dataDxfId="14"/>
-    <tableColumn id="12" name="Modify" dataDxfId="13"/>
-    <tableColumn id="27" name="Sum" dataDxfId="12">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Cost" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Damage" dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Cure" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Time" dataDxfId="17"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="Help" dataDxfId="16"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="Rate" dataDxfId="15"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0200-000012000000}" name="Atk" dataDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Modify" dataDxfId="13"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0200-00001B000000}" name="Sum" dataDxfId="12">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="11"/>
-    <tableColumn id="15" name="Target" dataDxfId="10"/>
-    <tableColumn id="25" name="Mark" dataDxfId="9"/>
-    <tableColumn id="22" name="Effect" dataDxfId="8"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="7"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="6"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="5"/>
-    <tableColumn id="26" name="JobId" dataDxfId="4"/>
-    <tableColumn id="19" name="Icon" dataDxfId="3"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="2"/>
-    <tableColumn id="29" name="IsHeroCard" dataDxfId="1"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Range" dataDxfId="11"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Target" dataDxfId="10"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0200-000019000000}" name="Mark" dataDxfId="9"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0200-000016000000}" name="Effect" dataDxfId="8"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0200-000018000000}" name="GetDescript" dataDxfId="7"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="UnitEffect" dataDxfId="6"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0200-00001C000000}" name="AreaEffect" dataDxfId="5"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0200-00001A000000}" name="JobId" dataDxfId="4"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0200-000013000000}" name="Icon" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="IsSpecial" dataDxfId="2"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0200-00001D000000}" name="IsHeroCard" dataDxfId="1"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0200-000017000000}" name="IsNew" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8713,7 +8654,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -9025,20 +8966,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="J88" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="U93" sqref="U93"/>
+      <selection pane="bottomRight" activeCell="R48" sqref="R48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.125" customWidth="1"/>
-    <col min="2" max="3" width="7.875" customWidth="1"/>
+    <col min="2" max="2" width="7.875" customWidth="1"/>
+    <col min="3" max="3" width="26.25" customWidth="1"/>
     <col min="4" max="4" width="10.875" customWidth="1"/>
     <col min="5" max="5" width="3.125" customWidth="1"/>
     <col min="6" max="6" width="3.625" customWidth="1"/>
@@ -9140,7 +9082,7 @@
         <v>352</v>
       </c>
       <c r="AB1" s="23" t="s">
-        <v>931</v>
+        <v>927</v>
       </c>
       <c r="AC1" s="23" t="s">
         <v>355</v>
@@ -9318,10 +9260,10 @@
         <v>353</v>
       </c>
       <c r="AB3" s="43" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="AC3" s="43" t="s">
-        <v>933</v>
+        <v>929</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="60" x14ac:dyDescent="0.15">
@@ -9649,7 +9591,7 @@
         <v>100</v>
       </c>
       <c r="U7" s="11" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="V7" s="7" t="s">
         <v>698</v>
@@ -9738,7 +9680,7 @@
         <v>100</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="V8" s="7" t="s">
         <v>341</v>
@@ -10525,10 +10467,10 @@
         <v>100</v>
       </c>
       <c r="U17" s="11" t="s">
-        <v>902</v>
+        <v>898</v>
       </c>
       <c r="V17" s="7" t="s">
-        <v>926</v>
+        <v>922</v>
       </c>
       <c r="W17" s="1" t="s">
         <v>448</v>
@@ -10703,7 +10645,7 @@
         <v>75</v>
       </c>
       <c r="U19" s="11" t="s">
-        <v>868</v>
+        <v>865</v>
       </c>
       <c r="V19" s="7" t="s">
         <v>330</v>
@@ -10881,7 +10823,7 @@
         <v>102</v>
       </c>
       <c r="U21" s="11" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
       <c r="V21" s="7" t="s">
         <v>527</v>
@@ -10970,7 +10912,7 @@
         <v>100</v>
       </c>
       <c r="U22" s="11" t="s">
-        <v>899</v>
+        <v>895</v>
       </c>
       <c r="V22" s="7" t="s">
         <v>476</v>
@@ -11061,7 +11003,7 @@
         <v>100</v>
       </c>
       <c r="U23" s="11" t="s">
-        <v>900</v>
+        <v>896</v>
       </c>
       <c r="V23" s="7" t="s">
         <v>474</v>
@@ -11152,7 +11094,7 @@
         <v>100</v>
       </c>
       <c r="U24" s="11" t="s">
-        <v>901</v>
+        <v>897</v>
       </c>
       <c r="V24" s="7" t="s">
         <v>477</v>
@@ -11332,7 +11274,7 @@
         <v>100</v>
       </c>
       <c r="U26" s="11" t="s">
-        <v>934</v>
+        <v>930</v>
       </c>
       <c r="V26" s="21" t="s">
         <v>382</v>
@@ -11508,7 +11450,7 @@
         <v>100</v>
       </c>
       <c r="U28" s="11" t="s">
-        <v>870</v>
+        <v>867</v>
       </c>
       <c r="V28" s="7" t="s">
         <v>470</v>
@@ -11686,7 +11628,7 @@
         <v>96</v>
       </c>
       <c r="U30" s="11" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
       <c r="V30" s="7" t="s">
         <v>760</v>
@@ -11773,7 +11715,7 @@
         <v>96</v>
       </c>
       <c r="U31" s="11" t="s">
-        <v>910</v>
+        <v>906</v>
       </c>
       <c r="V31" s="7" t="s">
         <v>761</v>
@@ -11947,7 +11889,7 @@
         <v>100</v>
       </c>
       <c r="U33" s="11" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
       <c r="V33" s="1" t="s">
         <v>733</v>
@@ -12036,7 +11978,7 @@
         <v>100</v>
       </c>
       <c r="U34" s="11" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="V34" s="1" t="s">
         <v>735</v>
@@ -12396,7 +12338,7 @@
         <v>100</v>
       </c>
       <c r="U38" s="11" t="s">
-        <v>921</v>
+        <v>917</v>
       </c>
       <c r="V38" s="7" t="s">
         <v>547</v>
@@ -12487,7 +12429,7 @@
         <v>100</v>
       </c>
       <c r="U39" s="11" t="s">
-        <v>927</v>
+        <v>923</v>
       </c>
       <c r="V39" s="1" t="s">
         <v>543</v>
@@ -12576,7 +12518,7 @@
         <v>100</v>
       </c>
       <c r="U40" s="11" t="s">
-        <v>905</v>
+        <v>901</v>
       </c>
       <c r="V40" s="7" t="s">
         <v>471</v>
@@ -12754,7 +12696,7 @@
         <v>85</v>
       </c>
       <c r="U42" s="11" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
       <c r="V42" s="1" t="s">
         <v>734</v>
@@ -12843,7 +12785,7 @@
         <v>100</v>
       </c>
       <c r="U43" s="11" t="s">
-        <v>874</v>
+        <v>871</v>
       </c>
       <c r="V43" s="1" t="s">
         <v>736</v>
@@ -13019,7 +12961,7 @@
         <v>110</v>
       </c>
       <c r="U45" s="11" t="s">
-        <v>805</v>
+        <v>935</v>
       </c>
       <c r="V45" s="7" t="s">
         <v>524</v>
@@ -13110,7 +13052,7 @@
         <v>100</v>
       </c>
       <c r="U46" s="11" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="V46" s="1" t="s">
         <v>486</v>
@@ -13199,7 +13141,7 @@
         <v>95</v>
       </c>
       <c r="U47" s="11" t="s">
-        <v>875</v>
+        <v>872</v>
       </c>
       <c r="V47" s="1" t="s">
         <v>737</v>
@@ -13224,7 +13166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:29" ht="72" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:29" ht="108" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>53000045</v>
       </c>
@@ -13279,7 +13221,7 @@
         <v>0</v>
       </c>
       <c r="R48" s="1">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="S48" s="7" t="s">
         <v>558</v>
@@ -13288,7 +13230,7 @@
         <v>100</v>
       </c>
       <c r="U48" s="11" t="s">
-        <v>807</v>
+        <v>936</v>
       </c>
       <c r="V48" s="1" t="s">
         <v>685</v>
@@ -13377,7 +13319,7 @@
         <v>100</v>
       </c>
       <c r="U49" s="11" t="s">
-        <v>808</v>
+        <v>933</v>
       </c>
       <c r="V49" s="7" t="s">
         <v>520</v>
@@ -13466,7 +13408,7 @@
         <v>100</v>
       </c>
       <c r="U50" s="11" t="s">
-        <v>809</v>
+        <v>934</v>
       </c>
       <c r="V50" s="7" t="s">
         <v>548</v>
@@ -13646,7 +13588,7 @@
         <v>105</v>
       </c>
       <c r="U52" s="11" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="V52" s="7" t="s">
         <v>529</v>
@@ -13737,7 +13679,7 @@
         <v>95</v>
       </c>
       <c r="U53" s="11" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="V53" s="7" t="s">
         <v>519</v>
@@ -13826,7 +13768,7 @@
         <v>100</v>
       </c>
       <c r="U54" s="11" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
       <c r="V54" s="1" t="s">
         <v>530</v>
@@ -13917,7 +13859,7 @@
         <v>95</v>
       </c>
       <c r="U55" s="11" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="V55" s="7" t="s">
         <v>686</v>
@@ -14006,7 +13948,7 @@
         <v>100</v>
       </c>
       <c r="U56" s="11" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="V56" s="7" t="s">
         <v>534</v>
@@ -14095,7 +14037,7 @@
         <v>100</v>
       </c>
       <c r="U57" s="11" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
       <c r="V57" s="7" t="s">
         <v>531</v>
@@ -14184,7 +14126,7 @@
         <v>100</v>
       </c>
       <c r="U58" s="11" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="V58" s="1" t="s">
         <v>488</v>
@@ -14267,16 +14209,16 @@
         <v>0</v>
       </c>
       <c r="S59" s="15" t="s">
-        <v>930</v>
+        <v>926</v>
       </c>
       <c r="T59">
         <v>100</v>
       </c>
       <c r="U59" s="11" t="s">
-        <v>929</v>
+        <v>925</v>
       </c>
       <c r="V59" s="1" t="s">
-        <v>928</v>
+        <v>924</v>
       </c>
       <c r="W59" s="1" t="s">
         <v>79</v>
@@ -14362,7 +14304,7 @@
         <v>100</v>
       </c>
       <c r="U60" s="11" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="V60" s="1" t="s">
         <v>484</v>
@@ -14451,7 +14393,7 @@
         <v>100</v>
       </c>
       <c r="U61" s="11" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="V61" s="7" t="s">
         <v>692</v>
@@ -14540,7 +14482,7 @@
         <v>100</v>
       </c>
       <c r="U62" s="11" t="s">
-        <v>894</v>
+        <v>890</v>
       </c>
       <c r="V62" s="7" t="s">
         <v>625</v>
@@ -14629,7 +14571,7 @@
         <v>100</v>
       </c>
       <c r="U63" s="11" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="V63" s="1" t="s">
         <v>384</v>
@@ -14718,7 +14660,7 @@
         <v>100</v>
       </c>
       <c r="U64" s="11" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
       <c r="V64" s="7" t="s">
         <v>349</v>
@@ -14807,7 +14749,7 @@
         <v>100</v>
       </c>
       <c r="U65" s="11" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
       <c r="V65" s="7" t="s">
         <v>332</v>
@@ -14896,7 +14838,7 @@
         <v>100</v>
       </c>
       <c r="U66" s="11" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="V66" s="7" t="s">
         <v>490</v>
@@ -14985,7 +14927,7 @@
         <v>100</v>
       </c>
       <c r="U67" s="11" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="V67" s="1" t="s">
         <v>491</v>
@@ -15074,7 +15016,7 @@
         <v>100</v>
       </c>
       <c r="U68" s="11" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="V68" s="1" t="s">
         <v>390</v>
@@ -15163,7 +15105,7 @@
         <v>85</v>
       </c>
       <c r="U69" s="11" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
       <c r="V69" s="1" t="s">
         <v>738</v>
@@ -15252,7 +15194,7 @@
         <v>100</v>
       </c>
       <c r="U70" s="11" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="V70" s="7" t="s">
         <v>563</v>
@@ -15341,7 +15283,7 @@
         <v>100</v>
       </c>
       <c r="U71" s="11" t="s">
-        <v>879</v>
+        <v>876</v>
       </c>
       <c r="V71" s="7" t="s">
         <v>497</v>
@@ -15432,7 +15374,7 @@
         <v>100</v>
       </c>
       <c r="U72" s="11" t="s">
-        <v>922</v>
+        <v>918</v>
       </c>
       <c r="V72" s="7" t="s">
         <v>624</v>
@@ -15521,7 +15463,7 @@
         <v>100</v>
       </c>
       <c r="U73" s="11" t="s">
-        <v>923</v>
+        <v>919</v>
       </c>
       <c r="V73" s="7" t="s">
         <v>498</v>
@@ -15610,7 +15552,7 @@
         <v>103</v>
       </c>
       <c r="U74" s="11" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="V74" s="7" t="s">
         <v>508</v>
@@ -15701,7 +15643,7 @@
         <v>102</v>
       </c>
       <c r="U75" s="11" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
       <c r="V75" s="1" t="s">
         <v>507</v>
@@ -15790,7 +15732,7 @@
         <v>100</v>
       </c>
       <c r="U76" s="11" t="s">
-        <v>881</v>
+        <v>878</v>
       </c>
       <c r="V76" s="7" t="s">
         <v>467</v>
@@ -15879,7 +15821,7 @@
         <v>103</v>
       </c>
       <c r="U77" s="11" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
       <c r="V77" s="7" t="s">
         <v>516</v>
@@ -15968,7 +15910,7 @@
         <v>95</v>
       </c>
       <c r="U78" s="11" t="s">
-        <v>915</v>
+        <v>911</v>
       </c>
       <c r="V78" s="7" t="s">
         <v>333</v>
@@ -16057,7 +15999,7 @@
         <v>100</v>
       </c>
       <c r="U79" s="11" t="s">
-        <v>882</v>
+        <v>879</v>
       </c>
       <c r="V79" s="7" t="s">
         <v>499</v>
@@ -16148,7 +16090,7 @@
         <v>107</v>
       </c>
       <c r="U80" s="11" t="s">
-        <v>883</v>
+        <v>880</v>
       </c>
       <c r="V80" s="7" t="s">
         <v>334</v>
@@ -16237,7 +16179,7 @@
         <v>100</v>
       </c>
       <c r="U81" s="37" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="V81" s="7" t="s">
         <v>629</v>
@@ -16324,7 +16266,7 @@
         <v>100</v>
       </c>
       <c r="U82" s="11" t="s">
-        <v>916</v>
+        <v>912</v>
       </c>
       <c r="V82" s="7" t="s">
         <v>500</v>
@@ -16415,7 +16357,7 @@
         <v>100</v>
       </c>
       <c r="U83" s="11" t="s">
-        <v>884</v>
+        <v>881</v>
       </c>
       <c r="V83" s="7" t="s">
         <v>525</v>
@@ -16506,7 +16448,7 @@
         <v>100</v>
       </c>
       <c r="U84" s="11" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="V84" s="7" t="s">
         <v>526</v>
@@ -16597,7 +16539,7 @@
         <v>100</v>
       </c>
       <c r="U85" s="11" t="s">
-        <v>895</v>
+        <v>891</v>
       </c>
       <c r="V85" s="7" t="s">
         <v>623</v>
@@ -16630,7 +16572,7 @@
         <v>160</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>885</v>
+        <v>932</v>
       </c>
       <c r="D86" s="25" t="s">
         <v>768</v>
@@ -16686,13 +16628,13 @@
         <v>100</v>
       </c>
       <c r="U86" s="11" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="V86" s="7" t="s">
         <v>502</v>
       </c>
       <c r="W86" s="1" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
       <c r="X86" s="1"/>
       <c r="Y86" s="1">
@@ -16775,7 +16717,7 @@
         <v>100</v>
       </c>
       <c r="U87" s="11" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
       <c r="V87" s="7" t="s">
         <v>515</v>
@@ -16866,7 +16808,7 @@
         <v>100</v>
       </c>
       <c r="U88" s="11" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
       <c r="V88" s="7" t="s">
         <v>777</v>
@@ -16957,7 +16899,7 @@
         <v>102</v>
       </c>
       <c r="U89" s="11" t="s">
-        <v>911</v>
+        <v>907</v>
       </c>
       <c r="V89" s="7" t="s">
         <v>764</v>
@@ -17046,7 +16988,7 @@
         <v>100</v>
       </c>
       <c r="U90" s="11" t="s">
-        <v>912</v>
+        <v>908</v>
       </c>
       <c r="V90" s="7" t="s">
         <v>528</v>
@@ -17137,7 +17079,7 @@
         <v>100</v>
       </c>
       <c r="U91" s="11" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="V91" s="7" t="s">
         <v>335</v>
@@ -17228,7 +17170,7 @@
         <v>100</v>
       </c>
       <c r="U92" s="11" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="V92" s="7" t="s">
         <v>518</v>
@@ -17319,7 +17261,7 @@
         <v>100</v>
       </c>
       <c r="U93" s="11" t="s">
-        <v>935</v>
+        <v>931</v>
       </c>
       <c r="V93" s="1" t="s">
         <v>350</v>
@@ -17408,7 +17350,7 @@
         <v>100</v>
       </c>
       <c r="U94" s="11" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="V94" s="7" t="s">
         <v>336</v>
@@ -17497,7 +17439,7 @@
         <v>100</v>
       </c>
       <c r="U95" s="11" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="V95" s="1" t="s">
         <v>553</v>
@@ -17586,7 +17528,7 @@
         <v>100</v>
       </c>
       <c r="U96" s="11" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="V96" s="7" t="s">
         <v>517</v>
@@ -17675,7 +17617,7 @@
         <v>100</v>
       </c>
       <c r="U97" s="11" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="V97" s="1" t="s">
         <v>492</v>
@@ -17764,7 +17706,7 @@
         <v>100</v>
       </c>
       <c r="U98" s="11" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="V98" s="7" t="s">
         <v>535</v>
@@ -17855,7 +17797,7 @@
         <v>104</v>
       </c>
       <c r="U99" s="11" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="V99" s="1" t="s">
         <v>510</v>
@@ -17944,7 +17886,7 @@
         <v>100</v>
       </c>
       <c r="U100" s="11" t="s">
-        <v>882</v>
+        <v>879</v>
       </c>
       <c r="V100" s="7" t="s">
         <v>512</v>
@@ -18033,7 +17975,7 @@
         <v>100</v>
       </c>
       <c r="U101" s="11" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="V101" s="7" t="s">
         <v>389</v>
@@ -18122,7 +18064,7 @@
         <v>100</v>
       </c>
       <c r="U102" s="11" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="V102" s="7" t="s">
         <v>513</v>
@@ -18211,7 +18153,7 @@
         <v>100</v>
       </c>
       <c r="U103" s="11" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="V103" s="1" t="s">
         <v>630</v>
@@ -18300,7 +18242,7 @@
         <v>100</v>
       </c>
       <c r="U104" s="11" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
       <c r="V104" s="1" t="s">
         <v>537</v>
@@ -18478,7 +18420,7 @@
         <v>105</v>
       </c>
       <c r="U106" s="11" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
       <c r="V106" s="7" t="s">
         <v>762</v>
@@ -18569,7 +18511,7 @@
         <v>105</v>
       </c>
       <c r="U107" s="11" t="s">
-        <v>914</v>
+        <v>910</v>
       </c>
       <c r="V107" s="7" t="s">
         <v>763</v>
@@ -18658,7 +18600,7 @@
         <v>100</v>
       </c>
       <c r="U108" s="11" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="V108" s="1" t="s">
         <v>493</v>
@@ -18747,7 +18689,7 @@
         <v>100</v>
       </c>
       <c r="U109" s="11" t="s">
-        <v>895</v>
+        <v>891</v>
       </c>
       <c r="V109" s="7" t="s">
         <v>622</v>
@@ -18836,7 +18778,7 @@
         <v>100</v>
       </c>
       <c r="U110" s="11" t="s">
-        <v>896</v>
+        <v>892</v>
       </c>
       <c r="V110" s="7" t="s">
         <v>621</v>
@@ -18925,7 +18867,7 @@
         <v>100</v>
       </c>
       <c r="U111" s="11" t="s">
-        <v>917</v>
+        <v>913</v>
       </c>
       <c r="V111" s="7" t="s">
         <v>506</v>
@@ -19014,7 +18956,7 @@
         <v>100</v>
       </c>
       <c r="U112" s="11" t="s">
-        <v>925</v>
+        <v>921</v>
       </c>
       <c r="V112" s="7" t="s">
         <v>778</v>
@@ -19103,7 +19045,7 @@
         <v>103</v>
       </c>
       <c r="U113" s="11" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="V113" s="7" t="s">
         <v>601</v>
@@ -19192,7 +19134,7 @@
         <v>100</v>
       </c>
       <c r="U114" s="11" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="V114" s="7" t="s">
         <v>567</v>
@@ -19283,7 +19225,7 @@
         <v>100</v>
       </c>
       <c r="U115" s="11" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="V115" s="7" t="s">
         <v>570</v>
@@ -19372,7 +19314,7 @@
         <v>100</v>
       </c>
       <c r="U116" s="11" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="V116" s="7" t="s">
         <v>603</v>
@@ -19461,7 +19403,7 @@
         <v>101</v>
       </c>
       <c r="U117" s="11" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="V117" s="7" t="s">
         <v>607</v>
@@ -19550,7 +19492,7 @@
         <v>100</v>
       </c>
       <c r="U118" s="11" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="V118" s="7" t="s">
         <v>612</v>
@@ -19641,7 +19583,7 @@
         <v>101</v>
       </c>
       <c r="U119" s="11" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="V119" s="7" t="s">
         <v>655</v>
@@ -19732,7 +19674,7 @@
         <v>100</v>
       </c>
       <c r="U120" s="11" t="s">
-        <v>897</v>
+        <v>893</v>
       </c>
       <c r="V120" s="7" t="s">
         <v>653</v>
@@ -19821,7 +19763,7 @@
         <v>100</v>
       </c>
       <c r="U121" s="11" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="V121" s="7" t="s">
         <v>631</v>
@@ -19910,7 +19852,7 @@
         <v>105</v>
       </c>
       <c r="U122" s="11" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="V122" s="7" t="s">
         <v>636</v>
@@ -20001,7 +19943,7 @@
         <v>100</v>
       </c>
       <c r="U123" s="11" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="V123" s="7" t="s">
         <v>641</v>
@@ -20090,7 +20032,7 @@
         <v>100</v>
       </c>
       <c r="U124" s="11" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="V124" s="1" t="s">
         <v>646</v>
@@ -20181,7 +20123,7 @@
         <v>101</v>
       </c>
       <c r="U125" s="11" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="V125" s="1" t="s">
         <v>660</v>
@@ -20272,7 +20214,7 @@
         <v>100</v>
       </c>
       <c r="U126" s="11" t="s">
-        <v>898</v>
+        <v>894</v>
       </c>
       <c r="V126" s="1" t="s">
         <v>656</v>
@@ -20363,7 +20305,7 @@
         <v>101</v>
       </c>
       <c r="U127" s="11" t="s">
-        <v>904</v>
+        <v>900</v>
       </c>
       <c r="V127" s="1" t="s">
         <v>661</v>
@@ -20454,7 +20396,7 @@
         <v>100</v>
       </c>
       <c r="U128" s="11" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
       <c r="V128" s="1" t="s">
         <v>693</v>
@@ -20543,7 +20485,7 @@
         <v>100</v>
       </c>
       <c r="U129" s="11" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
       <c r="V129" s="1" t="s">
         <v>678</v>
@@ -20634,7 +20576,7 @@
         <v>103</v>
       </c>
       <c r="U130" s="11" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="V130" s="1" t="s">
         <v>674</v>
@@ -20725,7 +20667,7 @@
         <v>100</v>
       </c>
       <c r="U131" s="11" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
       <c r="V131" s="1" t="s">
         <v>679</v>
@@ -20816,7 +20758,7 @@
         <v>103</v>
       </c>
       <c r="U132" s="11" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="V132" s="1" t="s">
         <v>694</v>
@@ -20907,7 +20849,7 @@
         <v>107</v>
       </c>
       <c r="U133" s="11" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
       <c r="V133" s="1" t="s">
         <v>699</v>
@@ -20998,7 +20940,7 @@
         <v>100</v>
       </c>
       <c r="U134" s="11" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="V134" s="1" t="s">
         <v>707</v>
@@ -21089,7 +21031,7 @@
         <v>102</v>
       </c>
       <c r="U135" s="11" t="s">
-        <v>903</v>
+        <v>899</v>
       </c>
       <c r="V135" s="1" t="s">
         <v>711</v>
@@ -21180,7 +21122,7 @@
         <v>100</v>
       </c>
       <c r="U136" s="11" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
       <c r="V136" s="1" t="s">
         <v>739</v>
@@ -21269,7 +21211,7 @@
         <v>103</v>
       </c>
       <c r="U137" s="11" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="V137" s="1" t="s">
         <v>740</v>
@@ -21358,7 +21300,7 @@
         <v>108</v>
       </c>
       <c r="U138" s="11" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="V138" s="1" t="s">
         <v>724</v>
@@ -21447,7 +21389,7 @@
         <v>100</v>
       </c>
       <c r="U139" s="11" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
       <c r="V139" s="1" t="s">
         <v>727</v>
@@ -21536,7 +21478,7 @@
         <v>102</v>
       </c>
       <c r="U140" s="11" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
       <c r="V140" s="1" t="s">
         <v>731</v>
@@ -21625,7 +21567,7 @@
         <v>105</v>
       </c>
       <c r="U141" s="11" t="s">
-        <v>918</v>
+        <v>914</v>
       </c>
       <c r="V141" s="1" t="s">
         <v>748</v>
@@ -21714,7 +21656,7 @@
         <v>103</v>
       </c>
       <c r="U142" s="11" t="s">
-        <v>893</v>
+        <v>889</v>
       </c>
       <c r="V142" s="1" t="s">
         <v>745</v>
@@ -21803,7 +21745,7 @@
         <v>100</v>
       </c>
       <c r="U143" s="11" t="s">
-        <v>919</v>
+        <v>915</v>
       </c>
       <c r="V143" s="1" t="s">
         <v>749</v>
@@ -21867,7 +21809,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21980,7 +21922,7 @@
         <v>352</v>
       </c>
       <c r="AB1" s="23" t="s">
-        <v>931</v>
+        <v>927</v>
       </c>
       <c r="AC1" s="23" t="s">
         <v>355</v>
@@ -22158,10 +22100,10 @@
         <v>353</v>
       </c>
       <c r="AB3" s="43" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="AC3" s="43" t="s">
-        <v>933</v>
+        <v>929</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="24" x14ac:dyDescent="0.15">
@@ -22224,7 +22166,7 @@
         <v>-1</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="V4" s="7" t="s">
         <v>337</v>
@@ -22390,7 +22332,7 @@
         <v>-1</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
       <c r="V6" s="7" t="s">
         <v>723</v>
@@ -22473,7 +22415,7 @@
         <v>-1</v>
       </c>
       <c r="U7" s="11" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="V7" s="7" t="s">
         <v>717</v>
@@ -22556,7 +22498,7 @@
         <v>-1</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="V8" s="7" t="s">
         <v>369</v>
@@ -22639,7 +22581,7 @@
         <v>-1</v>
       </c>
       <c r="U9" s="11" t="s">
-        <v>906</v>
+        <v>902</v>
       </c>
       <c r="V9" s="7" t="s">
         <v>367</v>
@@ -22722,7 +22664,7 @@
         <v>-1</v>
       </c>
       <c r="U10" s="11" t="s">
-        <v>907</v>
+        <v>903</v>
       </c>
       <c r="V10" s="7" t="s">
         <v>481</v>
@@ -22799,13 +22741,13 @@
         <v>0</v>
       </c>
       <c r="S11" s="15" t="s">
-        <v>930</v>
+        <v>926</v>
       </c>
       <c r="T11" s="1">
         <v>-1</v>
       </c>
       <c r="U11" s="11" t="s">
-        <v>908</v>
+        <v>904</v>
       </c>
       <c r="V11" s="7" t="s">
         <v>522</v>
@@ -22888,7 +22830,7 @@
         <v>-1</v>
       </c>
       <c r="U12" s="11" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="V12" s="7" t="s">
         <v>756</v>
@@ -22971,7 +22913,7 @@
         <v>-1</v>
       </c>
       <c r="U13" s="11" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="V13" s="7" t="s">
         <v>757</v>
@@ -23054,7 +22996,7 @@
         <v>-1</v>
       </c>
       <c r="U14" s="11" t="s">
-        <v>924</v>
+        <v>920</v>
       </c>
       <c r="V14" s="7" t="s">
         <v>755</v>
@@ -23198,7 +23140,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AC9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23312,7 +23254,7 @@
         <v>352</v>
       </c>
       <c r="AB1" s="23" t="s">
-        <v>931</v>
+        <v>927</v>
       </c>
       <c r="AC1" s="23" t="s">
         <v>355</v>
@@ -23490,10 +23432,10 @@
         <v>353</v>
       </c>
       <c r="AB3" s="43" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="AC3" s="43" t="s">
-        <v>933</v>
+        <v>929</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="36" x14ac:dyDescent="0.15">
@@ -23560,7 +23502,7 @@
         <v>115</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="V4" s="7" t="s">
         <v>368</v>
@@ -23647,7 +23589,7 @@
         <v>90</v>
       </c>
       <c r="U5" s="11" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="V5" s="7" t="s">
         <v>370</v>
@@ -23734,7 +23676,7 @@
         <v>115</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="V6" s="29" t="s">
         <v>409</v>
@@ -23906,7 +23848,7 @@
         <v>90</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
       <c r="V8" s="7" t="s">
         <v>379</v>
@@ -23995,7 +23937,7 @@
         <v>400</v>
       </c>
       <c r="U9" s="11" t="s">
-        <v>920</v>
+        <v>916</v>
       </c>
       <c r="V9" s="7" t="s">
         <v>331</v>
@@ -24054,7 +23996,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -24258,7 +24200,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
balance the spell cards
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{EEF10FDF-B551-48F4-B222-21C2E758BBA2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D995938C-4FD0-4E42-A562-CE9A92041588}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -637,7 +637,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="936">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="937">
   <si>
     <t>慈悲</t>
   </si>
@@ -2297,10 +2297,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>回复召唤师{3:0.0}点LP和MP，并抽一张牌</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>属性</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -2317,18 +2313,10 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>减少双方召唤师{3:0.0}点LP和MP</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>属性</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>属性</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>手牌</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -2401,10 +2389,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>{4:0.0}%几率直接杀死敌方单体</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>对敌方单体造成{0}点魔法伤害，并有{4:0.0}%几率一击必杀</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -2863,10 +2847,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>抽3张卡片,{4:0.0}%几率降低1点MP消耗</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>hit2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -3502,9 +3482,6 @@
     <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,spl.Target,spl.Shape,spl.Range,mouse))im.AddHp(spl.Cure);</t>
   </si>
   <si>
-    <t>p.Action.GetNextNCard(null,1);if(MathTool.GetRandom(100)&lt;spl.Rate) p.Action.AddCard(null,spl.Id, spl.Level);</t>
-  </si>
-  <si>
     <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,spl.Target,spl.Shape,spl.Range,mouse))im.Action.AddPArmor(spl.Cure);</t>
   </si>
   <si>
@@ -3529,9 +3506,6 @@
     <t>t.OnSpellDamage( spl.Damage,spl.Attr,0.15);</t>
   </si>
   <si>
-    <t>p.AddMp(spl.Help);p.AddLp(spl.Help);p.Action.GetNextNCard(null,1);</t>
-  </si>
-  <si>
     <t>p.AddLp(spl.Help);t.Action.SuddenDeath();</t>
   </si>
   <si>
@@ -3553,15 +3527,9 @@
     <t>foreach(IMonster im in m.GetAllMonster(mouse))im.OnSpellDamage( spl.Damage,spl.Attr);</t>
   </si>
   <si>
-    <t>t.OnSpellDamage( spl.Damage,spl.Attr);t.Action.Silent();</t>
-  </si>
-  <si>
     <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,spl.Target,spl.Shape,spl.Range,mouse))if(MathTool.GetRandom(100)&lt;spl.Rate)im.Action.Transform(51000229);</t>
   </si>
   <si>
-    <t>if(MathTool.GetRandom(100)&lt;spl.Rate)t.Action.SuddenDeath();</t>
-  </si>
-  <si>
     <t>p.Action.AddSpike(57000006);if(MathTool.GetRandom(100)&lt;spl.Rate) p.Action.GetNextNCard(null,1);</t>
   </si>
   <si>
@@ -3601,9 +3569,6 @@
     <t>foreach(IMonster im in m.GetAllMonster(mouse))if(im.Owner.IsLeft!=p.IsLeft)im.Action.BreakWeapon();if(MathTool.GetRandom(100)&lt;spl.Rate) p.Action.GetNextNCard(null,1);</t>
   </si>
   <si>
-    <t>p.AddLp(-spl.Help);p.AddMp(-spl.Help);r.AddLp(-spl.Help);r.AddMp(-spl.Help);</t>
-  </si>
-  <si>
     <t>p.Action.CopyRandomNCard(2,spl.Id);if(MathTool.GetRandom(100)&lt;spl.Rate) p.AddMp(4);</t>
   </si>
   <si>
@@ -3619,9 +3584,6 @@
     <t>if(t.HpRate&gt;=100) t.OnSpellDamage( spl.Damage*2,spl.Attr);else t.OnSpellDamage( spl.Damage,spl.Attr);</t>
   </si>
   <si>
-    <t>if(t.Owner.Combo) t.OnSpellDamage( spl.Damage*2,spl.Attr); else t.OnSpellDamage( spl.Damage,spl.Attr);</t>
-  </si>
-  <si>
     <t>if(MathTool.GetRandom(100)&lt;spl.Rate) p.Action.GetNextNCard(null,3);else p.Action.GetNextNCard(null,4);</t>
   </si>
   <si>
@@ -3740,9 +3702,6 @@
   </si>
   <si>
     <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,spl.Target,spl.Shape,spl.Range,mouse))im.Action.AddBuff(56000003,spl.Level,spl.Time);</t>
-  </si>
-  <si>
-    <t>sispl.Levelerlight</t>
   </si>
   <si>
     <t>t.AddHp(spl.Cure);p.Action.ExchangeMonster(t,spl.Level);</t>
@@ -3954,6 +3913,58 @@
   </si>
   <si>
     <t>p.Action.AddRandomMonster(-1,spl.Level,m.GetRandomPoint());</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>silverlight</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>t.OnSpellDamage( spl.Damage,spl.Attr);t.Action.Silent();</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>t.OnSpellDamage( spl.Damage,spl.Attr);if(MathTool.GetRandom(100)&lt;spl.Rate)t.Action.SuddenDeath();</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对敌方单体造成{0}点魔法伤害，{4:0.0}%几率直接将其杀死</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>p.AddLp(spl.Help);p.Action.GetNextNCard(null,1);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>回复召唤师{3:0.0}点LP，并抽一张牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>直接杀死目标,{4:0.0}%几率降低1点MP消耗</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>范围，直伤，状态</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>连击，直伤</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(t.Owner.Combo) t.OnSpellDamage( spl.Damage*2,spl.Attr); else t.OnSpellDamage( spl.Damage,spl.Attr);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>p.Action.GetNextNCard(null,1);if(MathTool.GetRandom(100)&lt;spl.Rate) p.Action.AddCard(null,spl.Id, spl.Level);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>t.OnSpellDamage( spl.Damage,spl.Attr);if(MathTool.GetRandom(100)&lt;spl.Rate) p.Action.AddCard(null,spl.Id, spl.Level);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>对敌方单体造成{0}点魔法伤害，使用后{4:0.0}%返回手牌</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -7745,7 +7756,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1</c:v>
@@ -8967,10 +8978,10 @@
   <dimension ref="A1:AC143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C84" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C104" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I87" sqref="I87"/>
+      <selection pane="bottomRight" activeCell="V108" sqref="V108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9040,7 +9051,7 @@
         <v>344</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="P1" s="17" t="s">
         <v>327</v>
@@ -9079,7 +9090,7 @@
         <v>352</v>
       </c>
       <c r="AB1" s="23" t="s">
-        <v>923</v>
+        <v>911</v>
       </c>
       <c r="AC1" s="23" t="s">
         <v>355</v>
@@ -9129,7 +9140,7 @@
         <v>345</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>328</v>
@@ -9218,7 +9229,7 @@
         <v>346</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="P3" s="20" t="s">
         <v>329</v>
@@ -9239,7 +9250,7 @@
         <v>442</v>
       </c>
       <c r="V3" s="6" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="W3" s="6" t="s">
         <v>317</v>
@@ -9257,10 +9268,10 @@
         <v>353</v>
       </c>
       <c r="AB3" s="43" t="s">
-        <v>924</v>
+        <v>912</v>
       </c>
       <c r="AC3" s="43" t="s">
-        <v>925</v>
+        <v>913</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="60" x14ac:dyDescent="0.15">
@@ -9274,7 +9285,7 @@
         <v>209</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
@@ -9327,10 +9338,10 @@
         <v>95</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>782</v>
+        <v>777</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>724</v>
+        <v>719</v>
       </c>
       <c r="W4" s="1" t="s">
         <v>2</v>
@@ -9361,7 +9372,7 @@
         <v>210</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -9414,7 +9425,7 @@
         <v>80</v>
       </c>
       <c r="U5" s="11" t="s">
-        <v>783</v>
+        <v>778</v>
       </c>
       <c r="V5" s="7" t="s">
         <v>485</v>
@@ -9448,7 +9459,7 @@
         <v>211</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="E6" s="1">
         <v>2</v>
@@ -9501,7 +9512,7 @@
         <v>100</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="V6" s="7" t="s">
         <v>370</v>
@@ -9535,7 +9546,7 @@
         <v>212</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
@@ -9588,10 +9599,10 @@
         <v>100</v>
       </c>
       <c r="U7" s="11" t="s">
-        <v>861</v>
+        <v>850</v>
       </c>
       <c r="V7" s="7" t="s">
-        <v>696</v>
+        <v>691</v>
       </c>
       <c r="W7" s="1" t="s">
         <v>9</v>
@@ -9624,7 +9635,7 @@
         <v>213</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>765</v>
+        <v>760</v>
       </c>
       <c r="E8" s="1">
         <v>3</v>
@@ -9677,7 +9688,7 @@
         <v>100</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>862</v>
+        <v>851</v>
       </c>
       <c r="V8" s="7" t="s">
         <v>341</v>
@@ -9713,7 +9724,7 @@
         <v>290</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
@@ -9766,7 +9777,7 @@
         <v>90</v>
       </c>
       <c r="U9" s="11" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="V9" s="7" t="s">
         <v>451</v>
@@ -9800,7 +9811,7 @@
         <v>291</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -9853,7 +9864,7 @@
         <v>90</v>
       </c>
       <c r="U10" s="11" t="s">
-        <v>786</v>
+        <v>781</v>
       </c>
       <c r="V10" s="7" t="s">
         <v>450</v>
@@ -9887,7 +9898,7 @@
         <v>292</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -9940,7 +9951,7 @@
         <v>90</v>
       </c>
       <c r="U11" s="11" t="s">
-        <v>787</v>
+        <v>782</v>
       </c>
       <c r="V11" s="7" t="s">
         <v>452</v>
@@ -9974,7 +9985,7 @@
         <v>293</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
@@ -10027,7 +10038,7 @@
         <v>90</v>
       </c>
       <c r="U12" s="11" t="s">
-        <v>788</v>
+        <v>783</v>
       </c>
       <c r="V12" s="7" t="s">
         <v>453</v>
@@ -10061,7 +10072,7 @@
         <v>214</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
@@ -10114,7 +10125,7 @@
         <v>90</v>
       </c>
       <c r="U13" s="11" t="s">
-        <v>789</v>
+        <v>784</v>
       </c>
       <c r="V13" s="7" t="s">
         <v>454</v>
@@ -10148,7 +10159,7 @@
         <v>208</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
@@ -10201,7 +10212,7 @@
         <v>90</v>
       </c>
       <c r="U14" s="11" t="s">
-        <v>790</v>
+        <v>785</v>
       </c>
       <c r="V14" s="7" t="s">
         <v>455</v>
@@ -10235,7 +10246,7 @@
         <v>215</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
@@ -10288,7 +10299,7 @@
         <v>90</v>
       </c>
       <c r="U15" s="11" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="V15" s="7" t="s">
         <v>456</v>
@@ -10322,7 +10333,7 @@
         <v>365</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="E16" s="15">
         <v>4</v>
@@ -10375,7 +10386,7 @@
         <v>100</v>
       </c>
       <c r="U16" s="11" t="s">
-        <v>792</v>
+        <v>787</v>
       </c>
       <c r="V16" s="7" t="s">
         <v>468</v>
@@ -10411,7 +10422,7 @@
         <v>446</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="E17" s="1">
         <v>2</v>
@@ -10464,10 +10475,10 @@
         <v>100</v>
       </c>
       <c r="U17" s="11" t="s">
-        <v>895</v>
+        <v>883</v>
       </c>
       <c r="V17" s="7" t="s">
-        <v>919</v>
+        <v>907</v>
       </c>
       <c r="W17" s="1" t="s">
         <v>448</v>
@@ -10500,7 +10511,7 @@
         <v>216</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="E18" s="1">
         <v>1</v>
@@ -10553,10 +10564,10 @@
         <v>75</v>
       </c>
       <c r="U18" s="11" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
       <c r="V18" s="7" t="s">
-        <v>774</v>
+        <v>769</v>
       </c>
       <c r="W18" s="1" t="s">
         <v>15</v>
@@ -10589,7 +10600,7 @@
         <v>217</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="E19" s="1">
         <v>3</v>
@@ -10642,7 +10653,7 @@
         <v>75</v>
       </c>
       <c r="U19" s="11" t="s">
-        <v>863</v>
+        <v>852</v>
       </c>
       <c r="V19" s="7" t="s">
         <v>330</v>
@@ -10678,7 +10689,7 @@
         <v>218</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="E20" s="1">
         <v>7</v>
@@ -10731,13 +10742,13 @@
         <v>100</v>
       </c>
       <c r="U20" s="11" t="s">
-        <v>794</v>
+        <v>789</v>
       </c>
       <c r="V20" s="7" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="X20" s="1"/>
       <c r="Y20" s="1">
@@ -10767,7 +10778,7 @@
         <v>219</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="E21" s="1">
         <v>3</v>
@@ -10820,10 +10831,10 @@
         <v>102</v>
       </c>
       <c r="U21" s="11" t="s">
-        <v>864</v>
+        <v>853</v>
       </c>
       <c r="V21" s="7" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="W21" s="1" t="s">
         <v>21</v>
@@ -10856,7 +10867,7 @@
         <v>220</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="E22" s="1">
         <v>4</v>
@@ -10903,13 +10914,13 @@
         <v>40</v>
       </c>
       <c r="S22" s="7" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="T22">
         <v>100</v>
       </c>
       <c r="U22" s="11" t="s">
-        <v>892</v>
+        <v>880</v>
       </c>
       <c r="V22" s="7" t="s">
         <v>476</v>
@@ -10947,7 +10958,7 @@
         <v>221</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="E23" s="1">
         <v>3</v>
@@ -10994,13 +11005,13 @@
         <v>60</v>
       </c>
       <c r="S23" s="7" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="T23">
         <v>100</v>
       </c>
       <c r="U23" s="11" t="s">
-        <v>893</v>
+        <v>881</v>
       </c>
       <c r="V23" s="7" t="s">
         <v>474</v>
@@ -11038,7 +11049,7 @@
         <v>222</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="E24" s="1">
         <v>3</v>
@@ -11085,13 +11096,13 @@
         <v>90</v>
       </c>
       <c r="S24" s="7" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="T24">
         <v>100</v>
       </c>
       <c r="U24" s="11" t="s">
-        <v>894</v>
+        <v>882</v>
       </c>
       <c r="V24" s="7" t="s">
         <v>477</v>
@@ -11129,7 +11140,7 @@
         <v>223</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="E25" s="1">
         <v>4</v>
@@ -11182,10 +11193,10 @@
         <v>107</v>
       </c>
       <c r="U25" s="11" t="s">
-        <v>795</v>
+        <v>790</v>
       </c>
       <c r="V25" s="7" t="s">
-        <v>666</v>
+        <v>661</v>
       </c>
       <c r="W25" s="1" t="s">
         <v>29</v>
@@ -11271,7 +11282,7 @@
         <v>100</v>
       </c>
       <c r="U26" s="11" t="s">
-        <v>926</v>
+        <v>914</v>
       </c>
       <c r="V26" s="21" t="s">
         <v>382</v>
@@ -11358,7 +11369,7 @@
         <v>90</v>
       </c>
       <c r="U27" s="11" t="s">
-        <v>796</v>
+        <v>791</v>
       </c>
       <c r="V27" s="7" t="s">
         <v>383</v>
@@ -11394,7 +11405,7 @@
         <v>226</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="E28" s="1">
         <v>3</v>
@@ -11447,7 +11458,7 @@
         <v>100</v>
       </c>
       <c r="U28" s="11" t="s">
-        <v>865</v>
+        <v>854</v>
       </c>
       <c r="V28" s="7" t="s">
         <v>470</v>
@@ -11483,7 +11494,7 @@
         <v>227</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="E29" s="1">
         <v>4</v>
@@ -11536,7 +11547,7 @@
         <v>100</v>
       </c>
       <c r="U29" s="11" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
       <c r="V29" s="7" t="s">
         <v>469</v>
@@ -11572,7 +11583,7 @@
         <v>228</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="E30" s="1">
         <v>1</v>
@@ -11625,10 +11636,10 @@
         <v>96</v>
       </c>
       <c r="U30" s="11" t="s">
-        <v>902</v>
+        <v>890</v>
       </c>
       <c r="V30" s="7" t="s">
-        <v>758</v>
+        <v>753</v>
       </c>
       <c r="W30" s="1" t="s">
         <v>39</v>
@@ -11659,7 +11670,7 @@
         <v>229</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
@@ -11712,10 +11723,10 @@
         <v>96</v>
       </c>
       <c r="U31" s="11" t="s">
-        <v>903</v>
+        <v>891</v>
       </c>
       <c r="V31" s="7" t="s">
-        <v>759</v>
+        <v>754</v>
       </c>
       <c r="W31" s="1" t="s">
         <v>41</v>
@@ -11746,7 +11757,7 @@
         <v>230</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="E32" s="1">
         <v>4</v>
@@ -11799,7 +11810,7 @@
         <v>100</v>
       </c>
       <c r="U32" s="11" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="V32" s="21" t="s">
         <v>338</v>
@@ -11886,10 +11897,10 @@
         <v>100</v>
       </c>
       <c r="U33" s="11" t="s">
-        <v>866</v>
+        <v>855</v>
       </c>
       <c r="V33" s="1" t="s">
-        <v>731</v>
+        <v>726</v>
       </c>
       <c r="W33" s="1" t="s">
         <v>4</v>
@@ -11975,10 +11986,10 @@
         <v>100</v>
       </c>
       <c r="U34" s="11" t="s">
-        <v>867</v>
+        <v>856</v>
       </c>
       <c r="V34" s="1" t="s">
-        <v>733</v>
+        <v>728</v>
       </c>
       <c r="W34" s="1" t="s">
         <v>4</v>
@@ -12011,7 +12022,7 @@
         <v>294</v>
       </c>
       <c r="D35" s="25" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="E35" s="1">
         <v>3</v>
@@ -12064,7 +12075,7 @@
         <v>100</v>
       </c>
       <c r="U35" s="11" t="s">
-        <v>798</v>
+        <v>793</v>
       </c>
       <c r="V35" s="7" t="s">
         <v>403</v>
@@ -12102,7 +12113,7 @@
         <v>295</v>
       </c>
       <c r="D36" s="25" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="E36" s="1">
         <v>4</v>
@@ -12155,7 +12166,7 @@
         <v>100</v>
       </c>
       <c r="U36" s="11" t="s">
-        <v>799</v>
+        <v>794</v>
       </c>
       <c r="V36" s="7" t="s">
         <v>348</v>
@@ -12246,7 +12257,7 @@
         <v>100</v>
       </c>
       <c r="U37" s="11" t="s">
-        <v>800</v>
+        <v>934</v>
       </c>
       <c r="V37" s="7" t="s">
         <v>351</v>
@@ -12282,7 +12293,7 @@
         <v>231</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="E38" s="1">
         <v>3</v>
@@ -12329,16 +12340,16 @@
         <v>15</v>
       </c>
       <c r="S38" s="1" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="T38">
         <v>100</v>
       </c>
       <c r="U38" s="11" t="s">
-        <v>914</v>
+        <v>902</v>
       </c>
       <c r="V38" s="7" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="W38" s="1" t="s">
         <v>49</v>
@@ -12373,7 +12384,7 @@
         <v>232</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="E39" s="1">
         <v>3</v>
@@ -12420,16 +12431,16 @@
         <v>12</v>
       </c>
       <c r="S39" s="1" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="T39">
         <v>100</v>
       </c>
       <c r="U39" s="11" t="s">
-        <v>935</v>
+        <v>923</v>
       </c>
       <c r="V39" s="1" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="W39" s="1" t="s">
         <v>51</v>
@@ -12462,7 +12473,7 @@
         <v>233</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="E40" s="1">
         <v>1</v>
@@ -12515,7 +12526,7 @@
         <v>100</v>
       </c>
       <c r="U40" s="11" t="s">
-        <v>898</v>
+        <v>886</v>
       </c>
       <c r="V40" s="7" t="s">
         <v>471</v>
@@ -12549,7 +12560,7 @@
         <v>234</v>
       </c>
       <c r="D41" s="25" t="s">
-        <v>767</v>
+        <v>762</v>
       </c>
       <c r="E41" s="1">
         <v>2</v>
@@ -12596,16 +12607,16 @@
         <v>12</v>
       </c>
       <c r="S41" s="1" t="s">
-        <v>680</v>
+        <v>675</v>
       </c>
       <c r="T41">
         <v>100</v>
       </c>
       <c r="U41" s="11" t="s">
-        <v>801</v>
+        <v>795</v>
       </c>
       <c r="V41" s="7" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
       <c r="W41" s="1" t="s">
         <v>55</v>
@@ -12693,10 +12704,10 @@
         <v>85</v>
       </c>
       <c r="U42" s="11" t="s">
-        <v>868</v>
+        <v>857</v>
       </c>
       <c r="V42" s="1" t="s">
-        <v>732</v>
+        <v>727</v>
       </c>
       <c r="W42" s="1" t="s">
         <v>4</v>
@@ -12782,10 +12793,10 @@
         <v>100</v>
       </c>
       <c r="U43" s="11" t="s">
-        <v>869</v>
+        <v>858</v>
       </c>
       <c r="V43" s="1" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
       <c r="W43" s="1" t="s">
         <v>4</v>
@@ -12815,10 +12826,10 @@
         <v>56</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>780</v>
+        <v>775</v>
       </c>
       <c r="D44" s="25" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="E44" s="1">
         <v>2</v>
@@ -12871,10 +12882,10 @@
         <v>100</v>
       </c>
       <c r="U44" s="11" t="s">
-        <v>802</v>
+        <v>796</v>
       </c>
       <c r="V44" s="7" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="W44" s="1" t="s">
         <v>57</v>
@@ -12894,7 +12905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:29" ht="72" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:29" ht="60" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>53000042</v>
       </c>
@@ -12905,7 +12916,7 @@
         <v>236</v>
       </c>
       <c r="D45" s="25" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="E45" s="1">
         <v>3</v>
@@ -12958,10 +12969,10 @@
         <v>110</v>
       </c>
       <c r="U45" s="11" t="s">
-        <v>931</v>
+        <v>919</v>
       </c>
       <c r="V45" s="7" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="W45" s="1" t="s">
         <v>59</v>
@@ -13049,7 +13060,7 @@
         <v>100</v>
       </c>
       <c r="U46" s="11" t="s">
-        <v>803</v>
+        <v>797</v>
       </c>
       <c r="V46" s="1" t="s">
         <v>486</v>
@@ -13138,10 +13149,10 @@
         <v>95</v>
       </c>
       <c r="U47" s="11" t="s">
-        <v>870</v>
+        <v>859</v>
       </c>
       <c r="V47" s="1" t="s">
-        <v>735</v>
+        <v>730</v>
       </c>
       <c r="W47" s="1" t="s">
         <v>4</v>
@@ -13163,7 +13174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:29" ht="108" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:29" ht="96" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>53000045</v>
       </c>
@@ -13221,16 +13232,16 @@
         <v>100</v>
       </c>
       <c r="S48" s="7" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="T48">
         <v>100</v>
       </c>
       <c r="U48" s="11" t="s">
-        <v>932</v>
+        <v>920</v>
       </c>
       <c r="V48" s="1" t="s">
-        <v>683</v>
+        <v>678</v>
       </c>
       <c r="W48" s="1" t="s">
         <v>318</v>
@@ -13263,7 +13274,7 @@
         <v>240</v>
       </c>
       <c r="D49" s="25" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="E49" s="1">
         <v>5</v>
@@ -13316,10 +13327,10 @@
         <v>100</v>
       </c>
       <c r="U49" s="11" t="s">
-        <v>929</v>
+        <v>917</v>
       </c>
       <c r="V49" s="7" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="W49" s="1" t="s">
         <v>63</v>
@@ -13352,7 +13363,7 @@
         <v>241</v>
       </c>
       <c r="D50" s="25" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="E50" s="1">
         <v>5</v>
@@ -13405,10 +13416,10 @@
         <v>100</v>
       </c>
       <c r="U50" s="11" t="s">
-        <v>930</v>
+        <v>918</v>
       </c>
       <c r="V50" s="7" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="W50" s="1" t="s">
         <v>65</v>
@@ -13443,7 +13454,7 @@
         <v>242</v>
       </c>
       <c r="D51" s="25" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="E51" s="1">
         <v>5</v>
@@ -13490,16 +13501,16 @@
         <v>0</v>
       </c>
       <c r="S51" s="1" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="T51">
         <v>100</v>
       </c>
       <c r="U51" s="11" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="V51" s="1" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="W51" s="1" t="s">
         <v>21</v>
@@ -13532,7 +13543,7 @@
         <v>243</v>
       </c>
       <c r="D52" s="25" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="E52" s="1">
         <v>3</v>
@@ -13585,10 +13596,10 @@
         <v>105</v>
       </c>
       <c r="U52" s="11" t="s">
-        <v>805</v>
+        <v>799</v>
       </c>
       <c r="V52" s="7" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="W52" s="1" t="s">
         <v>68</v>
@@ -13623,7 +13634,7 @@
         <v>244</v>
       </c>
       <c r="D53" s="25" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="E53" s="1">
         <v>4</v>
@@ -13676,10 +13687,10 @@
         <v>95</v>
       </c>
       <c r="U53" s="11" t="s">
-        <v>806</v>
+        <v>800</v>
       </c>
       <c r="V53" s="7" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="W53" s="1" t="s">
         <v>70</v>
@@ -13712,7 +13723,7 @@
         <v>245</v>
       </c>
       <c r="D54" s="25" t="s">
-        <v>768</v>
+        <v>763</v>
       </c>
       <c r="E54" s="1">
         <v>3</v>
@@ -13765,10 +13776,10 @@
         <v>100</v>
       </c>
       <c r="U54" s="11" t="s">
-        <v>871</v>
+        <v>860</v>
       </c>
       <c r="V54" s="1" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="W54" s="1" t="s">
         <v>72</v>
@@ -13797,13 +13808,13 @@
         <v>53000052</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="D55" s="25" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="E55" s="1">
         <v>1</v>
@@ -13850,19 +13861,19 @@
         <v>0</v>
       </c>
       <c r="S55" s="1" t="s">
-        <v>682</v>
+        <v>677</v>
       </c>
       <c r="T55">
         <v>95</v>
       </c>
       <c r="U55" s="11" t="s">
-        <v>807</v>
+        <v>801</v>
       </c>
       <c r="V55" s="7" t="s">
-        <v>684</v>
+        <v>679</v>
       </c>
       <c r="W55" s="1" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="X55" s="1"/>
       <c r="Y55" s="1">
@@ -13892,7 +13903,7 @@
         <v>246</v>
       </c>
       <c r="D56" s="25" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="E56" s="1">
         <v>3</v>
@@ -13939,16 +13950,16 @@
         <v>20</v>
       </c>
       <c r="S56" s="1" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="T56">
         <v>100</v>
       </c>
       <c r="U56" s="11" t="s">
-        <v>804</v>
+        <v>798</v>
       </c>
       <c r="V56" s="7" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="W56" s="1" t="s">
         <v>74</v>
@@ -13981,7 +13992,7 @@
         <v>195</v>
       </c>
       <c r="D57" s="25" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="E57" s="1">
         <v>3</v>
@@ -14034,10 +14045,10 @@
         <v>100</v>
       </c>
       <c r="U57" s="11" t="s">
-        <v>808</v>
+        <v>802</v>
       </c>
       <c r="V57" s="7" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="W57" s="1" t="s">
         <v>76</v>
@@ -14059,7 +14070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:29" ht="36" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:29" ht="24" x14ac:dyDescent="0.15">
       <c r="A58">
         <v>53000055</v>
       </c>
@@ -14070,7 +14081,7 @@
         <v>247</v>
       </c>
       <c r="D58" s="25" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="E58" s="1">
         <v>4</v>
@@ -14123,10 +14134,10 @@
         <v>100</v>
       </c>
       <c r="U58" s="11" t="s">
-        <v>809</v>
+        <v>928</v>
       </c>
       <c r="V58" s="1" t="s">
-        <v>488</v>
+        <v>929</v>
       </c>
       <c r="W58" s="1" t="s">
         <v>2</v>
@@ -14159,7 +14170,7 @@
         <v>248</v>
       </c>
       <c r="D59" s="25" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="E59" s="1">
         <v>2</v>
@@ -14206,16 +14217,16 @@
         <v>0</v>
       </c>
       <c r="S59" s="15" t="s">
-        <v>922</v>
+        <v>910</v>
       </c>
       <c r="T59">
         <v>100</v>
       </c>
       <c r="U59" s="11" t="s">
-        <v>921</v>
+        <v>909</v>
       </c>
       <c r="V59" s="1" t="s">
-        <v>920</v>
+        <v>908</v>
       </c>
       <c r="W59" s="1" t="s">
         <v>79</v>
@@ -14301,7 +14312,7 @@
         <v>100</v>
       </c>
       <c r="U60" s="11" t="s">
-        <v>810</v>
+        <v>803</v>
       </c>
       <c r="V60" s="1" t="s">
         <v>484</v>
@@ -14331,10 +14342,10 @@
         <v>53000058</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="D61" s="25" t="s">
         <v>400</v>
@@ -14384,16 +14395,16 @@
         <v>0</v>
       </c>
       <c r="S61" s="1" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="T61">
         <v>100</v>
       </c>
       <c r="U61" s="11" t="s">
-        <v>811</v>
+        <v>804</v>
       </c>
       <c r="V61" s="7" t="s">
-        <v>690</v>
+        <v>685</v>
       </c>
       <c r="W61" s="1" t="s">
         <v>15</v>
@@ -14426,7 +14437,7 @@
         <v>249</v>
       </c>
       <c r="D62" s="25" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="E62" s="1">
         <v>2</v>
@@ -14479,10 +14490,10 @@
         <v>100</v>
       </c>
       <c r="U62" s="11" t="s">
-        <v>887</v>
+        <v>875</v>
       </c>
       <c r="V62" s="7" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="W62" s="1" t="s">
         <v>83</v>
@@ -14515,7 +14526,7 @@
         <v>250</v>
       </c>
       <c r="D63" s="25" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="E63" s="1">
         <v>1</v>
@@ -14568,7 +14579,7 @@
         <v>100</v>
       </c>
       <c r="U63" s="11" t="s">
-        <v>812</v>
+        <v>805</v>
       </c>
       <c r="V63" s="1" t="s">
         <v>384</v>
@@ -14604,7 +14615,7 @@
         <v>251</v>
       </c>
       <c r="D64" s="25" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="E64" s="1">
         <v>4</v>
@@ -14657,7 +14668,7 @@
         <v>100</v>
       </c>
       <c r="U64" s="11" t="s">
-        <v>813</v>
+        <v>806</v>
       </c>
       <c r="V64" s="7" t="s">
         <v>349</v>
@@ -14693,7 +14704,7 @@
         <v>252</v>
       </c>
       <c r="D65" s="25" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="E65" s="1">
         <v>1</v>
@@ -14746,7 +14757,7 @@
         <v>100</v>
       </c>
       <c r="U65" s="11" t="s">
-        <v>872</v>
+        <v>861</v>
       </c>
       <c r="V65" s="7" t="s">
         <v>332</v>
@@ -14782,10 +14793,10 @@
         <v>253</v>
       </c>
       <c r="D66" s="25" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E66" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F66">
         <v>202</v>
@@ -14798,7 +14809,7 @@
         <v>1</v>
       </c>
       <c r="I66" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J66" s="1">
         <v>0</v>
@@ -14835,10 +14846,10 @@
         <v>100</v>
       </c>
       <c r="U66" s="11" t="s">
-        <v>814</v>
+        <v>807</v>
       </c>
       <c r="V66" s="7" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="W66" s="1" t="s">
         <v>90</v>
@@ -14924,10 +14935,10 @@
         <v>100</v>
       </c>
       <c r="U67" s="11" t="s">
-        <v>815</v>
+        <v>808</v>
       </c>
       <c r="V67" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="W67" s="1" t="s">
         <v>92</v>
@@ -14960,7 +14971,7 @@
         <v>197</v>
       </c>
       <c r="D68" s="25" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="E68" s="1">
         <v>6</v>
@@ -15013,7 +15024,7 @@
         <v>100</v>
       </c>
       <c r="U68" s="11" t="s">
-        <v>816</v>
+        <v>809</v>
       </c>
       <c r="V68" s="1" t="s">
         <v>390</v>
@@ -15102,10 +15113,10 @@
         <v>85</v>
       </c>
       <c r="U69" s="11" t="s">
-        <v>873</v>
+        <v>862</v>
       </c>
       <c r="V69" s="1" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
       <c r="W69" s="1" t="s">
         <v>4</v>
@@ -15138,7 +15149,7 @@
         <v>256</v>
       </c>
       <c r="D70" s="25" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="E70" s="1">
         <v>3</v>
@@ -15191,10 +15202,10 @@
         <v>100</v>
       </c>
       <c r="U70" s="11" t="s">
-        <v>817</v>
+        <v>925</v>
       </c>
       <c r="V70" s="7" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="W70" s="1" t="s">
         <v>95</v>
@@ -15227,7 +15238,7 @@
         <v>257</v>
       </c>
       <c r="D71" s="25" t="s">
-        <v>768</v>
+        <v>931</v>
       </c>
       <c r="E71" s="1">
         <v>2</v>
@@ -15280,10 +15291,10 @@
         <v>100</v>
       </c>
       <c r="U71" s="11" t="s">
-        <v>874</v>
+        <v>863</v>
       </c>
       <c r="V71" s="7" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="W71" s="1" t="s">
         <v>97</v>
@@ -15318,7 +15329,7 @@
         <v>200</v>
       </c>
       <c r="D72" s="25" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="E72" s="1">
         <v>2</v>
@@ -15371,13 +15382,13 @@
         <v>100</v>
       </c>
       <c r="U72" s="11" t="s">
-        <v>915</v>
+        <v>903</v>
       </c>
       <c r="V72" s="7" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="W72" s="1" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="X72" s="1"/>
       <c r="Y72" s="1">
@@ -15407,7 +15418,7 @@
         <v>202</v>
       </c>
       <c r="D73" s="25" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="E73" s="1">
         <v>2</v>
@@ -15460,10 +15471,10 @@
         <v>100</v>
       </c>
       <c r="U73" s="11" t="s">
-        <v>916</v>
+        <v>904</v>
       </c>
       <c r="V73" s="7" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="W73" s="1" t="s">
         <v>101</v>
@@ -15496,7 +15507,7 @@
         <v>199</v>
       </c>
       <c r="D74" s="25" t="s">
-        <v>769</v>
+        <v>764</v>
       </c>
       <c r="E74" s="1">
         <v>4</v>
@@ -15549,10 +15560,10 @@
         <v>103</v>
       </c>
       <c r="U74" s="11" t="s">
-        <v>818</v>
+        <v>810</v>
       </c>
       <c r="V74" s="7" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="W74" s="1" t="s">
         <v>103</v>
@@ -15587,7 +15598,7 @@
         <v>258</v>
       </c>
       <c r="D75" s="25" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="E75" s="1">
         <v>3</v>
@@ -15640,10 +15651,10 @@
         <v>102</v>
       </c>
       <c r="U75" s="11" t="s">
-        <v>875</v>
+        <v>864</v>
       </c>
       <c r="V75" s="1" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="W75" s="1" t="s">
         <v>105</v>
@@ -15676,7 +15687,7 @@
         <v>259</v>
       </c>
       <c r="D76" s="25" t="s">
-        <v>769</v>
+        <v>764</v>
       </c>
       <c r="E76" s="1">
         <v>3</v>
@@ -15729,7 +15740,7 @@
         <v>100</v>
       </c>
       <c r="U76" s="11" t="s">
-        <v>876</v>
+        <v>865</v>
       </c>
       <c r="V76" s="7" t="s">
         <v>467</v>
@@ -15754,7 +15765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:29" ht="36" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:29" ht="48" x14ac:dyDescent="0.15">
       <c r="A77">
         <v>53000074</v>
       </c>
@@ -15765,7 +15776,7 @@
         <v>296</v>
       </c>
       <c r="D77" s="25" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="E77" s="1">
         <v>3</v>
@@ -15784,7 +15795,7 @@
         <v>3</v>
       </c>
       <c r="J77" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="K77" s="1">
         <v>0</v>
@@ -15818,10 +15829,10 @@
         <v>103</v>
       </c>
       <c r="U77" s="11" t="s">
-        <v>819</v>
+        <v>926</v>
       </c>
       <c r="V77" s="7" t="s">
-        <v>514</v>
+        <v>927</v>
       </c>
       <c r="W77" s="1" t="s">
         <v>109</v>
@@ -15854,7 +15865,7 @@
         <v>260</v>
       </c>
       <c r="D78" s="25" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="E78" s="1">
         <v>4</v>
@@ -15907,7 +15918,7 @@
         <v>95</v>
       </c>
       <c r="U78" s="11" t="s">
-        <v>908</v>
+        <v>896</v>
       </c>
       <c r="V78" s="7" t="s">
         <v>333</v>
@@ -15943,7 +15954,7 @@
         <v>261</v>
       </c>
       <c r="D79" s="25" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="E79" s="1">
         <v>3</v>
@@ -15996,10 +16007,10 @@
         <v>100</v>
       </c>
       <c r="U79" s="11" t="s">
-        <v>877</v>
+        <v>866</v>
       </c>
       <c r="V79" s="7" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="W79" s="1" t="s">
         <v>113</v>
@@ -16034,7 +16045,7 @@
         <v>262</v>
       </c>
       <c r="D80" s="25" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="E80" s="1">
         <v>3</v>
@@ -16087,7 +16098,7 @@
         <v>107</v>
       </c>
       <c r="U80" s="11" t="s">
-        <v>878</v>
+        <v>867</v>
       </c>
       <c r="V80" s="7" t="s">
         <v>334</v>
@@ -16123,7 +16134,7 @@
         <v>263</v>
       </c>
       <c r="D81" s="25" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="E81" s="1">
         <v>1</v>
@@ -16176,10 +16187,10 @@
         <v>100</v>
       </c>
       <c r="U81" s="37" t="s">
-        <v>820</v>
+        <v>811</v>
       </c>
       <c r="V81" s="7" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="W81" s="1" t="s">
         <v>93</v>
@@ -16210,7 +16221,7 @@
         <v>264</v>
       </c>
       <c r="D82" s="25" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="E82" s="1">
         <v>3</v>
@@ -16263,10 +16274,10 @@
         <v>100</v>
       </c>
       <c r="U82" s="11" t="s">
-        <v>909</v>
+        <v>897</v>
       </c>
       <c r="V82" s="7" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="W82" s="1" t="s">
         <v>117</v>
@@ -16301,7 +16312,7 @@
         <v>265</v>
       </c>
       <c r="D83" s="25" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="E83" s="1">
         <v>2</v>
@@ -16348,16 +16359,16 @@
         <v>30</v>
       </c>
       <c r="S83" s="7" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="T83">
         <v>100</v>
       </c>
       <c r="U83" s="11" t="s">
-        <v>879</v>
+        <v>868</v>
       </c>
       <c r="V83" s="7" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="W83" s="1" t="s">
         <v>81</v>
@@ -16392,7 +16403,7 @@
         <v>266</v>
       </c>
       <c r="D84" s="25" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="E84" s="1">
         <v>2</v>
@@ -16439,16 +16450,16 @@
         <v>30</v>
       </c>
       <c r="S84" s="7" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="T84">
         <v>100</v>
       </c>
       <c r="U84" s="11" t="s">
-        <v>821</v>
+        <v>812</v>
       </c>
       <c r="V84" s="7" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="W84" s="1" t="s">
         <v>51</v>
@@ -16483,7 +16494,7 @@
         <v>267</v>
       </c>
       <c r="D85" s="25" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="E85" s="1">
         <v>3</v>
@@ -16536,10 +16547,10 @@
         <v>100</v>
       </c>
       <c r="U85" s="11" t="s">
-        <v>888</v>
+        <v>876</v>
       </c>
       <c r="V85" s="7" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="W85" s="1" t="s">
         <v>122</v>
@@ -16569,10 +16580,10 @@
         <v>160</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>928</v>
+        <v>916</v>
       </c>
       <c r="D86" s="25" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="E86" s="1">
         <v>3</v>
@@ -16625,13 +16636,13 @@
         <v>100</v>
       </c>
       <c r="U86" s="11" t="s">
-        <v>822</v>
+        <v>813</v>
       </c>
       <c r="V86" s="7" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="W86" s="1" t="s">
-        <v>880</v>
+        <v>924</v>
       </c>
       <c r="X86" s="1"/>
       <c r="Y86" s="1">
@@ -16661,7 +16672,7 @@
         <v>201</v>
       </c>
       <c r="D87" s="25" t="s">
-        <v>590</v>
+        <v>538</v>
       </c>
       <c r="E87" s="1">
         <v>6</v>
@@ -16714,16 +16725,16 @@
         <v>100</v>
       </c>
       <c r="U87" s="11" t="s">
-        <v>933</v>
+        <v>921</v>
       </c>
       <c r="V87" s="7" t="s">
-        <v>934</v>
+        <v>922</v>
       </c>
       <c r="W87" s="1" t="s">
-        <v>779</v>
+        <v>774</v>
       </c>
       <c r="X87" s="1" t="s">
-        <v>779</v>
+        <v>774</v>
       </c>
       <c r="Y87" s="1">
         <v>11000008</v>
@@ -16752,7 +16763,7 @@
         <v>203</v>
       </c>
       <c r="D88" s="25" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="E88" s="1">
         <v>3</v>
@@ -16799,22 +16810,22 @@
         <v>20</v>
       </c>
       <c r="S88" s="1" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="T88">
         <v>100</v>
       </c>
       <c r="U88" s="11" t="s">
-        <v>823</v>
+        <v>814</v>
       </c>
       <c r="V88" s="7" t="s">
-        <v>775</v>
+        <v>770</v>
       </c>
       <c r="W88" s="1" t="s">
-        <v>779</v>
+        <v>774</v>
       </c>
       <c r="X88" s="1" t="s">
-        <v>779</v>
+        <v>774</v>
       </c>
       <c r="Y88" s="1">
         <v>11000009</v>
@@ -16843,7 +16854,7 @@
         <v>204</v>
       </c>
       <c r="D89" s="25" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="E89" s="1">
         <v>2</v>
@@ -16896,10 +16907,10 @@
         <v>102</v>
       </c>
       <c r="U89" s="11" t="s">
-        <v>904</v>
+        <v>892</v>
       </c>
       <c r="V89" s="7" t="s">
-        <v>762</v>
+        <v>757</v>
       </c>
       <c r="W89" s="1" t="s">
         <v>2</v>
@@ -16932,7 +16943,7 @@
         <v>205</v>
       </c>
       <c r="D90" s="25" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="E90" s="1">
         <v>3</v>
@@ -16979,16 +16990,16 @@
         <v>40</v>
       </c>
       <c r="S90" s="7" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="T90">
         <v>100</v>
       </c>
       <c r="U90" s="11" t="s">
-        <v>905</v>
+        <v>893</v>
       </c>
       <c r="V90" s="7" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="W90" s="1" t="s">
         <v>59</v>
@@ -17023,7 +17034,7 @@
         <v>268</v>
       </c>
       <c r="D91" s="25" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="E91" s="1">
         <v>3</v>
@@ -17076,7 +17087,7 @@
         <v>100</v>
       </c>
       <c r="U91" s="11" t="s">
-        <v>804</v>
+        <v>798</v>
       </c>
       <c r="V91" s="7" t="s">
         <v>335</v>
@@ -17114,7 +17125,7 @@
         <v>269</v>
       </c>
       <c r="D92" s="25" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="E92" s="1">
         <v>4</v>
@@ -17167,10 +17178,10 @@
         <v>100</v>
       </c>
       <c r="U92" s="11" t="s">
-        <v>804</v>
+        <v>798</v>
       </c>
       <c r="V92" s="7" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="W92" s="1" t="s">
         <v>441</v>
@@ -17205,7 +17216,7 @@
         <v>286</v>
       </c>
       <c r="D93" s="25" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="E93" s="1">
         <v>2</v>
@@ -17258,7 +17269,7 @@
         <v>100</v>
       </c>
       <c r="U93" s="11" t="s">
-        <v>927</v>
+        <v>915</v>
       </c>
       <c r="V93" s="1" t="s">
         <v>350</v>
@@ -17294,7 +17305,7 @@
         <v>270</v>
       </c>
       <c r="D94" s="25" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="E94" s="1">
         <v>2</v>
@@ -17347,7 +17358,7 @@
         <v>100</v>
       </c>
       <c r="U94" s="11" t="s">
-        <v>824</v>
+        <v>815</v>
       </c>
       <c r="V94" s="7" t="s">
         <v>336</v>
@@ -17377,16 +17388,16 @@
         <v>53000092</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="D95" s="25" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="E95" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F95">
         <v>201</v>
@@ -17396,53 +17407,53 @@
       </c>
       <c r="H95" s="1">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I95" s="1">
+        <v>5</v>
+      </c>
+      <c r="J95" s="1">
+        <v>0</v>
+      </c>
+      <c r="K95" s="1">
+        <v>0</v>
+      </c>
+      <c r="L95" s="1">
+        <v>0</v>
+      </c>
+      <c r="M95" s="1">
+        <v>2</v>
+      </c>
+      <c r="N95" s="1">
+        <v>0</v>
+      </c>
+      <c r="O95" s="1">
+        <v>0</v>
+      </c>
+      <c r="P95" s="1">
         <v>3</v>
-      </c>
-      <c r="J95" s="1">
-        <v>0</v>
-      </c>
-      <c r="K95" s="1">
-        <v>0</v>
-      </c>
-      <c r="L95" s="1">
-        <v>0</v>
-      </c>
-      <c r="M95" s="1">
-        <v>1</v>
-      </c>
-      <c r="N95" s="1">
-        <v>0</v>
-      </c>
-      <c r="O95" s="1">
-        <v>0</v>
-      </c>
-      <c r="P95" s="1">
-        <v>0</v>
       </c>
       <c r="Q95" s="36">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R95" s="1">
         <v>0</v>
       </c>
       <c r="S95" s="7" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="T95">
         <v>100</v>
       </c>
       <c r="U95" s="11" t="s">
-        <v>825</v>
+        <v>816</v>
       </c>
       <c r="V95" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="W95" s="1" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="X95" s="1"/>
       <c r="Y95" s="1">
@@ -17472,7 +17483,7 @@
         <v>271</v>
       </c>
       <c r="D96" s="25" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="E96" s="1">
         <v>2</v>
@@ -17525,10 +17536,10 @@
         <v>100</v>
       </c>
       <c r="U96" s="11" t="s">
-        <v>826</v>
+        <v>817</v>
       </c>
       <c r="V96" s="7" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="W96" s="1" t="s">
         <v>133</v>
@@ -17561,7 +17572,7 @@
         <v>272</v>
       </c>
       <c r="D97" s="25" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="E97" s="1">
         <v>2</v>
@@ -17614,10 +17625,10 @@
         <v>100</v>
       </c>
       <c r="U97" s="11" t="s">
-        <v>827</v>
+        <v>818</v>
       </c>
       <c r="V97" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="W97" s="1" t="s">
         <v>136</v>
@@ -17650,7 +17661,7 @@
         <v>273</v>
       </c>
       <c r="D98" s="25" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="E98" s="1">
         <v>2</v>
@@ -17703,10 +17714,10 @@
         <v>100</v>
       </c>
       <c r="U98" s="11" t="s">
-        <v>828</v>
+        <v>819</v>
       </c>
       <c r="V98" s="7" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="W98" s="1" t="s">
         <v>138</v>
@@ -17741,10 +17752,10 @@
         <v>274</v>
       </c>
       <c r="D99" s="25" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="E99" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F99">
         <v>202</v>
@@ -17757,19 +17768,19 @@
         <v>2</v>
       </c>
       <c r="I99" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J99" s="1">
         <v>0</v>
       </c>
       <c r="K99" s="1">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="L99" s="1">
         <v>0</v>
       </c>
       <c r="M99" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N99" s="1">
         <v>0</v>
@@ -17788,16 +17799,16 @@
         <v>200</v>
       </c>
       <c r="S99" s="1" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="T99">
         <v>104</v>
       </c>
       <c r="U99" s="11" t="s">
-        <v>829</v>
+        <v>820</v>
       </c>
       <c r="V99" s="1" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="W99" s="1" t="s">
         <v>29</v>
@@ -17830,7 +17841,7 @@
         <v>275</v>
       </c>
       <c r="D100" s="25" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="E100" s="1">
         <v>2</v>
@@ -17883,10 +17894,10 @@
         <v>100</v>
       </c>
       <c r="U100" s="11" t="s">
-        <v>877</v>
+        <v>866</v>
       </c>
       <c r="V100" s="7" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="W100" s="1" t="s">
         <v>81</v>
@@ -17919,7 +17930,7 @@
         <v>287</v>
       </c>
       <c r="D101" s="25" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="E101" s="1">
         <v>1</v>
@@ -17972,7 +17983,7 @@
         <v>100</v>
       </c>
       <c r="U101" s="11" t="s">
-        <v>830</v>
+        <v>821</v>
       </c>
       <c r="V101" s="7" t="s">
         <v>389</v>
@@ -18008,10 +18019,10 @@
         <v>276</v>
       </c>
       <c r="D102" s="25" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="E102" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F102">
         <v>200</v>
@@ -18024,7 +18035,7 @@
         <v>1</v>
       </c>
       <c r="I102" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J102" s="1">
         <v>50</v>
@@ -18061,10 +18072,10 @@
         <v>100</v>
       </c>
       <c r="U102" s="11" t="s">
-        <v>831</v>
+        <v>822</v>
       </c>
       <c r="V102" s="7" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="W102" s="1" t="s">
         <v>97</v>
@@ -18097,7 +18108,7 @@
         <v>277</v>
       </c>
       <c r="D103" s="25" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="E103" s="1">
         <v>4</v>
@@ -18144,16 +18155,16 @@
         <v>0</v>
       </c>
       <c r="S103" s="1" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="T103">
         <v>100</v>
       </c>
       <c r="U103" s="11" t="s">
-        <v>832</v>
+        <v>823</v>
       </c>
       <c r="V103" s="1" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="W103" s="1" t="s">
         <v>143</v>
@@ -18186,7 +18197,7 @@
         <v>288</v>
       </c>
       <c r="D104" s="25" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="E104" s="1">
         <v>3</v>
@@ -18233,16 +18244,16 @@
         <v>0</v>
       </c>
       <c r="S104" s="1" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="T104">
         <v>100</v>
       </c>
       <c r="U104" s="11" t="s">
-        <v>881</v>
+        <v>869</v>
       </c>
       <c r="V104" s="1" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="W104" s="1" t="s">
         <v>166</v>
@@ -18275,7 +18286,7 @@
         <v>278</v>
       </c>
       <c r="D105" s="25" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="E105" s="1">
         <v>1</v>
@@ -18328,7 +18339,7 @@
         <v>100</v>
       </c>
       <c r="U105" s="11" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
       <c r="V105" s="7" t="s">
         <v>337</v>
@@ -18364,7 +18375,7 @@
         <v>279</v>
       </c>
       <c r="D106" s="25" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="E106" s="1">
         <v>3</v>
@@ -18417,10 +18428,10 @@
         <v>105</v>
       </c>
       <c r="U106" s="11" t="s">
-        <v>906</v>
+        <v>894</v>
       </c>
       <c r="V106" s="7" t="s">
-        <v>760</v>
+        <v>755</v>
       </c>
       <c r="W106" s="1" t="s">
         <v>146</v>
@@ -18455,7 +18466,7 @@
         <v>280</v>
       </c>
       <c r="D107" s="25" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="E107" s="1">
         <v>3</v>
@@ -18508,10 +18519,10 @@
         <v>105</v>
       </c>
       <c r="U107" s="11" t="s">
-        <v>907</v>
+        <v>895</v>
       </c>
       <c r="V107" s="7" t="s">
-        <v>761</v>
+        <v>756</v>
       </c>
       <c r="W107" s="1" t="s">
         <v>148</v>
@@ -18533,7 +18544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:29" ht="60" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:29" ht="72" x14ac:dyDescent="0.15">
       <c r="A108">
         <v>53000105</v>
       </c>
@@ -18544,13 +18555,13 @@
         <v>207</v>
       </c>
       <c r="D108" s="25" t="s">
-        <v>495</v>
+        <v>578</v>
       </c>
       <c r="E108" s="1">
         <v>3</v>
       </c>
       <c r="F108">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G108" s="1">
         <v>0</v>
@@ -18563,7 +18574,7 @@
         <v>3</v>
       </c>
       <c r="J108" s="1">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="K108" s="1">
         <v>0</v>
@@ -18571,11 +18582,9 @@
       <c r="L108" s="1">
         <v>0</v>
       </c>
-      <c r="M108" s="1">
-        <v>4</v>
-      </c>
+      <c r="M108" s="1"/>
       <c r="N108" s="1">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="O108" s="1">
         <v>0</v>
@@ -18588,19 +18597,19 @@
         <v>2</v>
       </c>
       <c r="R108" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="S108" s="1" t="s">
-        <v>135</v>
+        <v>366</v>
       </c>
       <c r="T108">
         <v>100</v>
       </c>
       <c r="U108" s="11" t="s">
-        <v>833</v>
+        <v>935</v>
       </c>
       <c r="V108" s="1" t="s">
-        <v>493</v>
+        <v>936</v>
       </c>
       <c r="W108" s="1" t="s">
         <v>150</v>
@@ -18633,7 +18642,7 @@
         <v>281</v>
       </c>
       <c r="D109" s="25" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="E109" s="1">
         <v>1</v>
@@ -18686,10 +18695,10 @@
         <v>100</v>
       </c>
       <c r="U109" s="11" t="s">
-        <v>888</v>
+        <v>876</v>
       </c>
       <c r="V109" s="7" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="W109" s="1" t="s">
         <v>152</v>
@@ -18722,7 +18731,7 @@
         <v>282</v>
       </c>
       <c r="D110" s="25" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="E110" s="1">
         <v>1</v>
@@ -18775,10 +18784,10 @@
         <v>100</v>
       </c>
       <c r="U110" s="11" t="s">
-        <v>889</v>
+        <v>877</v>
       </c>
       <c r="V110" s="7" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="W110" s="1" t="s">
         <v>154</v>
@@ -18811,7 +18820,7 @@
         <v>283</v>
       </c>
       <c r="D111" s="25" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="E111" s="1">
         <v>2</v>
@@ -18864,10 +18873,10 @@
         <v>100</v>
       </c>
       <c r="U111" s="11" t="s">
-        <v>910</v>
+        <v>898</v>
       </c>
       <c r="V111" s="7" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="W111" s="1" t="s">
         <v>156</v>
@@ -18900,7 +18909,7 @@
         <v>284</v>
       </c>
       <c r="D112" s="25" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="E112" s="1">
         <v>2</v>
@@ -18953,10 +18962,10 @@
         <v>100</v>
       </c>
       <c r="U112" s="11" t="s">
-        <v>918</v>
+        <v>906</v>
       </c>
       <c r="V112" s="7" t="s">
-        <v>776</v>
+        <v>771</v>
       </c>
       <c r="W112" s="1" t="s">
         <v>158</v>
@@ -18989,7 +18998,7 @@
         <v>285</v>
       </c>
       <c r="D113" s="25" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="E113" s="1">
         <v>3</v>
@@ -19042,10 +19051,10 @@
         <v>103</v>
       </c>
       <c r="U113" s="11" t="s">
-        <v>834</v>
+        <v>824</v>
       </c>
       <c r="V113" s="7" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="W113" s="1" t="s">
         <v>29</v>
@@ -19072,13 +19081,13 @@
         <v>53000111</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="D114" s="25" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="E114" s="1">
         <v>3</v>
@@ -19125,22 +19134,22 @@
         <v>20</v>
       </c>
       <c r="S114" s="1" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="T114">
         <v>100</v>
       </c>
       <c r="U114" s="11" t="s">
-        <v>835</v>
+        <v>825</v>
       </c>
       <c r="V114" s="7" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="W114" s="1" t="s">
-        <v>778</v>
+        <v>773</v>
       </c>
       <c r="X114" s="1" t="s">
-        <v>777</v>
+        <v>772</v>
       </c>
       <c r="Y114" s="1">
         <v>11000007</v>
@@ -19163,13 +19172,13 @@
         <v>53000112</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>781</v>
+        <v>776</v>
       </c>
       <c r="D115" s="25" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="E115" s="1">
         <v>3</v>
@@ -19216,22 +19225,22 @@
         <v>100</v>
       </c>
       <c r="S115" s="1" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="T115">
         <v>100</v>
       </c>
       <c r="U115" s="11" t="s">
-        <v>836</v>
+        <v>826</v>
       </c>
       <c r="V115" s="7" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="W115" s="1" t="s">
-        <v>779</v>
+        <v>774</v>
       </c>
       <c r="X115" s="1" t="s">
-        <v>779</v>
+        <v>774</v>
       </c>
       <c r="Y115" s="1">
         <v>11000009</v>
@@ -19254,10 +19263,10 @@
         <v>53000113</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="D116" s="25"/>
       <c r="E116" s="1">
@@ -19305,22 +19314,22 @@
         <v>0</v>
       </c>
       <c r="S116" s="1" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="T116">
         <v>100</v>
       </c>
       <c r="U116" s="11" t="s">
-        <v>837</v>
+        <v>827</v>
       </c>
       <c r="V116" s="7" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="W116" s="1" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="X116" s="1" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="Y116" s="1">
         <v>11000003</v>
@@ -19343,10 +19352,10 @@
         <v>53000114</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="D117" s="25"/>
       <c r="E117" s="1">
@@ -19394,16 +19403,16 @@
         <v>0</v>
       </c>
       <c r="S117" s="1" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="T117">
         <v>101</v>
       </c>
       <c r="U117" s="11" t="s">
-        <v>838</v>
+        <v>828</v>
       </c>
       <c r="V117" s="7" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="W117" s="1" t="s">
         <v>99</v>
@@ -19432,10 +19441,10 @@
         <v>53000115</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="D118" s="25"/>
       <c r="E118" s="1">
@@ -19483,16 +19492,16 @@
         <v>0</v>
       </c>
       <c r="S118" s="1" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="T118">
         <v>100</v>
       </c>
       <c r="U118" s="11" t="s">
-        <v>831</v>
+        <v>822</v>
       </c>
       <c r="V118" s="7" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="W118" s="1" t="s">
         <v>99</v>
@@ -19521,13 +19530,13 @@
         <v>53000116</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="D119" s="25" t="s">
-        <v>609</v>
+        <v>932</v>
       </c>
       <c r="E119" s="1">
         <v>2</v>
@@ -19580,10 +19589,10 @@
         <v>101</v>
       </c>
       <c r="U119" s="11" t="s">
-        <v>839</v>
+        <v>933</v>
       </c>
       <c r="V119" s="7" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="W119" s="1" t="s">
         <v>99</v>
@@ -19612,13 +19621,13 @@
         <v>53000117</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="D120" s="25" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="E120" s="1">
         <v>1</v>
@@ -19665,16 +19674,16 @@
         <v>0</v>
       </c>
       <c r="S120" s="1" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="T120">
         <v>100</v>
       </c>
       <c r="U120" s="11" t="s">
-        <v>890</v>
+        <v>878</v>
       </c>
       <c r="V120" s="7" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="W120" s="1" t="s">
         <v>99</v>
@@ -19703,10 +19712,10 @@
         <v>53000118</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="D121" s="25"/>
       <c r="E121" s="1">
@@ -19754,22 +19763,22 @@
         <v>0</v>
       </c>
       <c r="S121" s="1" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="T121">
         <v>100</v>
       </c>
       <c r="U121" s="11" t="s">
-        <v>840</v>
+        <v>829</v>
       </c>
       <c r="V121" s="7" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="W121" s="1" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="X121" s="1" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="Y121" s="1">
         <v>11000003</v>
@@ -19792,10 +19801,10 @@
         <v>53000119</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="D122" s="25"/>
       <c r="E122" s="1">
@@ -19843,22 +19852,22 @@
         <v>0</v>
       </c>
       <c r="S122" s="1" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="T122">
         <v>105</v>
       </c>
       <c r="U122" s="11" t="s">
-        <v>841</v>
+        <v>830</v>
       </c>
       <c r="V122" s="7" t="s">
-        <v>634</v>
+        <v>930</v>
       </c>
       <c r="W122" s="1" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="X122" s="1" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="Y122" s="1">
         <v>11000003</v>
@@ -19881,13 +19890,13 @@
         <v>53000120</v>
       </c>
       <c r="B123" s="22" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="C123" s="15" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="D123" s="25" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="E123" s="15">
         <v>1</v>
@@ -19940,10 +19949,10 @@
         <v>100</v>
       </c>
       <c r="U123" s="11" t="s">
-        <v>842</v>
+        <v>831</v>
       </c>
       <c r="V123" s="7" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="W123" s="15" t="s">
         <v>57</v>
@@ -19970,13 +19979,13 @@
         <v>53000121</v>
       </c>
       <c r="B124" s="22" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="C124" s="15" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
       <c r="D124" s="25" t="s">
-        <v>771</v>
+        <v>766</v>
       </c>
       <c r="E124" s="15">
         <v>1</v>
@@ -20023,22 +20032,22 @@
         <v>30</v>
       </c>
       <c r="S124" s="7" t="s">
-        <v>643</v>
+        <v>638</v>
       </c>
       <c r="T124">
         <v>100</v>
       </c>
       <c r="U124" s="11" t="s">
-        <v>843</v>
+        <v>832</v>
       </c>
       <c r="V124" s="1" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="W124" s="15" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="X124" s="15" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="Y124" s="1">
         <v>11000001</v>
@@ -20061,13 +20070,13 @@
         <v>53000122</v>
       </c>
       <c r="B125" s="22" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="C125" s="15" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="D125" s="25" t="s">
-        <v>770</v>
+        <v>765</v>
       </c>
       <c r="E125" s="15">
         <v>1</v>
@@ -20114,22 +20123,22 @@
         <v>0</v>
       </c>
       <c r="S125" s="7" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
       <c r="T125">
         <v>101</v>
       </c>
       <c r="U125" s="11" t="s">
-        <v>844</v>
+        <v>833</v>
       </c>
       <c r="V125" s="1" t="s">
-        <v>658</v>
+        <v>653</v>
       </c>
       <c r="W125" s="15" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="X125" s="15" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="Y125" s="1">
         <v>11000001</v>
@@ -20152,13 +20161,13 @@
         <v>53000123</v>
       </c>
       <c r="B126" s="22" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C126" s="15" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
       <c r="D126" s="25" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="E126" s="15">
         <v>1</v>
@@ -20205,22 +20214,22 @@
         <v>0</v>
       </c>
       <c r="S126" s="7" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
       <c r="T126">
         <v>100</v>
       </c>
       <c r="U126" s="11" t="s">
-        <v>891</v>
+        <v>879</v>
       </c>
       <c r="V126" s="1" t="s">
-        <v>654</v>
+        <v>649</v>
       </c>
       <c r="W126" s="15" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="X126" s="15" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="Y126" s="1">
         <v>11000001</v>
@@ -20243,13 +20252,13 @@
         <v>53000124</v>
       </c>
       <c r="B127" s="22" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
       <c r="C127" s="15" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
       <c r="D127" s="25" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="E127" s="15">
         <v>2</v>
@@ -20296,22 +20305,22 @@
         <v>0</v>
       </c>
       <c r="S127" s="7" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="T127">
         <v>101</v>
       </c>
       <c r="U127" s="11" t="s">
-        <v>897</v>
+        <v>885</v>
       </c>
       <c r="V127" s="1" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
       <c r="W127" s="15" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="X127" s="15" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="Y127" s="1">
         <v>11000001</v>
@@ -20334,13 +20343,13 @@
         <v>53000125</v>
       </c>
       <c r="B128" s="22" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="C128" s="15" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
       <c r="D128" s="25" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
       <c r="E128" s="15">
         <v>2</v>
@@ -20387,22 +20396,22 @@
         <v>0</v>
       </c>
       <c r="S128" s="7" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
       <c r="T128">
         <v>100</v>
       </c>
       <c r="U128" s="11" t="s">
-        <v>845</v>
+        <v>834</v>
       </c>
       <c r="V128" s="1" t="s">
-        <v>691</v>
+        <v>686</v>
       </c>
       <c r="W128" s="15" t="s">
-        <v>664</v>
+        <v>659</v>
       </c>
       <c r="X128" s="15" t="s">
-        <v>664</v>
+        <v>659</v>
       </c>
       <c r="Y128" s="1">
         <v>11000002</v>
@@ -20425,10 +20434,10 @@
         <v>53000126</v>
       </c>
       <c r="B129" s="22" t="s">
-        <v>668</v>
+        <v>663</v>
       </c>
       <c r="C129" s="15" t="s">
-        <v>667</v>
+        <v>662</v>
       </c>
       <c r="D129" s="25"/>
       <c r="E129" s="15">
@@ -20476,22 +20485,22 @@
         <v>0</v>
       </c>
       <c r="S129" s="7" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="T129">
         <v>100</v>
       </c>
       <c r="U129" s="11" t="s">
-        <v>882</v>
+        <v>870</v>
       </c>
       <c r="V129" s="1" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
       <c r="W129" s="1" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="X129" s="1" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="Y129" s="1">
         <v>11000001</v>
@@ -20514,13 +20523,13 @@
         <v>53000127</v>
       </c>
       <c r="B130" s="22" t="s">
-        <v>669</v>
+        <v>664</v>
       </c>
       <c r="C130" s="15" t="s">
-        <v>670</v>
+        <v>665</v>
       </c>
       <c r="D130" s="25" t="s">
-        <v>772</v>
+        <v>767</v>
       </c>
       <c r="E130" s="15">
         <v>4</v>
@@ -20567,22 +20576,22 @@
         <v>15</v>
       </c>
       <c r="S130" s="7" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
       <c r="T130">
         <v>103</v>
       </c>
       <c r="U130" s="11" t="s">
-        <v>843</v>
+        <v>832</v>
       </c>
       <c r="V130" s="1" t="s">
-        <v>672</v>
+        <v>667</v>
       </c>
       <c r="W130" s="1" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="X130" s="1" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="Y130" s="1">
         <v>11000001</v>
@@ -20605,13 +20614,13 @@
         <v>53000128</v>
       </c>
       <c r="B131" s="22" t="s">
-        <v>675</v>
+        <v>670</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>674</v>
+        <v>669</v>
       </c>
       <c r="D131" s="25" t="s">
-        <v>767</v>
+        <v>762</v>
       </c>
       <c r="E131" s="15">
         <v>1</v>
@@ -20658,22 +20667,22 @@
         <v>25</v>
       </c>
       <c r="S131" s="7" t="s">
-        <v>673</v>
+        <v>668</v>
       </c>
       <c r="T131">
         <v>100</v>
       </c>
       <c r="U131" s="11" t="s">
-        <v>846</v>
+        <v>835</v>
       </c>
       <c r="V131" s="1" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
       <c r="W131" s="1" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="X131" s="1" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="Y131" s="1">
         <v>11000001</v>
@@ -20696,13 +20705,13 @@
         <v>53000129</v>
       </c>
       <c r="B132" s="22" t="s">
-        <v>687</v>
+        <v>682</v>
       </c>
       <c r="C132" s="15" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="D132" s="25" t="s">
-        <v>688</v>
+        <v>683</v>
       </c>
       <c r="E132" s="15">
         <v>3</v>
@@ -20749,22 +20758,22 @@
         <v>0</v>
       </c>
       <c r="S132" s="7" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
       <c r="T132">
         <v>103</v>
       </c>
       <c r="U132" s="11" t="s">
-        <v>847</v>
+        <v>836</v>
       </c>
       <c r="V132" s="1" t="s">
-        <v>692</v>
+        <v>687</v>
       </c>
       <c r="W132" s="1" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
       <c r="X132" s="1" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
       <c r="Y132" s="1">
         <v>11000002</v>
@@ -20787,13 +20796,13 @@
         <v>53000130</v>
       </c>
       <c r="B133" s="22" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="C133" s="15" t="s">
-        <v>695</v>
+        <v>690</v>
       </c>
       <c r="D133" s="25" t="s">
-        <v>767</v>
+        <v>762</v>
       </c>
       <c r="E133" s="15">
         <v>5</v>
@@ -20840,22 +20849,22 @@
         <v>25</v>
       </c>
       <c r="S133" s="7" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
       <c r="T133">
         <v>107</v>
       </c>
       <c r="U133" s="11" t="s">
-        <v>883</v>
+        <v>871</v>
       </c>
       <c r="V133" s="1" t="s">
-        <v>697</v>
+        <v>692</v>
       </c>
       <c r="W133" s="1" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
       <c r="X133" s="1" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
       <c r="Y133" s="1">
         <v>11000002</v>
@@ -20878,13 +20887,13 @@
         <v>53000131</v>
       </c>
       <c r="B134" s="22" t="s">
-        <v>699</v>
+        <v>694</v>
       </c>
       <c r="C134" s="15" t="s">
-        <v>700</v>
+        <v>695</v>
       </c>
       <c r="D134" s="25" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="E134" s="15">
         <v>2</v>
@@ -20931,22 +20940,22 @@
         <v>30</v>
       </c>
       <c r="S134" s="7" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="T134">
         <v>100</v>
       </c>
       <c r="U134" s="11" t="s">
-        <v>843</v>
+        <v>832</v>
       </c>
       <c r="V134" s="1" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="W134" s="1" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="X134" s="1" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="Y134" s="1">
         <v>11000002</v>
@@ -20969,13 +20978,13 @@
         <v>53000132</v>
       </c>
       <c r="B135" s="22" t="s">
-        <v>701</v>
+        <v>696</v>
       </c>
       <c r="C135" s="15" t="s">
-        <v>702</v>
+        <v>697</v>
       </c>
       <c r="D135" s="25" t="s">
-        <v>703</v>
+        <v>698</v>
       </c>
       <c r="E135" s="15">
         <v>3</v>
@@ -21022,22 +21031,22 @@
         <v>0</v>
       </c>
       <c r="S135" s="7" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
       <c r="T135">
         <v>102</v>
       </c>
       <c r="U135" s="11" t="s">
-        <v>896</v>
+        <v>884</v>
       </c>
       <c r="V135" s="1" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="W135" s="1" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="X135" s="1" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="Y135" s="1">
         <v>11000002</v>
@@ -21060,13 +21069,13 @@
         <v>53000133</v>
       </c>
       <c r="B136" s="22" t="s">
-        <v>711</v>
+        <v>706</v>
       </c>
       <c r="C136" s="15" t="s">
-        <v>710</v>
+        <v>705</v>
       </c>
       <c r="D136" s="25" t="s">
-        <v>712</v>
+        <v>707</v>
       </c>
       <c r="E136" s="15">
         <v>2</v>
@@ -21119,10 +21128,10 @@
         <v>100</v>
       </c>
       <c r="U136" s="11" t="s">
-        <v>884</v>
+        <v>872</v>
       </c>
       <c r="V136" s="1" t="s">
-        <v>737</v>
+        <v>732</v>
       </c>
       <c r="W136" s="15" t="s">
         <v>4</v>
@@ -21149,13 +21158,13 @@
         <v>53000134</v>
       </c>
       <c r="B137" s="22" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
       <c r="C137" s="15" t="s">
-        <v>713</v>
+        <v>708</v>
       </c>
       <c r="D137" s="25" t="s">
-        <v>712</v>
+        <v>707</v>
       </c>
       <c r="E137" s="15">
         <v>2</v>
@@ -21208,10 +21217,10 @@
         <v>103</v>
       </c>
       <c r="U137" s="11" t="s">
-        <v>885</v>
+        <v>873</v>
       </c>
       <c r="V137" s="1" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
       <c r="W137" s="15" t="s">
         <v>4</v>
@@ -21238,13 +21247,13 @@
         <v>53000135</v>
       </c>
       <c r="B138" s="22" t="s">
-        <v>716</v>
+        <v>711</v>
       </c>
       <c r="C138" s="15" t="s">
-        <v>717</v>
+        <v>712</v>
       </c>
       <c r="D138" s="25" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="E138" s="15">
         <v>4</v>
@@ -21291,19 +21300,19 @@
         <v>20</v>
       </c>
       <c r="S138" s="15" t="s">
-        <v>720</v>
+        <v>715</v>
       </c>
       <c r="T138" s="15">
         <v>108</v>
       </c>
       <c r="U138" s="11" t="s">
-        <v>848</v>
+        <v>837</v>
       </c>
       <c r="V138" s="1" t="s">
-        <v>722</v>
+        <v>717</v>
       </c>
       <c r="W138" s="1" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="X138" s="15"/>
       <c r="Y138" s="15">
@@ -21327,13 +21336,13 @@
         <v>53000136</v>
       </c>
       <c r="B139" s="22" t="s">
-        <v>719</v>
+        <v>714</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="D139" s="25" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="E139" s="15">
         <v>4</v>
@@ -21380,19 +21389,19 @@
         <v>20</v>
       </c>
       <c r="S139" s="15" t="s">
-        <v>723</v>
+        <v>718</v>
       </c>
       <c r="T139" s="15">
         <v>100</v>
       </c>
       <c r="U139" s="11" t="s">
-        <v>849</v>
+        <v>838</v>
       </c>
       <c r="V139" s="1" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
       <c r="W139" s="15" t="s">
-        <v>749</v>
+        <v>744</v>
       </c>
       <c r="X139" s="15"/>
       <c r="Y139" s="15">
@@ -21416,13 +21425,13 @@
         <v>53000137</v>
       </c>
       <c r="B140" s="22" t="s">
-        <v>726</v>
+        <v>721</v>
       </c>
       <c r="C140" s="15" t="s">
-        <v>727</v>
+        <v>722</v>
       </c>
       <c r="D140" s="25" t="s">
-        <v>728</v>
+        <v>723</v>
       </c>
       <c r="E140" s="15">
         <v>2</v>
@@ -21469,16 +21478,16 @@
         <v>0</v>
       </c>
       <c r="S140" s="15" t="s">
-        <v>730</v>
+        <v>725</v>
       </c>
       <c r="T140" s="15">
         <v>102</v>
       </c>
       <c r="U140" s="11" t="s">
-        <v>850</v>
+        <v>839</v>
       </c>
       <c r="V140" s="1" t="s">
-        <v>729</v>
+        <v>724</v>
       </c>
       <c r="W140" s="15" t="s">
         <v>4</v>
@@ -21505,10 +21514,10 @@
         <v>53000138</v>
       </c>
       <c r="B141" s="22" t="s">
-        <v>739</v>
+        <v>734</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>740</v>
+        <v>735</v>
       </c>
       <c r="D141" s="25" t="s">
         <v>398</v>
@@ -21558,19 +21567,19 @@
         <v>1</v>
       </c>
       <c r="S141" s="15" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="T141" s="15">
         <v>105</v>
       </c>
       <c r="U141" s="11" t="s">
-        <v>911</v>
+        <v>899</v>
       </c>
       <c r="V141" s="1" t="s">
-        <v>746</v>
+        <v>741</v>
       </c>
       <c r="W141" s="1" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="X141" s="15"/>
       <c r="Y141" s="15">
@@ -21594,10 +21603,10 @@
         <v>53000139</v>
       </c>
       <c r="B142" s="22" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>742</v>
+        <v>737</v>
       </c>
       <c r="D142" s="25" t="s">
         <v>473</v>
@@ -21647,19 +21656,19 @@
         <v>2</v>
       </c>
       <c r="S142" s="15" t="s">
-        <v>730</v>
+        <v>725</v>
       </c>
       <c r="T142" s="15">
         <v>103</v>
       </c>
       <c r="U142" s="11" t="s">
-        <v>886</v>
+        <v>874</v>
       </c>
       <c r="V142" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="W142" s="15" t="s">
         <v>743</v>
-      </c>
-      <c r="W142" s="15" t="s">
-        <v>748</v>
       </c>
       <c r="X142" s="15"/>
       <c r="Y142" s="15">
@@ -21683,10 +21692,10 @@
         <v>53000140</v>
       </c>
       <c r="B143" s="22" t="s">
-        <v>744</v>
+        <v>739</v>
       </c>
       <c r="C143" s="15" t="s">
-        <v>745</v>
+        <v>740</v>
       </c>
       <c r="D143" s="25" t="s">
         <v>398</v>
@@ -21736,19 +21745,19 @@
         <v>3</v>
       </c>
       <c r="S143" s="15" t="s">
-        <v>730</v>
+        <v>725</v>
       </c>
       <c r="T143" s="15">
         <v>100</v>
       </c>
       <c r="U143" s="11" t="s">
-        <v>912</v>
+        <v>900</v>
       </c>
       <c r="V143" s="1" t="s">
-        <v>747</v>
+        <v>742</v>
       </c>
       <c r="W143" s="15" t="s">
-        <v>748</v>
+        <v>743</v>
       </c>
       <c r="X143" s="15"/>
       <c r="Y143" s="15">
@@ -21880,7 +21889,7 @@
         <v>344</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="P1" s="17" t="s">
         <v>327</v>
@@ -21919,7 +21928,7 @@
         <v>352</v>
       </c>
       <c r="AB1" s="23" t="s">
-        <v>923</v>
+        <v>911</v>
       </c>
       <c r="AC1" s="23" t="s">
         <v>355</v>
@@ -21969,7 +21978,7 @@
         <v>343</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>314</v>
@@ -22058,7 +22067,7 @@
         <v>346</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="P3" s="20" t="s">
         <v>329</v>
@@ -22097,10 +22106,10 @@
         <v>353</v>
       </c>
       <c r="AB3" s="43" t="s">
-        <v>924</v>
+        <v>912</v>
       </c>
       <c r="AC3" s="43" t="s">
-        <v>925</v>
+        <v>913</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="24" x14ac:dyDescent="0.15">
@@ -22163,7 +22172,7 @@
         <v>-1</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>851</v>
+        <v>840</v>
       </c>
       <c r="V4" s="7" t="s">
         <v>337</v>
@@ -22246,10 +22255,10 @@
         <v>-1</v>
       </c>
       <c r="U5" s="11" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
       <c r="V5" s="7" t="s">
-        <v>774</v>
+        <v>769</v>
       </c>
       <c r="W5" s="1" t="s">
         <v>15</v>
@@ -22323,16 +22332,16 @@
         <v>0</v>
       </c>
       <c r="S6" s="15" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="T6" s="1">
         <v>-1</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>852</v>
+        <v>841</v>
       </c>
       <c r="V6" s="7" t="s">
-        <v>721</v>
+        <v>716</v>
       </c>
       <c r="W6" s="15" t="s">
         <v>358</v>
@@ -22412,10 +22421,10 @@
         <v>-1</v>
       </c>
       <c r="U7" s="11" t="s">
-        <v>853</v>
+        <v>842</v>
       </c>
       <c r="V7" s="7" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
       <c r="W7" s="15" t="s">
         <v>2</v>
@@ -22495,7 +22504,7 @@
         <v>-1</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>854</v>
+        <v>843</v>
       </c>
       <c r="V8" s="7" t="s">
         <v>369</v>
@@ -22578,7 +22587,7 @@
         <v>-1</v>
       </c>
       <c r="U9" s="11" t="s">
-        <v>899</v>
+        <v>887</v>
       </c>
       <c r="V9" s="7" t="s">
         <v>367</v>
@@ -22661,7 +22670,7 @@
         <v>-1</v>
       </c>
       <c r="U10" s="11" t="s">
-        <v>900</v>
+        <v>888</v>
       </c>
       <c r="V10" s="7" t="s">
         <v>481</v>
@@ -22689,7 +22698,7 @@
         <v>53100007</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="32"/>
@@ -22738,16 +22747,16 @@
         <v>0</v>
       </c>
       <c r="S11" s="15" t="s">
-        <v>922</v>
+        <v>910</v>
       </c>
       <c r="T11" s="1">
         <v>-1</v>
       </c>
       <c r="U11" s="11" t="s">
-        <v>901</v>
+        <v>889</v>
       </c>
       <c r="V11" s="7" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="W11" s="15" t="s">
         <v>2</v>
@@ -22772,7 +22781,7 @@
         <v>53100008</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="32"/>
@@ -22821,16 +22830,16 @@
         <v>0</v>
       </c>
       <c r="S12" s="15" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="T12" s="1">
         <v>-1</v>
       </c>
       <c r="U12" s="11" t="s">
-        <v>855</v>
+        <v>844</v>
       </c>
       <c r="V12" s="7" t="s">
-        <v>754</v>
+        <v>749</v>
       </c>
       <c r="W12" s="15" t="s">
         <v>2</v>
@@ -22855,7 +22864,7 @@
         <v>53200001</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>752</v>
+        <v>747</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="32"/>
@@ -22904,19 +22913,19 @@
         <v>0</v>
       </c>
       <c r="S13" s="15" t="s">
-        <v>751</v>
+        <v>746</v>
       </c>
       <c r="T13" s="1">
         <v>-1</v>
       </c>
       <c r="U13" s="11" t="s">
-        <v>856</v>
+        <v>845</v>
       </c>
       <c r="V13" s="7" t="s">
-        <v>755</v>
+        <v>750</v>
       </c>
       <c r="W13" s="15" t="s">
-        <v>750</v>
+        <v>745</v>
       </c>
       <c r="X13" s="15"/>
       <c r="Y13" s="15"/>
@@ -22938,7 +22947,7 @@
         <v>53200002</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>756</v>
+        <v>751</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="42"/>
@@ -22987,16 +22996,16 @@
         <v>0</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>757</v>
+        <v>752</v>
       </c>
       <c r="T14">
         <v>-1</v>
       </c>
       <c r="U14" s="11" t="s">
-        <v>917</v>
+        <v>905</v>
       </c>
       <c r="V14" s="7" t="s">
-        <v>753</v>
+        <v>748</v>
       </c>
       <c r="W14" s="15" t="s">
         <v>2</v>
@@ -23021,7 +23030,7 @@
         <v>53200003</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>764</v>
+        <v>759</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="32"/>
@@ -23070,16 +23079,16 @@
         <v>0</v>
       </c>
       <c r="S15" s="15" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="T15" s="1">
         <v>-1</v>
       </c>
       <c r="U15" s="11" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
       <c r="V15" s="7" t="s">
-        <v>763</v>
+        <v>758</v>
       </c>
       <c r="W15" s="15" t="s">
         <v>2</v>
@@ -23212,7 +23221,7 @@
         <v>344</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="P1" s="17" t="s">
         <v>327</v>
@@ -23251,7 +23260,7 @@
         <v>352</v>
       </c>
       <c r="AB1" s="23" t="s">
-        <v>923</v>
+        <v>911</v>
       </c>
       <c r="AC1" s="23" t="s">
         <v>355</v>
@@ -23301,7 +23310,7 @@
         <v>343</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>314</v>
@@ -23390,7 +23399,7 @@
         <v>346</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="P3" s="20" t="s">
         <v>329</v>
@@ -23429,10 +23438,10 @@
         <v>353</v>
       </c>
       <c r="AB3" s="43" t="s">
-        <v>924</v>
+        <v>912</v>
       </c>
       <c r="AC3" s="43" t="s">
-        <v>925</v>
+        <v>913</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="36" x14ac:dyDescent="0.15">
@@ -23499,7 +23508,7 @@
         <v>115</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>857</v>
+        <v>846</v>
       </c>
       <c r="V4" s="7" t="s">
         <v>368</v>
@@ -23586,7 +23595,7 @@
         <v>90</v>
       </c>
       <c r="U5" s="11" t="s">
-        <v>858</v>
+        <v>847</v>
       </c>
       <c r="V5" s="7" t="s">
         <v>370</v>
@@ -23673,7 +23682,7 @@
         <v>115</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>859</v>
+        <v>848</v>
       </c>
       <c r="V6" s="29" t="s">
         <v>409</v>
@@ -23845,7 +23854,7 @@
         <v>90</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>860</v>
+        <v>849</v>
       </c>
       <c r="V8" s="7" t="s">
         <v>379</v>
@@ -23934,7 +23943,7 @@
         <v>400</v>
       </c>
       <c r="U9" s="11" t="s">
-        <v>913</v>
+        <v>901</v>
       </c>
       <c r="V9" s="7" t="s">
         <v>331</v>
@@ -24301,7 +24310,7 @@
       </c>
       <c r="B11">
         <f>COUNTIF(标准!D:D,"*属性*")</f>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
try use all cards on ai round
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E20154CE-28B8-4FC1-8289-ABCC78D71034}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{011BFAC2-3EE2-494F-8315-C500FAE490BC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -637,7 +637,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="963">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="964">
   <si>
     <t>慈悲</t>
   </si>
@@ -4078,6 +4078,10 @@
   </si>
   <si>
     <t>int count=0;foreach(IMonster im in m.GetRangeMonster(p.IsLeft,spl.Target,spl.Shape,spl.Range,mouse)){im.Action.AddAttrModify("Spell",spl.Id,"Spd",-spl.Help);count++;}if(count&gt;0)p.Tower.Action.AddPArmor(spl.Cure*count);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bleedglow</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -5104,201 +5108,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="127">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="122">
     <dxf>
       <font>
         <b val="0"/>
@@ -7869,6 +7679,142 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <color auto="1"/>
@@ -8842,135 +8788,135 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:AC148" totalsRowShown="0" headerRowDxfId="121" dataDxfId="120" tableBorderDxfId="119">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:AC148" totalsRowShown="0" headerRowDxfId="104" dataDxfId="103" tableBorderDxfId="102">
   <autoFilter ref="A3:AC148" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A4:AC113">
     <sortCondition ref="A3:A113"/>
   </sortState>
   <tableColumns count="29">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="118"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="117"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Ename" dataDxfId="116"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Remark" dataDxfId="115"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Star" dataDxfId="114"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Type" dataDxfId="113"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Attr" dataDxfId="112"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Quality" dataDxfId="111">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="101"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="100"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Ename" dataDxfId="99"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Remark" dataDxfId="98"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Star" dataDxfId="97"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Type" dataDxfId="96"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Attr" dataDxfId="95"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Quality" dataDxfId="94">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Cost" dataDxfId="110"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Damage" dataDxfId="109"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Cure" dataDxfId="108"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Time" dataDxfId="107"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Help" dataDxfId="106"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Rate" dataDxfId="105"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Atk" dataDxfId="104"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Modify" dataDxfId="103"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Sum" dataDxfId="102">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Cost" dataDxfId="93"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Damage" dataDxfId="92"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Cure" dataDxfId="91"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Time" dataDxfId="90"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Help" dataDxfId="89"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Rate" dataDxfId="88"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Atk" dataDxfId="87"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Modify" dataDxfId="86"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Sum" dataDxfId="85">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Range" dataDxfId="101"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Target" dataDxfId="100"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Mark" dataDxfId="99"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Effect" dataDxfId="98"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="GetDescript" dataDxfId="97"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="UnitEffect" dataDxfId="96"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="AreaEffect" dataDxfId="95"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="JobId" dataDxfId="94"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Icon" dataDxfId="93"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="IsSpecial" dataDxfId="92"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="IsHeroCard" dataDxfId="91"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="IsNew" dataDxfId="90"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Range" dataDxfId="84"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Target" dataDxfId="83"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Mark" dataDxfId="82"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Effect" dataDxfId="81"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="GetDescript" dataDxfId="80"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="UnitEffect" dataDxfId="79"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="AreaEffect" dataDxfId="78"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="JobId" dataDxfId="77"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Icon" dataDxfId="76"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="IsSpecial" dataDxfId="75"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="IsHeroCard" dataDxfId="74"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="IsNew" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表1_3" displayName="表1_3" ref="A3:AC15" totalsRowShown="0" headerRowDxfId="84" dataDxfId="83" tableBorderDxfId="82">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表1_3" displayName="表1_3" ref="A3:AC15" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66" tableBorderDxfId="65">
   <autoFilter ref="A3:AC15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="29">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id" dataDxfId="81"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="80"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="Ename" dataDxfId="79"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="Remark" dataDxfId="78"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Star" dataDxfId="77"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Type" dataDxfId="76"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Attr" dataDxfId="75"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Quality" dataDxfId="74">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id" dataDxfId="64"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="63"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="Ename" dataDxfId="62"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="Remark" dataDxfId="61"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Star" dataDxfId="60"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Type" dataDxfId="59"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Attr" dataDxfId="58"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Quality" dataDxfId="57">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Cost" dataDxfId="73"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Damage" dataDxfId="72"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Cure" dataDxfId="71"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Time" dataDxfId="70"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Help" dataDxfId="69"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Rate" dataDxfId="68"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Atk" dataDxfId="67"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Modify" dataDxfId="66"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0100-00001B000000}" name="Sum" dataDxfId="65">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Cost" dataDxfId="56"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Damage" dataDxfId="55"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Cure" dataDxfId="54"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Time" dataDxfId="53"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Help" dataDxfId="52"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Rate" dataDxfId="51"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Atk" dataDxfId="50"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Modify" dataDxfId="49"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0100-00001B000000}" name="Sum" dataDxfId="48">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Range" dataDxfId="64"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Target" dataDxfId="63"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0100-000019000000}" name="Mark" dataDxfId="62"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="Effect" dataDxfId="61"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0100-000018000000}" name="GetDescript" dataDxfId="60"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="UnitEffect" dataDxfId="59"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0100-00001C000000}" name="AreaEffect" dataDxfId="58"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0100-00001A000000}" name="JobId" dataDxfId="57"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="Icon" dataDxfId="56"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="IsSpecial" dataDxfId="55"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0100-00001D000000}" name="IsHeroCard" dataDxfId="54"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="IsNew" dataDxfId="53"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Range" dataDxfId="47"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Target" dataDxfId="46"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0100-000019000000}" name="Mark" dataDxfId="45"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="Effect" dataDxfId="44"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0100-000018000000}" name="GetDescript" dataDxfId="43"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="UnitEffect" dataDxfId="42"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0100-00001C000000}" name="AreaEffect" dataDxfId="41"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0100-00001A000000}" name="JobId" dataDxfId="40"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="Icon" dataDxfId="39"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="IsSpecial" dataDxfId="38"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0100-00001D000000}" name="IsHeroCard" dataDxfId="37"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="IsNew" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="表1_35" displayName="表1_35" ref="A3:AC9" totalsRowShown="0" headerRowDxfId="47" tableBorderDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="表1_35" displayName="表1_35" ref="A3:AC9" totalsRowShown="0" headerRowDxfId="30" tableBorderDxfId="29">
   <autoFilter ref="A3:AC9" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <sortState ref="A4:X138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="29">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Id" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="44"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0200-000014000000}" name="Ename" dataDxfId="43"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0200-000015000000}" name="Remark" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Star" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Type" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Attr" dataDxfId="39"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Quality" dataDxfId="38">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Id" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="27"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0200-000014000000}" name="Ename" dataDxfId="26"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0200-000015000000}" name="Remark" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Star" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Type" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Attr" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Quality" dataDxfId="21">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Cost" dataDxfId="37"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Damage" dataDxfId="36"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Cure" dataDxfId="35"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Time" dataDxfId="34"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="Help" dataDxfId="33"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="Rate" dataDxfId="32"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0200-000012000000}" name="Atk" dataDxfId="31"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Modify" dataDxfId="30"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0200-00001B000000}" name="Sum" dataDxfId="29">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Cost" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Damage" dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Cure" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Time" dataDxfId="17"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="Help" dataDxfId="16"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="Rate" dataDxfId="15"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0200-000012000000}" name="Atk" dataDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Modify" dataDxfId="13"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0200-00001B000000}" name="Sum" dataDxfId="12">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Range" dataDxfId="28"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Target" dataDxfId="27"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0200-000019000000}" name="Mark" dataDxfId="26"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0200-000016000000}" name="Effect" dataDxfId="25"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0200-000018000000}" name="GetDescript" dataDxfId="24"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="UnitEffect" dataDxfId="23"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0200-00001C000000}" name="AreaEffect" dataDxfId="22"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0200-00001A000000}" name="JobId" dataDxfId="21"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0200-000013000000}" name="Icon" dataDxfId="20"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="IsSpecial" dataDxfId="19"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0200-00001D000000}" name="IsHeroCard" dataDxfId="18"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0200-000017000000}" name="IsNew" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Range" dataDxfId="11"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Target" dataDxfId="10"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0200-000019000000}" name="Mark" dataDxfId="9"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0200-000016000000}" name="Effect" dataDxfId="8"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0200-000018000000}" name="GetDescript" dataDxfId="7"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="UnitEffect" dataDxfId="6"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0200-00001C000000}" name="AreaEffect" dataDxfId="5"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0200-00001A000000}" name="JobId" dataDxfId="4"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0200-000013000000}" name="Icon" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="IsSpecial" dataDxfId="2"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0200-00001D000000}" name="IsHeroCard" dataDxfId="1"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0200-000017000000}" name="IsNew" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9300,10 +9246,10 @@
   <dimension ref="A1:AC148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C105" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C141" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="U107" sqref="U107"/>
+      <selection pane="bottomRight" activeCell="W144" sqref="W144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -22263,7 +22209,7 @@
         <v>935</v>
       </c>
       <c r="W145" s="15" t="s">
-        <v>361</v>
+        <v>963</v>
       </c>
       <c r="X145" s="15"/>
       <c r="Y145" s="15">
@@ -22557,69 +22503,69 @@
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="H4:H146">
-    <cfRule type="cellIs" dxfId="126" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="24" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="25" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="26" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="27" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="118" priority="27" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:Q146">
-    <cfRule type="cellIs" dxfId="122" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="18" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H147">
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="9" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="10" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="11" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="113" priority="12" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J147:K147 M147:O147">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H148">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="5" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="6" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="108" priority="7" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J148:Q148">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L147">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P147:Q147">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22640,7 +22586,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H4" sqref="H4:H15"/>
+      <selection pane="bottomRight" activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -23929,21 +23875,21 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="J4:O15">
-    <cfRule type="cellIs" dxfId="89" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H15">
-    <cfRule type="cellIs" dxfId="88" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="2" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="68" priority="4" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24780,21 +24726,21 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="J4:P9">
-    <cfRule type="cellIs" dxfId="52" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="15" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H9">
-    <cfRule type="cellIs" dxfId="51" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="31" priority="4" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
ai can use hero power now
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CBD8136B-B692-4643-91EA-845B17010E1E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1FC9D67C-1732-4DCB-9939-003C6B5FC9EB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="标准" sheetId="1" r:id="rId1"/>
@@ -637,7 +637,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="967">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="979">
   <si>
     <t>慈悲</t>
   </si>
@@ -4094,6 +4094,51 @@
   </si>
   <si>
     <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fire Arrow</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heal</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Aim Shoot</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Transform</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Totems</t>
+  </si>
+  <si>
+    <t>Shield</t>
+  </si>
+  <si>
+    <t>Delivery</t>
+  </si>
+  <si>
+    <t>Explore</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dorsal Thorns</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Undead</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Iron Shield</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Train</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -5122,369 +5167,6 @@
   </cellStyles>
   <dxfs count="125">
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -5636,6 +5318,18 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -6292,6 +5986,64 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -6452,6 +6204,18 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -7110,6 +6874,64 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -7268,6 +7090,35 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -7925,6 +7776,200 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -8853,138 +8898,138 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:AD148" totalsRowShown="0" headerRowDxfId="124" dataDxfId="123" tableBorderDxfId="122">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:AD148" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106" tableBorderDxfId="105">
   <autoFilter ref="A3:AD148" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A4:AD113">
     <sortCondition ref="A3:A113"/>
   </sortState>
   <tableColumns count="30">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="121"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="120"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Ename" dataDxfId="119"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Remark" dataDxfId="118"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Star" dataDxfId="117"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Type" dataDxfId="116"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Attr" dataDxfId="115"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Quality" dataDxfId="114">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="104"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="103"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Ename" dataDxfId="102"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Remark" dataDxfId="101"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Star" dataDxfId="100"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Type" dataDxfId="99"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Attr" dataDxfId="98"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Quality" dataDxfId="97">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Cost" dataDxfId="113"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Damage" dataDxfId="112"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Cure" dataDxfId="111"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Time" dataDxfId="110"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Help" dataDxfId="109"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Rate" dataDxfId="108"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Atk" dataDxfId="107"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Modify" dataDxfId="106"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Sum" dataDxfId="105">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Cost" dataDxfId="96"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Damage" dataDxfId="95"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Cure" dataDxfId="94"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Time" dataDxfId="93"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Help" dataDxfId="92"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Rate" dataDxfId="91"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Atk" dataDxfId="90"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Modify" dataDxfId="89"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Sum" dataDxfId="88">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Range" dataDxfId="104"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Target" dataDxfId="103"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Mark" dataDxfId="102"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Effect" dataDxfId="101"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="GetDescript" dataDxfId="100"/>
-    <tableColumn id="30" xr3:uid="{855D43A6-6E98-4ADA-A6E2-774AEE3CD604}" name="AIGuide" dataDxfId="29"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="UnitEffect" dataDxfId="99"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="AreaEffect" dataDxfId="98"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="JobId" dataDxfId="97"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Icon" dataDxfId="96"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="IsSpecial" dataDxfId="95"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="IsHeroCard" dataDxfId="94"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="IsNew" dataDxfId="93"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Range" dataDxfId="87"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Target" dataDxfId="86"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Mark" dataDxfId="85"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Effect" dataDxfId="84"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="GetDescript" dataDxfId="83"/>
+    <tableColumn id="30" xr3:uid="{855D43A6-6E98-4ADA-A6E2-774AEE3CD604}" name="AIGuide" dataDxfId="82"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="UnitEffect" dataDxfId="81"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="AreaEffect" dataDxfId="80"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="JobId" dataDxfId="79"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Icon" dataDxfId="78"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="IsSpecial" dataDxfId="77"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="IsHeroCard" dataDxfId="76"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="IsNew" dataDxfId="75"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表1_3" displayName="表1_3" ref="A3:AD15" totalsRowShown="0" headerRowDxfId="92" dataDxfId="91" tableBorderDxfId="90">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表1_3" displayName="表1_3" ref="A3:AD15" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68" tableBorderDxfId="67">
   <autoFilter ref="A3:AD15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState ref="A4:Y138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="30">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id" dataDxfId="89"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="88"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="Ename" dataDxfId="87"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="Remark" dataDxfId="86"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Star" dataDxfId="85"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Type" dataDxfId="84"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Attr" dataDxfId="83"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Quality" dataDxfId="82">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="65"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="Ename" dataDxfId="64"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="Remark" dataDxfId="63"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Star" dataDxfId="62"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Type" dataDxfId="61"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Attr" dataDxfId="60"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Quality" dataDxfId="59">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Cost" dataDxfId="81"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Damage" dataDxfId="80"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Cure" dataDxfId="79"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Time" dataDxfId="78"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Help" dataDxfId="77"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Rate" dataDxfId="76"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Atk" dataDxfId="75"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Modify" dataDxfId="74"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0100-00001B000000}" name="Sum" dataDxfId="73">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Cost" dataDxfId="58"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Damage" dataDxfId="57"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Cure" dataDxfId="56"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Time" dataDxfId="55"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Help" dataDxfId="54"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Rate" dataDxfId="53"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Atk" dataDxfId="52"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Modify" dataDxfId="51"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0100-00001B000000}" name="Sum" dataDxfId="50">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Range" dataDxfId="72"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Target" dataDxfId="71"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0100-000019000000}" name="Mark" dataDxfId="70"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="Effect" dataDxfId="69"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0100-000018000000}" name="GetDescript" dataDxfId="68"/>
-    <tableColumn id="30" xr3:uid="{0DE86C9C-186F-4804-9A5E-1974A3DB9511}" name="AIGuide" dataDxfId="28"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="UnitEffect" dataDxfId="67"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0100-00001C000000}" name="AreaEffect" dataDxfId="66"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0100-00001A000000}" name="JobId" dataDxfId="65"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="Icon" dataDxfId="64"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="IsSpecial" dataDxfId="63"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0100-00001D000000}" name="IsHeroCard" dataDxfId="62"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="IsNew" dataDxfId="61"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Range" dataDxfId="49"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Target" dataDxfId="48"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0100-000019000000}" name="Mark" dataDxfId="47"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="Effect" dataDxfId="46"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0100-000018000000}" name="GetDescript" dataDxfId="45"/>
+    <tableColumn id="30" xr3:uid="{0DE86C9C-186F-4804-9A5E-1974A3DB9511}" name="AIGuide" dataDxfId="44"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="UnitEffect" dataDxfId="43"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0100-00001C000000}" name="AreaEffect" dataDxfId="42"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0100-00001A000000}" name="JobId" dataDxfId="41"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="Icon" dataDxfId="40"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="IsSpecial" dataDxfId="39"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0100-00001D000000}" name="IsHeroCard" dataDxfId="38"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="IsNew" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="表1_35" displayName="表1_35" ref="A3:AD9" totalsRowShown="0" headerRowDxfId="60" tableBorderDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="表1_35" displayName="表1_35" ref="A3:AD9" totalsRowShown="0" headerRowDxfId="31" tableBorderDxfId="30">
   <autoFilter ref="A3:AD9" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <sortState ref="A4:Y138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="30">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Id" dataDxfId="58"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="57"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0200-000014000000}" name="Ename" dataDxfId="56"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0200-000015000000}" name="Remark" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Star" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Type" dataDxfId="53"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Attr" dataDxfId="52"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Quality" dataDxfId="51">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Id" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="28"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0200-000014000000}" name="Ename" dataDxfId="27"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0200-000015000000}" name="Remark" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Star" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Type" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Attr" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Quality" dataDxfId="22">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Cost" dataDxfId="50"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Damage" dataDxfId="49"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Cure" dataDxfId="48"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Time" dataDxfId="47"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="Help" dataDxfId="46"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="Rate" dataDxfId="45"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0200-000012000000}" name="Atk" dataDxfId="44"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Modify" dataDxfId="43"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0200-00001B000000}" name="Sum" dataDxfId="42">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Cost" dataDxfId="21"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Damage" dataDxfId="20"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Cure" dataDxfId="19"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Time" dataDxfId="18"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="Help" dataDxfId="17"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="Rate" dataDxfId="16"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0200-000012000000}" name="Atk" dataDxfId="15"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Modify" dataDxfId="14"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0200-00001B000000}" name="Sum" dataDxfId="13">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Range" dataDxfId="41"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Target" dataDxfId="40"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0200-000019000000}" name="Mark" dataDxfId="39"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0200-000016000000}" name="Effect" dataDxfId="38"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0200-000018000000}" name="GetDescript" dataDxfId="37"/>
-    <tableColumn id="30" xr3:uid="{20990888-4397-404C-ADB5-103975BBDFBA}" name="AIGuide" dataDxfId="0"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="UnitEffect" dataDxfId="36"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0200-00001C000000}" name="AreaEffect" dataDxfId="35"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0200-00001A000000}" name="JobId" dataDxfId="34"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0200-000013000000}" name="Icon" dataDxfId="33"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="IsSpecial" dataDxfId="32"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0200-00001D000000}" name="IsHeroCard" dataDxfId="31"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0200-000017000000}" name="IsNew" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Range" dataDxfId="12"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Target" dataDxfId="11"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0200-000019000000}" name="Mark" dataDxfId="10"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0200-000016000000}" name="Effect" dataDxfId="9"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0200-000018000000}" name="GetDescript" dataDxfId="8"/>
+    <tableColumn id="30" xr3:uid="{20990888-4397-404C-ADB5-103975BBDFBA}" name="AIGuide" dataDxfId="7"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="UnitEffect" dataDxfId="6"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0200-00001C000000}" name="AreaEffect" dataDxfId="5"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0200-00001A000000}" name="JobId" dataDxfId="4"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0200-000013000000}" name="Icon" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="IsSpecial" dataDxfId="2"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0200-00001D000000}" name="IsHeroCard" dataDxfId="1"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0200-000017000000}" name="IsNew" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9313,11 +9358,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD148"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="J144" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C139" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W148" sqref="W148"/>
+      <selection pane="bottomRight" activeCell="K139" sqref="K139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -22908,69 +22953,69 @@
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="H4:H146">
-    <cfRule type="cellIs" dxfId="27" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="24" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="25" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="26" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="27" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="121" priority="27" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:Q146">
-    <cfRule type="cellIs" dxfId="23" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="18" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H147">
-    <cfRule type="cellIs" dxfId="22" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="9" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="10" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="11" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="12" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="116" priority="12" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J147:K147 M147:O147">
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H148">
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="5" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="6" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="111" priority="7" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J148:Q148">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L147">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P147:Q147">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22987,11 +23032,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W14" sqref="W14"/>
+      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -23298,7 +23343,9 @@
       <c r="B4" s="22" t="s">
         <v>354</v>
       </c>
-      <c r="C4" s="15"/>
+      <c r="C4" s="15" t="s">
+        <v>967</v>
+      </c>
       <c r="D4" s="32"/>
       <c r="E4" s="15">
         <v>1</v>
@@ -23384,7 +23431,9 @@
       <c r="B5" s="22" t="s">
         <v>322</v>
       </c>
-      <c r="C5" s="15"/>
+      <c r="C5" s="15" t="s">
+        <v>968</v>
+      </c>
       <c r="D5" s="32"/>
       <c r="E5" s="15">
         <v>1</v>
@@ -23470,7 +23519,9 @@
       <c r="B6" s="22" t="s">
         <v>357</v>
       </c>
-      <c r="C6" s="15"/>
+      <c r="C6" s="15" t="s">
+        <v>969</v>
+      </c>
       <c r="D6" s="32"/>
       <c r="E6" s="15">
         <v>1</v>
@@ -23554,7 +23605,9 @@
       <c r="B7" s="22" t="s">
         <v>358</v>
       </c>
-      <c r="C7" s="15"/>
+      <c r="C7" s="15" t="s">
+        <v>970</v>
+      </c>
       <c r="D7" s="32"/>
       <c r="E7" s="15">
         <v>1</v>
@@ -23638,7 +23691,9 @@
       <c r="B8" s="22" t="s">
         <v>359</v>
       </c>
-      <c r="C8" s="15"/>
+      <c r="C8" s="15" t="s">
+        <v>974</v>
+      </c>
       <c r="D8" s="32"/>
       <c r="E8" s="15">
         <v>1</v>
@@ -23722,7 +23777,9 @@
       <c r="B9" s="22" t="s">
         <v>360</v>
       </c>
-      <c r="C9" s="15"/>
+      <c r="C9" s="15" t="s">
+        <v>975</v>
+      </c>
       <c r="D9" s="32"/>
       <c r="E9" s="15">
         <v>1</v>
@@ -23808,7 +23865,9 @@
       <c r="B10" s="22" t="s">
         <v>476</v>
       </c>
-      <c r="C10" s="15"/>
+      <c r="C10" s="15" t="s">
+        <v>976</v>
+      </c>
       <c r="D10" s="32"/>
       <c r="E10" s="15">
         <v>1</v>
@@ -23892,7 +23951,9 @@
       <c r="B11" s="22" t="s">
         <v>510</v>
       </c>
-      <c r="C11" s="15"/>
+      <c r="C11" s="15" t="s">
+        <v>971</v>
+      </c>
       <c r="D11" s="32"/>
       <c r="E11" s="15">
         <v>1</v>
@@ -23976,7 +24037,9 @@
       <c r="B12" s="22" t="s">
         <v>668</v>
       </c>
-      <c r="C12" s="15"/>
+      <c r="C12" s="15" t="s">
+        <v>977</v>
+      </c>
       <c r="D12" s="32"/>
       <c r="E12" s="15">
         <v>1</v>
@@ -24060,7 +24123,9 @@
       <c r="B13" s="22" t="s">
         <v>741</v>
       </c>
-      <c r="C13" s="15"/>
+      <c r="C13" s="15" t="s">
+        <v>972</v>
+      </c>
       <c r="D13" s="32"/>
       <c r="E13" s="15">
         <v>1</v>
@@ -24146,7 +24211,9 @@
       <c r="B14" s="22" t="s">
         <v>745</v>
       </c>
-      <c r="C14" s="15"/>
+      <c r="C14" s="15" t="s">
+        <v>978</v>
+      </c>
       <c r="D14" s="42"/>
       <c r="E14" s="15">
         <v>1</v>
@@ -24232,7 +24299,9 @@
       <c r="B15" s="22" t="s">
         <v>752</v>
       </c>
-      <c r="C15" s="15"/>
+      <c r="C15" s="15" t="s">
+        <v>973</v>
+      </c>
       <c r="D15" s="32"/>
       <c r="E15" s="15">
         <v>1</v>
@@ -24314,21 +24383,21 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="J4:O15">
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H15">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="2" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="70" priority="4" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25181,21 +25250,21 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="J4:P9">
-    <cfRule type="cellIs" dxfId="5" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="15" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H9">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="2" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
support cell spell now
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="标准" sheetId="1" r:id="rId1"/>
@@ -9497,11 +9497,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE148"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="U29" sqref="U29"/>
+      <selection pane="bottomRight" activeCell="X59" sqref="X59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -14887,7 +14887,9 @@
       <c r="W59" s="1" t="s">
         <v>880</v>
       </c>
-      <c r="X59" s="1"/>
+      <c r="X59" s="1">
+        <v>300</v>
+      </c>
       <c r="Y59" s="1" t="s">
         <v>78</v>
       </c>
@@ -23209,11 +23211,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="V10" sqref="V10"/>
+      <selection pane="bottomRight" activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -24208,7 +24210,9 @@
       <c r="W11" s="7" t="s">
         <v>507</v>
       </c>
-      <c r="X11" s="7"/>
+      <c r="X11" s="7">
+        <v>300</v>
+      </c>
       <c r="Y11" s="15" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
distinguish from the different spells for AI
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="标准" sheetId="1" r:id="rId1"/>
@@ -636,7 +636,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="980">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="979">
   <si>
     <t>慈悲</t>
   </si>
@@ -2474,10 +2474,6 @@
   </si>
   <si>
     <t>降低1.5卡片范围内所有单位{3:0}%生命上限</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>对2卡片距离内敌方单位造成{0}点魔法伤害</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -4991,7 +4987,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5123,9 +5119,6 @@
     </xf>
     <xf numFmtId="0" fontId="33" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -9497,11 +9490,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE148"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="D60" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="X59" sqref="X59"/>
+      <selection pane="bottomRight" activeCell="R62" sqref="R62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9573,7 +9566,7 @@
         <v>340</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="P1" s="17" t="s">
         <v>325</v>
@@ -9591,7 +9584,7 @@
         <v>368</v>
       </c>
       <c r="U1" s="13" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="V1" s="13" t="s">
         <v>338</v>
@@ -9600,7 +9593,7 @@
         <v>298</v>
       </c>
       <c r="X1" s="13" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="Y1" s="13" t="s">
         <v>367</v>
@@ -9618,7 +9611,7 @@
         <v>348</v>
       </c>
       <c r="AD1" s="23" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="AE1" s="23" t="s">
         <v>351</v>
@@ -9668,7 +9661,7 @@
         <v>341</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>326</v>
@@ -9686,7 +9679,7 @@
         <v>456</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>314</v>
@@ -9695,7 +9688,7 @@
         <v>176</v>
       </c>
       <c r="X2" s="10" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="Y2" s="4" t="s">
         <v>176</v>
@@ -9763,7 +9756,7 @@
         <v>342</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="P3" s="20" t="s">
         <v>327</v>
@@ -9781,7 +9774,7 @@
         <v>369</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="V3" s="6" t="s">
         <v>438</v>
@@ -9790,7 +9783,7 @@
         <v>508</v>
       </c>
       <c r="X3" s="6" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="Y3" s="6" t="s">
         <v>315</v>
@@ -9808,10 +9801,10 @@
         <v>349</v>
       </c>
       <c r="AD3" s="43" t="s">
+        <v>883</v>
+      </c>
+      <c r="AE3" s="43" t="s">
         <v>884</v>
-      </c>
-      <c r="AE3" s="43" t="s">
-        <v>885</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="60" x14ac:dyDescent="0.15">
@@ -9825,7 +9818,7 @@
         <v>208</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
@@ -9878,10 +9871,10 @@
         <v>95</v>
       </c>
       <c r="V4" s="11" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="W4" s="7" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="X4" s="7"/>
       <c r="Y4" s="1" t="s">
@@ -9913,7 +9906,7 @@
         <v>209</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -9966,7 +9959,7 @@
         <v>80</v>
       </c>
       <c r="V5" s="11" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="W5" s="7" t="s">
         <v>480</v>
@@ -10001,7 +9994,7 @@
         <v>210</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="E6" s="1">
         <v>2</v>
@@ -10054,7 +10047,7 @@
         <v>100</v>
       </c>
       <c r="V6" s="11" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="W6" s="7" t="s">
         <v>366</v>
@@ -10091,7 +10084,7 @@
         <v>211</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
@@ -10144,10 +10137,10 @@
         <v>100</v>
       </c>
       <c r="V7" s="11" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="W7" s="7" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="X7" s="7">
         <v>100</v>
@@ -10183,7 +10176,7 @@
         <v>212</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E8" s="1">
         <v>2</v>
@@ -10236,13 +10229,13 @@
         <v>100</v>
       </c>
       <c r="V8" s="11" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="W8" s="7" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="X8" s="7">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Y8" s="1"/>
       <c r="Z8" s="1" t="s">
@@ -10275,7 +10268,7 @@
         <v>289</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
@@ -10328,7 +10321,7 @@
         <v>90</v>
       </c>
       <c r="V9" s="11" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="W9" s="7" t="s">
         <v>447</v>
@@ -10363,7 +10356,7 @@
         <v>290</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -10416,7 +10409,7 @@
         <v>90</v>
       </c>
       <c r="V10" s="11" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="W10" s="7" t="s">
         <v>446</v>
@@ -10451,7 +10444,7 @@
         <v>291</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -10504,7 +10497,7 @@
         <v>90</v>
       </c>
       <c r="V11" s="11" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="W11" s="7" t="s">
         <v>448</v>
@@ -10539,7 +10532,7 @@
         <v>292</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
@@ -10592,7 +10585,7 @@
         <v>90</v>
       </c>
       <c r="V12" s="11" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="W12" s="7" t="s">
         <v>449</v>
@@ -10627,7 +10620,7 @@
         <v>213</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
@@ -10680,7 +10673,7 @@
         <v>90</v>
       </c>
       <c r="V13" s="11" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="W13" s="7" t="s">
         <v>450</v>
@@ -10715,7 +10708,7 @@
         <v>207</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
@@ -10768,7 +10761,7 @@
         <v>90</v>
       </c>
       <c r="V14" s="11" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="W14" s="7" t="s">
         <v>451</v>
@@ -10803,7 +10796,7 @@
         <v>214</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
@@ -10856,7 +10849,7 @@
         <v>90</v>
       </c>
       <c r="V15" s="11" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="W15" s="7" t="s">
         <v>452</v>
@@ -10891,7 +10884,7 @@
         <v>361</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E16" s="15">
         <v>4</v>
@@ -10944,7 +10937,7 @@
         <v>100</v>
       </c>
       <c r="V16" s="11" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="W16" s="7" t="s">
         <v>464</v>
@@ -10983,7 +10976,7 @@
         <v>442</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="E17" s="1">
         <v>2</v>
@@ -11036,13 +11029,13 @@
         <v>100</v>
       </c>
       <c r="V17" s="11" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="W17" s="7" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="X17" s="7">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Y17" s="1" t="s">
         <v>444</v>
@@ -11075,7 +11068,7 @@
         <v>215</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E18" s="1">
         <v>1</v>
@@ -11128,13 +11121,13 @@
         <v>75</v>
       </c>
       <c r="V18" s="11" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="W18" s="7" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="X18" s="7">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="Y18" s="1" t="s">
         <v>15</v>
@@ -11167,7 +11160,7 @@
         <v>216</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="E19" s="1">
         <v>3</v>
@@ -11220,10 +11213,10 @@
         <v>95</v>
       </c>
       <c r="V19" s="11" t="s">
+        <v>934</v>
+      </c>
+      <c r="W19" s="7" t="s">
         <v>935</v>
-      </c>
-      <c r="W19" s="7" t="s">
-        <v>936</v>
       </c>
       <c r="X19" s="7">
         <v>100</v>
@@ -11259,7 +11252,7 @@
         <v>217</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E20" s="1">
         <v>7</v>
@@ -11312,16 +11305,16 @@
         <v>100</v>
       </c>
       <c r="V20" s="11" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="W20" s="7" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="X20" s="7">
         <v>100</v>
       </c>
       <c r="Y20" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="Z20" s="1"/>
       <c r="AA20" s="1">
@@ -11351,7 +11344,7 @@
         <v>218</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="E21" s="1">
         <v>3</v>
@@ -11404,7 +11397,7 @@
         <v>102</v>
       </c>
       <c r="V21" s="11" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="W21" s="7" t="s">
         <v>512</v>
@@ -11443,7 +11436,7 @@
         <v>219</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E22" s="1">
         <v>4</v>
@@ -11490,19 +11483,19 @@
         <v>40</v>
       </c>
       <c r="S22" s="7" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="T22">
         <v>100</v>
       </c>
       <c r="V22" s="11" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="W22" s="7" t="s">
         <v>472</v>
       </c>
       <c r="X22" s="7">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Y22" s="1" t="s">
         <v>23</v>
@@ -11537,7 +11530,7 @@
         <v>220</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E23" s="1">
         <v>3</v>
@@ -11584,19 +11577,19 @@
         <v>60</v>
       </c>
       <c r="S23" s="7" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="T23">
         <v>100</v>
       </c>
       <c r="V23" s="11" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="W23" s="7" t="s">
         <v>470</v>
       </c>
       <c r="X23" s="7">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Y23" s="1" t="s">
         <v>471</v>
@@ -11631,7 +11624,7 @@
         <v>221</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E24" s="1">
         <v>2</v>
@@ -11678,19 +11671,19 @@
         <v>90</v>
       </c>
       <c r="S24" s="7" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="T24">
         <v>100</v>
       </c>
       <c r="V24" s="11" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="W24" s="7" t="s">
         <v>473</v>
       </c>
       <c r="X24" s="7">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Y24" s="1" t="s">
         <v>26</v>
@@ -11778,10 +11771,10 @@
         <v>107</v>
       </c>
       <c r="V25" s="11" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="W25" s="7" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="X25" s="7"/>
       <c r="Y25" s="1" t="s">
@@ -11868,7 +11861,7 @@
         <v>100</v>
       </c>
       <c r="V26" s="11" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="W26" s="21" t="s">
         <v>378</v>
@@ -11956,7 +11949,7 @@
         <v>90</v>
       </c>
       <c r="V27" s="11" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="W27" s="7" t="s">
         <v>379</v>
@@ -11993,7 +11986,7 @@
         <v>225</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="E28" s="1">
         <v>3</v>
@@ -12046,7 +12039,7 @@
         <v>100</v>
       </c>
       <c r="V28" s="11" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="W28" s="7" t="s">
         <v>466</v>
@@ -12085,7 +12078,7 @@
         <v>226</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E29" s="1">
         <v>4</v>
@@ -12132,16 +12125,16 @@
         <v>10</v>
       </c>
       <c r="S29" s="1" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="T29">
         <v>100</v>
       </c>
       <c r="U29" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="V29" s="11" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="W29" s="7" t="s">
         <v>465</v>
@@ -12178,7 +12171,7 @@
         <v>227</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="E30" s="1">
         <v>1</v>
@@ -12231,10 +12224,10 @@
         <v>96</v>
       </c>
       <c r="V30" s="11" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="W30" s="7" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="X30" s="7">
         <v>200</v>
@@ -12268,7 +12261,7 @@
         <v>228</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
@@ -12321,10 +12314,10 @@
         <v>96</v>
       </c>
       <c r="V31" s="11" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="W31" s="7" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="X31" s="7">
         <v>100</v>
@@ -12358,7 +12351,7 @@
         <v>229</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E32" s="1">
         <v>4</v>
@@ -12411,7 +12404,7 @@
         <v>100</v>
       </c>
       <c r="V32" s="11" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="W32" s="21" t="s">
         <v>335</v>
@@ -12501,10 +12494,10 @@
         <v>100</v>
       </c>
       <c r="V33" s="11" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="W33" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="X33" s="1"/>
       <c r="Y33" s="1" t="s">
@@ -12591,10 +12584,10 @@
         <v>100</v>
       </c>
       <c r="V34" s="11" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="W34" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="X34" s="7"/>
       <c r="Y34" s="1" t="s">
@@ -12628,7 +12621,7 @@
         <v>293</v>
       </c>
       <c r="D35" s="25" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E35" s="1">
         <v>3</v>
@@ -12681,10 +12674,10 @@
         <v>100</v>
       </c>
       <c r="U35" t="s">
+        <v>973</v>
+      </c>
+      <c r="V35" s="11" t="s">
         <v>974</v>
-      </c>
-      <c r="V35" s="11" t="s">
-        <v>975</v>
       </c>
       <c r="W35" s="7" t="s">
         <v>399</v>
@@ -12723,7 +12716,7 @@
         <v>294</v>
       </c>
       <c r="D36" s="25" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E36" s="1">
         <v>4</v>
@@ -12776,13 +12769,13 @@
         <v>100</v>
       </c>
       <c r="V36" s="11" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="W36" s="7" t="s">
         <v>344</v>
       </c>
       <c r="X36" s="7">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="Y36" s="1" t="s">
         <v>35</v>
@@ -12870,7 +12863,7 @@
         <v>100</v>
       </c>
       <c r="V37" s="11" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="W37" s="7" t="s">
         <v>347</v>
@@ -12907,7 +12900,7 @@
         <v>230</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E38" s="1">
         <v>3</v>
@@ -12960,13 +12953,13 @@
         <v>100</v>
       </c>
       <c r="V38" s="11" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="W38" s="7" t="s">
         <v>532</v>
       </c>
       <c r="X38" s="7">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Y38" s="1" t="s">
         <v>48</v>
@@ -13054,7 +13047,7 @@
         <v>100</v>
       </c>
       <c r="V39" s="11" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="W39" s="1" t="s">
         <v>528</v>
@@ -13091,7 +13084,7 @@
         <v>232</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="E40" s="1">
         <v>1</v>
@@ -13144,7 +13137,7 @@
         <v>100</v>
       </c>
       <c r="V40" s="11" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="W40" s="7" t="s">
         <v>467</v>
@@ -13181,7 +13174,7 @@
         <v>233</v>
       </c>
       <c r="D41" s="25" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E41" s="1">
         <v>2</v>
@@ -13228,19 +13221,19 @@
         <v>12</v>
       </c>
       <c r="S41" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="T41">
         <v>100</v>
       </c>
       <c r="V41" s="11" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="W41" s="7" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="X41" s="7">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="Y41" s="1" t="s">
         <v>54</v>
@@ -13328,10 +13321,10 @@
         <v>85</v>
       </c>
       <c r="V42" s="11" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="W42" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="X42" s="1"/>
       <c r="Y42" s="1" t="s">
@@ -13418,10 +13411,10 @@
         <v>100</v>
       </c>
       <c r="V43" s="11" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="W43" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="X43" s="1"/>
       <c r="Y43" s="1" t="s">
@@ -13452,7 +13445,7 @@
         <v>55</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="D44" s="25" t="s">
         <v>491</v>
@@ -13508,7 +13501,7 @@
         <v>100</v>
       </c>
       <c r="V44" s="11" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="W44" s="7" t="s">
         <v>492</v>
@@ -13545,7 +13538,7 @@
         <v>235</v>
       </c>
       <c r="D45" s="25" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E45" s="1">
         <v>3</v>
@@ -13598,13 +13591,13 @@
         <v>110</v>
       </c>
       <c r="V45" s="11" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="W45" s="7" t="s">
         <v>509</v>
       </c>
       <c r="X45" s="7">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Y45" s="1" t="s">
         <v>58</v>
@@ -13639,7 +13632,7 @@
         <v>236</v>
       </c>
       <c r="D46" s="25" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E46" s="1">
         <v>2</v>
@@ -13692,10 +13685,10 @@
         <v>100</v>
       </c>
       <c r="V46" s="11" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="W46" s="1" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="X46" s="1"/>
       <c r="Y46" s="1" t="s">
@@ -13782,10 +13775,10 @@
         <v>95</v>
       </c>
       <c r="V47" s="11" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="W47" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="X47" s="1"/>
       <c r="Y47" s="1" t="s">
@@ -13866,19 +13859,19 @@
         <v>100</v>
       </c>
       <c r="S48" s="7" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="T48">
         <v>100</v>
       </c>
       <c r="V48" s="11" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="W48" s="1" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="X48" s="1">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Y48" s="1" t="s">
         <v>316</v>
@@ -13911,7 +13904,7 @@
         <v>239</v>
       </c>
       <c r="D49" s="25" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E49" s="1">
         <v>5</v>
@@ -13964,7 +13957,7 @@
         <v>100</v>
       </c>
       <c r="V49" s="11" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="W49" s="7" t="s">
         <v>505</v>
@@ -14001,7 +13994,7 @@
         <v>240</v>
       </c>
       <c r="D50" s="25" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E50" s="1">
         <v>5</v>
@@ -14054,13 +14047,13 @@
         <v>100</v>
       </c>
       <c r="V50" s="11" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="W50" s="7" t="s">
-        <v>533</v>
+        <v>519</v>
       </c>
       <c r="X50" s="7">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Y50" s="1" t="s">
         <v>64</v>
@@ -14095,7 +14088,7 @@
         <v>241</v>
       </c>
       <c r="D51" s="25" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E51" s="1">
         <v>6</v>
@@ -14142,13 +14135,13 @@
         <v>0</v>
       </c>
       <c r="S51" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="T51">
         <v>100</v>
       </c>
       <c r="V51" s="11" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="W51" s="1" t="s">
         <v>517</v>
@@ -14187,7 +14180,7 @@
         <v>242</v>
       </c>
       <c r="D52" s="25" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E52" s="1">
         <v>2</v>
@@ -14240,13 +14233,13 @@
         <v>100</v>
       </c>
       <c r="V52" s="11" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="W52" s="7" t="s">
         <v>514</v>
       </c>
       <c r="X52" s="7">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Y52" s="1" t="s">
         <v>67</v>
@@ -14281,7 +14274,7 @@
         <v>243</v>
       </c>
       <c r="D53" s="25" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E53" s="1">
         <v>4</v>
@@ -14334,7 +14327,7 @@
         <v>95</v>
       </c>
       <c r="V53" s="11" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="W53" s="7" t="s">
         <v>504</v>
@@ -14371,7 +14364,7 @@
         <v>244</v>
       </c>
       <c r="D54" s="25" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="E54" s="1">
         <v>3</v>
@@ -14424,13 +14417,13 @@
         <v>100</v>
       </c>
       <c r="V54" s="11" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="W54" s="1" t="s">
         <v>515</v>
       </c>
       <c r="X54" s="7">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Y54" s="1" t="s">
         <v>71</v>
@@ -14465,7 +14458,7 @@
         <v>525</v>
       </c>
       <c r="D55" s="25" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E55" s="1">
         <v>1</v>
@@ -14512,16 +14505,16 @@
         <v>0</v>
       </c>
       <c r="S55" s="1" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="T55">
         <v>95</v>
       </c>
       <c r="V55" s="11" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="W55" s="7" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="X55" s="7"/>
       <c r="Y55" s="1" t="s">
@@ -14555,7 +14548,7 @@
         <v>245</v>
       </c>
       <c r="D56" s="25" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E56" s="1">
         <v>3</v>
@@ -14608,7 +14601,7 @@
         <v>100</v>
       </c>
       <c r="V56" s="11" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="W56" s="7" t="s">
         <v>519</v>
@@ -14647,7 +14640,7 @@
         <v>194</v>
       </c>
       <c r="D57" s="25" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E57" s="1">
         <v>3</v>
@@ -14700,7 +14693,7 @@
         <v>100</v>
       </c>
       <c r="V57" s="11" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="W57" s="7" t="s">
         <v>516</v>
@@ -14739,7 +14732,7 @@
         <v>246</v>
       </c>
       <c r="D58" s="25" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E58" s="1">
         <v>4</v>
@@ -14792,10 +14785,10 @@
         <v>100</v>
       </c>
       <c r="V58" s="11" t="s">
+        <v>899</v>
+      </c>
+      <c r="W58" s="1" t="s">
         <v>900</v>
-      </c>
-      <c r="W58" s="1" t="s">
-        <v>901</v>
       </c>
       <c r="X58" s="1"/>
       <c r="Y58" s="1" t="s">
@@ -14876,16 +14869,16 @@
         <v>0</v>
       </c>
       <c r="S59" s="15" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="T59">
         <v>100</v>
       </c>
       <c r="V59" s="11" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="W59" s="1" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="X59" s="1">
         <v>300</v>
@@ -14974,13 +14967,13 @@
         <v>100</v>
       </c>
       <c r="V60" s="11" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="W60" s="1" t="s">
         <v>479</v>
       </c>
       <c r="X60" s="1">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="Y60" s="1" t="s">
         <v>477</v>
@@ -15060,16 +15053,16 @@
         <v>0</v>
       </c>
       <c r="S61" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="T61">
         <v>100</v>
       </c>
       <c r="V61" s="11" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="W61" s="7" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="X61" s="7"/>
       <c r="Y61" s="1" t="s">
@@ -15103,7 +15096,7 @@
         <v>248</v>
       </c>
       <c r="D62" s="25" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E62" s="1">
         <v>2</v>
@@ -15156,10 +15149,10 @@
         <v>100</v>
       </c>
       <c r="V62" s="11" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="W62" s="7" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="X62" s="7">
         <v>200</v>
@@ -15195,7 +15188,7 @@
         <v>249</v>
       </c>
       <c r="D63" s="25" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E63" s="1">
         <v>1</v>
@@ -15248,7 +15241,7 @@
         <v>100</v>
       </c>
       <c r="V63" s="11" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="W63" s="1" t="s">
         <v>380</v>
@@ -15287,7 +15280,7 @@
         <v>250</v>
       </c>
       <c r="D64" s="25" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E64" s="1">
         <v>4</v>
@@ -15340,13 +15333,13 @@
         <v>100</v>
       </c>
       <c r="V64" s="11" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="W64" s="7" t="s">
         <v>345</v>
       </c>
       <c r="X64" s="7">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="Y64" s="1" t="s">
         <v>15</v>
@@ -15379,7 +15372,7 @@
         <v>251</v>
       </c>
       <c r="D65" s="25" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E65" s="1">
         <v>1</v>
@@ -15432,7 +15425,7 @@
         <v>100</v>
       </c>
       <c r="V65" s="11" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="W65" s="7" t="s">
         <v>329</v>
@@ -15524,7 +15517,7 @@
         <v>100</v>
       </c>
       <c r="V66" s="11" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="W66" s="7" t="s">
         <v>482</v>
@@ -15608,16 +15601,16 @@
         <v>10</v>
       </c>
       <c r="S67" s="1" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="T67">
         <v>100</v>
       </c>
       <c r="V67" s="11" t="s">
+        <v>908</v>
+      </c>
+      <c r="W67" s="7" t="s">
         <v>909</v>
-      </c>
-      <c r="W67" s="7" t="s">
-        <v>910</v>
       </c>
       <c r="X67" s="7"/>
       <c r="Y67" s="1" t="s">
@@ -15653,7 +15646,7 @@
         <v>196</v>
       </c>
       <c r="D68" s="25" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E68" s="1">
         <v>6</v>
@@ -15706,7 +15699,7 @@
         <v>100</v>
       </c>
       <c r="V68" s="11" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="W68" s="1" t="s">
         <v>386</v>
@@ -15796,10 +15789,10 @@
         <v>85</v>
       </c>
       <c r="V69" s="11" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="W69" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="X69" s="1"/>
       <c r="Y69" s="1" t="s">
@@ -15833,7 +15826,7 @@
         <v>255</v>
       </c>
       <c r="D70" s="25" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="E70" s="1">
         <v>3</v>
@@ -15886,10 +15879,10 @@
         <v>100</v>
       </c>
       <c r="V70" s="11" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="W70" s="7" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="X70" s="7">
         <v>100</v>
@@ -15925,7 +15918,7 @@
         <v>256</v>
       </c>
       <c r="D71" s="25" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="E71" s="1">
         <v>2</v>
@@ -15978,13 +15971,13 @@
         <v>100</v>
       </c>
       <c r="V71" s="11" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="W71" s="7" t="s">
         <v>486</v>
       </c>
       <c r="X71" s="7">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Y71" s="1" t="s">
         <v>96</v>
@@ -16019,7 +16012,7 @@
         <v>199</v>
       </c>
       <c r="D72" s="25" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E72" s="1">
         <v>2</v>
@@ -16072,16 +16065,16 @@
         <v>100</v>
       </c>
       <c r="V72" s="11" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="W72" s="7" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="X72" s="7">
         <v>100</v>
       </c>
       <c r="Y72" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="Z72" s="1"/>
       <c r="AA72" s="1">
@@ -16111,7 +16104,7 @@
         <v>201</v>
       </c>
       <c r="D73" s="25" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E73" s="1">
         <v>2</v>
@@ -16164,7 +16157,7 @@
         <v>100</v>
       </c>
       <c r="V73" s="11" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="W73" s="7" t="s">
         <v>487</v>
@@ -16203,7 +16196,7 @@
         <v>198</v>
       </c>
       <c r="D74" s="25" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="E74" s="1">
         <v>4</v>
@@ -16256,13 +16249,13 @@
         <v>103</v>
       </c>
       <c r="V74" s="11" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="W74" s="7" t="s">
         <v>496</v>
       </c>
       <c r="X74" s="7">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Y74" s="1" t="s">
         <v>102</v>
@@ -16297,7 +16290,7 @@
         <v>257</v>
       </c>
       <c r="D75" s="25" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E75" s="1">
         <v>3</v>
@@ -16350,7 +16343,7 @@
         <v>102</v>
       </c>
       <c r="V75" s="11" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="W75" s="1" t="s">
         <v>495</v>
@@ -16389,7 +16382,7 @@
         <v>258</v>
       </c>
       <c r="D76" s="25" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="E76" s="1">
         <v>3</v>
@@ -16442,7 +16435,7 @@
         <v>100</v>
       </c>
       <c r="V76" s="11" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="W76" s="7" t="s">
         <v>463</v>
@@ -16479,7 +16472,7 @@
         <v>295</v>
       </c>
       <c r="D77" s="25" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E77" s="1">
         <v>3</v>
@@ -16532,10 +16525,10 @@
         <v>103</v>
       </c>
       <c r="V77" s="11" t="s">
+        <v>897</v>
+      </c>
+      <c r="W77" s="7" t="s">
         <v>898</v>
-      </c>
-      <c r="W77" s="7" t="s">
-        <v>899</v>
       </c>
       <c r="X77" s="7">
         <v>100</v>
@@ -16571,7 +16564,7 @@
         <v>259</v>
       </c>
       <c r="D78" s="25" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E78" s="1">
         <v>4</v>
@@ -16624,7 +16617,7 @@
         <v>95</v>
       </c>
       <c r="V78" s="11" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="W78" s="7" t="s">
         <v>330</v>
@@ -16663,7 +16656,7 @@
         <v>260</v>
       </c>
       <c r="D79" s="25" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E79" s="1">
         <v>3</v>
@@ -16716,13 +16709,13 @@
         <v>100</v>
       </c>
       <c r="V79" s="11" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="W79" s="7" t="s">
         <v>488</v>
       </c>
       <c r="X79" s="7">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Y79" s="1" t="s">
         <v>112</v>
@@ -16757,7 +16750,7 @@
         <v>261</v>
       </c>
       <c r="D80" s="25" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E80" s="1">
         <v>3</v>
@@ -16810,7 +16803,7 @@
         <v>107</v>
       </c>
       <c r="V80" s="11" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="W80" s="7" t="s">
         <v>331</v>
@@ -16847,7 +16840,7 @@
         <v>262</v>
       </c>
       <c r="D81" s="25" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E81" s="1">
         <v>1</v>
@@ -16900,10 +16893,10 @@
         <v>100</v>
       </c>
       <c r="V81" s="37" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="W81" s="7" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="X81" s="7"/>
       <c r="Y81" s="1" t="s">
@@ -16935,7 +16928,7 @@
         <v>263</v>
       </c>
       <c r="D82" s="25" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E82" s="1">
         <v>3</v>
@@ -16988,13 +16981,13 @@
         <v>100</v>
       </c>
       <c r="V82" s="11" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="W82" s="7" t="s">
         <v>489</v>
       </c>
       <c r="X82" s="7">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="Y82" s="1" t="s">
         <v>116</v>
@@ -17029,7 +17022,7 @@
         <v>264</v>
       </c>
       <c r="D83" s="25" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E83" s="1">
         <v>2</v>
@@ -17076,19 +17069,19 @@
         <v>30</v>
       </c>
       <c r="S83" s="7" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="T83">
         <v>100</v>
       </c>
       <c r="V83" s="11" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="W83" s="7" t="s">
         <v>510</v>
       </c>
       <c r="X83" s="7">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Y83" s="1" t="s">
         <v>80</v>
@@ -17123,7 +17116,7 @@
         <v>265</v>
       </c>
       <c r="D84" s="25" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E84" s="1">
         <v>2</v>
@@ -17170,19 +17163,19 @@
         <v>30</v>
       </c>
       <c r="S84" s="7" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="T84">
         <v>100</v>
       </c>
       <c r="V84" s="11" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="W84" s="7" t="s">
         <v>511</v>
       </c>
       <c r="X84" s="7">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Y84" s="1" t="s">
         <v>50</v>
@@ -17217,7 +17210,7 @@
         <v>266</v>
       </c>
       <c r="D85" s="25" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="E85" s="1">
         <v>3</v>
@@ -17270,13 +17263,13 @@
         <v>100</v>
       </c>
       <c r="V85" s="11" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="W85" s="7" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="X85" s="7">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="Y85" s="1" t="s">
         <v>121</v>
@@ -17306,10 +17299,10 @@
         <v>159</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="D86" s="25" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E86" s="1">
         <v>3</v>
@@ -17362,14 +17355,14 @@
         <v>100</v>
       </c>
       <c r="V86" s="11" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="W86" s="7" t="s">
         <v>490</v>
       </c>
       <c r="X86" s="7"/>
       <c r="Y86" s="1" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="Z86" s="1"/>
       <c r="AA86" s="1">
@@ -17452,17 +17445,17 @@
         <v>100</v>
       </c>
       <c r="V87" s="11" t="s">
+        <v>892</v>
+      </c>
+      <c r="W87" s="7" t="s">
         <v>893</v>
-      </c>
-      <c r="W87" s="7" t="s">
-        <v>894</v>
       </c>
       <c r="X87" s="7"/>
       <c r="Y87" s="1" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="Z87" s="1" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="AA87" s="1">
         <v>11000008</v>
@@ -17491,7 +17484,7 @@
         <v>202</v>
       </c>
       <c r="D88" s="25" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E88" s="1">
         <v>3</v>
@@ -17538,26 +17531,26 @@
         <v>20</v>
       </c>
       <c r="S88" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="T88">
         <v>100</v>
       </c>
       <c r="U88" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="V88" s="11" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="W88" s="7" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="X88" s="7"/>
       <c r="Y88" s="1" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="Z88" s="1" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="AA88" s="1">
         <v>11000009</v>
@@ -17586,7 +17579,7 @@
         <v>203</v>
       </c>
       <c r="D89" s="25" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E89" s="1">
         <v>2</v>
@@ -17639,13 +17632,13 @@
         <v>102</v>
       </c>
       <c r="V89" s="11" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="W89" s="7" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="X89" s="7">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="Y89" s="1" t="s">
         <v>2</v>
@@ -17678,7 +17671,7 @@
         <v>204</v>
       </c>
       <c r="D90" s="25" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="E90" s="1">
         <v>3</v>
@@ -17725,13 +17718,13 @@
         <v>40</v>
       </c>
       <c r="S90" s="7" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="T90">
         <v>100</v>
       </c>
       <c r="V90" s="11" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="W90" s="7" t="s">
         <v>513</v>
@@ -17772,7 +17765,7 @@
         <v>267</v>
       </c>
       <c r="D91" s="25" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E91" s="1">
         <v>4</v>
@@ -17825,13 +17818,13 @@
         <v>100</v>
       </c>
       <c r="V91" s="11" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="W91" s="7" t="s">
         <v>332</v>
       </c>
       <c r="X91" s="7">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Y91" s="1" t="s">
         <v>127</v>
@@ -17866,7 +17859,7 @@
         <v>268</v>
       </c>
       <c r="D92" s="25" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E92" s="1">
         <v>4</v>
@@ -17919,13 +17912,13 @@
         <v>100</v>
       </c>
       <c r="V92" s="11" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="W92" s="7" t="s">
         <v>503</v>
       </c>
       <c r="X92" s="7">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Y92" s="1" t="s">
         <v>437</v>
@@ -18013,7 +18006,7 @@
         <v>100</v>
       </c>
       <c r="V93" s="11" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="W93" s="1" t="s">
         <v>346</v>
@@ -18050,7 +18043,7 @@
         <v>269</v>
       </c>
       <c r="D94" s="25" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E94" s="1">
         <v>2</v>
@@ -18103,13 +18096,13 @@
         <v>100</v>
       </c>
       <c r="V94" s="11" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="W94" s="7" t="s">
         <v>333</v>
       </c>
       <c r="X94" s="7">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="Y94" s="1" t="s">
         <v>131</v>
@@ -18136,13 +18129,13 @@
         <v>53000092</v>
       </c>
       <c r="B95" s="8" t="s">
+        <v>533</v>
+      </c>
+      <c r="C95" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="C95" s="1" t="s">
-        <v>535</v>
-      </c>
       <c r="D95" s="25" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E95" s="1">
         <v>5</v>
@@ -18189,20 +18182,20 @@
         <v>0</v>
       </c>
       <c r="S95" s="7" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="T95">
         <v>100</v>
       </c>
       <c r="V95" s="11" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="W95" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="X95" s="1"/>
       <c r="Y95" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="Z95" s="1"/>
       <c r="AA95" s="1">
@@ -18232,7 +18225,7 @@
         <v>270</v>
       </c>
       <c r="D96" s="25" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E96" s="1">
         <v>2</v>
@@ -18285,7 +18278,7 @@
         <v>100</v>
       </c>
       <c r="V96" s="11" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="W96" s="7" t="s">
         <v>502</v>
@@ -18377,7 +18370,7 @@
         <v>100</v>
       </c>
       <c r="V97" s="11" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="W97" s="1" t="s">
         <v>483</v>
@@ -18414,7 +18407,7 @@
         <v>272</v>
       </c>
       <c r="D98" s="25" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E98" s="1">
         <v>2</v>
@@ -18467,13 +18460,13 @@
         <v>100</v>
       </c>
       <c r="V98" s="11" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="W98" s="7" t="s">
         <v>520</v>
       </c>
       <c r="X98" s="7">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="Y98" s="1" t="s">
         <v>137</v>
@@ -18508,7 +18501,7 @@
         <v>273</v>
       </c>
       <c r="D99" s="25" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="E99" s="1">
         <v>1</v>
@@ -18561,7 +18554,7 @@
         <v>104</v>
       </c>
       <c r="V99" s="11" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="W99" s="1" t="s">
         <v>498</v>
@@ -18598,7 +18591,7 @@
         <v>274</v>
       </c>
       <c r="D100" s="25" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E100" s="1">
         <v>2</v>
@@ -18651,13 +18644,13 @@
         <v>100</v>
       </c>
       <c r="V100" s="11" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="W100" s="7" t="s">
         <v>500</v>
       </c>
       <c r="X100" s="7">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Y100" s="1" t="s">
         <v>80</v>
@@ -18743,7 +18736,7 @@
         <v>100</v>
       </c>
       <c r="V101" s="11" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="W101" s="7" t="s">
         <v>385</v>
@@ -18780,7 +18773,7 @@
         <v>275</v>
       </c>
       <c r="D102" s="25" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E102" s="1">
         <v>2</v>
@@ -18833,7 +18826,7 @@
         <v>100</v>
       </c>
       <c r="V102" s="11" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="W102" s="7" t="s">
         <v>501</v>
@@ -18872,7 +18865,7 @@
         <v>276</v>
       </c>
       <c r="D103" s="25" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="E103" s="1">
         <v>4</v>
@@ -18925,10 +18918,10 @@
         <v>100</v>
       </c>
       <c r="V103" s="11" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="W103" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="X103" s="1"/>
       <c r="Y103" s="1" t="s">
@@ -18962,7 +18955,7 @@
         <v>287</v>
       </c>
       <c r="D104" s="25" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E104" s="1">
         <v>3</v>
@@ -19015,13 +19008,13 @@
         <v>100</v>
       </c>
       <c r="V104" s="11" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="W104" s="1" t="s">
         <v>522</v>
       </c>
       <c r="X104" s="1">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="Y104" s="1" t="s">
         <v>165</v>
@@ -19054,7 +19047,7 @@
         <v>277</v>
       </c>
       <c r="D105" s="25" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E105" s="1">
         <v>1</v>
@@ -19107,7 +19100,7 @@
         <v>100</v>
       </c>
       <c r="V105" s="11" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="W105" s="7" t="s">
         <v>334</v>
@@ -19146,7 +19139,7 @@
         <v>278</v>
       </c>
       <c r="D106" s="25" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E106" s="1">
         <v>3</v>
@@ -19199,13 +19192,13 @@
         <v>105</v>
       </c>
       <c r="V106" s="11" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="W106" s="7" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="X106" s="7">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="Y106" s="1" t="s">
         <v>145</v>
@@ -19240,7 +19233,7 @@
         <v>279</v>
       </c>
       <c r="D107" s="25" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E107" s="1">
         <v>3</v>
@@ -19293,13 +19286,13 @@
         <v>105</v>
       </c>
       <c r="V107" s="11" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="W107" s="7" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="X107" s="7">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Y107" s="1" t="s">
         <v>147</v>
@@ -19332,7 +19325,7 @@
         <v>206</v>
       </c>
       <c r="D108" s="25" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E108" s="1">
         <v>3</v>
@@ -19383,10 +19376,10 @@
         <v>100</v>
       </c>
       <c r="V108" s="11" t="s">
+        <v>906</v>
+      </c>
+      <c r="W108" s="1" t="s">
         <v>907</v>
-      </c>
-      <c r="W108" s="1" t="s">
-        <v>908</v>
       </c>
       <c r="X108" s="7">
         <v>100</v>
@@ -19422,7 +19415,7 @@
         <v>280</v>
       </c>
       <c r="D109" s="25" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E109" s="1">
         <v>1</v>
@@ -19475,10 +19468,10 @@
         <v>100</v>
       </c>
       <c r="V109" s="11" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="W109" s="7" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="X109" s="7">
         <v>200</v>
@@ -19514,7 +19507,7 @@
         <v>281</v>
       </c>
       <c r="D110" s="25" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E110" s="1">
         <v>1</v>
@@ -19567,13 +19560,13 @@
         <v>100</v>
       </c>
       <c r="V110" s="11" t="s">
+        <v>929</v>
+      </c>
+      <c r="W110" s="7" t="s">
         <v>930</v>
       </c>
-      <c r="W110" s="7" t="s">
-        <v>931</v>
-      </c>
       <c r="X110" s="7">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Y110" s="1" t="s">
         <v>153</v>
@@ -19608,7 +19601,7 @@
         <v>282</v>
       </c>
       <c r="D111" s="25" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E111" s="1">
         <v>2</v>
@@ -19661,7 +19654,7 @@
         <v>100</v>
       </c>
       <c r="V111" s="11" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="W111" s="7" t="s">
         <v>494</v>
@@ -19700,7 +19693,7 @@
         <v>283</v>
       </c>
       <c r="D112" s="25" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E112" s="1">
         <v>2</v>
@@ -19753,13 +19746,13 @@
         <v>100</v>
       </c>
       <c r="V112" s="11" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="W112" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="X112" s="7">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="Y112" s="1" t="s">
         <v>157</v>
@@ -19845,10 +19838,10 @@
         <v>103</v>
       </c>
       <c r="V113" s="11" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="W113" s="7" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="X113" s="7"/>
       <c r="Y113" s="1" t="s">
@@ -19876,13 +19869,13 @@
         <v>53000111</v>
       </c>
       <c r="B114" s="8" t="s">
+        <v>548</v>
+      </c>
+      <c r="C114" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="C114" s="1" t="s">
-        <v>550</v>
-      </c>
       <c r="D114" s="25" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E114" s="1">
         <v>3</v>
@@ -19929,25 +19922,25 @@
         <v>20</v>
       </c>
       <c r="S114" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="T114">
         <v>100</v>
       </c>
       <c r="V114" s="11" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="W114" s="7" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="X114" s="7">
         <v>100</v>
       </c>
       <c r="Y114" s="1" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="Z114" s="1" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="AA114" s="1">
         <v>11000007</v>
@@ -19970,13 +19963,13 @@
         <v>53000112</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="D115" s="25" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E115" s="1">
         <v>3</v>
@@ -20029,20 +20022,20 @@
         <v>100</v>
       </c>
       <c r="U115" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="V115" s="11" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="W115" s="7" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="X115" s="7"/>
       <c r="Y115" s="1" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="Z115" s="1" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="AA115" s="1">
         <v>11000009</v>
@@ -20065,10 +20058,10 @@
         <v>53000113</v>
       </c>
       <c r="B116" s="8" t="s">
+        <v>581</v>
+      </c>
+      <c r="C116" s="1" t="s">
         <v>582</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>583</v>
       </c>
       <c r="D116" s="25"/>
       <c r="E116" s="1">
@@ -20116,25 +20109,25 @@
         <v>0</v>
       </c>
       <c r="S116" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="T116">
         <v>100</v>
       </c>
       <c r="V116" s="11" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="W116" s="7" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="X116" s="7">
         <v>100</v>
       </c>
       <c r="Y116" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="Z116" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="AA116" s="1">
         <v>11000003</v>
@@ -20157,10 +20150,10 @@
         <v>53000114</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D117" s="25"/>
       <c r="E117" s="1">
@@ -20208,16 +20201,16 @@
         <v>0</v>
       </c>
       <c r="S117" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="T117">
         <v>101</v>
       </c>
       <c r="V117" s="11" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="W117" s="7" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="X117" s="7">
         <v>100</v>
@@ -20249,10 +20242,10 @@
         <v>53000115</v>
       </c>
       <c r="B118" s="8" t="s">
+        <v>591</v>
+      </c>
+      <c r="C118" s="1" t="s">
         <v>592</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>593</v>
       </c>
       <c r="D118" s="25"/>
       <c r="E118" s="1">
@@ -20300,19 +20293,19 @@
         <v>0</v>
       </c>
       <c r="S118" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="T118">
         <v>100</v>
       </c>
       <c r="V118" s="11" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="W118" s="7" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="X118" s="7">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="Y118" s="1" t="s">
         <v>98</v>
@@ -20341,13 +20334,13 @@
         <v>53000116</v>
       </c>
       <c r="B119" s="8" t="s">
+        <v>596</v>
+      </c>
+      <c r="C119" s="1" t="s">
         <v>597</v>
       </c>
-      <c r="C119" s="1" t="s">
-        <v>598</v>
-      </c>
       <c r="D119" s="25" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="E119" s="1">
         <v>2</v>
@@ -20400,10 +20393,10 @@
         <v>101</v>
       </c>
       <c r="V119" s="11" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="W119" s="7" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="X119" s="7">
         <v>100</v>
@@ -20435,13 +20428,13 @@
         <v>53000117</v>
       </c>
       <c r="B120" s="8" t="s">
+        <v>598</v>
+      </c>
+      <c r="C120" s="1" t="s">
         <v>599</v>
       </c>
-      <c r="C120" s="1" t="s">
-        <v>600</v>
-      </c>
       <c r="D120" s="25" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E120" s="1">
         <v>1</v>
@@ -20488,16 +20481,16 @@
         <v>0</v>
       </c>
       <c r="S120" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="T120">
         <v>100</v>
       </c>
       <c r="V120" s="11" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="W120" s="7" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="X120" s="7">
         <v>200</v>
@@ -20529,10 +20522,10 @@
         <v>53000118</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D121" s="25"/>
       <c r="E121" s="1">
@@ -20580,23 +20573,23 @@
         <v>0</v>
       </c>
       <c r="S121" s="1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="T121">
         <v>100</v>
       </c>
       <c r="V121" s="11" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="W121" s="7" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="X121" s="7"/>
       <c r="Y121" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="Z121" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AA121" s="1">
         <v>11000003</v>
@@ -20619,10 +20612,10 @@
         <v>53000119</v>
       </c>
       <c r="B122" s="8" t="s">
+        <v>616</v>
+      </c>
+      <c r="C122" s="1" t="s">
         <v>617</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>618</v>
       </c>
       <c r="D122" s="25"/>
       <c r="E122" s="1">
@@ -20670,25 +20663,25 @@
         <v>0</v>
       </c>
       <c r="S122" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="T122">
         <v>105</v>
       </c>
       <c r="V122" s="11" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="W122" s="7" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="X122" s="7">
         <v>100</v>
       </c>
       <c r="Y122" s="1" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="Z122" s="1" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="AA122" s="1">
         <v>11000003</v>
@@ -20711,13 +20704,13 @@
         <v>53000120</v>
       </c>
       <c r="B123" s="22" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C123" s="15" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D123" s="25" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E123" s="15">
         <v>1</v>
@@ -20771,10 +20764,10 @@
       </c>
       <c r="U123" s="15"/>
       <c r="V123" s="11" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="W123" s="7" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="X123" s="7">
         <v>200</v>
@@ -20804,13 +20797,13 @@
         <v>53000121</v>
       </c>
       <c r="B124" s="22" t="s">
+        <v>624</v>
+      </c>
+      <c r="C124" s="15" t="s">
         <v>625</v>
       </c>
-      <c r="C124" s="15" t="s">
-        <v>626</v>
-      </c>
       <c r="D124" s="25" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="E124" s="15">
         <v>1</v>
@@ -20857,25 +20850,25 @@
         <v>30</v>
       </c>
       <c r="S124" s="7" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="T124">
         <v>100</v>
       </c>
       <c r="V124" s="11" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="W124" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="X124" s="7">
+        <v>102</v>
+      </c>
+      <c r="Y124" s="15" t="s">
         <v>628</v>
       </c>
-      <c r="X124" s="7">
-        <v>100</v>
-      </c>
-      <c r="Y124" s="15" t="s">
-        <v>629</v>
-      </c>
       <c r="Z124" s="15" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AA124" s="1">
         <v>11000001</v>
@@ -20898,13 +20891,13 @@
         <v>53000122</v>
       </c>
       <c r="B125" s="22" t="s">
+        <v>629</v>
+      </c>
+      <c r="C125" s="15" t="s">
         <v>630</v>
       </c>
-      <c r="C125" s="15" t="s">
-        <v>631</v>
-      </c>
       <c r="D125" s="25" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="E125" s="15">
         <v>1</v>
@@ -20951,28 +20944,28 @@
         <v>0</v>
       </c>
       <c r="S125" s="7" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="T125">
         <v>101</v>
       </c>
       <c r="U125" s="11" t="s">
+        <v>970</v>
+      </c>
+      <c r="V125" s="11" t="s">
         <v>971</v>
       </c>
-      <c r="V125" s="11" t="s">
-        <v>972</v>
-      </c>
       <c r="W125" s="1" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="X125" s="7">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="Y125" s="15" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="Z125" s="15" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AA125" s="1">
         <v>11000001</v>
@@ -20995,13 +20988,13 @@
         <v>53000123</v>
       </c>
       <c r="B126" s="22" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C126" s="15" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D126" s="25" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E126" s="15">
         <v>1</v>
@@ -21048,25 +21041,25 @@
         <v>0</v>
       </c>
       <c r="S126" s="7" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="T126">
         <v>100</v>
       </c>
       <c r="V126" s="11" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="W126" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="X126" s="7">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="Y126" s="15" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="Z126" s="15" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AA126" s="1">
         <v>11000001</v>
@@ -21089,13 +21082,13 @@
         <v>53000124</v>
       </c>
       <c r="B127" s="22" t="s">
+        <v>638</v>
+      </c>
+      <c r="C127" s="15" t="s">
         <v>639</v>
       </c>
-      <c r="C127" s="15" t="s">
+      <c r="D127" s="25" t="s">
         <v>640</v>
-      </c>
-      <c r="D127" s="25" t="s">
-        <v>641</v>
       </c>
       <c r="E127" s="15">
         <v>2</v>
@@ -21142,25 +21135,25 @@
         <v>0</v>
       </c>
       <c r="S127" s="7" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="T127">
         <v>101</v>
       </c>
       <c r="V127" s="11" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="W127" s="1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="X127" s="1">
         <v>200</v>
       </c>
       <c r="Y127" s="15" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="Z127" s="15" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="AA127" s="1">
         <v>11000001</v>
@@ -21183,13 +21176,13 @@
         <v>53000125</v>
       </c>
       <c r="B128" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="C128" s="15" t="s">
         <v>644</v>
       </c>
-      <c r="C128" s="15" t="s">
+      <c r="D128" s="25" t="s">
         <v>645</v>
-      </c>
-      <c r="D128" s="25" t="s">
-        <v>646</v>
       </c>
       <c r="E128" s="15">
         <v>2</v>
@@ -21236,25 +21229,25 @@
         <v>0</v>
       </c>
       <c r="S128" s="7" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="T128">
         <v>100</v>
       </c>
       <c r="V128" s="11" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="W128" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="X128" s="7">
         <v>100</v>
       </c>
       <c r="Y128" s="15" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="Z128" s="15" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="AA128" s="1">
         <v>11000002</v>
@@ -21277,10 +21270,10 @@
         <v>53000126</v>
       </c>
       <c r="B129" s="22" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="C129" s="15" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="D129" s="25"/>
       <c r="E129" s="15">
@@ -21328,23 +21321,23 @@
         <v>0</v>
       </c>
       <c r="S129" s="7" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="T129">
         <v>100</v>
       </c>
       <c r="V129" s="11" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="W129" s="1" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="X129" s="1"/>
       <c r="Y129" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="Z129" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AA129" s="1">
         <v>11000001</v>
@@ -21367,13 +21360,13 @@
         <v>53000127</v>
       </c>
       <c r="B130" s="22" t="s">
+        <v>652</v>
+      </c>
+      <c r="C130" s="15" t="s">
         <v>653</v>
       </c>
-      <c r="C130" s="15" t="s">
-        <v>654</v>
-      </c>
       <c r="D130" s="25" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="E130" s="15">
         <v>2</v>
@@ -21420,25 +21413,25 @@
         <v>15</v>
       </c>
       <c r="S130" s="7" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="T130">
         <v>103</v>
       </c>
       <c r="V130" s="11" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="W130" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="X130" s="7">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Y130" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="Z130" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AA130" s="1">
         <v>11000001</v>
@@ -21461,13 +21454,13 @@
         <v>53000128</v>
       </c>
       <c r="B131" s="22" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D131" s="25" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E131" s="15">
         <v>1</v>
@@ -21514,25 +21507,25 @@
         <v>25</v>
       </c>
       <c r="S131" s="7" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="T131">
         <v>100</v>
       </c>
       <c r="V131" s="11" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="W131" s="1" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="X131" s="1">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="Y131" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="Z131" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="AA131" s="1">
         <v>11000001</v>
@@ -21555,13 +21548,13 @@
         <v>53000129</v>
       </c>
       <c r="B132" s="22" t="s">
+        <v>670</v>
+      </c>
+      <c r="C132" s="15" t="s">
+        <v>669</v>
+      </c>
+      <c r="D132" s="25" t="s">
         <v>671</v>
-      </c>
-      <c r="C132" s="15" t="s">
-        <v>670</v>
-      </c>
-      <c r="D132" s="25" t="s">
-        <v>672</v>
       </c>
       <c r="E132" s="15">
         <v>3</v>
@@ -21608,25 +21601,25 @@
         <v>0</v>
       </c>
       <c r="S132" s="7" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="T132">
         <v>103</v>
       </c>
       <c r="V132" s="11" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="W132" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="X132" s="7">
         <v>100</v>
       </c>
       <c r="Y132" s="1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="Z132" s="1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="AA132" s="1">
         <v>11000002</v>
@@ -21649,13 +21642,13 @@
         <v>53000130</v>
       </c>
       <c r="B133" s="22" t="s">
+        <v>677</v>
+      </c>
+      <c r="C133" s="15" t="s">
         <v>678</v>
       </c>
-      <c r="C133" s="15" t="s">
-        <v>679</v>
-      </c>
       <c r="D133" s="25" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E133" s="15">
         <v>5</v>
@@ -21702,25 +21695,25 @@
         <v>25</v>
       </c>
       <c r="S133" s="7" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="T133">
         <v>107</v>
       </c>
       <c r="V133" s="11" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="W133" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="X133" s="7">
+        <v>102</v>
+      </c>
+      <c r="Y133" s="1" t="s">
         <v>681</v>
       </c>
-      <c r="X133" s="7">
-        <v>100</v>
-      </c>
-      <c r="Y133" s="1" t="s">
-        <v>682</v>
-      </c>
       <c r="Z133" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="AA133" s="1">
         <v>11000002</v>
@@ -21743,13 +21736,13 @@
         <v>53000131</v>
       </c>
       <c r="B134" s="22" t="s">
+        <v>682</v>
+      </c>
+      <c r="C134" s="15" t="s">
         <v>683</v>
       </c>
-      <c r="C134" s="15" t="s">
-        <v>684</v>
-      </c>
       <c r="D134" s="25" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E134" s="15">
         <v>2</v>
@@ -21796,25 +21789,25 @@
         <v>30</v>
       </c>
       <c r="S134" s="7" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="T134">
         <v>100</v>
       </c>
       <c r="V134" s="11" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="W134" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="X134" s="7">
+        <v>102</v>
+      </c>
+      <c r="Y134" s="1" t="s">
         <v>689</v>
       </c>
-      <c r="X134" s="7">
-        <v>100</v>
-      </c>
-      <c r="Y134" s="1" t="s">
-        <v>690</v>
-      </c>
       <c r="Z134" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="AA134" s="1">
         <v>11000002</v>
@@ -21837,13 +21830,13 @@
         <v>53000132</v>
       </c>
       <c r="B135" s="22" t="s">
+        <v>684</v>
+      </c>
+      <c r="C135" s="15" t="s">
         <v>685</v>
       </c>
-      <c r="C135" s="15" t="s">
+      <c r="D135" s="25" t="s">
         <v>686</v>
-      </c>
-      <c r="D135" s="25" t="s">
-        <v>687</v>
       </c>
       <c r="E135" s="15">
         <v>3</v>
@@ -21890,25 +21883,25 @@
         <v>0</v>
       </c>
       <c r="S135" s="7" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="T135">
         <v>102</v>
       </c>
       <c r="V135" s="11" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="W135" s="1" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="X135" s="1">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="Y135" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="Z135" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="AA135" s="1">
         <v>11000002</v>
@@ -21931,13 +21924,13 @@
         <v>53000133</v>
       </c>
       <c r="B136" s="22" t="s">
+        <v>694</v>
+      </c>
+      <c r="C136" s="15" t="s">
+        <v>693</v>
+      </c>
+      <c r="D136" s="25" t="s">
         <v>695</v>
-      </c>
-      <c r="C136" s="15" t="s">
-        <v>694</v>
-      </c>
-      <c r="D136" s="25" t="s">
-        <v>696</v>
       </c>
       <c r="E136" s="15">
         <v>2</v>
@@ -21991,10 +21984,10 @@
       </c>
       <c r="U136" s="15"/>
       <c r="V136" s="11" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="W136" s="1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="X136" s="1"/>
       <c r="Y136" s="15" t="s">
@@ -22022,13 +22015,13 @@
         <v>53000134</v>
       </c>
       <c r="B137" s="22" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C137" s="15" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="D137" s="25" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E137" s="15">
         <v>2</v>
@@ -22082,10 +22075,10 @@
       </c>
       <c r="U137" s="15"/>
       <c r="V137" s="11" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="W137" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="X137" s="1"/>
       <c r="Y137" s="15" t="s">
@@ -22113,13 +22106,13 @@
         <v>53000135</v>
       </c>
       <c r="B138" s="22" t="s">
+        <v>699</v>
+      </c>
+      <c r="C138" s="15" t="s">
         <v>700</v>
       </c>
-      <c r="C138" s="15" t="s">
-        <v>701</v>
-      </c>
       <c r="D138" s="25" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E138" s="15">
         <v>4</v>
@@ -22166,23 +22159,23 @@
         <v>20</v>
       </c>
       <c r="S138" s="15" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="T138" s="15">
         <v>108</v>
       </c>
       <c r="U138" s="15"/>
       <c r="V138" s="11" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="W138" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="X138" s="7">
         <v>100</v>
       </c>
       <c r="Y138" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="Z138" s="15"/>
       <c r="AA138" s="15">
@@ -22206,13 +22199,13 @@
         <v>53000136</v>
       </c>
       <c r="B139" s="22" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D139" s="25" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E139" s="15">
         <v>3</v>
@@ -22259,23 +22252,23 @@
         <v>20</v>
       </c>
       <c r="S139" s="15" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="T139" s="15">
         <v>100</v>
       </c>
       <c r="U139" s="15"/>
       <c r="V139" s="11" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="W139" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="X139" s="7">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Y139" s="15" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="Z139" s="15"/>
       <c r="AA139" s="15">
@@ -22299,13 +22292,13 @@
         <v>53000137</v>
       </c>
       <c r="B140" s="22" t="s">
+        <v>709</v>
+      </c>
+      <c r="C140" s="15" t="s">
         <v>710</v>
       </c>
-      <c r="C140" s="15" t="s">
+      <c r="D140" s="25" t="s">
         <v>711</v>
-      </c>
-      <c r="D140" s="25" t="s">
-        <v>712</v>
       </c>
       <c r="E140" s="15">
         <v>2</v>
@@ -22352,17 +22345,17 @@
         <v>0</v>
       </c>
       <c r="S140" s="15" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="T140" s="15">
         <v>102</v>
       </c>
       <c r="U140" s="15"/>
       <c r="V140" s="11" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="W140" s="1" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="X140" s="1"/>
       <c r="Y140" s="15" t="s">
@@ -22390,10 +22383,10 @@
         <v>53000138</v>
       </c>
       <c r="B141" s="22" t="s">
+        <v>722</v>
+      </c>
+      <c r="C141" s="15" t="s">
         <v>723</v>
-      </c>
-      <c r="C141" s="15" t="s">
-        <v>724</v>
       </c>
       <c r="D141" s="25" t="s">
         <v>394</v>
@@ -22443,21 +22436,21 @@
         <v>1</v>
       </c>
       <c r="S141" s="15" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="T141" s="15">
         <v>105</v>
       </c>
       <c r="U141" s="15"/>
       <c r="V141" s="11" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="W141" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="X141" s="1"/>
       <c r="Y141" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="Z141" s="15"/>
       <c r="AA141" s="15">
@@ -22481,10 +22474,10 @@
         <v>53000139</v>
       </c>
       <c r="B142" s="22" t="s">
+        <v>724</v>
+      </c>
+      <c r="C142" s="15" t="s">
         <v>725</v>
-      </c>
-      <c r="C142" s="15" t="s">
-        <v>726</v>
       </c>
       <c r="D142" s="25" t="s">
         <v>469</v>
@@ -22534,21 +22527,21 @@
         <v>2</v>
       </c>
       <c r="S142" s="15" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="T142" s="15">
         <v>103</v>
       </c>
       <c r="U142" s="15"/>
       <c r="V142" s="11" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="W142" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="X142" s="1"/>
       <c r="Y142" s="15" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="Z142" s="15"/>
       <c r="AA142" s="15">
@@ -22572,10 +22565,10 @@
         <v>53000140</v>
       </c>
       <c r="B143" s="22" t="s">
+        <v>727</v>
+      </c>
+      <c r="C143" s="15" t="s">
         <v>728</v>
-      </c>
-      <c r="C143" s="15" t="s">
-        <v>729</v>
       </c>
       <c r="D143" s="25" t="s">
         <v>394</v>
@@ -22625,21 +22618,21 @@
         <v>3</v>
       </c>
       <c r="S143" s="15" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="T143" s="15">
         <v>100</v>
       </c>
       <c r="U143" s="15"/>
       <c r="V143" s="11" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="W143" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="X143" s="1"/>
       <c r="Y143" s="15" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="Z143" s="15"/>
       <c r="AA143" s="15">
@@ -22663,13 +22656,13 @@
         <v>53000141</v>
       </c>
       <c r="B144" s="22" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C144" s="15" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="D144" s="25" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="E144" s="15">
         <v>3</v>
@@ -22723,19 +22716,19 @@
       </c>
       <c r="U144" s="15"/>
       <c r="V144" s="11" t="s">
+        <v>914</v>
+      </c>
+      <c r="W144" s="1" t="s">
         <v>915</v>
       </c>
-      <c r="W144" s="1" t="s">
+      <c r="X144" s="7">
+        <v>102</v>
+      </c>
+      <c r="Y144" s="15" t="s">
         <v>916</v>
       </c>
-      <c r="X144" s="7">
-        <v>100</v>
-      </c>
-      <c r="Y144" s="15" t="s">
-        <v>917</v>
-      </c>
       <c r="Z144" s="15" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="AA144" s="15">
         <v>11000005</v>
@@ -22758,13 +22751,13 @@
         <v>53000142</v>
       </c>
       <c r="B145" s="22" t="s">
+        <v>919</v>
+      </c>
+      <c r="C145" s="15" t="s">
         <v>920</v>
       </c>
-      <c r="C145" s="15" t="s">
+      <c r="D145" s="44" t="s">
         <v>921</v>
-      </c>
-      <c r="D145" s="45" t="s">
-        <v>922</v>
       </c>
       <c r="E145" s="15">
         <v>3</v>
@@ -22817,17 +22810,17 @@
         <v>100</v>
       </c>
       <c r="U145" s="15"/>
-      <c r="V145" s="44" t="s">
+      <c r="V145" s="11" t="s">
+        <v>922</v>
+      </c>
+      <c r="W145" s="1" t="s">
         <v>923</v>
-      </c>
-      <c r="W145" s="1" t="s">
-        <v>924</v>
       </c>
       <c r="X145" s="7">
         <v>100</v>
       </c>
       <c r="Y145" s="15" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="Z145" s="15"/>
       <c r="AA145" s="15">
@@ -22851,10 +22844,10 @@
         <v>53000143</v>
       </c>
       <c r="B146" s="22" t="s">
+        <v>924</v>
+      </c>
+      <c r="C146" s="15" t="s">
         <v>925</v>
-      </c>
-      <c r="C146" s="15" t="s">
-        <v>926</v>
       </c>
       <c r="D146" s="25" t="s">
         <v>394</v>
@@ -22904,23 +22897,23 @@
         <v>0</v>
       </c>
       <c r="S146" s="15" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="T146" s="15">
         <v>105</v>
       </c>
       <c r="U146" s="15"/>
-      <c r="V146" s="44" t="s">
-        <v>929</v>
+      <c r="V146" s="11" t="s">
+        <v>928</v>
       </c>
       <c r="W146" s="1" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="X146" s="1">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="Y146" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="Z146" s="15"/>
       <c r="AA146" s="15">
@@ -22944,13 +22937,13 @@
         <v>53000144</v>
       </c>
       <c r="B147" s="22" t="s">
+        <v>938</v>
+      </c>
+      <c r="C147" s="15" t="s">
         <v>939</v>
       </c>
-      <c r="C147" s="15" t="s">
-        <v>940</v>
-      </c>
-      <c r="D147" s="45" t="s">
-        <v>922</v>
+      <c r="D147" s="44" t="s">
+        <v>921</v>
       </c>
       <c r="E147" s="15">
         <v>2</v>
@@ -23003,11 +22996,11 @@
         <v>105</v>
       </c>
       <c r="U147" s="15"/>
-      <c r="V147" s="44" t="s">
-        <v>944</v>
+      <c r="V147" s="11" t="s">
+        <v>943</v>
       </c>
       <c r="W147" s="1" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="X147" s="7">
         <v>100</v>
@@ -23037,10 +23030,10 @@
         <v>53000145</v>
       </c>
       <c r="B148" s="22" t="s">
+        <v>940</v>
+      </c>
+      <c r="C148" s="15" t="s">
         <v>941</v>
-      </c>
-      <c r="C148" s="15" t="s">
-        <v>942</v>
       </c>
       <c r="D148" s="25" t="s">
         <v>394</v>
@@ -23096,19 +23089,19 @@
         <v>102</v>
       </c>
       <c r="V148" s="11" t="s">
+        <v>946</v>
+      </c>
+      <c r="W148" s="1" t="s">
         <v>947</v>
       </c>
-      <c r="W148" s="1" t="s">
-        <v>948</v>
-      </c>
       <c r="X148" s="1">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="Y148" s="1" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="Z148" s="1" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="AA148" s="1">
         <v>11000001</v>
@@ -23211,11 +23204,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="X11" sqref="X11"/>
+      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -23284,7 +23277,7 @@
         <v>340</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="P1" s="17" t="s">
         <v>325</v>
@@ -23302,7 +23295,7 @@
         <v>368</v>
       </c>
       <c r="U1" s="13" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="V1" s="13" t="s">
         <v>338</v>
@@ -23311,7 +23304,7 @@
         <v>298</v>
       </c>
       <c r="X1" s="13" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="Y1" s="13" t="s">
         <v>367</v>
@@ -23329,7 +23322,7 @@
         <v>348</v>
       </c>
       <c r="AD1" s="23" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="AE1" s="23" t="s">
         <v>351</v>
@@ -23379,7 +23372,7 @@
         <v>339</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>312</v>
@@ -23397,7 +23390,7 @@
         <v>456</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>475</v>
@@ -23406,7 +23399,7 @@
         <v>176</v>
       </c>
       <c r="X2" s="10" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="Y2" s="4" t="s">
         <v>176</v>
@@ -23474,7 +23467,7 @@
         <v>342</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="P3" s="20" t="s">
         <v>327</v>
@@ -23492,7 +23485,7 @@
         <v>369</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="V3" s="6" t="s">
         <v>297</v>
@@ -23501,7 +23494,7 @@
         <v>299</v>
       </c>
       <c r="X3" s="6" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="Y3" s="6" t="s">
         <v>315</v>
@@ -23519,10 +23512,10 @@
         <v>349</v>
       </c>
       <c r="AD3" s="43" t="s">
+        <v>883</v>
+      </c>
+      <c r="AE3" s="43" t="s">
         <v>884</v>
-      </c>
-      <c r="AE3" s="43" t="s">
-        <v>885</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="24" x14ac:dyDescent="0.15">
@@ -23533,7 +23526,7 @@
         <v>352</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D4" s="32"/>
       <c r="E4" s="15">
@@ -23588,13 +23581,13 @@
       </c>
       <c r="U4" s="1"/>
       <c r="V4" s="11" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="W4" s="7" t="s">
         <v>334</v>
       </c>
       <c r="X4" s="7">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="Y4" s="15" t="s">
         <v>353</v>
@@ -23622,7 +23615,7 @@
         <v>320</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="D5" s="32"/>
       <c r="E5" s="15">
@@ -23677,13 +23670,13 @@
       </c>
       <c r="U5" s="1"/>
       <c r="V5" s="11" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="W5" s="7" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="X5" s="7">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="Y5" s="1" t="s">
         <v>15</v>
@@ -23711,7 +23704,7 @@
         <v>355</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="D6" s="32"/>
       <c r="E6" s="15">
@@ -23759,17 +23752,17 @@
         <v>0</v>
       </c>
       <c r="S6" s="15" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="T6" s="1">
         <v>-1</v>
       </c>
       <c r="U6" s="1"/>
       <c r="V6" s="11" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="W6" s="7" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="X6" s="7"/>
       <c r="Y6" s="15" t="s">
@@ -23798,7 +23791,7 @@
         <v>356</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="D7" s="32"/>
       <c r="E7" s="15">
@@ -23853,10 +23846,10 @@
       </c>
       <c r="U7" s="1"/>
       <c r="V7" s="11" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="W7" s="7" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="X7" s="7"/>
       <c r="Y7" s="15" t="s">
@@ -23885,7 +23878,7 @@
         <v>357</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="D8" s="32"/>
       <c r="E8" s="15">
@@ -23940,7 +23933,7 @@
       </c>
       <c r="U8" s="1"/>
       <c r="V8" s="11" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="W8" s="7" t="s">
         <v>365</v>
@@ -23972,7 +23965,7 @@
         <v>358</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="D9" s="32"/>
       <c r="E9" s="15">
@@ -24027,7 +24020,7 @@
       </c>
       <c r="U9" s="1"/>
       <c r="V9" s="11" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="W9" s="7" t="s">
         <v>363</v>
@@ -24061,7 +24054,7 @@
         <v>474</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="15">
@@ -24109,16 +24102,16 @@
         <v>0</v>
       </c>
       <c r="S10" s="15" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="T10" s="1">
         <v>-1</v>
       </c>
       <c r="U10" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="V10" s="11" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="W10" s="7" t="s">
         <v>476</v>
@@ -24150,7 +24143,7 @@
         <v>506</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="D11" s="32"/>
       <c r="E11" s="15">
@@ -24198,14 +24191,14 @@
         <v>0</v>
       </c>
       <c r="S11" s="15" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="T11" s="1">
         <v>-1</v>
       </c>
       <c r="U11" s="1"/>
       <c r="V11" s="11" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="W11" s="7" t="s">
         <v>507</v>
@@ -24236,10 +24229,10 @@
         <v>53100008</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="D12" s="32"/>
       <c r="E12" s="15">
@@ -24287,17 +24280,17 @@
         <v>0</v>
       </c>
       <c r="S12" s="15" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="T12" s="1">
         <v>-1</v>
       </c>
       <c r="U12" s="1"/>
       <c r="V12" s="11" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="W12" s="7" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="X12" s="7"/>
       <c r="Y12" s="15" t="s">
@@ -24323,10 +24316,10 @@
         <v>53200001</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="D13" s="32"/>
       <c r="E13" s="15">
@@ -24374,23 +24367,23 @@
         <v>0</v>
       </c>
       <c r="S13" s="15" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="T13" s="1">
         <v>-1</v>
       </c>
       <c r="U13" s="1"/>
       <c r="V13" s="11" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="W13" s="7" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="X13" s="7">
         <v>200</v>
       </c>
       <c r="Y13" s="15" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="Z13" s="15"/>
       <c r="AA13" s="15"/>
@@ -24412,10 +24405,10 @@
         <v>53200002</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="D14" s="42"/>
       <c r="E14" s="15">
@@ -24463,16 +24456,16 @@
         <v>0</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="T14">
         <v>-1</v>
       </c>
       <c r="V14" s="11" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="W14" s="7" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="X14" s="7">
         <v>200</v>
@@ -24500,10 +24493,10 @@
         <v>53200003</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="D15" s="32"/>
       <c r="E15" s="15">
@@ -24558,13 +24551,13 @@
       </c>
       <c r="U15" s="1"/>
       <c r="V15" s="11" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="W15" s="7" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="X15" s="7">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="Y15" s="15" t="s">
         <v>2</v>
@@ -24692,7 +24685,7 @@
         <v>340</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="P1" s="17" t="s">
         <v>325</v>
@@ -24710,7 +24703,7 @@
         <v>368</v>
       </c>
       <c r="U1" s="13" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="V1" s="13" t="s">
         <v>338</v>
@@ -24719,7 +24712,7 @@
         <v>298</v>
       </c>
       <c r="X1" s="13" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="Y1" s="13" t="s">
         <v>367</v>
@@ -24737,7 +24730,7 @@
         <v>348</v>
       </c>
       <c r="AD1" s="23" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="AE1" s="23" t="s">
         <v>351</v>
@@ -24787,7 +24780,7 @@
         <v>339</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>312</v>
@@ -24805,7 +24798,7 @@
         <v>456</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>314</v>
@@ -24814,7 +24807,7 @@
         <v>176</v>
       </c>
       <c r="X2" s="10" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="Y2" s="4" t="s">
         <v>176</v>
@@ -24882,7 +24875,7 @@
         <v>342</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="P3" s="20" t="s">
         <v>327</v>
@@ -24900,7 +24893,7 @@
         <v>369</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="V3" s="6" t="s">
         <v>297</v>
@@ -24909,7 +24902,7 @@
         <v>299</v>
       </c>
       <c r="X3" s="6" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="Y3" s="6" t="s">
         <v>315</v>
@@ -24927,10 +24920,10 @@
         <v>349</v>
       </c>
       <c r="AD3" s="43" t="s">
+        <v>883</v>
+      </c>
+      <c r="AE3" s="43" t="s">
         <v>884</v>
-      </c>
-      <c r="AE3" s="43" t="s">
-        <v>885</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="36" x14ac:dyDescent="0.15">
@@ -24997,7 +24990,7 @@
         <v>115</v>
       </c>
       <c r="V4" s="11" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="W4" s="7" t="s">
         <v>364</v>
@@ -25085,7 +25078,7 @@
         <v>90</v>
       </c>
       <c r="V5" s="11" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="W5" s="7" t="s">
         <v>366</v>
@@ -25173,7 +25166,7 @@
         <v>115</v>
       </c>
       <c r="V6" s="11" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="W6" s="29" t="s">
         <v>405</v>
@@ -25347,7 +25340,7 @@
         <v>90</v>
       </c>
       <c r="V8" s="11" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="W8" s="7" t="s">
         <v>375</v>
@@ -25437,7 +25430,7 @@
         <v>400</v>
       </c>
       <c r="V9" s="11" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="W9" s="7" t="s">
         <v>328</v>

</xml_diff>

<commit_message>
change some ai guides
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -9491,10 +9491,10 @@
   <dimension ref="A1:AE148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="D142" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W6" sqref="W6"/>
+      <selection pane="bottomRight" activeCell="W143" sqref="W143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -14520,7 +14520,9 @@
       <c r="W55" s="7" t="s">
         <v>667</v>
       </c>
-      <c r="X55" s="7"/>
+      <c r="X55" s="7">
+        <v>100</v>
+      </c>
       <c r="Y55" s="1" t="s">
         <v>527</v>
       </c>
@@ -14611,7 +14613,7 @@
         <v>519</v>
       </c>
       <c r="X56" s="7">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Y56" s="1" t="s">
         <v>73</v>

</xml_diff>

<commit_message>
expand GetRandomPoint method for map
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -3811,10 +3811,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>p.Action.AddRandomMonster(-1,spl.Level,m.GetRandomPoint());</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>silverlight</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -4145,6 +4141,10 @@
   </si>
   <si>
     <t>m.ReviveUnit(p,t,spl.Cure);</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>p.Action.AddRandomMonster(-1,spl.Level,m.GetRandomPoint(p.IsLeft, true, true));</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -9028,7 +9028,11 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AE148" totalsRowShown="0" headerRowDxfId="109" dataDxfId="108" tableBorderDxfId="107">
-  <autoFilter ref="A3:AE148"/>
+  <autoFilter ref="A3:AE148">
+    <filterColumn colId="23">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A4:AE113">
     <sortCondition ref="A3:A113"/>
   </sortState>
@@ -9491,10 +9495,10 @@
   <dimension ref="A1:AE148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="D142" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="D39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W143" sqref="W143"/>
+      <selection pane="bottomRight" activeCell="V39" sqref="V39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9584,7 +9588,7 @@
         <v>368</v>
       </c>
       <c r="U1" s="13" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="V1" s="13" t="s">
         <v>338</v>
@@ -9593,7 +9597,7 @@
         <v>298</v>
       </c>
       <c r="X1" s="13" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="Y1" s="13" t="s">
         <v>367</v>
@@ -9679,7 +9683,7 @@
         <v>456</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>314</v>
@@ -9688,7 +9692,7 @@
         <v>176</v>
       </c>
       <c r="X2" s="10" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="Y2" s="4" t="s">
         <v>176</v>
@@ -9774,7 +9778,7 @@
         <v>369</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="V3" s="6" t="s">
         <v>438</v>
@@ -9783,7 +9787,7 @@
         <v>508</v>
       </c>
       <c r="X3" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="Y3" s="6" t="s">
         <v>315</v>
@@ -9807,7 +9811,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>53000001</v>
       </c>
@@ -9871,12 +9875,14 @@
         <v>95</v>
       </c>
       <c r="V4" s="11" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="W4" s="7" t="s">
         <v>707</v>
       </c>
-      <c r="X4" s="7"/>
+      <c r="X4" s="7">
+        <v>1</v>
+      </c>
       <c r="Y4" s="1" t="s">
         <v>2</v>
       </c>
@@ -9983,7 +9989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>53000003</v>
       </c>
@@ -10073,7 +10079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" ht="48" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:31" ht="48" hidden="1" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>53000004</v>
       </c>
@@ -10137,7 +10143,7 @@
         <v>100</v>
       </c>
       <c r="V7" s="11" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="W7" s="7" t="s">
         <v>679</v>
@@ -10165,7 +10171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>53000005</v>
       </c>
@@ -10232,7 +10238,7 @@
         <v>827</v>
       </c>
       <c r="W8" s="7" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="X8" s="7">
         <v>102</v>
@@ -10873,7 +10879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>53000013</v>
       </c>
@@ -10965,7 +10971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>53000014</v>
       </c>
@@ -10976,7 +10982,7 @@
         <v>442</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="E17" s="1">
         <v>2</v>
@@ -11057,7 +11063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:31" hidden="1" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>53000015</v>
       </c>
@@ -11149,7 +11155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:31" ht="48" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:31" ht="48" hidden="1" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>53000016</v>
       </c>
@@ -11160,7 +11166,7 @@
         <v>216</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="E19" s="1">
         <v>3</v>
@@ -11213,10 +11219,10 @@
         <v>95</v>
       </c>
       <c r="V19" s="11" t="s">
+        <v>933</v>
+      </c>
+      <c r="W19" s="7" t="s">
         <v>934</v>
-      </c>
-      <c r="W19" s="7" t="s">
-        <v>935</v>
       </c>
       <c r="X19" s="7">
         <v>100</v>
@@ -11241,7 +11247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>53000017</v>
       </c>
@@ -11333,7 +11339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>53000018</v>
       </c>
@@ -11397,7 +11403,7 @@
         <v>102</v>
       </c>
       <c r="V21" s="11" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="W21" s="7" t="s">
         <v>512</v>
@@ -11425,7 +11431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>53000019</v>
       </c>
@@ -11519,7 +11525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>53000020</v>
       </c>
@@ -11613,7 +11619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>53000021</v>
       </c>
@@ -11707,7 +11713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>53000022</v>
       </c>
@@ -11776,7 +11782,9 @@
       <c r="W25" s="7" t="s">
         <v>649</v>
       </c>
-      <c r="X25" s="7"/>
+      <c r="X25" s="7">
+        <v>3</v>
+      </c>
       <c r="Y25" s="1" t="s">
         <v>29</v>
       </c>
@@ -11797,7 +11805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>53000023</v>
       </c>
@@ -11866,7 +11874,9 @@
       <c r="W26" s="21" t="s">
         <v>378</v>
       </c>
-      <c r="X26" s="21"/>
+      <c r="X26" s="21">
+        <v>2</v>
+      </c>
       <c r="Y26" s="1" t="s">
         <v>2</v>
       </c>
@@ -11885,7 +11895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>53000024</v>
       </c>
@@ -11954,7 +11964,9 @@
       <c r="W27" s="7" t="s">
         <v>379</v>
       </c>
-      <c r="X27" s="7"/>
+      <c r="X27" s="7">
+        <v>3</v>
+      </c>
       <c r="Y27" s="1" t="s">
         <v>29</v>
       </c>
@@ -11975,7 +11987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>53000025</v>
       </c>
@@ -12067,7 +12079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:31" hidden="1" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>53000026</v>
       </c>
@@ -12125,16 +12137,16 @@
         <v>10</v>
       </c>
       <c r="S29" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="T29">
         <v>100</v>
       </c>
       <c r="U29" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="V29" s="11" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="W29" s="7" t="s">
         <v>465</v>
@@ -12162,7 +12174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>53000027</v>
       </c>
@@ -12252,7 +12264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>53000028</v>
       </c>
@@ -12342,7 +12354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>53000029</v>
       </c>
@@ -12612,7 +12624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>53000032</v>
       </c>
@@ -12676,10 +12688,10 @@
         <v>100</v>
       </c>
       <c r="U35" t="s">
+        <v>972</v>
+      </c>
+      <c r="V35" s="11" t="s">
         <v>973</v>
-      </c>
-      <c r="V35" s="11" t="s">
-        <v>974</v>
       </c>
       <c r="W35" s="7" t="s">
         <v>399</v>
@@ -12709,7 +12721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>53000033</v>
       </c>
@@ -12803,7 +12815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>53000034</v>
       </c>
@@ -12867,12 +12879,14 @@
         <v>100</v>
       </c>
       <c r="V37" s="11" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="W37" s="7" t="s">
         <v>347</v>
       </c>
-      <c r="X37" s="7"/>
+      <c r="X37" s="7">
+        <v>1</v>
+      </c>
       <c r="Y37" s="1" t="s">
         <v>167</v>
       </c>
@@ -12893,7 +12907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>53000035</v>
       </c>
@@ -13051,7 +13065,7 @@
         <v>100</v>
       </c>
       <c r="V39" s="11" t="s">
-        <v>894</v>
+        <v>978</v>
       </c>
       <c r="W39" s="1" t="s">
         <v>528</v>
@@ -13077,7 +13091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>53000037</v>
       </c>
@@ -13167,7 +13181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>53000038</v>
       </c>
@@ -13441,7 +13455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>53000041</v>
       </c>
@@ -13531,7 +13545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>53000042</v>
       </c>
@@ -13689,10 +13703,10 @@
         <v>100</v>
       </c>
       <c r="V46" s="11" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="W46" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="X46" s="1"/>
       <c r="Y46" s="1" t="s">
@@ -13805,7 +13819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:31" ht="96" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:31" ht="96" hidden="1" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>53000045</v>
       </c>
@@ -13987,7 +14001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>53000047</v>
       </c>
@@ -14081,7 +14095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>53000048</v>
       </c>
@@ -14173,7 +14187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>53000049</v>
       </c>
@@ -14357,7 +14371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:31" ht="96" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:31" ht="96" hidden="1" x14ac:dyDescent="0.15">
       <c r="A54">
         <v>53000051</v>
       </c>
@@ -14451,7 +14465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A55">
         <v>53000052</v>
       </c>
@@ -14543,7 +14557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A56">
         <v>53000053</v>
       </c>
@@ -14635,7 +14649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A57">
         <v>53000054</v>
       </c>
@@ -14727,7 +14741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A58">
         <v>53000055</v>
       </c>
@@ -14791,12 +14805,14 @@
         <v>100</v>
       </c>
       <c r="V58" s="11" t="s">
+        <v>898</v>
+      </c>
+      <c r="W58" s="1" t="s">
         <v>899</v>
       </c>
-      <c r="W58" s="1" t="s">
-        <v>900</v>
-      </c>
-      <c r="X58" s="1"/>
+      <c r="X58" s="1">
+        <v>1</v>
+      </c>
       <c r="Y58" s="1" t="s">
         <v>2</v>
       </c>
@@ -14817,7 +14833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A59">
         <v>53000056</v>
       </c>
@@ -14909,7 +14925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A60">
         <v>53000057</v>
       </c>
@@ -15001,7 +15017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A61">
         <v>53000058</v>
       </c>
@@ -15070,7 +15086,9 @@
       <c r="W61" s="7" t="s">
         <v>673</v>
       </c>
-      <c r="X61" s="7"/>
+      <c r="X61" s="7">
+        <v>1</v>
+      </c>
       <c r="Y61" s="1" t="s">
         <v>15</v>
       </c>
@@ -15091,7 +15109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A62">
         <v>53000059</v>
       </c>
@@ -15183,7 +15201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A63">
         <v>53000060</v>
       </c>
@@ -15275,7 +15293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:31" ht="48" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:31" ht="48" hidden="1" x14ac:dyDescent="0.15">
       <c r="A64">
         <v>53000061</v>
       </c>
@@ -15367,7 +15385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A65">
         <v>53000062</v>
       </c>
@@ -15607,16 +15625,16 @@
         <v>10</v>
       </c>
       <c r="S67" s="1" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="T67">
         <v>100</v>
       </c>
       <c r="V67" s="11" t="s">
+        <v>907</v>
+      </c>
+      <c r="W67" s="7" t="s">
         <v>908</v>
-      </c>
-      <c r="W67" s="7" t="s">
-        <v>909</v>
       </c>
       <c r="X67" s="7"/>
       <c r="Y67" s="1" t="s">
@@ -15821,7 +15839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A70">
         <v>53000067</v>
       </c>
@@ -15885,7 +15903,7 @@
         <v>100</v>
       </c>
       <c r="V70" s="11" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="W70" s="7" t="s">
         <v>547</v>
@@ -15913,7 +15931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A71">
         <v>53000068</v>
       </c>
@@ -15924,7 +15942,7 @@
         <v>256</v>
       </c>
       <c r="D71" s="25" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E71" s="1">
         <v>2</v>
@@ -16007,7 +16025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A72">
         <v>53000069</v>
       </c>
@@ -16099,7 +16117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A73">
         <v>53000070</v>
       </c>
@@ -16191,7 +16209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A74">
         <v>53000071</v>
       </c>
@@ -16285,7 +16303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A75">
         <v>53000072</v>
       </c>
@@ -16467,7 +16485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:31" ht="48" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:31" ht="48" hidden="1" x14ac:dyDescent="0.15">
       <c r="A77">
         <v>53000074</v>
       </c>
@@ -16531,10 +16549,10 @@
         <v>103</v>
       </c>
       <c r="V77" s="11" t="s">
+        <v>896</v>
+      </c>
+      <c r="W77" s="7" t="s">
         <v>897</v>
-      </c>
-      <c r="W77" s="7" t="s">
-        <v>898</v>
       </c>
       <c r="X77" s="7">
         <v>100</v>
@@ -16559,7 +16577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:31" ht="120" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:31" ht="120" hidden="1" x14ac:dyDescent="0.15">
       <c r="A78">
         <v>53000075</v>
       </c>
@@ -16651,7 +16669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A79">
         <v>53000076</v>
       </c>
@@ -16899,7 +16917,7 @@
         <v>100</v>
       </c>
       <c r="V81" s="37" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="W81" s="7" t="s">
         <v>611</v>
@@ -16923,7 +16941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:31" ht="96" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:31" ht="96" hidden="1" x14ac:dyDescent="0.15">
       <c r="A82">
         <v>53000079</v>
       </c>
@@ -17017,7 +17035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A83">
         <v>53000080</v>
       </c>
@@ -17111,7 +17129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A84">
         <v>53000081</v>
       </c>
@@ -17205,7 +17223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A85">
         <v>53000082</v>
       </c>
@@ -17368,7 +17386,7 @@
       </c>
       <c r="X86" s="7"/>
       <c r="Y86" s="1" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="Z86" s="1"/>
       <c r="AA86" s="1">
@@ -17479,7 +17497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A88">
         <v>53000085</v>
       </c>
@@ -17543,10 +17561,10 @@
         <v>100</v>
       </c>
       <c r="U88" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="V88" s="11" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="W88" s="7" t="s">
         <v>757</v>
@@ -17576,7 +17594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A89">
         <v>53000086</v>
       </c>
@@ -17668,7 +17686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A90">
         <v>53000087</v>
       </c>
@@ -17762,7 +17780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A91">
         <v>53000088</v>
       </c>
@@ -17856,7 +17874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A92">
         <v>53000089</v>
       </c>
@@ -17950,7 +17968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A93">
         <v>53000090</v>
       </c>
@@ -18019,7 +18037,9 @@
       <c r="W93" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="X93" s="1"/>
+      <c r="X93" s="1">
+        <v>3</v>
+      </c>
       <c r="Y93" s="1" t="s">
         <v>161</v>
       </c>
@@ -18040,7 +18060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:31" ht="48" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:31" ht="48" hidden="1" x14ac:dyDescent="0.15">
       <c r="A94">
         <v>53000091</v>
       </c>
@@ -18132,7 +18152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A95">
         <v>53000092</v>
       </c>
@@ -18201,7 +18221,9 @@
       <c r="W95" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="X95" s="1"/>
+      <c r="X95" s="1">
+        <v>1</v>
+      </c>
       <c r="Y95" s="1" t="s">
         <v>538</v>
       </c>
@@ -18222,7 +18244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:31" ht="48" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:31" ht="48" hidden="1" x14ac:dyDescent="0.15">
       <c r="A96">
         <v>53000093</v>
       </c>
@@ -18404,7 +18426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A98">
         <v>53000095</v>
       </c>
@@ -18588,7 +18610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A100">
         <v>53000097</v>
       </c>
@@ -18680,7 +18702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A101">
         <v>53000098</v>
       </c>
@@ -18749,7 +18771,9 @@
       <c r="W101" s="7" t="s">
         <v>385</v>
       </c>
-      <c r="X101" s="7"/>
+      <c r="X101" s="7">
+        <v>3</v>
+      </c>
       <c r="Y101" s="1" t="s">
         <v>163</v>
       </c>
@@ -18770,7 +18794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A102">
         <v>53000099</v>
       </c>
@@ -18952,7 +18976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A104">
         <v>53000101</v>
       </c>
@@ -19044,7 +19068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A105">
         <v>53000102</v>
       </c>
@@ -19136,7 +19160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:31" ht="96" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:31" ht="96" hidden="1" x14ac:dyDescent="0.15">
       <c r="A106">
         <v>53000103</v>
       </c>
@@ -19230,7 +19254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:31" ht="132" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:31" ht="132" hidden="1" x14ac:dyDescent="0.15">
       <c r="A107">
         <v>53000104</v>
       </c>
@@ -19294,10 +19318,10 @@
         <v>105</v>
       </c>
       <c r="V107" s="11" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="W107" s="7" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="X107" s="7">
         <v>102</v>
@@ -19322,7 +19346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A108">
         <v>53000105</v>
       </c>
@@ -19384,10 +19408,10 @@
         <v>100</v>
       </c>
       <c r="V108" s="11" t="s">
+        <v>905</v>
+      </c>
+      <c r="W108" s="1" t="s">
         <v>906</v>
-      </c>
-      <c r="W108" s="1" t="s">
-        <v>907</v>
       </c>
       <c r="X108" s="7">
         <v>100</v>
@@ -19412,7 +19436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A109">
         <v>53000106</v>
       </c>
@@ -19504,7 +19528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A110">
         <v>53000107</v>
       </c>
@@ -19568,10 +19592,10 @@
         <v>100</v>
       </c>
       <c r="V110" s="11" t="s">
+        <v>928</v>
+      </c>
+      <c r="W110" s="7" t="s">
         <v>929</v>
-      </c>
-      <c r="W110" s="7" t="s">
-        <v>930</v>
       </c>
       <c r="X110" s="7">
         <v>102</v>
@@ -19598,7 +19622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:31" ht="120" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:31" ht="120" hidden="1" x14ac:dyDescent="0.15">
       <c r="A111">
         <v>53000108</v>
       </c>
@@ -19690,7 +19714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A112">
         <v>53000109</v>
       </c>
@@ -19782,7 +19806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:31" ht="48" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:31" ht="48" hidden="1" x14ac:dyDescent="0.15">
       <c r="A113">
         <v>53000110</v>
       </c>
@@ -19851,7 +19875,9 @@
       <c r="W113" s="7" t="s">
         <v>584</v>
       </c>
-      <c r="X113" s="7"/>
+      <c r="X113" s="7">
+        <v>2</v>
+      </c>
       <c r="Y113" s="1" t="s">
         <v>29</v>
       </c>
@@ -19872,7 +19898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A114">
         <v>53000111</v>
       </c>
@@ -19966,7 +19992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:31" ht="48" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:31" ht="48" hidden="1" x14ac:dyDescent="0.15">
       <c r="A115">
         <v>53000112</v>
       </c>
@@ -20030,10 +20056,10 @@
         <v>100</v>
       </c>
       <c r="U115" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="V115" s="11" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="W115" s="7" t="s">
         <v>553</v>
@@ -20063,7 +20089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A116">
         <v>53000113</v>
       </c>
@@ -20155,7 +20181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A117">
         <v>53000114</v>
       </c>
@@ -20247,7 +20273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A118">
         <v>53000115</v>
       </c>
@@ -20339,7 +20365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A119">
         <v>53000116</v>
       </c>
@@ -20350,7 +20376,7 @@
         <v>597</v>
       </c>
       <c r="D119" s="25" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="E119" s="1">
         <v>2</v>
@@ -20403,7 +20429,7 @@
         <v>101</v>
       </c>
       <c r="V119" s="11" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="W119" s="7" t="s">
         <v>636</v>
@@ -20433,7 +20459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A120">
         <v>53000117</v>
       </c>
@@ -20527,7 +20553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A121">
         <v>53000118</v>
       </c>
@@ -20594,7 +20620,9 @@
       <c r="W121" s="7" t="s">
         <v>613</v>
       </c>
-      <c r="X121" s="7"/>
+      <c r="X121" s="7">
+        <v>1</v>
+      </c>
       <c r="Y121" s="1" t="s">
         <v>614</v>
       </c>
@@ -20617,7 +20645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A122">
         <v>53000119</v>
       </c>
@@ -20682,7 +20710,7 @@
         <v>809</v>
       </c>
       <c r="W122" s="7" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="X122" s="7">
         <v>100</v>
@@ -20709,7 +20737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A123">
         <v>53000120</v>
       </c>
@@ -20802,7 +20830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A124">
         <v>53000121</v>
       </c>
@@ -20896,7 +20924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A125">
         <v>53000122</v>
       </c>
@@ -20960,10 +20988,10 @@
         <v>101</v>
       </c>
       <c r="U125" s="11" t="s">
+        <v>969</v>
+      </c>
+      <c r="V125" s="11" t="s">
         <v>970</v>
-      </c>
-      <c r="V125" s="11" t="s">
-        <v>971</v>
       </c>
       <c r="W125" s="1" t="s">
         <v>641</v>
@@ -20993,7 +21021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:31" ht="48" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:31" ht="48" hidden="1" x14ac:dyDescent="0.15">
       <c r="A126">
         <v>53000123</v>
       </c>
@@ -21087,7 +21115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A127">
         <v>53000124</v>
       </c>
@@ -21181,7 +21209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:31" ht="48" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:31" ht="48" hidden="1" x14ac:dyDescent="0.15">
       <c r="A128">
         <v>53000125</v>
       </c>
@@ -21275,7 +21303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A129">
         <v>53000126</v>
       </c>
@@ -21342,7 +21370,9 @@
       <c r="W129" s="1" t="s">
         <v>659</v>
       </c>
-      <c r="X129" s="1"/>
+      <c r="X129" s="1">
+        <v>200</v>
+      </c>
       <c r="Y129" s="1" t="s">
         <v>690</v>
       </c>
@@ -21365,7 +21395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A130">
         <v>53000127</v>
       </c>
@@ -21459,7 +21489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A131">
         <v>53000128</v>
       </c>
@@ -21553,7 +21583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A132">
         <v>53000129</v>
       </c>
@@ -21617,7 +21647,7 @@
         <v>103</v>
       </c>
       <c r="V132" s="11" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="W132" s="1" t="s">
         <v>675</v>
@@ -21647,7 +21677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:31" ht="96" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:31" ht="96" hidden="1" x14ac:dyDescent="0.15">
       <c r="A133">
         <v>53000130</v>
       </c>
@@ -21741,7 +21771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A134">
         <v>53000131</v>
       </c>
@@ -21835,7 +21865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A135">
         <v>53000132</v>
       </c>
@@ -22111,7 +22141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:31" ht="84" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:31" ht="84" hidden="1" x14ac:dyDescent="0.15">
       <c r="A138">
         <v>53000135</v>
       </c>
@@ -22204,7 +22234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:31" ht="108" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:31" ht="108" hidden="1" x14ac:dyDescent="0.15">
       <c r="A139">
         <v>53000136</v>
       </c>
@@ -22297,7 +22327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A140">
         <v>53000137</v>
       </c>
@@ -22367,7 +22397,9 @@
       <c r="W140" s="1" t="s">
         <v>712</v>
       </c>
-      <c r="X140" s="1"/>
+      <c r="X140" s="1">
+        <v>1</v>
+      </c>
       <c r="Y140" s="15" t="s">
         <v>4</v>
       </c>
@@ -22388,7 +22420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A141">
         <v>53000138</v>
       </c>
@@ -22458,7 +22490,9 @@
       <c r="W141" s="1" t="s">
         <v>729</v>
       </c>
-      <c r="X141" s="1"/>
+      <c r="X141" s="1">
+        <v>1</v>
+      </c>
       <c r="Y141" s="1" t="s">
         <v>614</v>
       </c>
@@ -22479,7 +22513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:31" ht="84" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:31" ht="84" hidden="1" x14ac:dyDescent="0.15">
       <c r="A142">
         <v>53000139</v>
       </c>
@@ -22549,7 +22583,9 @@
       <c r="W142" s="1" t="s">
         <v>726</v>
       </c>
-      <c r="X142" s="1"/>
+      <c r="X142" s="1">
+        <v>1</v>
+      </c>
       <c r="Y142" s="15" t="s">
         <v>731</v>
       </c>
@@ -22570,7 +22606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A143">
         <v>53000140</v>
       </c>
@@ -22640,7 +22676,9 @@
       <c r="W143" s="1" t="s">
         <v>730</v>
       </c>
-      <c r="X143" s="1"/>
+      <c r="X143" s="1">
+        <v>1</v>
+      </c>
       <c r="Y143" s="15" t="s">
         <v>731</v>
       </c>
@@ -22661,15 +22699,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:31" ht="144" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:31" ht="144" hidden="1" x14ac:dyDescent="0.15">
       <c r="A144">
         <v>53000141</v>
       </c>
       <c r="B144" s="22" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C144" s="15" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="D144" s="25" t="s">
         <v>753</v>
@@ -22726,19 +22764,19 @@
       </c>
       <c r="U144" s="15"/>
       <c r="V144" s="11" t="s">
+        <v>913</v>
+      </c>
+      <c r="W144" s="1" t="s">
         <v>914</v>
-      </c>
-      <c r="W144" s="1" t="s">
-        <v>915</v>
       </c>
       <c r="X144" s="7">
         <v>102</v>
       </c>
       <c r="Y144" s="15" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="Z144" s="15" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="AA144" s="15">
         <v>11000005</v>
@@ -22756,18 +22794,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:31" ht="48" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:31" ht="48" hidden="1" x14ac:dyDescent="0.15">
       <c r="A145">
         <v>53000142</v>
       </c>
       <c r="B145" s="22" t="s">
+        <v>918</v>
+      </c>
+      <c r="C145" s="15" t="s">
         <v>919</v>
       </c>
-      <c r="C145" s="15" t="s">
+      <c r="D145" s="44" t="s">
         <v>920</v>
-      </c>
-      <c r="D145" s="44" t="s">
-        <v>921</v>
       </c>
       <c r="E145" s="15">
         <v>3</v>
@@ -22821,16 +22859,16 @@
       </c>
       <c r="U145" s="15"/>
       <c r="V145" s="11" t="s">
+        <v>921</v>
+      </c>
+      <c r="W145" s="1" t="s">
         <v>922</v>
-      </c>
-      <c r="W145" s="1" t="s">
-        <v>923</v>
       </c>
       <c r="X145" s="7">
         <v>100</v>
       </c>
       <c r="Y145" s="15" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="Z145" s="15"/>
       <c r="AA145" s="15">
@@ -22849,15 +22887,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:31" ht="48" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:31" ht="48" hidden="1" x14ac:dyDescent="0.15">
       <c r="A146">
         <v>53000143</v>
       </c>
       <c r="B146" s="22" t="s">
+        <v>923</v>
+      </c>
+      <c r="C146" s="15" t="s">
         <v>924</v>
-      </c>
-      <c r="C146" s="15" t="s">
-        <v>925</v>
       </c>
       <c r="D146" s="25" t="s">
         <v>394</v>
@@ -22907,17 +22945,17 @@
         <v>0</v>
       </c>
       <c r="S146" s="15" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="T146" s="15">
         <v>105</v>
       </c>
       <c r="U146" s="15"/>
       <c r="V146" s="11" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="W146" s="1" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="X146" s="1">
         <v>201</v>
@@ -22942,18 +22980,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:31" ht="48" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:31" ht="48" hidden="1" x14ac:dyDescent="0.15">
       <c r="A147">
         <v>53000144</v>
       </c>
       <c r="B147" s="22" t="s">
+        <v>937</v>
+      </c>
+      <c r="C147" s="15" t="s">
         <v>938</v>
       </c>
-      <c r="C147" s="15" t="s">
-        <v>939</v>
-      </c>
       <c r="D147" s="44" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="E147" s="15">
         <v>2</v>
@@ -23007,10 +23045,10 @@
       </c>
       <c r="U147" s="15"/>
       <c r="V147" s="11" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="W147" s="1" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="X147" s="7">
         <v>100</v>
@@ -23035,15 +23073,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:31" ht="120" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:31" ht="120" hidden="1" x14ac:dyDescent="0.15">
       <c r="A148">
         <v>53000145</v>
       </c>
       <c r="B148" s="22" t="s">
+        <v>939</v>
+      </c>
+      <c r="C148" s="15" t="s">
         <v>940</v>
-      </c>
-      <c r="C148" s="15" t="s">
-        <v>941</v>
       </c>
       <c r="D148" s="25" t="s">
         <v>394</v>
@@ -23099,19 +23137,19 @@
         <v>102</v>
       </c>
       <c r="V148" s="11" t="s">
+        <v>945</v>
+      </c>
+      <c r="W148" s="1" t="s">
         <v>946</v>
-      </c>
-      <c r="W148" s="1" t="s">
-        <v>947</v>
       </c>
       <c r="X148" s="1">
         <v>202</v>
       </c>
       <c r="Y148" s="1" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="Z148" s="1" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="AA148" s="1">
         <v>11000001</v>
@@ -23305,7 +23343,7 @@
         <v>368</v>
       </c>
       <c r="U1" s="13" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="V1" s="13" t="s">
         <v>338</v>
@@ -23314,7 +23352,7 @@
         <v>298</v>
       </c>
       <c r="X1" s="13" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="Y1" s="13" t="s">
         <v>367</v>
@@ -23400,7 +23438,7 @@
         <v>456</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>475</v>
@@ -23409,7 +23447,7 @@
         <v>176</v>
       </c>
       <c r="X2" s="10" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="Y2" s="4" t="s">
         <v>176</v>
@@ -23495,7 +23533,7 @@
         <v>369</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="V3" s="6" t="s">
         <v>297</v>
@@ -23504,7 +23542,7 @@
         <v>299</v>
       </c>
       <c r="X3" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="Y3" s="6" t="s">
         <v>315</v>
@@ -23536,7 +23574,7 @@
         <v>352</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="D4" s="32"/>
       <c r="E4" s="15">
@@ -23625,7 +23663,7 @@
         <v>320</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D5" s="32"/>
       <c r="E5" s="15">
@@ -23714,7 +23752,7 @@
         <v>355</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="D6" s="32"/>
       <c r="E6" s="15">
@@ -23801,7 +23839,7 @@
         <v>356</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="D7" s="32"/>
       <c r="E7" s="15">
@@ -23888,7 +23926,7 @@
         <v>357</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="D8" s="32"/>
       <c r="E8" s="15">
@@ -23975,7 +24013,7 @@
         <v>358</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="D9" s="32"/>
       <c r="E9" s="15">
@@ -24064,7 +24102,7 @@
         <v>474</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="15">
@@ -24118,10 +24156,10 @@
         <v>-1</v>
       </c>
       <c r="U10" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="V10" s="11" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="W10" s="7" t="s">
         <v>476</v>
@@ -24155,7 +24193,7 @@
         <v>506</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="D11" s="32"/>
       <c r="E11" s="15">
@@ -24244,7 +24282,7 @@
         <v>662</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="D12" s="32"/>
       <c r="E12" s="15">
@@ -24331,7 +24369,7 @@
         <v>735</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="D13" s="32"/>
       <c r="E13" s="15">
@@ -24420,7 +24458,7 @@
         <v>739</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="D14" s="42"/>
       <c r="E14" s="15">
@@ -24508,7 +24546,7 @@
         <v>746</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="D15" s="32"/>
       <c r="E15" s="15">
@@ -24715,7 +24753,7 @@
         <v>368</v>
       </c>
       <c r="U1" s="13" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="V1" s="13" t="s">
         <v>338</v>
@@ -24724,7 +24762,7 @@
         <v>298</v>
       </c>
       <c r="X1" s="13" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="Y1" s="13" t="s">
         <v>367</v>
@@ -24810,7 +24848,7 @@
         <v>456</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>314</v>
@@ -24819,7 +24857,7 @@
         <v>176</v>
       </c>
       <c r="X2" s="10" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="Y2" s="4" t="s">
         <v>176</v>
@@ -24905,7 +24943,7 @@
         <v>369</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="V3" s="6" t="s">
         <v>297</v>
@@ -24914,7 +24952,7 @@
         <v>299</v>
       </c>
       <c r="X3" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="Y3" s="6" t="s">
         <v>315</v>

</xml_diff>

<commit_message>
TrapHolder shared by the system. show hand card count on player life clock
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -636,7 +636,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="979">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1485" uniqueCount="980">
   <si>
     <t>慈悲</t>
   </si>
@@ -4145,6 +4145,10 @@
   </si>
   <si>
     <t>p.Action.AddRandomMonster(-1,spl.Level,m.GetRandomPoint(p.IsLeft, true, true));</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>p.Action.CanUseTrap()</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -9494,7 +9498,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W6" sqref="W6"/>
+      <selection pane="bottomRight" activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -12503,6 +12507,9 @@
       <c r="T33">
         <v>100</v>
       </c>
+      <c r="U33" t="s">
+        <v>979</v>
+      </c>
       <c r="V33" s="11" t="s">
         <v>829</v>
       </c>
@@ -12593,6 +12600,9 @@
       <c r="T34">
         <v>100</v>
       </c>
+      <c r="U34" t="s">
+        <v>979</v>
+      </c>
       <c r="V34" s="11" t="s">
         <v>830</v>
       </c>
@@ -13334,6 +13344,9 @@
       <c r="T42">
         <v>85</v>
       </c>
+      <c r="U42" t="s">
+        <v>979</v>
+      </c>
       <c r="V42" s="11" t="s">
         <v>831</v>
       </c>
@@ -13424,6 +13437,9 @@
       <c r="T43">
         <v>100</v>
       </c>
+      <c r="U43" t="s">
+        <v>979</v>
+      </c>
       <c r="V43" s="11" t="s">
         <v>832</v>
       </c>
@@ -13788,6 +13804,9 @@
       <c r="T47">
         <v>95</v>
       </c>
+      <c r="U47" t="s">
+        <v>979</v>
+      </c>
       <c r="V47" s="11" t="s">
         <v>833</v>
       </c>
@@ -15812,6 +15831,9 @@
       <c r="T69">
         <v>85</v>
       </c>
+      <c r="U69" t="s">
+        <v>979</v>
+      </c>
       <c r="V69" s="11" t="s">
         <v>836</v>
       </c>
@@ -22030,7 +22052,9 @@
       <c r="T136" s="15">
         <v>100</v>
       </c>
-      <c r="U136" s="15"/>
+      <c r="U136" t="s">
+        <v>979</v>
+      </c>
       <c r="V136" s="11" t="s">
         <v>846</v>
       </c>
@@ -22121,7 +22145,9 @@
       <c r="T137" s="15">
         <v>103</v>
       </c>
-      <c r="U137" s="15"/>
+      <c r="U137" t="s">
+        <v>979</v>
+      </c>
       <c r="V137" s="11" t="s">
         <v>847</v>
       </c>

</xml_diff>

<commit_message>
add a hasweapon api
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -636,7 +636,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1485" uniqueCount="980">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="981">
   <si>
     <t>慈悲</t>
   </si>
@@ -4149,6 +4149,10 @@
   </si>
   <si>
     <t>p.Action.CanUseTrap()</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>t.Action.HasWeapon()</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -9032,7 +9036,16 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AE148" totalsRowShown="0" headerRowDxfId="109" dataDxfId="108" tableBorderDxfId="107">
-  <autoFilter ref="A3:AE148"/>
+  <autoFilter ref="A3:AE148">
+    <filterColumn colId="23">
+      <filters>
+        <filter val="100"/>
+        <filter val="101"/>
+        <filter val="200"/>
+        <filter val="201"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A4:AE113">
     <sortCondition ref="A3:A113"/>
   </sortState>
@@ -9495,10 +9508,10 @@
   <dimension ref="A1:AE148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="D129" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="T7" sqref="T7"/>
+      <selection pane="bottomRight" activeCell="U146" sqref="U146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9811,7 +9824,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>53000001</v>
       </c>
@@ -9901,7 +9914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:31" hidden="1" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>53000002</v>
       </c>
@@ -10171,7 +10184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>53000005</v>
       </c>
@@ -10263,7 +10276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="48" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:31" ht="48" hidden="1" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>53000006</v>
       </c>
@@ -10351,7 +10364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="48" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:31" ht="48" hidden="1" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>53000007</v>
       </c>
@@ -10439,7 +10452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:31" ht="48" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:31" ht="48" hidden="1" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>53000008</v>
       </c>
@@ -10527,7 +10540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="48" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:31" ht="48" hidden="1" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>53000009</v>
       </c>
@@ -10615,7 +10628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:31" ht="48" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:31" ht="48" hidden="1" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>53000010</v>
       </c>
@@ -10703,7 +10716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="48" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:31" ht="48" hidden="1" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>53000011</v>
       </c>
@@ -10791,7 +10804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:31" ht="48" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:31" ht="48" hidden="1" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>53000012</v>
       </c>
@@ -10971,7 +10984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>53000014</v>
       </c>
@@ -11431,7 +11444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>53000019</v>
       </c>
@@ -11525,7 +11538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>53000020</v>
       </c>
@@ -11619,7 +11632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>53000021</v>
       </c>
@@ -11713,7 +11726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>53000022</v>
       </c>
@@ -11805,7 +11818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>53000023</v>
       </c>
@@ -11895,7 +11908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>53000024</v>
       </c>
@@ -12079,7 +12092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:31" hidden="1" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>53000026</v>
       </c>
@@ -12444,7 +12457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>53000030</v>
       </c>
@@ -12537,7 +12550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>53000031</v>
       </c>
@@ -12630,7 +12643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>53000032</v>
       </c>
@@ -12727,7 +12740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>53000033</v>
       </c>
@@ -12821,7 +12834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>53000034</v>
       </c>
@@ -12913,7 +12926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>53000035</v>
       </c>
@@ -13007,7 +13020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>53000036</v>
       </c>
@@ -13187,7 +13200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>53000038</v>
       </c>
@@ -13281,7 +13294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>53000039</v>
       </c>
@@ -13374,7 +13387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>53000040</v>
       </c>
@@ -13557,7 +13570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>53000042</v>
       </c>
@@ -13651,7 +13664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>53000043</v>
       </c>
@@ -13741,7 +13754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>53000044</v>
       </c>
@@ -13834,7 +13847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:31" ht="96" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:31" ht="96" hidden="1" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>53000045</v>
       </c>
@@ -13926,7 +13939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:31" ht="48" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:31" ht="48" hidden="1" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>53000046</v>
       </c>
@@ -14018,7 +14031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>53000047</v>
       </c>
@@ -14204,7 +14217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>53000049</v>
       </c>
@@ -14298,7 +14311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A53">
         <v>53000050</v>
       </c>
@@ -14388,7 +14401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:31" ht="96" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:31" ht="96" hidden="1" x14ac:dyDescent="0.15">
       <c r="A54">
         <v>53000051</v>
       </c>
@@ -14574,7 +14587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A56">
         <v>53000053</v>
       </c>
@@ -14758,7 +14771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A58">
         <v>53000055</v>
       </c>
@@ -14850,7 +14863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A59">
         <v>53000056</v>
       </c>
@@ -15034,7 +15047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A61">
         <v>53000058</v>
       </c>
@@ -15310,7 +15323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:31" ht="48" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:31" ht="48" hidden="1" x14ac:dyDescent="0.15">
       <c r="A64">
         <v>53000061</v>
       </c>
@@ -15494,7 +15507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:31" hidden="1" x14ac:dyDescent="0.15">
       <c r="A66">
         <v>53000063</v>
       </c>
@@ -15584,7 +15597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A67">
         <v>53000064</v>
       </c>
@@ -15676,7 +15689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:31" ht="48" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:31" ht="48" hidden="1" x14ac:dyDescent="0.15">
       <c r="A68">
         <v>53000065</v>
       </c>
@@ -15768,7 +15781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A69">
         <v>53000066</v>
       </c>
@@ -15953,7 +15966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A71">
         <v>53000068</v>
       </c>
@@ -16231,7 +16244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A74">
         <v>53000071</v>
       </c>
@@ -16417,7 +16430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:31" ht="48" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:31" ht="48" hidden="1" x14ac:dyDescent="0.15">
       <c r="A76">
         <v>53000073</v>
       </c>
@@ -16693,7 +16706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A79">
         <v>53000076</v>
       </c>
@@ -16787,7 +16800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:31" ht="48" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:31" ht="48" hidden="1" x14ac:dyDescent="0.15">
       <c r="A80">
         <v>53000077</v>
       </c>
@@ -16879,7 +16892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A81">
         <v>53000078</v>
       </c>
@@ -16967,7 +16980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:31" ht="96" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:31" ht="96" hidden="1" x14ac:dyDescent="0.15">
       <c r="A82">
         <v>53000079</v>
       </c>
@@ -17061,7 +17074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A83">
         <v>53000080</v>
       </c>
@@ -17155,7 +17168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A84">
         <v>53000081</v>
       </c>
@@ -17341,7 +17354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:31" ht="48" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:31" ht="48" hidden="1" x14ac:dyDescent="0.15">
       <c r="A86">
         <v>53000083</v>
       </c>
@@ -17433,7 +17446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A87">
         <v>53000084</v>
       </c>
@@ -17525,7 +17538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A88">
         <v>53000085</v>
       </c>
@@ -17622,7 +17635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A89">
         <v>53000086</v>
       </c>
@@ -17808,7 +17821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A91">
         <v>53000088</v>
       </c>
@@ -17902,7 +17915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A92">
         <v>53000089</v>
       </c>
@@ -17996,7 +18009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A93">
         <v>53000090</v>
       </c>
@@ -18180,7 +18193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A95">
         <v>53000092</v>
       </c>
@@ -18364,7 +18377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A97">
         <v>53000094</v>
       </c>
@@ -18454,7 +18467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A98">
         <v>53000095</v>
       </c>
@@ -18548,7 +18561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A99">
         <v>53000096</v>
       </c>
@@ -18640,7 +18653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A100">
         <v>53000097</v>
       </c>
@@ -18732,7 +18745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:31" ht="24" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:31" ht="24" hidden="1" x14ac:dyDescent="0.15">
       <c r="A101">
         <v>53000098</v>
       </c>
@@ -18916,7 +18929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:31" ht="96" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:31" ht="96" hidden="1" x14ac:dyDescent="0.15">
       <c r="A103">
         <v>53000100</v>
       </c>
@@ -19190,7 +19203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:31" ht="96" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:31" ht="96" hidden="1" x14ac:dyDescent="0.15">
       <c r="A106">
         <v>53000103</v>
       </c>
@@ -19284,7 +19297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:31" ht="132" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:31" ht="132" hidden="1" x14ac:dyDescent="0.15">
       <c r="A107">
         <v>53000104</v>
       </c>
@@ -19558,7 +19571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A110">
         <v>53000107</v>
       </c>
@@ -19836,7 +19849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:31" ht="48" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:31" ht="48" hidden="1" x14ac:dyDescent="0.15">
       <c r="A113">
         <v>53000110</v>
       </c>
@@ -20022,7 +20035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:31" ht="48" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:31" ht="48" hidden="1" x14ac:dyDescent="0.15">
       <c r="A115">
         <v>53000112</v>
       </c>
@@ -20583,7 +20596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A121">
         <v>53000118</v>
       </c>
@@ -20860,7 +20873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A124">
         <v>53000121</v>
       </c>
@@ -21425,7 +21438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A130">
         <v>53000127</v>
       </c>
@@ -21519,7 +21532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A131">
         <v>53000128</v>
       </c>
@@ -21707,7 +21720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:31" ht="96" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:31" ht="96" hidden="1" x14ac:dyDescent="0.15">
       <c r="A133">
         <v>53000130</v>
       </c>
@@ -21801,7 +21814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A134">
         <v>53000131</v>
       </c>
@@ -21989,7 +22002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A136">
         <v>53000133</v>
       </c>
@@ -22082,7 +22095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:31" ht="36" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:31" ht="36" hidden="1" x14ac:dyDescent="0.15">
       <c r="A137">
         <v>53000134</v>
       </c>
@@ -22268,7 +22281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:31" ht="108" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:31" ht="108" hidden="1" x14ac:dyDescent="0.15">
       <c r="A139">
         <v>53000136</v>
       </c>
@@ -22361,7 +22374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A140">
         <v>53000137</v>
       </c>
@@ -22454,7 +22467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:31" ht="60" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.15">
       <c r="A141">
         <v>53000138</v>
       </c>
@@ -22547,7 +22560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:31" ht="84" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:31" ht="84" hidden="1" x14ac:dyDescent="0.15">
       <c r="A142">
         <v>53000139</v>
       </c>
@@ -22640,7 +22653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:31" ht="72" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:31" ht="72" hidden="1" x14ac:dyDescent="0.15">
       <c r="A143">
         <v>53000140</v>
       </c>
@@ -22733,7 +22746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:31" ht="144" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:31" ht="144" hidden="1" x14ac:dyDescent="0.15">
       <c r="A144">
         <v>53000141</v>
       </c>
@@ -22984,7 +22997,9 @@
       <c r="T146" s="15">
         <v>105</v>
       </c>
-      <c r="U146" s="15"/>
+      <c r="U146" s="11" t="s">
+        <v>980</v>
+      </c>
       <c r="V146" s="11" t="s">
         <v>927</v>
       </c>
@@ -23107,7 +23122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:31" ht="120" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:31" ht="120" hidden="1" x14ac:dyDescent="0.15">
       <c r="A148">
         <v>53000145</v>
       </c>

</xml_diff>

<commit_message>
fix a weapon return bug
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spell.xlsx
+++ b/ConfigData/Xlsx/Spell.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{97D75370-EF34-4D37-B981-5DE147DA37BD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="标准" sheetId="1" r:id="rId1"/>
@@ -23,13 +24,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>real</author>
     <author>Real</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -56,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -83,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -109,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -135,7 +136,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -161,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0">
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -187,7 +188,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V2" authorId="1" shapeId="0">
+    <comment ref="V2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -206,13 +207,13 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>real</author>
     <author>Real</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -239,7 +240,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -266,7 +267,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -292,7 +293,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -318,7 +319,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -344,7 +345,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V2" authorId="1" shapeId="0">
+    <comment ref="V2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -421,13 +422,13 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>real</author>
     <author>Real</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -454,7 +455,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -481,7 +482,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -507,7 +508,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -533,7 +534,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
       <text>
         <r>
           <rPr>
@@ -559,7 +560,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V2" authorId="1" shapeId="0">
+    <comment ref="V2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
       <text>
         <r>
           <rPr>
@@ -3937,10 +3938,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>t.Action.WeaponReturn();if(MathTool.GetRandom(100)&lt;spl.Rate)t.Action.WeaponReturn();</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>foreach(IMonster im in m.GetRangeMonster(p.IsLeft,spl.Target,spl.Shape,spl.Range,mouse))im.Action.AddAttrModify("Spell",spl.Id,"Atk",-spl.Atk);</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -4167,13 +4164,17 @@
   </si>
   <si>
     <t>firearrow</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>t.Action.WeaponReturn();if(MathTool.GetRandom(100)&lt;spl.Rate)t.Action.WeaponReturn();t.Action.BreakWeapon();</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -8056,74 +8057,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -9049,141 +8982,141 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AE148" totalsRowShown="0" headerRowDxfId="109" dataDxfId="108" tableBorderDxfId="107">
-  <autoFilter ref="A3:AE148"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:AE148" totalsRowShown="0" headerRowDxfId="109" dataDxfId="108" tableBorderDxfId="107">
+  <autoFilter ref="A3:AE148" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A4:AE113">
     <sortCondition ref="A3:A113"/>
   </sortState>
   <tableColumns count="31">
-    <tableColumn id="1" name="Id" dataDxfId="106"/>
-    <tableColumn id="2" name="Name" dataDxfId="105"/>
-    <tableColumn id="20" name="Ename" dataDxfId="104"/>
-    <tableColumn id="21" name="Remark" dataDxfId="103"/>
-    <tableColumn id="3" name="Star" dataDxfId="102"/>
-    <tableColumn id="4" name="Type" dataDxfId="101"/>
-    <tableColumn id="5" name="Attr" dataDxfId="100"/>
-    <tableColumn id="8" name="Quality" dataDxfId="99">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="106"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="105"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Ename" dataDxfId="104"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Remark" dataDxfId="103"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Star" dataDxfId="102"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Type" dataDxfId="101"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Attr" dataDxfId="100"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Quality" dataDxfId="99">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,IF(AND(Q4&gt;=-5,Q4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="98"/>
-    <tableColumn id="9" name="Damage" dataDxfId="97"/>
-    <tableColumn id="10" name="Cure" dataDxfId="96"/>
-    <tableColumn id="11" name="Time" dataDxfId="95"/>
-    <tableColumn id="13" name="Help" dataDxfId="94"/>
-    <tableColumn id="16" name="Rate" dataDxfId="93"/>
-    <tableColumn id="18" name="Atk" dataDxfId="92"/>
-    <tableColumn id="12" name="Modify" dataDxfId="91"/>
-    <tableColumn id="27" name="Sum" dataDxfId="90">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Cost" dataDxfId="98"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Damage" dataDxfId="97"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Cure" dataDxfId="96"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Time" dataDxfId="95"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Help" dataDxfId="94"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Rate" dataDxfId="93"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Atk" dataDxfId="92"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Modify" dataDxfId="91"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Sum" dataDxfId="90">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="89"/>
-    <tableColumn id="15" name="Target" dataDxfId="88"/>
-    <tableColumn id="25" name="Mark" dataDxfId="87"/>
-    <tableColumn id="31" name="CanCast" dataDxfId="86"/>
-    <tableColumn id="22" name="Effect" dataDxfId="85"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="84"/>
-    <tableColumn id="30" name="AIGuide" dataDxfId="83"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="82"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="81"/>
-    <tableColumn id="26" name="JobId" dataDxfId="80"/>
-    <tableColumn id="19" name="Icon" dataDxfId="79"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="78"/>
-    <tableColumn id="29" name="IsHeroCard" dataDxfId="77"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="76"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Range" dataDxfId="89"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Target" dataDxfId="88"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Mark" dataDxfId="87"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="CanCast" dataDxfId="86"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Effect" dataDxfId="85"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="GetDescript" dataDxfId="84"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="AIGuide" dataDxfId="83"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="UnitEffect" dataDxfId="82"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="AreaEffect" dataDxfId="81"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="JobId" dataDxfId="80"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Icon" dataDxfId="79"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="IsSpecial" dataDxfId="78"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="IsHeroCard" dataDxfId="77"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="IsNew" dataDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AE15" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69" tableBorderDxfId="68">
-  <autoFilter ref="A3:AE15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表1_3" displayName="表1_3" ref="A3:AE15" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69" tableBorderDxfId="68">
+  <autoFilter ref="A3:AE15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState ref="A4:Z138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="31">
-    <tableColumn id="1" name="Id" dataDxfId="67"/>
-    <tableColumn id="2" name="Name" dataDxfId="66"/>
-    <tableColumn id="20" name="Ename" dataDxfId="65"/>
-    <tableColumn id="21" name="Remark" dataDxfId="64"/>
-    <tableColumn id="3" name="Star" dataDxfId="63"/>
-    <tableColumn id="4" name="Type" dataDxfId="62"/>
-    <tableColumn id="5" name="Attr" dataDxfId="61"/>
-    <tableColumn id="8" name="Quality" dataDxfId="60">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id" dataDxfId="67"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="66"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="Ename" dataDxfId="65"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="Remark" dataDxfId="64"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Star" dataDxfId="63"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Type" dataDxfId="62"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Attr" dataDxfId="61"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Quality" dataDxfId="60">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="59"/>
-    <tableColumn id="9" name="Damage" dataDxfId="58"/>
-    <tableColumn id="10" name="Cure" dataDxfId="57"/>
-    <tableColumn id="11" name="Time" dataDxfId="56"/>
-    <tableColumn id="13" name="Help" dataDxfId="55"/>
-    <tableColumn id="16" name="Rate" dataDxfId="54"/>
-    <tableColumn id="18" name="Atk" dataDxfId="53"/>
-    <tableColumn id="12" name="Modify" dataDxfId="52"/>
-    <tableColumn id="27" name="Sum" dataDxfId="51">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Cost" dataDxfId="59"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Damage" dataDxfId="58"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Cure" dataDxfId="57"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Time" dataDxfId="56"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Help" dataDxfId="55"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Rate" dataDxfId="54"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Atk" dataDxfId="53"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Modify" dataDxfId="52"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0100-00001B000000}" name="Sum" dataDxfId="51">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="50"/>
-    <tableColumn id="15" name="Target" dataDxfId="49"/>
-    <tableColumn id="25" name="Mark" dataDxfId="48"/>
-    <tableColumn id="31" name="CanCast" dataDxfId="47"/>
-    <tableColumn id="22" name="Effect" dataDxfId="46"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="45"/>
-    <tableColumn id="30" name="AIGuide" dataDxfId="44"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="43"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="42"/>
-    <tableColumn id="26" name="JobId" dataDxfId="41"/>
-    <tableColumn id="19" name="Icon" dataDxfId="40"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="39"/>
-    <tableColumn id="29" name="IsHeroCard" dataDxfId="38"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Range" dataDxfId="50"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Target" dataDxfId="49"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0100-000019000000}" name="Mark" dataDxfId="48"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0100-00001F000000}" name="CanCast" dataDxfId="47"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="Effect" dataDxfId="46"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0100-000018000000}" name="GetDescript" dataDxfId="45"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0100-00001E000000}" name="AIGuide" dataDxfId="44"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="UnitEffect" dataDxfId="43"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0100-00001C000000}" name="AreaEffect" dataDxfId="42"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0100-00001A000000}" name="JobId" dataDxfId="41"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="Icon" dataDxfId="40"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="IsSpecial" dataDxfId="39"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0100-00001D000000}" name="IsHeroCard" dataDxfId="38"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="IsNew" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表1_35" displayName="表1_35" ref="A3:AE9" totalsRowShown="0" headerRowDxfId="31" tableBorderDxfId="30">
-  <autoFilter ref="A3:AE9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="表1_35" displayName="表1_35" ref="A3:AE9" totalsRowShown="0" headerRowDxfId="31" tableBorderDxfId="30">
+  <autoFilter ref="A3:AE9" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <sortState ref="A4:Z138">
     <sortCondition ref="A3:A138"/>
   </sortState>
   <tableColumns count="31">
-    <tableColumn id="1" name="Id" dataDxfId="29"/>
-    <tableColumn id="2" name="Name" dataDxfId="28"/>
-    <tableColumn id="20" name="Ename" dataDxfId="27"/>
-    <tableColumn id="21" name="Remark" dataDxfId="26"/>
-    <tableColumn id="3" name="Star" dataDxfId="25"/>
-    <tableColumn id="4" name="Type" dataDxfId="24"/>
-    <tableColumn id="5" name="Attr" dataDxfId="23"/>
-    <tableColumn id="8" name="Quality" dataDxfId="22">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Id" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="28"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0200-000014000000}" name="Ename" dataDxfId="27"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0200-000015000000}" name="Remark" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Star" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Type" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Attr" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Quality" dataDxfId="22">
       <calculatedColumnFormula>IF(AND(Q4&gt;=13,Q4&lt;=16),5,IF(AND(Q4&gt;=9,Q4&lt;=12),4,IF(AND(Q4&gt;=5,Q4&lt;=8),3,IF(AND(Q4&gt;=1,Q4&lt;=4),2,IF(AND(Q4&gt;=-3,Q4&lt;=0),1,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Cost" dataDxfId="21"/>
-    <tableColumn id="9" name="Damage" dataDxfId="20"/>
-    <tableColumn id="10" name="Cure" dataDxfId="19"/>
-    <tableColumn id="11" name="Time" dataDxfId="18"/>
-    <tableColumn id="13" name="Help" dataDxfId="17"/>
-    <tableColumn id="16" name="Rate" dataDxfId="16"/>
-    <tableColumn id="18" name="Atk" dataDxfId="15"/>
-    <tableColumn id="12" name="Modify" dataDxfId="14"/>
-    <tableColumn id="27" name="Sum" dataDxfId="13">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Cost" dataDxfId="21"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Damage" dataDxfId="20"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Cure" dataDxfId="19"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Time" dataDxfId="18"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="Help" dataDxfId="17"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="Rate" dataDxfId="16"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0200-000012000000}" name="Atk" dataDxfId="15"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Modify" dataDxfId="14"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0200-00001B000000}" name="Sum" dataDxfId="13">
       <calculatedColumnFormula>T4-100+P4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Range" dataDxfId="12"/>
-    <tableColumn id="15" name="Target" dataDxfId="11"/>
-    <tableColumn id="25" name="Mark" dataDxfId="10"/>
-    <tableColumn id="31" name="CanCast"/>
-    <tableColumn id="22" name="Effect" dataDxfId="9"/>
-    <tableColumn id="24" name="GetDescript" dataDxfId="8"/>
-    <tableColumn id="30" name="AIGuide" dataDxfId="7"/>
-    <tableColumn id="17" name="UnitEffect" dataDxfId="6"/>
-    <tableColumn id="28" name="AreaEffect" dataDxfId="5"/>
-    <tableColumn id="26" name="JobId" dataDxfId="4"/>
-    <tableColumn id="19" name="Icon" dataDxfId="3"/>
-    <tableColumn id="14" name="IsSpecial" dataDxfId="2"/>
-    <tableColumn id="29" name="IsHeroCard" dataDxfId="1"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Range" dataDxfId="12"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="Target" dataDxfId="11"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0200-000019000000}" name="Mark" dataDxfId="10"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0200-00001F000000}" name="CanCast"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0200-000016000000}" name="Effect" dataDxfId="9"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0200-000018000000}" name="GetDescript" dataDxfId="8"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0200-00001E000000}" name="AIGuide" dataDxfId="7"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0200-000011000000}" name="UnitEffect" dataDxfId="6"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0200-00001C000000}" name="AreaEffect" dataDxfId="5"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0200-00001A000000}" name="JobId" dataDxfId="4"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0200-000013000000}" name="Icon" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="IsSpecial" dataDxfId="2"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0200-00001D000000}" name="IsHeroCard" dataDxfId="1"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0200-000017000000}" name="IsNew" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9197,7 +9130,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -9509,14 +9442,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C145" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P7" sqref="P7"/>
+      <selection pane="bottomRight" activeCell="V146" sqref="V146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9606,7 +9539,7 @@
         <v>366</v>
       </c>
       <c r="U1" s="13" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="V1" s="13" t="s">
         <v>336</v>
@@ -9615,7 +9548,7 @@
         <v>296</v>
       </c>
       <c r="X1" s="13" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="Y1" s="13" t="s">
         <v>365</v>
@@ -9701,7 +9634,7 @@
         <v>454</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>312</v>
@@ -9710,7 +9643,7 @@
         <v>174</v>
       </c>
       <c r="X2" s="10" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="Y2" s="4" t="s">
         <v>174</v>
@@ -9796,7 +9729,7 @@
         <v>367</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="V3" s="6" t="s">
         <v>436</v>
@@ -9805,7 +9738,7 @@
         <v>506</v>
       </c>
       <c r="X3" s="6" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="Y3" s="6" t="s">
         <v>313</v>
@@ -9893,7 +9826,7 @@
         <v>95</v>
       </c>
       <c r="V4" s="11" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="W4" s="7" t="s">
         <v>705</v>
@@ -10161,7 +10094,7 @@
         <v>100</v>
       </c>
       <c r="V7" s="11" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="W7" s="7" t="s">
         <v>677</v>
@@ -10256,7 +10189,7 @@
         <v>825</v>
       </c>
       <c r="W8" s="7" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="X8" s="7">
         <v>102</v>
@@ -11000,7 +10933,7 @@
         <v>440</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="E17" s="1">
         <v>2</v>
@@ -11184,7 +11117,7 @@
         <v>214</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="E19" s="1">
         <v>3</v>
@@ -11237,10 +11170,10 @@
         <v>95</v>
       </c>
       <c r="V19" s="11" t="s">
+        <v>930</v>
+      </c>
+      <c r="W19" s="7" t="s">
         <v>931</v>
-      </c>
-      <c r="W19" s="7" t="s">
-        <v>932</v>
       </c>
       <c r="X19" s="7">
         <v>100</v>
@@ -11421,7 +11354,7 @@
         <v>102</v>
       </c>
       <c r="V21" s="11" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="W21" s="7" t="s">
         <v>510</v>
@@ -11522,7 +11455,7 @@
         <v>102</v>
       </c>
       <c r="Y22" s="1" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="Z22" s="1" t="s">
         <v>21</v>
@@ -12155,16 +12088,16 @@
         <v>10</v>
       </c>
       <c r="S29" s="1" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="T29">
         <v>100</v>
       </c>
       <c r="U29" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="V29" s="11" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="W29" s="7" t="s">
         <v>463</v>
@@ -12526,7 +12459,7 @@
         <v>100</v>
       </c>
       <c r="U33" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="V33" s="11" t="s">
         <v>827</v>
@@ -12619,7 +12552,7 @@
         <v>100</v>
       </c>
       <c r="U34" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="V34" s="11" t="s">
         <v>828</v>
@@ -12712,10 +12645,10 @@
         <v>100</v>
       </c>
       <c r="U35" t="s">
+        <v>969</v>
+      </c>
+      <c r="V35" s="11" t="s">
         <v>970</v>
-      </c>
-      <c r="V35" s="11" t="s">
-        <v>971</v>
       </c>
       <c r="W35" s="7" t="s">
         <v>397</v>
@@ -13089,7 +13022,7 @@
         <v>100</v>
       </c>
       <c r="V39" s="11" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="W39" s="1" t="s">
         <v>526</v>
@@ -13363,7 +13296,7 @@
         <v>85</v>
       </c>
       <c r="U42" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="V42" s="11" t="s">
         <v>829</v>
@@ -13456,7 +13389,7 @@
         <v>100</v>
       </c>
       <c r="U43" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="V43" s="11" t="s">
         <v>830</v>
@@ -13823,7 +13756,7 @@
         <v>95</v>
       </c>
       <c r="U47" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="V47" s="11" t="s">
         <v>831</v>
@@ -14203,7 +14136,7 @@
         <v>100</v>
       </c>
       <c r="Y51" s="1" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="Z51" s="1"/>
       <c r="AA51" s="1">
@@ -14665,7 +14598,7 @@
         <v>102</v>
       </c>
       <c r="Y56" s="1" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="Z56" s="1"/>
       <c r="AA56" s="1">
@@ -15850,7 +15783,7 @@
         <v>85</v>
       </c>
       <c r="U69" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="V69" s="11" t="s">
         <v>834</v>
@@ -17607,10 +17540,10 @@
         <v>100</v>
       </c>
       <c r="U88" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="V88" s="11" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="W88" s="7" t="s">
         <v>755</v>
@@ -19189,7 +19122,7 @@
         <v>100</v>
       </c>
       <c r="Y105" s="1" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="Z105" s="1"/>
       <c r="AA105" s="1">
@@ -19366,10 +19299,10 @@
         <v>105</v>
       </c>
       <c r="V107" s="11" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="W107" s="7" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="X107" s="7">
         <v>102</v>
@@ -19640,10 +19573,10 @@
         <v>100</v>
       </c>
       <c r="V110" s="11" t="s">
+        <v>925</v>
+      </c>
+      <c r="W110" s="7" t="s">
         <v>926</v>
-      </c>
-      <c r="W110" s="7" t="s">
-        <v>927</v>
       </c>
       <c r="X110" s="7">
         <v>102</v>
@@ -20104,10 +20037,10 @@
         <v>100</v>
       </c>
       <c r="U115" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="V115" s="11" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="W115" s="7" t="s">
         <v>551</v>
@@ -21036,10 +20969,10 @@
         <v>101</v>
       </c>
       <c r="U125" s="11" t="s">
+        <v>966</v>
+      </c>
+      <c r="V125" s="11" t="s">
         <v>967</v>
-      </c>
-      <c r="V125" s="11" t="s">
-        <v>968</v>
       </c>
       <c r="W125" s="1" t="s">
         <v>639</v>
@@ -21516,10 +21449,10 @@
         <v>102</v>
       </c>
       <c r="Y130" s="1" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="Z130" s="1" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="AA130" s="1">
         <v>11000001</v>
@@ -21695,7 +21628,7 @@
         <v>103</v>
       </c>
       <c r="V132" s="11" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="W132" s="1" t="s">
         <v>673</v>
@@ -22071,7 +22004,7 @@
         <v>100</v>
       </c>
       <c r="U136" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="V136" s="11" t="s">
         <v>844</v>
@@ -22164,7 +22097,7 @@
         <v>103</v>
       </c>
       <c r="U137" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="V137" s="11" t="s">
         <v>845</v>
@@ -22920,7 +22853,7 @@
         <v>100</v>
       </c>
       <c r="Y145" s="15" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="Z145" s="15"/>
       <c r="AA145" s="15">
@@ -23003,10 +22936,10 @@
         <v>105</v>
       </c>
       <c r="U146" s="11" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="V146" s="11" t="s">
-        <v>925</v>
+        <v>983</v>
       </c>
       <c r="W146" s="1" t="s">
         <v>924</v>
@@ -23039,10 +22972,10 @@
         <v>53000144</v>
       </c>
       <c r="B147" s="22" t="s">
+        <v>934</v>
+      </c>
+      <c r="C147" s="15" t="s">
         <v>935</v>
-      </c>
-      <c r="C147" s="15" t="s">
-        <v>936</v>
       </c>
       <c r="D147" s="44" t="s">
         <v>918</v>
@@ -23099,10 +23032,10 @@
       </c>
       <c r="U147" s="15"/>
       <c r="V147" s="11" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="W147" s="1" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="X147" s="7">
         <v>100</v>
@@ -23132,10 +23065,10 @@
         <v>53000145</v>
       </c>
       <c r="B148" s="22" t="s">
+        <v>936</v>
+      </c>
+      <c r="C148" s="15" t="s">
         <v>937</v>
-      </c>
-      <c r="C148" s="15" t="s">
-        <v>938</v>
       </c>
       <c r="D148" s="25" t="s">
         <v>392</v>
@@ -23191,19 +23124,19 @@
         <v>102</v>
       </c>
       <c r="V148" s="11" t="s">
+        <v>942</v>
+      </c>
+      <c r="W148" s="1" t="s">
         <v>943</v>
-      </c>
-      <c r="W148" s="1" t="s">
-        <v>944</v>
       </c>
       <c r="X148" s="1">
         <v>202</v>
       </c>
       <c r="Y148" s="1" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="Z148" s="1" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="AA148" s="1">
         <v>11000001</v>
@@ -23303,7 +23236,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23397,7 +23330,7 @@
         <v>366</v>
       </c>
       <c r="U1" s="13" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="V1" s="13" t="s">
         <v>336</v>
@@ -23406,7 +23339,7 @@
         <v>296</v>
       </c>
       <c r="X1" s="13" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="Y1" s="13" t="s">
         <v>365</v>
@@ -23492,7 +23425,7 @@
         <v>454</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>473</v>
@@ -23501,7 +23434,7 @@
         <v>174</v>
       </c>
       <c r="X2" s="10" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="Y2" s="4" t="s">
         <v>174</v>
@@ -23587,7 +23520,7 @@
         <v>367</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="V3" s="6" t="s">
         <v>295</v>
@@ -23596,7 +23529,7 @@
         <v>297</v>
       </c>
       <c r="X3" s="6" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="Y3" s="6" t="s">
         <v>313</v>
@@ -23628,7 +23561,7 @@
         <v>350</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="D4" s="32"/>
       <c r="E4" s="15">
@@ -23717,7 +23650,7 @@
         <v>318</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="D5" s="32"/>
       <c r="E5" s="15">
@@ -23806,7 +23739,7 @@
         <v>353</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="D6" s="32"/>
       <c r="E6" s="15">
@@ -23893,7 +23826,7 @@
         <v>354</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="D7" s="32"/>
       <c r="E7" s="15">
@@ -23980,7 +23913,7 @@
         <v>355</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="D8" s="32"/>
       <c r="E8" s="15">
@@ -24067,7 +24000,7 @@
         <v>356</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="D9" s="32"/>
       <c r="E9" s="15">
@@ -24156,7 +24089,7 @@
         <v>472</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="15">
@@ -24210,10 +24143,10 @@
         <v>-1</v>
       </c>
       <c r="U10" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="V10" s="11" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="W10" s="7" t="s">
         <v>474</v>
@@ -24247,7 +24180,7 @@
         <v>504</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D11" s="32"/>
       <c r="E11" s="15">
@@ -24336,7 +24269,7 @@
         <v>660</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="D12" s="32"/>
       <c r="E12" s="15">
@@ -24423,7 +24356,7 @@
         <v>733</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="D13" s="32"/>
       <c r="E13" s="15">
@@ -24512,7 +24445,7 @@
         <v>737</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="D14" s="42"/>
       <c r="E14" s="15">
@@ -24600,7 +24533,7 @@
         <v>744</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="D15" s="32"/>
       <c r="E15" s="15">
@@ -24712,7 +24645,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AE9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -24807,7 +24740,7 @@
         <v>366</v>
       </c>
       <c r="U1" s="13" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="V1" s="13" t="s">
         <v>336</v>
@@ -24816,7 +24749,7 @@
         <v>296</v>
       </c>
       <c r="X1" s="13" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="Y1" s="13" t="s">
         <v>365</v>
@@ -24902,7 +24835,7 @@
         <v>454</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>312</v>
@@ -24911,7 +24844,7 @@
         <v>174</v>
       </c>
       <c r="X2" s="10" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="Y2" s="4" t="s">
         <v>174</v>
@@ -24997,7 +24930,7 @@
         <v>367</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="V3" s="6" t="s">
         <v>295</v>
@@ -25006,7 +24939,7 @@
         <v>297</v>
       </c>
       <c r="X3" s="6" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="Y3" s="6" t="s">
         <v>313</v>
@@ -25589,7 +25522,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -25793,7 +25726,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>